<commit_message>
remove indexing from filenames in lab2
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>лр1</t>
+  </si>
+  <si>
+    <t>лр2</t>
   </si>
 </sst>
 </file>
@@ -354,14 +357,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:5">
+      <c r="D1">
+        <f ca="1">SUM(C:C)</f>
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>3743</v>
+      </c>
+    </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -370,16 +384,8 @@
         <v>1662</v>
       </c>
       <c r="C2">
-        <f ca="1">IF(B2=$E$2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f ca="1">SUM(C:C)</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7426</v>
+        <f ca="1">IF(B2=$E$1,1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -388,7 +394,7 @@
         <v>1860</v>
       </c>
       <c r="C3">
-        <f ca="1">IF(B3=$E$2,1,0)</f>
+        <f ca="1">IF(B3=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -398,7 +404,7 @@
         <v>4764</v>
       </c>
       <c r="C4">
-        <f ca="1">IF(B4=$E$2,1,0)</f>
+        <f ca="1">IF(B4=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -408,7 +414,7 @@
         <v>2429</v>
       </c>
       <c r="C5">
-        <f ca="1">IF(B5=$E$2,1,0)</f>
+        <f ca="1">IF(B5=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -418,7 +424,7 @@
         <v>7472</v>
       </c>
       <c r="C6">
-        <f ca="1">IF(B6=$E$2,1,0)</f>
+        <f ca="1">IF(B6=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -428,7 +434,7 @@
         <v>3862</v>
       </c>
       <c r="C7">
-        <f ca="1">IF(B7=$E$2,1,0)</f>
+        <f ca="1">IF(B7=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -438,7 +444,7 @@
         <v>9231</v>
       </c>
       <c r="C8">
-        <f ca="1">IF(B8=$E$2,1,0)</f>
+        <f ca="1">IF(B8=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -448,7 +454,7 @@
         <v>8624</v>
       </c>
       <c r="C9">
-        <f ca="1">IF(B9=$E$2,1,0)</f>
+        <f ca="1">IF(B9=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -458,7 +464,7 @@
         <v>2959</v>
       </c>
       <c r="C10">
-        <f ca="1">IF(B10=$E$2,1,0)</f>
+        <f ca="1">IF(B10=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -468,7 +474,7 @@
         <v>7271</v>
       </c>
       <c r="C11">
-        <f ca="1">IF(B11=$E$2,1,0)</f>
+        <f ca="1">IF(B11=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -478,7 +484,7 @@
         <v>2632</v>
       </c>
       <c r="C12">
-        <f ca="1">IF(B12=$E$2,1,0)</f>
+        <f ca="1">IF(B12=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -488,7 +494,7 @@
         <v>4343</v>
       </c>
       <c r="C13">
-        <f ca="1">IF(B13=$E$2,1,0)</f>
+        <f ca="1">IF(B13=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -498,7 +504,7 @@
         <v>1517</v>
       </c>
       <c r="C14">
-        <f ca="1">IF(B14=$E$2,1,0)</f>
+        <f ca="1">IF(B14=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -508,7 +514,7 @@
         <v>1413</v>
       </c>
       <c r="C15">
-        <f ca="1">IF(B15=$E$2,1,0)</f>
+        <f ca="1">IF(B15=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -518,13 +524,416 @@
         <v>9405</v>
       </c>
       <c r="C16">
-        <f ca="1">IF(B16=$E$2,1,0)</f>
+        <f ca="1">IF(B16=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>4411</v>
+      </c>
+      <c r="C17">
+        <f ca="1">IF(B17=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1"/>
+      <c r="B18">
+        <v>9298</v>
+      </c>
+      <c r="C18">
+        <f ca="1">IF(B18=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+      <c r="B19">
+        <v>3354</v>
+      </c>
+      <c r="C19">
+        <f ca="1">IF(B19=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+      <c r="B20">
+        <v>8569</v>
+      </c>
+      <c r="C20">
+        <f ca="1">IF(B20=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21">
+        <v>3730</v>
+      </c>
+      <c r="C21">
+        <f ca="1">IF(B21=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22">
+        <v>9007</v>
+      </c>
+      <c r="C22">
+        <f ca="1">IF(B22=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23">
+        <v>5201</v>
+      </c>
+      <c r="C23">
+        <f ca="1">IF(B23=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1"/>
+      <c r="B24">
+        <v>2981</v>
+      </c>
+      <c r="C24">
+        <f ca="1">IF(B24=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1"/>
+      <c r="B25">
+        <v>4312</v>
+      </c>
+      <c r="C25">
+        <f ca="1">IF(B25=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1"/>
+      <c r="B26">
+        <v>8428</v>
+      </c>
+      <c r="C26">
+        <f ca="1">IF(B26=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
+      <c r="B27">
+        <v>2361</v>
+      </c>
+      <c r="C27">
+        <f ca="1">IF(B27=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28">
+        <v>5063</v>
+      </c>
+      <c r="C28">
+        <f ca="1">IF(B28=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+      <c r="B29">
+        <v>7711</v>
+      </c>
+      <c r="C29">
+        <f ca="1">IF(B29=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1"/>
+      <c r="B30">
+        <v>8833</v>
+      </c>
+      <c r="C30">
+        <f ca="1">IF(B30=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1"/>
+      <c r="B31">
+        <v>1262</v>
+      </c>
+      <c r="C31">
+        <f ca="1">IF(B31=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1"/>
+      <c r="B32">
+        <v>9020</v>
+      </c>
+      <c r="C32">
+        <f ca="1">IF(B32=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+      <c r="B33">
+        <v>1934</v>
+      </c>
+      <c r="C33">
+        <f ca="1">IF(B33=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1"/>
+      <c r="B34">
+        <v>7237</v>
+      </c>
+      <c r="C34">
+        <f ca="1">IF(B34=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+      <c r="B35">
+        <v>3943</v>
+      </c>
+      <c r="C35">
+        <f ca="1">IF(B35=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
+      <c r="B36">
+        <v>7619</v>
+      </c>
+      <c r="C36">
+        <f ca="1">IF(B36=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+      <c r="B37">
+        <v>3832</v>
+      </c>
+      <c r="C37">
+        <f ca="1">IF(B37=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+      <c r="B38">
+        <v>1346</v>
+      </c>
+      <c r="C38">
+        <f ca="1">IF(B38=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+      <c r="B39">
+        <v>9622</v>
+      </c>
+      <c r="C39">
+        <f ca="1">IF(B39=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+      <c r="B40">
+        <v>8873</v>
+      </c>
+      <c r="C40">
+        <f ca="1">IF(B40=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1"/>
+      <c r="B41">
+        <v>7799</v>
+      </c>
+      <c r="C41">
+        <f ca="1">IF(B41=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1"/>
+      <c r="B42">
+        <v>9354</v>
+      </c>
+      <c r="C42">
+        <f ca="1">IF(B42=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1"/>
+      <c r="B43">
+        <v>9130</v>
+      </c>
+      <c r="C43">
+        <f ca="1">IF(B43=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1"/>
+      <c r="B44">
+        <v>5895</v>
+      </c>
+      <c r="C44">
+        <f ca="1">IF(B44=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1"/>
+      <c r="B45">
+        <v>2461</v>
+      </c>
+      <c r="C45">
+        <f ca="1">IF(B45=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1"/>
+      <c r="B46">
+        <v>2790</v>
+      </c>
+      <c r="C46">
+        <f ca="1">IF(B46=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1"/>
+      <c r="B47">
+        <v>2624</v>
+      </c>
+      <c r="C47">
+        <f ca="1">IF(B47=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1"/>
+      <c r="B48">
+        <v>5871</v>
+      </c>
+      <c r="C48">
+        <f ca="1">IF(B48=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1"/>
+      <c r="B49">
+        <v>9164</v>
+      </c>
+      <c r="C49">
+        <f ca="1">IF(B49=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1"/>
+      <c r="B50">
+        <v>7457</v>
+      </c>
+      <c r="C50">
+        <f ca="1">IF(B50=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1"/>
+      <c r="B51">
+        <v>9865</v>
+      </c>
+      <c r="C51">
+        <f ca="1">IF(B51=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1"/>
+      <c r="B52">
+        <v>3591</v>
+      </c>
+      <c r="C52">
+        <f ca="1">IF(B52=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1"/>
+      <c r="B53">
+        <v>3558</v>
+      </c>
+      <c r="C53">
+        <f ca="1">IF(B53=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1"/>
+      <c r="B54">
+        <v>4366</v>
+      </c>
+      <c r="C54">
+        <f ca="1">IF(B54=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1"/>
+      <c r="B55">
+        <v>5789</v>
+      </c>
+      <c r="C55">
+        <f ca="1">IF(B55=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1"/>
+      <c r="B56">
+        <v>6522</v>
+      </c>
+      <c r="C56">
+        <f ca="1">IF(B56=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove indexing from filenames in lab3
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>лр1</t>
   </si>
   <si>
     <t>лр2</t>
+  </si>
+  <si>
+    <t>лр3</t>
   </si>
 </sst>
 </file>
@@ -357,11 +360,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:A56"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,7 +376,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3743</v>
+        <v>5170</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -384,7 +387,7 @@
         <v>1662</v>
       </c>
       <c r="C2">
-        <f ca="1">IF(B2=$E$1,1,0)</f>
+        <f t="shared" ref="C2:C33" ca="1" si="0">IF(B2=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -394,7 +397,7 @@
         <v>1860</v>
       </c>
       <c r="C3">
-        <f ca="1">IF(B3=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -404,7 +407,7 @@
         <v>4764</v>
       </c>
       <c r="C4">
-        <f ca="1">IF(B4=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -414,7 +417,7 @@
         <v>2429</v>
       </c>
       <c r="C5">
-        <f ca="1">IF(B5=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -424,7 +427,7 @@
         <v>7472</v>
       </c>
       <c r="C6">
-        <f ca="1">IF(B6=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -434,7 +437,7 @@
         <v>3862</v>
       </c>
       <c r="C7">
-        <f ca="1">IF(B7=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -444,7 +447,7 @@
         <v>9231</v>
       </c>
       <c r="C8">
-        <f ca="1">IF(B8=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -454,7 +457,7 @@
         <v>8624</v>
       </c>
       <c r="C9">
-        <f ca="1">IF(B9=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -464,7 +467,7 @@
         <v>2959</v>
       </c>
       <c r="C10">
-        <f ca="1">IF(B10=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -474,7 +477,7 @@
         <v>7271</v>
       </c>
       <c r="C11">
-        <f ca="1">IF(B11=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -484,7 +487,7 @@
         <v>2632</v>
       </c>
       <c r="C12">
-        <f ca="1">IF(B12=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -494,7 +497,7 @@
         <v>4343</v>
       </c>
       <c r="C13">
-        <f ca="1">IF(B13=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -504,7 +507,7 @@
         <v>1517</v>
       </c>
       <c r="C14">
-        <f ca="1">IF(B14=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -514,7 +517,7 @@
         <v>1413</v>
       </c>
       <c r="C15">
-        <f ca="1">IF(B15=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -524,7 +527,7 @@
         <v>9405</v>
       </c>
       <c r="C16">
-        <f ca="1">IF(B16=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -536,7 +539,7 @@
         <v>4411</v>
       </c>
       <c r="C17">
-        <f ca="1">IF(B17=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -546,7 +549,7 @@
         <v>9298</v>
       </c>
       <c r="C18">
-        <f ca="1">IF(B18=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -556,7 +559,7 @@
         <v>3354</v>
       </c>
       <c r="C19">
-        <f ca="1">IF(B19=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -566,7 +569,7 @@
         <v>8569</v>
       </c>
       <c r="C20">
-        <f ca="1">IF(B20=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -576,7 +579,7 @@
         <v>3730</v>
       </c>
       <c r="C21">
-        <f ca="1">IF(B21=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -586,7 +589,7 @@
         <v>9007</v>
       </c>
       <c r="C22">
-        <f ca="1">IF(B22=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -596,7 +599,7 @@
         <v>5201</v>
       </c>
       <c r="C23">
-        <f ca="1">IF(B23=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -606,7 +609,7 @@
         <v>2981</v>
       </c>
       <c r="C24">
-        <f ca="1">IF(B24=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -616,7 +619,7 @@
         <v>4312</v>
       </c>
       <c r="C25">
-        <f ca="1">IF(B25=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -626,7 +629,7 @@
         <v>8428</v>
       </c>
       <c r="C26">
-        <f ca="1">IF(B26=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -636,7 +639,7 @@
         <v>2361</v>
       </c>
       <c r="C27">
-        <f ca="1">IF(B27=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -646,7 +649,7 @@
         <v>5063</v>
       </c>
       <c r="C28">
-        <f ca="1">IF(B28=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -656,7 +659,7 @@
         <v>7711</v>
       </c>
       <c r="C29">
-        <f ca="1">IF(B29=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -666,7 +669,7 @@
         <v>8833</v>
       </c>
       <c r="C30">
-        <f ca="1">IF(B30=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -676,7 +679,7 @@
         <v>1262</v>
       </c>
       <c r="C31">
-        <f ca="1">IF(B31=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -686,7 +689,7 @@
         <v>9020</v>
       </c>
       <c r="C32">
-        <f ca="1">IF(B32=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -696,7 +699,7 @@
         <v>1934</v>
       </c>
       <c r="C33">
-        <f ca="1">IF(B33=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -706,7 +709,7 @@
         <v>7237</v>
       </c>
       <c r="C34">
-        <f ca="1">IF(B34=$E$1,1,0)</f>
+        <f t="shared" ref="C34:C72" ca="1" si="1">IF(B34=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -716,7 +719,7 @@
         <v>3943</v>
       </c>
       <c r="C35">
-        <f ca="1">IF(B35=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -726,7 +729,7 @@
         <v>7619</v>
       </c>
       <c r="C36">
-        <f ca="1">IF(B36=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -736,7 +739,7 @@
         <v>3832</v>
       </c>
       <c r="C37">
-        <f ca="1">IF(B37=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -746,7 +749,7 @@
         <v>1346</v>
       </c>
       <c r="C38">
-        <f ca="1">IF(B38=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -756,7 +759,7 @@
         <v>9622</v>
       </c>
       <c r="C39">
-        <f ca="1">IF(B39=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -766,7 +769,7 @@
         <v>8873</v>
       </c>
       <c r="C40">
-        <f ca="1">IF(B40=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -776,7 +779,7 @@
         <v>7799</v>
       </c>
       <c r="C41">
-        <f ca="1">IF(B41=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -786,7 +789,7 @@
         <v>9354</v>
       </c>
       <c r="C42">
-        <f ca="1">IF(B42=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -796,7 +799,7 @@
         <v>9130</v>
       </c>
       <c r="C43">
-        <f ca="1">IF(B43=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -806,7 +809,7 @@
         <v>5895</v>
       </c>
       <c r="C44">
-        <f ca="1">IF(B44=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -816,7 +819,7 @@
         <v>2461</v>
       </c>
       <c r="C45">
-        <f ca="1">IF(B45=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -826,7 +829,7 @@
         <v>2790</v>
       </c>
       <c r="C46">
-        <f ca="1">IF(B46=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -836,7 +839,7 @@
         <v>2624</v>
       </c>
       <c r="C47">
-        <f ca="1">IF(B47=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -846,7 +849,7 @@
         <v>5871</v>
       </c>
       <c r="C48">
-        <f ca="1">IF(B48=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -856,7 +859,7 @@
         <v>9164</v>
       </c>
       <c r="C49">
-        <f ca="1">IF(B49=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -866,7 +869,7 @@
         <v>7457</v>
       </c>
       <c r="C50">
-        <f ca="1">IF(B50=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -876,7 +879,7 @@
         <v>9865</v>
       </c>
       <c r="C51">
-        <f ca="1">IF(B51=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -886,7 +889,7 @@
         <v>3591</v>
       </c>
       <c r="C52">
-        <f ca="1">IF(B52=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -896,7 +899,7 @@
         <v>3558</v>
       </c>
       <c r="C53">
-        <f ca="1">IF(B53=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -906,7 +909,7 @@
         <v>4366</v>
       </c>
       <c r="C54">
-        <f ca="1">IF(B54=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -916,7 +919,7 @@
         <v>5789</v>
       </c>
       <c r="C55">
-        <f ca="1">IF(B55=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -926,14 +929,177 @@
         <v>6522</v>
       </c>
       <c r="C56">
-        <f ca="1">IF(B56=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57">
+        <v>8545</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1"/>
+      <c r="B58">
+        <v>1288</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1"/>
+      <c r="B59">
+        <v>2614</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1"/>
+      <c r="B60">
+        <v>7170</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1"/>
+      <c r="B61">
+        <v>2709</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1"/>
+      <c r="B62">
+        <v>3402</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1"/>
+      <c r="B63">
+        <v>8781</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1"/>
+      <c r="B64">
+        <v>8771</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1"/>
+      <c r="B65">
+        <v>3091</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1"/>
+      <c r="B66">
+        <v>2195</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1"/>
+      <c r="B67">
+        <v>1184</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1"/>
+      <c r="B68">
+        <v>2667</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1"/>
+      <c r="B69">
+        <v>5917</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1"/>
+      <c r="B70">
+        <v>3929</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1"/>
+      <c r="B71">
+        <v>3083</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1"/>
+      <c r="B72">
+        <v>7546</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
+    <mergeCell ref="A57:A72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove indexing from filenames in lab6
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>лр1</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>лр5</t>
+  </si>
+  <si>
+    <t>лр6</t>
   </si>
 </sst>
 </file>
@@ -374,8 +377,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79:A118"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119:A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -387,7 +390,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7400</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1571,252 +1574,394 @@
       </c>
     </row>
     <row r="119" spans="1:3">
+      <c r="A119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119">
+        <v>7779</v>
+      </c>
       <c r="C119">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3">
+      <c r="A120" s="1"/>
+      <c r="B120">
+        <v>8495</v>
+      </c>
       <c r="C120">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:3">
+      <c r="A121" s="1"/>
+      <c r="B121">
+        <v>1315</v>
+      </c>
       <c r="C121">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3">
+      <c r="A122" s="1"/>
+      <c r="B122">
+        <v>6066</v>
+      </c>
       <c r="C122">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3">
+      <c r="A123" s="1"/>
+      <c r="B123">
+        <v>2565</v>
+      </c>
       <c r="C123">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:3">
+      <c r="A124" s="1"/>
+      <c r="B124">
+        <v>2594</v>
+      </c>
       <c r="C124">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:3">
+      <c r="A125" s="1"/>
+      <c r="B125">
+        <v>3762</v>
+      </c>
       <c r="C125">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3">
+      <c r="A126" s="1"/>
+      <c r="B126">
+        <v>3550</v>
+      </c>
       <c r="C126">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:3">
+      <c r="A127" s="1"/>
+      <c r="B127">
+        <v>2475</v>
+      </c>
       <c r="C127">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:3">
+      <c r="A128" s="1"/>
+      <c r="B128">
+        <v>9180</v>
+      </c>
       <c r="C128">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="3:3">
+    <row r="129" spans="1:3">
+      <c r="A129" s="1"/>
+      <c r="B129">
+        <v>1544</v>
+      </c>
       <c r="C129">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="3:3">
+    <row r="130" spans="1:3">
+      <c r="A130" s="1"/>
+      <c r="B130">
+        <v>9562</v>
+      </c>
       <c r="C130">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="1:3">
+      <c r="A131" s="1"/>
+      <c r="B131">
+        <v>3669</v>
+      </c>
       <c r="C131">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="3:3">
+    <row r="132" spans="1:3">
+      <c r="A132" s="1"/>
+      <c r="B132">
+        <v>5951</v>
+      </c>
       <c r="C132">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="3:3">
+    <row r="133" spans="1:3">
+      <c r="A133" s="1"/>
+      <c r="B133">
+        <v>2802</v>
+      </c>
       <c r="C133">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="3:3">
+    <row r="134" spans="1:3">
+      <c r="A134" s="1"/>
+      <c r="B134">
+        <v>6580</v>
+      </c>
       <c r="C134">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="3:3">
+    <row r="135" spans="1:3">
+      <c r="A135" s="1"/>
+      <c r="B135">
+        <v>7585</v>
+      </c>
       <c r="C135">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="3:3">
+    <row r="136" spans="1:3">
+      <c r="A136" s="1"/>
+      <c r="B136">
+        <v>8770</v>
+      </c>
       <c r="C136">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="3:3">
+    <row r="137" spans="1:3">
+      <c r="A137" s="1"/>
+      <c r="B137">
+        <v>4236</v>
+      </c>
       <c r="C137">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="3:3">
+    <row r="138" spans="1:3">
+      <c r="A138" s="1"/>
+      <c r="B138">
+        <v>5969</v>
+      </c>
       <c r="C138">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="3:3">
+    <row r="139" spans="1:3">
+      <c r="A139" s="1"/>
+      <c r="B139">
+        <v>8696</v>
+      </c>
       <c r="C139">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="3:3">
+    <row r="140" spans="1:3">
+      <c r="A140" s="1"/>
+      <c r="B140">
+        <v>8418</v>
+      </c>
       <c r="C140">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="3:3">
+    <row r="141" spans="1:3">
+      <c r="A141" s="1"/>
+      <c r="B141">
+        <v>8395</v>
+      </c>
       <c r="C141">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="3:3">
+    <row r="142" spans="1:3">
+      <c r="A142" s="1"/>
+      <c r="B142">
+        <v>5568</v>
+      </c>
       <c r="C142">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="3:3">
+    <row r="143" spans="1:3">
+      <c r="A143" s="1"/>
+      <c r="B143">
+        <v>2592</v>
+      </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="3:3">
+    <row r="144" spans="1:3">
+      <c r="A144" s="1"/>
+      <c r="B144">
+        <v>4075</v>
+      </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="3:3">
+    <row r="145" spans="1:3">
+      <c r="A145" s="1"/>
+      <c r="B145">
+        <v>7517</v>
+      </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="3:3">
+    <row r="146" spans="1:3">
+      <c r="A146" s="1"/>
+      <c r="B146">
+        <v>5448</v>
+      </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="3:3">
+    <row r="147" spans="1:3">
+      <c r="A147" s="1"/>
+      <c r="B147">
+        <v>6572</v>
+      </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="3:3">
+    <row r="148" spans="1:3">
+      <c r="A148" s="1"/>
+      <c r="B148">
+        <v>5238</v>
+      </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="3:3">
+    <row r="149" spans="1:3">
+      <c r="A149" s="1"/>
+      <c r="B149">
+        <v>2084</v>
+      </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="3:3">
+    <row r="150" spans="1:3">
+      <c r="A150" s="1"/>
+      <c r="B150">
+        <v>5411</v>
+      </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="3:3">
+    <row r="151" spans="1:3">
+      <c r="A151" s="1"/>
+      <c r="B151">
+        <v>5171</v>
+      </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="3:3">
+    <row r="152" spans="1:3">
+      <c r="A152" s="1"/>
+      <c r="B152">
+        <v>1862</v>
+      </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="3:3">
+    <row r="153" spans="1:3">
+      <c r="A153" s="1"/>
+      <c r="B153">
+        <v>9238</v>
+      </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="3:3">
+    <row r="154" spans="1:3">
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="3:3">
+    <row r="155" spans="1:3">
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="3:3">
+    <row r="156" spans="1:3">
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="3:3">
+    <row r="157" spans="1:3">
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="3:3">
+    <row r="158" spans="1:3">
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="3:3">
+    <row r="159" spans="1:3">
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="3:3">
+    <row r="160" spans="1:3">
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
@@ -6143,7 +6288,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A119:A153"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>

</xml_diff>

<commit_message>
remove indexing from filenames in lab7
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>лр1</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>лр6</t>
+  </si>
+  <si>
+    <t>лр7</t>
   </si>
 </sst>
 </file>
@@ -377,8 +380,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A119" sqref="A119:A153"/>
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A154" sqref="A154:A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -390,7 +393,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3778</v>
+        <v>8995</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1926,138 +1929,184 @@
       </c>
     </row>
     <row r="154" spans="1:3">
+      <c r="A154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154">
+        <v>8165</v>
+      </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:3">
+      <c r="A155" s="1"/>
+      <c r="B155">
+        <v>9001</v>
+      </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:3">
+      <c r="A156" s="1"/>
+      <c r="B156">
+        <v>9631</v>
+      </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3">
+      <c r="A157" s="1"/>
+      <c r="B157">
+        <v>9812</v>
+      </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3">
+      <c r="A158" s="1"/>
+      <c r="B158">
+        <v>5728</v>
+      </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:3">
+      <c r="A159" s="1"/>
+      <c r="B159">
+        <v>7491</v>
+      </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:3">
+      <c r="A160" s="1"/>
+      <c r="B160">
+        <v>5923</v>
+      </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="3:3">
+    <row r="161" spans="1:3">
+      <c r="A161" s="1"/>
+      <c r="B161">
+        <v>4265</v>
+      </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="3:3">
+    <row r="162" spans="1:3">
+      <c r="A162" s="1"/>
+      <c r="B162">
+        <v>2166</v>
+      </c>
       <c r="C162">
         <f t="shared" ref="C162:C225" ca="1" si="4">IF(B162=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="3:3">
+    <row r="163" spans="1:3">
+      <c r="A163" s="1"/>
+      <c r="B163">
+        <v>9116</v>
+      </c>
       <c r="C163">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="3:3">
+    <row r="164" spans="1:3">
+      <c r="A164" s="1"/>
+      <c r="B164">
+        <v>9925</v>
+      </c>
       <c r="C164">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="3:3">
+    <row r="165" spans="1:3">
       <c r="C165">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="3:3">
+    <row r="166" spans="1:3">
       <c r="C166">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="3:3">
+    <row r="167" spans="1:3">
       <c r="C167">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="3:3">
+    <row r="168" spans="1:3">
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="3:3">
+    <row r="169" spans="1:3">
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="3:3">
+    <row r="170" spans="1:3">
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="3:3">
+    <row r="171" spans="1:3">
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="3:3">
+    <row r="172" spans="1:3">
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="3:3">
+    <row r="173" spans="1:3">
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="3:3">
+    <row r="174" spans="1:3">
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="3:3">
+    <row r="175" spans="1:3">
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="3:3">
+    <row r="176" spans="1:3">
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6288,7 +6337,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A154:A164"/>
     <mergeCell ref="A119:A153"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>

</xml_diff>

<commit_message>
remove indexing from filenames in lab8
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>лр1</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>лр7</t>
+  </si>
+  <si>
+    <t>лр8</t>
   </si>
 </sst>
 </file>
@@ -380,8 +383,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A154" sqref="A154:A164"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165:A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -393,7 +396,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>8995</v>
+        <v>7506</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2041,168 +2044,274 @@
       </c>
     </row>
     <row r="165" spans="1:3">
+      <c r="A165" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165">
+        <v>2885</v>
+      </c>
       <c r="C165">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3">
+      <c r="A166" s="1"/>
+      <c r="B166">
+        <v>9931</v>
+      </c>
       <c r="C166">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3">
+      <c r="A167" s="1"/>
+      <c r="B167">
+        <v>1947</v>
+      </c>
       <c r="C167">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3">
+      <c r="A168" s="1"/>
+      <c r="B168">
+        <v>9696</v>
+      </c>
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:3">
+      <c r="A169" s="1"/>
+      <c r="B169">
+        <v>1223</v>
+      </c>
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:3">
+      <c r="A170" s="1"/>
+      <c r="B170">
+        <v>3946</v>
+      </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:3">
+      <c r="A171" s="1"/>
+      <c r="B171">
+        <v>8311</v>
+      </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:3">
+      <c r="A172" s="1"/>
+      <c r="B172">
+        <v>3134</v>
+      </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:3">
+      <c r="A173" s="1"/>
+      <c r="B173">
+        <v>9774</v>
+      </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:3">
+      <c r="A174" s="1"/>
+      <c r="B174">
+        <v>9711</v>
+      </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:3">
+      <c r="A175" s="1"/>
+      <c r="B175">
+        <v>3333</v>
+      </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:3">
+      <c r="A176" s="1"/>
+      <c r="B176">
+        <v>7290</v>
+      </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="3:3">
+    <row r="177" spans="1:3">
+      <c r="A177" s="1"/>
+      <c r="B177">
+        <v>5694</v>
+      </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="3:3">
+    <row r="178" spans="1:3">
+      <c r="A178" s="1"/>
+      <c r="B178">
+        <v>6806</v>
+      </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="3:3">
+    <row r="179" spans="1:3">
+      <c r="A179" s="1"/>
+      <c r="B179">
+        <v>4515</v>
+      </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="3:3">
+    <row r="180" spans="1:3">
+      <c r="A180" s="1"/>
+      <c r="B180">
+        <v>9271</v>
+      </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="3:3">
+    <row r="181" spans="1:3">
+      <c r="A181" s="1"/>
+      <c r="B181">
+        <v>8769</v>
+      </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="3:3">
+    <row r="182" spans="1:3">
+      <c r="A182" s="1"/>
+      <c r="B182">
+        <v>4497</v>
+      </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="3:3">
+    <row r="183" spans="1:3">
+      <c r="A183" s="1"/>
+      <c r="B183">
+        <v>8820</v>
+      </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="3:3">
+    <row r="184" spans="1:3">
+      <c r="A184" s="1"/>
+      <c r="B184">
+        <v>3218</v>
+      </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="3:3">
+    <row r="185" spans="1:3">
+      <c r="A185" s="1"/>
+      <c r="B185">
+        <v>4283</v>
+      </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="3:3">
+    <row r="186" spans="1:3">
+      <c r="A186" s="1"/>
+      <c r="B186">
+        <v>7703</v>
+      </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="3:3">
+    <row r="187" spans="1:3">
+      <c r="A187" s="1"/>
+      <c r="B187">
+        <v>9182</v>
+      </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="3:3">
+    <row r="188" spans="1:3">
+      <c r="A188" s="1"/>
+      <c r="B188">
+        <v>5541</v>
+      </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="3:3">
+    <row r="189" spans="1:3">
+      <c r="A189" s="1"/>
+      <c r="B189">
+        <v>2386</v>
+      </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="3:3">
+    <row r="190" spans="1:3">
+      <c r="A190" s="1"/>
+      <c r="B190">
+        <v>9159</v>
+      </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="3:3">
+    <row r="191" spans="1:3">
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="3:3">
+    <row r="192" spans="1:3">
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6337,7 +6446,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A165:A190"/>
     <mergeCell ref="A154:A164"/>
     <mergeCell ref="A119:A153"/>
     <mergeCell ref="A2:A16"/>

</xml_diff>

<commit_message>
remove indexing from filenames in lab9
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>лр1</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>лр8</t>
+  </si>
+  <si>
+    <t>лр9</t>
   </si>
 </sst>
 </file>
@@ -383,8 +386,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A165" sqref="A165:A190"/>
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A191" sqref="A191:A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -396,7 +399,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7506</v>
+        <v>7291</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2306,108 +2309,178 @@
       </c>
     </row>
     <row r="191" spans="1:3">
+      <c r="A191" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B191">
+        <v>6175</v>
+      </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:3">
+      <c r="A192" s="1"/>
+      <c r="B192">
+        <v>4642</v>
+      </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="3:3">
+    <row r="193" spans="1:3">
+      <c r="A193" s="1"/>
+      <c r="B193">
+        <v>9765</v>
+      </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="3:3">
+    <row r="194" spans="1:3">
+      <c r="A194" s="1"/>
+      <c r="B194">
+        <v>4954</v>
+      </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="3:3">
+    <row r="195" spans="1:3">
+      <c r="A195" s="1"/>
+      <c r="B195">
+        <v>5537</v>
+      </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="3:3">
+    <row r="196" spans="1:3">
+      <c r="A196" s="1"/>
+      <c r="B196">
+        <v>6431</v>
+      </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="3:3">
+    <row r="197" spans="1:3">
+      <c r="A197" s="1"/>
+      <c r="B197">
+        <v>7193</v>
+      </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="3:3">
+    <row r="198" spans="1:3">
+      <c r="A198" s="1"/>
+      <c r="B198">
+        <v>5621</v>
+      </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="3:3">
+    <row r="199" spans="1:3">
+      <c r="A199" s="1"/>
+      <c r="B199">
+        <v>5847</v>
+      </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="3:3">
+    <row r="200" spans="1:3">
+      <c r="A200" s="1"/>
+      <c r="B200">
+        <v>4769</v>
+      </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="3:3">
+    <row r="201" spans="1:3">
+      <c r="A201" s="1"/>
+      <c r="B201">
+        <v>9930</v>
+      </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="3:3">
+    <row r="202" spans="1:3">
+      <c r="A202" s="1"/>
+      <c r="B202">
+        <v>6861</v>
+      </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="3:3">
+    <row r="203" spans="1:3">
+      <c r="A203" s="1"/>
+      <c r="B203">
+        <v>2205</v>
+      </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="3:3">
+    <row r="204" spans="1:3">
+      <c r="A204" s="1"/>
+      <c r="B204">
+        <v>4372</v>
+      </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="3:3">
+    <row r="205" spans="1:3">
+      <c r="A205" s="1"/>
+      <c r="B205">
+        <v>4463</v>
+      </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="3:3">
+    <row r="206" spans="1:3">
+      <c r="A206" s="1"/>
+      <c r="B206">
+        <v>1668</v>
+      </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="3:3">
+    <row r="207" spans="1:3">
+      <c r="A207" s="1"/>
+      <c r="B207">
+        <v>2137</v>
+      </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="3:3">
+    <row r="208" spans="1:3">
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6446,7 +6519,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A191:A207"/>
     <mergeCell ref="A165:A190"/>
     <mergeCell ref="A154:A164"/>
     <mergeCell ref="A119:A153"/>

</xml_diff>

<commit_message>
remove indexing from filenames in lab10
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>лр1</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>лр9</t>
+  </si>
+  <si>
+    <t>лр10</t>
   </si>
 </sst>
 </file>
@@ -386,8 +389,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A191" sqref="A191:A207"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208:A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -399,7 +402,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7291</v>
+        <v>9730</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2481,102 +2484,124 @@
       </c>
     </row>
     <row r="208" spans="1:3">
+      <c r="A208" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208">
+        <v>9300</v>
+      </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="3:3">
+    <row r="209" spans="1:3">
+      <c r="A209" s="1"/>
+      <c r="B209">
+        <v>3951</v>
+      </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="3:3">
+    <row r="210" spans="1:3">
+      <c r="A210" s="1"/>
+      <c r="B210">
+        <v>6409</v>
+      </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="3:3">
+    <row r="211" spans="1:3">
+      <c r="A211" s="1"/>
+      <c r="B211">
+        <v>7343</v>
+      </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="3:3">
+    <row r="212" spans="1:3">
+      <c r="A212" s="1"/>
+      <c r="B212">
+        <v>7060</v>
+      </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="3:3">
+    <row r="213" spans="1:3">
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="3:3">
+    <row r="214" spans="1:3">
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="3:3">
+    <row r="215" spans="1:3">
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="3:3">
+    <row r="216" spans="1:3">
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="3:3">
+    <row r="217" spans="1:3">
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="3:3">
+    <row r="218" spans="1:3">
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="3:3">
+    <row r="219" spans="1:3">
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="3:3">
+    <row r="220" spans="1:3">
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="3:3">
+    <row r="221" spans="1:3">
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="3:3">
+    <row r="222" spans="1:3">
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="3:3">
+    <row r="223" spans="1:3">
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="3:3">
+    <row r="224" spans="1:3">
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6519,7 +6544,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A208:A212"/>
     <mergeCell ref="A191:A207"/>
     <mergeCell ref="A165:A190"/>
     <mergeCell ref="A154:A164"/>

</xml_diff>

<commit_message>
remove indexing from filenames in labs 11,12,14
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>лр1</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>лр10</t>
+  </si>
+  <si>
+    <t>лр11</t>
+  </si>
+  <si>
+    <t>лр12</t>
+  </si>
+  <si>
+    <t>лр14</t>
   </si>
 </sst>
 </file>
@@ -389,8 +398,8 @@
   <dimension ref="A1:E880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208:A212"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A222" sqref="A222:A238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -402,7 +411,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9730</v>
+        <v>9257</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2536,168 +2545,278 @@
       </c>
     </row>
     <row r="213" spans="1:3">
+      <c r="A213" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B213">
+        <v>9299</v>
+      </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:3">
+      <c r="A214" s="1"/>
+      <c r="B214">
+        <v>7560</v>
+      </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:3">
+      <c r="A215" s="1"/>
+      <c r="B215">
+        <v>9002</v>
+      </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:3">
+      <c r="A216" s="1"/>
+      <c r="B216">
+        <v>7432</v>
+      </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:3">
+      <c r="A217" s="1"/>
+      <c r="B217">
+        <v>1954</v>
+      </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:3">
+      <c r="A218" s="1"/>
+      <c r="B218">
+        <v>2048</v>
+      </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:3">
+      <c r="A219" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B219">
+        <v>3939</v>
+      </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:3">
+      <c r="A220" s="1"/>
+      <c r="B220">
+        <v>1516</v>
+      </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:3">
+      <c r="A221" s="1"/>
+      <c r="B221">
+        <v>9062</v>
+      </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:3">
+      <c r="A222" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B222">
+        <v>8403</v>
+      </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:3">
+      <c r="A223" s="1"/>
+      <c r="B223">
+        <v>3185</v>
+      </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3">
+      <c r="A224" s="1"/>
+      <c r="B224">
+        <v>9914</v>
+      </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="3:3">
+    <row r="225" spans="1:3">
+      <c r="A225" s="1"/>
+      <c r="B225">
+        <v>6011</v>
+      </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="3:3">
+    <row r="226" spans="1:3">
+      <c r="A226" s="1"/>
+      <c r="B226">
+        <v>6037</v>
+      </c>
       <c r="C226">
         <f t="shared" ref="C226:C289" ca="1" si="5">IF(B226=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="3:3">
+    <row r="227" spans="1:3">
+      <c r="A227" s="1"/>
+      <c r="B227">
+        <v>2809</v>
+      </c>
       <c r="C227">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="3:3">
+    <row r="228" spans="1:3">
+      <c r="A228" s="1"/>
+      <c r="B228">
+        <v>7297</v>
+      </c>
       <c r="C228">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="3:3">
+    <row r="229" spans="1:3">
+      <c r="A229" s="1"/>
+      <c r="B229">
+        <v>5242</v>
+      </c>
       <c r="C229">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="3:3">
+    <row r="230" spans="1:3">
+      <c r="A230" s="1"/>
+      <c r="B230">
+        <v>1379</v>
+      </c>
       <c r="C230">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="3:3">
+    <row r="231" spans="1:3">
+      <c r="A231" s="1"/>
+      <c r="B231">
+        <v>2401</v>
+      </c>
       <c r="C231">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="3:3">
+    <row r="232" spans="1:3">
+      <c r="A232" s="1"/>
+      <c r="B232">
+        <v>5421</v>
+      </c>
       <c r="C232">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="3:3">
+    <row r="233" spans="1:3">
+      <c r="A233" s="1"/>
+      <c r="B233">
+        <v>7301</v>
+      </c>
       <c r="C233">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="3:3">
+    <row r="234" spans="1:3">
+      <c r="A234" s="1"/>
+      <c r="B234">
+        <v>2000</v>
+      </c>
       <c r="C234">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="3:3">
+    <row r="235" spans="1:3">
+      <c r="A235" s="1"/>
+      <c r="B235">
+        <v>4147</v>
+      </c>
       <c r="C235">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="3:3">
+    <row r="236" spans="1:3">
+      <c r="A236" s="1"/>
+      <c r="B236">
+        <v>1953</v>
+      </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="3:3">
+    <row r="237" spans="1:3">
+      <c r="A237" s="1"/>
+      <c r="B237">
+        <v>3956</v>
+      </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="3:3">
+    <row r="238" spans="1:3">
+      <c r="A238" s="1"/>
+      <c r="B238">
+        <v>5463</v>
+      </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="3:3">
+    <row r="239" spans="1:3">
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="3:3">
+    <row r="240" spans="1:3">
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -6544,17 +6663,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="A213:A218"/>
+    <mergeCell ref="A219:A221"/>
+    <mergeCell ref="A222:A238"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A56"/>
+    <mergeCell ref="A57:A72"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="A79:A118"/>
     <mergeCell ref="A208:A212"/>
     <mergeCell ref="A191:A207"/>
     <mergeCell ref="A165:A190"/>
     <mergeCell ref="A154:A164"/>
     <mergeCell ref="A119:A153"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A17:A56"/>
-    <mergeCell ref="A57:A72"/>
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="A79:A118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 12 lab for js to master
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -395,11 +395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E880"/>
+  <dimension ref="A1:E881"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A222" sqref="A222:A238"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D225" sqref="D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,11 +407,11 @@
     <row r="1" spans="1:5">
       <c r="D1">
         <f ca="1">SUM(C:C)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9257</v>
+        <v>6556</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2034,7 +2034,7 @@
         <v>2166</v>
       </c>
       <c r="C162">
-        <f t="shared" ref="C162:C225" ca="1" si="4">IF(B162=$E$1,1,0)</f>
+        <f t="shared" ref="C162:C226" ca="1" si="4">IF(B162=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
     <row r="220" spans="1:3">
       <c r="A220" s="1"/>
       <c r="B220">
-        <v>1516</v>
+        <v>8861</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2631,7 +2631,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="1"/>
       <c r="B221">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2639,11 +2639,9 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A222" s="1"/>
       <c r="B222">
-        <v>8403</v>
+        <v>9062</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2651,9 +2649,11 @@
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="1"/>
+      <c r="A223" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B223">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2663,7 +2663,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="1"/>
       <c r="B224">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2673,7 +2673,7 @@
     <row r="225" spans="1:3">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2683,27 +2683,27 @@
     <row r="226" spans="1:3">
       <c r="A226" s="1"/>
       <c r="B226">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C226">
-        <f t="shared" ref="C226:C289" ca="1" si="5">IF(B226=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="1"/>
       <c r="B227">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C227">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C227:C290" ca="1" si="5">IF(B227=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="1"/>
       <c r="B228">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="5"/>
@@ -2713,7 +2713,7 @@
     <row r="229" spans="1:3">
       <c r="A229" s="1"/>
       <c r="B229">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="5"/>
@@ -2723,7 +2723,7 @@
     <row r="230" spans="1:3">
       <c r="A230" s="1"/>
       <c r="B230">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="5"/>
@@ -2733,7 +2733,7 @@
     <row r="231" spans="1:3">
       <c r="A231" s="1"/>
       <c r="B231">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="5"/>
@@ -2743,7 +2743,7 @@
     <row r="232" spans="1:3">
       <c r="A232" s="1"/>
       <c r="B232">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="5"/>
@@ -2753,7 +2753,7 @@
     <row r="233" spans="1:3">
       <c r="A233" s="1"/>
       <c r="B233">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="5"/>
@@ -2763,7 +2763,7 @@
     <row r="234" spans="1:3">
       <c r="A234" s="1"/>
       <c r="B234">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="5"/>
@@ -2773,7 +2773,7 @@
     <row r="235" spans="1:3">
       <c r="A235" s="1"/>
       <c r="B235">
-        <v>4147</v>
+        <v>2000</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="5"/>
@@ -2783,7 +2783,7 @@
     <row r="236" spans="1:3">
       <c r="A236" s="1"/>
       <c r="B236">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2793,7 +2793,7 @@
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2803,7 +2803,7 @@
     <row r="238" spans="1:3">
       <c r="A238" s="1"/>
       <c r="B238">
-        <v>5463</v>
+        <v>3956</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2811,6 +2811,10 @@
       </c>
     </row>
     <row r="239" spans="1:3">
+      <c r="A239" s="1"/>
+      <c r="B239">
+        <v>5463</v>
+      </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3118,13 +3122,13 @@
     </row>
     <row r="290" spans="3:3">
       <c r="C290">
-        <f t="shared" ref="C290:C353" ca="1" si="6">IF(B290=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="291" spans="3:3">
       <c r="C291">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C291:C354" ca="1" si="6">IF(B291=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3502,13 +3506,13 @@
     </row>
     <row r="354" spans="3:3">
       <c r="C354">
-        <f t="shared" ref="C354:C417" ca="1" si="7">IF(B354=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="355" spans="3:3">
       <c r="C355">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C355:C418" ca="1" si="7">IF(B355=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3886,13 +3890,13 @@
     </row>
     <row r="418" spans="3:3">
       <c r="C418">
-        <f t="shared" ref="C418:C481" ca="1" si="8">IF(B418=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="419" spans="3:3">
       <c r="C419">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C419:C482" ca="1" si="8">IF(B419=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4270,13 +4274,13 @@
     </row>
     <row r="482" spans="3:3">
       <c r="C482">
-        <f t="shared" ref="C482:C545" ca="1" si="9">IF(B482=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="483" spans="3:3">
       <c r="C483">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C483:C546" ca="1" si="9">IF(B483=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4654,13 +4658,13 @@
     </row>
     <row r="546" spans="3:3">
       <c r="C546">
-        <f t="shared" ref="C546:C609" ca="1" si="10">IF(B546=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="547" spans="3:3">
       <c r="C547">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C547:C610" ca="1" si="10">IF(B547=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5038,13 +5042,13 @@
     </row>
     <row r="610" spans="3:3">
       <c r="C610">
-        <f t="shared" ref="C610:C673" ca="1" si="11">IF(B610=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="611" spans="3:3">
       <c r="C611">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C611:C674" ca="1" si="11">IF(B611=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5422,13 +5426,13 @@
     </row>
     <row r="674" spans="3:3">
       <c r="C674">
-        <f t="shared" ref="C674:C737" ca="1" si="12">IF(B674=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="3:3">
       <c r="C675">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C675:C738" ca="1" si="12">IF(B675=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5806,13 +5810,13 @@
     </row>
     <row r="738" spans="3:3">
       <c r="C738">
-        <f t="shared" ref="C738:C801" ca="1" si="13">IF(B738=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="3:3">
       <c r="C739">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C739:C802" ca="1" si="13">IF(B739=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6190,13 +6194,13 @@
     </row>
     <row r="802" spans="3:3">
       <c r="C802">
-        <f t="shared" ref="C802:C865" ca="1" si="14">IF(B802=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="803" spans="3:3">
       <c r="C803">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C803:C866" ca="1" si="14">IF(B803=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6574,13 +6578,13 @@
     </row>
     <row r="866" spans="3:3">
       <c r="C866">
-        <f t="shared" ref="C866:C880" ca="1" si="15">IF(B866=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="867" spans="3:3">
       <c r="C867">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C867:C881" ca="1" si="15">IF(B867=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6662,11 +6666,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="881" spans="3:3">
+      <c r="C881">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A213:A218"/>
-    <mergeCell ref="A219:A221"/>
-    <mergeCell ref="A222:A238"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A239"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>

</xml_diff>

<commit_message>
add tasks for methods in java change wording of link text
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -91,8 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -395,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E881"/>
+  <dimension ref="A1:E884"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D225" sqref="D225"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,15 +410,15 @@
     <row r="1" spans="1:5">
       <c r="D1">
         <f ca="1">SUM(C:C)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>6556</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -427,7 +430,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3">
         <v>1860</v>
       </c>
@@ -437,7 +440,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4">
         <v>4764</v>
       </c>
@@ -447,7 +450,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5">
         <v>2429</v>
       </c>
@@ -457,7 +460,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6">
         <v>7472</v>
       </c>
@@ -467,7 +470,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7">
         <v>3862</v>
       </c>
@@ -477,7 +480,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8">
         <v>9231</v>
       </c>
@@ -487,7 +490,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9">
         <v>8624</v>
       </c>
@@ -497,7 +500,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10">
         <v>2959</v>
       </c>
@@ -507,7 +510,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11">
         <v>7271</v>
       </c>
@@ -517,7 +520,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12">
         <v>2632</v>
       </c>
@@ -527,7 +530,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13">
         <v>4343</v>
       </c>
@@ -537,7 +540,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14">
         <v>1517</v>
       </c>
@@ -547,7 +550,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15">
         <v>1413</v>
       </c>
@@ -557,7 +560,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="B16">
         <v>9405</v>
       </c>
@@ -567,7 +570,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B17">
@@ -579,7 +582,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18">
         <v>9298</v>
       </c>
@@ -589,7 +592,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19">
         <v>3354</v>
       </c>
@@ -599,7 +602,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
       <c r="B20">
         <v>8569</v>
       </c>
@@ -609,7 +612,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
       <c r="B21">
         <v>3730</v>
       </c>
@@ -619,7 +622,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
       <c r="B22">
         <v>9007</v>
       </c>
@@ -629,7 +632,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
       <c r="B23">
         <v>5201</v>
       </c>
@@ -639,7 +642,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
       <c r="B24">
         <v>2981</v>
       </c>
@@ -649,7 +652,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
       <c r="B25">
         <v>4312</v>
       </c>
@@ -659,7 +662,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
       <c r="B26">
         <v>8428</v>
       </c>
@@ -669,7 +672,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
       <c r="B27">
         <v>2361</v>
       </c>
@@ -679,7 +682,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
       <c r="B28">
         <v>5063</v>
       </c>
@@ -689,7 +692,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2"/>
       <c r="B29">
         <v>7711</v>
       </c>
@@ -699,7 +702,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
       <c r="B30">
         <v>8833</v>
       </c>
@@ -709,7 +712,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
       <c r="B31">
         <v>1262</v>
       </c>
@@ -719,7 +722,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
       <c r="B32">
         <v>9020</v>
       </c>
@@ -729,7 +732,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2"/>
       <c r="B33">
         <v>1934</v>
       </c>
@@ -739,7 +742,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1"/>
+      <c r="A34" s="2"/>
       <c r="B34">
         <v>7237</v>
       </c>
@@ -749,7 +752,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1"/>
+      <c r="A35" s="2"/>
       <c r="B35">
         <v>3943</v>
       </c>
@@ -759,7 +762,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="2"/>
       <c r="B36">
         <v>7619</v>
       </c>
@@ -769,7 +772,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1"/>
+      <c r="A37" s="2"/>
       <c r="B37">
         <v>3832</v>
       </c>
@@ -779,7 +782,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2"/>
       <c r="B38">
         <v>1346</v>
       </c>
@@ -789,7 +792,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1"/>
+      <c r="A39" s="2"/>
       <c r="B39">
         <v>9622</v>
       </c>
@@ -799,7 +802,7 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1"/>
+      <c r="A40" s="2"/>
       <c r="B40">
         <v>8873</v>
       </c>
@@ -809,7 +812,7 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2"/>
       <c r="B41">
         <v>7799</v>
       </c>
@@ -819,7 +822,7 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2"/>
       <c r="B42">
         <v>9354</v>
       </c>
@@ -829,7 +832,7 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1"/>
+      <c r="A43" s="2"/>
       <c r="B43">
         <v>9130</v>
       </c>
@@ -839,7 +842,7 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="1"/>
+      <c r="A44" s="2"/>
       <c r="B44">
         <v>5895</v>
       </c>
@@ -849,7 +852,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="1"/>
+      <c r="A45" s="2"/>
       <c r="B45">
         <v>2461</v>
       </c>
@@ -859,7 +862,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="1"/>
+      <c r="A46" s="2"/>
       <c r="B46">
         <v>2790</v>
       </c>
@@ -869,7 +872,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1"/>
+      <c r="A47" s="2"/>
       <c r="B47">
         <v>2624</v>
       </c>
@@ -879,7 +882,7 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="2"/>
       <c r="B48">
         <v>5871</v>
       </c>
@@ -889,7 +892,7 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="1"/>
+      <c r="A49" s="2"/>
       <c r="B49">
         <v>9164</v>
       </c>
@@ -899,7 +902,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1"/>
+      <c r="A50" s="2"/>
       <c r="B50">
         <v>7457</v>
       </c>
@@ -909,7 +912,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1"/>
+      <c r="A51" s="2"/>
       <c r="B51">
         <v>9865</v>
       </c>
@@ -919,7 +922,7 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="2"/>
       <c r="B52">
         <v>3591</v>
       </c>
@@ -929,7 +932,7 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="1"/>
+      <c r="A53" s="2"/>
       <c r="B53">
         <v>3558</v>
       </c>
@@ -939,7 +942,7 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="1"/>
+      <c r="A54" s="2"/>
       <c r="B54">
         <v>4366</v>
       </c>
@@ -949,7 +952,7 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="1"/>
+      <c r="A55" s="2"/>
       <c r="B55">
         <v>5789</v>
       </c>
@@ -959,7 +962,7 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="1"/>
+      <c r="A56" s="2"/>
       <c r="B56">
         <v>6522</v>
       </c>
@@ -969,7 +972,7 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B57">
@@ -981,7 +984,7 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="1"/>
+      <c r="A58" s="2"/>
       <c r="B58">
         <v>1288</v>
       </c>
@@ -991,7 +994,7 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="1"/>
+      <c r="A59" s="2"/>
       <c r="B59">
         <v>2614</v>
       </c>
@@ -1001,7 +1004,7 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="1"/>
+      <c r="A60" s="2"/>
       <c r="B60">
         <v>7170</v>
       </c>
@@ -1011,7 +1014,7 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="1"/>
+      <c r="A61" s="2"/>
       <c r="B61">
         <v>2709</v>
       </c>
@@ -1021,7 +1024,7 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="1"/>
+      <c r="A62" s="2"/>
       <c r="B62">
         <v>3402</v>
       </c>
@@ -1031,7 +1034,7 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="1"/>
+      <c r="A63" s="2"/>
       <c r="B63">
         <v>8781</v>
       </c>
@@ -1041,7 +1044,7 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="1"/>
+      <c r="A64" s="2"/>
       <c r="B64">
         <v>8771</v>
       </c>
@@ -1051,7 +1054,7 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="1"/>
+      <c r="A65" s="2"/>
       <c r="B65">
         <v>3091</v>
       </c>
@@ -1061,7 +1064,7 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1"/>
+      <c r="A66" s="2"/>
       <c r="B66">
         <v>2195</v>
       </c>
@@ -1071,7 +1074,7 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1"/>
+      <c r="A67" s="2"/>
       <c r="B67">
         <v>1184</v>
       </c>
@@ -1081,7 +1084,7 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="1"/>
+      <c r="A68" s="2"/>
       <c r="B68">
         <v>2667</v>
       </c>
@@ -1091,7 +1094,7 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="1"/>
+      <c r="A69" s="2"/>
       <c r="B69">
         <v>5917</v>
       </c>
@@ -1101,7 +1104,7 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="1"/>
+      <c r="A70" s="2"/>
       <c r="B70">
         <v>3929</v>
       </c>
@@ -1111,7 +1114,7 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="1"/>
+      <c r="A71" s="2"/>
       <c r="B71">
         <v>3083</v>
       </c>
@@ -1121,7 +1124,7 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1"/>
+      <c r="A72" s="2"/>
       <c r="B72">
         <v>7546</v>
       </c>
@@ -1131,7 +1134,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B73">
@@ -1143,7 +1146,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="1"/>
+      <c r="A74" s="2"/>
       <c r="B74">
         <v>6598</v>
       </c>
@@ -1153,7 +1156,7 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="1"/>
+      <c r="A75" s="2"/>
       <c r="B75">
         <v>3093</v>
       </c>
@@ -1163,7 +1166,7 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="1"/>
+      <c r="A76" s="2"/>
       <c r="B76">
         <v>8805</v>
       </c>
@@ -1173,7 +1176,7 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="1"/>
+      <c r="A77" s="2"/>
       <c r="B77">
         <v>8158</v>
       </c>
@@ -1183,7 +1186,7 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="1"/>
+      <c r="A78" s="2"/>
       <c r="B78">
         <v>6499</v>
       </c>
@@ -1193,7 +1196,7 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B79">
@@ -1205,7 +1208,7 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="1"/>
+      <c r="A80" s="2"/>
       <c r="B80">
         <v>2217</v>
       </c>
@@ -1215,7 +1218,7 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="1"/>
+      <c r="A81" s="2"/>
       <c r="B81">
         <v>1824</v>
       </c>
@@ -1225,7 +1228,7 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="1"/>
+      <c r="A82" s="2"/>
       <c r="B82">
         <v>2564</v>
       </c>
@@ -1235,7 +1238,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="1"/>
+      <c r="A83" s="2"/>
       <c r="B83">
         <v>8487</v>
       </c>
@@ -1245,7 +1248,7 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="1"/>
+      <c r="A84" s="2"/>
       <c r="B84">
         <v>8045</v>
       </c>
@@ -1255,7 +1258,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="1"/>
+      <c r="A85" s="2"/>
       <c r="B85">
         <v>8878</v>
       </c>
@@ -1265,7 +1268,7 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="1"/>
+      <c r="A86" s="2"/>
       <c r="B86">
         <v>3072</v>
       </c>
@@ -1275,7 +1278,7 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="1"/>
+      <c r="A87" s="2"/>
       <c r="B87">
         <v>5980</v>
       </c>
@@ -1285,7 +1288,7 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1"/>
+      <c r="A88" s="2"/>
       <c r="B88">
         <v>8174</v>
       </c>
@@ -1295,7 +1298,7 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="1"/>
+      <c r="A89" s="2"/>
       <c r="B89">
         <v>4257</v>
       </c>
@@ -1305,7 +1308,7 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="1"/>
+      <c r="A90" s="2"/>
       <c r="B90">
         <v>2291</v>
       </c>
@@ -1315,7 +1318,7 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="1"/>
+      <c r="A91" s="2"/>
       <c r="B91">
         <v>1763</v>
       </c>
@@ -1325,7 +1328,7 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="1"/>
+      <c r="A92" s="2"/>
       <c r="B92">
         <v>5662</v>
       </c>
@@ -1335,7 +1338,7 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="1"/>
+      <c r="A93" s="2"/>
       <c r="B93">
         <v>1945</v>
       </c>
@@ -1345,7 +1348,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="1"/>
+      <c r="A94" s="2"/>
       <c r="B94">
         <v>1186</v>
       </c>
@@ -1355,7 +1358,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="1"/>
+      <c r="A95" s="2"/>
       <c r="B95">
         <v>8715</v>
       </c>
@@ -1365,7 +1368,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="1"/>
+      <c r="A96" s="2"/>
       <c r="B96">
         <v>8518</v>
       </c>
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="1"/>
+      <c r="A97" s="2"/>
       <c r="B97">
         <v>4847</v>
       </c>
@@ -1385,17 +1388,17 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="1"/>
+      <c r="A98" s="2"/>
       <c r="B98">
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C161" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C162" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="1"/>
+      <c r="A99" s="2"/>
       <c r="B99">
         <v>6291</v>
       </c>
@@ -1405,7 +1408,7 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="1"/>
+      <c r="A100" s="2"/>
       <c r="B100">
         <v>3770</v>
       </c>
@@ -1415,7 +1418,7 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="1"/>
+      <c r="A101" s="2"/>
       <c r="B101">
         <v>7178</v>
       </c>
@@ -1425,7 +1428,7 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="1"/>
+      <c r="A102" s="2"/>
       <c r="B102">
         <v>3883</v>
       </c>
@@ -1435,7 +1438,7 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="1"/>
+      <c r="A103" s="2"/>
       <c r="B103">
         <v>4527</v>
       </c>
@@ -1445,17 +1448,17 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="1"/>
+      <c r="A104" s="2"/>
       <c r="B104">
         <v>6556</v>
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="1"/>
+      <c r="A105" s="2"/>
       <c r="B105">
         <v>5635</v>
       </c>
@@ -1465,7 +1468,7 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="1"/>
+      <c r="A106" s="2"/>
       <c r="B106">
         <v>3878</v>
       </c>
@@ -1475,7 +1478,7 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="1"/>
+      <c r="A107" s="2"/>
       <c r="B107">
         <v>1217</v>
       </c>
@@ -1485,7 +1488,7 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="1"/>
+      <c r="A108" s="2"/>
       <c r="B108">
         <v>1438</v>
       </c>
@@ -1495,7 +1498,7 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="1"/>
+      <c r="A109" s="2"/>
       <c r="B109">
         <v>2153</v>
       </c>
@@ -1505,7 +1508,7 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="1"/>
+      <c r="A110" s="2"/>
       <c r="B110">
         <v>7937</v>
       </c>
@@ -1515,7 +1518,7 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="1"/>
+      <c r="A111" s="2"/>
       <c r="B111">
         <v>1999</v>
       </c>
@@ -1525,7 +1528,7 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="1"/>
+      <c r="A112" s="2"/>
       <c r="B112">
         <v>4042</v>
       </c>
@@ -1535,7 +1538,7 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="1"/>
+      <c r="A113" s="2"/>
       <c r="B113">
         <v>6351</v>
       </c>
@@ -1545,7 +1548,7 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="1"/>
+      <c r="A114" s="2"/>
       <c r="B114">
         <v>5382</v>
       </c>
@@ -1555,7 +1558,7 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="1"/>
+      <c r="A115" s="2"/>
       <c r="B115">
         <v>7088</v>
       </c>
@@ -1565,7 +1568,7 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="1"/>
+      <c r="A116" s="2"/>
       <c r="B116">
         <v>7250</v>
       </c>
@@ -1575,7 +1578,7 @@
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="1"/>
+      <c r="A117" s="2"/>
       <c r="B117">
         <v>6740</v>
       </c>
@@ -1585,7 +1588,7 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="1"/>
+      <c r="A118" s="2"/>
       <c r="B118">
         <v>9038</v>
       </c>
@@ -1595,7 +1598,7 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B119">
@@ -1607,7 +1610,7 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="1"/>
+      <c r="A120" s="2"/>
       <c r="B120">
         <v>8495</v>
       </c>
@@ -1617,7 +1620,7 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="1"/>
+      <c r="A121" s="2"/>
       <c r="B121">
         <v>1315</v>
       </c>
@@ -1627,7 +1630,7 @@
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="1"/>
+      <c r="A122" s="2"/>
       <c r="B122">
         <v>6066</v>
       </c>
@@ -1637,7 +1640,7 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="1"/>
+      <c r="A123" s="2"/>
       <c r="B123">
         <v>2565</v>
       </c>
@@ -1647,7 +1650,7 @@
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="1"/>
+      <c r="A124" s="2"/>
       <c r="B124">
         <v>2594</v>
       </c>
@@ -1657,7 +1660,7 @@
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="1"/>
+      <c r="A125" s="2"/>
       <c r="B125">
         <v>3762</v>
       </c>
@@ -1667,7 +1670,7 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="1"/>
+      <c r="A126" s="2"/>
       <c r="B126">
         <v>3550</v>
       </c>
@@ -1677,7 +1680,7 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="1"/>
+      <c r="A127" s="2"/>
       <c r="B127">
         <v>2475</v>
       </c>
@@ -1687,7 +1690,7 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="1"/>
+      <c r="A128" s="2"/>
       <c r="B128">
         <v>9180</v>
       </c>
@@ -1697,7 +1700,7 @@
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="1"/>
+      <c r="A129" s="2"/>
       <c r="B129">
         <v>1544</v>
       </c>
@@ -1707,7 +1710,7 @@
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="1"/>
+      <c r="A130" s="2"/>
       <c r="B130">
         <v>9562</v>
       </c>
@@ -1717,7 +1720,7 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="1"/>
+      <c r="A131" s="2"/>
       <c r="B131">
         <v>3669</v>
       </c>
@@ -1727,7 +1730,7 @@
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="1"/>
+      <c r="A132" s="2"/>
       <c r="B132">
         <v>5951</v>
       </c>
@@ -1737,7 +1740,7 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="1"/>
+      <c r="A133" s="2"/>
       <c r="B133">
         <v>2802</v>
       </c>
@@ -1747,7 +1750,7 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="1"/>
+      <c r="A134" s="2"/>
       <c r="B134">
         <v>6580</v>
       </c>
@@ -1757,7 +1760,7 @@
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="1"/>
+      <c r="A135" s="2"/>
       <c r="B135">
         <v>7585</v>
       </c>
@@ -1767,7 +1770,7 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="1"/>
+      <c r="A136" s="2"/>
       <c r="B136">
         <v>8770</v>
       </c>
@@ -1777,7 +1780,7 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="1"/>
+      <c r="A137" s="2"/>
       <c r="B137">
         <v>4236</v>
       </c>
@@ -1787,7 +1790,7 @@
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="1"/>
+      <c r="A138" s="2"/>
       <c r="B138">
         <v>5969</v>
       </c>
@@ -1797,7 +1800,7 @@
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="1"/>
+      <c r="A139" s="2"/>
       <c r="B139">
         <v>8696</v>
       </c>
@@ -1807,7 +1810,7 @@
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="1"/>
+      <c r="A140" s="2"/>
       <c r="B140">
         <v>8418</v>
       </c>
@@ -1817,7 +1820,7 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="1"/>
+      <c r="A141" s="2"/>
       <c r="B141">
         <v>8395</v>
       </c>
@@ -1827,9 +1830,9 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="1"/>
+      <c r="A142" s="2"/>
       <c r="B142">
-        <v>5568</v>
+        <v>5170</v>
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="3"/>
@@ -1837,9 +1840,9 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="1"/>
+      <c r="A143" s="2"/>
       <c r="B143">
-        <v>2592</v>
+        <v>5568</v>
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
@@ -1847,9 +1850,9 @@
       </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="1"/>
+      <c r="A144" s="2"/>
       <c r="B144">
-        <v>4075</v>
+        <v>2592</v>
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
@@ -1857,9 +1860,9 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="1"/>
+      <c r="A145" s="2"/>
       <c r="B145">
-        <v>7517</v>
+        <v>4075</v>
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
@@ -1867,9 +1870,9 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="1"/>
+      <c r="A146" s="2"/>
       <c r="B146">
-        <v>5448</v>
+        <v>7517</v>
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
@@ -1877,9 +1880,9 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="1"/>
+      <c r="A147" s="2"/>
       <c r="B147">
-        <v>6572</v>
+        <v>5448</v>
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
@@ -1887,9 +1890,9 @@
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="1"/>
+      <c r="A148" s="2"/>
       <c r="B148">
-        <v>5238</v>
+        <v>6572</v>
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
@@ -1897,9 +1900,9 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="1"/>
+      <c r="A149" s="2"/>
       <c r="B149">
-        <v>2084</v>
+        <v>5238</v>
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
@@ -1907,9 +1910,9 @@
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="1"/>
+      <c r="A150" s="2"/>
       <c r="B150">
-        <v>5411</v>
+        <v>2084</v>
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
@@ -1917,9 +1920,9 @@
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="1"/>
+      <c r="A151" s="2"/>
       <c r="B151">
-        <v>5171</v>
+        <v>5411</v>
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
@@ -1927,9 +1930,9 @@
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="1"/>
+      <c r="A152" s="2"/>
       <c r="B152">
-        <v>1862</v>
+        <v>5171</v>
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
@@ -1937,9 +1940,9 @@
       </c>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" s="1"/>
+      <c r="A153" s="2"/>
       <c r="B153">
-        <v>9238</v>
+        <v>1862</v>
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
@@ -1947,11 +1950,9 @@
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A154" s="2"/>
       <c r="B154">
-        <v>8165</v>
+        <v>9238</v>
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
@@ -1959,9 +1960,11 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="1"/>
+      <c r="A155" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B155">
-        <v>9001</v>
+        <v>8165</v>
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
@@ -1969,9 +1972,9 @@
       </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="1"/>
+      <c r="A156" s="2"/>
       <c r="B156">
-        <v>9631</v>
+        <v>9001</v>
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
@@ -1979,9 +1982,9 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1"/>
+      <c r="A157" s="2"/>
       <c r="B157">
-        <v>9812</v>
+        <v>9631</v>
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
@@ -1989,9 +1992,9 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="1"/>
+      <c r="A158" s="2"/>
       <c r="B158">
-        <v>5728</v>
+        <v>9812</v>
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
@@ -1999,9 +2002,9 @@
       </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="1"/>
+      <c r="A159" s="2"/>
       <c r="B159">
-        <v>7491</v>
+        <v>5728</v>
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
@@ -2009,9 +2012,9 @@
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="1"/>
+      <c r="A160" s="2"/>
       <c r="B160">
-        <v>5923</v>
+        <v>7491</v>
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
@@ -2019,9 +2022,9 @@
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="1"/>
+      <c r="A161" s="2"/>
       <c r="B161">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
@@ -2029,29 +2032,29 @@
       </c>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" s="1"/>
+      <c r="A162" s="2"/>
       <c r="B162">
+        <v>4265</v>
+      </c>
+      <c r="C162">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="2"/>
+      <c r="B163">
         <v>2166</v>
       </c>
-      <c r="C162">
-        <f t="shared" ref="C162:C226" ca="1" si="4">IF(B162=$E$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="1"/>
-      <c r="B163">
+      <c r="C163">
+        <f t="shared" ref="C163:C229" ca="1" si="4">IF(B163=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="2"/>
+      <c r="B164">
         <v>9116</v>
-      </c>
-      <c r="C163">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="1"/>
-      <c r="B164">
-        <v>9925</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="4"/>
@@ -2059,11 +2062,9 @@
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A165" s="2"/>
       <c r="B165">
-        <v>2885</v>
+        <v>9925</v>
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="4"/>
@@ -2071,9 +2072,11 @@
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="1"/>
+      <c r="A166" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B166">
-        <v>9931</v>
+        <v>2885</v>
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="4"/>
@@ -2081,9 +2084,9 @@
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="1"/>
+      <c r="A167" s="2"/>
       <c r="B167">
-        <v>1947</v>
+        <v>9931</v>
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="4"/>
@@ -2091,9 +2094,9 @@
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="1"/>
+      <c r="A168" s="2"/>
       <c r="B168">
-        <v>9696</v>
+        <v>1947</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
@@ -2101,9 +2104,9 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="1"/>
+      <c r="A169" s="2"/>
       <c r="B169">
-        <v>1223</v>
+        <v>9696</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
@@ -2111,9 +2114,9 @@
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="1"/>
+      <c r="A170" s="2"/>
       <c r="B170">
-        <v>3946</v>
+        <v>1223</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2121,9 +2124,9 @@
       </c>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" s="1"/>
+      <c r="A171" s="2"/>
       <c r="B171">
-        <v>8311</v>
+        <v>3946</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2131,9 +2134,9 @@
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="1"/>
+      <c r="A172" s="2"/>
       <c r="B172">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2141,9 +2144,9 @@
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" s="1"/>
+      <c r="A173" s="2"/>
       <c r="B173">
-        <v>9774</v>
+        <v>3134</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2151,9 +2154,9 @@
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="1"/>
+      <c r="A174" s="2"/>
       <c r="B174">
-        <v>9711</v>
+        <v>9774</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2161,9 +2164,9 @@
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="1"/>
+      <c r="A175" s="2"/>
       <c r="B175">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2171,9 +2174,9 @@
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="1"/>
+      <c r="A176" s="2"/>
       <c r="B176">
-        <v>7290</v>
+        <v>3333</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2181,9 +2184,9 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="1"/>
+      <c r="A177" s="2"/>
       <c r="B177">
-        <v>5694</v>
+        <v>7290</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2191,9 +2194,9 @@
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="1"/>
+      <c r="A178" s="2"/>
       <c r="B178">
-        <v>6806</v>
+        <v>5694</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2201,9 +2204,9 @@
       </c>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="1"/>
+      <c r="A179" s="2"/>
       <c r="B179">
-        <v>4515</v>
+        <v>6806</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2211,9 +2214,9 @@
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="1"/>
+      <c r="A180" s="2"/>
       <c r="B180">
-        <v>9271</v>
+        <v>4515</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2221,9 +2224,9 @@
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="1"/>
+      <c r="A181" s="2"/>
       <c r="B181">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2231,9 +2234,9 @@
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" s="1"/>
+      <c r="A182" s="2"/>
       <c r="B182">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2241,9 +2244,9 @@
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="1"/>
+      <c r="A183" s="2"/>
       <c r="B183">
-        <v>8820</v>
+        <v>4497</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2251,9 +2254,9 @@
       </c>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" s="1"/>
+      <c r="A184" s="2"/>
       <c r="B184">
-        <v>3218</v>
+        <v>8820</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2261,9 +2264,9 @@
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="1"/>
+      <c r="A185" s="2"/>
       <c r="B185">
-        <v>4283</v>
+        <v>3218</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2271,9 +2274,9 @@
       </c>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" s="1"/>
+      <c r="A186" s="2"/>
       <c r="B186">
-        <v>7703</v>
+        <v>4283</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2281,9 +2284,9 @@
       </c>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" s="1"/>
+      <c r="A187" s="2"/>
       <c r="B187">
-        <v>9182</v>
+        <v>7703</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2291,9 +2294,9 @@
       </c>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" s="1"/>
+      <c r="A188" s="2"/>
       <c r="B188">
-        <v>5541</v>
+        <v>9182</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2301,9 +2304,9 @@
       </c>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" s="1"/>
+      <c r="A189" s="2"/>
       <c r="B189">
-        <v>2386</v>
+        <v>5541</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2311,9 +2314,9 @@
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="1"/>
+      <c r="A190" s="2"/>
       <c r="B190">
-        <v>9159</v>
+        <v>2386</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2321,11 +2324,9 @@
       </c>
     </row>
     <row r="191" spans="1:3">
-      <c r="A191" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A191" s="2"/>
       <c r="B191">
-        <v>6175</v>
+        <v>9159</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2333,9 +2334,11 @@
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="1"/>
+      <c r="A192" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B192">
-        <v>4642</v>
+        <v>6175</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2343,9 +2346,9 @@
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="1"/>
+      <c r="A193" s="2"/>
       <c r="B193">
-        <v>9765</v>
+        <v>4642</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2353,9 +2356,9 @@
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="1"/>
+      <c r="A194" s="2"/>
       <c r="B194">
-        <v>4954</v>
+        <v>9765</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
@@ -2363,9 +2366,9 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="1"/>
+      <c r="A195" s="2"/>
       <c r="B195">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2373,9 +2376,9 @@
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="1"/>
+      <c r="A196" s="2"/>
       <c r="B196">
-        <v>6431</v>
+        <v>5537</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2383,9 +2386,9 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="1"/>
+      <c r="A197" s="2"/>
       <c r="B197">
-        <v>7193</v>
+        <v>6431</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2393,9 +2396,9 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="1"/>
+      <c r="A198" s="2"/>
       <c r="B198">
-        <v>5621</v>
+        <v>7193</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2403,9 +2406,9 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1"/>
+      <c r="A199" s="2"/>
       <c r="B199">
-        <v>5847</v>
+        <v>5621</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2413,9 +2416,9 @@
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="1"/>
+      <c r="A200" s="2"/>
       <c r="B200">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2423,9 +2426,9 @@
       </c>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="1"/>
+      <c r="A201" s="2"/>
       <c r="B201">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2433,9 +2436,9 @@
       </c>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="1"/>
+      <c r="A202" s="2"/>
       <c r="B202">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2443,9 +2446,9 @@
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="1"/>
+      <c r="A203" s="2"/>
       <c r="B203">
-        <v>2205</v>
+        <v>6861</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2453,9 +2456,9 @@
       </c>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="1"/>
+      <c r="A204" s="2"/>
       <c r="B204">
-        <v>4372</v>
+        <v>2205</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2463,9 +2466,9 @@
       </c>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="1"/>
+      <c r="A205" s="2"/>
       <c r="B205">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2473,9 +2476,9 @@
       </c>
     </row>
     <row r="206" spans="1:3">
-      <c r="A206" s="1"/>
+      <c r="A206" s="2"/>
       <c r="B206">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2483,9 +2486,9 @@
       </c>
     </row>
     <row r="207" spans="1:3">
-      <c r="A207" s="1"/>
+      <c r="A207" s="2"/>
       <c r="B207">
-        <v>2137</v>
+        <v>1668</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2493,11 +2496,9 @@
       </c>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A208" s="2"/>
       <c r="B208">
-        <v>9300</v>
+        <v>2137</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2505,9 +2506,11 @@
       </c>
     </row>
     <row r="209" spans="1:3">
-      <c r="A209" s="1"/>
+      <c r="A209" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B209">
-        <v>3951</v>
+        <v>9300</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2515,9 +2518,9 @@
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210" s="1"/>
+      <c r="A210" s="2"/>
       <c r="B210">
-        <v>6409</v>
+        <v>3951</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2525,9 +2528,9 @@
       </c>
     </row>
     <row r="211" spans="1:3">
-      <c r="A211" s="1"/>
+      <c r="A211" s="2"/>
       <c r="B211">
-        <v>7343</v>
+        <v>6409</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2535,9 +2538,9 @@
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="1"/>
+      <c r="A212" s="2"/>
       <c r="B212">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2545,11 +2548,9 @@
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A213" s="2"/>
       <c r="B213">
-        <v>9299</v>
+        <v>7060</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2557,9 +2558,11 @@
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="1"/>
+      <c r="A214" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B214">
-        <v>7560</v>
+        <v>9299</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2567,9 +2570,9 @@
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="1"/>
+      <c r="A215" s="2"/>
       <c r="B215">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2577,9 +2580,9 @@
       </c>
     </row>
     <row r="216" spans="1:3">
-      <c r="A216" s="1"/>
+      <c r="A216" s="2"/>
       <c r="B216">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2587,9 +2590,9 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="1"/>
+      <c r="A217" s="2"/>
       <c r="B217">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2597,9 +2600,9 @@
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="1"/>
+      <c r="A218" s="2"/>
       <c r="B218">
-        <v>2048</v>
+        <v>1954</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2607,11 +2610,9 @@
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A219" s="2"/>
       <c r="B219">
-        <v>3939</v>
+        <v>2048</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2619,9 +2620,11 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="1"/>
+      <c r="A220" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B220">
-        <v>8861</v>
+        <v>3939</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2629,9 +2632,9 @@
       </c>
     </row>
     <row r="221" spans="1:3">
-      <c r="A221" s="1"/>
+      <c r="A221" s="2"/>
       <c r="B221">
-        <v>1516</v>
+        <v>8861</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2639,51 +2642,51 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="1"/>
+      <c r="A222" s="2"/>
       <c r="B222">
+        <v>1516</v>
+      </c>
+      <c r="C222">
+        <f ca="1">IF(B222=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="2"/>
+      <c r="B223">
         <v>9062</v>
       </c>
-      <c r="C222">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B223">
-        <v>8403</v>
-      </c>
       <c r="C223">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B223=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3">
-      <c r="A224" s="1"/>
+      <c r="A224" s="2"/>
       <c r="B224">
-        <v>3185</v>
+        <v>5164</v>
       </c>
       <c r="C224">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B224=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>9914</v>
+        <v>2354</v>
       </c>
       <c r="C225">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B225=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="1"/>
+      <c r="A226" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B226">
-        <v>6011</v>
+        <v>8403</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2691,49 +2694,49 @@
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="1"/>
+      <c r="A227" s="2"/>
       <c r="B227">
+        <v>3185</v>
+      </c>
+      <c r="C227">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="2"/>
+      <c r="B228">
+        <v>9914</v>
+      </c>
+      <c r="C228">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="2"/>
+      <c r="B229">
+        <v>6011</v>
+      </c>
+      <c r="C229">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="2"/>
+      <c r="B230">
         <v>6037</v>
       </c>
-      <c r="C227">
-        <f t="shared" ref="C227:C290" ca="1" si="5">IF(B227=$E$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="1"/>
-      <c r="B228">
+      <c r="C230">
+        <f t="shared" ref="C230:C293" ca="1" si="5">IF(B230=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="2"/>
+      <c r="B231">
         <v>2809</v>
-      </c>
-      <c r="C228">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="1"/>
-      <c r="B229">
-        <v>7297</v>
-      </c>
-      <c r="C229">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" s="1"/>
-      <c r="B230">
-        <v>5242</v>
-      </c>
-      <c r="C230">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" s="1"/>
-      <c r="B231">
-        <v>1379</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="5"/>
@@ -2741,9 +2744,9 @@
       </c>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="1"/>
+      <c r="A232" s="2"/>
       <c r="B232">
-        <v>2401</v>
+        <v>7297</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="5"/>
@@ -2751,9 +2754,9 @@
       </c>
     </row>
     <row r="233" spans="1:3">
-      <c r="A233" s="1"/>
+      <c r="A233" s="2"/>
       <c r="B233">
-        <v>5421</v>
+        <v>5242</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="5"/>
@@ -2761,9 +2764,9 @@
       </c>
     </row>
     <row r="234" spans="1:3">
-      <c r="A234" s="1"/>
+      <c r="A234" s="2"/>
       <c r="B234">
-        <v>7301</v>
+        <v>1379</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="5"/>
@@ -2771,9 +2774,9 @@
       </c>
     </row>
     <row r="235" spans="1:3">
-      <c r="A235" s="1"/>
+      <c r="A235" s="2"/>
       <c r="B235">
-        <v>2000</v>
+        <v>2401</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="5"/>
@@ -2781,9 +2784,9 @@
       </c>
     </row>
     <row r="236" spans="1:3">
-      <c r="A236" s="1"/>
+      <c r="A236" s="2"/>
       <c r="B236">
-        <v>4147</v>
+        <v>5421</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2791,9 +2794,9 @@
       </c>
     </row>
     <row r="237" spans="1:3">
-      <c r="A237" s="1"/>
+      <c r="A237" s="2"/>
       <c r="B237">
-        <v>1953</v>
+        <v>7301</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2801,9 +2804,9 @@
       </c>
     </row>
     <row r="238" spans="1:3">
-      <c r="A238" s="1"/>
+      <c r="A238" s="2"/>
       <c r="B238">
-        <v>3956</v>
+        <v>2000</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2811,9 +2814,9 @@
       </c>
     </row>
     <row r="239" spans="1:3">
-      <c r="A239" s="1"/>
+      <c r="A239" s="2"/>
       <c r="B239">
-        <v>5463</v>
+        <v>4147</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2821,102 +2824,114 @@
       </c>
     </row>
     <row r="240" spans="1:3">
+      <c r="A240" s="2"/>
+      <c r="B240">
+        <v>1953</v>
+      </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="3:3">
+    <row r="241" spans="1:3">
+      <c r="A241" s="2"/>
+      <c r="B241">
+        <v>3956</v>
+      </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="3:3">
+    <row r="242" spans="1:3">
+      <c r="A242" s="2"/>
+      <c r="B242">
+        <v>5463</v>
+      </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="3:3">
+    <row r="243" spans="1:3">
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="3:3">
+    <row r="244" spans="1:3">
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="3:3">
+    <row r="245" spans="1:3">
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="3:3">
+    <row r="246" spans="1:3">
       <c r="C246">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="3:3">
+    <row r="247" spans="1:3">
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="3:3">
+    <row r="248" spans="1:3">
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="3:3">
+    <row r="249" spans="1:3">
       <c r="C249">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="3:3">
+    <row r="250" spans="1:3">
       <c r="C250">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="3:3">
+    <row r="251" spans="1:3">
       <c r="C251">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="3:3">
+    <row r="252" spans="1:3">
       <c r="C252">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="3:3">
+    <row r="253" spans="1:3">
       <c r="C253">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="3:3">
+    <row r="254" spans="1:3">
       <c r="C254">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="3:3">
+    <row r="255" spans="1:3">
       <c r="C255">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="3:3">
+    <row r="256" spans="1:3">
       <c r="C256">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3128,25 +3143,25 @@
     </row>
     <row r="291" spans="3:3">
       <c r="C291">
-        <f t="shared" ref="C291:C354" ca="1" si="6">IF(B291=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="292" spans="3:3">
       <c r="C292">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="293" spans="3:3">
       <c r="C293">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="294" spans="3:3">
       <c r="C294">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C294:C357" ca="1" si="6">IF(B294=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3512,25 +3527,25 @@
     </row>
     <row r="355" spans="3:3">
       <c r="C355">
-        <f t="shared" ref="C355:C418" ca="1" si="7">IF(B355=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="356" spans="3:3">
       <c r="C356">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="357" spans="3:3">
       <c r="C357">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="358" spans="3:3">
       <c r="C358">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C358:C421" ca="1" si="7">IF(B358=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3896,25 +3911,25 @@
     </row>
     <row r="419" spans="3:3">
       <c r="C419">
-        <f t="shared" ref="C419:C482" ca="1" si="8">IF(B419=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="420" spans="3:3">
       <c r="C420">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="421" spans="3:3">
       <c r="C421">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="422" spans="3:3">
       <c r="C422">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C422:C485" ca="1" si="8">IF(B422=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4280,25 +4295,25 @@
     </row>
     <row r="483" spans="3:3">
       <c r="C483">
-        <f t="shared" ref="C483:C546" ca="1" si="9">IF(B483=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="484" spans="3:3">
       <c r="C484">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="485" spans="3:3">
       <c r="C485">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="486" spans="3:3">
       <c r="C486">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C486:C549" ca="1" si="9">IF(B486=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4664,25 +4679,25 @@
     </row>
     <row r="547" spans="3:3">
       <c r="C547">
-        <f t="shared" ref="C547:C610" ca="1" si="10">IF(B547=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="548" spans="3:3">
       <c r="C548">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="3:3">
       <c r="C549">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="550" spans="3:3">
       <c r="C550">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C550:C613" ca="1" si="10">IF(B550=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5048,25 +5063,25 @@
     </row>
     <row r="611" spans="3:3">
       <c r="C611">
-        <f t="shared" ref="C611:C674" ca="1" si="11">IF(B611=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="612" spans="3:3">
       <c r="C612">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="613" spans="3:3">
       <c r="C613">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="614" spans="3:3">
       <c r="C614">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C614:C677" ca="1" si="11">IF(B614=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5432,25 +5447,25 @@
     </row>
     <row r="675" spans="3:3">
       <c r="C675">
-        <f t="shared" ref="C675:C738" ca="1" si="12">IF(B675=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="3:3">
       <c r="C676">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="3:3">
       <c r="C677">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="3:3">
       <c r="C678">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C678:C741" ca="1" si="12">IF(B678=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5816,25 +5831,25 @@
     </row>
     <row r="739" spans="3:3">
       <c r="C739">
-        <f t="shared" ref="C739:C802" ca="1" si="13">IF(B739=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="3:3">
       <c r="C740">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="3:3">
       <c r="C741">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="3:3">
       <c r="C742">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C742:C805" ca="1" si="13">IF(B742=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6200,25 +6215,25 @@
     </row>
     <row r="803" spans="3:3">
       <c r="C803">
-        <f t="shared" ref="C803:C866" ca="1" si="14">IF(B803=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="804" spans="3:3">
       <c r="C804">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="3:3">
       <c r="C805">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="806" spans="3:3">
       <c r="C806">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C806:C869" ca="1" si="14">IF(B806=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6584,25 +6599,25 @@
     </row>
     <row r="867" spans="3:3">
       <c r="C867">
-        <f t="shared" ref="C867:C881" ca="1" si="15">IF(B867=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="868" spans="3:3">
       <c r="C868">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="869" spans="3:3">
       <c r="C869">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="870" spans="3:3">
       <c r="C870">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C870:C884" ca="1" si="15">IF(B870=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6672,21 +6687,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="882" spans="3:3">
+      <c r="C882">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="883" spans="3:3">
+      <c r="C883">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="884" spans="3:3">
+      <c r="C884">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A213:A218"/>
-    <mergeCell ref="A219:A222"/>
-    <mergeCell ref="A223:A239"/>
+    <mergeCell ref="A214:A219"/>
+    <mergeCell ref="A220:A224"/>
+    <mergeCell ref="A226:A242"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A208:A212"/>
-    <mergeCell ref="A191:A207"/>
-    <mergeCell ref="A165:A190"/>
-    <mergeCell ref="A154:A164"/>
-    <mergeCell ref="A119:A153"/>
+    <mergeCell ref="A209:A213"/>
+    <mergeCell ref="A192:A208"/>
+    <mergeCell ref="A166:A191"/>
+    <mergeCell ref="A155:A165"/>
+    <mergeCell ref="A119:A154"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improve lab06. remove some test for errors
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -400,11 +400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E885"/>
+  <dimension ref="A1:E887"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E170" sqref="E170"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>8085</v>
+        <v>5622</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C162" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C164" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136">
-        <v>8770</v>
+        <v>2321</v>
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="3"/>
@@ -1784,7 +1784,7 @@
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137">
-        <v>4236</v>
+        <v>5053</v>
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="3"/>
@@ -1794,7 +1794,7 @@
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138">
-        <v>5969</v>
+        <v>8770</v>
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="3"/>
@@ -1804,7 +1804,7 @@
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139">
-        <v>8696</v>
+        <v>4236</v>
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="3"/>
@@ -1814,7 +1814,7 @@
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140">
-        <v>8418</v>
+        <v>5969</v>
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="3"/>
@@ -1824,7 +1824,7 @@
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141">
-        <v>8395</v>
+        <v>8696</v>
       </c>
       <c r="C141">
         <f t="shared" ca="1" si="3"/>
@@ -1834,7 +1834,7 @@
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142">
-        <v>5170</v>
+        <v>8418</v>
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="3"/>
@@ -1844,7 +1844,7 @@
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143">
-        <v>5568</v>
+        <v>8395</v>
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
@@ -1854,7 +1854,7 @@
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144">
-        <v>2592</v>
+        <v>5170</v>
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
@@ -1864,7 +1864,7 @@
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145">
-        <v>4075</v>
+        <v>5568</v>
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
@@ -1874,7 +1874,7 @@
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146">
-        <v>7517</v>
+        <v>2592</v>
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
@@ -1884,7 +1884,7 @@
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147">
-        <v>5448</v>
+        <v>4075</v>
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
@@ -1894,7 +1894,7 @@
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148">
-        <v>6572</v>
+        <v>7517</v>
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
@@ -1904,7 +1904,7 @@
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149">
-        <v>5238</v>
+        <v>5448</v>
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
@@ -1914,7 +1914,7 @@
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150">
-        <v>2084</v>
+        <v>6572</v>
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
@@ -1924,7 +1924,7 @@
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151">
-        <v>5411</v>
+        <v>5238</v>
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
@@ -1934,7 +1934,7 @@
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152">
-        <v>5171</v>
+        <v>2084</v>
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
@@ -1944,7 +1944,7 @@
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153">
-        <v>1862</v>
+        <v>5411</v>
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
@@ -1954,7 +1954,7 @@
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154">
-        <v>9238</v>
+        <v>5171</v>
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
@@ -1962,11 +1962,9 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A155" s="2"/>
       <c r="B155">
-        <v>8165</v>
+        <v>1862</v>
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
@@ -1976,7 +1974,7 @@
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156">
-        <v>9001</v>
+        <v>9238</v>
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
@@ -1984,9 +1982,11 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="2"/>
+      <c r="A157" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B157">
-        <v>9631</v>
+        <v>8165</v>
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
@@ -1996,7 +1996,7 @@
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158">
-        <v>9812</v>
+        <v>9001</v>
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
@@ -2006,7 +2006,7 @@
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159">
-        <v>5728</v>
+        <v>9631</v>
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
@@ -2016,7 +2016,7 @@
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160">
-        <v>7491</v>
+        <v>9812</v>
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
@@ -2026,7 +2026,7 @@
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161">
-        <v>5923</v>
+        <v>5728</v>
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
@@ -2036,7 +2036,7 @@
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162">
-        <v>4265</v>
+        <v>7491</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
@@ -2046,39 +2046,37 @@
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163">
-        <v>2166</v>
+        <v>5923</v>
       </c>
       <c r="C163">
-        <f t="shared" ref="C163:C230" ca="1" si="4">IF(B163=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164">
-        <v>9116</v>
+        <v>4265</v>
       </c>
       <c r="C164">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165">
-        <v>9925</v>
+        <v>2166</v>
       </c>
       <c r="C165">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="C165:C232" ca="1" si="4">IF(B165=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A166" s="2"/>
       <c r="B166">
-        <v>2885</v>
+        <v>9116</v>
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="4"/>
@@ -2088,7 +2086,7 @@
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167">
-        <v>9931</v>
+        <v>9925</v>
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="4"/>
@@ -2096,9 +2094,11 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="2"/>
+      <c r="A168" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B168">
-        <v>1947</v>
+        <v>2885</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
@@ -2108,7 +2108,7 @@
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169">
-        <v>9696</v>
+        <v>9931</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
@@ -2118,7 +2118,7 @@
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170">
-        <v>1223</v>
+        <v>1947</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2128,7 +2128,7 @@
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171">
-        <v>3946</v>
+        <v>9696</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2138,7 +2138,7 @@
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172">
-        <v>8311</v>
+        <v>1223</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2148,7 +2148,7 @@
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173">
-        <v>3134</v>
+        <v>3946</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2158,7 +2158,7 @@
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174">
-        <v>9774</v>
+        <v>8311</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2168,7 +2168,7 @@
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175">
-        <v>9711</v>
+        <v>3134</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2178,7 +2178,7 @@
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176">
-        <v>3333</v>
+        <v>9774</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2188,7 +2188,7 @@
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177">
-        <v>7290</v>
+        <v>9711</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2198,7 +2198,7 @@
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178">
-        <v>5694</v>
+        <v>3333</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2208,7 +2208,7 @@
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179">
-        <v>6806</v>
+        <v>7290</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2218,7 +2218,7 @@
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180">
-        <v>4515</v>
+        <v>5694</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2228,7 +2228,7 @@
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181">
-        <v>9271</v>
+        <v>6806</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2238,7 +2238,7 @@
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182">
-        <v>8769</v>
+        <v>4515</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2248,7 +2248,7 @@
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183">
-        <v>4497</v>
+        <v>9271</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2258,7 +2258,7 @@
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184">
-        <v>3940</v>
+        <v>8769</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2268,7 +2268,7 @@
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185">
-        <v>8820</v>
+        <v>4497</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2278,7 +2278,7 @@
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186">
-        <v>3218</v>
+        <v>3940</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2288,7 +2288,7 @@
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187">
-        <v>4283</v>
+        <v>8820</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2298,7 +2298,7 @@
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188">
-        <v>7703</v>
+        <v>3218</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2308,7 +2308,7 @@
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189">
-        <v>9182</v>
+        <v>4283</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2318,7 +2318,7 @@
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190">
-        <v>5541</v>
+        <v>7703</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2328,7 +2328,7 @@
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191">
-        <v>2386</v>
+        <v>9182</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2338,7 +2338,7 @@
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192">
-        <v>9159</v>
+        <v>5541</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2346,11 +2346,9 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A193" s="2"/>
       <c r="B193">
-        <v>6175</v>
+        <v>2386</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2360,7 +2358,7 @@
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194">
-        <v>4642</v>
+        <v>9159</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
@@ -2368,9 +2366,11 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="2"/>
+      <c r="A195" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B195">
-        <v>9765</v>
+        <v>6175</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2380,7 +2380,7 @@
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196">
-        <v>4954</v>
+        <v>4642</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2390,7 +2390,7 @@
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197">
-        <v>5537</v>
+        <v>9765</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2400,7 +2400,7 @@
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198">
-        <v>6431</v>
+        <v>4954</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2410,7 +2410,7 @@
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199">
-        <v>7193</v>
+        <v>5537</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2420,7 +2420,7 @@
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200">
-        <v>5621</v>
+        <v>6431</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2430,7 +2430,7 @@
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201">
-        <v>5847</v>
+        <v>7193</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2440,7 +2440,7 @@
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202">
-        <v>4769</v>
+        <v>5621</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2450,7 +2450,7 @@
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203">
-        <v>9930</v>
+        <v>5847</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2460,7 +2460,7 @@
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204">
-        <v>6861</v>
+        <v>4769</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2470,7 +2470,7 @@
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205">
-        <v>2205</v>
+        <v>9930</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2480,7 +2480,7 @@
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206">
-        <v>4372</v>
+        <v>6861</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2490,7 +2490,7 @@
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207">
-        <v>4463</v>
+        <v>2205</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2500,7 +2500,7 @@
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208">
-        <v>1668</v>
+        <v>4372</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2510,7 +2510,7 @@
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209">
-        <v>2137</v>
+        <v>4463</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2518,11 +2518,9 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A210" s="2"/>
       <c r="B210">
-        <v>9300</v>
+        <v>1668</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2532,7 +2530,7 @@
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211">
-        <v>3951</v>
+        <v>2137</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2540,9 +2538,11 @@
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="2"/>
+      <c r="A212" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B212">
-        <v>6409</v>
+        <v>9300</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2552,7 +2552,7 @@
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2562,7 +2562,7 @@
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214">
-        <v>7060</v>
+        <v>6409</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2570,11 +2570,9 @@
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A215" s="2"/>
       <c r="B215">
-        <v>9299</v>
+        <v>7343</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2584,7 +2582,7 @@
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216">
-        <v>7560</v>
+        <v>7060</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2592,9 +2590,11 @@
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="2"/>
+      <c r="A217" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B217">
-        <v>9002</v>
+        <v>9299</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2604,7 +2604,7 @@
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2614,7 +2614,7 @@
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2624,7 +2624,7 @@
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220">
-        <v>2048</v>
+        <v>7432</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2632,11 +2632,9 @@
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A221" s="2"/>
       <c r="B221">
-        <v>3939</v>
+        <v>1954</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2646,7 +2644,7 @@
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222">
-        <v>8861</v>
+        <v>2048</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2654,29 +2652,31 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="2"/>
+      <c r="A223" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B223">
-        <v>1516</v>
+        <v>3939</v>
       </c>
       <c r="C223">
-        <f ca="1">IF(B223=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224">
-        <v>9062</v>
+        <v>8861</v>
       </c>
       <c r="C224">
-        <f ca="1">IF(B224=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225">
-        <v>5164</v>
+        <v>1516</v>
       </c>
       <c r="C225">
         <f ca="1">IF(B225=$E$1,1,0)</f>
@@ -2684,9 +2684,9 @@
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="1"/>
+      <c r="A226" s="2"/>
       <c r="B226">
-        <v>2354</v>
+        <v>9062</v>
       </c>
       <c r="C226">
         <f ca="1">IF(B226=$E$1,1,0)</f>
@@ -2694,31 +2694,31 @@
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+      <c r="A227" s="2"/>
+      <c r="B227">
+        <v>5164</v>
+      </c>
+      <c r="C227">
+        <f ca="1">IF(B227=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1"/>
+      <c r="B228">
+        <v>2354</v>
+      </c>
+      <c r="C228">
+        <f ca="1">IF(B228=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B227">
+      <c r="B229">
         <v>8403</v>
-      </c>
-      <c r="C227">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="2"/>
-      <c r="B228">
-        <v>3185</v>
-      </c>
-      <c r="C228">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="2"/>
-      <c r="B229">
-        <v>9914</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="4"/>
@@ -2728,7 +2728,7 @@
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="4"/>
@@ -2738,37 +2738,37 @@
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231">
-        <v>6037</v>
+        <v>9914</v>
       </c>
       <c r="C231">
-        <f t="shared" ref="C231:C294" ca="1" si="5">IF(B231=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232">
-        <v>2809</v>
+        <v>6011</v>
       </c>
       <c r="C232">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233">
-        <v>7297</v>
+        <v>6037</v>
       </c>
       <c r="C233">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C233:C296" ca="1" si="5">IF(B233=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234">
-        <v>5242</v>
+        <v>2809</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="5"/>
@@ -2778,7 +2778,7 @@
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="5"/>
@@ -2788,7 +2788,7 @@
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2798,7 +2798,7 @@
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2808,7 +2808,7 @@
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2818,7 +2818,7 @@
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2828,7 +2828,7 @@
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2838,7 +2838,7 @@
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2848,7 +2848,7 @@
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2858,7 +2858,7 @@
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243">
-        <v>5463</v>
+        <v>1953</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2866,12 +2866,20 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="2"/>
+      <c r="B244">
+        <v>3956</v>
+      </c>
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="2"/>
+      <c r="B245">
+        <v>5463</v>
+      </c>
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3173,19 +3181,19 @@
     </row>
     <row r="295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C295">
-        <f t="shared" ref="C295:C358" ca="1" si="6">IF(B295=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="296" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C296">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="297" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C297">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C297:C360" ca="1" si="6">IF(B297=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3557,19 +3565,19 @@
     </row>
     <row r="359" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C359">
-        <f t="shared" ref="C359:C422" ca="1" si="7">IF(B359=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="360" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C360">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="361" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C361">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C361:C424" ca="1" si="7">IF(B361=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3941,19 +3949,19 @@
     </row>
     <row r="423" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C423">
-        <f t="shared" ref="C423:C486" ca="1" si="8">IF(B423=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="424" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C424">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="425" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C425">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C425:C488" ca="1" si="8">IF(B425=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4325,19 +4333,19 @@
     </row>
     <row r="487" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C487">
-        <f t="shared" ref="C487:C550" ca="1" si="9">IF(B487=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="488" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C488">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="489" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C489">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C489:C552" ca="1" si="9">IF(B489=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4709,19 +4717,19 @@
     </row>
     <row r="551" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C551">
-        <f t="shared" ref="C551:C614" ca="1" si="10">IF(B551=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="552" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C552">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="553" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C553">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C553:C616" ca="1" si="10">IF(B553=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5093,19 +5101,19 @@
     </row>
     <row r="615" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C615">
-        <f t="shared" ref="C615:C678" ca="1" si="11">IF(B615=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="616" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C616">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="617" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C617">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C617:C680" ca="1" si="11">IF(B617=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5477,19 +5485,19 @@
     </row>
     <row r="679" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C679">
-        <f t="shared" ref="C679:C742" ca="1" si="12">IF(B679=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C680">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C681">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C681:C744" ca="1" si="12">IF(B681=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5861,19 +5869,19 @@
     </row>
     <row r="743" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C743">
-        <f t="shared" ref="C743:C806" ca="1" si="13">IF(B743=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C744">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C745">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C745:C808" ca="1" si="13">IF(B745=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6245,19 +6253,19 @@
     </row>
     <row r="807" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C807">
-        <f t="shared" ref="C807:C870" ca="1" si="14">IF(B807=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="808" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C808">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="809" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C809">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C809:C872" ca="1" si="14">IF(B809=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6629,19 +6637,19 @@
     </row>
     <row r="871" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C871">
-        <f t="shared" ref="C871:C885" ca="1" si="15">IF(B871=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="872" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C872">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="873" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C873">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C873:C887" ca="1" si="15">IF(B873=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6717,21 +6725,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="886" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C886">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="887" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C887">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A215:A220"/>
-    <mergeCell ref="A221:A225"/>
-    <mergeCell ref="A227:A243"/>
+    <mergeCell ref="A217:A222"/>
+    <mergeCell ref="A223:A227"/>
+    <mergeCell ref="A229:A245"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A210:A214"/>
-    <mergeCell ref="A193:A209"/>
-    <mergeCell ref="A166:A192"/>
-    <mergeCell ref="A155:A165"/>
-    <mergeCell ref="A119:A154"/>
+    <mergeCell ref="A212:A216"/>
+    <mergeCell ref="A195:A211"/>
+    <mergeCell ref="A168:A194"/>
+    <mergeCell ref="A157:A167"/>
+    <mergeCell ref="A119:A156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
solve all tasks in lab08. add some tasks in lab08
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -398,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E887"/>
+  <dimension ref="A1:E889"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G154" sqref="G154"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>8086</v>
+        <v>5483</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2067,7 +2067,7 @@
         <v>2166</v>
       </c>
       <c r="C165">
-        <f t="shared" ref="C165:C232" ca="1" si="4">IF(B165=$E$1,1,0)</f>
+        <f t="shared" ref="C165:C234" ca="1" si="4">IF(B165=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
     <row r="170" spans="1:3">
       <c r="A170" s="2"/>
       <c r="B170">
-        <v>1947</v>
+        <v>4425</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2126,7 +2126,7 @@
     <row r="171" spans="1:3">
       <c r="A171" s="2"/>
       <c r="B171">
-        <v>9696</v>
+        <v>1947</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2136,7 +2136,7 @@
     <row r="172" spans="1:3">
       <c r="A172" s="2"/>
       <c r="B172">
-        <v>1223</v>
+        <v>9696</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2146,7 +2146,7 @@
     <row r="173" spans="1:3">
       <c r="A173" s="2"/>
       <c r="B173">
-        <v>3946</v>
+        <v>1223</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2156,7 +2156,7 @@
     <row r="174" spans="1:3">
       <c r="A174" s="2"/>
       <c r="B174">
-        <v>8311</v>
+        <v>3946</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2166,7 +2166,7 @@
     <row r="175" spans="1:3">
       <c r="A175" s="2"/>
       <c r="B175">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2176,7 +2176,7 @@
     <row r="176" spans="1:3">
       <c r="A176" s="2"/>
       <c r="B176">
-        <v>9774</v>
+        <v>3134</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2186,7 +2186,7 @@
     <row r="177" spans="1:3">
       <c r="A177" s="2"/>
       <c r="B177">
-        <v>9711</v>
+        <v>9774</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2196,7 +2196,7 @@
     <row r="178" spans="1:3">
       <c r="A178" s="2"/>
       <c r="B178">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2206,7 +2206,7 @@
     <row r="179" spans="1:3">
       <c r="A179" s="2"/>
       <c r="B179">
-        <v>7290</v>
+        <v>3333</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2216,7 +2216,7 @@
     <row r="180" spans="1:3">
       <c r="A180" s="2"/>
       <c r="B180">
-        <v>5694</v>
+        <v>7290</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2226,7 +2226,7 @@
     <row r="181" spans="1:3">
       <c r="A181" s="2"/>
       <c r="B181">
-        <v>6806</v>
+        <v>5694</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2236,7 +2236,7 @@
     <row r="182" spans="1:3">
       <c r="A182" s="2"/>
       <c r="B182">
-        <v>4515</v>
+        <v>7035</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2246,7 +2246,7 @@
     <row r="183" spans="1:3">
       <c r="A183" s="2"/>
       <c r="B183">
-        <v>9271</v>
+        <v>6806</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2256,7 +2256,7 @@
     <row r="184" spans="1:3">
       <c r="A184" s="2"/>
       <c r="B184">
-        <v>8769</v>
+        <v>4515</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2266,7 +2266,7 @@
     <row r="185" spans="1:3">
       <c r="A185" s="2"/>
       <c r="B185">
-        <v>4497</v>
+        <v>9271</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2276,7 +2276,7 @@
     <row r="186" spans="1:3">
       <c r="A186" s="2"/>
       <c r="B186">
-        <v>3940</v>
+        <v>8769</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2286,7 +2286,7 @@
     <row r="187" spans="1:3">
       <c r="A187" s="2"/>
       <c r="B187">
-        <v>8820</v>
+        <v>4497</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2296,7 +2296,7 @@
     <row r="188" spans="1:3">
       <c r="A188" s="2"/>
       <c r="B188">
-        <v>3218</v>
+        <v>3940</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2306,7 +2306,7 @@
     <row r="189" spans="1:3">
       <c r="A189" s="2"/>
       <c r="B189">
-        <v>4283</v>
+        <v>8820</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2316,7 +2316,7 @@
     <row r="190" spans="1:3">
       <c r="A190" s="2"/>
       <c r="B190">
-        <v>7703</v>
+        <v>3218</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2326,7 +2326,7 @@
     <row r="191" spans="1:3">
       <c r="A191" s="2"/>
       <c r="B191">
-        <v>9182</v>
+        <v>4283</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2336,7 +2336,7 @@
     <row r="192" spans="1:3">
       <c r="A192" s="2"/>
       <c r="B192">
-        <v>5541</v>
+        <v>7703</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2346,7 +2346,7 @@
     <row r="193" spans="1:3">
       <c r="A193" s="2"/>
       <c r="B193">
-        <v>2386</v>
+        <v>9182</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2356,7 +2356,7 @@
     <row r="194" spans="1:3">
       <c r="A194" s="2"/>
       <c r="B194">
-        <v>9159</v>
+        <v>5541</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
@@ -2364,11 +2364,9 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A195" s="2"/>
       <c r="B195">
-        <v>6175</v>
+        <v>2386</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2378,7 +2376,7 @@
     <row r="196" spans="1:3">
       <c r="A196" s="2"/>
       <c r="B196">
-        <v>4642</v>
+        <v>9159</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2386,9 +2384,11 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="2"/>
+      <c r="A197" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B197">
-        <v>9765</v>
+        <v>6175</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2398,7 +2398,7 @@
     <row r="198" spans="1:3">
       <c r="A198" s="2"/>
       <c r="B198">
-        <v>4954</v>
+        <v>4642</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2408,7 +2408,7 @@
     <row r="199" spans="1:3">
       <c r="A199" s="2"/>
       <c r="B199">
-        <v>5537</v>
+        <v>9765</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2418,7 +2418,7 @@
     <row r="200" spans="1:3">
       <c r="A200" s="2"/>
       <c r="B200">
-        <v>6431</v>
+        <v>4954</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2428,7 +2428,7 @@
     <row r="201" spans="1:3">
       <c r="A201" s="2"/>
       <c r="B201">
-        <v>7193</v>
+        <v>5537</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2438,7 +2438,7 @@
     <row r="202" spans="1:3">
       <c r="A202" s="2"/>
       <c r="B202">
-        <v>5621</v>
+        <v>6431</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2448,7 +2448,7 @@
     <row r="203" spans="1:3">
       <c r="A203" s="2"/>
       <c r="B203">
-        <v>5847</v>
+        <v>7193</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2458,7 +2458,7 @@
     <row r="204" spans="1:3">
       <c r="A204" s="2"/>
       <c r="B204">
-        <v>4769</v>
+        <v>5621</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2468,7 +2468,7 @@
     <row r="205" spans="1:3">
       <c r="A205" s="2"/>
       <c r="B205">
-        <v>9930</v>
+        <v>5847</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2478,7 +2478,7 @@
     <row r="206" spans="1:3">
       <c r="A206" s="2"/>
       <c r="B206">
-        <v>6861</v>
+        <v>4769</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2488,7 +2488,7 @@
     <row r="207" spans="1:3">
       <c r="A207" s="2"/>
       <c r="B207">
-        <v>2205</v>
+        <v>9930</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2498,7 +2498,7 @@
     <row r="208" spans="1:3">
       <c r="A208" s="2"/>
       <c r="B208">
-        <v>4372</v>
+        <v>6861</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2508,7 +2508,7 @@
     <row r="209" spans="1:3">
       <c r="A209" s="2"/>
       <c r="B209">
-        <v>4463</v>
+        <v>2205</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2518,7 +2518,7 @@
     <row r="210" spans="1:3">
       <c r="A210" s="2"/>
       <c r="B210">
-        <v>1668</v>
+        <v>4372</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2528,7 +2528,7 @@
     <row r="211" spans="1:3">
       <c r="A211" s="2"/>
       <c r="B211">
-        <v>2137</v>
+        <v>4463</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2536,11 +2536,9 @@
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A212" s="2"/>
       <c r="B212">
-        <v>9300</v>
+        <v>1668</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2550,7 +2548,7 @@
     <row r="213" spans="1:3">
       <c r="A213" s="2"/>
       <c r="B213">
-        <v>3951</v>
+        <v>2137</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2558,9 +2556,11 @@
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="2"/>
+      <c r="A214" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B214">
-        <v>6409</v>
+        <v>9300</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2570,7 +2570,7 @@
     <row r="215" spans="1:3">
       <c r="A215" s="2"/>
       <c r="B215">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2580,7 +2580,7 @@
     <row r="216" spans="1:3">
       <c r="A216" s="2"/>
       <c r="B216">
-        <v>7060</v>
+        <v>6409</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2588,11 +2588,9 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A217" s="2"/>
       <c r="B217">
-        <v>9299</v>
+        <v>7343</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2602,7 +2600,7 @@
     <row r="218" spans="1:3">
       <c r="A218" s="2"/>
       <c r="B218">
-        <v>7560</v>
+        <v>7060</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2610,9 +2608,11 @@
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="2"/>
+      <c r="A219" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B219">
-        <v>9002</v>
+        <v>9299</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2622,7 +2622,7 @@
     <row r="220" spans="1:3">
       <c r="A220" s="2"/>
       <c r="B220">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2632,7 +2632,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="2"/>
       <c r="B221">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2642,7 +2642,7 @@
     <row r="222" spans="1:3">
       <c r="A222" s="2"/>
       <c r="B222">
-        <v>2048</v>
+        <v>7432</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2650,11 +2650,9 @@
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A223" s="2"/>
       <c r="B223">
-        <v>3939</v>
+        <v>1954</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2664,7 +2662,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="2"/>
       <c r="B224">
-        <v>8861</v>
+        <v>2048</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2672,29 +2670,31 @@
       </c>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="2"/>
+      <c r="A225" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B225">
-        <v>1516</v>
+        <v>3939</v>
       </c>
       <c r="C225">
-        <f ca="1">IF(B225=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="2"/>
       <c r="B226">
-        <v>9062</v>
+        <v>8861</v>
       </c>
       <c r="C226">
-        <f ca="1">IF(B226=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="2"/>
       <c r="B227">
-        <v>5164</v>
+        <v>1516</v>
       </c>
       <c r="C227">
         <f ca="1">IF(B227=$E$1,1,0)</f>
@@ -2702,9 +2702,9 @@
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="1"/>
+      <c r="A228" s="2"/>
       <c r="B228">
-        <v>2354</v>
+        <v>9062</v>
       </c>
       <c r="C228">
         <f ca="1">IF(B228=$E$1,1,0)</f>
@@ -2712,31 +2712,31 @@
       </c>
     </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="2" t="s">
+      <c r="A229" s="2"/>
+      <c r="B229">
+        <v>5164</v>
+      </c>
+      <c r="C229">
+        <f ca="1">IF(B229=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="1"/>
+      <c r="B230">
+        <v>2354</v>
+      </c>
+      <c r="C230">
+        <f ca="1">IF(B230=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B229">
+      <c r="B231">
         <v>8403</v>
-      </c>
-      <c r="C229">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" s="2"/>
-      <c r="B230">
-        <v>3185</v>
-      </c>
-      <c r="C230">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" s="2"/>
-      <c r="B231">
-        <v>9914</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="4"/>
@@ -2746,7 +2746,7 @@
     <row r="232" spans="1:3">
       <c r="A232" s="2"/>
       <c r="B232">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="4"/>
@@ -2756,37 +2756,37 @@
     <row r="233" spans="1:3">
       <c r="A233" s="2"/>
       <c r="B233">
-        <v>6037</v>
+        <v>9914</v>
       </c>
       <c r="C233">
-        <f t="shared" ref="C233:C296" ca="1" si="5">IF(B233=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="2"/>
       <c r="B234">
-        <v>2809</v>
+        <v>6011</v>
       </c>
       <c r="C234">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="2"/>
       <c r="B235">
-        <v>7297</v>
+        <v>6037</v>
       </c>
       <c r="C235">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C235:C298" ca="1" si="5">IF(B235=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="2"/>
       <c r="B236">
-        <v>5242</v>
+        <v>2809</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2796,7 +2796,7 @@
     <row r="237" spans="1:3">
       <c r="A237" s="2"/>
       <c r="B237">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2806,7 +2806,7 @@
     <row r="238" spans="1:3">
       <c r="A238" s="2"/>
       <c r="B238">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2816,7 +2816,7 @@
     <row r="239" spans="1:3">
       <c r="A239" s="2"/>
       <c r="B239">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2826,7 +2826,7 @@
     <row r="240" spans="1:3">
       <c r="A240" s="2"/>
       <c r="B240">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2836,7 +2836,7 @@
     <row r="241" spans="1:3">
       <c r="A241" s="2"/>
       <c r="B241">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2846,7 +2846,7 @@
     <row r="242" spans="1:3">
       <c r="A242" s="2"/>
       <c r="B242">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2856,7 +2856,7 @@
     <row r="243" spans="1:3">
       <c r="A243" s="2"/>
       <c r="B243">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2866,7 +2866,7 @@
     <row r="244" spans="1:3">
       <c r="A244" s="2"/>
       <c r="B244">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
@@ -2876,7 +2876,7 @@
     <row r="245" spans="1:3">
       <c r="A245" s="2"/>
       <c r="B245">
-        <v>5463</v>
+        <v>1953</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
@@ -2884,12 +2884,20 @@
       </c>
     </row>
     <row r="246" spans="1:3">
+      <c r="A246" s="2"/>
+      <c r="B246">
+        <v>3956</v>
+      </c>
       <c r="C246">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:3">
+      <c r="A247" s="2"/>
+      <c r="B247">
+        <v>5463</v>
+      </c>
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3191,19 +3199,19 @@
     </row>
     <row r="297" spans="3:3">
       <c r="C297">
-        <f t="shared" ref="C297:C360" ca="1" si="6">IF(B297=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="298" spans="3:3">
       <c r="C298">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="3:3">
       <c r="C299">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C299:C362" ca="1" si="6">IF(B299=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3575,19 +3583,19 @@
     </row>
     <row r="361" spans="3:3">
       <c r="C361">
-        <f t="shared" ref="C361:C424" ca="1" si="7">IF(B361=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="362" spans="3:3">
       <c r="C362">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="363" spans="3:3">
       <c r="C363">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C363:C426" ca="1" si="7">IF(B363=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3959,19 +3967,19 @@
     </row>
     <row r="425" spans="3:3">
       <c r="C425">
-        <f t="shared" ref="C425:C488" ca="1" si="8">IF(B425=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="426" spans="3:3">
       <c r="C426">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="427" spans="3:3">
       <c r="C427">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C427:C490" ca="1" si="8">IF(B427=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4343,19 +4351,19 @@
     </row>
     <row r="489" spans="3:3">
       <c r="C489">
-        <f t="shared" ref="C489:C552" ca="1" si="9">IF(B489=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="490" spans="3:3">
       <c r="C490">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="491" spans="3:3">
       <c r="C491">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C491:C554" ca="1" si="9">IF(B491=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4727,19 +4735,19 @@
     </row>
     <row r="553" spans="3:3">
       <c r="C553">
-        <f t="shared" ref="C553:C616" ca="1" si="10">IF(B553=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="554" spans="3:3">
       <c r="C554">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="555" spans="3:3">
       <c r="C555">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C555:C618" ca="1" si="10">IF(B555=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5111,19 +5119,19 @@
     </row>
     <row r="617" spans="3:3">
       <c r="C617">
-        <f t="shared" ref="C617:C680" ca="1" si="11">IF(B617=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="618" spans="3:3">
       <c r="C618">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="619" spans="3:3">
       <c r="C619">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C619:C682" ca="1" si="11">IF(B619=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5495,19 +5503,19 @@
     </row>
     <row r="681" spans="3:3">
       <c r="C681">
-        <f t="shared" ref="C681:C744" ca="1" si="12">IF(B681=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="3:3">
       <c r="C682">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="3:3">
       <c r="C683">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C683:C746" ca="1" si="12">IF(B683=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5879,19 +5887,19 @@
     </row>
     <row r="745" spans="3:3">
       <c r="C745">
-        <f t="shared" ref="C745:C808" ca="1" si="13">IF(B745=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="3:3">
       <c r="C746">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="3:3">
       <c r="C747">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C747:C810" ca="1" si="13">IF(B747=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6263,19 +6271,19 @@
     </row>
     <row r="809" spans="3:3">
       <c r="C809">
-        <f t="shared" ref="C809:C872" ca="1" si="14">IF(B809=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="810" spans="3:3">
       <c r="C810">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="811" spans="3:3">
       <c r="C811">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C811:C874" ca="1" si="14">IF(B811=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6647,19 +6655,19 @@
     </row>
     <row r="873" spans="3:3">
       <c r="C873">
-        <f t="shared" ref="C873:C887" ca="1" si="15">IF(B873=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="874" spans="3:3">
       <c r="C874">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="875" spans="3:3">
       <c r="C875">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C875:C889" ca="1" si="15">IF(B875=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6735,19 +6743,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="888" spans="3:3">
+      <c r="C888">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="889" spans="3:3">
+      <c r="C889">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A217:A222"/>
-    <mergeCell ref="A223:A227"/>
-    <mergeCell ref="A229:A245"/>
+    <mergeCell ref="A219:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A231:A247"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A212:A216"/>
-    <mergeCell ref="A195:A211"/>
-    <mergeCell ref="A168:A194"/>
+    <mergeCell ref="A214:A218"/>
+    <mergeCell ref="A197:A213"/>
+    <mergeCell ref="A168:A196"/>
     <mergeCell ref="A157:A167"/>
     <mergeCell ref="A119:A156"/>
   </mergeCells>

</xml_diff>

<commit_message>
directory structure of java solution now contains all data files
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -398,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E889"/>
+  <dimension ref="A1:E890"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>5483</v>
+        <v>5277</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2067,7 +2067,7 @@
         <v>2166</v>
       </c>
       <c r="C165">
-        <f t="shared" ref="C165:C234" ca="1" si="4">IF(B165=$E$1,1,0)</f>
+        <f t="shared" ref="C165:C235" ca="1" si="4">IF(B165=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
     <row r="199" spans="1:3">
       <c r="A199" s="2"/>
       <c r="B199">
-        <v>9765</v>
+        <v>4488</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2418,7 +2418,7 @@
     <row r="200" spans="1:3">
       <c r="A200" s="2"/>
       <c r="B200">
-        <v>4954</v>
+        <v>9765</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2428,7 +2428,7 @@
     <row r="201" spans="1:3">
       <c r="A201" s="2"/>
       <c r="B201">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2438,7 +2438,7 @@
     <row r="202" spans="1:3">
       <c r="A202" s="2"/>
       <c r="B202">
-        <v>6431</v>
+        <v>5537</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2448,7 +2448,7 @@
     <row r="203" spans="1:3">
       <c r="A203" s="2"/>
       <c r="B203">
-        <v>7193</v>
+        <v>6431</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2458,7 +2458,7 @@
     <row r="204" spans="1:3">
       <c r="A204" s="2"/>
       <c r="B204">
-        <v>5621</v>
+        <v>7193</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2468,7 +2468,7 @@
     <row r="205" spans="1:3">
       <c r="A205" s="2"/>
       <c r="B205">
-        <v>5847</v>
+        <v>5621</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2478,7 +2478,7 @@
     <row r="206" spans="1:3">
       <c r="A206" s="2"/>
       <c r="B206">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2488,7 +2488,7 @@
     <row r="207" spans="1:3">
       <c r="A207" s="2"/>
       <c r="B207">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2498,7 +2498,7 @@
     <row r="208" spans="1:3">
       <c r="A208" s="2"/>
       <c r="B208">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2508,7 +2508,7 @@
     <row r="209" spans="1:3">
       <c r="A209" s="2"/>
       <c r="B209">
-        <v>2205</v>
+        <v>6861</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2518,7 +2518,7 @@
     <row r="210" spans="1:3">
       <c r="A210" s="2"/>
       <c r="B210">
-        <v>4372</v>
+        <v>2205</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2528,7 +2528,7 @@
     <row r="211" spans="1:3">
       <c r="A211" s="2"/>
       <c r="B211">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2538,7 +2538,7 @@
     <row r="212" spans="1:3">
       <c r="A212" s="2"/>
       <c r="B212">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2548,7 +2548,7 @@
     <row r="213" spans="1:3">
       <c r="A213" s="2"/>
       <c r="B213">
-        <v>2137</v>
+        <v>1668</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2556,11 +2556,9 @@
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A214" s="2"/>
       <c r="B214">
-        <v>9300</v>
+        <v>2137</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2568,9 +2566,11 @@
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="2"/>
+      <c r="A215" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B215">
-        <v>3951</v>
+        <v>9300</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2580,7 +2580,7 @@
     <row r="216" spans="1:3">
       <c r="A216" s="2"/>
       <c r="B216">
-        <v>6409</v>
+        <v>3951</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2590,7 +2590,7 @@
     <row r="217" spans="1:3">
       <c r="A217" s="2"/>
       <c r="B217">
-        <v>7343</v>
+        <v>6409</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2600,7 +2600,7 @@
     <row r="218" spans="1:3">
       <c r="A218" s="2"/>
       <c r="B218">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2608,11 +2608,9 @@
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A219" s="2"/>
       <c r="B219">
-        <v>9299</v>
+        <v>7060</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2620,9 +2618,11 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="2"/>
+      <c r="A220" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B220">
-        <v>7560</v>
+        <v>9299</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2632,7 +2632,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="2"/>
       <c r="B221">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2642,7 +2642,7 @@
     <row r="222" spans="1:3">
       <c r="A222" s="2"/>
       <c r="B222">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2652,7 +2652,7 @@
     <row r="223" spans="1:3">
       <c r="A223" s="2"/>
       <c r="B223">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2662,7 +2662,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="2"/>
       <c r="B224">
-        <v>2048</v>
+        <v>1954</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2670,11 +2670,9 @@
       </c>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A225" s="2"/>
       <c r="B225">
-        <v>3939</v>
+        <v>2048</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2682,9 +2680,11 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="2"/>
+      <c r="A226" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B226">
-        <v>8861</v>
+        <v>3939</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2694,17 +2694,17 @@
     <row r="227" spans="1:3">
       <c r="A227" s="2"/>
       <c r="B227">
-        <v>1516</v>
+        <v>8861</v>
       </c>
       <c r="C227">
-        <f ca="1">IF(B227=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="2"/>
       <c r="B228">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C228">
         <f ca="1">IF(B228=$E$1,1,0)</f>
@@ -2714,7 +2714,7 @@
     <row r="229" spans="1:3">
       <c r="A229" s="2"/>
       <c r="B229">
-        <v>5164</v>
+        <v>9062</v>
       </c>
       <c r="C229">
         <f ca="1">IF(B229=$E$1,1,0)</f>
@@ -2722,9 +2722,9 @@
       </c>
     </row>
     <row r="230" spans="1:3">
-      <c r="A230" s="1"/>
+      <c r="A230" s="2"/>
       <c r="B230">
-        <v>2354</v>
+        <v>5164</v>
       </c>
       <c r="C230">
         <f ca="1">IF(B230=$E$1,1,0)</f>
@@ -2732,21 +2732,21 @@
       </c>
     </row>
     <row r="231" spans="1:3">
-      <c r="A231" s="2" t="s">
+      <c r="A231" s="1"/>
+      <c r="B231">
+        <v>2354</v>
+      </c>
+      <c r="C231">
+        <f ca="1">IF(B231=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B231">
+      <c r="B232">
         <v>8403</v>
-      </c>
-      <c r="C231">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" s="2"/>
-      <c r="B232">
-        <v>3185</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="4"/>
@@ -2756,7 +2756,7 @@
     <row r="233" spans="1:3">
       <c r="A233" s="2"/>
       <c r="B233">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="4"/>
@@ -2766,7 +2766,7 @@
     <row r="234" spans="1:3">
       <c r="A234" s="2"/>
       <c r="B234">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="4"/>
@@ -2776,27 +2776,27 @@
     <row r="235" spans="1:3">
       <c r="A235" s="2"/>
       <c r="B235">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C235">
-        <f t="shared" ref="C235:C298" ca="1" si="5">IF(B235=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="2"/>
       <c r="B236">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C236">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C236:C299" ca="1" si="5">IF(B236=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="2"/>
       <c r="B237">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2806,7 +2806,7 @@
     <row r="238" spans="1:3">
       <c r="A238" s="2"/>
       <c r="B238">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2816,7 +2816,7 @@
     <row r="239" spans="1:3">
       <c r="A239" s="2"/>
       <c r="B239">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2826,7 +2826,7 @@
     <row r="240" spans="1:3">
       <c r="A240" s="2"/>
       <c r="B240">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2836,7 +2836,7 @@
     <row r="241" spans="1:3">
       <c r="A241" s="2"/>
       <c r="B241">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2846,7 +2846,7 @@
     <row r="242" spans="1:3">
       <c r="A242" s="2"/>
       <c r="B242">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2856,7 +2856,7 @@
     <row r="243" spans="1:3">
       <c r="A243" s="2"/>
       <c r="B243">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2866,7 +2866,7 @@
     <row r="244" spans="1:3">
       <c r="A244" s="2"/>
       <c r="B244">
-        <v>4147</v>
+        <v>2000</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
@@ -2876,7 +2876,7 @@
     <row r="245" spans="1:3">
       <c r="A245" s="2"/>
       <c r="B245">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
@@ -2886,7 +2886,7 @@
     <row r="246" spans="1:3">
       <c r="A246" s="2"/>
       <c r="B246">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="5"/>
@@ -2896,7 +2896,7 @@
     <row r="247" spans="1:3">
       <c r="A247" s="2"/>
       <c r="B247">
-        <v>5463</v>
+        <v>3956</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
@@ -2904,6 +2904,10 @@
       </c>
     </row>
     <row r="248" spans="1:3">
+      <c r="A248" s="2"/>
+      <c r="B248">
+        <v>5463</v>
+      </c>
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3211,13 +3215,13 @@
     </row>
     <row r="299" spans="3:3">
       <c r="C299">
-        <f t="shared" ref="C299:C362" ca="1" si="6">IF(B299=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="300" spans="3:3">
       <c r="C300">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C300:C363" ca="1" si="6">IF(B300=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3595,13 +3599,13 @@
     </row>
     <row r="363" spans="3:3">
       <c r="C363">
-        <f t="shared" ref="C363:C426" ca="1" si="7">IF(B363=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="364" spans="3:3">
       <c r="C364">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C364:C427" ca="1" si="7">IF(B364=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3979,13 +3983,13 @@
     </row>
     <row r="427" spans="3:3">
       <c r="C427">
-        <f t="shared" ref="C427:C490" ca="1" si="8">IF(B427=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="428" spans="3:3">
       <c r="C428">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C428:C491" ca="1" si="8">IF(B428=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4363,13 +4367,13 @@
     </row>
     <row r="491" spans="3:3">
       <c r="C491">
-        <f t="shared" ref="C491:C554" ca="1" si="9">IF(B491=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="492" spans="3:3">
       <c r="C492">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C492:C555" ca="1" si="9">IF(B492=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4747,13 +4751,13 @@
     </row>
     <row r="555" spans="3:3">
       <c r="C555">
-        <f t="shared" ref="C555:C618" ca="1" si="10">IF(B555=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="556" spans="3:3">
       <c r="C556">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C556:C619" ca="1" si="10">IF(B556=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5131,13 +5135,13 @@
     </row>
     <row r="619" spans="3:3">
       <c r="C619">
-        <f t="shared" ref="C619:C682" ca="1" si="11">IF(B619=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="620" spans="3:3">
       <c r="C620">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C620:C683" ca="1" si="11">IF(B620=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5515,13 +5519,13 @@
     </row>
     <row r="683" spans="3:3">
       <c r="C683">
-        <f t="shared" ref="C683:C746" ca="1" si="12">IF(B683=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="3:3">
       <c r="C684">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C684:C747" ca="1" si="12">IF(B684=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5899,13 +5903,13 @@
     </row>
     <row r="747" spans="3:3">
       <c r="C747">
-        <f t="shared" ref="C747:C810" ca="1" si="13">IF(B747=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="3:3">
       <c r="C748">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C748:C811" ca="1" si="13">IF(B748=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6283,13 +6287,13 @@
     </row>
     <row r="811" spans="3:3">
       <c r="C811">
-        <f t="shared" ref="C811:C874" ca="1" si="14">IF(B811=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="812" spans="3:3">
       <c r="C812">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C812:C875" ca="1" si="14">IF(B812=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6667,13 +6671,13 @@
     </row>
     <row r="875" spans="3:3">
       <c r="C875">
-        <f t="shared" ref="C875:C889" ca="1" si="15">IF(B875=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="876" spans="3:3">
       <c r="C876">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C876:C890" ca="1" si="15">IF(B876=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6755,23 +6759,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="890" spans="3:3">
+      <c r="C890">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A219:A224"/>
-    <mergeCell ref="A225:A229"/>
-    <mergeCell ref="A231:A247"/>
+    <mergeCell ref="A220:A225"/>
+    <mergeCell ref="A226:A230"/>
+    <mergeCell ref="A232:A248"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A214:A218"/>
-    <mergeCell ref="A197:A213"/>
+    <mergeCell ref="A215:A219"/>
+    <mergeCell ref="A197:A214"/>
     <mergeCell ref="A168:A196"/>
     <mergeCell ref="A157:A167"/>
     <mergeCell ref="A119:A156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solve some tasks in lab09. remove and add tasks to lab09. add tasks to lab07
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -398,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E890"/>
+  <dimension ref="A1:E892"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B200" sqref="B200"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>5277</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1393,7 +1393,7 @@
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C164" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C165" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2034,7 +2034,7 @@
     <row r="162" spans="1:3">
       <c r="A162" s="2"/>
       <c r="B162">
-        <v>7491</v>
+        <v>1618</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
@@ -2044,7 +2044,7 @@
     <row r="163" spans="1:3">
       <c r="A163" s="2"/>
       <c r="B163">
-        <v>5923</v>
+        <v>7491</v>
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="3"/>
@@ -2054,7 +2054,7 @@
     <row r="164" spans="1:3">
       <c r="A164" s="2"/>
       <c r="B164">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="3"/>
@@ -2064,27 +2064,27 @@
     <row r="165" spans="1:3">
       <c r="A165" s="2"/>
       <c r="B165">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C165">
-        <f t="shared" ref="C165:C235" ca="1" si="4">IF(B165=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="2"/>
       <c r="B166">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C166">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="C166:C237" ca="1" si="4">IF(B166=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="2"/>
       <c r="B167">
-        <v>9925</v>
+        <v>9116</v>
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="4"/>
@@ -2092,11 +2092,9 @@
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A168" s="2"/>
       <c r="B168">
-        <v>2885</v>
+        <v>9925</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
@@ -2104,9 +2102,11 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="2"/>
+      <c r="A169" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B169">
-        <v>9931</v>
+        <v>2885</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
@@ -2116,7 +2116,7 @@
     <row r="170" spans="1:3">
       <c r="A170" s="2"/>
       <c r="B170">
-        <v>4425</v>
+        <v>9931</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2126,7 +2126,7 @@
     <row r="171" spans="1:3">
       <c r="A171" s="2"/>
       <c r="B171">
-        <v>1947</v>
+        <v>4425</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2136,7 +2136,7 @@
     <row r="172" spans="1:3">
       <c r="A172" s="2"/>
       <c r="B172">
-        <v>9696</v>
+        <v>1947</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2146,7 +2146,7 @@
     <row r="173" spans="1:3">
       <c r="A173" s="2"/>
       <c r="B173">
-        <v>1223</v>
+        <v>9696</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2156,7 +2156,7 @@
     <row r="174" spans="1:3">
       <c r="A174" s="2"/>
       <c r="B174">
-        <v>3946</v>
+        <v>1223</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2166,7 +2166,7 @@
     <row r="175" spans="1:3">
       <c r="A175" s="2"/>
       <c r="B175">
-        <v>8311</v>
+        <v>3946</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2176,7 +2176,7 @@
     <row r="176" spans="1:3">
       <c r="A176" s="2"/>
       <c r="B176">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2186,7 +2186,7 @@
     <row r="177" spans="1:3">
       <c r="A177" s="2"/>
       <c r="B177">
-        <v>9774</v>
+        <v>3134</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2196,7 +2196,7 @@
     <row r="178" spans="1:3">
       <c r="A178" s="2"/>
       <c r="B178">
-        <v>9711</v>
+        <v>9774</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2206,7 +2206,7 @@
     <row r="179" spans="1:3">
       <c r="A179" s="2"/>
       <c r="B179">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2216,7 +2216,7 @@
     <row r="180" spans="1:3">
       <c r="A180" s="2"/>
       <c r="B180">
-        <v>7290</v>
+        <v>3333</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2226,7 +2226,7 @@
     <row r="181" spans="1:3">
       <c r="A181" s="2"/>
       <c r="B181">
-        <v>5694</v>
+        <v>7290</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2236,7 +2236,7 @@
     <row r="182" spans="1:3">
       <c r="A182" s="2"/>
       <c r="B182">
-        <v>7035</v>
+        <v>5694</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2246,7 +2246,7 @@
     <row r="183" spans="1:3">
       <c r="A183" s="2"/>
       <c r="B183">
-        <v>6806</v>
+        <v>7035</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2256,7 +2256,7 @@
     <row r="184" spans="1:3">
       <c r="A184" s="2"/>
       <c r="B184">
-        <v>4515</v>
+        <v>6806</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2266,7 +2266,7 @@
     <row r="185" spans="1:3">
       <c r="A185" s="2"/>
       <c r="B185">
-        <v>9271</v>
+        <v>4515</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2276,7 +2276,7 @@
     <row r="186" spans="1:3">
       <c r="A186" s="2"/>
       <c r="B186">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2286,7 +2286,7 @@
     <row r="187" spans="1:3">
       <c r="A187" s="2"/>
       <c r="B187">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2296,7 +2296,7 @@
     <row r="188" spans="1:3">
       <c r="A188" s="2"/>
       <c r="B188">
-        <v>3940</v>
+        <v>4497</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2306,7 +2306,7 @@
     <row r="189" spans="1:3">
       <c r="A189" s="2"/>
       <c r="B189">
-        <v>8820</v>
+        <v>3940</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2316,7 +2316,7 @@
     <row r="190" spans="1:3">
       <c r="A190" s="2"/>
       <c r="B190">
-        <v>3218</v>
+        <v>8820</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2326,7 +2326,7 @@
     <row r="191" spans="1:3">
       <c r="A191" s="2"/>
       <c r="B191">
-        <v>4283</v>
+        <v>3218</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2336,7 +2336,7 @@
     <row r="192" spans="1:3">
       <c r="A192" s="2"/>
       <c r="B192">
-        <v>7703</v>
+        <v>4283</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2346,7 +2346,7 @@
     <row r="193" spans="1:3">
       <c r="A193" s="2"/>
       <c r="B193">
-        <v>9182</v>
+        <v>7703</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2356,7 +2356,7 @@
     <row r="194" spans="1:3">
       <c r="A194" s="2"/>
       <c r="B194">
-        <v>5541</v>
+        <v>9182</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
@@ -2366,7 +2366,7 @@
     <row r="195" spans="1:3">
       <c r="A195" s="2"/>
       <c r="B195">
-        <v>2386</v>
+        <v>5541</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2376,7 +2376,7 @@
     <row r="196" spans="1:3">
       <c r="A196" s="2"/>
       <c r="B196">
-        <v>9159</v>
+        <v>2386</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2384,11 +2384,9 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A197" s="2"/>
       <c r="B197">
-        <v>6175</v>
+        <v>9159</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2396,9 +2394,11 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="2"/>
+      <c r="A198" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B198">
-        <v>4642</v>
+        <v>6175</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2408,7 +2408,7 @@
     <row r="199" spans="1:3">
       <c r="A199" s="2"/>
       <c r="B199">
-        <v>4488</v>
+        <v>4642</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2418,7 +2418,7 @@
     <row r="200" spans="1:3">
       <c r="A200" s="2"/>
       <c r="B200">
-        <v>9765</v>
+        <v>4488</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2428,7 +2428,7 @@
     <row r="201" spans="1:3">
       <c r="A201" s="2"/>
       <c r="B201">
-        <v>4954</v>
+        <v>9765</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2438,7 +2438,7 @@
     <row r="202" spans="1:3">
       <c r="A202" s="2"/>
       <c r="B202">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2448,7 +2448,7 @@
     <row r="203" spans="1:3">
       <c r="A203" s="2"/>
       <c r="B203">
-        <v>6431</v>
+        <v>5537</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2458,7 +2458,7 @@
     <row r="204" spans="1:3">
       <c r="A204" s="2"/>
       <c r="B204">
-        <v>7193</v>
+        <v>6431</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2468,7 +2468,7 @@
     <row r="205" spans="1:3">
       <c r="A205" s="2"/>
       <c r="B205">
-        <v>5621</v>
+        <v>7193</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2478,7 +2478,7 @@
     <row r="206" spans="1:3">
       <c r="A206" s="2"/>
       <c r="B206">
-        <v>5847</v>
+        <v>5621</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2488,7 +2488,7 @@
     <row r="207" spans="1:3">
       <c r="A207" s="2"/>
       <c r="B207">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2498,7 +2498,7 @@
     <row r="208" spans="1:3">
       <c r="A208" s="2"/>
       <c r="B208">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2508,7 +2508,7 @@
     <row r="209" spans="1:3">
       <c r="A209" s="2"/>
       <c r="B209">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2518,7 +2518,7 @@
     <row r="210" spans="1:3">
       <c r="A210" s="2"/>
       <c r="B210">
-        <v>2205</v>
+        <v>3226</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2528,7 +2528,7 @@
     <row r="211" spans="1:3">
       <c r="A211" s="2"/>
       <c r="B211">
-        <v>4372</v>
+        <v>6861</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2538,7 +2538,7 @@
     <row r="212" spans="1:3">
       <c r="A212" s="2"/>
       <c r="B212">
-        <v>4463</v>
+        <v>2205</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2548,7 +2548,7 @@
     <row r="213" spans="1:3">
       <c r="A213" s="2"/>
       <c r="B213">
-        <v>1668</v>
+        <v>4372</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2558,7 +2558,7 @@
     <row r="214" spans="1:3">
       <c r="A214" s="2"/>
       <c r="B214">
-        <v>2137</v>
+        <v>4463</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2566,11 +2566,9 @@
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A215" s="2"/>
       <c r="B215">
-        <v>9300</v>
+        <v>1668</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2580,7 +2578,7 @@
     <row r="216" spans="1:3">
       <c r="A216" s="2"/>
       <c r="B216">
-        <v>3951</v>
+        <v>2137</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2588,9 +2586,11 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="2"/>
+      <c r="A217" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B217">
-        <v>6409</v>
+        <v>9300</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2600,7 +2600,7 @@
     <row r="218" spans="1:3">
       <c r="A218" s="2"/>
       <c r="B218">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2610,7 +2610,7 @@
     <row r="219" spans="1:3">
       <c r="A219" s="2"/>
       <c r="B219">
-        <v>7060</v>
+        <v>6409</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2618,11 +2618,9 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A220" s="2"/>
       <c r="B220">
-        <v>9299</v>
+        <v>7343</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2632,7 +2630,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="2"/>
       <c r="B221">
-        <v>7560</v>
+        <v>7060</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2640,9 +2638,11 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="2"/>
+      <c r="A222" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B222">
-        <v>9002</v>
+        <v>9299</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2652,7 +2652,7 @@
     <row r="223" spans="1:3">
       <c r="A223" s="2"/>
       <c r="B223">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2662,7 +2662,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="2"/>
       <c r="B224">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2672,7 +2672,7 @@
     <row r="225" spans="1:3">
       <c r="A225" s="2"/>
       <c r="B225">
-        <v>2048</v>
+        <v>7432</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2680,11 +2680,9 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A226" s="2"/>
       <c r="B226">
-        <v>3939</v>
+        <v>1954</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2694,7 +2692,7 @@
     <row r="227" spans="1:3">
       <c r="A227" s="2"/>
       <c r="B227">
-        <v>8861</v>
+        <v>2048</v>
       </c>
       <c r="C227">
         <f t="shared" ca="1" si="4"/>
@@ -2702,29 +2700,31 @@
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="2"/>
+      <c r="A228" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B228">
-        <v>1516</v>
+        <v>3939</v>
       </c>
       <c r="C228">
-        <f ca="1">IF(B228=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="2"/>
       <c r="B229">
-        <v>9062</v>
+        <v>8861</v>
       </c>
       <c r="C229">
-        <f ca="1">IF(B229=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="2"/>
       <c r="B230">
-        <v>5164</v>
+        <v>1516</v>
       </c>
       <c r="C230">
         <f ca="1">IF(B230=$E$1,1,0)</f>
@@ -2732,9 +2732,9 @@
       </c>
     </row>
     <row r="231" spans="1:3">
-      <c r="A231" s="1"/>
+      <c r="A231" s="2"/>
       <c r="B231">
-        <v>2354</v>
+        <v>9062</v>
       </c>
       <c r="C231">
         <f ca="1">IF(B231=$E$1,1,0)</f>
@@ -2742,31 +2742,31 @@
       </c>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="2" t="s">
+      <c r="A232" s="2"/>
+      <c r="B232">
+        <v>5164</v>
+      </c>
+      <c r="C232">
+        <f ca="1">IF(B232=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="1"/>
+      <c r="B233">
+        <v>2354</v>
+      </c>
+      <c r="C233">
+        <f ca="1">IF(B233=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B232">
+      <c r="B234">
         <v>8403</v>
-      </c>
-      <c r="C232">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="2"/>
-      <c r="B233">
-        <v>3185</v>
-      </c>
-      <c r="C233">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234" s="2"/>
-      <c r="B234">
-        <v>9914</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="4"/>
@@ -2776,7 +2776,7 @@
     <row r="235" spans="1:3">
       <c r="A235" s="2"/>
       <c r="B235">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="4"/>
@@ -2786,37 +2786,37 @@
     <row r="236" spans="1:3">
       <c r="A236" s="2"/>
       <c r="B236">
-        <v>6037</v>
+        <v>9914</v>
       </c>
       <c r="C236">
-        <f t="shared" ref="C236:C299" ca="1" si="5">IF(B236=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="2"/>
       <c r="B237">
-        <v>2809</v>
+        <v>6011</v>
       </c>
       <c r="C237">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="2"/>
       <c r="B238">
-        <v>7297</v>
+        <v>6037</v>
       </c>
       <c r="C238">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C238:C301" ca="1" si="5">IF(B238=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="2"/>
       <c r="B239">
-        <v>5242</v>
+        <v>2809</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2826,7 +2826,7 @@
     <row r="240" spans="1:3">
       <c r="A240" s="2"/>
       <c r="B240">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2836,7 +2836,7 @@
     <row r="241" spans="1:3">
       <c r="A241" s="2"/>
       <c r="B241">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2846,7 +2846,7 @@
     <row r="242" spans="1:3">
       <c r="A242" s="2"/>
       <c r="B242">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2856,7 +2856,7 @@
     <row r="243" spans="1:3">
       <c r="A243" s="2"/>
       <c r="B243">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2866,7 +2866,7 @@
     <row r="244" spans="1:3">
       <c r="A244" s="2"/>
       <c r="B244">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
@@ -2876,7 +2876,7 @@
     <row r="245" spans="1:3">
       <c r="A245" s="2"/>
       <c r="B245">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
@@ -2886,7 +2886,7 @@
     <row r="246" spans="1:3">
       <c r="A246" s="2"/>
       <c r="B246">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="5"/>
@@ -2896,7 +2896,7 @@
     <row r="247" spans="1:3">
       <c r="A247" s="2"/>
       <c r="B247">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
@@ -2906,7 +2906,7 @@
     <row r="248" spans="1:3">
       <c r="A248" s="2"/>
       <c r="B248">
-        <v>5463</v>
+        <v>1953</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
@@ -2914,12 +2914,20 @@
       </c>
     </row>
     <row r="249" spans="1:3">
+      <c r="A249" s="2"/>
+      <c r="B249">
+        <v>3956</v>
+      </c>
       <c r="C249">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:3">
+      <c r="A250" s="2"/>
+      <c r="B250">
+        <v>5463</v>
+      </c>
       <c r="C250">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3221,19 +3229,19 @@
     </row>
     <row r="300" spans="3:3">
       <c r="C300">
-        <f t="shared" ref="C300:C363" ca="1" si="6">IF(B300=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="301" spans="3:3">
       <c r="C301">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="302" spans="3:3">
       <c r="C302">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C302:C365" ca="1" si="6">IF(B302=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3605,19 +3613,19 @@
     </row>
     <row r="364" spans="3:3">
       <c r="C364">
-        <f t="shared" ref="C364:C427" ca="1" si="7">IF(B364=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="365" spans="3:3">
       <c r="C365">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="366" spans="3:3">
       <c r="C366">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C366:C429" ca="1" si="7">IF(B366=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3989,19 +3997,19 @@
     </row>
     <row r="428" spans="3:3">
       <c r="C428">
-        <f t="shared" ref="C428:C491" ca="1" si="8">IF(B428=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="429" spans="3:3">
       <c r="C429">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="430" spans="3:3">
       <c r="C430">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C430:C493" ca="1" si="8">IF(B430=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4373,19 +4381,19 @@
     </row>
     <row r="492" spans="3:3">
       <c r="C492">
-        <f t="shared" ref="C492:C555" ca="1" si="9">IF(B492=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="493" spans="3:3">
       <c r="C493">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="494" spans="3:3">
       <c r="C494">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C494:C557" ca="1" si="9">IF(B494=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4757,19 +4765,19 @@
     </row>
     <row r="556" spans="3:3">
       <c r="C556">
-        <f t="shared" ref="C556:C619" ca="1" si="10">IF(B556=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="557" spans="3:3">
       <c r="C557">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="558" spans="3:3">
       <c r="C558">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C558:C621" ca="1" si="10">IF(B558=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5141,19 +5149,19 @@
     </row>
     <row r="620" spans="3:3">
       <c r="C620">
-        <f t="shared" ref="C620:C683" ca="1" si="11">IF(B620=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="621" spans="3:3">
       <c r="C621">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="3:3">
       <c r="C622">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C622:C685" ca="1" si="11">IF(B622=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5525,19 +5533,19 @@
     </row>
     <row r="684" spans="3:3">
       <c r="C684">
-        <f t="shared" ref="C684:C747" ca="1" si="12">IF(B684=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="3:3">
       <c r="C685">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="3:3">
       <c r="C686">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C686:C749" ca="1" si="12">IF(B686=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5909,19 +5917,19 @@
     </row>
     <row r="748" spans="3:3">
       <c r="C748">
-        <f t="shared" ref="C748:C811" ca="1" si="13">IF(B748=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="3:3">
       <c r="C749">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="3:3">
       <c r="C750">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C750:C813" ca="1" si="13">IF(B750=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6293,19 +6301,19 @@
     </row>
     <row r="812" spans="3:3">
       <c r="C812">
-        <f t="shared" ref="C812:C875" ca="1" si="14">IF(B812=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="3:3">
       <c r="C813">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="814" spans="3:3">
       <c r="C814">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C814:C877" ca="1" si="14">IF(B814=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6677,19 +6685,19 @@
     </row>
     <row r="876" spans="3:3">
       <c r="C876">
-        <f t="shared" ref="C876:C890" ca="1" si="15">IF(B876=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="877" spans="3:3">
       <c r="C877">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="878" spans="3:3">
       <c r="C878">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C878:C892" ca="1" si="15">IF(B878=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6765,20 +6773,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="891" spans="3:3">
+      <c r="C891">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="892" spans="3:3">
+      <c r="C892">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A220:A225"/>
-    <mergeCell ref="A226:A230"/>
-    <mergeCell ref="A232:A248"/>
+    <mergeCell ref="A222:A227"/>
+    <mergeCell ref="A228:A232"/>
+    <mergeCell ref="A234:A250"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A215:A219"/>
-    <mergeCell ref="A197:A214"/>
-    <mergeCell ref="A168:A196"/>
-    <mergeCell ref="A157:A167"/>
+    <mergeCell ref="A217:A221"/>
+    <mergeCell ref="A198:A216"/>
+    <mergeCell ref="A169:A197"/>
+    <mergeCell ref="A157:A168"/>
     <mergeCell ref="A119:A156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add more tasks for lab12 fill missing tasks from existing tasks from lab12 regroup solutions by task from lab12
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -91,11 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -398,11 +395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E892"/>
+  <dimension ref="A1:E894"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H229" sqref="H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,11 +411,11 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>2120</v>
+        <v>9389</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -430,7 +427,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
+      <c r="A3" s="1"/>
       <c r="B3">
         <v>1860</v>
       </c>
@@ -440,7 +437,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
       <c r="B4">
         <v>4764</v>
       </c>
@@ -450,7 +447,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
       <c r="B5">
         <v>2429</v>
       </c>
@@ -460,7 +457,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
       <c r="B6">
         <v>7472</v>
       </c>
@@ -470,7 +467,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7">
         <v>3862</v>
       </c>
@@ -480,7 +477,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
       <c r="B8">
         <v>9231</v>
       </c>
@@ -490,7 +487,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9">
         <v>8624</v>
       </c>
@@ -500,7 +497,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
       <c r="B10">
         <v>2959</v>
       </c>
@@ -510,7 +507,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11">
         <v>7271</v>
       </c>
@@ -520,7 +517,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
+      <c r="A12" s="1"/>
       <c r="B12">
         <v>2632</v>
       </c>
@@ -530,7 +527,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
       <c r="B13">
         <v>4343</v>
       </c>
@@ -540,7 +537,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
+      <c r="A14" s="1"/>
       <c r="B14">
         <v>1517</v>
       </c>
@@ -550,7 +547,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
+      <c r="A15" s="1"/>
       <c r="B15">
         <v>1413</v>
       </c>
@@ -560,7 +557,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2"/>
+      <c r="A16" s="1"/>
       <c r="B16">
         <v>9405</v>
       </c>
@@ -570,7 +567,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B17">
@@ -582,7 +579,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="1"/>
       <c r="B18">
         <v>9298</v>
       </c>
@@ -592,7 +589,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="B19">
         <v>3354</v>
       </c>
@@ -602,7 +599,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
       <c r="B20">
         <v>8569</v>
       </c>
@@ -612,7 +609,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="2"/>
+      <c r="A21" s="1"/>
       <c r="B21">
         <v>3730</v>
       </c>
@@ -622,7 +619,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2"/>
+      <c r="A22" s="1"/>
       <c r="B22">
         <v>9007</v>
       </c>
@@ -632,7 +629,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1"/>
       <c r="B23">
         <v>5201</v>
       </c>
@@ -642,7 +639,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="1"/>
       <c r="B24">
         <v>2981</v>
       </c>
@@ -652,7 +649,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="1"/>
       <c r="B25">
         <v>4312</v>
       </c>
@@ -662,7 +659,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="1"/>
       <c r="B26">
         <v>8428</v>
       </c>
@@ -672,7 +669,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="1"/>
       <c r="B27">
         <v>2361</v>
       </c>
@@ -682,7 +679,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="2"/>
+      <c r="A28" s="1"/>
       <c r="B28">
         <v>5063</v>
       </c>
@@ -692,7 +689,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2"/>
+      <c r="A29" s="1"/>
       <c r="B29">
         <v>7711</v>
       </c>
@@ -702,7 +699,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="2"/>
+      <c r="A30" s="1"/>
       <c r="B30">
         <v>8833</v>
       </c>
@@ -712,7 +709,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
       <c r="B31">
         <v>1262</v>
       </c>
@@ -722,7 +719,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1"/>
       <c r="B32">
         <v>9020</v>
       </c>
@@ -732,7 +729,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1"/>
       <c r="B33">
         <v>1934</v>
       </c>
@@ -742,7 +739,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
+      <c r="A34" s="1"/>
       <c r="B34">
         <v>7237</v>
       </c>
@@ -752,7 +749,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2"/>
+      <c r="A35" s="1"/>
       <c r="B35">
         <v>3943</v>
       </c>
@@ -762,7 +759,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
+      <c r="A36" s="1"/>
       <c r="B36">
         <v>7619</v>
       </c>
@@ -772,7 +769,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2"/>
+      <c r="A37" s="1"/>
       <c r="B37">
         <v>3832</v>
       </c>
@@ -782,7 +779,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
+      <c r="A38" s="1"/>
       <c r="B38">
         <v>1346</v>
       </c>
@@ -792,7 +789,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2"/>
+      <c r="A39" s="1"/>
       <c r="B39">
         <v>9622</v>
       </c>
@@ -802,7 +799,7 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2"/>
+      <c r="A40" s="1"/>
       <c r="B40">
         <v>8873</v>
       </c>
@@ -812,7 +809,7 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2"/>
+      <c r="A41" s="1"/>
       <c r="B41">
         <v>7799</v>
       </c>
@@ -822,7 +819,7 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2"/>
+      <c r="A42" s="1"/>
       <c r="B42">
         <v>9354</v>
       </c>
@@ -832,7 +829,7 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2"/>
+      <c r="A43" s="1"/>
       <c r="B43">
         <v>9130</v>
       </c>
@@ -842,7 +839,7 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2"/>
+      <c r="A44" s="1"/>
       <c r="B44">
         <v>5895</v>
       </c>
@@ -852,7 +849,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="1"/>
       <c r="B45">
         <v>2461</v>
       </c>
@@ -862,7 +859,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
+      <c r="A46" s="1"/>
       <c r="B46">
         <v>2790</v>
       </c>
@@ -872,7 +869,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="1"/>
       <c r="B47">
         <v>2624</v>
       </c>
@@ -882,7 +879,7 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2"/>
+      <c r="A48" s="1"/>
       <c r="B48">
         <v>5871</v>
       </c>
@@ -892,7 +889,7 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2"/>
+      <c r="A49" s="1"/>
       <c r="B49">
         <v>9164</v>
       </c>
@@ -902,7 +899,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2"/>
+      <c r="A50" s="1"/>
       <c r="B50">
         <v>7457</v>
       </c>
@@ -912,7 +909,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
+      <c r="A51" s="1"/>
       <c r="B51">
         <v>9865</v>
       </c>
@@ -922,7 +919,7 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
+      <c r="A52" s="1"/>
       <c r="B52">
         <v>3591</v>
       </c>
@@ -932,7 +929,7 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
+      <c r="A53" s="1"/>
       <c r="B53">
         <v>3558</v>
       </c>
@@ -942,7 +939,7 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2"/>
+      <c r="A54" s="1"/>
       <c r="B54">
         <v>4366</v>
       </c>
@@ -952,7 +949,7 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
+      <c r="A55" s="1"/>
       <c r="B55">
         <v>5789</v>
       </c>
@@ -962,7 +959,7 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2"/>
+      <c r="A56" s="1"/>
       <c r="B56">
         <v>6522</v>
       </c>
@@ -972,7 +969,7 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B57">
@@ -984,7 +981,7 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2"/>
+      <c r="A58" s="1"/>
       <c r="B58">
         <v>1288</v>
       </c>
@@ -994,7 +991,7 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="1"/>
       <c r="B59">
         <v>2614</v>
       </c>
@@ -1004,7 +1001,7 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2"/>
+      <c r="A60" s="1"/>
       <c r="B60">
         <v>7170</v>
       </c>
@@ -1014,7 +1011,7 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2"/>
+      <c r="A61" s="1"/>
       <c r="B61">
         <v>2709</v>
       </c>
@@ -1024,7 +1021,7 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2"/>
+      <c r="A62" s="1"/>
       <c r="B62">
         <v>3402</v>
       </c>
@@ -1034,7 +1031,7 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2"/>
+      <c r="A63" s="1"/>
       <c r="B63">
         <v>8781</v>
       </c>
@@ -1044,7 +1041,7 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="2"/>
+      <c r="A64" s="1"/>
       <c r="B64">
         <v>8771</v>
       </c>
@@ -1054,7 +1051,7 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="2"/>
+      <c r="A65" s="1"/>
       <c r="B65">
         <v>3091</v>
       </c>
@@ -1064,7 +1061,7 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="2"/>
+      <c r="A66" s="1"/>
       <c r="B66">
         <v>2195</v>
       </c>
@@ -1074,7 +1071,7 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="2"/>
+      <c r="A67" s="1"/>
       <c r="B67">
         <v>1184</v>
       </c>
@@ -1084,7 +1081,7 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="2"/>
+      <c r="A68" s="1"/>
       <c r="B68">
         <v>2667</v>
       </c>
@@ -1094,7 +1091,7 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2"/>
+      <c r="A69" s="1"/>
       <c r="B69">
         <v>5917</v>
       </c>
@@ -1104,7 +1101,7 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="2"/>
+      <c r="A70" s="1"/>
       <c r="B70">
         <v>3929</v>
       </c>
@@ -1114,7 +1111,7 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="2"/>
+      <c r="A71" s="1"/>
       <c r="B71">
         <v>3083</v>
       </c>
@@ -1124,7 +1121,7 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="2"/>
+      <c r="A72" s="1"/>
       <c r="B72">
         <v>7546</v>
       </c>
@@ -1134,7 +1131,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B73">
@@ -1146,7 +1143,7 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2"/>
+      <c r="A74" s="1"/>
       <c r="B74">
         <v>6598</v>
       </c>
@@ -1156,7 +1153,7 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="2"/>
+      <c r="A75" s="1"/>
       <c r="B75">
         <v>3093</v>
       </c>
@@ -1166,7 +1163,7 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="2"/>
+      <c r="A76" s="1"/>
       <c r="B76">
         <v>8805</v>
       </c>
@@ -1176,7 +1173,7 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="2"/>
+      <c r="A77" s="1"/>
       <c r="B77">
         <v>8158</v>
       </c>
@@ -1186,7 +1183,7 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="2"/>
+      <c r="A78" s="1"/>
       <c r="B78">
         <v>6499</v>
       </c>
@@ -1196,7 +1193,7 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B79">
@@ -1208,7 +1205,7 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="1"/>
       <c r="B80">
         <v>2217</v>
       </c>
@@ -1218,7 +1215,7 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="2"/>
+      <c r="A81" s="1"/>
       <c r="B81">
         <v>1824</v>
       </c>
@@ -1228,7 +1225,7 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="2"/>
+      <c r="A82" s="1"/>
       <c r="B82">
         <v>2564</v>
       </c>
@@ -1238,7 +1235,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="2"/>
+      <c r="A83" s="1"/>
       <c r="B83">
         <v>8487</v>
       </c>
@@ -1248,7 +1245,7 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="2"/>
+      <c r="A84" s="1"/>
       <c r="B84">
         <v>8045</v>
       </c>
@@ -1258,7 +1255,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="2"/>
+      <c r="A85" s="1"/>
       <c r="B85">
         <v>8878</v>
       </c>
@@ -1268,7 +1265,7 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="2"/>
+      <c r="A86" s="1"/>
       <c r="B86">
         <v>3072</v>
       </c>
@@ -1278,7 +1275,7 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="2"/>
+      <c r="A87" s="1"/>
       <c r="B87">
         <v>5980</v>
       </c>
@@ -1288,7 +1285,7 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="2"/>
+      <c r="A88" s="1"/>
       <c r="B88">
         <v>8174</v>
       </c>
@@ -1298,7 +1295,7 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="2"/>
+      <c r="A89" s="1"/>
       <c r="B89">
         <v>4257</v>
       </c>
@@ -1308,7 +1305,7 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="2"/>
+      <c r="A90" s="1"/>
       <c r="B90">
         <v>2291</v>
       </c>
@@ -1318,7 +1315,7 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="2"/>
+      <c r="A91" s="1"/>
       <c r="B91">
         <v>1763</v>
       </c>
@@ -1328,7 +1325,7 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="2"/>
+      <c r="A92" s="1"/>
       <c r="B92">
         <v>5662</v>
       </c>
@@ -1338,7 +1335,7 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="2"/>
+      <c r="A93" s="1"/>
       <c r="B93">
         <v>1945</v>
       </c>
@@ -1348,7 +1345,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="2"/>
+      <c r="A94" s="1"/>
       <c r="B94">
         <v>1186</v>
       </c>
@@ -1358,7 +1355,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="1"/>
       <c r="B95">
         <v>8715</v>
       </c>
@@ -1368,7 +1365,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="2"/>
+      <c r="A96" s="1"/>
       <c r="B96">
         <v>8518</v>
       </c>
@@ -1378,7 +1375,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="2"/>
+      <c r="A97" s="1"/>
       <c r="B97">
         <v>4847</v>
       </c>
@@ -1388,7 +1385,7 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="2"/>
+      <c r="A98" s="1"/>
       <c r="B98">
         <v>7991</v>
       </c>
@@ -1398,7 +1395,7 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="2"/>
+      <c r="A99" s="1"/>
       <c r="B99">
         <v>6291</v>
       </c>
@@ -1408,7 +1405,7 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="2"/>
+      <c r="A100" s="1"/>
       <c r="B100">
         <v>3770</v>
       </c>
@@ -1418,7 +1415,7 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="2"/>
+      <c r="A101" s="1"/>
       <c r="B101">
         <v>7178</v>
       </c>
@@ -1428,7 +1425,7 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="2"/>
+      <c r="A102" s="1"/>
       <c r="B102">
         <v>3883</v>
       </c>
@@ -1438,7 +1435,7 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="2"/>
+      <c r="A103" s="1"/>
       <c r="B103">
         <v>4527</v>
       </c>
@@ -1448,7 +1445,7 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="2"/>
+      <c r="A104" s="1"/>
       <c r="B104">
         <v>6556</v>
       </c>
@@ -1458,7 +1455,7 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="2"/>
+      <c r="A105" s="1"/>
       <c r="B105">
         <v>5635</v>
       </c>
@@ -1468,7 +1465,7 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="2"/>
+      <c r="A106" s="1"/>
       <c r="B106">
         <v>3878</v>
       </c>
@@ -1478,7 +1475,7 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="2"/>
+      <c r="A107" s="1"/>
       <c r="B107">
         <v>1217</v>
       </c>
@@ -1488,7 +1485,7 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="2"/>
+      <c r="A108" s="1"/>
       <c r="B108">
         <v>1438</v>
       </c>
@@ -1498,7 +1495,7 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="2"/>
+      <c r="A109" s="1"/>
       <c r="B109">
         <v>2153</v>
       </c>
@@ -1508,7 +1505,7 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="2"/>
+      <c r="A110" s="1"/>
       <c r="B110">
         <v>7937</v>
       </c>
@@ -1518,7 +1515,7 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="2"/>
+      <c r="A111" s="1"/>
       <c r="B111">
         <v>1999</v>
       </c>
@@ -1528,7 +1525,7 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="2"/>
+      <c r="A112" s="1"/>
       <c r="B112">
         <v>4042</v>
       </c>
@@ -1538,7 +1535,7 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="2"/>
+      <c r="A113" s="1"/>
       <c r="B113">
         <v>6351</v>
       </c>
@@ -1548,7 +1545,7 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="2"/>
+      <c r="A114" s="1"/>
       <c r="B114">
         <v>5382</v>
       </c>
@@ -1558,7 +1555,7 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="2"/>
+      <c r="A115" s="1"/>
       <c r="B115">
         <v>7088</v>
       </c>
@@ -1568,7 +1565,7 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="2"/>
+      <c r="A116" s="1"/>
       <c r="B116">
         <v>7250</v>
       </c>
@@ -1578,7 +1575,7 @@
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="2"/>
+      <c r="A117" s="1"/>
       <c r="B117">
         <v>6740</v>
       </c>
@@ -1588,7 +1585,7 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="2"/>
+      <c r="A118" s="1"/>
       <c r="B118">
         <v>9038</v>
       </c>
@@ -1598,7 +1595,7 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B119">
@@ -1610,7 +1607,7 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="2"/>
+      <c r="A120" s="1"/>
       <c r="B120">
         <v>8495</v>
       </c>
@@ -1620,7 +1617,7 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="2"/>
+      <c r="A121" s="1"/>
       <c r="B121">
         <v>1315</v>
       </c>
@@ -1630,7 +1627,7 @@
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="2"/>
+      <c r="A122" s="1"/>
       <c r="B122">
         <v>6066</v>
       </c>
@@ -1640,7 +1637,7 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="2"/>
+      <c r="A123" s="1"/>
       <c r="B123">
         <v>2565</v>
       </c>
@@ -1650,7 +1647,7 @@
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="2"/>
+      <c r="A124" s="1"/>
       <c r="B124">
         <v>2594</v>
       </c>
@@ -1660,7 +1657,7 @@
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="2"/>
+      <c r="A125" s="1"/>
       <c r="B125">
         <v>3762</v>
       </c>
@@ -1670,7 +1667,7 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="2"/>
+      <c r="A126" s="1"/>
       <c r="B126">
         <v>3550</v>
       </c>
@@ -1680,7 +1677,7 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="2"/>
+      <c r="A127" s="1"/>
       <c r="B127">
         <v>2475</v>
       </c>
@@ -1690,7 +1687,7 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="2"/>
+      <c r="A128" s="1"/>
       <c r="B128">
         <v>9180</v>
       </c>
@@ -1700,7 +1697,7 @@
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="2"/>
+      <c r="A129" s="1"/>
       <c r="B129">
         <v>1544</v>
       </c>
@@ -1710,7 +1707,7 @@
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="2"/>
+      <c r="A130" s="1"/>
       <c r="B130">
         <v>9562</v>
       </c>
@@ -1720,7 +1717,7 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="2"/>
+      <c r="A131" s="1"/>
       <c r="B131">
         <v>3669</v>
       </c>
@@ -1730,7 +1727,7 @@
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="2"/>
+      <c r="A132" s="1"/>
       <c r="B132">
         <v>5951</v>
       </c>
@@ -1740,7 +1737,7 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="2"/>
+      <c r="A133" s="1"/>
       <c r="B133">
         <v>2802</v>
       </c>
@@ -1750,7 +1747,7 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="2"/>
+      <c r="A134" s="1"/>
       <c r="B134">
         <v>6580</v>
       </c>
@@ -1760,7 +1757,7 @@
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="2"/>
+      <c r="A135" s="1"/>
       <c r="B135">
         <v>7585</v>
       </c>
@@ -1770,7 +1767,7 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="2"/>
+      <c r="A136" s="1"/>
       <c r="B136">
         <v>2321</v>
       </c>
@@ -1780,7 +1777,7 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="2"/>
+      <c r="A137" s="1"/>
       <c r="B137">
         <v>5053</v>
       </c>
@@ -1790,7 +1787,7 @@
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="2"/>
+      <c r="A138" s="1"/>
       <c r="B138">
         <v>3983</v>
       </c>
@@ -1800,7 +1797,7 @@
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="2"/>
+      <c r="A139" s="1"/>
       <c r="B139">
         <v>8770</v>
       </c>
@@ -1810,7 +1807,7 @@
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="2"/>
+      <c r="A140" s="1"/>
       <c r="B140">
         <v>4236</v>
       </c>
@@ -1820,7 +1817,7 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="2"/>
+      <c r="A141" s="1"/>
       <c r="B141">
         <v>5969</v>
       </c>
@@ -1830,7 +1827,7 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="2"/>
+      <c r="A142" s="1"/>
       <c r="B142">
         <v>8696</v>
       </c>
@@ -1840,7 +1837,7 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="2"/>
+      <c r="A143" s="1"/>
       <c r="B143">
         <v>8418</v>
       </c>
@@ -1850,7 +1847,7 @@
       </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="2"/>
+      <c r="A144" s="1"/>
       <c r="B144">
         <v>8395</v>
       </c>
@@ -1860,7 +1857,7 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="2"/>
+      <c r="A145" s="1"/>
       <c r="B145">
         <v>5170</v>
       </c>
@@ -1870,7 +1867,7 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="2"/>
+      <c r="A146" s="1"/>
       <c r="B146">
         <v>5568</v>
       </c>
@@ -1880,7 +1877,7 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="2"/>
+      <c r="A147" s="1"/>
       <c r="B147">
         <v>2592</v>
       </c>
@@ -1890,7 +1887,7 @@
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="2"/>
+      <c r="A148" s="1"/>
       <c r="B148">
         <v>4075</v>
       </c>
@@ -1900,7 +1897,7 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="2"/>
+      <c r="A149" s="1"/>
       <c r="B149">
         <v>7517</v>
       </c>
@@ -1910,7 +1907,7 @@
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="2"/>
+      <c r="A150" s="1"/>
       <c r="B150">
         <v>5448</v>
       </c>
@@ -1920,7 +1917,7 @@
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="2"/>
+      <c r="A151" s="1"/>
       <c r="B151">
         <v>6572</v>
       </c>
@@ -1930,7 +1927,7 @@
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="2"/>
+      <c r="A152" s="1"/>
       <c r="B152">
         <v>5238</v>
       </c>
@@ -1940,7 +1937,7 @@
       </c>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" s="2"/>
+      <c r="A153" s="1"/>
       <c r="B153">
         <v>2084</v>
       </c>
@@ -1950,7 +1947,7 @@
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="2"/>
+      <c r="A154" s="1"/>
       <c r="B154">
         <v>5411</v>
       </c>
@@ -1960,7 +1957,7 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="2"/>
+      <c r="A155" s="1"/>
       <c r="B155">
         <v>5171</v>
       </c>
@@ -1970,7 +1967,7 @@
       </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="2"/>
+      <c r="A156" s="1"/>
       <c r="B156">
         <v>1862</v>
       </c>
@@ -1980,7 +1977,7 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B157">
@@ -1992,7 +1989,7 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="2"/>
+      <c r="A158" s="1"/>
       <c r="B158">
         <v>9001</v>
       </c>
@@ -2002,7 +1999,7 @@
       </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="2"/>
+      <c r="A159" s="1"/>
       <c r="B159">
         <v>9631</v>
       </c>
@@ -2012,7 +2009,7 @@
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="2"/>
+      <c r="A160" s="1"/>
       <c r="B160">
         <v>9812</v>
       </c>
@@ -2022,7 +2019,7 @@
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="2"/>
+      <c r="A161" s="1"/>
       <c r="B161">
         <v>5728</v>
       </c>
@@ -2032,7 +2029,7 @@
       </c>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" s="2"/>
+      <c r="A162" s="1"/>
       <c r="B162">
         <v>1618</v>
       </c>
@@ -2042,7 +2039,7 @@
       </c>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" s="2"/>
+      <c r="A163" s="1"/>
       <c r="B163">
         <v>7491</v>
       </c>
@@ -2052,7 +2049,7 @@
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="2"/>
+      <c r="A164" s="1"/>
       <c r="B164">
         <v>5923</v>
       </c>
@@ -2062,7 +2059,7 @@
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="2"/>
+      <c r="A165" s="1"/>
       <c r="B165">
         <v>4265</v>
       </c>
@@ -2072,17 +2069,17 @@
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="2"/>
+      <c r="A166" s="1"/>
       <c r="B166">
         <v>2166</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:C237" ca="1" si="4">IF(B166=$E$1,1,0)</f>
+        <f t="shared" ref="C166:C239" ca="1" si="4">IF(B166=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="2"/>
+      <c r="A167" s="1"/>
       <c r="B167">
         <v>9116</v>
       </c>
@@ -2092,7 +2089,7 @@
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="2"/>
+      <c r="A168" s="1"/>
       <c r="B168">
         <v>9925</v>
       </c>
@@ -2102,7 +2099,7 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B169">
@@ -2114,7 +2111,7 @@
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="2"/>
+      <c r="A170" s="1"/>
       <c r="B170">
         <v>9931</v>
       </c>
@@ -2124,7 +2121,7 @@
       </c>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" s="2"/>
+      <c r="A171" s="1"/>
       <c r="B171">
         <v>4425</v>
       </c>
@@ -2134,7 +2131,7 @@
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="2"/>
+      <c r="A172" s="1"/>
       <c r="B172">
         <v>1947</v>
       </c>
@@ -2144,7 +2141,7 @@
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" s="2"/>
+      <c r="A173" s="1"/>
       <c r="B173">
         <v>9696</v>
       </c>
@@ -2154,7 +2151,7 @@
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="2"/>
+      <c r="A174" s="1"/>
       <c r="B174">
         <v>1223</v>
       </c>
@@ -2164,7 +2161,7 @@
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="2"/>
+      <c r="A175" s="1"/>
       <c r="B175">
         <v>3946</v>
       </c>
@@ -2174,7 +2171,7 @@
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="2"/>
+      <c r="A176" s="1"/>
       <c r="B176">
         <v>8311</v>
       </c>
@@ -2184,7 +2181,7 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="2"/>
+      <c r="A177" s="1"/>
       <c r="B177">
         <v>3134</v>
       </c>
@@ -2194,7 +2191,7 @@
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="2"/>
+      <c r="A178" s="1"/>
       <c r="B178">
         <v>9774</v>
       </c>
@@ -2204,7 +2201,7 @@
       </c>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="2"/>
+      <c r="A179" s="1"/>
       <c r="B179">
         <v>9711</v>
       </c>
@@ -2214,7 +2211,7 @@
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="2"/>
+      <c r="A180" s="1"/>
       <c r="B180">
         <v>3333</v>
       </c>
@@ -2224,7 +2221,7 @@
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="2"/>
+      <c r="A181" s="1"/>
       <c r="B181">
         <v>7290</v>
       </c>
@@ -2234,7 +2231,7 @@
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" s="2"/>
+      <c r="A182" s="1"/>
       <c r="B182">
         <v>5694</v>
       </c>
@@ -2244,7 +2241,7 @@
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="2"/>
+      <c r="A183" s="1"/>
       <c r="B183">
         <v>7035</v>
       </c>
@@ -2254,7 +2251,7 @@
       </c>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" s="2"/>
+      <c r="A184" s="1"/>
       <c r="B184">
         <v>6806</v>
       </c>
@@ -2264,7 +2261,7 @@
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="2"/>
+      <c r="A185" s="1"/>
       <c r="B185">
         <v>4515</v>
       </c>
@@ -2274,7 +2271,7 @@
       </c>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" s="2"/>
+      <c r="A186" s="1"/>
       <c r="B186">
         <v>9271</v>
       </c>
@@ -2284,7 +2281,7 @@
       </c>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" s="2"/>
+      <c r="A187" s="1"/>
       <c r="B187">
         <v>8769</v>
       </c>
@@ -2294,7 +2291,7 @@
       </c>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" s="2"/>
+      <c r="A188" s="1"/>
       <c r="B188">
         <v>4497</v>
       </c>
@@ -2304,7 +2301,7 @@
       </c>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" s="2"/>
+      <c r="A189" s="1"/>
       <c r="B189">
         <v>3940</v>
       </c>
@@ -2314,7 +2311,7 @@
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="2"/>
+      <c r="A190" s="1"/>
       <c r="B190">
         <v>8820</v>
       </c>
@@ -2324,7 +2321,7 @@
       </c>
     </row>
     <row r="191" spans="1:3">
-      <c r="A191" s="2"/>
+      <c r="A191" s="1"/>
       <c r="B191">
         <v>3218</v>
       </c>
@@ -2334,7 +2331,7 @@
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="2"/>
+      <c r="A192" s="1"/>
       <c r="B192">
         <v>4283</v>
       </c>
@@ -2344,7 +2341,7 @@
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="2"/>
+      <c r="A193" s="1"/>
       <c r="B193">
         <v>7703</v>
       </c>
@@ -2354,7 +2351,7 @@
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="2"/>
+      <c r="A194" s="1"/>
       <c r="B194">
         <v>9182</v>
       </c>
@@ -2364,7 +2361,7 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="2"/>
+      <c r="A195" s="1"/>
       <c r="B195">
         <v>5541</v>
       </c>
@@ -2374,7 +2371,7 @@
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="2"/>
+      <c r="A196" s="1"/>
       <c r="B196">
         <v>2386</v>
       </c>
@@ -2384,7 +2381,7 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="2"/>
+      <c r="A197" s="1"/>
       <c r="B197">
         <v>9159</v>
       </c>
@@ -2394,7 +2391,7 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B198">
@@ -2406,7 +2403,7 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="2"/>
+      <c r="A199" s="1"/>
       <c r="B199">
         <v>4642</v>
       </c>
@@ -2416,7 +2413,7 @@
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="2"/>
+      <c r="A200" s="1"/>
       <c r="B200">
         <v>4488</v>
       </c>
@@ -2426,7 +2423,7 @@
       </c>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="2"/>
+      <c r="A201" s="1"/>
       <c r="B201">
         <v>9765</v>
       </c>
@@ -2436,7 +2433,7 @@
       </c>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="2"/>
+      <c r="A202" s="1"/>
       <c r="B202">
         <v>4954</v>
       </c>
@@ -2446,7 +2443,7 @@
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="2"/>
+      <c r="A203" s="1"/>
       <c r="B203">
         <v>5537</v>
       </c>
@@ -2456,7 +2453,7 @@
       </c>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="2"/>
+      <c r="A204" s="1"/>
       <c r="B204">
         <v>6431</v>
       </c>
@@ -2466,7 +2463,7 @@
       </c>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="2"/>
+      <c r="A205" s="1"/>
       <c r="B205">
         <v>7193</v>
       </c>
@@ -2476,7 +2473,7 @@
       </c>
     </row>
     <row r="206" spans="1:3">
-      <c r="A206" s="2"/>
+      <c r="A206" s="1"/>
       <c r="B206">
         <v>5621</v>
       </c>
@@ -2486,7 +2483,7 @@
       </c>
     </row>
     <row r="207" spans="1:3">
-      <c r="A207" s="2"/>
+      <c r="A207" s="1"/>
       <c r="B207">
         <v>5847</v>
       </c>
@@ -2496,7 +2493,7 @@
       </c>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="2"/>
+      <c r="A208" s="1"/>
       <c r="B208">
         <v>4769</v>
       </c>
@@ -2506,7 +2503,7 @@
       </c>
     </row>
     <row r="209" spans="1:3">
-      <c r="A209" s="2"/>
+      <c r="A209" s="1"/>
       <c r="B209">
         <v>9930</v>
       </c>
@@ -2516,7 +2513,7 @@
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210" s="2"/>
+      <c r="A210" s="1"/>
       <c r="B210">
         <v>3226</v>
       </c>
@@ -2526,7 +2523,7 @@
       </c>
     </row>
     <row r="211" spans="1:3">
-      <c r="A211" s="2"/>
+      <c r="A211" s="1"/>
       <c r="B211">
         <v>6861</v>
       </c>
@@ -2536,7 +2533,7 @@
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="2"/>
+      <c r="A212" s="1"/>
       <c r="B212">
         <v>2205</v>
       </c>
@@ -2546,7 +2543,7 @@
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="2"/>
+      <c r="A213" s="1"/>
       <c r="B213">
         <v>4372</v>
       </c>
@@ -2556,7 +2553,7 @@
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="2"/>
+      <c r="A214" s="1"/>
       <c r="B214">
         <v>4463</v>
       </c>
@@ -2566,7 +2563,7 @@
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="2"/>
+      <c r="A215" s="1"/>
       <c r="B215">
         <v>1668</v>
       </c>
@@ -2576,7 +2573,7 @@
       </c>
     </row>
     <row r="216" spans="1:3">
-      <c r="A216" s="2"/>
+      <c r="A216" s="1"/>
       <c r="B216">
         <v>2137</v>
       </c>
@@ -2586,7 +2583,7 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="2" t="s">
+      <c r="A217" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B217">
@@ -2598,7 +2595,7 @@
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="2"/>
+      <c r="A218" s="1"/>
       <c r="B218">
         <v>3951</v>
       </c>
@@ -2608,7 +2605,7 @@
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="2"/>
+      <c r="A219" s="1"/>
       <c r="B219">
         <v>6409</v>
       </c>
@@ -2618,7 +2615,7 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="2"/>
+      <c r="A220" s="1"/>
       <c r="B220">
         <v>7343</v>
       </c>
@@ -2628,7 +2625,7 @@
       </c>
     </row>
     <row r="221" spans="1:3">
-      <c r="A221" s="2"/>
+      <c r="A221" s="1"/>
       <c r="B221">
         <v>7060</v>
       </c>
@@ -2638,7 +2635,7 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="2" t="s">
+      <c r="A222" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B222">
@@ -2650,7 +2647,7 @@
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="2"/>
+      <c r="A223" s="1"/>
       <c r="B223">
         <v>7560</v>
       </c>
@@ -2660,7 +2657,7 @@
       </c>
     </row>
     <row r="224" spans="1:3">
-      <c r="A224" s="2"/>
+      <c r="A224" s="1"/>
       <c r="B224">
         <v>9002</v>
       </c>
@@ -2670,7 +2667,7 @@
       </c>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="2"/>
+      <c r="A225" s="1"/>
       <c r="B225">
         <v>7432</v>
       </c>
@@ -2680,7 +2677,7 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="2"/>
+      <c r="A226" s="1"/>
       <c r="B226">
         <v>1954</v>
       </c>
@@ -2690,7 +2687,7 @@
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="2"/>
+      <c r="A227" s="1"/>
       <c r="B227">
         <v>2048</v>
       </c>
@@ -2700,7 +2697,7 @@
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="2" t="s">
+      <c r="A228" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B228">
@@ -2712,7 +2709,7 @@
       </c>
     </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="2"/>
+      <c r="A229" s="1"/>
       <c r="B229">
         <v>8861</v>
       </c>
@@ -2722,7 +2719,7 @@
       </c>
     </row>
     <row r="230" spans="1:3">
-      <c r="A230" s="2"/>
+      <c r="A230" s="1"/>
       <c r="B230">
         <v>1516</v>
       </c>
@@ -2732,7 +2729,7 @@
       </c>
     </row>
     <row r="231" spans="1:3">
-      <c r="A231" s="2"/>
+      <c r="A231" s="1"/>
       <c r="B231">
         <v>9062</v>
       </c>
@@ -2742,7 +2739,7 @@
       </c>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="2"/>
+      <c r="A232" s="1"/>
       <c r="B232">
         <v>5164</v>
       </c>
@@ -2754,7 +2751,7 @@
     <row r="233" spans="1:3">
       <c r="A233" s="1"/>
       <c r="B233">
-        <v>2354</v>
+        <v>2030</v>
       </c>
       <c r="C233">
         <f ca="1">IF(B233=$E$1,1,0)</f>
@@ -2762,31 +2759,31 @@
       </c>
     </row>
     <row r="234" spans="1:3">
-      <c r="A234" s="2" t="s">
+      <c r="A234" s="1"/>
+      <c r="B234">
+        <v>7649</v>
+      </c>
+      <c r="C234">
+        <f ca="1">IF(B234=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="1"/>
+      <c r="B235">
+        <v>2354</v>
+      </c>
+      <c r="C235">
+        <f ca="1">IF(B235=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B234">
+      <c r="B236">
         <v>8403</v>
-      </c>
-      <c r="C234">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="2"/>
-      <c r="B235">
-        <v>3185</v>
-      </c>
-      <c r="C235">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" s="2"/>
-      <c r="B236">
-        <v>9914</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="4"/>
@@ -2794,9 +2791,9 @@
       </c>
     </row>
     <row r="237" spans="1:3">
-      <c r="A237" s="2"/>
+      <c r="A237" s="1"/>
       <c r="B237">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="4"/>
@@ -2804,39 +2801,39 @@
       </c>
     </row>
     <row r="238" spans="1:3">
-      <c r="A238" s="2"/>
+      <c r="A238" s="1"/>
       <c r="B238">
+        <v>9914</v>
+      </c>
+      <c r="C238">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="1"/>
+      <c r="B239">
+        <v>6011</v>
+      </c>
+      <c r="C239">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="1"/>
+      <c r="B240">
         <v>6037</v>
       </c>
-      <c r="C238">
-        <f t="shared" ref="C238:C301" ca="1" si="5">IF(B238=$E$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" s="2"/>
-      <c r="B239">
+      <c r="C240">
+        <f t="shared" ref="C240:C303" ca="1" si="5">IF(B240=$E$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="1"/>
+      <c r="B241">
         <v>2809</v>
-      </c>
-      <c r="C239">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="2"/>
-      <c r="B240">
-        <v>7297</v>
-      </c>
-      <c r="C240">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241" s="2"/>
-      <c r="B241">
-        <v>5242</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2844,9 +2841,9 @@
       </c>
     </row>
     <row r="242" spans="1:3">
-      <c r="A242" s="2"/>
+      <c r="A242" s="1"/>
       <c r="B242">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2854,9 +2851,9 @@
       </c>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="2"/>
+      <c r="A243" s="1"/>
       <c r="B243">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2864,9 +2861,9 @@
       </c>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="2"/>
+      <c r="A244" s="1"/>
       <c r="B244">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="5"/>
@@ -2874,9 +2871,9 @@
       </c>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="2"/>
+      <c r="A245" s="1"/>
       <c r="B245">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="5"/>
@@ -2884,9 +2881,9 @@
       </c>
     </row>
     <row r="246" spans="1:3">
-      <c r="A246" s="2"/>
+      <c r="A246" s="1"/>
       <c r="B246">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="5"/>
@@ -2894,9 +2891,9 @@
       </c>
     </row>
     <row r="247" spans="1:3">
-      <c r="A247" s="2"/>
+      <c r="A247" s="1"/>
       <c r="B247">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
@@ -2904,9 +2901,9 @@
       </c>
     </row>
     <row r="248" spans="1:3">
-      <c r="A248" s="2"/>
+      <c r="A248" s="1"/>
       <c r="B248">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
@@ -2914,9 +2911,9 @@
       </c>
     </row>
     <row r="249" spans="1:3">
-      <c r="A249" s="2"/>
+      <c r="A249" s="1"/>
       <c r="B249">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="5"/>
@@ -2924,9 +2921,9 @@
       </c>
     </row>
     <row r="250" spans="1:3">
-      <c r="A250" s="2"/>
+      <c r="A250" s="1"/>
       <c r="B250">
-        <v>5463</v>
+        <v>1953</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="5"/>
@@ -2934,12 +2931,20 @@
       </c>
     </row>
     <row r="251" spans="1:3">
+      <c r="A251" s="1"/>
+      <c r="B251">
+        <v>3956</v>
+      </c>
       <c r="C251">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:3">
+      <c r="A252" s="1"/>
+      <c r="B252">
+        <v>5463</v>
+      </c>
       <c r="C252">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -3241,19 +3246,19 @@
     </row>
     <row r="302" spans="3:3">
       <c r="C302">
-        <f t="shared" ref="C302:C365" ca="1" si="6">IF(B302=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="303" spans="3:3">
       <c r="C303">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="304" spans="3:3">
       <c r="C304">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C304:C367" ca="1" si="6">IF(B304=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3625,19 +3630,19 @@
     </row>
     <row r="366" spans="3:3">
       <c r="C366">
-        <f t="shared" ref="C366:C429" ca="1" si="7">IF(B366=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="367" spans="3:3">
       <c r="C367">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="368" spans="3:3">
       <c r="C368">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C368:C431" ca="1" si="7">IF(B368=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4009,19 +4014,19 @@
     </row>
     <row r="430" spans="3:3">
       <c r="C430">
-        <f t="shared" ref="C430:C493" ca="1" si="8">IF(B430=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="431" spans="3:3">
       <c r="C431">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="432" spans="3:3">
       <c r="C432">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C432:C495" ca="1" si="8">IF(B432=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4393,19 +4398,19 @@
     </row>
     <row r="494" spans="3:3">
       <c r="C494">
-        <f t="shared" ref="C494:C557" ca="1" si="9">IF(B494=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="495" spans="3:3">
       <c r="C495">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="496" spans="3:3">
       <c r="C496">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C496:C559" ca="1" si="9">IF(B496=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4777,19 +4782,19 @@
     </row>
     <row r="558" spans="3:3">
       <c r="C558">
-        <f t="shared" ref="C558:C621" ca="1" si="10">IF(B558=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="559" spans="3:3">
       <c r="C559">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="560" spans="3:3">
       <c r="C560">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C560:C623" ca="1" si="10">IF(B560=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5161,19 +5166,19 @@
     </row>
     <row r="622" spans="3:3">
       <c r="C622">
-        <f t="shared" ref="C622:C685" ca="1" si="11">IF(B622=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="623" spans="3:3">
       <c r="C623">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="624" spans="3:3">
       <c r="C624">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C624:C687" ca="1" si="11">IF(B624=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5545,19 +5550,19 @@
     </row>
     <row r="686" spans="3:3">
       <c r="C686">
-        <f t="shared" ref="C686:C749" ca="1" si="12">IF(B686=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="3:3">
       <c r="C687">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="3:3">
       <c r="C688">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C688:C751" ca="1" si="12">IF(B688=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5929,19 +5934,19 @@
     </row>
     <row r="750" spans="3:3">
       <c r="C750">
-        <f t="shared" ref="C750:C813" ca="1" si="13">IF(B750=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="3:3">
       <c r="C751">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="3:3">
       <c r="C752">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C752:C815" ca="1" si="13">IF(B752=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6313,19 +6318,19 @@
     </row>
     <row r="814" spans="3:3">
       <c r="C814">
-        <f t="shared" ref="C814:C877" ca="1" si="14">IF(B814=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="3:3">
       <c r="C815">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="816" spans="3:3">
       <c r="C816">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C816:C879" ca="1" si="14">IF(B816=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6697,19 +6702,19 @@
     </row>
     <row r="878" spans="3:3">
       <c r="C878">
-        <f t="shared" ref="C878:C892" ca="1" si="15">IF(B878=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="879" spans="3:3">
       <c r="C879">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="880" spans="3:3">
       <c r="C880">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C880:C894" ca="1" si="15">IF(B880=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6785,11 +6790,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="893" spans="3:3">
+      <c r="C893">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="894" spans="3:3">
+      <c r="C894">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A222:A227"/>
-    <mergeCell ref="A228:A232"/>
-    <mergeCell ref="A234:A250"/>
+    <mergeCell ref="A236:A252"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
@@ -6800,6 +6816,7 @@
     <mergeCell ref="A169:A197"/>
     <mergeCell ref="A157:A168"/>
     <mergeCell ref="A119:A156"/>
+    <mergeCell ref="A228:A235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
error messages became more detailed. tasks were regrouped add tasks to lab about exceptions
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>лр1</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>лр14</t>
+  </si>
+  <si>
+    <t>лр13</t>
   </si>
 </sst>
 </file>
@@ -395,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E894"/>
+  <dimension ref="A1:E896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H229" sqref="H229"/>
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F231" sqref="F231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,7 +414,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9389</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2074,7 +2077,7 @@
         <v>2166</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:C239" ca="1" si="4">IF(B166=$E$1,1,0)</f>
+        <f t="shared" ref="C166:C241" ca="1" si="4">IF(B166=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2724,7 +2727,7 @@
         <v>1516</v>
       </c>
       <c r="C230">
-        <f ca="1">IF(B230=$E$1,1,0)</f>
+        <f t="shared" ref="C230:C237" ca="1" si="5">IF(B230=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2734,7 +2737,7 @@
         <v>9062</v>
       </c>
       <c r="C231">
-        <f ca="1">IF(B231=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2744,7 +2747,7 @@
         <v>5164</v>
       </c>
       <c r="C232">
-        <f ca="1">IF(B232=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2754,7 +2757,7 @@
         <v>2030</v>
       </c>
       <c r="C233">
-        <f ca="1">IF(B233=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2764,7 +2767,7 @@
         <v>7649</v>
       </c>
       <c r="C234">
-        <f ca="1">IF(B234=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2774,36 +2777,38 @@
         <v>2354</v>
       </c>
       <c r="C235">
-        <f ca="1">IF(B235=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B236">
-        <v>8403</v>
+        <v>9701</v>
       </c>
       <c r="C236">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>3185</v>
+        <v>6732</v>
       </c>
       <c r="C237">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3">
-      <c r="A238" s="1"/>
+      <c r="A238" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B238">
-        <v>9914</v>
+        <v>8403</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="4"/>
@@ -2813,7 +2818,7 @@
     <row r="239" spans="1:3">
       <c r="A239" s="1"/>
       <c r="B239">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="4"/>
@@ -2823,442 +2828,450 @@
     <row r="240" spans="1:3">
       <c r="A240" s="1"/>
       <c r="B240">
-        <v>6037</v>
+        <v>9914</v>
       </c>
       <c r="C240">
-        <f t="shared" ref="C240:C303" ca="1" si="5">IF(B240=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="1"/>
       <c r="B241">
-        <v>2809</v>
+        <v>6011</v>
       </c>
       <c r="C241">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="1"/>
       <c r="B242">
-        <v>7297</v>
+        <v>6037</v>
       </c>
       <c r="C242">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C242:C305" ca="1" si="6">IF(B242=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="1"/>
       <c r="B243">
-        <v>5242</v>
+        <v>2809</v>
       </c>
       <c r="C243">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1"/>
       <c r="B244">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C244">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C245">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="1"/>
       <c r="B246">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C246">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C247">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C248">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C249">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C250">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C251">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
+        <v>1953</v>
+      </c>
+      <c r="C252">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="1"/>
+      <c r="B253">
+        <v>3956</v>
+      </c>
+      <c r="C253">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="1"/>
+      <c r="B254">
         <v>5463</v>
       </c>
-      <c r="C252">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
-      <c r="C253">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
       <c r="C254">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="C255">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="C256">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="3:3">
       <c r="C257">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="258" spans="3:3">
       <c r="C258">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="259" spans="3:3">
       <c r="C259">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="3:3">
       <c r="C260">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="261" spans="3:3">
       <c r="C261">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="3:3">
       <c r="C262">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="3:3">
       <c r="C263">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="3:3">
       <c r="C264">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="3:3">
       <c r="C265">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="266" spans="3:3">
       <c r="C266">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="267" spans="3:3">
       <c r="C267">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="268" spans="3:3">
       <c r="C268">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="269" spans="3:3">
       <c r="C269">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="3:3">
       <c r="C270">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="271" spans="3:3">
       <c r="C271">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="272" spans="3:3">
       <c r="C272">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="273" spans="3:3">
       <c r="C273">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="274" spans="3:3">
       <c r="C274">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="275" spans="3:3">
       <c r="C275">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="276" spans="3:3">
       <c r="C276">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="277" spans="3:3">
       <c r="C277">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="278" spans="3:3">
       <c r="C278">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="279" spans="3:3">
       <c r="C279">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="3:3">
       <c r="C280">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="3:3">
       <c r="C281">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="282" spans="3:3">
       <c r="C282">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="283" spans="3:3">
       <c r="C283">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="284" spans="3:3">
       <c r="C284">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="285" spans="3:3">
       <c r="C285">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="286" spans="3:3">
       <c r="C286">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="287" spans="3:3">
       <c r="C287">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="288" spans="3:3">
       <c r="C288">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="289" spans="3:3">
       <c r="C289">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="290" spans="3:3">
       <c r="C290">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="291" spans="3:3">
       <c r="C291">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="292" spans="3:3">
       <c r="C292">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="293" spans="3:3">
       <c r="C293">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="294" spans="3:3">
       <c r="C294">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="295" spans="3:3">
       <c r="C295">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="296" spans="3:3">
       <c r="C296">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="297" spans="3:3">
       <c r="C297">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="298" spans="3:3">
       <c r="C298">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="3:3">
       <c r="C299">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="300" spans="3:3">
       <c r="C300">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="301" spans="3:3">
       <c r="C301">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="302" spans="3:3">
       <c r="C302">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="303" spans="3:3">
       <c r="C303">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="304" spans="3:3">
       <c r="C304">
-        <f t="shared" ref="C304:C367" ca="1" si="6">IF(B304=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3270,379 +3283,379 @@
     </row>
     <row r="306" spans="3:3">
       <c r="C306">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C306:C369" ca="1" si="7">IF(B306=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="3:3">
       <c r="C307">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="308" spans="3:3">
       <c r="C308">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="309" spans="3:3">
       <c r="C309">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="310" spans="3:3">
       <c r="C310">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="311" spans="3:3">
       <c r="C311">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="3:3">
       <c r="C312">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="313" spans="3:3">
       <c r="C313">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="3:3">
       <c r="C314">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="3:3">
       <c r="C315">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="316" spans="3:3">
       <c r="C316">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="317" spans="3:3">
       <c r="C317">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="318" spans="3:3">
       <c r="C318">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="319" spans="3:3">
       <c r="C319">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="320" spans="3:3">
       <c r="C320">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="3:3">
       <c r="C321">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="322" spans="3:3">
       <c r="C322">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="323" spans="3:3">
       <c r="C323">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="324" spans="3:3">
       <c r="C324">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="325" spans="3:3">
       <c r="C325">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="326" spans="3:3">
       <c r="C326">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="327" spans="3:3">
       <c r="C327">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="328" spans="3:3">
       <c r="C328">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="329" spans="3:3">
       <c r="C329">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="330" spans="3:3">
       <c r="C330">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="331" spans="3:3">
       <c r="C331">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="332" spans="3:3">
       <c r="C332">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="333" spans="3:3">
       <c r="C333">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="334" spans="3:3">
       <c r="C334">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="335" spans="3:3">
       <c r="C335">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="336" spans="3:3">
       <c r="C336">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="337" spans="3:3">
       <c r="C337">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="338" spans="3:3">
       <c r="C338">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="339" spans="3:3">
       <c r="C339">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="340" spans="3:3">
       <c r="C340">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="341" spans="3:3">
       <c r="C341">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="342" spans="3:3">
       <c r="C342">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="343" spans="3:3">
       <c r="C343">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="344" spans="3:3">
       <c r="C344">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="345" spans="3:3">
       <c r="C345">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="346" spans="3:3">
       <c r="C346">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="347" spans="3:3">
       <c r="C347">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="348" spans="3:3">
       <c r="C348">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="349" spans="3:3">
       <c r="C349">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="350" spans="3:3">
       <c r="C350">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="351" spans="3:3">
       <c r="C351">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="352" spans="3:3">
       <c r="C352">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="353" spans="3:3">
       <c r="C353">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="354" spans="3:3">
       <c r="C354">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="355" spans="3:3">
       <c r="C355">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="356" spans="3:3">
       <c r="C356">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="357" spans="3:3">
       <c r="C357">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="358" spans="3:3">
       <c r="C358">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="359" spans="3:3">
       <c r="C359">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="360" spans="3:3">
       <c r="C360">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="361" spans="3:3">
       <c r="C361">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="362" spans="3:3">
       <c r="C362">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="363" spans="3:3">
       <c r="C363">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="364" spans="3:3">
       <c r="C364">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="365" spans="3:3">
       <c r="C365">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="366" spans="3:3">
       <c r="C366">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="367" spans="3:3">
       <c r="C367">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="368" spans="3:3">
       <c r="C368">
-        <f t="shared" ref="C368:C431" ca="1" si="7">IF(B368=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3654,379 +3667,379 @@
     </row>
     <row r="370" spans="3:3">
       <c r="C370">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C370:C433" ca="1" si="8">IF(B370=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="371" spans="3:3">
       <c r="C371">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="372" spans="3:3">
       <c r="C372">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="373" spans="3:3">
       <c r="C373">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="374" spans="3:3">
       <c r="C374">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="375" spans="3:3">
       <c r="C375">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="376" spans="3:3">
       <c r="C376">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="377" spans="3:3">
       <c r="C377">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="378" spans="3:3">
       <c r="C378">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="379" spans="3:3">
       <c r="C379">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="380" spans="3:3">
       <c r="C380">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="381" spans="3:3">
       <c r="C381">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="382" spans="3:3">
       <c r="C382">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="383" spans="3:3">
       <c r="C383">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="384" spans="3:3">
       <c r="C384">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="385" spans="3:3">
       <c r="C385">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="386" spans="3:3">
       <c r="C386">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="387" spans="3:3">
       <c r="C387">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="388" spans="3:3">
       <c r="C388">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="389" spans="3:3">
       <c r="C389">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="390" spans="3:3">
       <c r="C390">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="391" spans="3:3">
       <c r="C391">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="392" spans="3:3">
       <c r="C392">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="393" spans="3:3">
       <c r="C393">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="394" spans="3:3">
       <c r="C394">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="395" spans="3:3">
       <c r="C395">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="396" spans="3:3">
       <c r="C396">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="397" spans="3:3">
       <c r="C397">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="398" spans="3:3">
       <c r="C398">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="399" spans="3:3">
       <c r="C399">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="400" spans="3:3">
       <c r="C400">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="401" spans="3:3">
       <c r="C401">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="402" spans="3:3">
       <c r="C402">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="403" spans="3:3">
       <c r="C403">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="404" spans="3:3">
       <c r="C404">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="405" spans="3:3">
       <c r="C405">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="406" spans="3:3">
       <c r="C406">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="407" spans="3:3">
       <c r="C407">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="408" spans="3:3">
       <c r="C408">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="409" spans="3:3">
       <c r="C409">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="410" spans="3:3">
       <c r="C410">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="411" spans="3:3">
       <c r="C411">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="412" spans="3:3">
       <c r="C412">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="413" spans="3:3">
       <c r="C413">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="414" spans="3:3">
       <c r="C414">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="415" spans="3:3">
       <c r="C415">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="416" spans="3:3">
       <c r="C416">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="417" spans="3:3">
       <c r="C417">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="418" spans="3:3">
       <c r="C418">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="419" spans="3:3">
       <c r="C419">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="420" spans="3:3">
       <c r="C420">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="421" spans="3:3">
       <c r="C421">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="422" spans="3:3">
       <c r="C422">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="423" spans="3:3">
       <c r="C423">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="424" spans="3:3">
       <c r="C424">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="425" spans="3:3">
       <c r="C425">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="426" spans="3:3">
       <c r="C426">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="427" spans="3:3">
       <c r="C427">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="428" spans="3:3">
       <c r="C428">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="429" spans="3:3">
       <c r="C429">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="430" spans="3:3">
       <c r="C430">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="431" spans="3:3">
       <c r="C431">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="432" spans="3:3">
       <c r="C432">
-        <f t="shared" ref="C432:C495" ca="1" si="8">IF(B432=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4038,379 +4051,379 @@
     </row>
     <row r="434" spans="3:3">
       <c r="C434">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C434:C497" ca="1" si="9">IF(B434=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="435" spans="3:3">
       <c r="C435">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="436" spans="3:3">
       <c r="C436">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="437" spans="3:3">
       <c r="C437">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="438" spans="3:3">
       <c r="C438">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="439" spans="3:3">
       <c r="C439">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="440" spans="3:3">
       <c r="C440">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="441" spans="3:3">
       <c r="C441">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="442" spans="3:3">
       <c r="C442">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="443" spans="3:3">
       <c r="C443">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="444" spans="3:3">
       <c r="C444">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="445" spans="3:3">
       <c r="C445">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="446" spans="3:3">
       <c r="C446">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="447" spans="3:3">
       <c r="C447">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="448" spans="3:3">
       <c r="C448">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="449" spans="3:3">
       <c r="C449">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="450" spans="3:3">
       <c r="C450">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="451" spans="3:3">
       <c r="C451">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="452" spans="3:3">
       <c r="C452">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="453" spans="3:3">
       <c r="C453">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="454" spans="3:3">
       <c r="C454">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="455" spans="3:3">
       <c r="C455">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="456" spans="3:3">
       <c r="C456">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="457" spans="3:3">
       <c r="C457">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="458" spans="3:3">
       <c r="C458">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="459" spans="3:3">
       <c r="C459">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="460" spans="3:3">
       <c r="C460">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="461" spans="3:3">
       <c r="C461">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="462" spans="3:3">
       <c r="C462">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="463" spans="3:3">
       <c r="C463">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="464" spans="3:3">
       <c r="C464">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="465" spans="3:3">
       <c r="C465">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="466" spans="3:3">
       <c r="C466">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="467" spans="3:3">
       <c r="C467">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="468" spans="3:3">
       <c r="C468">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="469" spans="3:3">
       <c r="C469">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="470" spans="3:3">
       <c r="C470">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="471" spans="3:3">
       <c r="C471">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="472" spans="3:3">
       <c r="C472">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="473" spans="3:3">
       <c r="C473">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="474" spans="3:3">
       <c r="C474">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="475" spans="3:3">
       <c r="C475">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="476" spans="3:3">
       <c r="C476">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="477" spans="3:3">
       <c r="C477">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="478" spans="3:3">
       <c r="C478">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="479" spans="3:3">
       <c r="C479">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="480" spans="3:3">
       <c r="C480">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="481" spans="3:3">
       <c r="C481">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="482" spans="3:3">
       <c r="C482">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="483" spans="3:3">
       <c r="C483">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="484" spans="3:3">
       <c r="C484">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="485" spans="3:3">
       <c r="C485">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="486" spans="3:3">
       <c r="C486">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="487" spans="3:3">
       <c r="C487">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="488" spans="3:3">
       <c r="C488">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="489" spans="3:3">
       <c r="C489">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="490" spans="3:3">
       <c r="C490">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="491" spans="3:3">
       <c r="C491">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="492" spans="3:3">
       <c r="C492">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="493" spans="3:3">
       <c r="C493">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="494" spans="3:3">
       <c r="C494">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="495" spans="3:3">
       <c r="C495">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="496" spans="3:3">
       <c r="C496">
-        <f t="shared" ref="C496:C559" ca="1" si="9">IF(B496=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4422,379 +4435,379 @@
     </row>
     <row r="498" spans="3:3">
       <c r="C498">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C498:C561" ca="1" si="10">IF(B498=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="499" spans="3:3">
       <c r="C499">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="500" spans="3:3">
       <c r="C500">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="501" spans="3:3">
       <c r="C501">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="502" spans="3:3">
       <c r="C502">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="503" spans="3:3">
       <c r="C503">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="504" spans="3:3">
       <c r="C504">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="505" spans="3:3">
       <c r="C505">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="506" spans="3:3">
       <c r="C506">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="507" spans="3:3">
       <c r="C507">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="508" spans="3:3">
       <c r="C508">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="509" spans="3:3">
       <c r="C509">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="510" spans="3:3">
       <c r="C510">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="511" spans="3:3">
       <c r="C511">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="512" spans="3:3">
       <c r="C512">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="513" spans="3:3">
       <c r="C513">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="514" spans="3:3">
       <c r="C514">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="515" spans="3:3">
       <c r="C515">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="516" spans="3:3">
       <c r="C516">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="517" spans="3:3">
       <c r="C517">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="518" spans="3:3">
       <c r="C518">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="519" spans="3:3">
       <c r="C519">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="520" spans="3:3">
       <c r="C520">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="521" spans="3:3">
       <c r="C521">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="522" spans="3:3">
       <c r="C522">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="523" spans="3:3">
       <c r="C523">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="524" spans="3:3">
       <c r="C524">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="525" spans="3:3">
       <c r="C525">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="526" spans="3:3">
       <c r="C526">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="527" spans="3:3">
       <c r="C527">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="528" spans="3:3">
       <c r="C528">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="529" spans="3:3">
       <c r="C529">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="530" spans="3:3">
       <c r="C530">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="531" spans="3:3">
       <c r="C531">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="532" spans="3:3">
       <c r="C532">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="533" spans="3:3">
       <c r="C533">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="534" spans="3:3">
       <c r="C534">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="535" spans="3:3">
       <c r="C535">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="536" spans="3:3">
       <c r="C536">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="537" spans="3:3">
       <c r="C537">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="538" spans="3:3">
       <c r="C538">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="539" spans="3:3">
       <c r="C539">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="540" spans="3:3">
       <c r="C540">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="541" spans="3:3">
       <c r="C541">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="542" spans="3:3">
       <c r="C542">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="543" spans="3:3">
       <c r="C543">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="544" spans="3:3">
       <c r="C544">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="545" spans="3:3">
       <c r="C545">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="546" spans="3:3">
       <c r="C546">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="547" spans="3:3">
       <c r="C547">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="548" spans="3:3">
       <c r="C548">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="3:3">
       <c r="C549">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="550" spans="3:3">
       <c r="C550">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="551" spans="3:3">
       <c r="C551">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="552" spans="3:3">
       <c r="C552">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="553" spans="3:3">
       <c r="C553">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="554" spans="3:3">
       <c r="C554">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="555" spans="3:3">
       <c r="C555">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="556" spans="3:3">
       <c r="C556">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="557" spans="3:3">
       <c r="C557">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="558" spans="3:3">
       <c r="C558">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="559" spans="3:3">
       <c r="C559">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="560" spans="3:3">
       <c r="C560">
-        <f t="shared" ref="C560:C623" ca="1" si="10">IF(B560=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4806,379 +4819,379 @@
     </row>
     <row r="562" spans="3:3">
       <c r="C562">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C562:C625" ca="1" si="11">IF(B562=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="563" spans="3:3">
       <c r="C563">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="564" spans="3:3">
       <c r="C564">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="565" spans="3:3">
       <c r="C565">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="566" spans="3:3">
       <c r="C566">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="567" spans="3:3">
       <c r="C567">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="568" spans="3:3">
       <c r="C568">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="569" spans="3:3">
       <c r="C569">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="570" spans="3:3">
       <c r="C570">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="571" spans="3:3">
       <c r="C571">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="572" spans="3:3">
       <c r="C572">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="573" spans="3:3">
       <c r="C573">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="574" spans="3:3">
       <c r="C574">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="575" spans="3:3">
       <c r="C575">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="576" spans="3:3">
       <c r="C576">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="577" spans="3:3">
       <c r="C577">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="578" spans="3:3">
       <c r="C578">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="579" spans="3:3">
       <c r="C579">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="580" spans="3:3">
       <c r="C580">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="581" spans="3:3">
       <c r="C581">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="582" spans="3:3">
       <c r="C582">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="583" spans="3:3">
       <c r="C583">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="584" spans="3:3">
       <c r="C584">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="585" spans="3:3">
       <c r="C585">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="586" spans="3:3">
       <c r="C586">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="587" spans="3:3">
       <c r="C587">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="588" spans="3:3">
       <c r="C588">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="589" spans="3:3">
       <c r="C589">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="590" spans="3:3">
       <c r="C590">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="591" spans="3:3">
       <c r="C591">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="592" spans="3:3">
       <c r="C592">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="593" spans="3:3">
       <c r="C593">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="594" spans="3:3">
       <c r="C594">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="595" spans="3:3">
       <c r="C595">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="596" spans="3:3">
       <c r="C596">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="597" spans="3:3">
       <c r="C597">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="598" spans="3:3">
       <c r="C598">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="599" spans="3:3">
       <c r="C599">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="600" spans="3:3">
       <c r="C600">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="601" spans="3:3">
       <c r="C601">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="602" spans="3:3">
       <c r="C602">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="603" spans="3:3">
       <c r="C603">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="604" spans="3:3">
       <c r="C604">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="605" spans="3:3">
       <c r="C605">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="606" spans="3:3">
       <c r="C606">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="607" spans="3:3">
       <c r="C607">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="608" spans="3:3">
       <c r="C608">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="609" spans="3:3">
       <c r="C609">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="610" spans="3:3">
       <c r="C610">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="611" spans="3:3">
       <c r="C611">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="612" spans="3:3">
       <c r="C612">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="613" spans="3:3">
       <c r="C613">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="614" spans="3:3">
       <c r="C614">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="615" spans="3:3">
       <c r="C615">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="616" spans="3:3">
       <c r="C616">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="617" spans="3:3">
       <c r="C617">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="618" spans="3:3">
       <c r="C618">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="619" spans="3:3">
       <c r="C619">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="620" spans="3:3">
       <c r="C620">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="621" spans="3:3">
       <c r="C621">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="3:3">
       <c r="C622">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="623" spans="3:3">
       <c r="C623">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="624" spans="3:3">
       <c r="C624">
-        <f t="shared" ref="C624:C687" ca="1" si="11">IF(B624=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5190,379 +5203,379 @@
     </row>
     <row r="626" spans="3:3">
       <c r="C626">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C626:C689" ca="1" si="12">IF(B626=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="627" spans="3:3">
       <c r="C627">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="628" spans="3:3">
       <c r="C628">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="629" spans="3:3">
       <c r="C629">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="630" spans="3:3">
       <c r="C630">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="631" spans="3:3">
       <c r="C631">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="632" spans="3:3">
       <c r="C632">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="633" spans="3:3">
       <c r="C633">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="3:3">
       <c r="C634">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="635" spans="3:3">
       <c r="C635">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="636" spans="3:3">
       <c r="C636">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="637" spans="3:3">
       <c r="C637">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="638" spans="3:3">
       <c r="C638">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="3:3">
       <c r="C639">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="3:3">
       <c r="C640">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="3:3">
       <c r="C641">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="3:3">
       <c r="C642">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="643" spans="3:3">
       <c r="C643">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="644" spans="3:3">
       <c r="C644">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="645" spans="3:3">
       <c r="C645">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="646" spans="3:3">
       <c r="C646">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="647" spans="3:3">
       <c r="C647">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="648" spans="3:3">
       <c r="C648">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="3:3">
       <c r="C649">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="3:3">
       <c r="C650">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="3:3">
       <c r="C651">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="3:3">
       <c r="C652">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="653" spans="3:3">
       <c r="C653">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="654" spans="3:3">
       <c r="C654">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="655" spans="3:3">
       <c r="C655">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="3:3">
       <c r="C656">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="657" spans="3:3">
       <c r="C657">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="3:3">
       <c r="C658">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="659" spans="3:3">
       <c r="C659">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="660" spans="3:3">
       <c r="C660">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="661" spans="3:3">
       <c r="C661">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="662" spans="3:3">
       <c r="C662">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="3:3">
       <c r="C663">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="3:3">
       <c r="C664">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="665" spans="3:3">
       <c r="C665">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="666" spans="3:3">
       <c r="C666">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="3:3">
       <c r="C667">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="3:3">
       <c r="C668">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="3:3">
       <c r="C669">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="3:3">
       <c r="C670">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="3:3">
       <c r="C671">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="3:3">
       <c r="C672">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="3:3">
       <c r="C673">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="674" spans="3:3">
       <c r="C674">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="675" spans="3:3">
       <c r="C675">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="3:3">
       <c r="C676">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="3:3">
       <c r="C677">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="678" spans="3:3">
       <c r="C678">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="679" spans="3:3">
       <c r="C679">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="680" spans="3:3">
       <c r="C680">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="681" spans="3:3">
       <c r="C681">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="682" spans="3:3">
       <c r="C682">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="683" spans="3:3">
       <c r="C683">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="684" spans="3:3">
       <c r="C684">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="3:3">
       <c r="C685">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="3:3">
       <c r="C686">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="3:3">
       <c r="C687">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="688" spans="3:3">
       <c r="C688">
-        <f t="shared" ref="C688:C751" ca="1" si="12">IF(B688=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -5574,379 +5587,379 @@
     </row>
     <row r="690" spans="3:3">
       <c r="C690">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C690:C753" ca="1" si="13">IF(B690=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="3:3">
       <c r="C691">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="3:3">
       <c r="C692">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="3:3">
       <c r="C693">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="3:3">
       <c r="C694">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="3:3">
       <c r="C695">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="3:3">
       <c r="C696">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="3:3">
       <c r="C697">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="3:3">
       <c r="C698">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="699" spans="3:3">
       <c r="C699">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="700" spans="3:3">
       <c r="C700">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="701" spans="3:3">
       <c r="C701">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="702" spans="3:3">
       <c r="C702">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="3:3">
       <c r="C703">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="3:3">
       <c r="C704">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="3:3">
       <c r="C705">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="3:3">
       <c r="C706">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="707" spans="3:3">
       <c r="C707">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="708" spans="3:3">
       <c r="C708">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="709" spans="3:3">
       <c r="C709">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="710" spans="3:3">
       <c r="C710">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="711" spans="3:3">
       <c r="C711">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="712" spans="3:3">
       <c r="C712">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="3:3">
       <c r="C713">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="3:3">
       <c r="C714">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="3:3">
       <c r="C715">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="3:3">
       <c r="C716">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="717" spans="3:3">
       <c r="C717">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="718" spans="3:3">
       <c r="C718">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="719" spans="3:3">
       <c r="C719">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="3:3">
       <c r="C720">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="721" spans="3:3">
       <c r="C721">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="3:3">
       <c r="C722">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="723" spans="3:3">
       <c r="C723">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="724" spans="3:3">
       <c r="C724">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="725" spans="3:3">
       <c r="C725">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="726" spans="3:3">
       <c r="C726">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="3:3">
       <c r="C727">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="3:3">
       <c r="C728">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="729" spans="3:3">
       <c r="C729">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="730" spans="3:3">
       <c r="C730">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="3:3">
       <c r="C731">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="3:3">
       <c r="C732">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="3:3">
       <c r="C733">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="3:3">
       <c r="C734">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="3:3">
       <c r="C735">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="3:3">
       <c r="C736">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="3:3">
       <c r="C737">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="738" spans="3:3">
       <c r="C738">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="739" spans="3:3">
       <c r="C739">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="3:3">
       <c r="C740">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="3:3">
       <c r="C741">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="742" spans="3:3">
       <c r="C742">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="743" spans="3:3">
       <c r="C743">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="744" spans="3:3">
       <c r="C744">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="745" spans="3:3">
       <c r="C745">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="746" spans="3:3">
       <c r="C746">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="747" spans="3:3">
       <c r="C747">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="748" spans="3:3">
       <c r="C748">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="3:3">
       <c r="C749">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="3:3">
       <c r="C750">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="3:3">
       <c r="C751">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="752" spans="3:3">
       <c r="C752">
-        <f t="shared" ref="C752:C815" ca="1" si="13">IF(B752=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5958,379 +5971,379 @@
     </row>
     <row r="754" spans="3:3">
       <c r="C754">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C754:C817" ca="1" si="14">IF(B754=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="3:3">
       <c r="C755">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="3:3">
       <c r="C756">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="3:3">
       <c r="C757">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="3:3">
       <c r="C758">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="3:3">
       <c r="C759">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="3:3">
       <c r="C760">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="3:3">
       <c r="C761">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="3:3">
       <c r="C762">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="763" spans="3:3">
       <c r="C763">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="764" spans="3:3">
       <c r="C764">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="765" spans="3:3">
       <c r="C765">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="766" spans="3:3">
       <c r="C766">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="3:3">
       <c r="C767">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="3:3">
       <c r="C768">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="3:3">
       <c r="C769">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="3:3">
       <c r="C770">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="771" spans="3:3">
       <c r="C771">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="772" spans="3:3">
       <c r="C772">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="773" spans="3:3">
       <c r="C773">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="774" spans="3:3">
       <c r="C774">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="775" spans="3:3">
       <c r="C775">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="776" spans="3:3">
       <c r="C776">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="3:3">
       <c r="C777">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="3:3">
       <c r="C778">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="3:3">
       <c r="C779">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="3:3">
       <c r="C780">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="781" spans="3:3">
       <c r="C781">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="782" spans="3:3">
       <c r="C782">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="783" spans="3:3">
       <c r="C783">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="3:3">
       <c r="C784">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="785" spans="3:3">
       <c r="C785">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="3:3">
       <c r="C786">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="787" spans="3:3">
       <c r="C787">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="788" spans="3:3">
       <c r="C788">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="789" spans="3:3">
       <c r="C789">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="790" spans="3:3">
       <c r="C790">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="3:3">
       <c r="C791">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="3:3">
       <c r="C792">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="793" spans="3:3">
       <c r="C793">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="794" spans="3:3">
       <c r="C794">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="3:3">
       <c r="C795">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="3:3">
       <c r="C796">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="3:3">
       <c r="C797">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="798" spans="3:3">
       <c r="C798">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="799" spans="3:3">
       <c r="C799">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="3:3">
       <c r="C800">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="3:3">
       <c r="C801">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="802" spans="3:3">
       <c r="C802">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="803" spans="3:3">
       <c r="C803">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="804" spans="3:3">
       <c r="C804">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="3:3">
       <c r="C805">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="806" spans="3:3">
       <c r="C806">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="807" spans="3:3">
       <c r="C807">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="808" spans="3:3">
       <c r="C808">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="809" spans="3:3">
       <c r="C809">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="810" spans="3:3">
       <c r="C810">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="811" spans="3:3">
       <c r="C811">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="812" spans="3:3">
       <c r="C812">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="3:3">
       <c r="C813">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="814" spans="3:3">
       <c r="C814">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="3:3">
       <c r="C815">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="816" spans="3:3">
       <c r="C816">
-        <f t="shared" ref="C816:C879" ca="1" si="14">IF(B816=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -6342,379 +6355,379 @@
     </row>
     <row r="818" spans="3:3">
       <c r="C818">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C818:C881" ca="1" si="15">IF(B818=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="819" spans="3:3">
       <c r="C819">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="820" spans="3:3">
       <c r="C820">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="821" spans="3:3">
       <c r="C821">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="822" spans="3:3">
       <c r="C822">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="823" spans="3:3">
       <c r="C823">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="824" spans="3:3">
       <c r="C824">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="825" spans="3:3">
       <c r="C825">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="826" spans="3:3">
       <c r="C826">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="827" spans="3:3">
       <c r="C827">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="828" spans="3:3">
       <c r="C828">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="829" spans="3:3">
       <c r="C829">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="830" spans="3:3">
       <c r="C830">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="831" spans="3:3">
       <c r="C831">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="832" spans="3:3">
       <c r="C832">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="833" spans="3:3">
       <c r="C833">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="834" spans="3:3">
       <c r="C834">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="835" spans="3:3">
       <c r="C835">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="836" spans="3:3">
       <c r="C836">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="837" spans="3:3">
       <c r="C837">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="838" spans="3:3">
       <c r="C838">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="839" spans="3:3">
       <c r="C839">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="840" spans="3:3">
       <c r="C840">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="841" spans="3:3">
       <c r="C841">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="842" spans="3:3">
       <c r="C842">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="843" spans="3:3">
       <c r="C843">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="844" spans="3:3">
       <c r="C844">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="845" spans="3:3">
       <c r="C845">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="846" spans="3:3">
       <c r="C846">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="847" spans="3:3">
       <c r="C847">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="848" spans="3:3">
       <c r="C848">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="849" spans="3:3">
       <c r="C849">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="850" spans="3:3">
       <c r="C850">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="851" spans="3:3">
       <c r="C851">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="852" spans="3:3">
       <c r="C852">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="853" spans="3:3">
       <c r="C853">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="854" spans="3:3">
       <c r="C854">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="855" spans="3:3">
       <c r="C855">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="856" spans="3:3">
       <c r="C856">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="857" spans="3:3">
       <c r="C857">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="858" spans="3:3">
       <c r="C858">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="859" spans="3:3">
       <c r="C859">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="860" spans="3:3">
       <c r="C860">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="861" spans="3:3">
       <c r="C861">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="862" spans="3:3">
       <c r="C862">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="863" spans="3:3">
       <c r="C863">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="864" spans="3:3">
       <c r="C864">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="865" spans="3:3">
       <c r="C865">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="866" spans="3:3">
       <c r="C866">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="867" spans="3:3">
       <c r="C867">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="868" spans="3:3">
       <c r="C868">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="869" spans="3:3">
       <c r="C869">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="870" spans="3:3">
       <c r="C870">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="871" spans="3:3">
       <c r="C871">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="872" spans="3:3">
       <c r="C872">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="873" spans="3:3">
       <c r="C873">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="874" spans="3:3">
       <c r="C874">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="875" spans="3:3">
       <c r="C875">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="876" spans="3:3">
       <c r="C876">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="877" spans="3:3">
       <c r="C877">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="878" spans="3:3">
       <c r="C878">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="879" spans="3:3">
       <c r="C879">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="880" spans="3:3">
       <c r="C880">
-        <f t="shared" ref="C880:C894" ca="1" si="15">IF(B880=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6726,86 +6739,98 @@
     </row>
     <row r="882" spans="3:3">
       <c r="C882">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C882:C896" ca="1" si="16">IF(B882=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="883" spans="3:3">
       <c r="C883">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="884" spans="3:3">
       <c r="C884">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="885" spans="3:3">
       <c r="C885">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="886" spans="3:3">
       <c r="C886">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="887" spans="3:3">
       <c r="C887">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="888" spans="3:3">
       <c r="C888">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="889" spans="3:3">
       <c r="C889">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="890" spans="3:3">
       <c r="C890">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="891" spans="3:3">
       <c r="C891">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="892" spans="3:3">
       <c r="C892">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="893" spans="3:3">
       <c r="C893">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="894" spans="3:3">
       <c r="C894">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="895" spans="3:3">
+      <c r="C895">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="896" spans="3:3">
+      <c r="C896">
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A222:A227"/>
-    <mergeCell ref="A236:A252"/>
+    <mergeCell ref="A238:A254"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
@@ -6817,6 +6842,7 @@
     <mergeCell ref="A157:A168"/>
     <mergeCell ref="A119:A156"/>
     <mergeCell ref="A228:A235"/>
+    <mergeCell ref="A236:A237"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rewrite all error messages regroup tasks in java solution add task to lab13
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -398,11 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E896"/>
+  <dimension ref="A1:E897"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F231" sqref="F231"/>
+      <selection pane="bottomLeft" activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>4012</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2077,7 +2077,7 @@
         <v>2166</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:C241" ca="1" si="4">IF(B166=$E$1,1,0)</f>
+        <f t="shared" ref="C166:C242" ca="1" si="4">IF(B166=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2727,7 +2727,7 @@
         <v>1516</v>
       </c>
       <c r="C230">
-        <f t="shared" ref="C230:C237" ca="1" si="5">IF(B230=$E$1,1,0)</f>
+        <f t="shared" ref="C230:C238" ca="1" si="5">IF(B230=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2796,7 +2796,7 @@
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2804,21 +2804,21 @@
       </c>
     </row>
     <row r="238" spans="1:3">
-      <c r="A238" s="1" t="s">
+      <c r="A238" s="1"/>
+      <c r="B238">
+        <v>6732</v>
+      </c>
+      <c r="C238">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B238">
+      <c r="B239">
         <v>8403</v>
-      </c>
-      <c r="C238">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" s="1"/>
-      <c r="B239">
-        <v>3185</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="4"/>
@@ -2828,7 +2828,7 @@
     <row r="240" spans="1:3">
       <c r="A240" s="1"/>
       <c r="B240">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="4"/>
@@ -2838,7 +2838,7 @@
     <row r="241" spans="1:3">
       <c r="A241" s="1"/>
       <c r="B241">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="4"/>
@@ -2848,27 +2848,27 @@
     <row r="242" spans="1:3">
       <c r="A242" s="1"/>
       <c r="B242">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C242">
-        <f t="shared" ref="C242:C305" ca="1" si="6">IF(B242=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="1"/>
       <c r="B243">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C243">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C243:C306" ca="1" si="6">IF(B243=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1"/>
       <c r="B244">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="6"/>
@@ -2878,7 +2878,7 @@
     <row r="245" spans="1:3">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="6"/>
@@ -2888,7 +2888,7 @@
     <row r="246" spans="1:3">
       <c r="A246" s="1"/>
       <c r="B246">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="6"/>
@@ -2898,7 +2898,7 @@
     <row r="247" spans="1:3">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="6"/>
@@ -2908,7 +2908,7 @@
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="6"/>
@@ -2918,7 +2918,7 @@
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="6"/>
@@ -2928,7 +2928,7 @@
     <row r="250" spans="1:3">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="6"/>
@@ -2938,7 +2938,7 @@
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>4147</v>
+        <v>2000</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="6"/>
@@ -2948,7 +2948,7 @@
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="6"/>
@@ -2958,7 +2958,7 @@
     <row r="253" spans="1:3">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="6"/>
@@ -2968,7 +2968,7 @@
     <row r="254" spans="1:3">
       <c r="A254" s="1"/>
       <c r="B254">
-        <v>5463</v>
+        <v>3956</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="6"/>
@@ -2976,6 +2976,10 @@
       </c>
     </row>
     <row r="255" spans="1:3">
+      <c r="A255" s="1"/>
+      <c r="B255">
+        <v>5463</v>
+      </c>
       <c r="C255">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3283,13 +3287,13 @@
     </row>
     <row r="306" spans="3:3">
       <c r="C306">
-        <f t="shared" ref="C306:C369" ca="1" si="7">IF(B306=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="3:3">
       <c r="C307">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C307:C370" ca="1" si="7">IF(B307=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3667,13 +3671,13 @@
     </row>
     <row r="370" spans="3:3">
       <c r="C370">
-        <f t="shared" ref="C370:C433" ca="1" si="8">IF(B370=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="371" spans="3:3">
       <c r="C371">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C371:C434" ca="1" si="8">IF(B371=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4051,13 +4055,13 @@
     </row>
     <row r="434" spans="3:3">
       <c r="C434">
-        <f t="shared" ref="C434:C497" ca="1" si="9">IF(B434=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="435" spans="3:3">
       <c r="C435">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C435:C498" ca="1" si="9">IF(B435=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4435,13 +4439,13 @@
     </row>
     <row r="498" spans="3:3">
       <c r="C498">
-        <f t="shared" ref="C498:C561" ca="1" si="10">IF(B498=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="499" spans="3:3">
       <c r="C499">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C499:C562" ca="1" si="10">IF(B499=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4819,13 +4823,13 @@
     </row>
     <row r="562" spans="3:3">
       <c r="C562">
-        <f t="shared" ref="C562:C625" ca="1" si="11">IF(B562=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="563" spans="3:3">
       <c r="C563">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C563:C626" ca="1" si="11">IF(B563=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5203,13 +5207,13 @@
     </row>
     <row r="626" spans="3:3">
       <c r="C626">
-        <f t="shared" ref="C626:C689" ca="1" si="12">IF(B626=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="627" spans="3:3">
       <c r="C627">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C627:C690" ca="1" si="12">IF(B627=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5587,13 +5591,13 @@
     </row>
     <row r="690" spans="3:3">
       <c r="C690">
-        <f t="shared" ref="C690:C753" ca="1" si="13">IF(B690=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="691" spans="3:3">
       <c r="C691">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C691:C754" ca="1" si="13">IF(B691=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5971,13 +5975,13 @@
     </row>
     <row r="754" spans="3:3">
       <c r="C754">
-        <f t="shared" ref="C754:C817" ca="1" si="14">IF(B754=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="755" spans="3:3">
       <c r="C755">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C755:C818" ca="1" si="14">IF(B755=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6355,13 +6359,13 @@
     </row>
     <row r="818" spans="3:3">
       <c r="C818">
-        <f t="shared" ref="C818:C881" ca="1" si="15">IF(B818=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="819" spans="3:3">
       <c r="C819">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C819:C882" ca="1" si="15">IF(B819=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6739,13 +6743,13 @@
     </row>
     <row r="882" spans="3:3">
       <c r="C882">
-        <f t="shared" ref="C882:C896" ca="1" si="16">IF(B882=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="883" spans="3:3">
       <c r="C883">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C883:C897" ca="1" si="16">IF(B883=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6827,10 +6831,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="897" spans="3:3">
+      <c r="C897">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A222:A227"/>
-    <mergeCell ref="A238:A254"/>
+    <mergeCell ref="A239:A255"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
@@ -6842,7 +6852,7 @@
     <mergeCell ref="A157:A168"/>
     <mergeCell ref="A119:A156"/>
     <mergeCell ref="A228:A235"/>
-    <mergeCell ref="A236:A237"/>
+    <mergeCell ref="A236:A238"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
solve lab08 in csharp. rename files in solution to reflect lab number make tasks for lab12,13,15 for csharp remove some labs from navigation. I'm not sure whether I need to keep them or not.
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>лр1</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>лр13</t>
+  </si>
+  <si>
+    <t>лр15</t>
   </si>
 </sst>
 </file>
@@ -401,8 +404,8 @@
   <dimension ref="A1:E897"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B238" sqref="B238"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F259" sqref="F259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -414,7 +417,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>1708</v>
+        <v>7169</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2986,6 +2989,12 @@
       </c>
     </row>
     <row r="256" spans="1:3">
+      <c r="A256" t="s">
+        <v>14</v>
+      </c>
+      <c r="B256">
+        <v>8787</v>
+      </c>
       <c r="C256">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>

</xml_diff>

<commit_message>
add more tasks to lab10 add pictures to some sophisticated tasks in lab05 change task 9020 move task with random generation of numbers to lab10 mark tasks as "example" or "supervision" classes in nav
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -401,11 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E897"/>
+  <dimension ref="A1:E901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F259" sqref="F259"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,7 +417,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7169</v>
+        <v>3349</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2080,7 +2080,7 @@
         <v>2166</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:C242" ca="1" si="4">IF(B166=$E$1,1,0)</f>
+        <f t="shared" ref="C166:C246" ca="1" si="4">IF(B166=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2352,7 +2352,7 @@
         <v>7703</v>
       </c>
       <c r="C193">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B193=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2623,7 +2623,7 @@
     <row r="220" spans="1:3">
       <c r="A220" s="1"/>
       <c r="B220">
-        <v>7343</v>
+        <v>3290</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2633,7 +2633,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="1"/>
       <c r="B221">
-        <v>7060</v>
+        <v>5309</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2641,11 +2641,9 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A222" s="1"/>
       <c r="B222">
-        <v>9299</v>
+        <v>5345</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2655,7 +2653,7 @@
     <row r="223" spans="1:3">
       <c r="A223" s="1"/>
       <c r="B223">
-        <v>7560</v>
+        <v>6812</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2665,7 +2663,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="1"/>
       <c r="B224">
-        <v>9002</v>
+        <v>7343</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2675,7 +2673,7 @@
     <row r="225" spans="1:3">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>7432</v>
+        <v>7060</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2683,9 +2681,11 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="1"/>
+      <c r="A226" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B226">
-        <v>1954</v>
+        <v>9299</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2695,7 +2695,7 @@
     <row r="227" spans="1:3">
       <c r="A227" s="1"/>
       <c r="B227">
-        <v>2048</v>
+        <v>7560</v>
       </c>
       <c r="C227">
         <f t="shared" ca="1" si="4"/>
@@ -2703,11 +2703,9 @@
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A228" s="1"/>
       <c r="B228">
-        <v>3939</v>
+        <v>9002</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="4"/>
@@ -2717,7 +2715,7 @@
     <row r="229" spans="1:3">
       <c r="A229" s="1"/>
       <c r="B229">
-        <v>8861</v>
+        <v>7432</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="4"/>
@@ -2727,57 +2725,59 @@
     <row r="230" spans="1:3">
       <c r="A230" s="1"/>
       <c r="B230">
-        <v>1516</v>
+        <v>1954</v>
       </c>
       <c r="C230">
-        <f t="shared" ref="C230:C238" ca="1" si="5">IF(B230=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="1"/>
       <c r="B231">
-        <v>9062</v>
+        <v>2048</v>
       </c>
       <c r="C231">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="1"/>
+      <c r="A232" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B232">
-        <v>5164</v>
+        <v>3939</v>
       </c>
       <c r="C232">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="1"/>
       <c r="B233">
-        <v>2030</v>
+        <v>8861</v>
       </c>
       <c r="C233">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="1"/>
       <c r="B234">
-        <v>7649</v>
+        <v>1516</v>
       </c>
       <c r="C234">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C234:C242" ca="1" si="5">IF(B234=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="1"/>
       <c r="B235">
-        <v>2354</v>
+        <v>9062</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="5"/>
@@ -2785,11 +2785,9 @@
       </c>
     </row>
     <row r="236" spans="1:3">
-      <c r="A236" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A236" s="1"/>
       <c r="B236">
-        <v>9701</v>
+        <v>5164</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2799,7 +2797,7 @@
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>3784</v>
+        <v>2030</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2809,7 +2807,7 @@
     <row r="238" spans="1:3">
       <c r="A238" s="1"/>
       <c r="B238">
-        <v>6732</v>
+        <v>7649</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2817,101 +2815,103 @@
       </c>
     </row>
     <row r="239" spans="1:3">
-      <c r="A239" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A239" s="1"/>
       <c r="B239">
-        <v>8403</v>
+        <v>2354</v>
       </c>
       <c r="C239">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:3">
-      <c r="A240" s="1"/>
+      <c r="A240" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B240">
-        <v>3185</v>
+        <v>9701</v>
       </c>
       <c r="C240">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="1"/>
       <c r="B241">
-        <v>9914</v>
+        <v>3784</v>
       </c>
       <c r="C241">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="1"/>
       <c r="B242">
-        <v>6011</v>
+        <v>6732</v>
       </c>
       <c r="C242">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B243">
+        <v>8403</v>
+      </c>
+      <c r="C243">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" s="1"/>
-      <c r="B243">
-        <v>6037</v>
-      </c>
-      <c r="C243">
-        <f t="shared" ref="C243:C306" ca="1" si="6">IF(B243=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1"/>
       <c r="B244">
-        <v>2809</v>
+        <v>3185</v>
       </c>
       <c r="C244">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>7297</v>
+        <v>9914</v>
       </c>
       <c r="C245">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="1"/>
       <c r="B246">
-        <v>5242</v>
+        <v>6011</v>
       </c>
       <c r="C246">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>1379</v>
+        <v>6037</v>
       </c>
       <c r="C247">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C247:C310" ca="1" si="6">IF(B247=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>2401</v>
+        <v>2809</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="6"/>
@@ -2921,7 +2921,7 @@
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>5421</v>
+        <v>7297</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="6"/>
@@ -2931,7 +2931,7 @@
     <row r="250" spans="1:3">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>7301</v>
+        <v>5242</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="6"/>
@@ -2941,7 +2941,7 @@
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>2000</v>
+        <v>1379</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="6"/>
@@ -2951,7 +2951,7 @@
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
-        <v>4147</v>
+        <v>2401</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="6"/>
@@ -2961,7 +2961,7 @@
     <row r="253" spans="1:3">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>1953</v>
+        <v>5421</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="6"/>
@@ -2971,7 +2971,7 @@
     <row r="254" spans="1:3">
       <c r="A254" s="1"/>
       <c r="B254">
-        <v>3956</v>
+        <v>7301</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="6"/>
@@ -2981,7 +2981,7 @@
     <row r="255" spans="1:3">
       <c r="A255" s="1"/>
       <c r="B255">
-        <v>5463</v>
+        <v>2000</v>
       </c>
       <c r="C255">
         <f t="shared" ca="1" si="6"/>
@@ -2989,108 +2989,124 @@
       </c>
     </row>
     <row r="256" spans="1:3">
-      <c r="A256" t="s">
-        <v>14</v>
-      </c>
+      <c r="A256" s="1"/>
       <c r="B256">
-        <v>8787</v>
+        <v>4147</v>
       </c>
       <c r="C256">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="3:3">
+    <row r="257" spans="1:3">
+      <c r="A257" s="1"/>
+      <c r="B257">
+        <v>1953</v>
+      </c>
       <c r="C257">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="3:3">
+    <row r="258" spans="1:3">
+      <c r="A258" s="1"/>
+      <c r="B258">
+        <v>3956</v>
+      </c>
       <c r="C258">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="3:3">
+    <row r="259" spans="1:3">
+      <c r="A259" s="1"/>
+      <c r="B259">
+        <v>5463</v>
+      </c>
       <c r="C259">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="3:3">
+    <row r="260" spans="1:3">
+      <c r="A260" t="s">
+        <v>14</v>
+      </c>
+      <c r="B260">
+        <v>8787</v>
+      </c>
       <c r="C260">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="3:3">
+    <row r="261" spans="1:3">
       <c r="C261">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="3:3">
+    <row r="262" spans="1:3">
       <c r="C262">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="3:3">
+    <row r="263" spans="1:3">
       <c r="C263">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="3:3">
+    <row r="264" spans="1:3">
       <c r="C264">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="3:3">
+    <row r="265" spans="1:3">
       <c r="C265">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="3:3">
+    <row r="266" spans="1:3">
       <c r="C266">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="3:3">
+    <row r="267" spans="1:3">
       <c r="C267">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="3:3">
+    <row r="268" spans="1:3">
       <c r="C268">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="3:3">
+    <row r="269" spans="1:3">
       <c r="C269">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="3:3">
+    <row r="270" spans="1:3">
       <c r="C270">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="3:3">
+    <row r="271" spans="1:3">
       <c r="C271">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="3:3">
+    <row r="272" spans="1:3">
       <c r="C272">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3302,31 +3318,31 @@
     </row>
     <row r="307" spans="3:3">
       <c r="C307">
-        <f t="shared" ref="C307:C370" ca="1" si="7">IF(B307=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="308" spans="3:3">
       <c r="C308">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="309" spans="3:3">
       <c r="C309">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="310" spans="3:3">
       <c r="C310">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="311" spans="3:3">
       <c r="C311">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C311:C374" ca="1" si="7">IF(B311=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3686,31 +3702,31 @@
     </row>
     <row r="371" spans="3:3">
       <c r="C371">
-        <f t="shared" ref="C371:C434" ca="1" si="8">IF(B371=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="372" spans="3:3">
       <c r="C372">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="373" spans="3:3">
       <c r="C373">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="374" spans="3:3">
       <c r="C374">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="375" spans="3:3">
       <c r="C375">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C375:C438" ca="1" si="8">IF(B375=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4070,31 +4086,31 @@
     </row>
     <row r="435" spans="3:3">
       <c r="C435">
-        <f t="shared" ref="C435:C498" ca="1" si="9">IF(B435=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="436" spans="3:3">
       <c r="C436">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="437" spans="3:3">
       <c r="C437">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="438" spans="3:3">
       <c r="C438">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="439" spans="3:3">
       <c r="C439">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C439:C502" ca="1" si="9">IF(B439=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4454,31 +4470,31 @@
     </row>
     <row r="499" spans="3:3">
       <c r="C499">
-        <f t="shared" ref="C499:C562" ca="1" si="10">IF(B499=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="500" spans="3:3">
       <c r="C500">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="501" spans="3:3">
       <c r="C501">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="502" spans="3:3">
       <c r="C502">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="503" spans="3:3">
       <c r="C503">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C503:C566" ca="1" si="10">IF(B503=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4838,31 +4854,31 @@
     </row>
     <row r="563" spans="3:3">
       <c r="C563">
-        <f t="shared" ref="C563:C626" ca="1" si="11">IF(B563=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="564" spans="3:3">
       <c r="C564">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="565" spans="3:3">
       <c r="C565">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="566" spans="3:3">
       <c r="C566">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="567" spans="3:3">
       <c r="C567">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C567:C630" ca="1" si="11">IF(B567=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5222,31 +5238,31 @@
     </row>
     <row r="627" spans="3:3">
       <c r="C627">
-        <f t="shared" ref="C627:C690" ca="1" si="12">IF(B627=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="628" spans="3:3">
       <c r="C628">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="629" spans="3:3">
       <c r="C629">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="630" spans="3:3">
       <c r="C630">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="631" spans="3:3">
       <c r="C631">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C631:C694" ca="1" si="12">IF(B631=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5606,31 +5622,31 @@
     </row>
     <row r="691" spans="3:3">
       <c r="C691">
-        <f t="shared" ref="C691:C754" ca="1" si="13">IF(B691=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="692" spans="3:3">
       <c r="C692">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="693" spans="3:3">
       <c r="C693">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="694" spans="3:3">
       <c r="C694">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="695" spans="3:3">
       <c r="C695">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C695:C758" ca="1" si="13">IF(B695=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5990,31 +6006,31 @@
     </row>
     <row r="755" spans="3:3">
       <c r="C755">
-        <f t="shared" ref="C755:C818" ca="1" si="14">IF(B755=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="756" spans="3:3">
       <c r="C756">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="757" spans="3:3">
       <c r="C757">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="758" spans="3:3">
       <c r="C758">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="759" spans="3:3">
       <c r="C759">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C759:C822" ca="1" si="14">IF(B759=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6374,31 +6390,31 @@
     </row>
     <row r="819" spans="3:3">
       <c r="C819">
-        <f t="shared" ref="C819:C882" ca="1" si="15">IF(B819=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="820" spans="3:3">
       <c r="C820">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="821" spans="3:3">
       <c r="C821">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="822" spans="3:3">
       <c r="C822">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="823" spans="3:3">
       <c r="C823">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C823:C886" ca="1" si="15">IF(B823=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6758,31 +6774,31 @@
     </row>
     <row r="883" spans="3:3">
       <c r="C883">
-        <f t="shared" ref="C883:C897" ca="1" si="16">IF(B883=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="884" spans="3:3">
       <c r="C884">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="885" spans="3:3">
       <c r="C885">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="886" spans="3:3">
       <c r="C886">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="887" spans="3:3">
       <c r="C887">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C887:C901" ca="1" si="16">IF(B887=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6846,22 +6862,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="898" spans="3:3">
+      <c r="C898">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="899" spans="3:3">
+      <c r="C899">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="900" spans="3:3">
+      <c r="C900">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="901" spans="3:3">
+      <c r="C901">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A222:A227"/>
-    <mergeCell ref="A239:A255"/>
+    <mergeCell ref="A226:A231"/>
+    <mergeCell ref="A243:A259"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A217:A221"/>
+    <mergeCell ref="A217:A225"/>
     <mergeCell ref="A198:A216"/>
     <mergeCell ref="A169:A197"/>
     <mergeCell ref="A157:A168"/>
     <mergeCell ref="A119:A156"/>
-    <mergeCell ref="A228:A235"/>
-    <mergeCell ref="A236:A238"/>
+    <mergeCell ref="A232:A239"/>
+    <mergeCell ref="A240:A242"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add more obvious variant of task3983 solve all tasks in lab03 and 1-20 tasks in lab04 move tasks with graphics in lab05. they are before complex tasks now
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -401,11 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E901"/>
+  <dimension ref="A1:E902"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B224" sqref="B224"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,7 +417,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3349</v>
+        <v>9186</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1396,7 +1396,7 @@
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C165" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C166" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
     <row r="143" spans="1:3">
       <c r="A143" s="1"/>
       <c r="B143">
-        <v>8418</v>
+        <v>1483</v>
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
@@ -1855,7 +1855,7 @@
     <row r="144" spans="1:3">
       <c r="A144" s="1"/>
       <c r="B144">
-        <v>8395</v>
+        <v>8418</v>
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
@@ -1865,7 +1865,7 @@
     <row r="145" spans="1:3">
       <c r="A145" s="1"/>
       <c r="B145">
-        <v>5170</v>
+        <v>8395</v>
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
@@ -1875,7 +1875,7 @@
     <row r="146" spans="1:3">
       <c r="A146" s="1"/>
       <c r="B146">
-        <v>5568</v>
+        <v>5170</v>
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
@@ -1885,7 +1885,7 @@
     <row r="147" spans="1:3">
       <c r="A147" s="1"/>
       <c r="B147">
-        <v>2592</v>
+        <v>5568</v>
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
@@ -1895,7 +1895,7 @@
     <row r="148" spans="1:3">
       <c r="A148" s="1"/>
       <c r="B148">
-        <v>4075</v>
+        <v>2592</v>
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
@@ -1905,7 +1905,7 @@
     <row r="149" spans="1:3">
       <c r="A149" s="1"/>
       <c r="B149">
-        <v>7517</v>
+        <v>4075</v>
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
@@ -1915,7 +1915,7 @@
     <row r="150" spans="1:3">
       <c r="A150" s="1"/>
       <c r="B150">
-        <v>5448</v>
+        <v>7517</v>
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
@@ -1925,7 +1925,7 @@
     <row r="151" spans="1:3">
       <c r="A151" s="1"/>
       <c r="B151">
-        <v>6572</v>
+        <v>5448</v>
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
@@ -1935,7 +1935,7 @@
     <row r="152" spans="1:3">
       <c r="A152" s="1"/>
       <c r="B152">
-        <v>5238</v>
+        <v>6572</v>
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
@@ -1945,7 +1945,7 @@
     <row r="153" spans="1:3">
       <c r="A153" s="1"/>
       <c r="B153">
-        <v>2084</v>
+        <v>5238</v>
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
@@ -1955,7 +1955,7 @@
     <row r="154" spans="1:3">
       <c r="A154" s="1"/>
       <c r="B154">
-        <v>5411</v>
+        <v>2084</v>
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
@@ -1965,7 +1965,7 @@
     <row r="155" spans="1:3">
       <c r="A155" s="1"/>
       <c r="B155">
-        <v>5171</v>
+        <v>5411</v>
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
@@ -1975,7 +1975,7 @@
     <row r="156" spans="1:3">
       <c r="A156" s="1"/>
       <c r="B156">
-        <v>1862</v>
+        <v>5171</v>
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
@@ -1983,11 +1983,9 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A157" s="1"/>
       <c r="B157">
-        <v>8165</v>
+        <v>1862</v>
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
@@ -1995,9 +1993,11 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B158">
-        <v>9001</v>
+        <v>8165</v>
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
@@ -2007,7 +2007,7 @@
     <row r="159" spans="1:3">
       <c r="A159" s="1"/>
       <c r="B159">
-        <v>9631</v>
+        <v>9001</v>
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
@@ -2017,7 +2017,7 @@
     <row r="160" spans="1:3">
       <c r="A160" s="1"/>
       <c r="B160">
-        <v>9812</v>
+        <v>9631</v>
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
@@ -2027,7 +2027,7 @@
     <row r="161" spans="1:3">
       <c r="A161" s="1"/>
       <c r="B161">
-        <v>5728</v>
+        <v>9812</v>
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
@@ -2037,7 +2037,7 @@
     <row r="162" spans="1:3">
       <c r="A162" s="1"/>
       <c r="B162">
-        <v>1618</v>
+        <v>5728</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
@@ -2047,7 +2047,7 @@
     <row r="163" spans="1:3">
       <c r="A163" s="1"/>
       <c r="B163">
-        <v>7491</v>
+        <v>1618</v>
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="3"/>
@@ -2057,7 +2057,7 @@
     <row r="164" spans="1:3">
       <c r="A164" s="1"/>
       <c r="B164">
-        <v>5923</v>
+        <v>7491</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="3"/>
@@ -2067,7 +2067,7 @@
     <row r="165" spans="1:3">
       <c r="A165" s="1"/>
       <c r="B165">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="3"/>
@@ -2077,27 +2077,27 @@
     <row r="166" spans="1:3">
       <c r="A166" s="1"/>
       <c r="B166">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:C246" ca="1" si="4">IF(B166=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="1"/>
       <c r="B167">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C167">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="C167:C247" ca="1" si="4">IF(B167=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="1"/>
       <c r="B168">
-        <v>9925</v>
+        <v>9116</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="4"/>
@@ -2105,11 +2105,9 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A169" s="1"/>
       <c r="B169">
-        <v>2885</v>
+        <v>9925</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="4"/>
@@ -2117,9 +2115,11 @@
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="1"/>
+      <c r="A170" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B170">
-        <v>9931</v>
+        <v>2885</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2129,7 +2129,7 @@
     <row r="171" spans="1:3">
       <c r="A171" s="1"/>
       <c r="B171">
-        <v>4425</v>
+        <v>9931</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2139,7 +2139,7 @@
     <row r="172" spans="1:3">
       <c r="A172" s="1"/>
       <c r="B172">
-        <v>1947</v>
+        <v>4425</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2149,7 +2149,7 @@
     <row r="173" spans="1:3">
       <c r="A173" s="1"/>
       <c r="B173">
-        <v>9696</v>
+        <v>1947</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2159,7 +2159,7 @@
     <row r="174" spans="1:3">
       <c r="A174" s="1"/>
       <c r="B174">
-        <v>1223</v>
+        <v>9696</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2169,7 +2169,7 @@
     <row r="175" spans="1:3">
       <c r="A175" s="1"/>
       <c r="B175">
-        <v>3946</v>
+        <v>1223</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2179,7 +2179,7 @@
     <row r="176" spans="1:3">
       <c r="A176" s="1"/>
       <c r="B176">
-        <v>8311</v>
+        <v>3946</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2189,7 +2189,7 @@
     <row r="177" spans="1:3">
       <c r="A177" s="1"/>
       <c r="B177">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2199,7 +2199,7 @@
     <row r="178" spans="1:3">
       <c r="A178" s="1"/>
       <c r="B178">
-        <v>9774</v>
+        <v>3134</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2209,7 +2209,7 @@
     <row r="179" spans="1:3">
       <c r="A179" s="1"/>
       <c r="B179">
-        <v>9711</v>
+        <v>9774</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2219,7 +2219,7 @@
     <row r="180" spans="1:3">
       <c r="A180" s="1"/>
       <c r="B180">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2229,7 +2229,7 @@
     <row r="181" spans="1:3">
       <c r="A181" s="1"/>
       <c r="B181">
-        <v>7290</v>
+        <v>3333</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2239,7 +2239,7 @@
     <row r="182" spans="1:3">
       <c r="A182" s="1"/>
       <c r="B182">
-        <v>5694</v>
+        <v>7290</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2249,7 +2249,7 @@
     <row r="183" spans="1:3">
       <c r="A183" s="1"/>
       <c r="B183">
-        <v>7035</v>
+        <v>5694</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2259,7 +2259,7 @@
     <row r="184" spans="1:3">
       <c r="A184" s="1"/>
       <c r="B184">
-        <v>6806</v>
+        <v>7035</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2269,7 +2269,7 @@
     <row r="185" spans="1:3">
       <c r="A185" s="1"/>
       <c r="B185">
-        <v>4515</v>
+        <v>6806</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2279,7 +2279,7 @@
     <row r="186" spans="1:3">
       <c r="A186" s="1"/>
       <c r="B186">
-        <v>9271</v>
+        <v>4515</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2289,7 +2289,7 @@
     <row r="187" spans="1:3">
       <c r="A187" s="1"/>
       <c r="B187">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2299,7 +2299,7 @@
     <row r="188" spans="1:3">
       <c r="A188" s="1"/>
       <c r="B188">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2309,7 +2309,7 @@
     <row r="189" spans="1:3">
       <c r="A189" s="1"/>
       <c r="B189">
-        <v>3940</v>
+        <v>4497</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2319,7 +2319,7 @@
     <row r="190" spans="1:3">
       <c r="A190" s="1"/>
       <c r="B190">
-        <v>8820</v>
+        <v>3940</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2329,7 +2329,7 @@
     <row r="191" spans="1:3">
       <c r="A191" s="1"/>
       <c r="B191">
-        <v>3218</v>
+        <v>8820</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2339,7 +2339,7 @@
     <row r="192" spans="1:3">
       <c r="A192" s="1"/>
       <c r="B192">
-        <v>4283</v>
+        <v>3218</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2349,27 +2349,27 @@
     <row r="193" spans="1:3">
       <c r="A193" s="1"/>
       <c r="B193">
-        <v>7703</v>
+        <v>4283</v>
       </c>
       <c r="C193">
-        <f ca="1">IF(B193=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1"/>
       <c r="B194">
-        <v>9182</v>
+        <v>7703</v>
       </c>
       <c r="C194">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B194=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1"/>
       <c r="B195">
-        <v>5541</v>
+        <v>9182</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2379,7 +2379,7 @@
     <row r="196" spans="1:3">
       <c r="A196" s="1"/>
       <c r="B196">
-        <v>2386</v>
+        <v>5541</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2389,7 +2389,7 @@
     <row r="197" spans="1:3">
       <c r="A197" s="1"/>
       <c r="B197">
-        <v>9159</v>
+        <v>2386</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2397,11 +2397,9 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A198" s="1"/>
       <c r="B198">
-        <v>6175</v>
+        <v>9159</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2409,9 +2407,11 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1"/>
+      <c r="A199" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B199">
-        <v>4642</v>
+        <v>6175</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2421,7 +2421,7 @@
     <row r="200" spans="1:3">
       <c r="A200" s="1"/>
       <c r="B200">
-        <v>4488</v>
+        <v>4642</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2431,7 +2431,7 @@
     <row r="201" spans="1:3">
       <c r="A201" s="1"/>
       <c r="B201">
-        <v>9765</v>
+        <v>4488</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2441,7 +2441,7 @@
     <row r="202" spans="1:3">
       <c r="A202" s="1"/>
       <c r="B202">
-        <v>4954</v>
+        <v>9765</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2451,7 +2451,7 @@
     <row r="203" spans="1:3">
       <c r="A203" s="1"/>
       <c r="B203">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2461,7 +2461,7 @@
     <row r="204" spans="1:3">
       <c r="A204" s="1"/>
       <c r="B204">
-        <v>6431</v>
+        <v>5537</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2471,7 +2471,7 @@
     <row r="205" spans="1:3">
       <c r="A205" s="1"/>
       <c r="B205">
-        <v>7193</v>
+        <v>6431</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2481,7 +2481,7 @@
     <row r="206" spans="1:3">
       <c r="A206" s="1"/>
       <c r="B206">
-        <v>5621</v>
+        <v>7193</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2491,7 +2491,7 @@
     <row r="207" spans="1:3">
       <c r="A207" s="1"/>
       <c r="B207">
-        <v>5847</v>
+        <v>5621</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2501,7 +2501,7 @@
     <row r="208" spans="1:3">
       <c r="A208" s="1"/>
       <c r="B208">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2511,7 +2511,7 @@
     <row r="209" spans="1:3">
       <c r="A209" s="1"/>
       <c r="B209">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2521,7 +2521,7 @@
     <row r="210" spans="1:3">
       <c r="A210" s="1"/>
       <c r="B210">
-        <v>3226</v>
+        <v>9930</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2531,7 +2531,7 @@
     <row r="211" spans="1:3">
       <c r="A211" s="1"/>
       <c r="B211">
-        <v>6861</v>
+        <v>3226</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2541,7 +2541,7 @@
     <row r="212" spans="1:3">
       <c r="A212" s="1"/>
       <c r="B212">
-        <v>2205</v>
+        <v>6861</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2551,7 +2551,7 @@
     <row r="213" spans="1:3">
       <c r="A213" s="1"/>
       <c r="B213">
-        <v>4372</v>
+        <v>2205</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2561,7 +2561,7 @@
     <row r="214" spans="1:3">
       <c r="A214" s="1"/>
       <c r="B214">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2571,7 +2571,7 @@
     <row r="215" spans="1:3">
       <c r="A215" s="1"/>
       <c r="B215">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2581,7 +2581,7 @@
     <row r="216" spans="1:3">
       <c r="A216" s="1"/>
       <c r="B216">
-        <v>2137</v>
+        <v>1668</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2589,11 +2589,9 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A217" s="1"/>
       <c r="B217">
-        <v>9300</v>
+        <v>2137</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2601,9 +2599,11 @@
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="1"/>
+      <c r="A218" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B218">
-        <v>3951</v>
+        <v>9300</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2613,7 +2613,7 @@
     <row r="219" spans="1:3">
       <c r="A219" s="1"/>
       <c r="B219">
-        <v>6409</v>
+        <v>3951</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2623,7 +2623,7 @@
     <row r="220" spans="1:3">
       <c r="A220" s="1"/>
       <c r="B220">
-        <v>3290</v>
+        <v>6409</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2633,7 +2633,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="1"/>
       <c r="B221">
-        <v>5309</v>
+        <v>3290</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2643,7 +2643,7 @@
     <row r="222" spans="1:3">
       <c r="A222" s="1"/>
       <c r="B222">
-        <v>5345</v>
+        <v>5309</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2653,7 +2653,7 @@
     <row r="223" spans="1:3">
       <c r="A223" s="1"/>
       <c r="B223">
-        <v>6812</v>
+        <v>5345</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2663,7 +2663,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="1"/>
       <c r="B224">
-        <v>7343</v>
+        <v>6812</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2673,7 +2673,7 @@
     <row r="225" spans="1:3">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2681,11 +2681,9 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A226" s="1"/>
       <c r="B226">
-        <v>9299</v>
+        <v>7060</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2693,9 +2691,11 @@
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="1"/>
+      <c r="A227" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B227">
-        <v>7560</v>
+        <v>9299</v>
       </c>
       <c r="C227">
         <f t="shared" ca="1" si="4"/>
@@ -2705,7 +2705,7 @@
     <row r="228" spans="1:3">
       <c r="A228" s="1"/>
       <c r="B228">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="4"/>
@@ -2715,7 +2715,7 @@
     <row r="229" spans="1:3">
       <c r="A229" s="1"/>
       <c r="B229">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="4"/>
@@ -2725,7 +2725,7 @@
     <row r="230" spans="1:3">
       <c r="A230" s="1"/>
       <c r="B230">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="4"/>
@@ -2735,7 +2735,7 @@
     <row r="231" spans="1:3">
       <c r="A231" s="1"/>
       <c r="B231">
-        <v>2048</v>
+        <v>1954</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="4"/>
@@ -2743,11 +2743,9 @@
       </c>
     </row>
     <row r="232" spans="1:3">
-      <c r="A232" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A232" s="1"/>
       <c r="B232">
-        <v>3939</v>
+        <v>2048</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="4"/>
@@ -2755,9 +2753,11 @@
       </c>
     </row>
     <row r="233" spans="1:3">
-      <c r="A233" s="1"/>
+      <c r="A233" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B233">
-        <v>8861</v>
+        <v>3939</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="4"/>
@@ -2767,27 +2767,27 @@
     <row r="234" spans="1:3">
       <c r="A234" s="1"/>
       <c r="B234">
-        <v>1516</v>
+        <v>8861</v>
       </c>
       <c r="C234">
-        <f t="shared" ref="C234:C242" ca="1" si="5">IF(B234=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="1"/>
       <c r="B235">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C235">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C235:C243" ca="1" si="5">IF(B235=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1"/>
       <c r="B236">
-        <v>5164</v>
+        <v>9062</v>
       </c>
       <c r="C236">
         <f t="shared" ca="1" si="5"/>
@@ -2797,7 +2797,7 @@
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>2030</v>
+        <v>5164</v>
       </c>
       <c r="C237">
         <f t="shared" ca="1" si="5"/>
@@ -2807,7 +2807,7 @@
     <row r="238" spans="1:3">
       <c r="A238" s="1"/>
       <c r="B238">
-        <v>7649</v>
+        <v>2030</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2817,7 +2817,7 @@
     <row r="239" spans="1:3">
       <c r="A239" s="1"/>
       <c r="B239">
-        <v>2354</v>
+        <v>7649</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2825,11 +2825,9 @@
       </c>
     </row>
     <row r="240" spans="1:3">
-      <c r="A240" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A240" s="1"/>
       <c r="B240">
-        <v>9701</v>
+        <v>2354</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2837,9 +2835,11 @@
       </c>
     </row>
     <row r="241" spans="1:3">
-      <c r="A241" s="1"/>
+      <c r="A241" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B241">
-        <v>3784</v>
+        <v>9701</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2849,7 +2849,7 @@
     <row r="242" spans="1:3">
       <c r="A242" s="1"/>
       <c r="B242">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2857,21 +2857,21 @@
       </c>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="1" t="s">
+      <c r="A243" s="1"/>
+      <c r="B243">
+        <v>6732</v>
+      </c>
+      <c r="C243">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B243">
+      <c r="B244">
         <v>8403</v>
-      </c>
-      <c r="C243">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244" s="1"/>
-      <c r="B244">
-        <v>3185</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="4"/>
@@ -2881,7 +2881,7 @@
     <row r="245" spans="1:3">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C245">
         <f t="shared" ca="1" si="4"/>
@@ -2891,7 +2891,7 @@
     <row r="246" spans="1:3">
       <c r="A246" s="1"/>
       <c r="B246">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="4"/>
@@ -2901,27 +2901,27 @@
     <row r="247" spans="1:3">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C247">
-        <f t="shared" ref="C247:C310" ca="1" si="6">IF(B247=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C248">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C248:C311" ca="1" si="6">IF(B248=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="6"/>
@@ -2931,7 +2931,7 @@
     <row r="250" spans="1:3">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="6"/>
@@ -2941,7 +2941,7 @@
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="6"/>
@@ -2951,7 +2951,7 @@
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="6"/>
@@ -2961,7 +2961,7 @@
     <row r="253" spans="1:3">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="6"/>
@@ -2971,7 +2971,7 @@
     <row r="254" spans="1:3">
       <c r="A254" s="1"/>
       <c r="B254">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="6"/>
@@ -2981,7 +2981,7 @@
     <row r="255" spans="1:3">
       <c r="A255" s="1"/>
       <c r="B255">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C255">
         <f t="shared" ca="1" si="6"/>
@@ -2991,7 +2991,7 @@
     <row r="256" spans="1:3">
       <c r="A256" s="1"/>
       <c r="B256">
-        <v>4147</v>
+        <v>2000</v>
       </c>
       <c r="C256">
         <f t="shared" ca="1" si="6"/>
@@ -3001,7 +3001,7 @@
     <row r="257" spans="1:3">
       <c r="A257" s="1"/>
       <c r="B257">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C257">
         <f t="shared" ca="1" si="6"/>
@@ -3011,7 +3011,7 @@
     <row r="258" spans="1:3">
       <c r="A258" s="1"/>
       <c r="B258">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C258">
         <f t="shared" ca="1" si="6"/>
@@ -3021,7 +3021,7 @@
     <row r="259" spans="1:3">
       <c r="A259" s="1"/>
       <c r="B259">
-        <v>5463</v>
+        <v>3956</v>
       </c>
       <c r="C259">
         <f t="shared" ca="1" si="6"/>
@@ -3029,11 +3029,9 @@
       </c>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" t="s">
-        <v>14</v>
-      </c>
+      <c r="A260" s="1"/>
       <c r="B260">
-        <v>8787</v>
+        <v>5463</v>
       </c>
       <c r="C260">
         <f t="shared" ca="1" si="6"/>
@@ -3041,6 +3039,12 @@
       </c>
     </row>
     <row r="261" spans="1:3">
+      <c r="A261" t="s">
+        <v>14</v>
+      </c>
+      <c r="B261">
+        <v>8787</v>
+      </c>
       <c r="C261">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3342,13 +3346,13 @@
     </row>
     <row r="311" spans="3:3">
       <c r="C311">
-        <f t="shared" ref="C311:C374" ca="1" si="7">IF(B311=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="3:3">
       <c r="C312">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C312:C375" ca="1" si="7">IF(B312=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3726,13 +3730,13 @@
     </row>
     <row r="375" spans="3:3">
       <c r="C375">
-        <f t="shared" ref="C375:C438" ca="1" si="8">IF(B375=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="376" spans="3:3">
       <c r="C376">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C376:C439" ca="1" si="8">IF(B376=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4110,13 +4114,13 @@
     </row>
     <row r="439" spans="3:3">
       <c r="C439">
-        <f t="shared" ref="C439:C502" ca="1" si="9">IF(B439=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="440" spans="3:3">
       <c r="C440">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C440:C503" ca="1" si="9">IF(B440=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4494,13 +4498,13 @@
     </row>
     <row r="503" spans="3:3">
       <c r="C503">
-        <f t="shared" ref="C503:C566" ca="1" si="10">IF(B503=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="504" spans="3:3">
       <c r="C504">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C504:C567" ca="1" si="10">IF(B504=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4878,13 +4882,13 @@
     </row>
     <row r="567" spans="3:3">
       <c r="C567">
-        <f t="shared" ref="C567:C630" ca="1" si="11">IF(B567=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="568" spans="3:3">
       <c r="C568">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C568:C631" ca="1" si="11">IF(B568=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5262,13 +5266,13 @@
     </row>
     <row r="631" spans="3:3">
       <c r="C631">
-        <f t="shared" ref="C631:C694" ca="1" si="12">IF(B631=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="632" spans="3:3">
       <c r="C632">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C632:C695" ca="1" si="12">IF(B632=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5646,13 +5650,13 @@
     </row>
     <row r="695" spans="3:3">
       <c r="C695">
-        <f t="shared" ref="C695:C758" ca="1" si="13">IF(B695=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="696" spans="3:3">
       <c r="C696">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C696:C759" ca="1" si="13">IF(B696=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6030,13 +6034,13 @@
     </row>
     <row r="759" spans="3:3">
       <c r="C759">
-        <f t="shared" ref="C759:C822" ca="1" si="14">IF(B759=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="760" spans="3:3">
       <c r="C760">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C760:C823" ca="1" si="14">IF(B760=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6414,13 +6418,13 @@
     </row>
     <row r="823" spans="3:3">
       <c r="C823">
-        <f t="shared" ref="C823:C886" ca="1" si="15">IF(B823=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="824" spans="3:3">
       <c r="C824">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C824:C887" ca="1" si="15">IF(B824=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6798,13 +6802,13 @@
     </row>
     <row r="887" spans="3:3">
       <c r="C887">
-        <f t="shared" ref="C887:C901" ca="1" si="16">IF(B887=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="888" spans="3:3">
       <c r="C888">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C888:C902" ca="1" si="16">IF(B888=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6886,22 +6890,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="902" spans="3:3">
+      <c r="C902">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A226:A231"/>
-    <mergeCell ref="A243:A259"/>
+    <mergeCell ref="A227:A232"/>
+    <mergeCell ref="A244:A260"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A217:A225"/>
-    <mergeCell ref="A198:A216"/>
-    <mergeCell ref="A169:A197"/>
-    <mergeCell ref="A157:A168"/>
-    <mergeCell ref="A119:A156"/>
-    <mergeCell ref="A232:A239"/>
-    <mergeCell ref="A240:A242"/>
+    <mergeCell ref="A218:A226"/>
+    <mergeCell ref="A199:A217"/>
+    <mergeCell ref="A170:A198"/>
+    <mergeCell ref="A158:A169"/>
+    <mergeCell ref="A119:A157"/>
+    <mergeCell ref="A233:A240"/>
+    <mergeCell ref="A241:A243"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
solve all tasks from lab07 in js add 2 tasks to lab07
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -401,11 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E902"/>
+  <dimension ref="A1:E904"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M139" sqref="M139"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,7 +417,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9186</v>
+        <v>4131</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1396,7 +1396,7 @@
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C166" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C168" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
     <row r="162" spans="1:3">
       <c r="A162" s="1"/>
       <c r="B162">
-        <v>5728</v>
+        <v>4845</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
@@ -2047,7 +2047,7 @@
     <row r="163" spans="1:3">
       <c r="A163" s="1"/>
       <c r="B163">
-        <v>1618</v>
+        <v>5728</v>
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="3"/>
@@ -2057,7 +2057,7 @@
     <row r="164" spans="1:3">
       <c r="A164" s="1"/>
       <c r="B164">
-        <v>7491</v>
+        <v>1618</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="3"/>
@@ -2067,7 +2067,7 @@
     <row r="165" spans="1:3">
       <c r="A165" s="1"/>
       <c r="B165">
-        <v>5923</v>
+        <v>9279</v>
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="3"/>
@@ -2077,7 +2077,7 @@
     <row r="166" spans="1:3">
       <c r="A166" s="1"/>
       <c r="B166">
-        <v>4265</v>
+        <v>7491</v>
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="3"/>
@@ -2087,39 +2087,37 @@
     <row r="167" spans="1:3">
       <c r="A167" s="1"/>
       <c r="B167">
-        <v>2166</v>
+        <v>5923</v>
       </c>
       <c r="C167">
-        <f t="shared" ref="C167:C247" ca="1" si="4">IF(B167=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="1"/>
       <c r="B168">
-        <v>9116</v>
+        <v>4265</v>
       </c>
       <c r="C168">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="1"/>
       <c r="B169">
-        <v>9925</v>
+        <v>2166</v>
       </c>
       <c r="C169">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="C169:C249" ca="1" si="4">IF(B169=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A170" s="1"/>
       <c r="B170">
-        <v>2885</v>
+        <v>9116</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="4"/>
@@ -2129,7 +2127,7 @@
     <row r="171" spans="1:3">
       <c r="A171" s="1"/>
       <c r="B171">
-        <v>9931</v>
+        <v>9925</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="4"/>
@@ -2137,9 +2135,11 @@
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B172">
-        <v>4425</v>
+        <v>2885</v>
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="4"/>
@@ -2149,7 +2149,7 @@
     <row r="173" spans="1:3">
       <c r="A173" s="1"/>
       <c r="B173">
-        <v>1947</v>
+        <v>9931</v>
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="4"/>
@@ -2159,7 +2159,7 @@
     <row r="174" spans="1:3">
       <c r="A174" s="1"/>
       <c r="B174">
-        <v>9696</v>
+        <v>4425</v>
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="4"/>
@@ -2169,7 +2169,7 @@
     <row r="175" spans="1:3">
       <c r="A175" s="1"/>
       <c r="B175">
-        <v>1223</v>
+        <v>1947</v>
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="4"/>
@@ -2179,7 +2179,7 @@
     <row r="176" spans="1:3">
       <c r="A176" s="1"/>
       <c r="B176">
-        <v>3946</v>
+        <v>9696</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2189,7 +2189,7 @@
     <row r="177" spans="1:3">
       <c r="A177" s="1"/>
       <c r="B177">
-        <v>8311</v>
+        <v>1223</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2199,7 +2199,7 @@
     <row r="178" spans="1:3">
       <c r="A178" s="1"/>
       <c r="B178">
-        <v>3134</v>
+        <v>3946</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2209,7 +2209,7 @@
     <row r="179" spans="1:3">
       <c r="A179" s="1"/>
       <c r="B179">
-        <v>9774</v>
+        <v>8311</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2219,7 +2219,7 @@
     <row r="180" spans="1:3">
       <c r="A180" s="1"/>
       <c r="B180">
-        <v>9711</v>
+        <v>3134</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2229,7 +2229,7 @@
     <row r="181" spans="1:3">
       <c r="A181" s="1"/>
       <c r="B181">
-        <v>3333</v>
+        <v>9774</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2239,7 +2239,7 @@
     <row r="182" spans="1:3">
       <c r="A182" s="1"/>
       <c r="B182">
-        <v>7290</v>
+        <v>9711</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2249,7 +2249,7 @@
     <row r="183" spans="1:3">
       <c r="A183" s="1"/>
       <c r="B183">
-        <v>5694</v>
+        <v>3333</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2259,7 +2259,7 @@
     <row r="184" spans="1:3">
       <c r="A184" s="1"/>
       <c r="B184">
-        <v>7035</v>
+        <v>7290</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2269,7 +2269,7 @@
     <row r="185" spans="1:3">
       <c r="A185" s="1"/>
       <c r="B185">
-        <v>6806</v>
+        <v>5694</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2279,7 +2279,7 @@
     <row r="186" spans="1:3">
       <c r="A186" s="1"/>
       <c r="B186">
-        <v>4515</v>
+        <v>7035</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2289,7 +2289,7 @@
     <row r="187" spans="1:3">
       <c r="A187" s="1"/>
       <c r="B187">
-        <v>9271</v>
+        <v>6806</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2299,7 +2299,7 @@
     <row r="188" spans="1:3">
       <c r="A188" s="1"/>
       <c r="B188">
-        <v>8769</v>
+        <v>4515</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2309,7 +2309,7 @@
     <row r="189" spans="1:3">
       <c r="A189" s="1"/>
       <c r="B189">
-        <v>4497</v>
+        <v>9271</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2319,7 +2319,7 @@
     <row r="190" spans="1:3">
       <c r="A190" s="1"/>
       <c r="B190">
-        <v>3940</v>
+        <v>8769</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2329,7 +2329,7 @@
     <row r="191" spans="1:3">
       <c r="A191" s="1"/>
       <c r="B191">
-        <v>8820</v>
+        <v>4497</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2339,7 +2339,7 @@
     <row r="192" spans="1:3">
       <c r="A192" s="1"/>
       <c r="B192">
-        <v>3218</v>
+        <v>3940</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2349,7 +2349,7 @@
     <row r="193" spans="1:3">
       <c r="A193" s="1"/>
       <c r="B193">
-        <v>4283</v>
+        <v>8820</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2359,17 +2359,17 @@
     <row r="194" spans="1:3">
       <c r="A194" s="1"/>
       <c r="B194">
-        <v>7703</v>
+        <v>3218</v>
       </c>
       <c r="C194">
-        <f ca="1">IF(B194=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1"/>
       <c r="B195">
-        <v>9182</v>
+        <v>4283</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2379,17 +2379,17 @@
     <row r="196" spans="1:3">
       <c r="A196" s="1"/>
       <c r="B196">
-        <v>5541</v>
+        <v>7703</v>
       </c>
       <c r="C196">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B196=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1"/>
       <c r="B197">
-        <v>2386</v>
+        <v>9182</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2399,7 +2399,7 @@
     <row r="198" spans="1:3">
       <c r="A198" s="1"/>
       <c r="B198">
-        <v>9159</v>
+        <v>5541</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2407,11 +2407,9 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A199" s="1"/>
       <c r="B199">
-        <v>6175</v>
+        <v>2386</v>
       </c>
       <c r="C199">
         <f t="shared" ca="1" si="4"/>
@@ -2421,7 +2419,7 @@
     <row r="200" spans="1:3">
       <c r="A200" s="1"/>
       <c r="B200">
-        <v>4642</v>
+        <v>9159</v>
       </c>
       <c r="C200">
         <f t="shared" ca="1" si="4"/>
@@ -2429,9 +2427,11 @@
       </c>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="1"/>
+      <c r="A201" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B201">
-        <v>4488</v>
+        <v>6175</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2441,7 +2441,7 @@
     <row r="202" spans="1:3">
       <c r="A202" s="1"/>
       <c r="B202">
-        <v>9765</v>
+        <v>4642</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2451,7 +2451,7 @@
     <row r="203" spans="1:3">
       <c r="A203" s="1"/>
       <c r="B203">
-        <v>4954</v>
+        <v>4488</v>
       </c>
       <c r="C203">
         <f t="shared" ca="1" si="4"/>
@@ -2461,7 +2461,7 @@
     <row r="204" spans="1:3">
       <c r="A204" s="1"/>
       <c r="B204">
-        <v>5537</v>
+        <v>9765</v>
       </c>
       <c r="C204">
         <f t="shared" ca="1" si="4"/>
@@ -2471,7 +2471,7 @@
     <row r="205" spans="1:3">
       <c r="A205" s="1"/>
       <c r="B205">
-        <v>6431</v>
+        <v>4954</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2481,7 +2481,7 @@
     <row r="206" spans="1:3">
       <c r="A206" s="1"/>
       <c r="B206">
-        <v>7193</v>
+        <v>5537</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2491,7 +2491,7 @@
     <row r="207" spans="1:3">
       <c r="A207" s="1"/>
       <c r="B207">
-        <v>5621</v>
+        <v>6431</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2501,7 +2501,7 @@
     <row r="208" spans="1:3">
       <c r="A208" s="1"/>
       <c r="B208">
-        <v>5847</v>
+        <v>7193</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2511,7 +2511,7 @@
     <row r="209" spans="1:3">
       <c r="A209" s="1"/>
       <c r="B209">
-        <v>4769</v>
+        <v>5621</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2521,7 +2521,7 @@
     <row r="210" spans="1:3">
       <c r="A210" s="1"/>
       <c r="B210">
-        <v>9930</v>
+        <v>5847</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2531,7 +2531,7 @@
     <row r="211" spans="1:3">
       <c r="A211" s="1"/>
       <c r="B211">
-        <v>3226</v>
+        <v>4769</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2541,7 +2541,7 @@
     <row r="212" spans="1:3">
       <c r="A212" s="1"/>
       <c r="B212">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2551,7 +2551,7 @@
     <row r="213" spans="1:3">
       <c r="A213" s="1"/>
       <c r="B213">
-        <v>2205</v>
+        <v>3226</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2561,7 +2561,7 @@
     <row r="214" spans="1:3">
       <c r="A214" s="1"/>
       <c r="B214">
-        <v>4372</v>
+        <v>6861</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2571,7 +2571,7 @@
     <row r="215" spans="1:3">
       <c r="A215" s="1"/>
       <c r="B215">
-        <v>4463</v>
+        <v>2205</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2581,7 +2581,7 @@
     <row r="216" spans="1:3">
       <c r="A216" s="1"/>
       <c r="B216">
-        <v>1668</v>
+        <v>4372</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2591,7 +2591,7 @@
     <row r="217" spans="1:3">
       <c r="A217" s="1"/>
       <c r="B217">
-        <v>2137</v>
+        <v>4463</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2599,11 +2599,9 @@
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A218" s="1"/>
       <c r="B218">
-        <v>9300</v>
+        <v>1668</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2613,7 +2611,7 @@
     <row r="219" spans="1:3">
       <c r="A219" s="1"/>
       <c r="B219">
-        <v>3951</v>
+        <v>2137</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2621,9 +2619,11 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="1"/>
+      <c r="A220" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B220">
-        <v>6409</v>
+        <v>9300</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2633,7 +2633,7 @@
     <row r="221" spans="1:3">
       <c r="A221" s="1"/>
       <c r="B221">
-        <v>3290</v>
+        <v>3951</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2643,7 +2643,7 @@
     <row r="222" spans="1:3">
       <c r="A222" s="1"/>
       <c r="B222">
-        <v>5309</v>
+        <v>6409</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2653,7 +2653,7 @@
     <row r="223" spans="1:3">
       <c r="A223" s="1"/>
       <c r="B223">
-        <v>5345</v>
+        <v>3290</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2663,7 +2663,7 @@
     <row r="224" spans="1:3">
       <c r="A224" s="1"/>
       <c r="B224">
-        <v>6812</v>
+        <v>5309</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2673,7 +2673,7 @@
     <row r="225" spans="1:3">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>7343</v>
+        <v>5345</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2683,7 +2683,7 @@
     <row r="226" spans="1:3">
       <c r="A226" s="1"/>
       <c r="B226">
-        <v>7060</v>
+        <v>6812</v>
       </c>
       <c r="C226">
         <f t="shared" ca="1" si="4"/>
@@ -2691,11 +2691,9 @@
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A227" s="1"/>
       <c r="B227">
-        <v>9299</v>
+        <v>7343</v>
       </c>
       <c r="C227">
         <f t="shared" ca="1" si="4"/>
@@ -2705,7 +2703,7 @@
     <row r="228" spans="1:3">
       <c r="A228" s="1"/>
       <c r="B228">
-        <v>7560</v>
+        <v>7060</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="4"/>
@@ -2713,9 +2711,11 @@
       </c>
     </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="1"/>
+      <c r="A229" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B229">
-        <v>9002</v>
+        <v>9299</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="4"/>
@@ -2725,7 +2725,7 @@
     <row r="230" spans="1:3">
       <c r="A230" s="1"/>
       <c r="B230">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="4"/>
@@ -2735,7 +2735,7 @@
     <row r="231" spans="1:3">
       <c r="A231" s="1"/>
       <c r="B231">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="4"/>
@@ -2745,7 +2745,7 @@
     <row r="232" spans="1:3">
       <c r="A232" s="1"/>
       <c r="B232">
-        <v>2048</v>
+        <v>7432</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="4"/>
@@ -2753,11 +2753,9 @@
       </c>
     </row>
     <row r="233" spans="1:3">
-      <c r="A233" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A233" s="1"/>
       <c r="B233">
-        <v>3939</v>
+        <v>1954</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="4"/>
@@ -2767,7 +2765,7 @@
     <row r="234" spans="1:3">
       <c r="A234" s="1"/>
       <c r="B234">
-        <v>8861</v>
+        <v>2048</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="4"/>
@@ -2775,39 +2773,41 @@
       </c>
     </row>
     <row r="235" spans="1:3">
-      <c r="A235" s="1"/>
+      <c r="A235" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B235">
-        <v>1516</v>
+        <v>3939</v>
       </c>
       <c r="C235">
-        <f t="shared" ref="C235:C243" ca="1" si="5">IF(B235=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1"/>
       <c r="B236">
-        <v>9062</v>
+        <v>8861</v>
       </c>
       <c r="C236">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="1"/>
       <c r="B237">
-        <v>5164</v>
+        <v>1516</v>
       </c>
       <c r="C237">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C237:C245" ca="1" si="5">IF(B237=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="1"/>
       <c r="B238">
-        <v>2030</v>
+        <v>9062</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="5"/>
@@ -2817,7 +2817,7 @@
     <row r="239" spans="1:3">
       <c r="A239" s="1"/>
       <c r="B239">
-        <v>7649</v>
+        <v>5164</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="5"/>
@@ -2827,7 +2827,7 @@
     <row r="240" spans="1:3">
       <c r="A240" s="1"/>
       <c r="B240">
-        <v>2354</v>
+        <v>2030</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="5"/>
@@ -2835,11 +2835,9 @@
       </c>
     </row>
     <row r="241" spans="1:3">
-      <c r="A241" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A241" s="1"/>
       <c r="B241">
-        <v>9701</v>
+        <v>7649</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="5"/>
@@ -2849,7 +2847,7 @@
     <row r="242" spans="1:3">
       <c r="A242" s="1"/>
       <c r="B242">
-        <v>3784</v>
+        <v>2354</v>
       </c>
       <c r="C242">
         <f t="shared" ca="1" si="5"/>
@@ -2857,9 +2855,11 @@
       </c>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="1"/>
+      <c r="A243" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B243">
-        <v>6732</v>
+        <v>9701</v>
       </c>
       <c r="C243">
         <f t="shared" ca="1" si="5"/>
@@ -2867,31 +2867,31 @@
       </c>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A244" s="1"/>
       <c r="B244">
-        <v>8403</v>
+        <v>3784</v>
       </c>
       <c r="C244">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>3185</v>
+        <v>6732</v>
       </c>
       <c r="C245">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:3">
-      <c r="A246" s="1"/>
+      <c r="A246" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B246">
-        <v>9914</v>
+        <v>8403</v>
       </c>
       <c r="C246">
         <f t="shared" ca="1" si="4"/>
@@ -2901,7 +2901,7 @@
     <row r="247" spans="1:3">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>6011</v>
+        <v>3185</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="4"/>
@@ -2911,37 +2911,37 @@
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>6037</v>
+        <v>9914</v>
       </c>
       <c r="C248">
-        <f t="shared" ref="C248:C311" ca="1" si="6">IF(B248=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>2809</v>
+        <v>6011</v>
       </c>
       <c r="C249">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>7297</v>
+        <v>6037</v>
       </c>
       <c r="C250">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C250:C313" ca="1" si="6">IF(B250=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>5242</v>
+        <v>2809</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="6"/>
@@ -2951,7 +2951,7 @@
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="6"/>
@@ -2961,7 +2961,7 @@
     <row r="253" spans="1:3">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="6"/>
@@ -2971,7 +2971,7 @@
     <row r="254" spans="1:3">
       <c r="A254" s="1"/>
       <c r="B254">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="6"/>
@@ -2981,7 +2981,7 @@
     <row r="255" spans="1:3">
       <c r="A255" s="1"/>
       <c r="B255">
-        <v>7301</v>
+        <v>2401</v>
       </c>
       <c r="C255">
         <f t="shared" ca="1" si="6"/>
@@ -2991,7 +2991,7 @@
     <row r="256" spans="1:3">
       <c r="A256" s="1"/>
       <c r="B256">
-        <v>2000</v>
+        <v>5421</v>
       </c>
       <c r="C256">
         <f t="shared" ca="1" si="6"/>
@@ -3001,7 +3001,7 @@
     <row r="257" spans="1:3">
       <c r="A257" s="1"/>
       <c r="B257">
-        <v>4147</v>
+        <v>7301</v>
       </c>
       <c r="C257">
         <f t="shared" ca="1" si="6"/>
@@ -3011,7 +3011,7 @@
     <row r="258" spans="1:3">
       <c r="A258" s="1"/>
       <c r="B258">
-        <v>1953</v>
+        <v>2000</v>
       </c>
       <c r="C258">
         <f t="shared" ca="1" si="6"/>
@@ -3021,7 +3021,7 @@
     <row r="259" spans="1:3">
       <c r="A259" s="1"/>
       <c r="B259">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C259">
         <f t="shared" ca="1" si="6"/>
@@ -3031,7 +3031,7 @@
     <row r="260" spans="1:3">
       <c r="A260" s="1"/>
       <c r="B260">
-        <v>5463</v>
+        <v>1953</v>
       </c>
       <c r="C260">
         <f t="shared" ca="1" si="6"/>
@@ -3039,11 +3039,9 @@
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" t="s">
-        <v>14</v>
-      </c>
+      <c r="A261" s="1"/>
       <c r="B261">
-        <v>8787</v>
+        <v>3956</v>
       </c>
       <c r="C261">
         <f t="shared" ca="1" si="6"/>
@@ -3051,12 +3049,22 @@
       </c>
     </row>
     <row r="262" spans="1:3">
+      <c r="A262" s="1"/>
+      <c r="B262">
+        <v>5463</v>
+      </c>
       <c r="C262">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:3">
+      <c r="A263" t="s">
+        <v>14</v>
+      </c>
+      <c r="B263">
+        <v>8787</v>
+      </c>
       <c r="C263">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3352,19 +3360,19 @@
     </row>
     <row r="312" spans="3:3">
       <c r="C312">
-        <f t="shared" ref="C312:C375" ca="1" si="7">IF(B312=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="313" spans="3:3">
       <c r="C313">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="3:3">
       <c r="C314">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C314:C377" ca="1" si="7">IF(B314=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3736,19 +3744,19 @@
     </row>
     <row r="376" spans="3:3">
       <c r="C376">
-        <f t="shared" ref="C376:C439" ca="1" si="8">IF(B376=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="377" spans="3:3">
       <c r="C377">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="378" spans="3:3">
       <c r="C378">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C378:C441" ca="1" si="8">IF(B378=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4120,19 +4128,19 @@
     </row>
     <row r="440" spans="3:3">
       <c r="C440">
-        <f t="shared" ref="C440:C503" ca="1" si="9">IF(B440=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="441" spans="3:3">
       <c r="C441">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="442" spans="3:3">
       <c r="C442">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C442:C505" ca="1" si="9">IF(B442=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4504,19 +4512,19 @@
     </row>
     <row r="504" spans="3:3">
       <c r="C504">
-        <f t="shared" ref="C504:C567" ca="1" si="10">IF(B504=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="505" spans="3:3">
       <c r="C505">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="506" spans="3:3">
       <c r="C506">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C506:C569" ca="1" si="10">IF(B506=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4888,19 +4896,19 @@
     </row>
     <row r="568" spans="3:3">
       <c r="C568">
-        <f t="shared" ref="C568:C631" ca="1" si="11">IF(B568=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="569" spans="3:3">
       <c r="C569">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="570" spans="3:3">
       <c r="C570">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C570:C633" ca="1" si="11">IF(B570=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5272,19 +5280,19 @@
     </row>
     <row r="632" spans="3:3">
       <c r="C632">
-        <f t="shared" ref="C632:C695" ca="1" si="12">IF(B632=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="633" spans="3:3">
       <c r="C633">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="634" spans="3:3">
       <c r="C634">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C634:C697" ca="1" si="12">IF(B634=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5656,19 +5664,19 @@
     </row>
     <row r="696" spans="3:3">
       <c r="C696">
-        <f t="shared" ref="C696:C759" ca="1" si="13">IF(B696=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="697" spans="3:3">
       <c r="C697">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="698" spans="3:3">
       <c r="C698">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C698:C761" ca="1" si="13">IF(B698=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6040,19 +6048,19 @@
     </row>
     <row r="760" spans="3:3">
       <c r="C760">
-        <f t="shared" ref="C760:C823" ca="1" si="14">IF(B760=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="761" spans="3:3">
       <c r="C761">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="762" spans="3:3">
       <c r="C762">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C762:C825" ca="1" si="14">IF(B762=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6424,19 +6432,19 @@
     </row>
     <row r="824" spans="3:3">
       <c r="C824">
-        <f t="shared" ref="C824:C887" ca="1" si="15">IF(B824=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="825" spans="3:3">
       <c r="C825">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="826" spans="3:3">
       <c r="C826">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C826:C889" ca="1" si="15">IF(B826=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6808,19 +6816,19 @@
     </row>
     <row r="888" spans="3:3">
       <c r="C888">
-        <f t="shared" ref="C888:C902" ca="1" si="16">IF(B888=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="889" spans="3:3">
       <c r="C889">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="890" spans="3:3">
       <c r="C890">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C890:C904" ca="1" si="16">IF(B890=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6896,22 +6904,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="903" spans="3:3">
+      <c r="C903">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="904" spans="3:3">
+      <c r="C904">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A227:A232"/>
-    <mergeCell ref="A244:A260"/>
+    <mergeCell ref="A229:A234"/>
+    <mergeCell ref="A246:A262"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A218:A226"/>
-    <mergeCell ref="A199:A217"/>
-    <mergeCell ref="A170:A198"/>
-    <mergeCell ref="A158:A169"/>
+    <mergeCell ref="A220:A228"/>
+    <mergeCell ref="A201:A219"/>
+    <mergeCell ref="A172:A200"/>
+    <mergeCell ref="A158:A171"/>
     <mergeCell ref="A119:A157"/>
-    <mergeCell ref="A233:A240"/>
-    <mergeCell ref="A241:A243"/>
+    <mergeCell ref="A235:A242"/>
+    <mergeCell ref="A243:A245"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change ids of duplicated tasks
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -401,11 +401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E908"/>
+  <dimension ref="A1:E912"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B217" sqref="B217"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,7 +417,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>1335</v>
+        <v>9573</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2110,7 +2110,7 @@
         <v>2166</v>
       </c>
       <c r="C169">
-        <f t="shared" ref="C169:C253" ca="1" si="4">IF(B169=$E$1,1,0)</f>
+        <f t="shared" ref="C169:C257" ca="1" si="4">IF(B169=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2840,7 +2840,7 @@
         <v>1516</v>
       </c>
       <c r="C241">
-        <f t="shared" ref="C241:C249" ca="1" si="5">IF(B241=$E$1,1,0)</f>
+        <f t="shared" ref="C241:C253" ca="1" si="5">IF(B241=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
     <row r="248" spans="1:3">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>3784</v>
+        <v>1212</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
@@ -2919,7 +2919,7 @@
     <row r="249" spans="1:3">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>6732</v>
+        <v>9472</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="5"/>
@@ -2927,101 +2927,101 @@
       </c>
     </row>
     <row r="250" spans="1:3">
-      <c r="A250" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A250" s="1"/>
       <c r="B250">
-        <v>8403</v>
+        <v>5081</v>
       </c>
       <c r="C250">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="1"/>
       <c r="B251">
-        <v>3185</v>
+        <v>6882</v>
       </c>
       <c r="C251">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="1"/>
       <c r="B252">
-        <v>9914</v>
+        <v>3784</v>
       </c>
       <c r="C252">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>6011</v>
+        <v>6732</v>
       </c>
       <c r="C253">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:3">
-      <c r="A254" s="1"/>
+      <c r="A254" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B254">
-        <v>6037</v>
+        <v>8403</v>
       </c>
       <c r="C254">
-        <f t="shared" ref="C254:C317" ca="1" si="6">IF(B254=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="1"/>
       <c r="B255">
-        <v>2809</v>
+        <v>3185</v>
       </c>
       <c r="C255">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="1"/>
       <c r="B256">
-        <v>7297</v>
+        <v>9914</v>
       </c>
       <c r="C256">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="1"/>
       <c r="B257">
-        <v>5242</v>
+        <v>6011</v>
       </c>
       <c r="C257">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="1"/>
       <c r="B258">
-        <v>1379</v>
+        <v>6037</v>
       </c>
       <c r="C258">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C258:C321" ca="1" si="6">IF(B258=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="1"/>
       <c r="B259">
-        <v>2401</v>
+        <v>2809</v>
       </c>
       <c r="C259">
         <f t="shared" ca="1" si="6"/>
@@ -3031,7 +3031,7 @@
     <row r="260" spans="1:3">
       <c r="A260" s="1"/>
       <c r="B260">
-        <v>5421</v>
+        <v>7297</v>
       </c>
       <c r="C260">
         <f t="shared" ca="1" si="6"/>
@@ -3041,7 +3041,7 @@
     <row r="261" spans="1:3">
       <c r="A261" s="1"/>
       <c r="B261">
-        <v>7301</v>
+        <v>5242</v>
       </c>
       <c r="C261">
         <f t="shared" ca="1" si="6"/>
@@ -3051,7 +3051,7 @@
     <row r="262" spans="1:3">
       <c r="A262" s="1"/>
       <c r="B262">
-        <v>2000</v>
+        <v>1379</v>
       </c>
       <c r="C262">
         <f t="shared" ca="1" si="6"/>
@@ -3061,7 +3061,7 @@
     <row r="263" spans="1:3">
       <c r="A263" s="1"/>
       <c r="B263">
-        <v>4147</v>
+        <v>2401</v>
       </c>
       <c r="C263">
         <f t="shared" ca="1" si="6"/>
@@ -3071,7 +3071,7 @@
     <row r="264" spans="1:3">
       <c r="A264" s="1"/>
       <c r="B264">
-        <v>1953</v>
+        <v>5421</v>
       </c>
       <c r="C264">
         <f t="shared" ca="1" si="6"/>
@@ -3081,7 +3081,7 @@
     <row r="265" spans="1:3">
       <c r="A265" s="1"/>
       <c r="B265">
-        <v>3956</v>
+        <v>7301</v>
       </c>
       <c r="C265">
         <f t="shared" ca="1" si="6"/>
@@ -3091,7 +3091,7 @@
     <row r="266" spans="1:3">
       <c r="A266" s="1"/>
       <c r="B266">
-        <v>5463</v>
+        <v>2000</v>
       </c>
       <c r="C266">
         <f t="shared" ca="1" si="6"/>
@@ -3099,11 +3099,9 @@
       </c>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" t="s">
-        <v>14</v>
-      </c>
+      <c r="A267" s="1"/>
       <c r="B267">
-        <v>8787</v>
+        <v>4147</v>
       </c>
       <c r="C267">
         <f t="shared" ca="1" si="6"/>
@@ -3111,24 +3109,42 @@
       </c>
     </row>
     <row r="268" spans="1:3">
+      <c r="A268" s="1"/>
+      <c r="B268">
+        <v>1953</v>
+      </c>
       <c r="C268">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:3">
+      <c r="A269" s="1"/>
+      <c r="B269">
+        <v>3956</v>
+      </c>
       <c r="C269">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:3">
+      <c r="A270" s="1"/>
+      <c r="B270">
+        <v>5463</v>
+      </c>
       <c r="C270">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>14</v>
+      </c>
+      <c r="B271">
+        <v>8787</v>
+      </c>
       <c r="C271">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3412,31 +3428,31 @@
     </row>
     <row r="318" spans="3:3">
       <c r="C318">
-        <f t="shared" ref="C318:C381" ca="1" si="7">IF(B318=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="319" spans="3:3">
       <c r="C319">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="320" spans="3:3">
       <c r="C320">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="3:3">
       <c r="C321">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="322" spans="3:3">
       <c r="C322">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C322:C385" ca="1" si="7">IF(B322=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3796,31 +3812,31 @@
     </row>
     <row r="382" spans="3:3">
       <c r="C382">
-        <f t="shared" ref="C382:C445" ca="1" si="8">IF(B382=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="383" spans="3:3">
       <c r="C383">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="384" spans="3:3">
       <c r="C384">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="385" spans="3:3">
       <c r="C385">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="386" spans="3:3">
       <c r="C386">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C386:C449" ca="1" si="8">IF(B386=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4180,31 +4196,31 @@
     </row>
     <row r="446" spans="3:3">
       <c r="C446">
-        <f t="shared" ref="C446:C509" ca="1" si="9">IF(B446=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="447" spans="3:3">
       <c r="C447">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="448" spans="3:3">
       <c r="C448">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="449" spans="3:3">
       <c r="C449">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="450" spans="3:3">
       <c r="C450">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C450:C513" ca="1" si="9">IF(B450=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4564,31 +4580,31 @@
     </row>
     <row r="510" spans="3:3">
       <c r="C510">
-        <f t="shared" ref="C510:C573" ca="1" si="10">IF(B510=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="511" spans="3:3">
       <c r="C511">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="512" spans="3:3">
       <c r="C512">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="513" spans="3:3">
       <c r="C513">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="514" spans="3:3">
       <c r="C514">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C514:C577" ca="1" si="10">IF(B514=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4948,31 +4964,31 @@
     </row>
     <row r="574" spans="3:3">
       <c r="C574">
-        <f t="shared" ref="C574:C637" ca="1" si="11">IF(B574=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="575" spans="3:3">
       <c r="C575">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="576" spans="3:3">
       <c r="C576">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="577" spans="3:3">
       <c r="C577">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="578" spans="3:3">
       <c r="C578">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C578:C641" ca="1" si="11">IF(B578=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5332,31 +5348,31 @@
     </row>
     <row r="638" spans="3:3">
       <c r="C638">
-        <f t="shared" ref="C638:C701" ca="1" si="12">IF(B638=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="639" spans="3:3">
       <c r="C639">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="640" spans="3:3">
       <c r="C640">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="641" spans="3:3">
       <c r="C641">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="642" spans="3:3">
       <c r="C642">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C642:C705" ca="1" si="12">IF(B642=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5716,31 +5732,31 @@
     </row>
     <row r="702" spans="3:3">
       <c r="C702">
-        <f t="shared" ref="C702:C765" ca="1" si="13">IF(B702=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="703" spans="3:3">
       <c r="C703">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="704" spans="3:3">
       <c r="C704">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="705" spans="3:3">
       <c r="C705">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="706" spans="3:3">
       <c r="C706">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C706:C769" ca="1" si="13">IF(B706=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6100,31 +6116,31 @@
     </row>
     <row r="766" spans="3:3">
       <c r="C766">
-        <f t="shared" ref="C766:C829" ca="1" si="14">IF(B766=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="767" spans="3:3">
       <c r="C767">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="768" spans="3:3">
       <c r="C768">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="769" spans="3:3">
       <c r="C769">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="770" spans="3:3">
       <c r="C770">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C770:C833" ca="1" si="14">IF(B770=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6484,31 +6500,31 @@
     </row>
     <row r="830" spans="3:3">
       <c r="C830">
-        <f t="shared" ref="C830:C893" ca="1" si="15">IF(B830=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="831" spans="3:3">
       <c r="C831">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="832" spans="3:3">
       <c r="C832">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="833" spans="3:3">
       <c r="C833">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="834" spans="3:3">
       <c r="C834">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C834:C897" ca="1" si="15">IF(B834=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6868,31 +6884,31 @@
     </row>
     <row r="894" spans="3:3">
       <c r="C894">
-        <f t="shared" ref="C894:C908" ca="1" si="16">IF(B894=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="895" spans="3:3">
       <c r="C895">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="896" spans="3:3">
       <c r="C896">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="897" spans="3:3">
       <c r="C897">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="898" spans="3:3">
       <c r="C898">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C898:C912" ca="1" si="16">IF(B898=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6956,10 +6972,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="909" spans="3:3">
+      <c r="C909">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="910" spans="3:3">
+      <c r="C910">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="911" spans="3:3">
+      <c r="C911">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="912" spans="3:3">
+      <c r="C912">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A233:A238"/>
-    <mergeCell ref="A250:A266"/>
+    <mergeCell ref="A254:A270"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
@@ -6971,7 +7011,7 @@
     <mergeCell ref="A158:A171"/>
     <mergeCell ref="A119:A157"/>
     <mergeCell ref="A239:A246"/>
-    <mergeCell ref="A247:A249"/>
+    <mergeCell ref="A247:A253"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
prototype refactoring add 1 task to lab16
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -408,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B282" sqref="B282"/>
+      <selection pane="bottomLeft" activeCell="A281" sqref="A281:A282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,7 +420,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>4718</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3244,7 +3244,7 @@
       </c>
     </row>
     <row r="281" spans="1:3">
-      <c r="A281" t="s">
+      <c r="A281" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B281">
@@ -3256,6 +3256,10 @@
       </c>
     </row>
     <row r="282" spans="1:3">
+      <c r="A282" s="1"/>
+      <c r="B282">
+        <v>2070</v>
+      </c>
       <c r="C282">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7072,7 +7076,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A281:A282"/>
     <mergeCell ref="A276:A280"/>
     <mergeCell ref="A237:A242"/>
     <mergeCell ref="A258:A275"/>

</xml_diff>

<commit_message>
add 1 task to lab16
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -408,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281:A282"/>
+      <selection pane="bottomLeft" activeCell="A281" sqref="A281:A283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,7 +420,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3916</v>
+        <v>6111</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3266,6 +3266,10 @@
       </c>
     </row>
     <row r="283" spans="1:3">
+      <c r="A283" s="1"/>
+      <c r="B283">
+        <v>7693</v>
+      </c>
       <c r="C283">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7077,7 +7081,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A281:A282"/>
+    <mergeCell ref="A281:A283"/>
     <mergeCell ref="A276:A280"/>
     <mergeCell ref="A237:A242"/>
     <mergeCell ref="A258:A275"/>

</xml_diff>

<commit_message>
add 2 more task to lab16
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -408,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281:A283"/>
+      <selection pane="bottomLeft" activeCell="A281" sqref="A281:A285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,7 +420,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>6111</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3276,12 +3276,20 @@
       </c>
     </row>
     <row r="284" spans="1:3">
+      <c r="A284" s="1"/>
+      <c r="B284">
+        <v>8718</v>
+      </c>
       <c r="C284">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:3">
+      <c r="A285" s="1"/>
+      <c r="B285">
+        <v>7248</v>
+      </c>
       <c r="C285">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7081,7 +7089,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A281:A283"/>
+    <mergeCell ref="A281:A285"/>
     <mergeCell ref="A276:A280"/>
     <mergeCell ref="A237:A242"/>
     <mergeCell ref="A258:A275"/>

</xml_diff>

<commit_message>
add task to lab06 about defining pattern in sequences of numbers
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -406,11 +406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E918"/>
+  <dimension ref="A1:E919"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B256" sqref="B256"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +422,7 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>6308</v>
+        <v>9763</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>7991</v>
       </c>
       <c r="C98">
-        <f t="shared" ref="C98:C171" ca="1" si="3">IF(B98=$E$1,1,0)</f>
+        <f t="shared" ref="C98:C172" ca="1" si="3">IF(B98=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121">
-        <v>1315</v>
+        <v>1881</v>
       </c>
       <c r="C121">
         <f t="shared" ca="1" si="3"/>
@@ -1640,7 +1640,7 @@
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122">
-        <v>6066</v>
+        <v>1315</v>
       </c>
       <c r="C122">
         <f t="shared" ca="1" si="3"/>
@@ -1650,7 +1650,7 @@
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123">
-        <v>2565</v>
+        <v>6066</v>
       </c>
       <c r="C123">
         <f t="shared" ca="1" si="3"/>
@@ -1660,7 +1660,7 @@
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124">
-        <v>2594</v>
+        <v>2565</v>
       </c>
       <c r="C124">
         <f t="shared" ca="1" si="3"/>
@@ -1670,7 +1670,7 @@
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125">
-        <v>3762</v>
+        <v>2594</v>
       </c>
       <c r="C125">
         <f t="shared" ca="1" si="3"/>
@@ -1680,7 +1680,7 @@
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126">
-        <v>3550</v>
+        <v>3762</v>
       </c>
       <c r="C126">
         <f t="shared" ca="1" si="3"/>
@@ -1690,7 +1690,7 @@
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127">
-        <v>2475</v>
+        <v>3550</v>
       </c>
       <c r="C127">
         <f t="shared" ca="1" si="3"/>
@@ -1700,7 +1700,7 @@
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128">
-        <v>9180</v>
+        <v>2475</v>
       </c>
       <c r="C128">
         <f t="shared" ca="1" si="3"/>
@@ -1710,7 +1710,7 @@
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129">
-        <v>1544</v>
+        <v>9180</v>
       </c>
       <c r="C129">
         <f t="shared" ca="1" si="3"/>
@@ -1720,7 +1720,7 @@
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130">
-        <v>9562</v>
+        <v>1544</v>
       </c>
       <c r="C130">
         <f t="shared" ca="1" si="3"/>
@@ -1730,7 +1730,7 @@
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131">
-        <v>3669</v>
+        <v>9562</v>
       </c>
       <c r="C131">
         <f t="shared" ca="1" si="3"/>
@@ -1740,7 +1740,7 @@
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132">
-        <v>5951</v>
+        <v>3669</v>
       </c>
       <c r="C132">
         <f t="shared" ca="1" si="3"/>
@@ -1750,7 +1750,7 @@
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133">
-        <v>2802</v>
+        <v>5951</v>
       </c>
       <c r="C133">
         <f t="shared" ca="1" si="3"/>
@@ -1760,7 +1760,7 @@
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134">
-        <v>6580</v>
+        <v>2802</v>
       </c>
       <c r="C134">
         <f t="shared" ca="1" si="3"/>
@@ -1770,7 +1770,7 @@
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135">
-        <v>7585</v>
+        <v>6580</v>
       </c>
       <c r="C135">
         <f t="shared" ca="1" si="3"/>
@@ -1780,7 +1780,7 @@
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136">
-        <v>2321</v>
+        <v>7585</v>
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="3"/>
@@ -1790,7 +1790,7 @@
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137">
-        <v>5053</v>
+        <v>2321</v>
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="3"/>
@@ -1800,7 +1800,7 @@
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138">
-        <v>3983</v>
+        <v>5053</v>
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="3"/>
@@ -1810,7 +1810,7 @@
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139">
-        <v>8770</v>
+        <v>3983</v>
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="3"/>
@@ -1820,7 +1820,7 @@
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140">
-        <v>4236</v>
+        <v>8770</v>
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="3"/>
@@ -1830,7 +1830,7 @@
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141">
-        <v>5969</v>
+        <v>4236</v>
       </c>
       <c r="C141">
         <f t="shared" ca="1" si="3"/>
@@ -1840,7 +1840,7 @@
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142">
-        <v>8696</v>
+        <v>5969</v>
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="3"/>
@@ -1850,7 +1850,7 @@
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143">
-        <v>1483</v>
+        <v>8696</v>
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="3"/>
@@ -1860,7 +1860,7 @@
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144">
-        <v>8418</v>
+        <v>1483</v>
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="3"/>
@@ -1870,7 +1870,7 @@
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145">
-        <v>8395</v>
+        <v>8418</v>
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="3"/>
@@ -1880,7 +1880,7 @@
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146">
-        <v>5170</v>
+        <v>8395</v>
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="3"/>
@@ -1890,7 +1890,7 @@
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147">
-        <v>5568</v>
+        <v>5170</v>
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="3"/>
@@ -1900,7 +1900,7 @@
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148">
-        <v>2592</v>
+        <v>5568</v>
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="3"/>
@@ -1910,7 +1910,7 @@
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149">
-        <v>4075</v>
+        <v>2592</v>
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="3"/>
@@ -1920,7 +1920,7 @@
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150">
-        <v>7517</v>
+        <v>4075</v>
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="3"/>
@@ -1930,7 +1930,7 @@
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151">
-        <v>5448</v>
+        <v>7517</v>
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="3"/>
@@ -1940,7 +1940,7 @@
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152">
-        <v>6572</v>
+        <v>5448</v>
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="3"/>
@@ -1950,7 +1950,7 @@
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153">
-        <v>5238</v>
+        <v>6572</v>
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="3"/>
@@ -1960,7 +1960,7 @@
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154">
-        <v>2084</v>
+        <v>5238</v>
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="3"/>
@@ -1970,7 +1970,7 @@
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155">
-        <v>5411</v>
+        <v>2084</v>
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="3"/>
@@ -1980,7 +1980,7 @@
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156">
-        <v>5171</v>
+        <v>5411</v>
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="3"/>
@@ -1990,7 +1990,7 @@
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157">
-        <v>1862</v>
+        <v>5171</v>
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="3"/>
@@ -1998,11 +1998,9 @@
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A158" s="1"/>
       <c r="B158">
-        <v>8165</v>
+        <v>1862</v>
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="3"/>
@@ -2010,9 +2008,11 @@
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B159">
-        <v>9001</v>
+        <v>8165</v>
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="3"/>
@@ -2022,7 +2022,7 @@
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160">
-        <v>9631</v>
+        <v>9001</v>
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="3"/>
@@ -2032,7 +2032,7 @@
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161">
-        <v>9812</v>
+        <v>9631</v>
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="3"/>
@@ -2042,7 +2042,7 @@
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162">
-        <v>4845</v>
+        <v>9812</v>
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="3"/>
@@ -2052,7 +2052,7 @@
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163">
-        <v>5728</v>
+        <v>4845</v>
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="3"/>
@@ -2062,7 +2062,7 @@
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164">
-        <v>1618</v>
+        <v>5728</v>
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="3"/>
@@ -2072,7 +2072,7 @@
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165">
-        <v>9279</v>
+        <v>1618</v>
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="3"/>
@@ -2082,7 +2082,7 @@
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166">
-        <v>6599</v>
+        <v>9279</v>
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="3"/>
@@ -2092,7 +2092,7 @@
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167">
-        <v>7222</v>
+        <v>6599</v>
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="3"/>
@@ -2102,7 +2102,7 @@
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168">
-        <v>3657</v>
+        <v>7222</v>
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="3"/>
@@ -2112,7 +2112,7 @@
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169">
-        <v>7491</v>
+        <v>3657</v>
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="3"/>
@@ -2122,7 +2122,7 @@
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170">
-        <v>5923</v>
+        <v>7491</v>
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="3"/>
@@ -2132,7 +2132,7 @@
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="3"/>
@@ -2142,49 +2142,49 @@
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C172">
-        <f t="shared" ref="C172:C262" ca="1" si="4">IF(B172=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C173">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="C173:C263" ca="1" si="4">IF(B173=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174">
+        <v>9116</v>
+      </c>
+      <c r="C174">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+      <c r="B175">
         <v>9925</v>
       </c>
-      <c r="C174">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
+      <c r="C175">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B175">
+      <c r="B176">
         <v>2885</v>
-      </c>
-      <c r="C175">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
-      <c r="B176">
-        <v>9931</v>
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="4"/>
@@ -2194,7 +2194,7 @@
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177">
-        <v>4425</v>
+        <v>9931</v>
       </c>
       <c r="C177">
         <f t="shared" ca="1" si="4"/>
@@ -2204,7 +2204,7 @@
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178">
-        <v>1947</v>
+        <v>4425</v>
       </c>
       <c r="C178">
         <f t="shared" ca="1" si="4"/>
@@ -2214,7 +2214,7 @@
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179">
-        <v>9696</v>
+        <v>1947</v>
       </c>
       <c r="C179">
         <f t="shared" ca="1" si="4"/>
@@ -2224,7 +2224,7 @@
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180">
-        <v>1223</v>
+        <v>9696</v>
       </c>
       <c r="C180">
         <f t="shared" ca="1" si="4"/>
@@ -2234,7 +2234,7 @@
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181">
-        <v>3946</v>
+        <v>1223</v>
       </c>
       <c r="C181">
         <f t="shared" ca="1" si="4"/>
@@ -2244,7 +2244,7 @@
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182">
-        <v>8311</v>
+        <v>3946</v>
       </c>
       <c r="C182">
         <f t="shared" ca="1" si="4"/>
@@ -2254,7 +2254,7 @@
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C183">
         <f t="shared" ca="1" si="4"/>
@@ -2264,7 +2264,7 @@
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184">
-        <v>9774</v>
+        <v>3134</v>
       </c>
       <c r="C184">
         <f t="shared" ca="1" si="4"/>
@@ -2274,7 +2274,7 @@
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185">
-        <v>9711</v>
+        <v>9774</v>
       </c>
       <c r="C185">
         <f t="shared" ca="1" si="4"/>
@@ -2284,7 +2284,7 @@
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C186">
         <f t="shared" ca="1" si="4"/>
@@ -2294,7 +2294,7 @@
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187">
-        <v>7290</v>
+        <v>3333</v>
       </c>
       <c r="C187">
         <f t="shared" ca="1" si="4"/>
@@ -2304,7 +2304,7 @@
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188">
-        <v>5694</v>
+        <v>7290</v>
       </c>
       <c r="C188">
         <f t="shared" ca="1" si="4"/>
@@ -2314,7 +2314,7 @@
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189">
-        <v>7035</v>
+        <v>5694</v>
       </c>
       <c r="C189">
         <f t="shared" ca="1" si="4"/>
@@ -2324,7 +2324,7 @@
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190">
-        <v>6806</v>
+        <v>7035</v>
       </c>
       <c r="C190">
         <f t="shared" ca="1" si="4"/>
@@ -2334,7 +2334,7 @@
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191">
-        <v>4515</v>
+        <v>6806</v>
       </c>
       <c r="C191">
         <f t="shared" ca="1" si="4"/>
@@ -2344,7 +2344,7 @@
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192">
-        <v>9271</v>
+        <v>4515</v>
       </c>
       <c r="C192">
         <f t="shared" ca="1" si="4"/>
@@ -2354,7 +2354,7 @@
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C193">
         <f t="shared" ca="1" si="4"/>
@@ -2364,7 +2364,7 @@
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C194">
         <f t="shared" ca="1" si="4"/>
@@ -2374,7 +2374,7 @@
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195">
-        <v>3940</v>
+        <v>4497</v>
       </c>
       <c r="C195">
         <f t="shared" ca="1" si="4"/>
@@ -2384,7 +2384,7 @@
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196">
-        <v>8820</v>
+        <v>3940</v>
       </c>
       <c r="C196">
         <f t="shared" ca="1" si="4"/>
@@ -2394,7 +2394,7 @@
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197">
-        <v>3218</v>
+        <v>8820</v>
       </c>
       <c r="C197">
         <f t="shared" ca="1" si="4"/>
@@ -2404,7 +2404,7 @@
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198">
-        <v>4283</v>
+        <v>3218</v>
       </c>
       <c r="C198">
         <f t="shared" ca="1" si="4"/>
@@ -2414,27 +2414,27 @@
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199">
-        <v>7703</v>
+        <v>4283</v>
       </c>
       <c r="C199">
-        <f ca="1">IF(B199=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200">
-        <v>9182</v>
+        <v>7703</v>
       </c>
       <c r="C200">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(B200=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201">
-        <v>5541</v>
+        <v>9182</v>
       </c>
       <c r="C201">
         <f t="shared" ca="1" si="4"/>
@@ -2444,7 +2444,7 @@
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202">
-        <v>2386</v>
+        <v>5541</v>
       </c>
       <c r="C202">
         <f t="shared" ca="1" si="4"/>
@@ -2454,29 +2454,29 @@
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203">
+        <v>2386</v>
+      </c>
+      <c r="C203">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+      <c r="B204">
         <v>9159</v>
       </c>
-      <c r="C203">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
+      <c r="C204">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B204">
+      <c r="B205">
         <v>6175</v>
-      </c>
-      <c r="C204">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="1"/>
-      <c r="B205">
-        <v>4642</v>
       </c>
       <c r="C205">
         <f t="shared" ca="1" si="4"/>
@@ -2486,7 +2486,7 @@
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206">
-        <v>4488</v>
+        <v>4642</v>
       </c>
       <c r="C206">
         <f t="shared" ca="1" si="4"/>
@@ -2496,7 +2496,7 @@
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207">
-        <v>9765</v>
+        <v>4488</v>
       </c>
       <c r="C207">
         <f t="shared" ca="1" si="4"/>
@@ -2506,7 +2506,7 @@
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208">
-        <v>4954</v>
+        <v>9765</v>
       </c>
       <c r="C208">
         <f t="shared" ca="1" si="4"/>
@@ -2516,7 +2516,7 @@
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C209">
         <f t="shared" ca="1" si="4"/>
@@ -2526,7 +2526,7 @@
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210">
-        <v>6431</v>
+        <v>5537</v>
       </c>
       <c r="C210">
         <f t="shared" ca="1" si="4"/>
@@ -2536,7 +2536,7 @@
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211">
-        <v>7193</v>
+        <v>6431</v>
       </c>
       <c r="C211">
         <f t="shared" ca="1" si="4"/>
@@ -2546,7 +2546,7 @@
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212">
-        <v>5621</v>
+        <v>7193</v>
       </c>
       <c r="C212">
         <f t="shared" ca="1" si="4"/>
@@ -2556,7 +2556,7 @@
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213">
-        <v>5847</v>
+        <v>5621</v>
       </c>
       <c r="C213">
         <f t="shared" ca="1" si="4"/>
@@ -2566,7 +2566,7 @@
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C214">
         <f t="shared" ca="1" si="4"/>
@@ -2576,7 +2576,7 @@
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C215">
         <f t="shared" ca="1" si="4"/>
@@ -2586,7 +2586,7 @@
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216">
-        <v>3226</v>
+        <v>9930</v>
       </c>
       <c r="C216">
         <f t="shared" ca="1" si="4"/>
@@ -2596,7 +2596,7 @@
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217">
-        <v>6861</v>
+        <v>3226</v>
       </c>
       <c r="C217">
         <f t="shared" ca="1" si="4"/>
@@ -2606,7 +2606,7 @@
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218">
-        <v>5032</v>
+        <v>6861</v>
       </c>
       <c r="C218">
         <f t="shared" ca="1" si="4"/>
@@ -2616,7 +2616,7 @@
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219">
-        <v>2033</v>
+        <v>5032</v>
       </c>
       <c r="C219">
         <f t="shared" ca="1" si="4"/>
@@ -2626,7 +2626,7 @@
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220">
-        <v>5108</v>
+        <v>2033</v>
       </c>
       <c r="C220">
         <f t="shared" ca="1" si="4"/>
@@ -2636,7 +2636,7 @@
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221">
-        <v>3567</v>
+        <v>5108</v>
       </c>
       <c r="C221">
         <f t="shared" ca="1" si="4"/>
@@ -2646,7 +2646,7 @@
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222">
-        <v>2205</v>
+        <v>3567</v>
       </c>
       <c r="C222">
         <f t="shared" ca="1" si="4"/>
@@ -2656,7 +2656,7 @@
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223">
-        <v>4372</v>
+        <v>2205</v>
       </c>
       <c r="C223">
         <f t="shared" ca="1" si="4"/>
@@ -2666,7 +2666,7 @@
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C224">
         <f t="shared" ca="1" si="4"/>
@@ -2676,7 +2676,7 @@
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C225">
         <f t="shared" ca="1" si="4"/>
@@ -2686,29 +2686,29 @@
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226">
+        <v>1668</v>
+      </c>
+      <c r="C226">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="1"/>
+      <c r="B227">
         <v>2137</v>
       </c>
-      <c r="C226">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
+      <c r="C227">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B227">
+      <c r="B228">
         <v>9300</v>
-      </c>
-      <c r="C227">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="1"/>
-      <c r="B228">
-        <v>3951</v>
       </c>
       <c r="C228">
         <f t="shared" ca="1" si="4"/>
@@ -2718,7 +2718,7 @@
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229">
-        <v>6409</v>
+        <v>3951</v>
       </c>
       <c r="C229">
         <f t="shared" ca="1" si="4"/>
@@ -2728,7 +2728,7 @@
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230">
-        <v>3290</v>
+        <v>6409</v>
       </c>
       <c r="C230">
         <f t="shared" ca="1" si="4"/>
@@ -2738,7 +2738,7 @@
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231">
-        <v>4342</v>
+        <v>3290</v>
       </c>
       <c r="C231">
         <f t="shared" ca="1" si="4"/>
@@ -2748,7 +2748,7 @@
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232">
-        <v>5309</v>
+        <v>4342</v>
       </c>
       <c r="C232">
         <f t="shared" ca="1" si="4"/>
@@ -2758,7 +2758,7 @@
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233">
-        <v>5345</v>
+        <v>5309</v>
       </c>
       <c r="C233">
         <f t="shared" ca="1" si="4"/>
@@ -2768,7 +2768,7 @@
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234">
-        <v>6812</v>
+        <v>5345</v>
       </c>
       <c r="C234">
         <f t="shared" ca="1" si="4"/>
@@ -2778,7 +2778,7 @@
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235">
-        <v>7343</v>
+        <v>6812</v>
       </c>
       <c r="C235">
         <f t="shared" ca="1" si="4"/>
@@ -2788,29 +2788,29 @@
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236">
+        <v>7343</v>
+      </c>
+      <c r="C236">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="1"/>
+      <c r="B237">
         <v>7060</v>
       </c>
-      <c r="C236">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
+      <c r="C237">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B237">
+      <c r="B238">
         <v>9299</v>
-      </c>
-      <c r="C237">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="1"/>
-      <c r="B238">
-        <v>7560</v>
       </c>
       <c r="C238">
         <f t="shared" ca="1" si="4"/>
@@ -2820,7 +2820,7 @@
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C239">
         <f t="shared" ca="1" si="4"/>
@@ -2830,7 +2830,7 @@
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C240">
         <f t="shared" ca="1" si="4"/>
@@ -2840,7 +2840,7 @@
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C241">
         <f t="shared" ca="1" si="4"/>
@@ -2850,29 +2850,29 @@
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242">
+        <v>1954</v>
+      </c>
+      <c r="C242">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1"/>
+      <c r="B243">
         <v>2048</v>
       </c>
-      <c r="C242">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
+      <c r="C243">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B243">
+      <c r="B244">
         <v>3939</v>
-      </c>
-      <c r="C243">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="1"/>
-      <c r="B244">
-        <v>8861</v>
       </c>
       <c r="C244">
         <f t="shared" ca="1" si="4"/>
@@ -2882,27 +2882,27 @@
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245">
-        <v>1516</v>
+        <v>8861</v>
       </c>
       <c r="C245">
-        <f t="shared" ref="C245:C258" ca="1" si="5">IF(B245=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C246">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ref="C246:C259" ca="1" si="5">IF(B246=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247">
-        <v>5164</v>
+        <v>9062</v>
       </c>
       <c r="C247">
         <f t="shared" ca="1" si="5"/>
@@ -2912,7 +2912,7 @@
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248">
-        <v>2030</v>
+        <v>5164</v>
       </c>
       <c r="C248">
         <f t="shared" ca="1" si="5"/>
@@ -2922,7 +2922,7 @@
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249">
-        <v>7649</v>
+        <v>2030</v>
       </c>
       <c r="C249">
         <f t="shared" ca="1" si="5"/>
@@ -2932,7 +2932,7 @@
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250">
-        <v>2354</v>
+        <v>7649</v>
       </c>
       <c r="C250">
         <f t="shared" ca="1" si="5"/>
@@ -2940,11 +2940,9 @@
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A251" s="1"/>
       <c r="B251">
-        <v>9701</v>
+        <v>2354</v>
       </c>
       <c r="C251">
         <f t="shared" ca="1" si="5"/>
@@ -2952,9 +2950,11 @@
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="1"/>
+      <c r="A252" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B252">
-        <v>1212</v>
+        <v>9701</v>
       </c>
       <c r="C252">
         <f t="shared" ca="1" si="5"/>
@@ -2964,7 +2964,7 @@
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C253">
         <f t="shared" ca="1" si="5"/>
@@ -2974,7 +2974,7 @@
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C254">
         <f t="shared" ca="1" si="5"/>
@@ -2984,7 +2984,7 @@
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255">
-        <v>6454</v>
+        <v>5081</v>
       </c>
       <c r="C255">
         <f t="shared" ca="1" si="5"/>
@@ -2994,7 +2994,7 @@
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256">
-        <v>6882</v>
+        <v>6454</v>
       </c>
       <c r="C256">
         <f t="shared" ca="1" si="5"/>
@@ -3004,7 +3004,7 @@
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257">
-        <v>3784</v>
+        <v>6882</v>
       </c>
       <c r="C257">
         <f t="shared" ca="1" si="5"/>
@@ -3014,7 +3014,7 @@
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C258">
         <f t="shared" ca="1" si="5"/>
@@ -3022,21 +3022,21 @@
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
+      <c r="A259" s="1"/>
+      <c r="B259">
+        <v>6732</v>
+      </c>
+      <c r="C259">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B259">
+      <c r="B260">
         <v>8403</v>
-      </c>
-      <c r="C259">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="1"/>
-      <c r="B260">
-        <v>3185</v>
       </c>
       <c r="C260">
         <f t="shared" ca="1" si="4"/>
@@ -3046,7 +3046,7 @@
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C261">
         <f t="shared" ca="1" si="4"/>
@@ -3056,7 +3056,7 @@
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C262">
         <f t="shared" ca="1" si="4"/>
@@ -3066,27 +3066,27 @@
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C263">
-        <f t="shared" ref="C263:C327" ca="1" si="6">IF(B263=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C264">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="C264:C328" ca="1" si="6">IF(B264=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C265">
         <f t="shared" ca="1" si="6"/>
@@ -3096,7 +3096,7 @@
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C266">
         <f t="shared" ca="1" si="6"/>
@@ -3106,7 +3106,7 @@
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C267">
         <f t="shared" ca="1" si="6"/>
@@ -3116,7 +3116,7 @@
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C268">
         <f t="shared" ca="1" si="6"/>
@@ -3126,7 +3126,7 @@
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C269">
         <f t="shared" ca="1" si="6"/>
@@ -3136,7 +3136,7 @@
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C270">
         <f t="shared" ca="1" si="6"/>
@@ -3146,7 +3146,7 @@
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271">
-        <v>6981</v>
+        <v>7301</v>
       </c>
       <c r="C271">
         <f t="shared" ca="1" si="6"/>
@@ -3156,7 +3156,7 @@
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272">
-        <v>2000</v>
+        <v>6981</v>
       </c>
       <c r="C272">
         <f t="shared" ca="1" si="6"/>
@@ -3166,7 +3166,7 @@
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273">
-        <v>4147</v>
+        <v>2000</v>
       </c>
       <c r="C273">
         <f t="shared" ca="1" si="6"/>
@@ -3176,7 +3176,7 @@
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C274">
         <f t="shared" ca="1" si="6"/>
@@ -3186,7 +3186,7 @@
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C275">
         <f t="shared" ca="1" si="6"/>
@@ -3196,7 +3196,7 @@
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276">
-        <v>5463</v>
+        <v>3956</v>
       </c>
       <c r="C276">
         <f t="shared" ca="1" si="6"/>
@@ -3204,11 +3204,9 @@
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A277" s="1"/>
       <c r="B277">
-        <v>8787</v>
+        <v>5463</v>
       </c>
       <c r="C277">
         <f t="shared" ca="1" si="6"/>
@@ -3216,9 +3214,11 @@
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" s="1"/>
+      <c r="A278" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B278">
-        <v>5087</v>
+        <v>8787</v>
       </c>
       <c r="C278">
         <f t="shared" ca="1" si="6"/>
@@ -3228,7 +3228,7 @@
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279">
-        <v>9990</v>
+        <v>5087</v>
       </c>
       <c r="C279">
         <f t="shared" ca="1" si="6"/>
@@ -3238,7 +3238,7 @@
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280">
-        <v>9924</v>
+        <v>9990</v>
       </c>
       <c r="C280">
         <f t="shared" ca="1" si="6"/>
@@ -3248,7 +3248,7 @@
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281">
-        <v>7657</v>
+        <v>9924</v>
       </c>
       <c r="C281">
         <f t="shared" ca="1" si="6"/>
@@ -3256,11 +3256,9 @@
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A282" s="1"/>
       <c r="B282">
-        <v>4304</v>
+        <v>7657</v>
       </c>
       <c r="C282">
         <f t="shared" ca="1" si="6"/>
@@ -3268,9 +3266,11 @@
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="1"/>
+      <c r="A283" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B283">
-        <v>2070</v>
+        <v>4304</v>
       </c>
       <c r="C283">
         <f t="shared" ca="1" si="6"/>
@@ -3280,7 +3280,7 @@
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C284">
         <f t="shared" ca="1" si="6"/>
@@ -3290,7 +3290,7 @@
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C285">
         <f t="shared" ca="1" si="6"/>
@@ -3300,7 +3300,7 @@
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286">
-        <v>7248</v>
+        <v>8718</v>
       </c>
       <c r="C286">
         <f t="shared" ca="1" si="6"/>
@@ -3308,6 +3308,10 @@
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="1"/>
+      <c r="B287">
+        <v>7248</v>
+      </c>
       <c r="C287">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -3555,13 +3559,13 @@
     </row>
     <row r="328" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C328">
-        <f t="shared" ref="C328:C391" ca="1" si="7">IF(B328=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="C329:C392" ca="1" si="7">IF(B329=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3939,13 +3943,13 @@
     </row>
     <row r="392" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C392">
-        <f t="shared" ref="C392:C455" ca="1" si="8">IF(B392=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="393" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C393">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="C393:C456" ca="1" si="8">IF(B393=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4323,13 +4327,13 @@
     </row>
     <row r="456" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C456">
-        <f t="shared" ref="C456:C519" ca="1" si="9">IF(B456=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="457" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C457">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="C457:C520" ca="1" si="9">IF(B457=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4707,13 +4711,13 @@
     </row>
     <row r="520" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C520">
-        <f t="shared" ref="C520:C583" ca="1" si="10">IF(B520=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="521" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C521">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="C521:C584" ca="1" si="10">IF(B521=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5091,13 +5095,13 @@
     </row>
     <row r="584" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C584">
-        <f t="shared" ref="C584:C647" ca="1" si="11">IF(B584=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="585" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C585">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="C585:C648" ca="1" si="11">IF(B585=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5475,13 +5479,13 @@
     </row>
     <row r="648" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C648">
-        <f t="shared" ref="C648:C711" ca="1" si="12">IF(B648=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="649" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C649">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="C649:C712" ca="1" si="12">IF(B649=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5859,13 +5863,13 @@
     </row>
     <row r="712" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C712">
-        <f t="shared" ref="C712:C775" ca="1" si="13">IF(B712=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="713" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C713">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="C713:C776" ca="1" si="13">IF(B713=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6243,13 +6247,13 @@
     </row>
     <row r="776" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C776">
-        <f t="shared" ref="C776:C839" ca="1" si="14">IF(B776=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="777" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C777">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="C777:C840" ca="1" si="14">IF(B777=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6627,13 +6631,13 @@
     </row>
     <row r="840" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C840">
-        <f t="shared" ref="C840:C903" ca="1" si="15">IF(B840=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="841" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C841">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="C841:C904" ca="1" si="15">IF(B841=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7011,13 +7015,13 @@
     </row>
     <row r="904" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C904">
-        <f t="shared" ref="C904:C918" ca="1" si="16">IF(B904=$E$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="905" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C905">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="C905:C919" ca="1" si="16">IF(B905=$E$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7099,24 +7103,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="919" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C919">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A282:A286"/>
-    <mergeCell ref="A277:A281"/>
-    <mergeCell ref="A237:A242"/>
-    <mergeCell ref="A259:A276"/>
+    <mergeCell ref="A283:A287"/>
+    <mergeCell ref="A278:A282"/>
+    <mergeCell ref="A238:A243"/>
+    <mergeCell ref="A260:A277"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A56"/>
     <mergeCell ref="A57:A72"/>
     <mergeCell ref="A73:A78"/>
     <mergeCell ref="A79:A118"/>
-    <mergeCell ref="A227:A236"/>
-    <mergeCell ref="A204:A226"/>
-    <mergeCell ref="A175:A203"/>
-    <mergeCell ref="A158:A174"/>
-    <mergeCell ref="A119:A157"/>
-    <mergeCell ref="A243:A250"/>
-    <mergeCell ref="A251:A258"/>
+    <mergeCell ref="A228:A237"/>
+    <mergeCell ref="A205:A227"/>
+    <mergeCell ref="A176:A204"/>
+    <mergeCell ref="A159:A175"/>
+    <mergeCell ref="A119:A158"/>
+    <mergeCell ref="A244:A251"/>
+    <mergeCell ref="A252:A259"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add illustration of equals and hashCode
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$270</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$272</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -842,11 +842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W902"/>
+  <dimension ref="A1:W904"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z246" sqref="Z246"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>8000</v>
+        <v>4916</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6383,7 +6383,7 @@
       <c r="S198" s="2"/>
       <c r="T198" s="5"/>
       <c r="U198">
-        <f t="shared" ref="U198:U264" ca="1" si="5">IF(B198=$W$1,1,0)</f>
+        <f t="shared" ref="U198:U266" ca="1" si="5">IF(B198=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7990,7 +7990,7 @@
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="20"/>
       <c r="B256" s="2">
-        <v>4147</v>
+        <v>5449</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8018,7 +8018,7 @@
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="20"/>
       <c r="B257" s="2">
-        <v>1953</v>
+        <v>2662</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8046,7 +8046,7 @@
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="20"/>
       <c r="B258" s="2">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8071,115 +8071,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="21"/>
-      <c r="B259" s="6">
-        <v>8403</v>
-      </c>
-      <c r="C259" s="6"/>
-      <c r="D259" s="6"/>
-      <c r="E259" s="6"/>
-      <c r="F259" s="6"/>
-      <c r="G259" s="6"/>
-      <c r="H259" s="6"/>
-      <c r="I259" s="6"/>
-      <c r="J259" s="6"/>
-      <c r="K259" s="6"/>
-      <c r="L259" s="6"/>
-      <c r="M259" s="6"/>
-      <c r="N259" s="6"/>
-      <c r="O259" s="6"/>
-      <c r="P259" s="6"/>
-      <c r="Q259" s="6"/>
-      <c r="R259" s="6"/>
-      <c r="S259" s="6"/>
-      <c r="T259" s="7"/>
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A259" s="20"/>
+      <c r="B259" s="2">
+        <v>1953</v>
+      </c>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="2"/>
+      <c r="F259" s="2"/>
+      <c r="G259" s="2"/>
+      <c r="H259" s="2"/>
+      <c r="I259" s="2"/>
+      <c r="J259" s="2"/>
+      <c r="K259" s="2"/>
+      <c r="L259" s="2"/>
+      <c r="M259" s="2"/>
+      <c r="N259" s="2"/>
+      <c r="O259" s="2"/>
+      <c r="P259" s="2"/>
+      <c r="Q259" s="2"/>
+      <c r="R259" s="2"/>
+      <c r="S259" s="2"/>
+      <c r="T259" s="5"/>
       <c r="U259">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B260" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C260" s="8"/>
-      <c r="D260" s="8"/>
-      <c r="E260" s="8"/>
-      <c r="F260" s="8"/>
-      <c r="G260" s="8"/>
-      <c r="H260" s="8"/>
-      <c r="I260" s="8"/>
-      <c r="J260" s="8"/>
-      <c r="K260" s="8"/>
-      <c r="L260" s="8"/>
-      <c r="M260" s="8"/>
-      <c r="N260" s="8"/>
-      <c r="O260" s="8"/>
-      <c r="P260" s="8"/>
-      <c r="Q260" s="8"/>
-      <c r="R260" s="8"/>
-      <c r="S260" s="8"/>
-      <c r="T260" s="14"/>
+      <c r="A260" s="20"/>
+      <c r="B260" s="2">
+        <v>3956</v>
+      </c>
+      <c r="C260" s="2"/>
+      <c r="D260" s="2"/>
+      <c r="E260" s="2"/>
+      <c r="F260" s="2"/>
+      <c r="G260" s="2"/>
+      <c r="H260" s="2"/>
+      <c r="I260" s="2"/>
+      <c r="J260" s="2"/>
+      <c r="K260" s="2"/>
+      <c r="L260" s="2"/>
+      <c r="M260" s="2"/>
+      <c r="N260" s="2"/>
+      <c r="O260" s="2"/>
+      <c r="P260" s="2"/>
+      <c r="Q260" s="2"/>
+      <c r="R260" s="2"/>
+      <c r="S260" s="2"/>
+      <c r="T260" s="5"/>
       <c r="U260">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A261" s="20"/>
-      <c r="B261" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C261" s="2"/>
-      <c r="D261" s="2"/>
-      <c r="E261" s="2"/>
-      <c r="F261" s="2"/>
-      <c r="G261" s="2"/>
-      <c r="H261" s="2"/>
-      <c r="I261" s="2"/>
-      <c r="J261" s="2"/>
-      <c r="K261" s="2"/>
-      <c r="L261" s="2"/>
-      <c r="M261" s="2"/>
-      <c r="N261" s="2"/>
-      <c r="O261" s="2"/>
-      <c r="P261" s="2"/>
-      <c r="Q261" s="2"/>
-      <c r="R261" s="2"/>
-      <c r="S261" s="2"/>
-      <c r="T261" s="5"/>
+    <row r="261" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="21"/>
+      <c r="B261" s="6">
+        <v>8403</v>
+      </c>
+      <c r="C261" s="6"/>
+      <c r="D261" s="6"/>
+      <c r="E261" s="6"/>
+      <c r="F261" s="6"/>
+      <c r="G261" s="6"/>
+      <c r="H261" s="6"/>
+      <c r="I261" s="6"/>
+      <c r="J261" s="6"/>
+      <c r="K261" s="6"/>
+      <c r="L261" s="6"/>
+      <c r="M261" s="6"/>
+      <c r="N261" s="6"/>
+      <c r="O261" s="6"/>
+      <c r="P261" s="6"/>
+      <c r="Q261" s="6"/>
+      <c r="R261" s="6"/>
+      <c r="S261" s="6"/>
+      <c r="T261" s="7"/>
       <c r="U261">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="20"/>
-      <c r="B262" s="2">
-        <v>9990</v>
-      </c>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2"/>
-      <c r="E262" s="2"/>
-      <c r="F262" s="2"/>
-      <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
-      <c r="I262" s="2"/>
-      <c r="J262" s="2"/>
-      <c r="K262" s="2"/>
-      <c r="L262" s="2"/>
-      <c r="M262" s="2"/>
-      <c r="N262" s="2"/>
-      <c r="O262" s="2"/>
-      <c r="P262" s="2"/>
-      <c r="Q262" s="2"/>
-      <c r="R262" s="2"/>
-      <c r="S262" s="2"/>
-      <c r="T262" s="5"/>
+      <c r="A262" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B262" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C262" s="8"/>
+      <c r="D262" s="8"/>
+      <c r="E262" s="8"/>
+      <c r="F262" s="8"/>
+      <c r="G262" s="8"/>
+      <c r="H262" s="8"/>
+      <c r="I262" s="8"/>
+      <c r="J262" s="8"/>
+      <c r="K262" s="8"/>
+      <c r="L262" s="8"/>
+      <c r="M262" s="8"/>
+      <c r="N262" s="8"/>
+      <c r="O262" s="8"/>
+      <c r="P262" s="8"/>
+      <c r="Q262" s="8"/>
+      <c r="R262" s="8"/>
+      <c r="S262" s="8"/>
+      <c r="T262" s="14"/>
       <c r="U262">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -8188,7 +8188,7 @@
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="20"/>
       <c r="B263" s="2">
-        <v>7738</v>
+        <v>5087</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8216,7 +8216,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="20"/>
       <c r="B264" s="2">
-        <v>9924</v>
+        <v>9990</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8241,115 +8241,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="21"/>
-      <c r="B265" s="6">
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A265" s="20"/>
+      <c r="B265" s="2">
+        <v>7738</v>
+      </c>
+      <c r="C265" s="2"/>
+      <c r="D265" s="2"/>
+      <c r="E265" s="2"/>
+      <c r="F265" s="2"/>
+      <c r="G265" s="2"/>
+      <c r="H265" s="2"/>
+      <c r="I265" s="2"/>
+      <c r="J265" s="2"/>
+      <c r="K265" s="2"/>
+      <c r="L265" s="2"/>
+      <c r="M265" s="2"/>
+      <c r="N265" s="2"/>
+      <c r="O265" s="2"/>
+      <c r="P265" s="2"/>
+      <c r="Q265" s="2"/>
+      <c r="R265" s="2"/>
+      <c r="S265" s="2"/>
+      <c r="T265" s="5"/>
+      <c r="U265">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A266" s="20"/>
+      <c r="B266" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+      <c r="E266" s="2"/>
+      <c r="F266" s="2"/>
+      <c r="G266" s="2"/>
+      <c r="H266" s="2"/>
+      <c r="I266" s="2"/>
+      <c r="J266" s="2"/>
+      <c r="K266" s="2"/>
+      <c r="L266" s="2"/>
+      <c r="M266" s="2"/>
+      <c r="N266" s="2"/>
+      <c r="O266" s="2"/>
+      <c r="P266" s="2"/>
+      <c r="Q266" s="2"/>
+      <c r="R266" s="2"/>
+      <c r="S266" s="2"/>
+      <c r="T266" s="5"/>
+      <c r="U266">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="21"/>
+      <c r="B267" s="6">
         <v>7657</v>
       </c>
-      <c r="C265" s="6"/>
-      <c r="D265" s="6"/>
-      <c r="E265" s="6"/>
-      <c r="F265" s="6"/>
-      <c r="G265" s="6"/>
-      <c r="H265" s="6"/>
-      <c r="I265" s="6"/>
-      <c r="J265" s="6"/>
-      <c r="K265" s="6"/>
-      <c r="L265" s="6"/>
-      <c r="M265" s="6"/>
-      <c r="N265" s="6"/>
-      <c r="O265" s="6"/>
-      <c r="P265" s="6"/>
-      <c r="Q265" s="6"/>
-      <c r="R265" s="6"/>
-      <c r="S265" s="6"/>
-      <c r="T265" s="7"/>
-      <c r="U265">
-        <f t="shared" ref="U265:U328" ca="1" si="6">IF(B265=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="19" t="s">
+      <c r="C267" s="6"/>
+      <c r="D267" s="6"/>
+      <c r="E267" s="6"/>
+      <c r="F267" s="6"/>
+      <c r="G267" s="6"/>
+      <c r="H267" s="6"/>
+      <c r="I267" s="6"/>
+      <c r="J267" s="6"/>
+      <c r="K267" s="6"/>
+      <c r="L267" s="6"/>
+      <c r="M267" s="6"/>
+      <c r="N267" s="6"/>
+      <c r="O267" s="6"/>
+      <c r="P267" s="6"/>
+      <c r="Q267" s="6"/>
+      <c r="R267" s="6"/>
+      <c r="S267" s="6"/>
+      <c r="T267" s="7"/>
+      <c r="U267">
+        <f t="shared" ref="U267:U330" ca="1" si="6">IF(B267=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A268" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B266" s="8">
+      <c r="B268" s="8">
         <v>4304</v>
       </c>
-      <c r="C266" s="8"/>
-      <c r="D266" s="8"/>
-      <c r="E266" s="8"/>
-      <c r="F266" s="8"/>
-      <c r="G266" s="8"/>
-      <c r="H266" s="8"/>
-      <c r="I266" s="8"/>
-      <c r="J266" s="8"/>
-      <c r="K266" s="8"/>
-      <c r="L266" s="8"/>
-      <c r="M266" s="8"/>
-      <c r="N266" s="8"/>
-      <c r="O266" s="8"/>
-      <c r="P266" s="8"/>
-      <c r="Q266" s="8"/>
-      <c r="R266" s="8"/>
-      <c r="S266" s="8"/>
-      <c r="T266" s="14"/>
-      <c r="U266">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="20"/>
-      <c r="B267" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C267" s="2"/>
-      <c r="D267" s="2"/>
-      <c r="E267" s="2"/>
-      <c r="F267" s="2"/>
-      <c r="G267" s="2"/>
-      <c r="H267" s="2"/>
-      <c r="I267" s="2"/>
-      <c r="J267" s="2"/>
-      <c r="K267" s="2"/>
-      <c r="L267" s="2"/>
-      <c r="M267" s="2"/>
-      <c r="N267" s="2"/>
-      <c r="O267" s="2"/>
-      <c r="P267" s="2"/>
-      <c r="Q267" s="2"/>
-      <c r="R267" s="2"/>
-      <c r="S267" s="2"/>
-      <c r="T267" s="5"/>
-      <c r="U267">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="20"/>
-      <c r="B268" s="2">
-        <v>7693</v>
-      </c>
-      <c r="C268" s="2"/>
-      <c r="D268" s="2"/>
-      <c r="E268" s="2"/>
-      <c r="F268" s="2"/>
-      <c r="G268" s="2"/>
-      <c r="H268" s="2"/>
-      <c r="I268" s="2"/>
-      <c r="J268" s="2"/>
-      <c r="K268" s="2"/>
-      <c r="L268" s="2"/>
-      <c r="M268" s="2"/>
-      <c r="N268" s="2"/>
-      <c r="O268" s="2"/>
-      <c r="P268" s="2"/>
-      <c r="Q268" s="2"/>
-      <c r="R268" s="2"/>
-      <c r="S268" s="2"/>
-      <c r="T268" s="5"/>
+      <c r="C268" s="8"/>
+      <c r="D268" s="8"/>
+      <c r="E268" s="8"/>
+      <c r="F268" s="8"/>
+      <c r="G268" s="8"/>
+      <c r="H268" s="8"/>
+      <c r="I268" s="8"/>
+      <c r="J268" s="8"/>
+      <c r="K268" s="8"/>
+      <c r="L268" s="8"/>
+      <c r="M268" s="8"/>
+      <c r="N268" s="8"/>
+      <c r="O268" s="8"/>
+      <c r="P268" s="8"/>
+      <c r="Q268" s="8"/>
+      <c r="R268" s="8"/>
+      <c r="S268" s="8"/>
+      <c r="T268" s="14"/>
       <c r="U268">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8358,7 +8358,7 @@
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="20"/>
       <c r="B269" s="2">
-        <v>8718</v>
+        <v>2070</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8383,124 +8383,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="21"/>
-      <c r="B270" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C270" s="6"/>
-      <c r="D270" s="6"/>
-      <c r="E270" s="6"/>
-      <c r="F270" s="6"/>
-      <c r="G270" s="6"/>
-      <c r="H270" s="6"/>
-      <c r="I270" s="6"/>
-      <c r="J270" s="6"/>
-      <c r="K270" s="6"/>
-      <c r="L270" s="6"/>
-      <c r="M270" s="6"/>
-      <c r="N270" s="6"/>
-      <c r="O270" s="6"/>
-      <c r="P270" s="6"/>
-      <c r="Q270" s="6"/>
-      <c r="R270" s="6"/>
-      <c r="S270" s="6"/>
-      <c r="T270" s="7"/>
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A270" s="20"/>
+      <c r="B270" s="2">
+        <v>7693</v>
+      </c>
+      <c r="C270" s="2"/>
+      <c r="D270" s="2"/>
+      <c r="E270" s="2"/>
+      <c r="F270" s="2"/>
+      <c r="G270" s="2"/>
+      <c r="H270" s="2"/>
+      <c r="I270" s="2"/>
+      <c r="J270" s="2"/>
+      <c r="K270" s="2"/>
+      <c r="L270" s="2"/>
+      <c r="M270" s="2"/>
+      <c r="N270" s="2"/>
+      <c r="O270" s="2"/>
+      <c r="P270" s="2"/>
+      <c r="Q270" s="2"/>
+      <c r="R270" s="2"/>
+      <c r="S270" s="2"/>
+      <c r="T270" s="5"/>
       <c r="U270">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A271" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B271" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C271" s="8"/>
-      <c r="D271" s="8"/>
-      <c r="E271" s="8"/>
-      <c r="F271" s="8"/>
-      <c r="G271" s="8"/>
-      <c r="H271" s="8"/>
-      <c r="I271" s="8"/>
-      <c r="J271" s="8"/>
-      <c r="K271" s="8"/>
-      <c r="L271" s="8"/>
-      <c r="M271" s="8"/>
-      <c r="N271" s="8"/>
-      <c r="O271" s="8"/>
-      <c r="P271" s="8"/>
-      <c r="Q271" s="8"/>
-      <c r="R271" s="8"/>
-      <c r="S271" s="8"/>
-      <c r="T271" s="14"/>
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A271" s="20"/>
+      <c r="B271" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C271" s="2"/>
+      <c r="D271" s="2"/>
+      <c r="E271" s="2"/>
+      <c r="F271" s="2"/>
+      <c r="G271" s="2"/>
+      <c r="H271" s="2"/>
+      <c r="I271" s="2"/>
+      <c r="J271" s="2"/>
+      <c r="K271" s="2"/>
+      <c r="L271" s="2"/>
+      <c r="M271" s="2"/>
+      <c r="N271" s="2"/>
+      <c r="O271" s="2"/>
+      <c r="P271" s="2"/>
+      <c r="Q271" s="2"/>
+      <c r="R271" s="2"/>
+      <c r="S271" s="2"/>
+      <c r="T271" s="5"/>
       <c r="U271">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A272" s="20"/>
-      <c r="B272" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C272" s="2"/>
-      <c r="D272" s="2"/>
-      <c r="E272" s="2"/>
-      <c r="F272" s="2"/>
-      <c r="G272" s="2"/>
-      <c r="H272" s="2"/>
-      <c r="I272" s="2"/>
-      <c r="J272" s="2"/>
-      <c r="K272" s="2"/>
-      <c r="L272" s="2"/>
-      <c r="M272" s="2"/>
-      <c r="N272" s="2"/>
-      <c r="O272" s="2"/>
-      <c r="P272" s="2"/>
-      <c r="Q272" s="2"/>
-      <c r="R272" s="2"/>
-      <c r="S272" s="2"/>
-      <c r="T272" s="5"/>
+    <row r="272" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="21"/>
+      <c r="B272" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C272" s="6"/>
+      <c r="D272" s="6"/>
+      <c r="E272" s="6"/>
+      <c r="F272" s="6"/>
+      <c r="G272" s="6"/>
+      <c r="H272" s="6"/>
+      <c r="I272" s="6"/>
+      <c r="J272" s="6"/>
+      <c r="K272" s="6"/>
+      <c r="L272" s="6"/>
+      <c r="M272" s="6"/>
+      <c r="N272" s="6"/>
+      <c r="O272" s="6"/>
+      <c r="P272" s="6"/>
+      <c r="Q272" s="6"/>
+      <c r="R272" s="6"/>
+      <c r="S272" s="6"/>
+      <c r="T272" s="7"/>
       <c r="U272">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A273" s="20"/>
-      <c r="B273" s="12">
-        <v>7546</v>
-      </c>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="E273" s="2"/>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="2"/>
-      <c r="J273" s="2"/>
-      <c r="K273" s="2"/>
-      <c r="L273" s="2"/>
-      <c r="M273" s="2"/>
-      <c r="N273" s="2"/>
-      <c r="O273" s="2"/>
-      <c r="P273" s="2"/>
-      <c r="Q273" s="2"/>
-      <c r="R273" s="2"/>
-      <c r="S273" s="2"/>
-      <c r="T273" s="5"/>
+      <c r="A273" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B273" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C273" s="8"/>
+      <c r="D273" s="8"/>
+      <c r="E273" s="8"/>
+      <c r="F273" s="8"/>
+      <c r="G273" s="8"/>
+      <c r="H273" s="8"/>
+      <c r="I273" s="8"/>
+      <c r="J273" s="8"/>
+      <c r="K273" s="8"/>
+      <c r="L273" s="8"/>
+      <c r="M273" s="8"/>
+      <c r="N273" s="8"/>
+      <c r="O273" s="8"/>
+      <c r="P273" s="8"/>
+      <c r="Q273" s="8"/>
+      <c r="R273" s="8"/>
+      <c r="S273" s="8"/>
+      <c r="T273" s="14"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A274" s="20"/>
-      <c r="B274" s="2">
-        <v>7170</v>
+      <c r="B274" s="12">
+        <v>3083</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8525,10 +8525,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A275" s="20"/>
-      <c r="B275" s="2">
-        <v>2709</v>
+      <c r="B275" s="12">
+        <v>7546</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8556,7 +8556,7 @@
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A276" s="20"/>
       <c r="B276" s="2">
-        <v>3402</v>
+        <v>7170</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8584,7 +8584,7 @@
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" s="20"/>
       <c r="B277" s="2">
-        <v>8781</v>
+        <v>2709</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8612,7 +8612,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="20"/>
       <c r="B278" s="2">
-        <v>8771</v>
+        <v>3402</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8640,7 +8640,7 @@
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" s="20"/>
       <c r="B279" s="2">
-        <v>3091</v>
+        <v>8781</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8668,7 +8668,7 @@
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" s="20"/>
       <c r="B280" s="2">
-        <v>2195</v>
+        <v>8771</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8696,7 +8696,7 @@
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="20"/>
       <c r="B281" s="2">
-        <v>1184</v>
+        <v>3091</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8724,7 +8724,7 @@
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="20"/>
       <c r="B282" s="2">
-        <v>2667</v>
+        <v>2195</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8752,7 +8752,7 @@
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" s="20"/>
       <c r="B283" s="2">
-        <v>5917</v>
+        <v>1184</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8780,7 +8780,7 @@
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" s="20"/>
       <c r="B284" s="2">
-        <v>8545</v>
+        <v>2667</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8808,7 +8808,7 @@
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A285" s="20"/>
       <c r="B285" s="2">
-        <v>1288</v>
+        <v>5917</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8833,115 +8833,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="21"/>
-      <c r="B286" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C286" s="6"/>
-      <c r="D286" s="6"/>
-      <c r="E286" s="6"/>
-      <c r="F286" s="6"/>
-      <c r="G286" s="6"/>
-      <c r="H286" s="6"/>
-      <c r="I286" s="6"/>
-      <c r="J286" s="6"/>
-      <c r="K286" s="6"/>
-      <c r="L286" s="6"/>
-      <c r="M286" s="6"/>
-      <c r="N286" s="6"/>
-      <c r="O286" s="6"/>
-      <c r="P286" s="6"/>
-      <c r="Q286" s="6"/>
-      <c r="R286" s="6"/>
-      <c r="S286" s="6"/>
-      <c r="T286" s="7"/>
+    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A286" s="20"/>
+      <c r="B286" s="2">
+        <v>8545</v>
+      </c>
+      <c r="C286" s="2"/>
+      <c r="D286" s="2"/>
+      <c r="E286" s="2"/>
+      <c r="F286" s="2"/>
+      <c r="G286" s="2"/>
+      <c r="H286" s="2"/>
+      <c r="I286" s="2"/>
+      <c r="J286" s="2"/>
+      <c r="K286" s="2"/>
+      <c r="L286" s="2"/>
+      <c r="M286" s="2"/>
+      <c r="N286" s="2"/>
+      <c r="O286" s="2"/>
+      <c r="P286" s="2"/>
+      <c r="Q286" s="2"/>
+      <c r="R286" s="2"/>
+      <c r="S286" s="2"/>
+      <c r="T286" s="5"/>
       <c r="U286">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B287" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C287" s="8"/>
-      <c r="D287" s="8"/>
-      <c r="E287" s="8"/>
-      <c r="F287" s="8"/>
-      <c r="G287" s="8"/>
-      <c r="H287" s="8"/>
-      <c r="I287" s="8"/>
-      <c r="J287" s="8"/>
-      <c r="K287" s="8"/>
-      <c r="L287" s="8"/>
-      <c r="M287" s="8"/>
-      <c r="N287" s="8"/>
-      <c r="O287" s="8"/>
-      <c r="P287" s="8"/>
-      <c r="Q287" s="8"/>
-      <c r="R287" s="8"/>
-      <c r="S287" s="8"/>
-      <c r="T287" s="14"/>
+      <c r="A287" s="20"/>
+      <c r="B287" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
+      <c r="E287" s="2"/>
+      <c r="F287" s="2"/>
+      <c r="G287" s="2"/>
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+      <c r="J287" s="2"/>
+      <c r="K287" s="2"/>
+      <c r="L287" s="2"/>
+      <c r="M287" s="2"/>
+      <c r="N287" s="2"/>
+      <c r="O287" s="2"/>
+      <c r="P287" s="2"/>
+      <c r="Q287" s="2"/>
+      <c r="R287" s="2"/>
+      <c r="S287" s="2"/>
+      <c r="T287" s="5"/>
       <c r="U287">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="20"/>
-      <c r="B288" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2"/>
-      <c r="E288" s="2"/>
-      <c r="F288" s="2"/>
-      <c r="G288" s="2"/>
-      <c r="H288" s="2"/>
-      <c r="I288" s="2"/>
-      <c r="J288" s="2"/>
-      <c r="K288" s="2"/>
-      <c r="L288" s="2"/>
-      <c r="M288" s="2"/>
-      <c r="N288" s="2"/>
-      <c r="O288" s="2"/>
-      <c r="P288" s="2"/>
-      <c r="Q288" s="2"/>
-      <c r="R288" s="2"/>
-      <c r="S288" s="2"/>
-      <c r="T288" s="5"/>
+    <row r="288" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="21"/>
+      <c r="B288" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C288" s="6"/>
+      <c r="D288" s="6"/>
+      <c r="E288" s="6"/>
+      <c r="F288" s="6"/>
+      <c r="G288" s="6"/>
+      <c r="H288" s="6"/>
+      <c r="I288" s="6"/>
+      <c r="J288" s="6"/>
+      <c r="K288" s="6"/>
+      <c r="L288" s="6"/>
+      <c r="M288" s="6"/>
+      <c r="N288" s="6"/>
+      <c r="O288" s="6"/>
+      <c r="P288" s="6"/>
+      <c r="Q288" s="6"/>
+      <c r="R288" s="6"/>
+      <c r="S288" s="6"/>
+      <c r="T288" s="7"/>
       <c r="U288">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="20"/>
-      <c r="B289" s="2">
-        <v>3093</v>
-      </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="E289" s="2"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
-      <c r="I289" s="2"/>
-      <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-      <c r="N289" s="2"/>
-      <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-      <c r="Q289" s="2"/>
-      <c r="R289" s="2"/>
-      <c r="S289" s="2"/>
-      <c r="T289" s="5"/>
+      <c r="A289" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B289" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C289" s="8"/>
+      <c r="D289" s="8"/>
+      <c r="E289" s="8"/>
+      <c r="F289" s="8"/>
+      <c r="G289" s="8"/>
+      <c r="H289" s="8"/>
+      <c r="I289" s="8"/>
+      <c r="J289" s="8"/>
+      <c r="K289" s="8"/>
+      <c r="L289" s="8"/>
+      <c r="M289" s="8"/>
+      <c r="N289" s="8"/>
+      <c r="O289" s="8"/>
+      <c r="P289" s="8"/>
+      <c r="Q289" s="8"/>
+      <c r="R289" s="8"/>
+      <c r="S289" s="8"/>
+      <c r="T289" s="14"/>
       <c r="U289">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8950,7 +8950,7 @@
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="20"/>
       <c r="B290" s="2">
-        <v>8805</v>
+        <v>6598</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8978,7 +8978,7 @@
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="20"/>
       <c r="B291" s="2">
-        <v>8158</v>
+        <v>3093</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9003,115 +9003,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="21"/>
-      <c r="B292" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="6"/>
-      <c r="H292" s="6"/>
-      <c r="I292" s="6"/>
-      <c r="J292" s="6"/>
-      <c r="K292" s="6"/>
-      <c r="L292" s="6"/>
-      <c r="M292" s="6"/>
-      <c r="N292" s="6"/>
-      <c r="O292" s="6"/>
-      <c r="P292" s="6"/>
-      <c r="Q292" s="6"/>
-      <c r="R292" s="6"/>
-      <c r="S292" s="6"/>
-      <c r="T292" s="7"/>
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A292" s="20"/>
+      <c r="B292" s="2">
+        <v>8805</v>
+      </c>
+      <c r="C292" s="2"/>
+      <c r="D292" s="2"/>
+      <c r="E292" s="2"/>
+      <c r="F292" s="2"/>
+      <c r="G292" s="2"/>
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+      <c r="J292" s="2"/>
+      <c r="K292" s="2"/>
+      <c r="L292" s="2"/>
+      <c r="M292" s="2"/>
+      <c r="N292" s="2"/>
+      <c r="O292" s="2"/>
+      <c r="P292" s="2"/>
+      <c r="Q292" s="2"/>
+      <c r="R292" s="2"/>
+      <c r="S292" s="2"/>
+      <c r="T292" s="5"/>
       <c r="U292">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B293" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="14"/>
+      <c r="A293" s="20"/>
+      <c r="B293" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C293" s="2"/>
+      <c r="D293" s="2"/>
+      <c r="E293" s="2"/>
+      <c r="F293" s="2"/>
+      <c r="G293" s="2"/>
+      <c r="H293" s="2"/>
+      <c r="I293" s="2"/>
+      <c r="J293" s="2"/>
+      <c r="K293" s="2"/>
+      <c r="L293" s="2"/>
+      <c r="M293" s="2"/>
+      <c r="N293" s="2"/>
+      <c r="O293" s="2"/>
+      <c r="P293" s="2"/>
+      <c r="Q293" s="2"/>
+      <c r="R293" s="2"/>
+      <c r="S293" s="2"/>
+      <c r="T293" s="5"/>
       <c r="U293">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="20"/>
-      <c r="B294" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
-      <c r="E294" s="2"/>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
-      <c r="H294" s="2"/>
-      <c r="I294" s="2"/>
-      <c r="J294" s="2"/>
-      <c r="K294" s="2"/>
-      <c r="L294" s="2"/>
-      <c r="M294" s="2"/>
-      <c r="N294" s="2"/>
-      <c r="O294" s="2"/>
-      <c r="P294" s="2"/>
-      <c r="Q294" s="2"/>
-      <c r="R294" s="2"/>
-      <c r="S294" s="2"/>
-      <c r="T294" s="5"/>
+    <row r="294" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="21"/>
+      <c r="B294" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C294" s="6"/>
+      <c r="D294" s="6"/>
+      <c r="E294" s="6"/>
+      <c r="F294" s="6"/>
+      <c r="G294" s="6"/>
+      <c r="H294" s="6"/>
+      <c r="I294" s="6"/>
+      <c r="J294" s="6"/>
+      <c r="K294" s="6"/>
+      <c r="L294" s="6"/>
+      <c r="M294" s="6"/>
+      <c r="N294" s="6"/>
+      <c r="O294" s="6"/>
+      <c r="P294" s="6"/>
+      <c r="Q294" s="6"/>
+      <c r="R294" s="6"/>
+      <c r="S294" s="6"/>
+      <c r="T294" s="7"/>
       <c r="U294">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="20"/>
-      <c r="B295" s="2">
-        <v>9002</v>
-      </c>
-      <c r="C295" s="2"/>
-      <c r="D295" s="2"/>
-      <c r="E295" s="2"/>
-      <c r="F295" s="2"/>
-      <c r="G295" s="2"/>
-      <c r="H295" s="2"/>
-      <c r="I295" s="2"/>
-      <c r="J295" s="2"/>
-      <c r="K295" s="2"/>
-      <c r="L295" s="2"/>
-      <c r="M295" s="2"/>
-      <c r="N295" s="2"/>
-      <c r="O295" s="2"/>
-      <c r="P295" s="2"/>
-      <c r="Q295" s="2"/>
-      <c r="R295" s="2"/>
-      <c r="S295" s="2"/>
-      <c r="T295" s="5"/>
+      <c r="A295" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B295" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C295" s="8"/>
+      <c r="D295" s="8"/>
+      <c r="E295" s="8"/>
+      <c r="F295" s="8"/>
+      <c r="G295" s="8"/>
+      <c r="H295" s="8"/>
+      <c r="I295" s="8"/>
+      <c r="J295" s="8"/>
+      <c r="K295" s="8"/>
+      <c r="L295" s="8"/>
+      <c r="M295" s="8"/>
+      <c r="N295" s="8"/>
+      <c r="O295" s="8"/>
+      <c r="P295" s="8"/>
+      <c r="Q295" s="8"/>
+      <c r="R295" s="8"/>
+      <c r="S295" s="8"/>
+      <c r="T295" s="14"/>
       <c r="U295">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9120,7 +9120,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="20"/>
       <c r="B296" s="2">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9148,7 +9148,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="20"/>
       <c r="B297" s="2">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9173,41 +9173,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="21"/>
-      <c r="B298" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C298" s="6"/>
-      <c r="D298" s="6"/>
-      <c r="E298" s="6"/>
-      <c r="F298" s="6"/>
-      <c r="G298" s="6"/>
-      <c r="H298" s="6"/>
-      <c r="I298" s="6"/>
-      <c r="J298" s="6"/>
-      <c r="K298" s="6"/>
-      <c r="L298" s="6"/>
-      <c r="M298" s="6"/>
-      <c r="N298" s="6"/>
-      <c r="O298" s="6"/>
-      <c r="P298" s="6"/>
-      <c r="Q298" s="6"/>
-      <c r="R298" s="6"/>
-      <c r="S298" s="6"/>
-      <c r="T298" s="7"/>
+    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A298" s="20"/>
+      <c r="B298" s="2">
+        <v>7432</v>
+      </c>
+      <c r="C298" s="2"/>
+      <c r="D298" s="2"/>
+      <c r="E298" s="2"/>
+      <c r="F298" s="2"/>
+      <c r="G298" s="2"/>
+      <c r="H298" s="2"/>
+      <c r="I298" s="2"/>
+      <c r="J298" s="2"/>
+      <c r="K298" s="2"/>
+      <c r="L298" s="2"/>
+      <c r="M298" s="2"/>
+      <c r="N298" s="2"/>
+      <c r="O298" s="2"/>
+      <c r="P298" s="2"/>
+      <c r="Q298" s="2"/>
+      <c r="R298" s="2"/>
+      <c r="S298" s="2"/>
+      <c r="T298" s="5"/>
       <c r="U298">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A299" s="20"/>
+      <c r="B299" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C299" s="2"/>
+      <c r="D299" s="2"/>
+      <c r="E299" s="2"/>
+      <c r="F299" s="2"/>
+      <c r="G299" s="2"/>
+      <c r="H299" s="2"/>
+      <c r="I299" s="2"/>
+      <c r="J299" s="2"/>
+      <c r="K299" s="2"/>
+      <c r="L299" s="2"/>
+      <c r="M299" s="2"/>
+      <c r="N299" s="2"/>
+      <c r="O299" s="2"/>
+      <c r="P299" s="2"/>
+      <c r="Q299" s="2"/>
+      <c r="R299" s="2"/>
+      <c r="S299" s="2"/>
+      <c r="T299" s="5"/>
       <c r="U299">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="21"/>
+      <c r="B300" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C300" s="6"/>
+      <c r="D300" s="6"/>
+      <c r="E300" s="6"/>
+      <c r="F300" s="6"/>
+      <c r="G300" s="6"/>
+      <c r="H300" s="6"/>
+      <c r="I300" s="6"/>
+      <c r="J300" s="6"/>
+      <c r="K300" s="6"/>
+      <c r="L300" s="6"/>
+      <c r="M300" s="6"/>
+      <c r="N300" s="6"/>
+      <c r="O300" s="6"/>
+      <c r="P300" s="6"/>
+      <c r="Q300" s="6"/>
+      <c r="R300" s="6"/>
+      <c r="S300" s="6"/>
+      <c r="T300" s="7"/>
       <c r="U300">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9383,19 +9427,19 @@
     </row>
     <row r="329" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U329">
-        <f t="shared" ref="U329:U392" ca="1" si="7">IF(B329=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="330" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U330">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="331" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U331">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="U331:U394" ca="1" si="7">IF(B331=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9767,19 +9811,19 @@
     </row>
     <row r="393" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U393">
-        <f t="shared" ref="U393:U456" ca="1" si="8">IF(B393=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="394" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U394">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="395" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U395">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U395:U458" ca="1" si="8">IF(B395=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10151,19 +10195,19 @@
     </row>
     <row r="457" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U457">
-        <f t="shared" ref="U457:U520" ca="1" si="9">IF(B457=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="458" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U458">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="459" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U459">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U459:U522" ca="1" si="9">IF(B459=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10535,19 +10579,19 @@
     </row>
     <row r="521" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U521">
-        <f t="shared" ref="U521:U584" ca="1" si="10">IF(B521=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="522" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U522">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="523" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U523">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U523:U586" ca="1" si="10">IF(B523=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10919,19 +10963,19 @@
     </row>
     <row r="585" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U585">
-        <f t="shared" ref="U585:U648" ca="1" si="11">IF(B585=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="586" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U586">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="587" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U587">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U587:U650" ca="1" si="11">IF(B587=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11303,19 +11347,19 @@
     </row>
     <row r="649" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U649">
-        <f t="shared" ref="U649:U712" ca="1" si="12">IF(B649=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="650" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U650">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="651" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U651">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U651:U714" ca="1" si="12">IF(B651=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11687,19 +11731,19 @@
     </row>
     <row r="713" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U713">
-        <f t="shared" ref="U713:U776" ca="1" si="13">IF(B713=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="714" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U714">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="715" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U715">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U715:U778" ca="1" si="13">IF(B715=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12071,19 +12115,19 @@
     </row>
     <row r="777" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U777">
-        <f t="shared" ref="U777:U840" ca="1" si="14">IF(B777=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="778" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U778">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="779" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U779">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U779:U842" ca="1" si="14">IF(B779=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12455,19 +12499,19 @@
     </row>
     <row r="841" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U841">
-        <f t="shared" ref="U841:U902" ca="1" si="15">IF(B841=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="842" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U842">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="843" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U843">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U843:U904" ca="1" si="15">IF(B843=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12825,13 +12869,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="903" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U903">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="904" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U904">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A293:A298"/>
-    <mergeCell ref="A242:A259"/>
+    <mergeCell ref="A295:A300"/>
+    <mergeCell ref="A242:A261"/>
     <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A271:A286"/>
-    <mergeCell ref="A287:A292"/>
+    <mergeCell ref="A273:A288"/>
+    <mergeCell ref="A289:A294"/>
     <mergeCell ref="A61:A100"/>
     <mergeCell ref="A214:A225"/>
     <mergeCell ref="A191:A213"/>
@@ -12843,8 +12899,8 @@
     <mergeCell ref="A234:A241"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A266:A270"/>
-    <mergeCell ref="A260:A265"/>
+    <mergeCell ref="A268:A272"/>
+    <mergeCell ref="A262:A267"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task about comparator
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$272</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$273</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -505,6 +505,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,24 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,11 +842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W904"/>
+  <dimension ref="A1:W905"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B258" sqref="B258"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D268" sqref="D268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,56 +863,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>4916</v>
+        <v>8602</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="30"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -942,7 +942,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -972,7 +972,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="9">
         <v>4764</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="13">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="12">
         <v>3730</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="12">
         <v>9007</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="12">
         <v>9578</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="2">
         <v>4411</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="2">
         <v>9298</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="2">
         <v>3354</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="2">
         <v>5201</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2">
         <v>2981</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2">
         <v>4312</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2">
         <v>8428</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2">
         <v>2361</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="2">
         <v>5063</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2">
         <v>7711</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2">
         <v>8833</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2">
         <v>1262</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="2">
         <v>9020</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="2">
         <v>1934</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="2">
         <v>7237</v>
       </c>
@@ -1898,7 +1898,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="2">
         <v>3943</v>
       </c>
@@ -1926,7 +1926,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="2">
         <v>7619</v>
       </c>
@@ -1954,7 +1954,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="2">
         <v>3832</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="2">
         <v>1346</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="2">
         <v>9622</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="2">
         <v>8873</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="2">
         <v>7799</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="2">
         <v>9354</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="2">
         <v>9130</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="2">
         <v>5895</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="2">
         <v>2461</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="2">
         <v>2790</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="2">
         <v>2624</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="2">
         <v>5871</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="2">
         <v>9164</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="2">
         <v>7457</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="2">
         <v>9865</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="2">
         <v>3591</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="2">
         <v>3558</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="2">
         <v>4366</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="2">
         <v>5789</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="33"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="6">
         <v>6522</v>
       </c>
@@ -6383,7 +6383,7 @@
       <c r="S198" s="2"/>
       <c r="T198" s="5"/>
       <c r="U198">
-        <f t="shared" ref="U198:U266" ca="1" si="5">IF(B198=$W$1,1,0)</f>
+        <f t="shared" ref="U198:U267" ca="1" si="5">IF(B198=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8297,87 +8297,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="21"/>
-      <c r="B267" s="6">
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A267" s="24"/>
+      <c r="B267" s="9">
         <v>7657</v>
       </c>
-      <c r="C267" s="6"/>
-      <c r="D267" s="6"/>
-      <c r="E267" s="6"/>
-      <c r="F267" s="6"/>
-      <c r="G267" s="6"/>
-      <c r="H267" s="6"/>
-      <c r="I267" s="6"/>
-      <c r="J267" s="6"/>
-      <c r="K267" s="6"/>
-      <c r="L267" s="6"/>
-      <c r="M267" s="6"/>
-      <c r="N267" s="6"/>
-      <c r="O267" s="6"/>
-      <c r="P267" s="6"/>
-      <c r="Q267" s="6"/>
-      <c r="R267" s="6"/>
-      <c r="S267" s="6"/>
-      <c r="T267" s="7"/>
+      <c r="C267" s="9"/>
+      <c r="D267" s="9"/>
+      <c r="E267" s="9"/>
+      <c r="F267" s="9"/>
+      <c r="G267" s="9"/>
+      <c r="H267" s="9"/>
+      <c r="I267" s="9"/>
+      <c r="J267" s="9"/>
+      <c r="K267" s="9"/>
+      <c r="L267" s="9"/>
+      <c r="M267" s="9"/>
+      <c r="N267" s="9"/>
+      <c r="O267" s="9"/>
+      <c r="P267" s="9"/>
+      <c r="Q267" s="9"/>
+      <c r="R267" s="9"/>
+      <c r="S267" s="9"/>
+      <c r="T267" s="15"/>
       <c r="U267">
-        <f t="shared" ref="U267:U330" ca="1" si="6">IF(B267=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="19" t="s">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="21"/>
+      <c r="B268" s="6">
+        <v>8258</v>
+      </c>
+      <c r="C268" s="6"/>
+      <c r="D268" s="6"/>
+      <c r="E268" s="6"/>
+      <c r="F268" s="6"/>
+      <c r="G268" s="6"/>
+      <c r="H268" s="6"/>
+      <c r="I268" s="6"/>
+      <c r="J268" s="6"/>
+      <c r="K268" s="6"/>
+      <c r="L268" s="6"/>
+      <c r="M268" s="6"/>
+      <c r="N268" s="6"/>
+      <c r="O268" s="6"/>
+      <c r="P268" s="6"/>
+      <c r="Q268" s="6"/>
+      <c r="R268" s="6"/>
+      <c r="S268" s="6"/>
+      <c r="T268" s="7"/>
+      <c r="U268">
+        <f t="shared" ref="U268:U331" ca="1" si="6">IF(B268=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A269" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B268" s="8">
+      <c r="B269" s="8">
         <v>4304</v>
       </c>
-      <c r="C268" s="8"/>
-      <c r="D268" s="8"/>
-      <c r="E268" s="8"/>
-      <c r="F268" s="8"/>
-      <c r="G268" s="8"/>
-      <c r="H268" s="8"/>
-      <c r="I268" s="8"/>
-      <c r="J268" s="8"/>
-      <c r="K268" s="8"/>
-      <c r="L268" s="8"/>
-      <c r="M268" s="8"/>
-      <c r="N268" s="8"/>
-      <c r="O268" s="8"/>
-      <c r="P268" s="8"/>
-      <c r="Q268" s="8"/>
-      <c r="R268" s="8"/>
-      <c r="S268" s="8"/>
-      <c r="T268" s="14"/>
-      <c r="U268">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="20"/>
-      <c r="B269" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="E269" s="2"/>
-      <c r="F269" s="2"/>
-      <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
-      <c r="I269" s="2"/>
-      <c r="J269" s="2"/>
-      <c r="K269" s="2"/>
-      <c r="L269" s="2"/>
-      <c r="M269" s="2"/>
-      <c r="N269" s="2"/>
-      <c r="O269" s="2"/>
-      <c r="P269" s="2"/>
-      <c r="Q269" s="2"/>
-      <c r="R269" s="2"/>
-      <c r="S269" s="2"/>
-      <c r="T269" s="5"/>
+      <c r="C269" s="8"/>
+      <c r="D269" s="8"/>
+      <c r="E269" s="8"/>
+      <c r="F269" s="8"/>
+      <c r="G269" s="8"/>
+      <c r="H269" s="8"/>
+      <c r="I269" s="8"/>
+      <c r="J269" s="8"/>
+      <c r="K269" s="8"/>
+      <c r="L269" s="8"/>
+      <c r="M269" s="8"/>
+      <c r="N269" s="8"/>
+      <c r="O269" s="8"/>
+      <c r="P269" s="8"/>
+      <c r="Q269" s="8"/>
+      <c r="R269" s="8"/>
+      <c r="S269" s="8"/>
+      <c r="T269" s="14"/>
       <c r="U269">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8386,7 +8386,7 @@
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="20"/>
       <c r="B270" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8414,7 +8414,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="20"/>
       <c r="B271" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8439,87 +8439,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="21"/>
-      <c r="B272" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C272" s="6"/>
-      <c r="D272" s="6"/>
-      <c r="E272" s="6"/>
-      <c r="F272" s="6"/>
-      <c r="G272" s="6"/>
-      <c r="H272" s="6"/>
-      <c r="I272" s="6"/>
-      <c r="J272" s="6"/>
-      <c r="K272" s="6"/>
-      <c r="L272" s="6"/>
-      <c r="M272" s="6"/>
-      <c r="N272" s="6"/>
-      <c r="O272" s="6"/>
-      <c r="P272" s="6"/>
-      <c r="Q272" s="6"/>
-      <c r="R272" s="6"/>
-      <c r="S272" s="6"/>
-      <c r="T272" s="7"/>
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A272" s="20"/>
+      <c r="B272" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C272" s="2"/>
+      <c r="D272" s="2"/>
+      <c r="E272" s="2"/>
+      <c r="F272" s="2"/>
+      <c r="G272" s="2"/>
+      <c r="H272" s="2"/>
+      <c r="I272" s="2"/>
+      <c r="J272" s="2"/>
+      <c r="K272" s="2"/>
+      <c r="L272" s="2"/>
+      <c r="M272" s="2"/>
+      <c r="N272" s="2"/>
+      <c r="O272" s="2"/>
+      <c r="P272" s="2"/>
+      <c r="Q272" s="2"/>
+      <c r="R272" s="2"/>
+      <c r="S272" s="2"/>
+      <c r="T272" s="5"/>
       <c r="U272">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A273" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B273" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C273" s="8"/>
-      <c r="D273" s="8"/>
-      <c r="E273" s="8"/>
-      <c r="F273" s="8"/>
-      <c r="G273" s="8"/>
-      <c r="H273" s="8"/>
-      <c r="I273" s="8"/>
-      <c r="J273" s="8"/>
-      <c r="K273" s="8"/>
-      <c r="L273" s="8"/>
-      <c r="M273" s="8"/>
-      <c r="N273" s="8"/>
-      <c r="O273" s="8"/>
-      <c r="P273" s="8"/>
-      <c r="Q273" s="8"/>
-      <c r="R273" s="8"/>
-      <c r="S273" s="8"/>
-      <c r="T273" s="14"/>
+    <row r="273" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A273" s="21"/>
+      <c r="B273" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C273" s="6"/>
+      <c r="D273" s="6"/>
+      <c r="E273" s="6"/>
+      <c r="F273" s="6"/>
+      <c r="G273" s="6"/>
+      <c r="H273" s="6"/>
+      <c r="I273" s="6"/>
+      <c r="J273" s="6"/>
+      <c r="K273" s="6"/>
+      <c r="L273" s="6"/>
+      <c r="M273" s="6"/>
+      <c r="N273" s="6"/>
+      <c r="O273" s="6"/>
+      <c r="P273" s="6"/>
+      <c r="Q273" s="6"/>
+      <c r="R273" s="6"/>
+      <c r="S273" s="6"/>
+      <c r="T273" s="7"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A274" s="20"/>
-      <c r="B274" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2"/>
-      <c r="E274" s="2"/>
-      <c r="F274" s="2"/>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="2"/>
-      <c r="J274" s="2"/>
-      <c r="K274" s="2"/>
-      <c r="L274" s="2"/>
-      <c r="M274" s="2"/>
-      <c r="N274" s="2"/>
-      <c r="O274" s="2"/>
-      <c r="P274" s="2"/>
-      <c r="Q274" s="2"/>
-      <c r="R274" s="2"/>
-      <c r="S274" s="2"/>
-      <c r="T274" s="5"/>
+      <c r="A274" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B274" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C274" s="8"/>
+      <c r="D274" s="8"/>
+      <c r="E274" s="8"/>
+      <c r="F274" s="8"/>
+      <c r="G274" s="8"/>
+      <c r="H274" s="8"/>
+      <c r="I274" s="8"/>
+      <c r="J274" s="8"/>
+      <c r="K274" s="8"/>
+      <c r="L274" s="8"/>
+      <c r="M274" s="8"/>
+      <c r="N274" s="8"/>
+      <c r="O274" s="8"/>
+      <c r="P274" s="8"/>
+      <c r="Q274" s="8"/>
+      <c r="R274" s="8"/>
+      <c r="S274" s="8"/>
+      <c r="T274" s="14"/>
       <c r="U274">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8528,7 +8528,7 @@
     <row r="275" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A275" s="20"/>
       <c r="B275" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8553,10 +8553,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A276" s="20"/>
-      <c r="B276" s="2">
-        <v>7170</v>
+      <c r="B276" s="12">
+        <v>7546</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8584,7 +8584,7 @@
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" s="20"/>
       <c r="B277" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8612,7 +8612,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="20"/>
       <c r="B278" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8640,7 +8640,7 @@
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" s="20"/>
       <c r="B279" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8668,7 +8668,7 @@
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" s="20"/>
       <c r="B280" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8696,7 +8696,7 @@
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="20"/>
       <c r="B281" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8724,7 +8724,7 @@
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="20"/>
       <c r="B282" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8752,7 +8752,7 @@
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" s="20"/>
       <c r="B283" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8780,7 +8780,7 @@
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" s="20"/>
       <c r="B284" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8808,7 +8808,7 @@
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A285" s="20"/>
       <c r="B285" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8836,7 +8836,7 @@
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A286" s="20"/>
       <c r="B286" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8864,7 +8864,7 @@
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A287" s="20"/>
       <c r="B287" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8889,87 +8889,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="21"/>
-      <c r="B288" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C288" s="6"/>
-      <c r="D288" s="6"/>
-      <c r="E288" s="6"/>
-      <c r="F288" s="6"/>
-      <c r="G288" s="6"/>
-      <c r="H288" s="6"/>
-      <c r="I288" s="6"/>
-      <c r="J288" s="6"/>
-      <c r="K288" s="6"/>
-      <c r="L288" s="6"/>
-      <c r="M288" s="6"/>
-      <c r="N288" s="6"/>
-      <c r="O288" s="6"/>
-      <c r="P288" s="6"/>
-      <c r="Q288" s="6"/>
-      <c r="R288" s="6"/>
-      <c r="S288" s="6"/>
-      <c r="T288" s="7"/>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A288" s="20"/>
+      <c r="B288" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C288" s="2"/>
+      <c r="D288" s="2"/>
+      <c r="E288" s="2"/>
+      <c r="F288" s="2"/>
+      <c r="G288" s="2"/>
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+      <c r="J288" s="2"/>
+      <c r="K288" s="2"/>
+      <c r="L288" s="2"/>
+      <c r="M288" s="2"/>
+      <c r="N288" s="2"/>
+      <c r="O288" s="2"/>
+      <c r="P288" s="2"/>
+      <c r="Q288" s="2"/>
+      <c r="R288" s="2"/>
+      <c r="S288" s="2"/>
+      <c r="T288" s="5"/>
       <c r="U288">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B289" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C289" s="8"/>
-      <c r="D289" s="8"/>
-      <c r="E289" s="8"/>
-      <c r="F289" s="8"/>
-      <c r="G289" s="8"/>
-      <c r="H289" s="8"/>
-      <c r="I289" s="8"/>
-      <c r="J289" s="8"/>
-      <c r="K289" s="8"/>
-      <c r="L289" s="8"/>
-      <c r="M289" s="8"/>
-      <c r="N289" s="8"/>
-      <c r="O289" s="8"/>
-      <c r="P289" s="8"/>
-      <c r="Q289" s="8"/>
-      <c r="R289" s="8"/>
-      <c r="S289" s="8"/>
-      <c r="T289" s="14"/>
+    <row r="289" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="21"/>
+      <c r="B289" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
+      <c r="E289" s="6"/>
+      <c r="F289" s="6"/>
+      <c r="G289" s="6"/>
+      <c r="H289" s="6"/>
+      <c r="I289" s="6"/>
+      <c r="J289" s="6"/>
+      <c r="K289" s="6"/>
+      <c r="L289" s="6"/>
+      <c r="M289" s="6"/>
+      <c r="N289" s="6"/>
+      <c r="O289" s="6"/>
+      <c r="P289" s="6"/>
+      <c r="Q289" s="6"/>
+      <c r="R289" s="6"/>
+      <c r="S289" s="6"/>
+      <c r="T289" s="7"/>
       <c r="U289">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="20"/>
-      <c r="B290" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="E290" s="2"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
-      <c r="I290" s="2"/>
-      <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-      <c r="N290" s="2"/>
-      <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-      <c r="Q290" s="2"/>
-      <c r="R290" s="2"/>
-      <c r="S290" s="2"/>
-      <c r="T290" s="5"/>
+      <c r="A290" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B290" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C290" s="8"/>
+      <c r="D290" s="8"/>
+      <c r="E290" s="8"/>
+      <c r="F290" s="8"/>
+      <c r="G290" s="8"/>
+      <c r="H290" s="8"/>
+      <c r="I290" s="8"/>
+      <c r="J290" s="8"/>
+      <c r="K290" s="8"/>
+      <c r="L290" s="8"/>
+      <c r="M290" s="8"/>
+      <c r="N290" s="8"/>
+      <c r="O290" s="8"/>
+      <c r="P290" s="8"/>
+      <c r="Q290" s="8"/>
+      <c r="R290" s="8"/>
+      <c r="S290" s="8"/>
+      <c r="T290" s="14"/>
       <c r="U290">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8978,7 +8978,7 @@
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="20"/>
       <c r="B291" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9006,7 +9006,7 @@
     <row r="292" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A292" s="20"/>
       <c r="B292" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9034,7 +9034,7 @@
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293" s="20"/>
       <c r="B293" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9059,87 +9059,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A294" s="21"/>
-      <c r="B294" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C294" s="6"/>
-      <c r="D294" s="6"/>
-      <c r="E294" s="6"/>
-      <c r="F294" s="6"/>
-      <c r="G294" s="6"/>
-      <c r="H294" s="6"/>
-      <c r="I294" s="6"/>
-      <c r="J294" s="6"/>
-      <c r="K294" s="6"/>
-      <c r="L294" s="6"/>
-      <c r="M294" s="6"/>
-      <c r="N294" s="6"/>
-      <c r="O294" s="6"/>
-      <c r="P294" s="6"/>
-      <c r="Q294" s="6"/>
-      <c r="R294" s="6"/>
-      <c r="S294" s="6"/>
-      <c r="T294" s="7"/>
+    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A294" s="20"/>
+      <c r="B294" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C294" s="2"/>
+      <c r="D294" s="2"/>
+      <c r="E294" s="2"/>
+      <c r="F294" s="2"/>
+      <c r="G294" s="2"/>
+      <c r="H294" s="2"/>
+      <c r="I294" s="2"/>
+      <c r="J294" s="2"/>
+      <c r="K294" s="2"/>
+      <c r="L294" s="2"/>
+      <c r="M294" s="2"/>
+      <c r="N294" s="2"/>
+      <c r="O294" s="2"/>
+      <c r="P294" s="2"/>
+      <c r="Q294" s="2"/>
+      <c r="R294" s="2"/>
+      <c r="S294" s="2"/>
+      <c r="T294" s="5"/>
       <c r="U294">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B295" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C295" s="8"/>
-      <c r="D295" s="8"/>
-      <c r="E295" s="8"/>
-      <c r="F295" s="8"/>
-      <c r="G295" s="8"/>
-      <c r="H295" s="8"/>
-      <c r="I295" s="8"/>
-      <c r="J295" s="8"/>
-      <c r="K295" s="8"/>
-      <c r="L295" s="8"/>
-      <c r="M295" s="8"/>
-      <c r="N295" s="8"/>
-      <c r="O295" s="8"/>
-      <c r="P295" s="8"/>
-      <c r="Q295" s="8"/>
-      <c r="R295" s="8"/>
-      <c r="S295" s="8"/>
-      <c r="T295" s="14"/>
+    <row r="295" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="21"/>
+      <c r="B295" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C295" s="6"/>
+      <c r="D295" s="6"/>
+      <c r="E295" s="6"/>
+      <c r="F295" s="6"/>
+      <c r="G295" s="6"/>
+      <c r="H295" s="6"/>
+      <c r="I295" s="6"/>
+      <c r="J295" s="6"/>
+      <c r="K295" s="6"/>
+      <c r="L295" s="6"/>
+      <c r="M295" s="6"/>
+      <c r="N295" s="6"/>
+      <c r="O295" s="6"/>
+      <c r="P295" s="6"/>
+      <c r="Q295" s="6"/>
+      <c r="R295" s="6"/>
+      <c r="S295" s="6"/>
+      <c r="T295" s="7"/>
       <c r="U295">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A296" s="20"/>
-      <c r="B296" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C296" s="2"/>
-      <c r="D296" s="2"/>
-      <c r="E296" s="2"/>
-      <c r="F296" s="2"/>
-      <c r="G296" s="2"/>
-      <c r="H296" s="2"/>
-      <c r="I296" s="2"/>
-      <c r="J296" s="2"/>
-      <c r="K296" s="2"/>
-      <c r="L296" s="2"/>
-      <c r="M296" s="2"/>
-      <c r="N296" s="2"/>
-      <c r="O296" s="2"/>
-      <c r="P296" s="2"/>
-      <c r="Q296" s="2"/>
-      <c r="R296" s="2"/>
-      <c r="S296" s="2"/>
-      <c r="T296" s="5"/>
+      <c r="A296" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B296" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C296" s="8"/>
+      <c r="D296" s="8"/>
+      <c r="E296" s="8"/>
+      <c r="F296" s="8"/>
+      <c r="G296" s="8"/>
+      <c r="H296" s="8"/>
+      <c r="I296" s="8"/>
+      <c r="J296" s="8"/>
+      <c r="K296" s="8"/>
+      <c r="L296" s="8"/>
+      <c r="M296" s="8"/>
+      <c r="N296" s="8"/>
+      <c r="O296" s="8"/>
+      <c r="P296" s="8"/>
+      <c r="Q296" s="8"/>
+      <c r="R296" s="8"/>
+      <c r="S296" s="8"/>
+      <c r="T296" s="14"/>
       <c r="U296">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9148,7 +9148,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="20"/>
       <c r="B297" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9176,7 +9176,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="20"/>
       <c r="B298" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9204,7 +9204,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="20"/>
       <c r="B299" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9229,35 +9229,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="21"/>
-      <c r="B300" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-      <c r="E300" s="6"/>
-      <c r="F300" s="6"/>
-      <c r="G300" s="6"/>
-      <c r="H300" s="6"/>
-      <c r="I300" s="6"/>
-      <c r="J300" s="6"/>
-      <c r="K300" s="6"/>
-      <c r="L300" s="6"/>
-      <c r="M300" s="6"/>
-      <c r="N300" s="6"/>
-      <c r="O300" s="6"/>
-      <c r="P300" s="6"/>
-      <c r="Q300" s="6"/>
-      <c r="R300" s="6"/>
-      <c r="S300" s="6"/>
-      <c r="T300" s="7"/>
+    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A300" s="20"/>
+      <c r="B300" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C300" s="2"/>
+      <c r="D300" s="2"/>
+      <c r="E300" s="2"/>
+      <c r="F300" s="2"/>
+      <c r="G300" s="2"/>
+      <c r="H300" s="2"/>
+      <c r="I300" s="2"/>
+      <c r="J300" s="2"/>
+      <c r="K300" s="2"/>
+      <c r="L300" s="2"/>
+      <c r="M300" s="2"/>
+      <c r="N300" s="2"/>
+      <c r="O300" s="2"/>
+      <c r="P300" s="2"/>
+      <c r="Q300" s="2"/>
+      <c r="R300" s="2"/>
+      <c r="S300" s="2"/>
+      <c r="T300" s="5"/>
       <c r="U300">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="21"/>
+      <c r="B301" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
+      <c r="H301" s="6"/>
+      <c r="I301" s="6"/>
+      <c r="J301" s="6"/>
+      <c r="K301" s="6"/>
+      <c r="L301" s="6"/>
+      <c r="M301" s="6"/>
+      <c r="N301" s="6"/>
+      <c r="O301" s="6"/>
+      <c r="P301" s="6"/>
+      <c r="Q301" s="6"/>
+      <c r="R301" s="6"/>
+      <c r="S301" s="6"/>
+      <c r="T301" s="7"/>
       <c r="U301">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9439,13 +9461,13 @@
     </row>
     <row r="331" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U331">
-        <f t="shared" ref="U331:U394" ca="1" si="7">IF(B331=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="332" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U332">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="U332:U395" ca="1" si="7">IF(B332=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9823,13 +9845,13 @@
     </row>
     <row r="395" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U395">
-        <f t="shared" ref="U395:U458" ca="1" si="8">IF(B395=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="396" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U396">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U396:U459" ca="1" si="8">IF(B396=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10207,13 +10229,13 @@
     </row>
     <row r="459" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U459">
-        <f t="shared" ref="U459:U522" ca="1" si="9">IF(B459=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="460" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U460">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U460:U523" ca="1" si="9">IF(B460=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10591,13 +10613,13 @@
     </row>
     <row r="523" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U523">
-        <f t="shared" ref="U523:U586" ca="1" si="10">IF(B523=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="524" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U524">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U524:U587" ca="1" si="10">IF(B524=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10975,13 +10997,13 @@
     </row>
     <row r="587" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U587">
-        <f t="shared" ref="U587:U650" ca="1" si="11">IF(B587=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="588" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U588">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U588:U651" ca="1" si="11">IF(B588=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11359,13 +11381,13 @@
     </row>
     <row r="651" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U651">
-        <f t="shared" ref="U651:U714" ca="1" si="12">IF(B651=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="652" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U652">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U652:U715" ca="1" si="12">IF(B652=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11743,13 +11765,13 @@
     </row>
     <row r="715" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U715">
-        <f t="shared" ref="U715:U778" ca="1" si="13">IF(B715=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="716" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U716">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U716:U779" ca="1" si="13">IF(B716=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12127,13 +12149,13 @@
     </row>
     <row r="779" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U779">
-        <f t="shared" ref="U779:U842" ca="1" si="14">IF(B779=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="780" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U780">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U780:U843" ca="1" si="14">IF(B780=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12511,13 +12533,13 @@
     </row>
     <row r="843" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U843">
-        <f t="shared" ref="U843:U904" ca="1" si="15">IF(B843=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="844" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U844">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U844:U905" ca="1" si="15">IF(B844=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12881,13 +12903,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="905" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U905">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A295:A300"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A269:A273"/>
+    <mergeCell ref="A262:A268"/>
+    <mergeCell ref="A296:A301"/>
     <mergeCell ref="A242:A261"/>
     <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A273:A288"/>
-    <mergeCell ref="A289:A294"/>
+    <mergeCell ref="A274:A289"/>
+    <mergeCell ref="A290:A295"/>
     <mergeCell ref="A61:A100"/>
     <mergeCell ref="A214:A225"/>
     <mergeCell ref="A191:A213"/>
@@ -12897,10 +12929,6 @@
     <mergeCell ref="A20:A60"/>
     <mergeCell ref="A226:A233"/>
     <mergeCell ref="A234:A241"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A268:A272"/>
-    <mergeCell ref="A262:A267"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task for excercising ToString
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$276</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$277</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -496,33 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,6 +513,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,11 +842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W908"/>
+  <dimension ref="A1:W909"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B271" sqref="B271"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,56 +863,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>7159</v>
+        <v>9494</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="33"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="30"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -942,7 +942,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -972,7 +972,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3">
         <v>2429</v>
       </c>
@@ -1056,7 +1056,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2">
         <v>7472</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="2">
         <v>3862</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="2">
         <v>9231</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2">
         <v>8624</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="2">
         <v>2959</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="2">
         <v>7271</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2">
         <v>2632</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="2">
         <v>4343</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="2">
         <v>1662</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="2">
         <v>1860</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9">
         <v>4764</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="13">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="12">
         <v>3730</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="12">
         <v>9007</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="12">
         <v>9578</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="2">
         <v>4411</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="2">
         <v>9298</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="2">
         <v>3354</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="2">
         <v>5201</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="2">
         <v>2981</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="2">
         <v>4312</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="2">
         <v>8428</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="2">
         <v>2361</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="2">
         <v>5063</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="2">
         <v>7711</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="2">
         <v>8833</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="2">
         <v>1262</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="2">
         <v>9020</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="2">
         <v>1934</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="2">
         <v>7237</v>
       </c>
@@ -1898,7 +1898,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="2">
         <v>3943</v>
       </c>
@@ -1926,7 +1926,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="2">
         <v>7619</v>
       </c>
@@ -1954,7 +1954,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="2">
         <v>3832</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="2">
         <v>1346</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="2">
         <v>9622</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="2">
         <v>8873</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="2">
         <v>7799</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="2">
         <v>9354</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="2">
         <v>9130</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="2">
         <v>5895</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="2">
         <v>2461</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="2">
         <v>2790</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="2">
         <v>2624</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="2">
         <v>5871</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="2">
         <v>9164</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="2">
         <v>7457</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="2">
         <v>9865</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="2">
         <v>3591</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="2">
         <v>3558</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="2">
         <v>4366</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="2">
         <v>5789</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="27"/>
+      <c r="A60" s="33"/>
       <c r="B60" s="6">
         <v>6522</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="13">
@@ -2544,7 +2544,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="12">
         <v>2217</v>
       </c>
@@ -2572,7 +2572,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12">
         <v>1824</v>
       </c>
@@ -2600,7 +2600,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12">
         <v>2564</v>
       </c>
@@ -2628,7 +2628,7 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="12">
         <v>8487</v>
       </c>
@@ -2656,7 +2656,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="12">
         <v>8045</v>
       </c>
@@ -2684,7 +2684,7 @@
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="2">
         <v>8878</v>
       </c>
@@ -2712,7 +2712,7 @@
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="2">
         <v>3072</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="2">
         <v>5980</v>
       </c>
@@ -2768,7 +2768,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="2">
         <v>8174</v>
       </c>
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="2">
         <v>4257</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="2">
         <v>2291</v>
       </c>
@@ -2852,7 +2852,7 @@
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="2">
         <v>1763</v>
       </c>
@@ -2880,7 +2880,7 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="2">
         <v>5662</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="20"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="2">
         <v>1945</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="2">
         <v>1186</v>
       </c>
@@ -2964,7 +2964,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="2">
         <v>8715</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="2">
         <v>8518</v>
       </c>
@@ -3020,7 +3020,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="2">
         <v>4847</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="2">
         <v>7991</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="2">
         <v>6291</v>
       </c>
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="2">
         <v>3770</v>
       </c>
@@ -3132,7 +3132,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="2">
         <v>7178</v>
       </c>
@@ -3160,7 +3160,7 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="2">
         <v>3883</v>
       </c>
@@ -3188,7 +3188,7 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="2">
         <v>4527</v>
       </c>
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="2">
         <v>6556</v>
       </c>
@@ -3244,7 +3244,7 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="2">
         <v>5635</v>
       </c>
@@ -3272,7 +3272,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="2">
         <v>3878</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="2">
         <v>1217</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="2">
         <v>1438</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="20"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="2">
         <v>2153</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
+      <c r="A92" s="26"/>
       <c r="B92" s="2">
         <v>7937</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="2">
         <v>1999</v>
       </c>
@@ -3440,7 +3440,7 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="20"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="2">
         <v>4042</v>
       </c>
@@ -3468,7 +3468,7 @@
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="20"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="2">
         <v>6351</v>
       </c>
@@ -3496,7 +3496,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="20"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="2">
         <v>5382</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="20"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="2">
         <v>7088</v>
       </c>
@@ -3552,7 +3552,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="20"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="2">
         <v>7250</v>
       </c>
@@ -3580,7 +3580,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="20"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="2">
         <v>6740</v>
       </c>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="21"/>
+      <c r="A100" s="27"/>
       <c r="B100" s="6">
         <v>9038</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B101" s="13">
@@ -3666,7 +3666,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="20"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="12">
         <v>1881</v>
       </c>
@@ -3694,7 +3694,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="20"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="2">
         <v>8495</v>
       </c>
@@ -3722,7 +3722,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A104" s="20"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="2">
         <v>1315</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A105" s="20"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="2">
         <v>6066</v>
       </c>
@@ -3778,7 +3778,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A106" s="20"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="2">
         <v>2565</v>
       </c>
@@ -3806,7 +3806,7 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" s="20"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="2">
         <v>2594</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" s="20"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="2">
         <v>3762</v>
       </c>
@@ -3862,7 +3862,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A109" s="20"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="2">
         <v>3550</v>
       </c>
@@ -3890,7 +3890,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A110" s="20"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="2">
         <v>2475</v>
       </c>
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A111" s="20"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="2">
         <v>9180</v>
       </c>
@@ -3946,7 +3946,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="20"/>
+      <c r="A112" s="26"/>
       <c r="B112" s="2">
         <v>1544</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" s="20"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="2">
         <v>9562</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
+      <c r="A114" s="26"/>
       <c r="B114" s="2">
         <v>3669</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
+      <c r="A115" s="26"/>
       <c r="B115" s="2">
         <v>5951</v>
       </c>
@@ -4058,7 +4058,7 @@
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
+      <c r="A116" s="26"/>
       <c r="B116" s="2">
         <v>2802</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" s="20"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="2">
         <v>6580</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="20"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="2">
         <v>2324</v>
       </c>
@@ -4142,7 +4142,7 @@
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119" s="20"/>
+      <c r="A119" s="26"/>
       <c r="B119" s="2">
         <v>8731</v>
       </c>
@@ -4170,7 +4170,7 @@
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" s="20"/>
+      <c r="A120" s="26"/>
       <c r="B120" s="2">
         <v>4082</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="20"/>
+      <c r="A121" s="26"/>
       <c r="B121" s="2">
         <v>7585</v>
       </c>
@@ -4226,7 +4226,7 @@
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122" s="20"/>
+      <c r="A122" s="26"/>
       <c r="B122" s="2">
         <v>2321</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="20"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="2">
         <v>5053</v>
       </c>
@@ -4282,7 +4282,7 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="20"/>
+      <c r="A124" s="26"/>
       <c r="B124" s="2">
         <v>3983</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="20"/>
+      <c r="A125" s="26"/>
       <c r="B125" s="2">
         <v>8770</v>
       </c>
@@ -4338,7 +4338,7 @@
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126" s="20"/>
+      <c r="A126" s="26"/>
       <c r="B126" s="2">
         <v>4236</v>
       </c>
@@ -4366,7 +4366,7 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127" s="20"/>
+      <c r="A127" s="26"/>
       <c r="B127" s="2">
         <v>5969</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128" s="20"/>
+      <c r="A128" s="26"/>
       <c r="B128" s="2">
         <v>8696</v>
       </c>
@@ -4422,7 +4422,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A129" s="20"/>
+      <c r="A129" s="26"/>
       <c r="B129" s="2">
         <v>1483</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A130" s="20"/>
+      <c r="A130" s="26"/>
       <c r="B130" s="2">
         <v>8418</v>
       </c>
@@ -4478,7 +4478,7 @@
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A131" s="20"/>
+      <c r="A131" s="26"/>
       <c r="B131" s="2">
         <v>8395</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="20"/>
+      <c r="A132" s="26"/>
       <c r="B132" s="2">
         <v>5170</v>
       </c>
@@ -4534,7 +4534,7 @@
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A133" s="20"/>
+      <c r="A133" s="26"/>
       <c r="B133" s="2">
         <v>5568</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A134" s="20"/>
+      <c r="A134" s="26"/>
       <c r="B134" s="2">
         <v>2592</v>
       </c>
@@ -4590,7 +4590,7 @@
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A135" s="20"/>
+      <c r="A135" s="26"/>
       <c r="B135" s="2">
         <v>4075</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A136" s="20"/>
+      <c r="A136" s="26"/>
       <c r="B136" s="2">
         <v>7517</v>
       </c>
@@ -4646,7 +4646,7 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A137" s="20"/>
+      <c r="A137" s="26"/>
       <c r="B137" s="2">
         <v>5448</v>
       </c>
@@ -4674,7 +4674,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A138" s="20"/>
+      <c r="A138" s="26"/>
       <c r="B138" s="2">
         <v>6572</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A139" s="20"/>
+      <c r="A139" s="26"/>
       <c r="B139" s="2">
         <v>5238</v>
       </c>
@@ -4730,7 +4730,7 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="20"/>
+      <c r="A140" s="26"/>
       <c r="B140" s="2">
         <v>2084</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A141" s="20"/>
+      <c r="A141" s="26"/>
       <c r="B141" s="2">
         <v>5411</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A142" s="20"/>
+      <c r="A142" s="26"/>
       <c r="B142" s="2">
         <v>5171</v>
       </c>
@@ -4814,7 +4814,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="21"/>
+      <c r="A143" s="27"/>
       <c r="B143" s="6">
         <v>1862</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="19" t="s">
+      <c r="A144" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B144" s="13">
@@ -4872,7 +4872,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="20"/>
+      <c r="A145" s="26"/>
       <c r="B145" s="12">
         <v>9001</v>
       </c>
@@ -4900,7 +4900,7 @@
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A146" s="20"/>
+      <c r="A146" s="26"/>
       <c r="B146" s="2">
         <v>9631</v>
       </c>
@@ -4928,7 +4928,7 @@
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A147" s="20"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="2">
         <v>9812</v>
       </c>
@@ -4956,7 +4956,7 @@
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A148" s="20"/>
+      <c r="A148" s="26"/>
       <c r="B148" s="2">
         <v>4845</v>
       </c>
@@ -4984,7 +4984,7 @@
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A149" s="20"/>
+      <c r="A149" s="26"/>
       <c r="B149" s="2">
         <v>5728</v>
       </c>
@@ -5012,7 +5012,7 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A150" s="20"/>
+      <c r="A150" s="26"/>
       <c r="B150" s="2">
         <v>1618</v>
       </c>
@@ -5040,7 +5040,7 @@
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A151" s="20"/>
+      <c r="A151" s="26"/>
       <c r="B151" s="2">
         <v>9279</v>
       </c>
@@ -5068,7 +5068,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A152" s="20"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="2">
         <v>6599</v>
       </c>
@@ -5096,7 +5096,7 @@
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A153" s="20"/>
+      <c r="A153" s="26"/>
       <c r="B153" s="2">
         <v>7222</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A154" s="20"/>
+      <c r="A154" s="26"/>
       <c r="B154" s="2">
         <v>3657</v>
       </c>
@@ -5152,7 +5152,7 @@
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A155" s="20"/>
+      <c r="A155" s="26"/>
       <c r="B155" s="2">
         <v>7491</v>
       </c>
@@ -5180,7 +5180,7 @@
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A156" s="20"/>
+      <c r="A156" s="26"/>
       <c r="B156" s="2">
         <v>5923</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A157" s="20"/>
+      <c r="A157" s="26"/>
       <c r="B157" s="2">
         <v>4265</v>
       </c>
@@ -5236,7 +5236,7 @@
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A158" s="20"/>
+      <c r="A158" s="26"/>
       <c r="B158" s="2">
         <v>2166</v>
       </c>
@@ -5264,7 +5264,7 @@
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="20"/>
+      <c r="A159" s="26"/>
       <c r="B159" s="2">
         <v>9116</v>
       </c>
@@ -5292,7 +5292,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="21"/>
+      <c r="A160" s="27"/>
       <c r="B160" s="6">
         <v>9925</v>
       </c>
@@ -5320,7 +5320,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="19" t="s">
+      <c r="A161" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B161" s="13">
@@ -5350,7 +5350,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
+      <c r="A162" s="26"/>
       <c r="B162" s="12">
         <v>9931</v>
       </c>
@@ -5378,7 +5378,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
+      <c r="A163" s="26"/>
       <c r="B163" s="12">
         <v>9696</v>
       </c>
@@ -5406,7 +5406,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="20"/>
+      <c r="A164" s="26"/>
       <c r="B164" s="12">
         <v>1947</v>
       </c>
@@ -5434,7 +5434,7 @@
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A165" s="20"/>
+      <c r="A165" s="26"/>
       <c r="B165" s="2">
         <v>4425</v>
       </c>
@@ -5462,7 +5462,7 @@
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A166" s="20"/>
+      <c r="A166" s="26"/>
       <c r="B166" s="2">
         <v>5683</v>
       </c>
@@ -5490,7 +5490,7 @@
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A167" s="20"/>
+      <c r="A167" s="26"/>
       <c r="B167" s="2">
         <v>1223</v>
       </c>
@@ -5518,7 +5518,7 @@
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168" s="20"/>
+      <c r="A168" s="26"/>
       <c r="B168" s="2">
         <v>3946</v>
       </c>
@@ -5546,7 +5546,7 @@
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A169" s="20"/>
+      <c r="A169" s="26"/>
       <c r="B169" s="2">
         <v>3940</v>
       </c>
@@ -5574,7 +5574,7 @@
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A170" s="20"/>
+      <c r="A170" s="26"/>
       <c r="B170" s="2">
         <v>8311</v>
       </c>
@@ -5602,7 +5602,7 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A171" s="20"/>
+      <c r="A171" s="26"/>
       <c r="B171" s="2">
         <v>3134</v>
       </c>
@@ -5630,7 +5630,7 @@
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A172" s="20"/>
+      <c r="A172" s="26"/>
       <c r="B172" s="2">
         <v>9774</v>
       </c>
@@ -5658,7 +5658,7 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173" s="20"/>
+      <c r="A173" s="26"/>
       <c r="B173" s="2">
         <v>9711</v>
       </c>
@@ -5686,7 +5686,7 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="20"/>
+      <c r="A174" s="26"/>
       <c r="B174" s="2">
         <v>3333</v>
       </c>
@@ -5714,7 +5714,7 @@
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A175" s="20"/>
+      <c r="A175" s="26"/>
       <c r="B175" s="2">
         <v>8820</v>
       </c>
@@ -5742,7 +5742,7 @@
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" s="20"/>
+      <c r="A176" s="26"/>
       <c r="B176" s="2">
         <v>7290</v>
       </c>
@@ -5770,7 +5770,7 @@
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A177" s="20"/>
+      <c r="A177" s="26"/>
       <c r="B177" s="2">
         <v>5694</v>
       </c>
@@ -5798,7 +5798,7 @@
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A178" s="20"/>
+      <c r="A178" s="26"/>
       <c r="B178" s="2">
         <v>6806</v>
       </c>
@@ -5826,7 +5826,7 @@
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A179" s="20"/>
+      <c r="A179" s="26"/>
       <c r="B179" s="2">
         <v>7369</v>
       </c>
@@ -5854,7 +5854,7 @@
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A180" s="20"/>
+      <c r="A180" s="26"/>
       <c r="B180" s="2">
         <v>5894</v>
       </c>
@@ -5882,7 +5882,7 @@
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A181" s="20"/>
+      <c r="A181" s="26"/>
       <c r="B181" s="2">
         <v>4515</v>
       </c>
@@ -5910,7 +5910,7 @@
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A182" s="20"/>
+      <c r="A182" s="26"/>
       <c r="B182" s="2">
         <v>7035</v>
       </c>
@@ -5938,7 +5938,7 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A183" s="20"/>
+      <c r="A183" s="26"/>
       <c r="B183" s="2">
         <v>9271</v>
       </c>
@@ -5966,7 +5966,7 @@
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="20"/>
+      <c r="A184" s="26"/>
       <c r="B184" s="2">
         <v>8769</v>
       </c>
@@ -5994,7 +5994,7 @@
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A185" s="20"/>
+      <c r="A185" s="26"/>
       <c r="B185" s="2">
         <v>4497</v>
       </c>
@@ -6022,7 +6022,7 @@
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A186" s="20"/>
+      <c r="A186" s="26"/>
       <c r="B186" s="2">
         <v>3218</v>
       </c>
@@ -6050,7 +6050,7 @@
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A187" s="20"/>
+      <c r="A187" s="26"/>
       <c r="B187" s="2">
         <v>4283</v>
       </c>
@@ -6078,7 +6078,7 @@
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="20"/>
+      <c r="A188" s="26"/>
       <c r="B188" s="2">
         <v>7703</v>
       </c>
@@ -6106,7 +6106,7 @@
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A189" s="20"/>
+      <c r="A189" s="26"/>
       <c r="B189" s="2">
         <v>5541</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="21"/>
+      <c r="A190" s="27"/>
       <c r="B190" s="6">
         <v>9182</v>
       </c>
@@ -6162,7 +6162,7 @@
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A191" s="19" t="s">
+      <c r="A191" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B191" s="8">
@@ -6192,7 +6192,7 @@
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A192" s="20"/>
+      <c r="A192" s="26"/>
       <c r="B192" s="2">
         <v>4642</v>
       </c>
@@ -6220,7 +6220,7 @@
       </c>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A193" s="20"/>
+      <c r="A193" s="26"/>
       <c r="B193" s="2">
         <v>4488</v>
       </c>
@@ -6248,7 +6248,7 @@
       </c>
     </row>
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A194" s="20"/>
+      <c r="A194" s="26"/>
       <c r="B194" s="2">
         <v>9765</v>
       </c>
@@ -6276,7 +6276,7 @@
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="20"/>
+      <c r="A195" s="26"/>
       <c r="B195" s="2">
         <v>4954</v>
       </c>
@@ -6304,7 +6304,7 @@
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A196" s="20"/>
+      <c r="A196" s="26"/>
       <c r="B196" s="2">
         <v>5537</v>
       </c>
@@ -6332,7 +6332,7 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="20"/>
+      <c r="A197" s="26"/>
       <c r="B197" s="2">
         <v>6431</v>
       </c>
@@ -6360,7 +6360,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="20"/>
+      <c r="A198" s="26"/>
       <c r="B198" s="2">
         <v>7193</v>
       </c>
@@ -6383,12 +6383,12 @@
       <c r="S198" s="2"/>
       <c r="T198" s="5"/>
       <c r="U198">
-        <f t="shared" ref="U198:U270" ca="1" si="5">IF(B198=$W$1,1,0)</f>
+        <f t="shared" ref="U198:U271" ca="1" si="5">IF(B198=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="20"/>
+      <c r="A199" s="26"/>
       <c r="B199" s="2">
         <v>5621</v>
       </c>
@@ -6416,7 +6416,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="20"/>
+      <c r="A200" s="26"/>
       <c r="B200" s="2">
         <v>5847</v>
       </c>
@@ -6444,7 +6444,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="20"/>
+      <c r="A201" s="26"/>
       <c r="B201" s="2">
         <v>4769</v>
       </c>
@@ -6472,7 +6472,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="20"/>
+      <c r="A202" s="26"/>
       <c r="B202" s="2">
         <v>9930</v>
       </c>
@@ -6500,7 +6500,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="20"/>
+      <c r="A203" s="26"/>
       <c r="B203" s="2">
         <v>3226</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="20"/>
+      <c r="A204" s="26"/>
       <c r="B204" s="2">
         <v>6861</v>
       </c>
@@ -6556,7 +6556,7 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="20"/>
+      <c r="A205" s="26"/>
       <c r="B205" s="2">
         <v>5032</v>
       </c>
@@ -6584,7 +6584,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="20"/>
+      <c r="A206" s="26"/>
       <c r="B206" s="2">
         <v>2033</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="20"/>
+      <c r="A207" s="26"/>
       <c r="B207" s="2">
         <v>5108</v>
       </c>
@@ -6640,7 +6640,7 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="20"/>
+      <c r="A208" s="26"/>
       <c r="B208" s="2">
         <v>3567</v>
       </c>
@@ -6668,7 +6668,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="20"/>
+      <c r="A209" s="26"/>
       <c r="B209" s="2">
         <v>2205</v>
       </c>
@@ -6696,7 +6696,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="20"/>
+      <c r="A210" s="26"/>
       <c r="B210" s="2">
         <v>4372</v>
       </c>
@@ -6724,7 +6724,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="20"/>
+      <c r="A211" s="26"/>
       <c r="B211" s="2">
         <v>4463</v>
       </c>
@@ -6752,7 +6752,7 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="20"/>
+      <c r="A212" s="26"/>
       <c r="B212" s="2">
         <v>1668</v>
       </c>
@@ -6780,7 +6780,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="21"/>
+      <c r="A213" s="27"/>
       <c r="B213" s="6">
         <v>2137</v>
       </c>
@@ -6808,7 +6808,7 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="19" t="s">
+      <c r="A214" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B214" s="8">
@@ -6838,7 +6838,7 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="20"/>
+      <c r="A215" s="26"/>
       <c r="B215" s="2">
         <v>3951</v>
       </c>
@@ -6866,7 +6866,7 @@
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A216" s="20"/>
+      <c r="A216" s="26"/>
       <c r="B216" s="2">
         <v>6409</v>
       </c>
@@ -6894,7 +6894,7 @@
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A217" s="20"/>
+      <c r="A217" s="26"/>
       <c r="B217" s="2">
         <v>3290</v>
       </c>
@@ -6922,7 +6922,7 @@
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A218" s="20"/>
+      <c r="A218" s="26"/>
       <c r="B218" s="2">
         <v>4342</v>
       </c>
@@ -6950,7 +6950,7 @@
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A219" s="20"/>
+      <c r="A219" s="26"/>
       <c r="B219" s="2">
         <v>2386</v>
       </c>
@@ -6978,7 +6978,7 @@
       </c>
     </row>
     <row r="220" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="20"/>
+      <c r="A220" s="26"/>
       <c r="B220" s="6">
         <v>9159</v>
       </c>
@@ -7002,7 +7002,7 @@
       <c r="T220" s="5"/>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A221" s="20"/>
+      <c r="A221" s="26"/>
       <c r="B221" s="2">
         <v>5309</v>
       </c>
@@ -7030,7 +7030,7 @@
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A222" s="20"/>
+      <c r="A222" s="26"/>
       <c r="B222" s="2">
         <v>5345</v>
       </c>
@@ -7058,7 +7058,7 @@
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A223" s="20"/>
+      <c r="A223" s="26"/>
       <c r="B223" s="2">
         <v>6812</v>
       </c>
@@ -7086,7 +7086,7 @@
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A224" s="20"/>
+      <c r="A224" s="26"/>
       <c r="B224" s="2">
         <v>7343</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
     </row>
     <row r="225" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="21"/>
+      <c r="A225" s="27"/>
       <c r="B225" s="6">
         <v>7060</v>
       </c>
@@ -7142,7 +7142,7 @@
       </c>
     </row>
     <row r="226" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="19" t="s">
+      <c r="A226" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B226" s="13">
@@ -7172,7 +7172,7 @@
       </c>
     </row>
     <row r="227" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="20"/>
+      <c r="A227" s="26"/>
       <c r="B227" s="12">
         <v>1516</v>
       </c>
@@ -7200,7 +7200,7 @@
       </c>
     </row>
     <row r="228" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A228" s="20"/>
+      <c r="A228" s="26"/>
       <c r="B228" s="12">
         <v>9062</v>
       </c>
@@ -7228,7 +7228,7 @@
       </c>
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A229" s="20"/>
+      <c r="A229" s="26"/>
       <c r="B229" s="2">
         <v>8861</v>
       </c>
@@ -7256,7 +7256,7 @@
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A230" s="20"/>
+      <c r="A230" s="26"/>
       <c r="B230" s="2">
         <v>5164</v>
       </c>
@@ -7284,7 +7284,7 @@
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A231" s="20"/>
+      <c r="A231" s="26"/>
       <c r="B231" s="2">
         <v>2030</v>
       </c>
@@ -7312,7 +7312,7 @@
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A232" s="20"/>
+      <c r="A232" s="26"/>
       <c r="B232" s="2">
         <v>7649</v>
       </c>
@@ -7340,7 +7340,7 @@
       </c>
     </row>
     <row r="233" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="21"/>
+      <c r="A233" s="27"/>
       <c r="B233" s="6">
         <v>2354</v>
       </c>
@@ -7368,7 +7368,7 @@
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A234" s="19" t="s">
+      <c r="A234" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B234" s="8">
@@ -7398,7 +7398,7 @@
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A235" s="20"/>
+      <c r="A235" s="26"/>
       <c r="B235" s="2">
         <v>1212</v>
       </c>
@@ -7426,7 +7426,7 @@
       </c>
     </row>
     <row r="236" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A236" s="20"/>
+      <c r="A236" s="26"/>
       <c r="B236" s="2">
         <v>9472</v>
       </c>
@@ -7454,7 +7454,7 @@
       </c>
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A237" s="20"/>
+      <c r="A237" s="26"/>
       <c r="B237" s="2">
         <v>5081</v>
       </c>
@@ -7482,7 +7482,7 @@
       </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="20"/>
+      <c r="A238" s="26"/>
       <c r="B238" s="2">
         <v>6454</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="20"/>
+      <c r="A239" s="26"/>
       <c r="B239" s="2">
         <v>6882</v>
       </c>
@@ -7538,7 +7538,7 @@
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A240" s="20"/>
+      <c r="A240" s="26"/>
       <c r="B240" s="2">
         <v>3784</v>
       </c>
@@ -7566,7 +7566,7 @@
       </c>
     </row>
     <row r="241" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="21"/>
+      <c r="A241" s="27"/>
       <c r="B241" s="6">
         <v>6732</v>
       </c>
@@ -7594,7 +7594,7 @@
       </c>
     </row>
     <row r="242" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="19" t="s">
+      <c r="A242" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B242" s="13">
@@ -7624,7 +7624,7 @@
       </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="20"/>
+      <c r="A243" s="26"/>
       <c r="B243" s="2">
         <v>3185</v>
       </c>
@@ -7652,7 +7652,7 @@
       </c>
     </row>
     <row r="244" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A244" s="20"/>
+      <c r="A244" s="26"/>
       <c r="B244" s="2">
         <v>9914</v>
       </c>
@@ -7680,7 +7680,7 @@
       </c>
     </row>
     <row r="245" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A245" s="20"/>
+      <c r="A245" s="26"/>
       <c r="B245" s="2">
         <v>6011</v>
       </c>
@@ -7708,7 +7708,7 @@
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="20"/>
+      <c r="A246" s="26"/>
       <c r="B246" s="2">
         <v>6037</v>
       </c>
@@ -7736,7 +7736,7 @@
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="20"/>
+      <c r="A247" s="26"/>
       <c r="B247" s="2">
         <v>2809</v>
       </c>
@@ -7764,7 +7764,7 @@
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A248" s="20"/>
+      <c r="A248" s="26"/>
       <c r="B248" s="2">
         <v>7297</v>
       </c>
@@ -7792,7 +7792,7 @@
       </c>
     </row>
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A249" s="20"/>
+      <c r="A249" s="26"/>
       <c r="B249" s="2">
         <v>5242</v>
       </c>
@@ -7820,7 +7820,7 @@
       </c>
     </row>
     <row r="250" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A250" s="20"/>
+      <c r="A250" s="26"/>
       <c r="B250" s="2">
         <v>1379</v>
       </c>
@@ -7848,7 +7848,7 @@
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="20"/>
+      <c r="A251" s="26"/>
       <c r="B251" s="2">
         <v>2401</v>
       </c>
@@ -7876,7 +7876,7 @@
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A252" s="20"/>
+      <c r="A252" s="26"/>
       <c r="B252" s="2">
         <v>5421</v>
       </c>
@@ -7904,9 +7904,9 @@
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A253" s="20"/>
+      <c r="A253" s="26"/>
       <c r="B253" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7932,9 +7932,9 @@
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" s="20"/>
+      <c r="A254" s="26"/>
       <c r="B254" s="2">
-        <v>6981</v>
+        <v>7301</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7960,9 +7960,9 @@
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A255" s="20"/>
+      <c r="A255" s="26"/>
       <c r="B255" s="2">
-        <v>2000</v>
+        <v>6981</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -7988,9 +7988,9 @@
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="20"/>
+      <c r="A256" s="26"/>
       <c r="B256" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8016,9 +8016,9 @@
       </c>
     </row>
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A257" s="20"/>
+      <c r="A257" s="26"/>
       <c r="B257" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8044,9 +8044,9 @@
       </c>
     </row>
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A258" s="20"/>
+      <c r="A258" s="26"/>
       <c r="B258" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8072,9 +8072,9 @@
       </c>
     </row>
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A259" s="20"/>
+      <c r="A259" s="26"/>
       <c r="B259" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8100,9 +8100,9 @@
       </c>
     </row>
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="20"/>
+      <c r="A260" s="26"/>
       <c r="B260" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8127,96 +8127,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="21"/>
-      <c r="B261" s="6">
-        <v>8403</v>
-      </c>
-      <c r="C261" s="6"/>
-      <c r="D261" s="6"/>
-      <c r="E261" s="6"/>
-      <c r="F261" s="6"/>
-      <c r="G261" s="6"/>
-      <c r="H261" s="6"/>
-      <c r="I261" s="6"/>
-      <c r="J261" s="6"/>
-      <c r="K261" s="6"/>
-      <c r="L261" s="6"/>
-      <c r="M261" s="6"/>
-      <c r="N261" s="6"/>
-      <c r="O261" s="6"/>
-      <c r="P261" s="6"/>
-      <c r="Q261" s="6"/>
-      <c r="R261" s="6"/>
-      <c r="S261" s="6"/>
-      <c r="T261" s="7"/>
+    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A261" s="26"/>
+      <c r="B261" s="2">
+        <v>3956</v>
+      </c>
+      <c r="C261" s="2"/>
+      <c r="D261" s="2"/>
+      <c r="E261" s="2"/>
+      <c r="F261" s="2"/>
+      <c r="G261" s="2"/>
+      <c r="H261" s="2"/>
+      <c r="I261" s="2"/>
+      <c r="J261" s="2"/>
+      <c r="K261" s="2"/>
+      <c r="L261" s="2"/>
+      <c r="M261" s="2"/>
+      <c r="N261" s="2"/>
+      <c r="O261" s="2"/>
+      <c r="P261" s="2"/>
+      <c r="Q261" s="2"/>
+      <c r="R261" s="2"/>
+      <c r="S261" s="2"/>
+      <c r="T261" s="5"/>
       <c r="U261">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B262" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C262" s="8"/>
-      <c r="D262" s="8"/>
-      <c r="E262" s="8"/>
-      <c r="F262" s="8"/>
-      <c r="G262" s="8"/>
-      <c r="H262" s="8"/>
-      <c r="I262" s="8"/>
-      <c r="J262" s="8"/>
-      <c r="K262" s="8"/>
-      <c r="L262" s="8"/>
-      <c r="M262" s="8"/>
-      <c r="N262" s="8"/>
-      <c r="O262" s="8"/>
-      <c r="P262" s="8"/>
-      <c r="Q262" s="8"/>
-      <c r="R262" s="8"/>
-      <c r="S262" s="8"/>
-      <c r="T262" s="14"/>
+    <row r="262" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="27"/>
+      <c r="B262" s="6">
+        <v>8403</v>
+      </c>
+      <c r="C262" s="6"/>
+      <c r="D262" s="6"/>
+      <c r="E262" s="6"/>
+      <c r="F262" s="6"/>
+      <c r="G262" s="6"/>
+      <c r="H262" s="6"/>
+      <c r="I262" s="6"/>
+      <c r="J262" s="6"/>
+      <c r="K262" s="6"/>
+      <c r="L262" s="6"/>
+      <c r="M262" s="6"/>
+      <c r="N262" s="6"/>
+      <c r="O262" s="6"/>
+      <c r="P262" s="6"/>
+      <c r="Q262" s="6"/>
+      <c r="R262" s="6"/>
+      <c r="S262" s="6"/>
+      <c r="T262" s="7"/>
       <c r="U262">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A263" s="20"/>
-      <c r="B263" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2"/>
-      <c r="E263" s="2"/>
-      <c r="F263" s="2"/>
-      <c r="G263" s="2"/>
-      <c r="H263" s="2"/>
-      <c r="I263" s="2"/>
-      <c r="J263" s="2"/>
-      <c r="K263" s="2"/>
-      <c r="L263" s="2"/>
-      <c r="M263" s="2"/>
-      <c r="N263" s="2"/>
-      <c r="O263" s="2"/>
-      <c r="P263" s="2"/>
-      <c r="Q263" s="2"/>
-      <c r="R263" s="2"/>
-      <c r="S263" s="2"/>
-      <c r="T263" s="5"/>
+      <c r="A263" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B263" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C263" s="8"/>
+      <c r="D263" s="8"/>
+      <c r="E263" s="8"/>
+      <c r="F263" s="8"/>
+      <c r="G263" s="8"/>
+      <c r="H263" s="8"/>
+      <c r="I263" s="8"/>
+      <c r="J263" s="8"/>
+      <c r="K263" s="8"/>
+      <c r="L263" s="8"/>
+      <c r="M263" s="8"/>
+      <c r="N263" s="8"/>
+      <c r="O263" s="8"/>
+      <c r="P263" s="8"/>
+      <c r="Q263" s="8"/>
+      <c r="R263" s="8"/>
+      <c r="S263" s="8"/>
+      <c r="T263" s="14"/>
       <c r="U263">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A264" s="20"/>
+      <c r="A264" s="26"/>
       <c r="B264" s="2">
-        <v>9990</v>
+        <v>5087</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8242,9 +8242,9 @@
       </c>
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A265" s="20"/>
+      <c r="A265" s="26"/>
       <c r="B265" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8270,9 +8270,9 @@
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="20"/>
+      <c r="A266" s="26"/>
       <c r="B266" s="2">
-        <v>9924</v>
+        <v>7738</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8298,37 +8298,37 @@
       </c>
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="24"/>
-      <c r="B267" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C267" s="9"/>
-      <c r="D267" s="9"/>
-      <c r="E267" s="9"/>
-      <c r="F267" s="9"/>
-      <c r="G267" s="9"/>
-      <c r="H267" s="9"/>
-      <c r="I267" s="9"/>
-      <c r="J267" s="9"/>
-      <c r="K267" s="9"/>
-      <c r="L267" s="9"/>
-      <c r="M267" s="9"/>
-      <c r="N267" s="9"/>
-      <c r="O267" s="9"/>
-      <c r="P267" s="9"/>
-      <c r="Q267" s="9"/>
-      <c r="R267" s="9"/>
-      <c r="S267" s="9"/>
-      <c r="T267" s="15"/>
+      <c r="A267" s="26"/>
+      <c r="B267" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C267" s="2"/>
+      <c r="D267" s="2"/>
+      <c r="E267" s="2"/>
+      <c r="F267" s="2"/>
+      <c r="G267" s="2"/>
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+      <c r="J267" s="2"/>
+      <c r="K267" s="2"/>
+      <c r="L267" s="2"/>
+      <c r="M267" s="2"/>
+      <c r="N267" s="2"/>
+      <c r="O267" s="2"/>
+      <c r="P267" s="2"/>
+      <c r="Q267" s="2"/>
+      <c r="R267" s="2"/>
+      <c r="S267" s="2"/>
+      <c r="T267" s="5"/>
       <c r="U267">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="24"/>
+      <c r="A268" s="28"/>
       <c r="B268" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C268" s="9"/>
       <c r="D268" s="9"/>
@@ -8354,9 +8354,9 @@
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="24"/>
+      <c r="A269" s="28"/>
       <c r="B269" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C269" s="9"/>
       <c r="D269" s="9"/>
@@ -8382,9 +8382,9 @@
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="24"/>
+      <c r="A270" s="28"/>
       <c r="B270" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C270" s="9"/>
       <c r="D270" s="9"/>
@@ -8409,96 +8409,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="21"/>
-      <c r="B271" s="6">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A271" s="28"/>
+      <c r="B271" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C271" s="9"/>
+      <c r="D271" s="9"/>
+      <c r="E271" s="9"/>
+      <c r="F271" s="9"/>
+      <c r="G271" s="9"/>
+      <c r="H271" s="9"/>
+      <c r="I271" s="9"/>
+      <c r="J271" s="9"/>
+      <c r="K271" s="9"/>
+      <c r="L271" s="9"/>
+      <c r="M271" s="9"/>
+      <c r="N271" s="9"/>
+      <c r="O271" s="9"/>
+      <c r="P271" s="9"/>
+      <c r="Q271" s="9"/>
+      <c r="R271" s="9"/>
+      <c r="S271" s="9"/>
+      <c r="T271" s="15"/>
+      <c r="U271">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="27"/>
+      <c r="B272" s="6">
         <v>6876</v>
       </c>
-      <c r="C271" s="6"/>
-      <c r="D271" s="6"/>
-      <c r="E271" s="6"/>
-      <c r="F271" s="6"/>
-      <c r="G271" s="6"/>
-      <c r="H271" s="6"/>
-      <c r="I271" s="6"/>
-      <c r="J271" s="6"/>
-      <c r="K271" s="6"/>
-      <c r="L271" s="6"/>
-      <c r="M271" s="6"/>
-      <c r="N271" s="6"/>
-      <c r="O271" s="6"/>
-      <c r="P271" s="6"/>
-      <c r="Q271" s="6"/>
-      <c r="R271" s="6"/>
-      <c r="S271" s="6"/>
-      <c r="T271" s="7"/>
-      <c r="U271">
-        <f t="shared" ref="U271:U334" ca="1" si="6">IF(B271=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="19" t="s">
+      <c r="C272" s="6"/>
+      <c r="D272" s="6"/>
+      <c r="E272" s="6"/>
+      <c r="F272" s="6"/>
+      <c r="G272" s="6"/>
+      <c r="H272" s="6"/>
+      <c r="I272" s="6"/>
+      <c r="J272" s="6"/>
+      <c r="K272" s="6"/>
+      <c r="L272" s="6"/>
+      <c r="M272" s="6"/>
+      <c r="N272" s="6"/>
+      <c r="O272" s="6"/>
+      <c r="P272" s="6"/>
+      <c r="Q272" s="6"/>
+      <c r="R272" s="6"/>
+      <c r="S272" s="6"/>
+      <c r="T272" s="7"/>
+      <c r="U272">
+        <f t="shared" ref="U272:U335" ca="1" si="6">IF(B272=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A273" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B272" s="8">
+      <c r="B273" s="8">
         <v>4304</v>
       </c>
-      <c r="C272" s="8"/>
-      <c r="D272" s="8"/>
-      <c r="E272" s="8"/>
-      <c r="F272" s="8"/>
-      <c r="G272" s="8"/>
-      <c r="H272" s="8"/>
-      <c r="I272" s="8"/>
-      <c r="J272" s="8"/>
-      <c r="K272" s="8"/>
-      <c r="L272" s="8"/>
-      <c r="M272" s="8"/>
-      <c r="N272" s="8"/>
-      <c r="O272" s="8"/>
-      <c r="P272" s="8"/>
-      <c r="Q272" s="8"/>
-      <c r="R272" s="8"/>
-      <c r="S272" s="8"/>
-      <c r="T272" s="14"/>
-      <c r="U272">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="20"/>
-      <c r="B273" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="E273" s="2"/>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="2"/>
-      <c r="J273" s="2"/>
-      <c r="K273" s="2"/>
-      <c r="L273" s="2"/>
-      <c r="M273" s="2"/>
-      <c r="N273" s="2"/>
-      <c r="O273" s="2"/>
-      <c r="P273" s="2"/>
-      <c r="Q273" s="2"/>
-      <c r="R273" s="2"/>
-      <c r="S273" s="2"/>
-      <c r="T273" s="5"/>
+      <c r="C273" s="8"/>
+      <c r="D273" s="8"/>
+      <c r="E273" s="8"/>
+      <c r="F273" s="8"/>
+      <c r="G273" s="8"/>
+      <c r="H273" s="8"/>
+      <c r="I273" s="8"/>
+      <c r="J273" s="8"/>
+      <c r="K273" s="8"/>
+      <c r="L273" s="8"/>
+      <c r="M273" s="8"/>
+      <c r="N273" s="8"/>
+      <c r="O273" s="8"/>
+      <c r="P273" s="8"/>
+      <c r="Q273" s="8"/>
+      <c r="R273" s="8"/>
+      <c r="S273" s="8"/>
+      <c r="T273" s="14"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="20"/>
+      <c r="A274" s="26"/>
       <c r="B274" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8524,9 +8524,9 @@
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="20"/>
+      <c r="A275" s="26"/>
       <c r="B275" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8551,96 +8551,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="21"/>
-      <c r="B276" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C276" s="6"/>
-      <c r="D276" s="6"/>
-      <c r="E276" s="6"/>
-      <c r="F276" s="6"/>
-      <c r="G276" s="6"/>
-      <c r="H276" s="6"/>
-      <c r="I276" s="6"/>
-      <c r="J276" s="6"/>
-      <c r="K276" s="6"/>
-      <c r="L276" s="6"/>
-      <c r="M276" s="6"/>
-      <c r="N276" s="6"/>
-      <c r="O276" s="6"/>
-      <c r="P276" s="6"/>
-      <c r="Q276" s="6"/>
-      <c r="R276" s="6"/>
-      <c r="S276" s="6"/>
-      <c r="T276" s="7"/>
+    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A276" s="26"/>
+      <c r="B276" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C276" s="2"/>
+      <c r="D276" s="2"/>
+      <c r="E276" s="2"/>
+      <c r="F276" s="2"/>
+      <c r="G276" s="2"/>
+      <c r="H276" s="2"/>
+      <c r="I276" s="2"/>
+      <c r="J276" s="2"/>
+      <c r="K276" s="2"/>
+      <c r="L276" s="2"/>
+      <c r="M276" s="2"/>
+      <c r="N276" s="2"/>
+      <c r="O276" s="2"/>
+      <c r="P276" s="2"/>
+      <c r="Q276" s="2"/>
+      <c r="R276" s="2"/>
+      <c r="S276" s="2"/>
+      <c r="T276" s="5"/>
       <c r="U276">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A277" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B277" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C277" s="8"/>
-      <c r="D277" s="8"/>
-      <c r="E277" s="8"/>
-      <c r="F277" s="8"/>
-      <c r="G277" s="8"/>
-      <c r="H277" s="8"/>
-      <c r="I277" s="8"/>
-      <c r="J277" s="8"/>
-      <c r="K277" s="8"/>
-      <c r="L277" s="8"/>
-      <c r="M277" s="8"/>
-      <c r="N277" s="8"/>
-      <c r="O277" s="8"/>
-      <c r="P277" s="8"/>
-      <c r="Q277" s="8"/>
-      <c r="R277" s="8"/>
-      <c r="S277" s="8"/>
-      <c r="T277" s="14"/>
+    <row r="277" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A277" s="27"/>
+      <c r="B277" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C277" s="6"/>
+      <c r="D277" s="6"/>
+      <c r="E277" s="6"/>
+      <c r="F277" s="6"/>
+      <c r="G277" s="6"/>
+      <c r="H277" s="6"/>
+      <c r="I277" s="6"/>
+      <c r="J277" s="6"/>
+      <c r="K277" s="6"/>
+      <c r="L277" s="6"/>
+      <c r="M277" s="6"/>
+      <c r="N277" s="6"/>
+      <c r="O277" s="6"/>
+      <c r="P277" s="6"/>
+      <c r="Q277" s="6"/>
+      <c r="R277" s="6"/>
+      <c r="S277" s="6"/>
+      <c r="T277" s="7"/>
       <c r="U277">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A278" s="20"/>
-      <c r="B278" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
-      <c r="E278" s="2"/>
-      <c r="F278" s="2"/>
-      <c r="G278" s="2"/>
-      <c r="H278" s="2"/>
-      <c r="I278" s="2"/>
-      <c r="J278" s="2"/>
-      <c r="K278" s="2"/>
-      <c r="L278" s="2"/>
-      <c r="M278" s="2"/>
-      <c r="N278" s="2"/>
-      <c r="O278" s="2"/>
-      <c r="P278" s="2"/>
-      <c r="Q278" s="2"/>
-      <c r="R278" s="2"/>
-      <c r="S278" s="2"/>
-      <c r="T278" s="5"/>
+      <c r="A278" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B278" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C278" s="8"/>
+      <c r="D278" s="8"/>
+      <c r="E278" s="8"/>
+      <c r="F278" s="8"/>
+      <c r="G278" s="8"/>
+      <c r="H278" s="8"/>
+      <c r="I278" s="8"/>
+      <c r="J278" s="8"/>
+      <c r="K278" s="8"/>
+      <c r="L278" s="8"/>
+      <c r="M278" s="8"/>
+      <c r="N278" s="8"/>
+      <c r="O278" s="8"/>
+      <c r="P278" s="8"/>
+      <c r="Q278" s="8"/>
+      <c r="R278" s="8"/>
+      <c r="S278" s="8"/>
+      <c r="T278" s="14"/>
       <c r="U278">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A279" s="20"/>
+      <c r="A279" s="26"/>
       <c r="B279" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8665,10 +8665,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="20"/>
-      <c r="B280" s="2">
-        <v>7170</v>
+    <row r="280" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A280" s="26"/>
+      <c r="B280" s="12">
+        <v>7546</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8694,9 +8694,9 @@
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="20"/>
+      <c r="A281" s="26"/>
       <c r="B281" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8722,9 +8722,9 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="20"/>
+      <c r="A282" s="26"/>
       <c r="B282" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8750,9 +8750,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="20"/>
+      <c r="A283" s="26"/>
       <c r="B283" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8778,9 +8778,9 @@
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="20"/>
+      <c r="A284" s="26"/>
       <c r="B284" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8806,9 +8806,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="20"/>
+      <c r="A285" s="26"/>
       <c r="B285" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8834,9 +8834,9 @@
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="20"/>
+      <c r="A286" s="26"/>
       <c r="B286" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8862,9 +8862,9 @@
       </c>
     </row>
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="20"/>
+      <c r="A287" s="26"/>
       <c r="B287" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8890,9 +8890,9 @@
       </c>
     </row>
     <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="20"/>
+      <c r="A288" s="26"/>
       <c r="B288" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -8918,9 +8918,9 @@
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="20"/>
+      <c r="A289" s="26"/>
       <c r="B289" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -8946,9 +8946,9 @@
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="20"/>
+      <c r="A290" s="26"/>
       <c r="B290" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8974,9 +8974,9 @@
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A291" s="20"/>
+      <c r="A291" s="26"/>
       <c r="B291" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9001,96 +9001,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="21"/>
-      <c r="B292" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="6"/>
-      <c r="H292" s="6"/>
-      <c r="I292" s="6"/>
-      <c r="J292" s="6"/>
-      <c r="K292" s="6"/>
-      <c r="L292" s="6"/>
-      <c r="M292" s="6"/>
-      <c r="N292" s="6"/>
-      <c r="O292" s="6"/>
-      <c r="P292" s="6"/>
-      <c r="Q292" s="6"/>
-      <c r="R292" s="6"/>
-      <c r="S292" s="6"/>
-      <c r="T292" s="7"/>
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A292" s="26"/>
+      <c r="B292" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C292" s="2"/>
+      <c r="D292" s="2"/>
+      <c r="E292" s="2"/>
+      <c r="F292" s="2"/>
+      <c r="G292" s="2"/>
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+      <c r="J292" s="2"/>
+      <c r="K292" s="2"/>
+      <c r="L292" s="2"/>
+      <c r="M292" s="2"/>
+      <c r="N292" s="2"/>
+      <c r="O292" s="2"/>
+      <c r="P292" s="2"/>
+      <c r="Q292" s="2"/>
+      <c r="R292" s="2"/>
+      <c r="S292" s="2"/>
+      <c r="T292" s="5"/>
       <c r="U292">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B293" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="14"/>
+    <row r="293" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="27"/>
+      <c r="B293" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C293" s="6"/>
+      <c r="D293" s="6"/>
+      <c r="E293" s="6"/>
+      <c r="F293" s="6"/>
+      <c r="G293" s="6"/>
+      <c r="H293" s="6"/>
+      <c r="I293" s="6"/>
+      <c r="J293" s="6"/>
+      <c r="K293" s="6"/>
+      <c r="L293" s="6"/>
+      <c r="M293" s="6"/>
+      <c r="N293" s="6"/>
+      <c r="O293" s="6"/>
+      <c r="P293" s="6"/>
+      <c r="Q293" s="6"/>
+      <c r="R293" s="6"/>
+      <c r="S293" s="6"/>
+      <c r="T293" s="7"/>
       <c r="U293">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="20"/>
-      <c r="B294" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
-      <c r="E294" s="2"/>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
-      <c r="H294" s="2"/>
-      <c r="I294" s="2"/>
-      <c r="J294" s="2"/>
-      <c r="K294" s="2"/>
-      <c r="L294" s="2"/>
-      <c r="M294" s="2"/>
-      <c r="N294" s="2"/>
-      <c r="O294" s="2"/>
-      <c r="P294" s="2"/>
-      <c r="Q294" s="2"/>
-      <c r="R294" s="2"/>
-      <c r="S294" s="2"/>
-      <c r="T294" s="5"/>
+      <c r="A294" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B294" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C294" s="8"/>
+      <c r="D294" s="8"/>
+      <c r="E294" s="8"/>
+      <c r="F294" s="8"/>
+      <c r="G294" s="8"/>
+      <c r="H294" s="8"/>
+      <c r="I294" s="8"/>
+      <c r="J294" s="8"/>
+      <c r="K294" s="8"/>
+      <c r="L294" s="8"/>
+      <c r="M294" s="8"/>
+      <c r="N294" s="8"/>
+      <c r="O294" s="8"/>
+      <c r="P294" s="8"/>
+      <c r="Q294" s="8"/>
+      <c r="R294" s="8"/>
+      <c r="S294" s="8"/>
+      <c r="T294" s="14"/>
       <c r="U294">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="20"/>
+      <c r="A295" s="26"/>
       <c r="B295" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9116,9 +9116,9 @@
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A296" s="20"/>
+      <c r="A296" s="26"/>
       <c r="B296" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9144,9 +9144,9 @@
       </c>
     </row>
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A297" s="20"/>
+      <c r="A297" s="26"/>
       <c r="B297" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9171,96 +9171,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="21"/>
-      <c r="B298" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C298" s="6"/>
-      <c r="D298" s="6"/>
-      <c r="E298" s="6"/>
-      <c r="F298" s="6"/>
-      <c r="G298" s="6"/>
-      <c r="H298" s="6"/>
-      <c r="I298" s="6"/>
-      <c r="J298" s="6"/>
-      <c r="K298" s="6"/>
-      <c r="L298" s="6"/>
-      <c r="M298" s="6"/>
-      <c r="N298" s="6"/>
-      <c r="O298" s="6"/>
-      <c r="P298" s="6"/>
-      <c r="Q298" s="6"/>
-      <c r="R298" s="6"/>
-      <c r="S298" s="6"/>
-      <c r="T298" s="7"/>
+    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A298" s="26"/>
+      <c r="B298" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C298" s="2"/>
+      <c r="D298" s="2"/>
+      <c r="E298" s="2"/>
+      <c r="F298" s="2"/>
+      <c r="G298" s="2"/>
+      <c r="H298" s="2"/>
+      <c r="I298" s="2"/>
+      <c r="J298" s="2"/>
+      <c r="K298" s="2"/>
+      <c r="L298" s="2"/>
+      <c r="M298" s="2"/>
+      <c r="N298" s="2"/>
+      <c r="O298" s="2"/>
+      <c r="P298" s="2"/>
+      <c r="Q298" s="2"/>
+      <c r="R298" s="2"/>
+      <c r="S298" s="2"/>
+      <c r="T298" s="5"/>
       <c r="U298">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A299" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B299" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C299" s="8"/>
-      <c r="D299" s="8"/>
-      <c r="E299" s="8"/>
-      <c r="F299" s="8"/>
-      <c r="G299" s="8"/>
-      <c r="H299" s="8"/>
-      <c r="I299" s="8"/>
-      <c r="J299" s="8"/>
-      <c r="K299" s="8"/>
-      <c r="L299" s="8"/>
-      <c r="M299" s="8"/>
-      <c r="N299" s="8"/>
-      <c r="O299" s="8"/>
-      <c r="P299" s="8"/>
-      <c r="Q299" s="8"/>
-      <c r="R299" s="8"/>
-      <c r="S299" s="8"/>
-      <c r="T299" s="14"/>
+    <row r="299" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A299" s="27"/>
+      <c r="B299" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C299" s="6"/>
+      <c r="D299" s="6"/>
+      <c r="E299" s="6"/>
+      <c r="F299" s="6"/>
+      <c r="G299" s="6"/>
+      <c r="H299" s="6"/>
+      <c r="I299" s="6"/>
+      <c r="J299" s="6"/>
+      <c r="K299" s="6"/>
+      <c r="L299" s="6"/>
+      <c r="M299" s="6"/>
+      <c r="N299" s="6"/>
+      <c r="O299" s="6"/>
+      <c r="P299" s="6"/>
+      <c r="Q299" s="6"/>
+      <c r="R299" s="6"/>
+      <c r="S299" s="6"/>
+      <c r="T299" s="7"/>
       <c r="U299">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A300" s="20"/>
-      <c r="B300" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C300" s="2"/>
-      <c r="D300" s="2"/>
-      <c r="E300" s="2"/>
-      <c r="F300" s="2"/>
-      <c r="G300" s="2"/>
-      <c r="H300" s="2"/>
-      <c r="I300" s="2"/>
-      <c r="J300" s="2"/>
-      <c r="K300" s="2"/>
-      <c r="L300" s="2"/>
-      <c r="M300" s="2"/>
-      <c r="N300" s="2"/>
-      <c r="O300" s="2"/>
-      <c r="P300" s="2"/>
-      <c r="Q300" s="2"/>
-      <c r="R300" s="2"/>
-      <c r="S300" s="2"/>
-      <c r="T300" s="5"/>
+      <c r="A300" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B300" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C300" s="8"/>
+      <c r="D300" s="8"/>
+      <c r="E300" s="8"/>
+      <c r="F300" s="8"/>
+      <c r="G300" s="8"/>
+      <c r="H300" s="8"/>
+      <c r="I300" s="8"/>
+      <c r="J300" s="8"/>
+      <c r="K300" s="8"/>
+      <c r="L300" s="8"/>
+      <c r="M300" s="8"/>
+      <c r="N300" s="8"/>
+      <c r="O300" s="8"/>
+      <c r="P300" s="8"/>
+      <c r="Q300" s="8"/>
+      <c r="R300" s="8"/>
+      <c r="S300" s="8"/>
+      <c r="T300" s="14"/>
       <c r="U300">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="20"/>
+      <c r="A301" s="26"/>
       <c r="B301" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9285,10 +9285,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A302" s="20"/>
+    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A302" s="26"/>
       <c r="B302" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9314,9 +9314,9 @@
       </c>
     </row>
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A303" s="20"/>
+      <c r="A303" s="26"/>
       <c r="B303" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9341,125 +9341,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="21"/>
-      <c r="B304" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C304" s="6"/>
-      <c r="D304" s="6"/>
-      <c r="E304" s="6"/>
-      <c r="F304" s="6"/>
-      <c r="G304" s="6"/>
-      <c r="H304" s="6"/>
-      <c r="I304" s="6"/>
-      <c r="J304" s="6"/>
-      <c r="K304" s="6"/>
-      <c r="L304" s="6"/>
-      <c r="M304" s="6"/>
-      <c r="N304" s="6"/>
-      <c r="O304" s="6"/>
-      <c r="P304" s="6"/>
-      <c r="Q304" s="6"/>
-      <c r="R304" s="6"/>
-      <c r="S304" s="6"/>
-      <c r="T304" s="7"/>
+    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A304" s="26"/>
+      <c r="B304" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C304" s="2"/>
+      <c r="D304" s="2"/>
+      <c r="E304" s="2"/>
+      <c r="F304" s="2"/>
+      <c r="G304" s="2"/>
+      <c r="H304" s="2"/>
+      <c r="I304" s="2"/>
+      <c r="J304" s="2"/>
+      <c r="K304" s="2"/>
+      <c r="L304" s="2"/>
+      <c r="M304" s="2"/>
+      <c r="N304" s="2"/>
+      <c r="O304" s="2"/>
+      <c r="P304" s="2"/>
+      <c r="Q304" s="2"/>
+      <c r="R304" s="2"/>
+      <c r="S304" s="2"/>
+      <c r="T304" s="5"/>
       <c r="U304">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="27"/>
+      <c r="B305" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C305" s="6"/>
+      <c r="D305" s="6"/>
+      <c r="E305" s="6"/>
+      <c r="F305" s="6"/>
+      <c r="G305" s="6"/>
+      <c r="H305" s="6"/>
+      <c r="I305" s="6"/>
+      <c r="J305" s="6"/>
+      <c r="K305" s="6"/>
+      <c r="L305" s="6"/>
+      <c r="M305" s="6"/>
+      <c r="N305" s="6"/>
+      <c r="O305" s="6"/>
+      <c r="P305" s="6"/>
+      <c r="Q305" s="6"/>
+      <c r="R305" s="6"/>
+      <c r="S305" s="6"/>
+      <c r="T305" s="7"/>
       <c r="U305">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U306">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U307">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U308">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U309">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U310">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U311">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U312">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U313">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U314">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U315">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U316">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U317">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U318">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U319">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U320">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9551,13 +9573,13 @@
     </row>
     <row r="335" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U335">
-        <f t="shared" ref="U335:U398" ca="1" si="7">IF(B335=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="336" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U336">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="U336:U399" ca="1" si="7">IF(B336=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9935,13 +9957,13 @@
     </row>
     <row r="399" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U399">
-        <f t="shared" ref="U399:U462" ca="1" si="8">IF(B399=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="400" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U400">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U400:U463" ca="1" si="8">IF(B400=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10319,13 +10341,13 @@
     </row>
     <row r="463" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U463">
-        <f t="shared" ref="U463:U526" ca="1" si="9">IF(B463=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="464" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U464">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U464:U527" ca="1" si="9">IF(B464=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10703,13 +10725,13 @@
     </row>
     <row r="527" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U527">
-        <f t="shared" ref="U527:U590" ca="1" si="10">IF(B527=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="528" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U528">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U528:U591" ca="1" si="10">IF(B528=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11087,13 +11109,13 @@
     </row>
     <row r="591" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U591">
-        <f t="shared" ref="U591:U654" ca="1" si="11">IF(B591=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="592" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U592">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U592:U655" ca="1" si="11">IF(B592=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11471,13 +11493,13 @@
     </row>
     <row r="655" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U655">
-        <f t="shared" ref="U655:U718" ca="1" si="12">IF(B655=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="656" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U656">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U656:U719" ca="1" si="12">IF(B656=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11855,13 +11877,13 @@
     </row>
     <row r="719" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U719">
-        <f t="shared" ref="U719:U782" ca="1" si="13">IF(B719=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="720" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U720">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U720:U783" ca="1" si="13">IF(B720=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12239,13 +12261,13 @@
     </row>
     <row r="783" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U783">
-        <f t="shared" ref="U783:U846" ca="1" si="14">IF(B783=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="784" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U784">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U784:U847" ca="1" si="14">IF(B784=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12623,13 +12645,13 @@
     </row>
     <row r="847" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U847">
-        <f t="shared" ref="U847:U908" ca="1" si="15">IF(B847=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="848" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U848">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U848:U909" ca="1" si="15">IF(B848=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12993,17 +13015,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="909" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U909">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A226:A233"/>
+    <mergeCell ref="A234:A241"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A272:A276"/>
-    <mergeCell ref="A262:A271"/>
-    <mergeCell ref="A299:A304"/>
-    <mergeCell ref="A242:A261"/>
+    <mergeCell ref="A273:A277"/>
+    <mergeCell ref="A263:A272"/>
+    <mergeCell ref="A300:A305"/>
+    <mergeCell ref="A242:A262"/>
     <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A277:A292"/>
-    <mergeCell ref="A293:A298"/>
+    <mergeCell ref="A278:A293"/>
+    <mergeCell ref="A294:A299"/>
     <mergeCell ref="A61:A100"/>
     <mergeCell ref="A214:A225"/>
     <mergeCell ref="A191:A213"/>
@@ -13011,8 +13041,6 @@
     <mergeCell ref="A144:A160"/>
     <mergeCell ref="A101:A143"/>
     <mergeCell ref="A20:A60"/>
-    <mergeCell ref="A226:A233"/>
-    <mergeCell ref="A234:A241"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task for processing multiple files based on special file
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$278</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$279</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -505,6 +505,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,24 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,11 +840,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W910"/>
+  <dimension ref="A1:W911"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y197" sqref="Y197"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B216" sqref="B216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -861,56 +861,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9706</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="30"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -940,7 +940,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -970,7 +970,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75">
-      <c r="A6" s="30"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75">
-      <c r="A7" s="30"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A19" s="28"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="9">
         <v>4764</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="13">
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75">
-      <c r="A21" s="32"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="12">
         <v>3730</v>
       </c>
@@ -1420,7 +1420,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75">
-      <c r="A22" s="32"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="12">
         <v>9007</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75">
-      <c r="A23" s="32"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="12">
         <v>9578</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="32"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="2">
         <v>4411</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="32"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="2">
         <v>9298</v>
       </c>
@@ -1532,7 +1532,7 @@
       </c>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="32"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="2">
         <v>3354</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="32"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="2">
         <v>5201</v>
       </c>
@@ -1588,7 +1588,7 @@
       </c>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="32"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2">
         <v>2981</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="32"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2">
         <v>4312</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="32"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2">
         <v>8428</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="32"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2">
         <v>2361</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="32"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="2">
         <v>5063</v>
       </c>
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="32"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2">
         <v>7711</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="32"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2">
         <v>8833</v>
       </c>
@@ -1784,7 +1784,7 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="32"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2">
         <v>1262</v>
       </c>
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="32"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="2">
         <v>9020</v>
       </c>
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="37" spans="1:21">
-      <c r="A37" s="32"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="2">
         <v>1934</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="38" spans="1:21">
-      <c r="A38" s="32"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="2">
         <v>7237</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="32"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="2">
         <v>3943</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="32"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="2">
         <v>7619</v>
       </c>
@@ -1952,7 +1952,7 @@
       </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="32"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="2">
         <v>3832</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="32"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="2">
         <v>1346</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="43" spans="1:21">
-      <c r="A43" s="32"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="2">
         <v>9622</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="32"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="2">
         <v>8873</v>
       </c>
@@ -2064,7 +2064,7 @@
       </c>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="32"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="2">
         <v>7799</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46" s="32"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="2">
         <v>9354</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="32"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="2">
         <v>9130</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="48" spans="1:21">
-      <c r="A48" s="32"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="2">
         <v>5895</v>
       </c>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="49" spans="1:21">
-      <c r="A49" s="32"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="2">
         <v>2461</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="50" spans="1:21">
-      <c r="A50" s="32"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="2">
         <v>2790</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
     </row>
     <row r="51" spans="1:21">
-      <c r="A51" s="32"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="2">
         <v>2624</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="52" spans="1:21">
-      <c r="A52" s="32"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="2">
         <v>5871</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="53" spans="1:21">
-      <c r="A53" s="32"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="2">
         <v>9164</v>
       </c>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="54" spans="1:21">
-      <c r="A54" s="32"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="2">
         <v>7457</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
     </row>
     <row r="55" spans="1:21">
-      <c r="A55" s="32"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="2">
         <v>9865</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="56" spans="1:21">
-      <c r="A56" s="32"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="2">
         <v>3591</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="57" spans="1:21">
-      <c r="A57" s="32"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="2">
         <v>3558</v>
       </c>
@@ -2428,7 +2428,7 @@
       </c>
     </row>
     <row r="58" spans="1:21">
-      <c r="A58" s="32"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="2">
         <v>4366</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
     </row>
     <row r="59" spans="1:21">
-      <c r="A59" s="32"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="2">
         <v>5789</v>
       </c>
@@ -2484,7 +2484,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A60" s="33"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="6">
         <v>6522</v>
       </c>
@@ -6381,7 +6381,7 @@
       <c r="S198" s="2"/>
       <c r="T198" s="5"/>
       <c r="U198">
-        <f t="shared" ref="U198:U272" ca="1" si="5">IF(B198=$W$1,1,0)</f>
+        <f t="shared" ref="U198:U273" ca="1" si="5">IF(B198=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6778,7 +6778,7 @@
       </c>
     </row>
     <row r="213" spans="1:21">
-      <c r="A213" s="28"/>
+      <c r="A213" s="24"/>
       <c r="B213" s="9">
         <v>2137</v>
       </c>
@@ -6805,87 +6805,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A214" s="21"/>
-      <c r="B214" s="6">
+    <row r="214" spans="1:21">
+      <c r="A214" s="24"/>
+      <c r="B214" s="9">
         <v>9417</v>
       </c>
-      <c r="C214" s="6"/>
-      <c r="D214" s="6"/>
-      <c r="E214" s="6"/>
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
-      <c r="H214" s="6"/>
-      <c r="I214" s="6"/>
-      <c r="J214" s="6"/>
-      <c r="K214" s="6"/>
-      <c r="L214" s="6"/>
-      <c r="M214" s="6"/>
-      <c r="N214" s="6"/>
-      <c r="O214" s="6"/>
-      <c r="P214" s="6"/>
-      <c r="Q214" s="6"/>
-      <c r="R214" s="6"/>
-      <c r="S214" s="6"/>
-      <c r="T214" s="7"/>
+      <c r="C214" s="9"/>
+      <c r="D214" s="9"/>
+      <c r="E214" s="9"/>
+      <c r="F214" s="9"/>
+      <c r="G214" s="9"/>
+      <c r="H214" s="9"/>
+      <c r="I214" s="9"/>
+      <c r="J214" s="9"/>
+      <c r="K214" s="9"/>
+      <c r="L214" s="9"/>
+      <c r="M214" s="9"/>
+      <c r="N214" s="9"/>
+      <c r="O214" s="9"/>
+      <c r="P214" s="9"/>
+      <c r="Q214" s="9"/>
+      <c r="R214" s="9"/>
+      <c r="S214" s="9"/>
+      <c r="T214" s="15"/>
       <c r="U214">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:21">
-      <c r="A215" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B215" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C215" s="8"/>
-      <c r="D215" s="8"/>
-      <c r="E215" s="8"/>
-      <c r="F215" s="8"/>
-      <c r="G215" s="8"/>
-      <c r="H215" s="8"/>
-      <c r="I215" s="8"/>
-      <c r="J215" s="8"/>
-      <c r="K215" s="8"/>
-      <c r="L215" s="8"/>
-      <c r="M215" s="8"/>
-      <c r="N215" s="8"/>
-      <c r="O215" s="8"/>
-      <c r="P215" s="8"/>
-      <c r="Q215" s="8"/>
-      <c r="R215" s="8"/>
-      <c r="S215" s="8"/>
-      <c r="T215" s="14"/>
+    <row r="215" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A215" s="21"/>
+      <c r="B215" s="6">
+        <v>3148</v>
+      </c>
+      <c r="C215" s="6"/>
+      <c r="D215" s="6"/>
+      <c r="E215" s="6"/>
+      <c r="F215" s="6"/>
+      <c r="G215" s="6"/>
+      <c r="H215" s="6"/>
+      <c r="I215" s="6"/>
+      <c r="J215" s="6"/>
+      <c r="K215" s="6"/>
+      <c r="L215" s="6"/>
+      <c r="M215" s="6"/>
+      <c r="N215" s="6"/>
+      <c r="O215" s="6"/>
+      <c r="P215" s="6"/>
+      <c r="Q215" s="6"/>
+      <c r="R215" s="6"/>
+      <c r="S215" s="6"/>
+      <c r="T215" s="7"/>
       <c r="U215">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:21">
-      <c r="A216" s="20"/>
-      <c r="B216" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C216" s="2"/>
-      <c r="D216" s="2"/>
-      <c r="E216" s="2"/>
-      <c r="F216" s="2"/>
-      <c r="G216" s="2"/>
-      <c r="H216" s="2"/>
-      <c r="I216" s="2"/>
-      <c r="J216" s="2"/>
-      <c r="K216" s="2"/>
-      <c r="L216" s="2"/>
-      <c r="M216" s="2"/>
-      <c r="N216" s="2"/>
-      <c r="O216" s="2"/>
-      <c r="P216" s="2"/>
-      <c r="Q216" s="2"/>
-      <c r="R216" s="2"/>
-      <c r="S216" s="2"/>
-      <c r="T216" s="5"/>
+      <c r="A216" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B216" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C216" s="8"/>
+      <c r="D216" s="8"/>
+      <c r="E216" s="8"/>
+      <c r="F216" s="8"/>
+      <c r="G216" s="8"/>
+      <c r="H216" s="8"/>
+      <c r="I216" s="8"/>
+      <c r="J216" s="8"/>
+      <c r="K216" s="8"/>
+      <c r="L216" s="8"/>
+      <c r="M216" s="8"/>
+      <c r="N216" s="8"/>
+      <c r="O216" s="8"/>
+      <c r="P216" s="8"/>
+      <c r="Q216" s="8"/>
+      <c r="R216" s="8"/>
+      <c r="S216" s="8"/>
+      <c r="T216" s="14"/>
       <c r="U216">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -6894,7 +6894,7 @@
     <row r="217" spans="1:21">
       <c r="A217" s="20"/>
       <c r="B217" s="2">
-        <v>6409</v>
+        <v>3951</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6922,7 +6922,7 @@
     <row r="218" spans="1:21">
       <c r="A218" s="20"/>
       <c r="B218" s="2">
-        <v>3290</v>
+        <v>6409</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6950,7 +6950,7 @@
     <row r="219" spans="1:21">
       <c r="A219" s="20"/>
       <c r="B219" s="2">
-        <v>4342</v>
+        <v>3290</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -6978,7 +6978,7 @@
     <row r="220" spans="1:21">
       <c r="A220" s="20"/>
       <c r="B220" s="2">
-        <v>2386</v>
+        <v>4342</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -7003,10 +7003,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="15.75" thickBot="1">
+    <row r="221" spans="1:21">
       <c r="A221" s="20"/>
-      <c r="B221" s="6">
-        <v>9159</v>
+      <c r="B221" s="2">
+        <v>2386</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
@@ -7026,11 +7026,15 @@
       <c r="R221" s="2"/>
       <c r="S221" s="2"/>
       <c r="T221" s="5"/>
-    </row>
-    <row r="222" spans="1:21">
+      <c r="U221">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:21" ht="15.75" thickBot="1">
       <c r="A222" s="20"/>
-      <c r="B222" s="2">
-        <v>5309</v>
+      <c r="B222" s="6">
+        <v>9159</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -7050,15 +7054,11 @@
       <c r="R222" s="2"/>
       <c r="S222" s="2"/>
       <c r="T222" s="5"/>
-      <c r="U222">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="223" spans="1:21">
       <c r="A223" s="20"/>
       <c r="B223" s="2">
-        <v>5345</v>
+        <v>5309</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
@@ -7086,7 +7086,7 @@
     <row r="224" spans="1:21">
       <c r="A224" s="20"/>
       <c r="B224" s="2">
-        <v>6812</v>
+        <v>5345</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7114,7 +7114,7 @@
     <row r="225" spans="1:21">
       <c r="A225" s="20"/>
       <c r="B225" s="2">
-        <v>7343</v>
+        <v>6812</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -7139,87 +7139,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A226" s="21"/>
-      <c r="B226" s="6">
-        <v>7060</v>
-      </c>
-      <c r="C226" s="6"/>
-      <c r="D226" s="6"/>
-      <c r="E226" s="6"/>
-      <c r="F226" s="6"/>
-      <c r="G226" s="6"/>
-      <c r="H226" s="6"/>
-      <c r="I226" s="6"/>
-      <c r="J226" s="6"/>
-      <c r="K226" s="6"/>
-      <c r="L226" s="6"/>
-      <c r="M226" s="6"/>
-      <c r="N226" s="6"/>
-      <c r="O226" s="6"/>
-      <c r="P226" s="6"/>
-      <c r="Q226" s="6"/>
-      <c r="R226" s="6"/>
-      <c r="S226" s="6"/>
-      <c r="T226" s="7"/>
+    <row r="226" spans="1:21">
+      <c r="A226" s="20"/>
+      <c r="B226" s="2">
+        <v>7343</v>
+      </c>
+      <c r="C226" s="2"/>
+      <c r="D226" s="2"/>
+      <c r="E226" s="2"/>
+      <c r="F226" s="2"/>
+      <c r="G226" s="2"/>
+      <c r="H226" s="2"/>
+      <c r="I226" s="2"/>
+      <c r="J226" s="2"/>
+      <c r="K226" s="2"/>
+      <c r="L226" s="2"/>
+      <c r="M226" s="2"/>
+      <c r="N226" s="2"/>
+      <c r="O226" s="2"/>
+      <c r="P226" s="2"/>
+      <c r="Q226" s="2"/>
+      <c r="R226" s="2"/>
+      <c r="S226" s="2"/>
+      <c r="T226" s="5"/>
       <c r="U226">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="15.75">
-      <c r="A227" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B227" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C227" s="8"/>
-      <c r="D227" s="8"/>
-      <c r="E227" s="8"/>
-      <c r="F227" s="8"/>
-      <c r="G227" s="8"/>
-      <c r="H227" s="8"/>
-      <c r="I227" s="8"/>
-      <c r="J227" s="8"/>
-      <c r="K227" s="8"/>
-      <c r="L227" s="8"/>
-      <c r="M227" s="8"/>
-      <c r="N227" s="8"/>
-      <c r="O227" s="8"/>
-      <c r="P227" s="8"/>
-      <c r="Q227" s="8"/>
-      <c r="R227" s="8"/>
-      <c r="S227" s="8"/>
-      <c r="T227" s="14"/>
+    <row r="227" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A227" s="21"/>
+      <c r="B227" s="6">
+        <v>7060</v>
+      </c>
+      <c r="C227" s="6"/>
+      <c r="D227" s="6"/>
+      <c r="E227" s="6"/>
+      <c r="F227" s="6"/>
+      <c r="G227" s="6"/>
+      <c r="H227" s="6"/>
+      <c r="I227" s="6"/>
+      <c r="J227" s="6"/>
+      <c r="K227" s="6"/>
+      <c r="L227" s="6"/>
+      <c r="M227" s="6"/>
+      <c r="N227" s="6"/>
+      <c r="O227" s="6"/>
+      <c r="P227" s="6"/>
+      <c r="Q227" s="6"/>
+      <c r="R227" s="6"/>
+      <c r="S227" s="6"/>
+      <c r="T227" s="7"/>
       <c r="U227">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:21" ht="15.75">
-      <c r="A228" s="20"/>
-      <c r="B228" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C228" s="2"/>
-      <c r="D228" s="2"/>
-      <c r="E228" s="2"/>
-      <c r="F228" s="2"/>
-      <c r="G228" s="2"/>
-      <c r="H228" s="2"/>
-      <c r="I228" s="2"/>
-      <c r="J228" s="2"/>
-      <c r="K228" s="2"/>
-      <c r="L228" s="2"/>
-      <c r="M228" s="2"/>
-      <c r="N228" s="2"/>
-      <c r="O228" s="2"/>
-      <c r="P228" s="2"/>
-      <c r="Q228" s="2"/>
-      <c r="R228" s="2"/>
-      <c r="S228" s="2"/>
-      <c r="T228" s="5"/>
+      <c r="A228" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B228" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C228" s="8"/>
+      <c r="D228" s="8"/>
+      <c r="E228" s="8"/>
+      <c r="F228" s="8"/>
+      <c r="G228" s="8"/>
+      <c r="H228" s="8"/>
+      <c r="I228" s="8"/>
+      <c r="J228" s="8"/>
+      <c r="K228" s="8"/>
+      <c r="L228" s="8"/>
+      <c r="M228" s="8"/>
+      <c r="N228" s="8"/>
+      <c r="O228" s="8"/>
+      <c r="P228" s="8"/>
+      <c r="Q228" s="8"/>
+      <c r="R228" s="8"/>
+      <c r="S228" s="8"/>
+      <c r="T228" s="14"/>
       <c r="U228">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -7228,7 +7228,7 @@
     <row r="229" spans="1:21" ht="15.75">
       <c r="A229" s="20"/>
       <c r="B229" s="12">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -7253,10 +7253,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:21">
+    <row r="230" spans="1:21" ht="15.75">
       <c r="A230" s="20"/>
-      <c r="B230" s="2">
-        <v>8861</v>
+      <c r="B230" s="12">
+        <v>9062</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
@@ -7284,7 +7284,7 @@
     <row r="231" spans="1:21">
       <c r="A231" s="20"/>
       <c r="B231" s="2">
-        <v>5164</v>
+        <v>8861</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
@@ -7312,7 +7312,7 @@
     <row r="232" spans="1:21">
       <c r="A232" s="20"/>
       <c r="B232" s="2">
-        <v>2030</v>
+        <v>5164</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -7340,7 +7340,7 @@
     <row r="233" spans="1:21">
       <c r="A233" s="20"/>
       <c r="B233" s="2">
-        <v>7649</v>
+        <v>2030</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
@@ -7365,87 +7365,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A234" s="21"/>
-      <c r="B234" s="6">
-        <v>2354</v>
-      </c>
-      <c r="C234" s="6"/>
-      <c r="D234" s="6"/>
-      <c r="E234" s="6"/>
-      <c r="F234" s="6"/>
-      <c r="G234" s="6"/>
-      <c r="H234" s="6"/>
-      <c r="I234" s="6"/>
-      <c r="J234" s="6"/>
-      <c r="K234" s="6"/>
-      <c r="L234" s="6"/>
-      <c r="M234" s="6"/>
-      <c r="N234" s="6"/>
-      <c r="O234" s="6"/>
-      <c r="P234" s="6"/>
-      <c r="Q234" s="6"/>
-      <c r="R234" s="6"/>
-      <c r="S234" s="6"/>
-      <c r="T234" s="7"/>
+    <row r="234" spans="1:21">
+      <c r="A234" s="20"/>
+      <c r="B234" s="2">
+        <v>7649</v>
+      </c>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="2"/>
+      <c r="F234" s="2"/>
+      <c r="G234" s="2"/>
+      <c r="H234" s="2"/>
+      <c r="I234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="K234" s="2"/>
+      <c r="L234" s="2"/>
+      <c r="M234" s="2"/>
+      <c r="N234" s="2"/>
+      <c r="O234" s="2"/>
+      <c r="P234" s="2"/>
+      <c r="Q234" s="2"/>
+      <c r="R234" s="2"/>
+      <c r="S234" s="2"/>
+      <c r="T234" s="5"/>
       <c r="U234">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:21">
-      <c r="A235" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B235" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C235" s="8"/>
-      <c r="D235" s="8"/>
-      <c r="E235" s="8"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="8"/>
-      <c r="H235" s="8"/>
-      <c r="I235" s="8"/>
-      <c r="J235" s="8"/>
-      <c r="K235" s="8"/>
-      <c r="L235" s="8"/>
-      <c r="M235" s="8"/>
-      <c r="N235" s="8"/>
-      <c r="O235" s="8"/>
-      <c r="P235" s="8"/>
-      <c r="Q235" s="8"/>
-      <c r="R235" s="8"/>
-      <c r="S235" s="8"/>
-      <c r="T235" s="14"/>
+    <row r="235" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A235" s="21"/>
+      <c r="B235" s="6">
+        <v>2354</v>
+      </c>
+      <c r="C235" s="6"/>
+      <c r="D235" s="6"/>
+      <c r="E235" s="6"/>
+      <c r="F235" s="6"/>
+      <c r="G235" s="6"/>
+      <c r="H235" s="6"/>
+      <c r="I235" s="6"/>
+      <c r="J235" s="6"/>
+      <c r="K235" s="6"/>
+      <c r="L235" s="6"/>
+      <c r="M235" s="6"/>
+      <c r="N235" s="6"/>
+      <c r="O235" s="6"/>
+      <c r="P235" s="6"/>
+      <c r="Q235" s="6"/>
+      <c r="R235" s="6"/>
+      <c r="S235" s="6"/>
+      <c r="T235" s="7"/>
       <c r="U235">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:21">
-      <c r="A236" s="20"/>
-      <c r="B236" s="2">
-        <v>1212</v>
-      </c>
-      <c r="C236" s="2"/>
-      <c r="D236" s="2"/>
-      <c r="E236" s="2"/>
-      <c r="F236" s="2"/>
-      <c r="G236" s="2"/>
-      <c r="H236" s="2"/>
-      <c r="I236" s="2"/>
-      <c r="J236" s="2"/>
-      <c r="K236" s="2"/>
-      <c r="L236" s="2"/>
-      <c r="M236" s="2"/>
-      <c r="N236" s="2"/>
-      <c r="O236" s="2"/>
-      <c r="P236" s="2"/>
-      <c r="Q236" s="2"/>
-      <c r="R236" s="2"/>
-      <c r="S236" s="2"/>
-      <c r="T236" s="5"/>
+      <c r="A236" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B236" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C236" s="8"/>
+      <c r="D236" s="8"/>
+      <c r="E236" s="8"/>
+      <c r="F236" s="8"/>
+      <c r="G236" s="8"/>
+      <c r="H236" s="8"/>
+      <c r="I236" s="8"/>
+      <c r="J236" s="8"/>
+      <c r="K236" s="8"/>
+      <c r="L236" s="8"/>
+      <c r="M236" s="8"/>
+      <c r="N236" s="8"/>
+      <c r="O236" s="8"/>
+      <c r="P236" s="8"/>
+      <c r="Q236" s="8"/>
+      <c r="R236" s="8"/>
+      <c r="S236" s="8"/>
+      <c r="T236" s="14"/>
       <c r="U236">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -7454,7 +7454,7 @@
     <row r="237" spans="1:21">
       <c r="A237" s="20"/>
       <c r="B237" s="2">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
@@ -7482,7 +7482,7 @@
     <row r="238" spans="1:21">
       <c r="A238" s="20"/>
       <c r="B238" s="2">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -7510,7 +7510,7 @@
     <row r="239" spans="1:21">
       <c r="A239" s="20"/>
       <c r="B239" s="2">
-        <v>6454</v>
+        <v>5081</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -7538,7 +7538,7 @@
     <row r="240" spans="1:21">
       <c r="A240" s="20"/>
       <c r="B240" s="2">
-        <v>6882</v>
+        <v>6454</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
@@ -7566,7 +7566,7 @@
     <row r="241" spans="1:21">
       <c r="A241" s="20"/>
       <c r="B241" s="2">
-        <v>3784</v>
+        <v>6882</v>
       </c>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
@@ -7591,87 +7591,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A242" s="21"/>
-      <c r="B242" s="6">
-        <v>6732</v>
-      </c>
-      <c r="C242" s="6"/>
-      <c r="D242" s="6"/>
-      <c r="E242" s="6"/>
-      <c r="F242" s="6"/>
-      <c r="G242" s="6"/>
-      <c r="H242" s="6"/>
-      <c r="I242" s="6"/>
-      <c r="J242" s="6"/>
-      <c r="K242" s="6"/>
-      <c r="L242" s="6"/>
-      <c r="M242" s="6"/>
-      <c r="N242" s="6"/>
-      <c r="O242" s="6"/>
-      <c r="P242" s="6"/>
-      <c r="Q242" s="6"/>
-      <c r="R242" s="6"/>
-      <c r="S242" s="6"/>
-      <c r="T242" s="7"/>
+    <row r="242" spans="1:21">
+      <c r="A242" s="20"/>
+      <c r="B242" s="2">
+        <v>3784</v>
+      </c>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="2"/>
+      <c r="F242" s="2"/>
+      <c r="G242" s="2"/>
+      <c r="H242" s="2"/>
+      <c r="I242" s="2"/>
+      <c r="J242" s="2"/>
+      <c r="K242" s="2"/>
+      <c r="L242" s="2"/>
+      <c r="M242" s="2"/>
+      <c r="N242" s="2"/>
+      <c r="O242" s="2"/>
+      <c r="P242" s="2"/>
+      <c r="Q242" s="2"/>
+      <c r="R242" s="2"/>
+      <c r="S242" s="2"/>
+      <c r="T242" s="5"/>
       <c r="U242">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="15.75">
-      <c r="A243" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B243" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C243" s="8"/>
-      <c r="D243" s="8"/>
-      <c r="E243" s="8"/>
-      <c r="F243" s="8"/>
-      <c r="G243" s="8"/>
-      <c r="H243" s="8"/>
-      <c r="I243" s="8"/>
-      <c r="J243" s="8"/>
-      <c r="K243" s="8"/>
-      <c r="L243" s="8"/>
-      <c r="M243" s="8"/>
-      <c r="N243" s="8"/>
-      <c r="O243" s="8"/>
-      <c r="P243" s="8"/>
-      <c r="Q243" s="8"/>
-      <c r="R243" s="8"/>
-      <c r="S243" s="8"/>
-      <c r="T243" s="14"/>
+    <row r="243" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A243" s="21"/>
+      <c r="B243" s="6">
+        <v>6732</v>
+      </c>
+      <c r="C243" s="6"/>
+      <c r="D243" s="6"/>
+      <c r="E243" s="6"/>
+      <c r="F243" s="6"/>
+      <c r="G243" s="6"/>
+      <c r="H243" s="6"/>
+      <c r="I243" s="6"/>
+      <c r="J243" s="6"/>
+      <c r="K243" s="6"/>
+      <c r="L243" s="6"/>
+      <c r="M243" s="6"/>
+      <c r="N243" s="6"/>
+      <c r="O243" s="6"/>
+      <c r="P243" s="6"/>
+      <c r="Q243" s="6"/>
+      <c r="R243" s="6"/>
+      <c r="S243" s="6"/>
+      <c r="T243" s="7"/>
       <c r="U243">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:21">
-      <c r="A244" s="20"/>
-      <c r="B244" s="2">
-        <v>3185</v>
-      </c>
-      <c r="C244" s="2"/>
-      <c r="D244" s="2"/>
-      <c r="E244" s="2"/>
-      <c r="F244" s="2"/>
-      <c r="G244" s="2"/>
-      <c r="H244" s="2"/>
-      <c r="I244" s="2"/>
-      <c r="J244" s="2"/>
-      <c r="K244" s="2"/>
-      <c r="L244" s="2"/>
-      <c r="M244" s="2"/>
-      <c r="N244" s="2"/>
-      <c r="O244" s="2"/>
-      <c r="P244" s="2"/>
-      <c r="Q244" s="2"/>
-      <c r="R244" s="2"/>
-      <c r="S244" s="2"/>
-      <c r="T244" s="5"/>
+    <row r="244" spans="1:21" ht="15.75">
+      <c r="A244" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B244" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C244" s="8"/>
+      <c r="D244" s="8"/>
+      <c r="E244" s="8"/>
+      <c r="F244" s="8"/>
+      <c r="G244" s="8"/>
+      <c r="H244" s="8"/>
+      <c r="I244" s="8"/>
+      <c r="J244" s="8"/>
+      <c r="K244" s="8"/>
+      <c r="L244" s="8"/>
+      <c r="M244" s="8"/>
+      <c r="N244" s="8"/>
+      <c r="O244" s="8"/>
+      <c r="P244" s="8"/>
+      <c r="Q244" s="8"/>
+      <c r="R244" s="8"/>
+      <c r="S244" s="8"/>
+      <c r="T244" s="14"/>
       <c r="U244">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -7680,7 +7680,7 @@
     <row r="245" spans="1:21">
       <c r="A245" s="20"/>
       <c r="B245" s="2">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7708,7 +7708,7 @@
     <row r="246" spans="1:21">
       <c r="A246" s="20"/>
       <c r="B246" s="2">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7736,7 +7736,7 @@
     <row r="247" spans="1:21">
       <c r="A247" s="20"/>
       <c r="B247" s="2">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7764,7 +7764,7 @@
     <row r="248" spans="1:21">
       <c r="A248" s="20"/>
       <c r="B248" s="2">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7792,7 +7792,7 @@
     <row r="249" spans="1:21">
       <c r="A249" s="20"/>
       <c r="B249" s="2">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -7820,7 +7820,7 @@
     <row r="250" spans="1:21">
       <c r="A250" s="20"/>
       <c r="B250" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -7848,7 +7848,7 @@
     <row r="251" spans="1:21">
       <c r="A251" s="20"/>
       <c r="B251" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7876,7 +7876,7 @@
     <row r="252" spans="1:21">
       <c r="A252" s="20"/>
       <c r="B252" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7904,7 +7904,7 @@
     <row r="253" spans="1:21">
       <c r="A253" s="20"/>
       <c r="B253" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7932,7 +7932,7 @@
     <row r="254" spans="1:21">
       <c r="A254" s="20"/>
       <c r="B254" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7960,7 +7960,7 @@
     <row r="255" spans="1:21">
       <c r="A255" s="20"/>
       <c r="B255" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -7988,7 +7988,7 @@
     <row r="256" spans="1:21">
       <c r="A256" s="20"/>
       <c r="B256" s="2">
-        <v>6981</v>
+        <v>7301</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8016,7 +8016,7 @@
     <row r="257" spans="1:21">
       <c r="A257" s="20"/>
       <c r="B257" s="2">
-        <v>2000</v>
+        <v>6981</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8044,7 +8044,7 @@
     <row r="258" spans="1:21">
       <c r="A258" s="20"/>
       <c r="B258" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8072,7 +8072,7 @@
     <row r="259" spans="1:21">
       <c r="A259" s="20"/>
       <c r="B259" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8100,7 +8100,7 @@
     <row r="260" spans="1:21">
       <c r="A260" s="20"/>
       <c r="B260" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8128,7 +8128,7 @@
     <row r="261" spans="1:21">
       <c r="A261" s="20"/>
       <c r="B261" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8156,7 +8156,7 @@
     <row r="262" spans="1:21">
       <c r="A262" s="20"/>
       <c r="B262" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8181,87 +8181,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A263" s="21"/>
-      <c r="B263" s="6">
-        <v>8403</v>
-      </c>
-      <c r="C263" s="6"/>
-      <c r="D263" s="6"/>
-      <c r="E263" s="6"/>
-      <c r="F263" s="6"/>
-      <c r="G263" s="6"/>
-      <c r="H263" s="6"/>
-      <c r="I263" s="6"/>
-      <c r="J263" s="6"/>
-      <c r="K263" s="6"/>
-      <c r="L263" s="6"/>
-      <c r="M263" s="6"/>
-      <c r="N263" s="6"/>
-      <c r="O263" s="6"/>
-      <c r="P263" s="6"/>
-      <c r="Q263" s="6"/>
-      <c r="R263" s="6"/>
-      <c r="S263" s="6"/>
-      <c r="T263" s="7"/>
+    <row r="263" spans="1:21">
+      <c r="A263" s="20"/>
+      <c r="B263" s="2">
+        <v>3956</v>
+      </c>
+      <c r="C263" s="2"/>
+      <c r="D263" s="2"/>
+      <c r="E263" s="2"/>
+      <c r="F263" s="2"/>
+      <c r="G263" s="2"/>
+      <c r="H263" s="2"/>
+      <c r="I263" s="2"/>
+      <c r="J263" s="2"/>
+      <c r="K263" s="2"/>
+      <c r="L263" s="2"/>
+      <c r="M263" s="2"/>
+      <c r="N263" s="2"/>
+      <c r="O263" s="2"/>
+      <c r="P263" s="2"/>
+      <c r="Q263" s="2"/>
+      <c r="R263" s="2"/>
+      <c r="S263" s="2"/>
+      <c r="T263" s="5"/>
       <c r="U263">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:21">
-      <c r="A264" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B264" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C264" s="8"/>
-      <c r="D264" s="8"/>
-      <c r="E264" s="8"/>
-      <c r="F264" s="8"/>
-      <c r="G264" s="8"/>
-      <c r="H264" s="8"/>
-      <c r="I264" s="8"/>
-      <c r="J264" s="8"/>
-      <c r="K264" s="8"/>
-      <c r="L264" s="8"/>
-      <c r="M264" s="8"/>
-      <c r="N264" s="8"/>
-      <c r="O264" s="8"/>
-      <c r="P264" s="8"/>
-      <c r="Q264" s="8"/>
-      <c r="R264" s="8"/>
-      <c r="S264" s="8"/>
-      <c r="T264" s="14"/>
+    <row r="264" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A264" s="21"/>
+      <c r="B264" s="6">
+        <v>8403</v>
+      </c>
+      <c r="C264" s="6"/>
+      <c r="D264" s="6"/>
+      <c r="E264" s="6"/>
+      <c r="F264" s="6"/>
+      <c r="G264" s="6"/>
+      <c r="H264" s="6"/>
+      <c r="I264" s="6"/>
+      <c r="J264" s="6"/>
+      <c r="K264" s="6"/>
+      <c r="L264" s="6"/>
+      <c r="M264" s="6"/>
+      <c r="N264" s="6"/>
+      <c r="O264" s="6"/>
+      <c r="P264" s="6"/>
+      <c r="Q264" s="6"/>
+      <c r="R264" s="6"/>
+      <c r="S264" s="6"/>
+      <c r="T264" s="7"/>
       <c r="U264">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:21">
-      <c r="A265" s="20"/>
-      <c r="B265" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C265" s="2"/>
-      <c r="D265" s="2"/>
-      <c r="E265" s="2"/>
-      <c r="F265" s="2"/>
-      <c r="G265" s="2"/>
-      <c r="H265" s="2"/>
-      <c r="I265" s="2"/>
-      <c r="J265" s="2"/>
-      <c r="K265" s="2"/>
-      <c r="L265" s="2"/>
-      <c r="M265" s="2"/>
-      <c r="N265" s="2"/>
-      <c r="O265" s="2"/>
-      <c r="P265" s="2"/>
-      <c r="Q265" s="2"/>
-      <c r="R265" s="2"/>
-      <c r="S265" s="2"/>
-      <c r="T265" s="5"/>
+      <c r="A265" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B265" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C265" s="8"/>
+      <c r="D265" s="8"/>
+      <c r="E265" s="8"/>
+      <c r="F265" s="8"/>
+      <c r="G265" s="8"/>
+      <c r="H265" s="8"/>
+      <c r="I265" s="8"/>
+      <c r="J265" s="8"/>
+      <c r="K265" s="8"/>
+      <c r="L265" s="8"/>
+      <c r="M265" s="8"/>
+      <c r="N265" s="8"/>
+      <c r="O265" s="8"/>
+      <c r="P265" s="8"/>
+      <c r="Q265" s="8"/>
+      <c r="R265" s="8"/>
+      <c r="S265" s="8"/>
+      <c r="T265" s="14"/>
       <c r="U265">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -8270,7 +8270,7 @@
     <row r="266" spans="1:21">
       <c r="A266" s="20"/>
       <c r="B266" s="2">
-        <v>9990</v>
+        <v>5087</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8298,7 +8298,7 @@
     <row r="267" spans="1:21">
       <c r="A267" s="20"/>
       <c r="B267" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8326,7 +8326,7 @@
     <row r="268" spans="1:21">
       <c r="A268" s="20"/>
       <c r="B268" s="2">
-        <v>9924</v>
+        <v>7738</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8352,37 +8352,37 @@
       </c>
     </row>
     <row r="269" spans="1:21">
-      <c r="A269" s="28"/>
-      <c r="B269" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C269" s="9"/>
-      <c r="D269" s="9"/>
-      <c r="E269" s="9"/>
-      <c r="F269" s="9"/>
-      <c r="G269" s="9"/>
-      <c r="H269" s="9"/>
-      <c r="I269" s="9"/>
-      <c r="J269" s="9"/>
-      <c r="K269" s="9"/>
-      <c r="L269" s="9"/>
-      <c r="M269" s="9"/>
-      <c r="N269" s="9"/>
-      <c r="O269" s="9"/>
-      <c r="P269" s="9"/>
-      <c r="Q269" s="9"/>
-      <c r="R269" s="9"/>
-      <c r="S269" s="9"/>
-      <c r="T269" s="15"/>
+      <c r="A269" s="20"/>
+      <c r="B269" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C269" s="2"/>
+      <c r="D269" s="2"/>
+      <c r="E269" s="2"/>
+      <c r="F269" s="2"/>
+      <c r="G269" s="2"/>
+      <c r="H269" s="2"/>
+      <c r="I269" s="2"/>
+      <c r="J269" s="2"/>
+      <c r="K269" s="2"/>
+      <c r="L269" s="2"/>
+      <c r="M269" s="2"/>
+      <c r="N269" s="2"/>
+      <c r="O269" s="2"/>
+      <c r="P269" s="2"/>
+      <c r="Q269" s="2"/>
+      <c r="R269" s="2"/>
+      <c r="S269" s="2"/>
+      <c r="T269" s="5"/>
       <c r="U269">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:21">
-      <c r="A270" s="28"/>
+      <c r="A270" s="24"/>
       <c r="B270" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C270" s="9"/>
       <c r="D270" s="9"/>
@@ -8408,9 +8408,9 @@
       </c>
     </row>
     <row r="271" spans="1:21">
-      <c r="A271" s="28"/>
+      <c r="A271" s="24"/>
       <c r="B271" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C271" s="9"/>
       <c r="D271" s="9"/>
@@ -8436,9 +8436,9 @@
       </c>
     </row>
     <row r="272" spans="1:21">
-      <c r="A272" s="28"/>
+      <c r="A272" s="24"/>
       <c r="B272" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C272" s="9"/>
       <c r="D272" s="9"/>
@@ -8463,87 +8463,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A273" s="21"/>
-      <c r="B273" s="6">
+    <row r="273" spans="1:21">
+      <c r="A273" s="24"/>
+      <c r="B273" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C273" s="9"/>
+      <c r="D273" s="9"/>
+      <c r="E273" s="9"/>
+      <c r="F273" s="9"/>
+      <c r="G273" s="9"/>
+      <c r="H273" s="9"/>
+      <c r="I273" s="9"/>
+      <c r="J273" s="9"/>
+      <c r="K273" s="9"/>
+      <c r="L273" s="9"/>
+      <c r="M273" s="9"/>
+      <c r="N273" s="9"/>
+      <c r="O273" s="9"/>
+      <c r="P273" s="9"/>
+      <c r="Q273" s="9"/>
+      <c r="R273" s="9"/>
+      <c r="S273" s="9"/>
+      <c r="T273" s="15"/>
+      <c r="U273">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A274" s="21"/>
+      <c r="B274" s="6">
         <v>6876</v>
       </c>
-      <c r="C273" s="6"/>
-      <c r="D273" s="6"/>
-      <c r="E273" s="6"/>
-      <c r="F273" s="6"/>
-      <c r="G273" s="6"/>
-      <c r="H273" s="6"/>
-      <c r="I273" s="6"/>
-      <c r="J273" s="6"/>
-      <c r="K273" s="6"/>
-      <c r="L273" s="6"/>
-      <c r="M273" s="6"/>
-      <c r="N273" s="6"/>
-      <c r="O273" s="6"/>
-      <c r="P273" s="6"/>
-      <c r="Q273" s="6"/>
-      <c r="R273" s="6"/>
-      <c r="S273" s="6"/>
-      <c r="T273" s="7"/>
-      <c r="U273">
-        <f t="shared" ref="U273:U336" ca="1" si="6">IF(B273=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:21">
-      <c r="A274" s="19" t="s">
+      <c r="C274" s="6"/>
+      <c r="D274" s="6"/>
+      <c r="E274" s="6"/>
+      <c r="F274" s="6"/>
+      <c r="G274" s="6"/>
+      <c r="H274" s="6"/>
+      <c r="I274" s="6"/>
+      <c r="J274" s="6"/>
+      <c r="K274" s="6"/>
+      <c r="L274" s="6"/>
+      <c r="M274" s="6"/>
+      <c r="N274" s="6"/>
+      <c r="O274" s="6"/>
+      <c r="P274" s="6"/>
+      <c r="Q274" s="6"/>
+      <c r="R274" s="6"/>
+      <c r="S274" s="6"/>
+      <c r="T274" s="7"/>
+      <c r="U274">
+        <f t="shared" ref="U274:U337" ca="1" si="6">IF(B274=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:21">
+      <c r="A275" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B274" s="8">
+      <c r="B275" s="8">
         <v>4304</v>
       </c>
-      <c r="C274" s="8"/>
-      <c r="D274" s="8"/>
-      <c r="E274" s="8"/>
-      <c r="F274" s="8"/>
-      <c r="G274" s="8"/>
-      <c r="H274" s="8"/>
-      <c r="I274" s="8"/>
-      <c r="J274" s="8"/>
-      <c r="K274" s="8"/>
-      <c r="L274" s="8"/>
-      <c r="M274" s="8"/>
-      <c r="N274" s="8"/>
-      <c r="O274" s="8"/>
-      <c r="P274" s="8"/>
-      <c r="Q274" s="8"/>
-      <c r="R274" s="8"/>
-      <c r="S274" s="8"/>
-      <c r="T274" s="14"/>
-      <c r="U274">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:21">
-      <c r="A275" s="20"/>
-      <c r="B275" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2"/>
-      <c r="E275" s="2"/>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="2"/>
-      <c r="J275" s="2"/>
-      <c r="K275" s="2"/>
-      <c r="L275" s="2"/>
-      <c r="M275" s="2"/>
-      <c r="N275" s="2"/>
-      <c r="O275" s="2"/>
-      <c r="P275" s="2"/>
-      <c r="Q275" s="2"/>
-      <c r="R275" s="2"/>
-      <c r="S275" s="2"/>
-      <c r="T275" s="5"/>
+      <c r="C275" s="8"/>
+      <c r="D275" s="8"/>
+      <c r="E275" s="8"/>
+      <c r="F275" s="8"/>
+      <c r="G275" s="8"/>
+      <c r="H275" s="8"/>
+      <c r="I275" s="8"/>
+      <c r="J275" s="8"/>
+      <c r="K275" s="8"/>
+      <c r="L275" s="8"/>
+      <c r="M275" s="8"/>
+      <c r="N275" s="8"/>
+      <c r="O275" s="8"/>
+      <c r="P275" s="8"/>
+      <c r="Q275" s="8"/>
+      <c r="R275" s="8"/>
+      <c r="S275" s="8"/>
+      <c r="T275" s="14"/>
       <c r="U275">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8552,7 +8552,7 @@
     <row r="276" spans="1:21">
       <c r="A276" s="20"/>
       <c r="B276" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8580,7 +8580,7 @@
     <row r="277" spans="1:21">
       <c r="A277" s="20"/>
       <c r="B277" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8605,87 +8605,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A278" s="21"/>
-      <c r="B278" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C278" s="6"/>
-      <c r="D278" s="6"/>
-      <c r="E278" s="6"/>
-      <c r="F278" s="6"/>
-      <c r="G278" s="6"/>
-      <c r="H278" s="6"/>
-      <c r="I278" s="6"/>
-      <c r="J278" s="6"/>
-      <c r="K278" s="6"/>
-      <c r="L278" s="6"/>
-      <c r="M278" s="6"/>
-      <c r="N278" s="6"/>
-      <c r="O278" s="6"/>
-      <c r="P278" s="6"/>
-      <c r="Q278" s="6"/>
-      <c r="R278" s="6"/>
-      <c r="S278" s="6"/>
-      <c r="T278" s="7"/>
+    <row r="278" spans="1:21">
+      <c r="A278" s="20"/>
+      <c r="B278" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C278" s="2"/>
+      <c r="D278" s="2"/>
+      <c r="E278" s="2"/>
+      <c r="F278" s="2"/>
+      <c r="G278" s="2"/>
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+      <c r="L278" s="2"/>
+      <c r="M278" s="2"/>
+      <c r="N278" s="2"/>
+      <c r="O278" s="2"/>
+      <c r="P278" s="2"/>
+      <c r="Q278" s="2"/>
+      <c r="R278" s="2"/>
+      <c r="S278" s="2"/>
+      <c r="T278" s="5"/>
       <c r="U278">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="15.75">
-      <c r="A279" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B279" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C279" s="8"/>
-      <c r="D279" s="8"/>
-      <c r="E279" s="8"/>
-      <c r="F279" s="8"/>
-      <c r="G279" s="8"/>
-      <c r="H279" s="8"/>
-      <c r="I279" s="8"/>
-      <c r="J279" s="8"/>
-      <c r="K279" s="8"/>
-      <c r="L279" s="8"/>
-      <c r="M279" s="8"/>
-      <c r="N279" s="8"/>
-      <c r="O279" s="8"/>
-      <c r="P279" s="8"/>
-      <c r="Q279" s="8"/>
-      <c r="R279" s="8"/>
-      <c r="S279" s="8"/>
-      <c r="T279" s="14"/>
+    <row r="279" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A279" s="21"/>
+      <c r="B279" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C279" s="6"/>
+      <c r="D279" s="6"/>
+      <c r="E279" s="6"/>
+      <c r="F279" s="6"/>
+      <c r="G279" s="6"/>
+      <c r="H279" s="6"/>
+      <c r="I279" s="6"/>
+      <c r="J279" s="6"/>
+      <c r="K279" s="6"/>
+      <c r="L279" s="6"/>
+      <c r="M279" s="6"/>
+      <c r="N279" s="6"/>
+      <c r="O279" s="6"/>
+      <c r="P279" s="6"/>
+      <c r="Q279" s="6"/>
+      <c r="R279" s="6"/>
+      <c r="S279" s="6"/>
+      <c r="T279" s="7"/>
       <c r="U279">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:21" ht="15.75">
-      <c r="A280" s="20"/>
-      <c r="B280" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="E280" s="2"/>
-      <c r="F280" s="2"/>
-      <c r="G280" s="2"/>
-      <c r="H280" s="2"/>
-      <c r="I280" s="2"/>
-      <c r="J280" s="2"/>
-      <c r="K280" s="2"/>
-      <c r="L280" s="2"/>
-      <c r="M280" s="2"/>
-      <c r="N280" s="2"/>
-      <c r="O280" s="2"/>
-      <c r="P280" s="2"/>
-      <c r="Q280" s="2"/>
-      <c r="R280" s="2"/>
-      <c r="S280" s="2"/>
-      <c r="T280" s="5"/>
+      <c r="A280" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B280" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C280" s="8"/>
+      <c r="D280" s="8"/>
+      <c r="E280" s="8"/>
+      <c r="F280" s="8"/>
+      <c r="G280" s="8"/>
+      <c r="H280" s="8"/>
+      <c r="I280" s="8"/>
+      <c r="J280" s="8"/>
+      <c r="K280" s="8"/>
+      <c r="L280" s="8"/>
+      <c r="M280" s="8"/>
+      <c r="N280" s="8"/>
+      <c r="O280" s="8"/>
+      <c r="P280" s="8"/>
+      <c r="Q280" s="8"/>
+      <c r="R280" s="8"/>
+      <c r="S280" s="8"/>
+      <c r="T280" s="14"/>
       <c r="U280">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8694,7 +8694,7 @@
     <row r="281" spans="1:21" ht="15.75">
       <c r="A281" s="20"/>
       <c r="B281" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8719,10 +8719,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:21">
+    <row r="282" spans="1:21" ht="15.75">
       <c r="A282" s="20"/>
-      <c r="B282" s="2">
-        <v>7170</v>
+      <c r="B282" s="12">
+        <v>7546</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8750,7 +8750,7 @@
     <row r="283" spans="1:21">
       <c r="A283" s="20"/>
       <c r="B283" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8778,7 +8778,7 @@
     <row r="284" spans="1:21">
       <c r="A284" s="20"/>
       <c r="B284" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8806,7 +8806,7 @@
     <row r="285" spans="1:21">
       <c r="A285" s="20"/>
       <c r="B285" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8834,7 +8834,7 @@
     <row r="286" spans="1:21">
       <c r="A286" s="20"/>
       <c r="B286" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8862,7 +8862,7 @@
     <row r="287" spans="1:21">
       <c r="A287" s="20"/>
       <c r="B287" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8890,7 +8890,7 @@
     <row r="288" spans="1:21">
       <c r="A288" s="20"/>
       <c r="B288" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -8918,7 +8918,7 @@
     <row r="289" spans="1:21">
       <c r="A289" s="20"/>
       <c r="B289" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -8946,7 +8946,7 @@
     <row r="290" spans="1:21">
       <c r="A290" s="20"/>
       <c r="B290" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8974,7 +8974,7 @@
     <row r="291" spans="1:21">
       <c r="A291" s="20"/>
       <c r="B291" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9002,7 +9002,7 @@
     <row r="292" spans="1:21">
       <c r="A292" s="20"/>
       <c r="B292" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9030,7 +9030,7 @@
     <row r="293" spans="1:21">
       <c r="A293" s="20"/>
       <c r="B293" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9055,87 +9055,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A294" s="21"/>
-      <c r="B294" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C294" s="6"/>
-      <c r="D294" s="6"/>
-      <c r="E294" s="6"/>
-      <c r="F294" s="6"/>
-      <c r="G294" s="6"/>
-      <c r="H294" s="6"/>
-      <c r="I294" s="6"/>
-      <c r="J294" s="6"/>
-      <c r="K294" s="6"/>
-      <c r="L294" s="6"/>
-      <c r="M294" s="6"/>
-      <c r="N294" s="6"/>
-      <c r="O294" s="6"/>
-      <c r="P294" s="6"/>
-      <c r="Q294" s="6"/>
-      <c r="R294" s="6"/>
-      <c r="S294" s="6"/>
-      <c r="T294" s="7"/>
+    <row r="294" spans="1:21">
+      <c r="A294" s="20"/>
+      <c r="B294" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C294" s="2"/>
+      <c r="D294" s="2"/>
+      <c r="E294" s="2"/>
+      <c r="F294" s="2"/>
+      <c r="G294" s="2"/>
+      <c r="H294" s="2"/>
+      <c r="I294" s="2"/>
+      <c r="J294" s="2"/>
+      <c r="K294" s="2"/>
+      <c r="L294" s="2"/>
+      <c r="M294" s="2"/>
+      <c r="N294" s="2"/>
+      <c r="O294" s="2"/>
+      <c r="P294" s="2"/>
+      <c r="Q294" s="2"/>
+      <c r="R294" s="2"/>
+      <c r="S294" s="2"/>
+      <c r="T294" s="5"/>
       <c r="U294">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:21">
-      <c r="A295" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B295" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C295" s="8"/>
-      <c r="D295" s="8"/>
-      <c r="E295" s="8"/>
-      <c r="F295" s="8"/>
-      <c r="G295" s="8"/>
-      <c r="H295" s="8"/>
-      <c r="I295" s="8"/>
-      <c r="J295" s="8"/>
-      <c r="K295" s="8"/>
-      <c r="L295" s="8"/>
-      <c r="M295" s="8"/>
-      <c r="N295" s="8"/>
-      <c r="O295" s="8"/>
-      <c r="P295" s="8"/>
-      <c r="Q295" s="8"/>
-      <c r="R295" s="8"/>
-      <c r="S295" s="8"/>
-      <c r="T295" s="14"/>
+    <row r="295" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A295" s="21"/>
+      <c r="B295" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C295" s="6"/>
+      <c r="D295" s="6"/>
+      <c r="E295" s="6"/>
+      <c r="F295" s="6"/>
+      <c r="G295" s="6"/>
+      <c r="H295" s="6"/>
+      <c r="I295" s="6"/>
+      <c r="J295" s="6"/>
+      <c r="K295" s="6"/>
+      <c r="L295" s="6"/>
+      <c r="M295" s="6"/>
+      <c r="N295" s="6"/>
+      <c r="O295" s="6"/>
+      <c r="P295" s="6"/>
+      <c r="Q295" s="6"/>
+      <c r="R295" s="6"/>
+      <c r="S295" s="6"/>
+      <c r="T295" s="7"/>
       <c r="U295">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:21">
-      <c r="A296" s="20"/>
-      <c r="B296" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C296" s="2"/>
-      <c r="D296" s="2"/>
-      <c r="E296" s="2"/>
-      <c r="F296" s="2"/>
-      <c r="G296" s="2"/>
-      <c r="H296" s="2"/>
-      <c r="I296" s="2"/>
-      <c r="J296" s="2"/>
-      <c r="K296" s="2"/>
-      <c r="L296" s="2"/>
-      <c r="M296" s="2"/>
-      <c r="N296" s="2"/>
-      <c r="O296" s="2"/>
-      <c r="P296" s="2"/>
-      <c r="Q296" s="2"/>
-      <c r="R296" s="2"/>
-      <c r="S296" s="2"/>
-      <c r="T296" s="5"/>
+      <c r="A296" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B296" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C296" s="8"/>
+      <c r="D296" s="8"/>
+      <c r="E296" s="8"/>
+      <c r="F296" s="8"/>
+      <c r="G296" s="8"/>
+      <c r="H296" s="8"/>
+      <c r="I296" s="8"/>
+      <c r="J296" s="8"/>
+      <c r="K296" s="8"/>
+      <c r="L296" s="8"/>
+      <c r="M296" s="8"/>
+      <c r="N296" s="8"/>
+      <c r="O296" s="8"/>
+      <c r="P296" s="8"/>
+      <c r="Q296" s="8"/>
+      <c r="R296" s="8"/>
+      <c r="S296" s="8"/>
+      <c r="T296" s="14"/>
       <c r="U296">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9144,7 +9144,7 @@
     <row r="297" spans="1:21">
       <c r="A297" s="20"/>
       <c r="B297" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9172,7 +9172,7 @@
     <row r="298" spans="1:21">
       <c r="A298" s="20"/>
       <c r="B298" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9200,7 +9200,7 @@
     <row r="299" spans="1:21">
       <c r="A299" s="20"/>
       <c r="B299" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9225,87 +9225,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A300" s="21"/>
-      <c r="B300" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-      <c r="E300" s="6"/>
-      <c r="F300" s="6"/>
-      <c r="G300" s="6"/>
-      <c r="H300" s="6"/>
-      <c r="I300" s="6"/>
-      <c r="J300" s="6"/>
-      <c r="K300" s="6"/>
-      <c r="L300" s="6"/>
-      <c r="M300" s="6"/>
-      <c r="N300" s="6"/>
-      <c r="O300" s="6"/>
-      <c r="P300" s="6"/>
-      <c r="Q300" s="6"/>
-      <c r="R300" s="6"/>
-      <c r="S300" s="6"/>
-      <c r="T300" s="7"/>
+    <row r="300" spans="1:21">
+      <c r="A300" s="20"/>
+      <c r="B300" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C300" s="2"/>
+      <c r="D300" s="2"/>
+      <c r="E300" s="2"/>
+      <c r="F300" s="2"/>
+      <c r="G300" s="2"/>
+      <c r="H300" s="2"/>
+      <c r="I300" s="2"/>
+      <c r="J300" s="2"/>
+      <c r="K300" s="2"/>
+      <c r="L300" s="2"/>
+      <c r="M300" s="2"/>
+      <c r="N300" s="2"/>
+      <c r="O300" s="2"/>
+      <c r="P300" s="2"/>
+      <c r="Q300" s="2"/>
+      <c r="R300" s="2"/>
+      <c r="S300" s="2"/>
+      <c r="T300" s="5"/>
       <c r="U300">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:21">
-      <c r="A301" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B301" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
-      <c r="F301" s="8"/>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-      <c r="K301" s="8"/>
-      <c r="L301" s="8"/>
-      <c r="M301" s="8"/>
-      <c r="N301" s="8"/>
-      <c r="O301" s="8"/>
-      <c r="P301" s="8"/>
-      <c r="Q301" s="8"/>
-      <c r="R301" s="8"/>
-      <c r="S301" s="8"/>
-      <c r="T301" s="14"/>
+    <row r="301" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A301" s="21"/>
+      <c r="B301" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
+      <c r="H301" s="6"/>
+      <c r="I301" s="6"/>
+      <c r="J301" s="6"/>
+      <c r="K301" s="6"/>
+      <c r="L301" s="6"/>
+      <c r="M301" s="6"/>
+      <c r="N301" s="6"/>
+      <c r="O301" s="6"/>
+      <c r="P301" s="6"/>
+      <c r="Q301" s="6"/>
+      <c r="R301" s="6"/>
+      <c r="S301" s="6"/>
+      <c r="T301" s="7"/>
       <c r="U301">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:21">
-      <c r="A302" s="20"/>
-      <c r="B302" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2"/>
-      <c r="E302" s="2"/>
-      <c r="F302" s="2"/>
-      <c r="G302" s="2"/>
-      <c r="H302" s="2"/>
-      <c r="I302" s="2"/>
-      <c r="J302" s="2"/>
-      <c r="K302" s="2"/>
-      <c r="L302" s="2"/>
-      <c r="M302" s="2"/>
-      <c r="N302" s="2"/>
-      <c r="O302" s="2"/>
-      <c r="P302" s="2"/>
-      <c r="Q302" s="2"/>
-      <c r="R302" s="2"/>
-      <c r="S302" s="2"/>
-      <c r="T302" s="5"/>
+      <c r="A302" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B302" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C302" s="8"/>
+      <c r="D302" s="8"/>
+      <c r="E302" s="8"/>
+      <c r="F302" s="8"/>
+      <c r="G302" s="8"/>
+      <c r="H302" s="8"/>
+      <c r="I302" s="8"/>
+      <c r="J302" s="8"/>
+      <c r="K302" s="8"/>
+      <c r="L302" s="8"/>
+      <c r="M302" s="8"/>
+      <c r="N302" s="8"/>
+      <c r="O302" s="8"/>
+      <c r="P302" s="8"/>
+      <c r="Q302" s="8"/>
+      <c r="R302" s="8"/>
+      <c r="S302" s="8"/>
+      <c r="T302" s="14"/>
       <c r="U302">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9314,7 +9314,7 @@
     <row r="303" spans="1:21">
       <c r="A303" s="20"/>
       <c r="B303" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9342,7 +9342,7 @@
     <row r="304" spans="1:21">
       <c r="A304" s="20"/>
       <c r="B304" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9370,7 +9370,7 @@
     <row r="305" spans="1:21">
       <c r="A305" s="20"/>
       <c r="B305" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9395,35 +9395,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A306" s="21"/>
-      <c r="B306" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C306" s="6"/>
-      <c r="D306" s="6"/>
-      <c r="E306" s="6"/>
-      <c r="F306" s="6"/>
-      <c r="G306" s="6"/>
-      <c r="H306" s="6"/>
-      <c r="I306" s="6"/>
-      <c r="J306" s="6"/>
-      <c r="K306" s="6"/>
-      <c r="L306" s="6"/>
-      <c r="M306" s="6"/>
-      <c r="N306" s="6"/>
-      <c r="O306" s="6"/>
-      <c r="P306" s="6"/>
-      <c r="Q306" s="6"/>
-      <c r="R306" s="6"/>
-      <c r="S306" s="6"/>
-      <c r="T306" s="7"/>
+    <row r="306" spans="1:21">
+      <c r="A306" s="20"/>
+      <c r="B306" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C306" s="2"/>
+      <c r="D306" s="2"/>
+      <c r="E306" s="2"/>
+      <c r="F306" s="2"/>
+      <c r="G306" s="2"/>
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+      <c r="J306" s="2"/>
+      <c r="K306" s="2"/>
+      <c r="L306" s="2"/>
+      <c r="M306" s="2"/>
+      <c r="N306" s="2"/>
+      <c r="O306" s="2"/>
+      <c r="P306" s="2"/>
+      <c r="Q306" s="2"/>
+      <c r="R306" s="2"/>
+      <c r="S306" s="2"/>
+      <c r="T306" s="5"/>
       <c r="U306">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:21">
+    <row r="307" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A307" s="21"/>
+      <c r="B307" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C307" s="6"/>
+      <c r="D307" s="6"/>
+      <c r="E307" s="6"/>
+      <c r="F307" s="6"/>
+      <c r="G307" s="6"/>
+      <c r="H307" s="6"/>
+      <c r="I307" s="6"/>
+      <c r="J307" s="6"/>
+      <c r="K307" s="6"/>
+      <c r="L307" s="6"/>
+      <c r="M307" s="6"/>
+      <c r="N307" s="6"/>
+      <c r="O307" s="6"/>
+      <c r="P307" s="6"/>
+      <c r="Q307" s="6"/>
+      <c r="R307" s="6"/>
+      <c r="S307" s="6"/>
+      <c r="T307" s="7"/>
       <c r="U307">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9605,13 +9627,13 @@
     </row>
     <row r="337" spans="21:21">
       <c r="U337">
-        <f t="shared" ref="U337:U400" ca="1" si="7">IF(B337=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="338" spans="21:21">
       <c r="U338">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ref="U338:U401" ca="1" si="7">IF(B338=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -9989,13 +10011,13 @@
     </row>
     <row r="401" spans="21:21">
       <c r="U401">
-        <f t="shared" ref="U401:U464" ca="1" si="8">IF(B401=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="402" spans="21:21">
       <c r="U402">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U402:U465" ca="1" si="8">IF(B402=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10373,13 +10395,13 @@
     </row>
     <row r="465" spans="21:21">
       <c r="U465">
-        <f t="shared" ref="U465:U528" ca="1" si="9">IF(B465=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="466" spans="21:21">
       <c r="U466">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U466:U529" ca="1" si="9">IF(B466=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10757,13 +10779,13 @@
     </row>
     <row r="529" spans="21:21">
       <c r="U529">
-        <f t="shared" ref="U529:U592" ca="1" si="10">IF(B529=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="530" spans="21:21">
       <c r="U530">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U530:U593" ca="1" si="10">IF(B530=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11141,13 +11163,13 @@
     </row>
     <row r="593" spans="21:21">
       <c r="U593">
-        <f t="shared" ref="U593:U656" ca="1" si="11">IF(B593=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="594" spans="21:21">
       <c r="U594">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U594:U657" ca="1" si="11">IF(B594=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11525,13 +11547,13 @@
     </row>
     <row r="657" spans="21:21">
       <c r="U657">
-        <f t="shared" ref="U657:U720" ca="1" si="12">IF(B657=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="658" spans="21:21">
       <c r="U658">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U658:U721" ca="1" si="12">IF(B658=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11909,13 +11931,13 @@
     </row>
     <row r="721" spans="21:21">
       <c r="U721">
-        <f t="shared" ref="U721:U784" ca="1" si="13">IF(B721=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="722" spans="21:21">
       <c r="U722">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U722:U785" ca="1" si="13">IF(B722=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12293,13 +12315,13 @@
     </row>
     <row r="785" spans="21:21">
       <c r="U785">
-        <f t="shared" ref="U785:U848" ca="1" si="14">IF(B785=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="786" spans="21:21">
       <c r="U786">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U786:U849" ca="1" si="14">IF(B786=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12677,13 +12699,13 @@
     </row>
     <row r="849" spans="21:21">
       <c r="U849">
-        <f t="shared" ref="U849:U910" ca="1" si="15">IF(B849=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="850" spans="21:21">
       <c r="U850">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U850:U911" ca="1" si="15">IF(B850=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13047,26 +13069,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="911" spans="21:21">
+      <c r="U911">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A301:A306"/>
-    <mergeCell ref="A243:A263"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A275:A279"/>
+    <mergeCell ref="A265:A274"/>
+    <mergeCell ref="A302:A307"/>
+    <mergeCell ref="A244:A264"/>
     <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A279:A294"/>
-    <mergeCell ref="A295:A300"/>
+    <mergeCell ref="A280:A295"/>
+    <mergeCell ref="A296:A301"/>
     <mergeCell ref="A61:A100"/>
-    <mergeCell ref="A215:A226"/>
-    <mergeCell ref="A191:A214"/>
+    <mergeCell ref="A216:A227"/>
+    <mergeCell ref="A191:A215"/>
     <mergeCell ref="A161:A190"/>
     <mergeCell ref="A144:A160"/>
     <mergeCell ref="A101:A143"/>
     <mergeCell ref="A20:A60"/>
-    <mergeCell ref="A227:A234"/>
-    <mergeCell ref="A235:A242"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A274:A278"/>
-    <mergeCell ref="A264:A273"/>
+    <mergeCell ref="A228:A235"/>
+    <mergeCell ref="A236:A243"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update numbers in numbersMap.xlsx
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="7680"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$279</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -496,33 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,6 +513,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,8 +843,8 @@
   <dimension ref="A1:W911"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B216" sqref="B216"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -861,56 +861,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>2514</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="33"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="30"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -940,7 +940,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -970,7 +970,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75">
-      <c r="A6" s="23"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75">
-      <c r="A7" s="23"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1026,9 +1026,9 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="20"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3">
-        <v>2429</v>
+        <v>1662</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1054,9 +1054,9 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="20"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2">
-        <v>7472</v>
+        <v>1860</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1082,9 +1082,9 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="20"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="2">
-        <v>3862</v>
+        <v>4764</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1110,9 +1110,9 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="20"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="2">
-        <v>9231</v>
+        <v>2429</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1138,9 +1138,9 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="20"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2">
-        <v>8624</v>
+        <v>7472</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1166,9 +1166,9 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="20"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="2">
-        <v>2959</v>
+        <v>3862</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1194,9 +1194,9 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="20"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="2">
-        <v>7271</v>
+        <v>9231</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1222,9 +1222,9 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="20"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2">
-        <v>2632</v>
+        <v>8624</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1250,9 +1250,9 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="20"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="2">
-        <v>4343</v>
+        <v>2959</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1278,9 +1278,9 @@
       </c>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="20"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="2">
-        <v>1662</v>
+        <v>7271</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1306,9 +1306,9 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="20"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="2">
-        <v>1860</v>
+        <v>2632</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1334,9 +1334,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A19" s="24"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9">
-        <v>4764</v>
+        <v>4343</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1362,7 +1362,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="13">
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75">
-      <c r="A21" s="26"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="12">
         <v>3730</v>
       </c>
@@ -1420,7 +1420,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75">
-      <c r="A22" s="26"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="12">
         <v>9007</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75">
-      <c r="A23" s="26"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="12">
         <v>9578</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="26"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="2">
         <v>4411</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="26"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="2">
         <v>9298</v>
       </c>
@@ -1532,7 +1532,7 @@
       </c>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="26"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="2">
         <v>3354</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="26"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="2">
         <v>5201</v>
       </c>
@@ -1588,7 +1588,7 @@
       </c>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="26"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="2">
         <v>2981</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="26"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="2">
         <v>4312</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="26"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="2">
         <v>8428</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="26"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="2">
         <v>2361</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="26"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="2">
         <v>5063</v>
       </c>
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="26"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="2">
         <v>7711</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="26"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="2">
         <v>8833</v>
       </c>
@@ -1784,7 +1784,7 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="26"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="2">
         <v>1262</v>
       </c>
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="26"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="2">
         <v>9020</v>
       </c>
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="37" spans="1:21">
-      <c r="A37" s="26"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="2">
         <v>1934</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="38" spans="1:21">
-      <c r="A38" s="26"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="2">
         <v>7237</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="26"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="2">
         <v>3943</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="26"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="2">
         <v>7619</v>
       </c>
@@ -1952,7 +1952,7 @@
       </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="26"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="2">
         <v>3832</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="26"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="2">
         <v>1346</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="43" spans="1:21">
-      <c r="A43" s="26"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="2">
         <v>9622</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="26"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="2">
         <v>8873</v>
       </c>
@@ -2064,7 +2064,7 @@
       </c>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="26"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="2">
         <v>7799</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46" s="26"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="2">
         <v>9354</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="26"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="2">
         <v>9130</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="48" spans="1:21">
-      <c r="A48" s="26"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="2">
         <v>5895</v>
       </c>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="49" spans="1:21">
-      <c r="A49" s="26"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="2">
         <v>2461</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="50" spans="1:21">
-      <c r="A50" s="26"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="2">
         <v>2790</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
     </row>
     <row r="51" spans="1:21">
-      <c r="A51" s="26"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="2">
         <v>2624</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="52" spans="1:21">
-      <c r="A52" s="26"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="2">
         <v>5871</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="53" spans="1:21">
-      <c r="A53" s="26"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="2">
         <v>9164</v>
       </c>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="54" spans="1:21">
-      <c r="A54" s="26"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="2">
         <v>7457</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
     </row>
     <row r="55" spans="1:21">
-      <c r="A55" s="26"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="2">
         <v>9865</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="56" spans="1:21">
-      <c r="A56" s="26"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="2">
         <v>3591</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="57" spans="1:21">
-      <c r="A57" s="26"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="2">
         <v>3558</v>
       </c>
@@ -2428,7 +2428,7 @@
       </c>
     </row>
     <row r="58" spans="1:21">
-      <c r="A58" s="26"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="2">
         <v>4366</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
     </row>
     <row r="59" spans="1:21">
-      <c r="A59" s="26"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="2">
         <v>5789</v>
       </c>
@@ -2484,7 +2484,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A60" s="27"/>
+      <c r="A60" s="33"/>
       <c r="B60" s="6">
         <v>6522</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15.75">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="13">
@@ -2542,7 +2542,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="15.75">
-      <c r="A62" s="20"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="12">
         <v>2217</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75">
-      <c r="A63" s="20"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12">
         <v>1824</v>
       </c>
@@ -2598,7 +2598,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="15.75">
-      <c r="A64" s="20"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12">
         <v>2564</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="15.75">
-      <c r="A65" s="20"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="12">
         <v>8487</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75">
-      <c r="A66" s="20"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="12">
         <v>8045</v>
       </c>
@@ -2682,7 +2682,7 @@
       </c>
     </row>
     <row r="67" spans="1:21">
-      <c r="A67" s="20"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="2">
         <v>8878</v>
       </c>
@@ -2710,7 +2710,7 @@
       </c>
     </row>
     <row r="68" spans="1:21">
-      <c r="A68" s="20"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="2">
         <v>3072</v>
       </c>
@@ -2738,7 +2738,7 @@
       </c>
     </row>
     <row r="69" spans="1:21">
-      <c r="A69" s="20"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="2">
         <v>5980</v>
       </c>
@@ -2766,7 +2766,7 @@
       </c>
     </row>
     <row r="70" spans="1:21">
-      <c r="A70" s="20"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="2">
         <v>8174</v>
       </c>
@@ -2794,7 +2794,7 @@
       </c>
     </row>
     <row r="71" spans="1:21">
-      <c r="A71" s="20"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="2">
         <v>4257</v>
       </c>
@@ -2822,7 +2822,7 @@
       </c>
     </row>
     <row r="72" spans="1:21">
-      <c r="A72" s="20"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="2">
         <v>2291</v>
       </c>
@@ -2850,7 +2850,7 @@
       </c>
     </row>
     <row r="73" spans="1:21">
-      <c r="A73" s="20"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="2">
         <v>1763</v>
       </c>
@@ -2878,7 +2878,7 @@
       </c>
     </row>
     <row r="74" spans="1:21">
-      <c r="A74" s="20"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="2">
         <v>5662</v>
       </c>
@@ -2906,7 +2906,7 @@
       </c>
     </row>
     <row r="75" spans="1:21">
-      <c r="A75" s="20"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="2">
         <v>1945</v>
       </c>
@@ -2934,7 +2934,7 @@
       </c>
     </row>
     <row r="76" spans="1:21">
-      <c r="A76" s="20"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="2">
         <v>1186</v>
       </c>
@@ -2962,7 +2962,7 @@
       </c>
     </row>
     <row r="77" spans="1:21">
-      <c r="A77" s="20"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="2">
         <v>8715</v>
       </c>
@@ -2990,7 +2990,7 @@
       </c>
     </row>
     <row r="78" spans="1:21">
-      <c r="A78" s="20"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="2">
         <v>8518</v>
       </c>
@@ -3018,7 +3018,7 @@
       </c>
     </row>
     <row r="79" spans="1:21">
-      <c r="A79" s="20"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="2">
         <v>4847</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="80" spans="1:21">
-      <c r="A80" s="20"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="2">
         <v>7991</v>
       </c>
@@ -3074,7 +3074,7 @@
       </c>
     </row>
     <row r="81" spans="1:21">
-      <c r="A81" s="20"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="2">
         <v>6291</v>
       </c>
@@ -3102,7 +3102,7 @@
       </c>
     </row>
     <row r="82" spans="1:21">
-      <c r="A82" s="20"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="2">
         <v>3770</v>
       </c>
@@ -3130,7 +3130,7 @@
       </c>
     </row>
     <row r="83" spans="1:21">
-      <c r="A83" s="20"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="2">
         <v>7178</v>
       </c>
@@ -3158,7 +3158,7 @@
       </c>
     </row>
     <row r="84" spans="1:21">
-      <c r="A84" s="20"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="2">
         <v>3883</v>
       </c>
@@ -3186,9 +3186,9 @@
       </c>
     </row>
     <row r="85" spans="1:21">
-      <c r="A85" s="20"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="2">
-        <v>4527</v>
+        <v>1999</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -3214,9 +3214,9 @@
       </c>
     </row>
     <row r="86" spans="1:21">
-      <c r="A86" s="20"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="2">
-        <v>6556</v>
+        <v>4042</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -3242,9 +3242,9 @@
       </c>
     </row>
     <row r="87" spans="1:21">
-      <c r="A87" s="20"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="2">
-        <v>5635</v>
+        <v>6351</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3270,9 +3270,9 @@
       </c>
     </row>
     <row r="88" spans="1:21">
-      <c r="A88" s="20"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="2">
-        <v>3878</v>
+        <v>5382</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -3298,9 +3298,9 @@
       </c>
     </row>
     <row r="89" spans="1:21">
-      <c r="A89" s="20"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="2">
-        <v>1217</v>
+        <v>7088</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3326,9 +3326,9 @@
       </c>
     </row>
     <row r="90" spans="1:21">
-      <c r="A90" s="20"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="2">
-        <v>1438</v>
+        <v>7250</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -3354,9 +3354,9 @@
       </c>
     </row>
     <row r="91" spans="1:21">
-      <c r="A91" s="20"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="2">
-        <v>2153</v>
+        <v>6740</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -3382,9 +3382,9 @@
       </c>
     </row>
     <row r="92" spans="1:21">
-      <c r="A92" s="20"/>
+      <c r="A92" s="26"/>
       <c r="B92" s="2">
-        <v>7937</v>
+        <v>9038</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -3410,9 +3410,9 @@
       </c>
     </row>
     <row r="93" spans="1:21">
-      <c r="A93" s="20"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="2">
-        <v>1999</v>
+        <v>4527</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -3438,9 +3438,9 @@
       </c>
     </row>
     <row r="94" spans="1:21">
-      <c r="A94" s="20"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="2">
-        <v>4042</v>
+        <v>6556</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -3466,9 +3466,9 @@
       </c>
     </row>
     <row r="95" spans="1:21">
-      <c r="A95" s="20"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="2">
-        <v>6351</v>
+        <v>5635</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -3494,9 +3494,9 @@
       </c>
     </row>
     <row r="96" spans="1:21">
-      <c r="A96" s="20"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="2">
-        <v>5382</v>
+        <v>3878</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -3522,9 +3522,9 @@
       </c>
     </row>
     <row r="97" spans="1:21">
-      <c r="A97" s="20"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="2">
-        <v>7088</v>
+        <v>1217</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -3550,9 +3550,9 @@
       </c>
     </row>
     <row r="98" spans="1:21">
-      <c r="A98" s="20"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="2">
-        <v>7250</v>
+        <v>1438</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -3578,9 +3578,9 @@
       </c>
     </row>
     <row r="99" spans="1:21">
-      <c r="A99" s="20"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="2">
-        <v>6740</v>
+        <v>2153</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3606,9 +3606,9 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A100" s="21"/>
+      <c r="A100" s="27"/>
       <c r="B100" s="6">
-        <v>9038</v>
+        <v>7937</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
@@ -3634,7 +3634,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" ht="15.75">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B101" s="13">
@@ -3664,7 +3664,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="15.75">
-      <c r="A102" s="20"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="12">
         <v>1881</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
     </row>
     <row r="103" spans="1:21">
-      <c r="A103" s="20"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="2">
         <v>8495</v>
       </c>
@@ -3720,7 +3720,7 @@
       </c>
     </row>
     <row r="104" spans="1:21">
-      <c r="A104" s="20"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="2">
         <v>1315</v>
       </c>
@@ -3748,7 +3748,7 @@
       </c>
     </row>
     <row r="105" spans="1:21">
-      <c r="A105" s="20"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="2">
         <v>6066</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="106" spans="1:21">
-      <c r="A106" s="20"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="2">
         <v>2565</v>
       </c>
@@ -3804,7 +3804,7 @@
       </c>
     </row>
     <row r="107" spans="1:21">
-      <c r="A107" s="20"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="2">
         <v>2594</v>
       </c>
@@ -3832,9 +3832,9 @@
       </c>
     </row>
     <row r="108" spans="1:21">
-      <c r="A108" s="20"/>
+      <c r="A108" s="26"/>
       <c r="B108" s="2">
-        <v>3762</v>
+        <v>2321</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -3860,9 +3860,9 @@
       </c>
     </row>
     <row r="109" spans="1:21">
-      <c r="A109" s="20"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="2">
-        <v>3550</v>
+        <v>5053</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -3888,9 +3888,9 @@
       </c>
     </row>
     <row r="110" spans="1:21">
-      <c r="A110" s="20"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="2">
-        <v>2475</v>
+        <v>3762</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -3916,9 +3916,9 @@
       </c>
     </row>
     <row r="111" spans="1:21">
-      <c r="A111" s="20"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="2">
-        <v>9180</v>
+        <v>3550</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -3944,9 +3944,9 @@
       </c>
     </row>
     <row r="112" spans="1:21">
-      <c r="A112" s="20"/>
+      <c r="A112" s="26"/>
       <c r="B112" s="2">
-        <v>1544</v>
+        <v>2475</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -3972,9 +3972,9 @@
       </c>
     </row>
     <row r="113" spans="1:21">
-      <c r="A113" s="20"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="2">
-        <v>9562</v>
+        <v>9180</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -4000,9 +4000,9 @@
       </c>
     </row>
     <row r="114" spans="1:21">
-      <c r="A114" s="20"/>
+      <c r="A114" s="26"/>
       <c r="B114" s="2">
-        <v>3669</v>
+        <v>1544</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -4028,9 +4028,9 @@
       </c>
     </row>
     <row r="115" spans="1:21">
-      <c r="A115" s="20"/>
+      <c r="A115" s="26"/>
       <c r="B115" s="2">
-        <v>5951</v>
+        <v>9562</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -4056,9 +4056,9 @@
       </c>
     </row>
     <row r="116" spans="1:21">
-      <c r="A116" s="20"/>
+      <c r="A116" s="26"/>
       <c r="B116" s="2">
-        <v>2802</v>
+        <v>3669</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -4084,9 +4084,9 @@
       </c>
     </row>
     <row r="117" spans="1:21">
-      <c r="A117" s="20"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="2">
-        <v>6580</v>
+        <v>5951</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -4112,9 +4112,9 @@
       </c>
     </row>
     <row r="118" spans="1:21">
-      <c r="A118" s="20"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="2">
-        <v>2324</v>
+        <v>2802</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -4140,9 +4140,9 @@
       </c>
     </row>
     <row r="119" spans="1:21">
-      <c r="A119" s="20"/>
+      <c r="A119" s="26"/>
       <c r="B119" s="2">
-        <v>8731</v>
+        <v>2324</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -4168,9 +4168,9 @@
       </c>
     </row>
     <row r="120" spans="1:21">
-      <c r="A120" s="20"/>
+      <c r="A120" s="26"/>
       <c r="B120" s="2">
-        <v>4082</v>
+        <v>8731</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -4196,9 +4196,9 @@
       </c>
     </row>
     <row r="121" spans="1:21">
-      <c r="A121" s="20"/>
+      <c r="A121" s="26"/>
       <c r="B121" s="2">
-        <v>7585</v>
+        <v>4082</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -4224,9 +4224,9 @@
       </c>
     </row>
     <row r="122" spans="1:21">
-      <c r="A122" s="20"/>
+      <c r="A122" s="26"/>
       <c r="B122" s="2">
-        <v>2321</v>
+        <v>6280</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -4252,9 +4252,9 @@
       </c>
     </row>
     <row r="123" spans="1:21">
-      <c r="A123" s="20"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="2">
-        <v>5053</v>
+        <v>7585</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -4280,9 +4280,9 @@
       </c>
     </row>
     <row r="124" spans="1:21">
-      <c r="A124" s="20"/>
+      <c r="A124" s="26"/>
       <c r="B124" s="2">
-        <v>3983</v>
+        <v>1483</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -4308,9 +4308,9 @@
       </c>
     </row>
     <row r="125" spans="1:21">
-      <c r="A125" s="20"/>
+      <c r="A125" s="26"/>
       <c r="B125" s="2">
-        <v>8770</v>
+        <v>3983</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -4336,9 +4336,9 @@
       </c>
     </row>
     <row r="126" spans="1:21">
-      <c r="A126" s="20"/>
+      <c r="A126" s="26"/>
       <c r="B126" s="2">
-        <v>4236</v>
+        <v>8770</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -4364,9 +4364,9 @@
       </c>
     </row>
     <row r="127" spans="1:21">
-      <c r="A127" s="20"/>
+      <c r="A127" s="26"/>
       <c r="B127" s="2">
-        <v>5969</v>
+        <v>4236</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -4392,7 +4392,7 @@
       </c>
     </row>
     <row r="128" spans="1:21">
-      <c r="A128" s="20"/>
+      <c r="A128" s="26"/>
       <c r="B128" s="2">
         <v>8696</v>
       </c>
@@ -4420,9 +4420,9 @@
       </c>
     </row>
     <row r="129" spans="1:21">
-      <c r="A129" s="20"/>
+      <c r="A129" s="26"/>
       <c r="B129" s="2">
-        <v>1483</v>
+        <v>5969</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -4448,7 +4448,7 @@
       </c>
     </row>
     <row r="130" spans="1:21">
-      <c r="A130" s="20"/>
+      <c r="A130" s="26"/>
       <c r="B130" s="2">
         <v>8418</v>
       </c>
@@ -4476,9 +4476,9 @@
       </c>
     </row>
     <row r="131" spans="1:21">
-      <c r="A131" s="20"/>
+      <c r="A131" s="26"/>
       <c r="B131" s="2">
-        <v>8395</v>
+        <v>5170</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -4504,9 +4504,9 @@
       </c>
     </row>
     <row r="132" spans="1:21">
-      <c r="A132" s="20"/>
+      <c r="A132" s="26"/>
       <c r="B132" s="2">
-        <v>5170</v>
+        <v>8395</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -4532,7 +4532,7 @@
       </c>
     </row>
     <row r="133" spans="1:21">
-      <c r="A133" s="20"/>
+      <c r="A133" s="26"/>
       <c r="B133" s="2">
         <v>5568</v>
       </c>
@@ -4560,7 +4560,7 @@
       </c>
     </row>
     <row r="134" spans="1:21">
-      <c r="A134" s="20"/>
+      <c r="A134" s="26"/>
       <c r="B134" s="2">
         <v>2592</v>
       </c>
@@ -4588,7 +4588,7 @@
       </c>
     </row>
     <row r="135" spans="1:21">
-      <c r="A135" s="20"/>
+      <c r="A135" s="26"/>
       <c r="B135" s="2">
         <v>4075</v>
       </c>
@@ -4616,7 +4616,7 @@
       </c>
     </row>
     <row r="136" spans="1:21">
-      <c r="A136" s="20"/>
+      <c r="A136" s="26"/>
       <c r="B136" s="2">
         <v>7517</v>
       </c>
@@ -4644,7 +4644,7 @@
       </c>
     </row>
     <row r="137" spans="1:21">
-      <c r="A137" s="20"/>
+      <c r="A137" s="26"/>
       <c r="B137" s="2">
         <v>5448</v>
       </c>
@@ -4672,9 +4672,9 @@
       </c>
     </row>
     <row r="138" spans="1:21">
-      <c r="A138" s="20"/>
+      <c r="A138" s="26"/>
       <c r="B138" s="2">
-        <v>6572</v>
+        <v>6582</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -4700,7 +4700,7 @@
       </c>
     </row>
     <row r="139" spans="1:21">
-      <c r="A139" s="20"/>
+      <c r="A139" s="26"/>
       <c r="B139" s="2">
         <v>5238</v>
       </c>
@@ -4728,7 +4728,7 @@
       </c>
     </row>
     <row r="140" spans="1:21">
-      <c r="A140" s="20"/>
+      <c r="A140" s="26"/>
       <c r="B140" s="2">
         <v>2084</v>
       </c>
@@ -4756,7 +4756,7 @@
       </c>
     </row>
     <row r="141" spans="1:21">
-      <c r="A141" s="20"/>
+      <c r="A141" s="26"/>
       <c r="B141" s="2">
         <v>5411</v>
       </c>
@@ -4784,7 +4784,7 @@
       </c>
     </row>
     <row r="142" spans="1:21">
-      <c r="A142" s="20"/>
+      <c r="A142" s="26"/>
       <c r="B142" s="2">
         <v>5171</v>
       </c>
@@ -4812,7 +4812,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A143" s="21"/>
+      <c r="A143" s="27"/>
       <c r="B143" s="6">
         <v>1862</v>
       </c>
@@ -4840,7 +4840,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" ht="15.75">
-      <c r="A144" s="19" t="s">
+      <c r="A144" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B144" s="13">
@@ -4870,7 +4870,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" ht="15.75">
-      <c r="A145" s="20"/>
+      <c r="A145" s="26"/>
       <c r="B145" s="12">
         <v>9001</v>
       </c>
@@ -4898,7 +4898,7 @@
       </c>
     </row>
     <row r="146" spans="1:21">
-      <c r="A146" s="20"/>
+      <c r="A146" s="26"/>
       <c r="B146" s="2">
         <v>9631</v>
       </c>
@@ -4926,7 +4926,7 @@
       </c>
     </row>
     <row r="147" spans="1:21">
-      <c r="A147" s="20"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="2">
         <v>9812</v>
       </c>
@@ -4954,7 +4954,7 @@
       </c>
     </row>
     <row r="148" spans="1:21">
-      <c r="A148" s="20"/>
+      <c r="A148" s="26"/>
       <c r="B148" s="2">
         <v>4845</v>
       </c>
@@ -4982,7 +4982,7 @@
       </c>
     </row>
     <row r="149" spans="1:21">
-      <c r="A149" s="20"/>
+      <c r="A149" s="26"/>
       <c r="B149" s="2">
         <v>5728</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
     </row>
     <row r="150" spans="1:21">
-      <c r="A150" s="20"/>
+      <c r="A150" s="26"/>
       <c r="B150" s="2">
         <v>1618</v>
       </c>
@@ -5038,7 +5038,7 @@
       </c>
     </row>
     <row r="151" spans="1:21">
-      <c r="A151" s="20"/>
+      <c r="A151" s="26"/>
       <c r="B151" s="2">
         <v>9279</v>
       </c>
@@ -5066,7 +5066,7 @@
       </c>
     </row>
     <row r="152" spans="1:21">
-      <c r="A152" s="20"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="2">
         <v>6599</v>
       </c>
@@ -5094,7 +5094,7 @@
       </c>
     </row>
     <row r="153" spans="1:21">
-      <c r="A153" s="20"/>
+      <c r="A153" s="26"/>
       <c r="B153" s="2">
         <v>7222</v>
       </c>
@@ -5122,7 +5122,7 @@
       </c>
     </row>
     <row r="154" spans="1:21">
-      <c r="A154" s="20"/>
+      <c r="A154" s="26"/>
       <c r="B154" s="2">
         <v>3657</v>
       </c>
@@ -5150,7 +5150,7 @@
       </c>
     </row>
     <row r="155" spans="1:21">
-      <c r="A155" s="20"/>
+      <c r="A155" s="26"/>
       <c r="B155" s="2">
         <v>7491</v>
       </c>
@@ -5178,7 +5178,7 @@
       </c>
     </row>
     <row r="156" spans="1:21">
-      <c r="A156" s="20"/>
+      <c r="A156" s="26"/>
       <c r="B156" s="2">
         <v>5923</v>
       </c>
@@ -5206,7 +5206,7 @@
       </c>
     </row>
     <row r="157" spans="1:21">
-      <c r="A157" s="20"/>
+      <c r="A157" s="26"/>
       <c r="B157" s="2">
         <v>4265</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
     </row>
     <row r="158" spans="1:21">
-      <c r="A158" s="20"/>
+      <c r="A158" s="26"/>
       <c r="B158" s="2">
         <v>2166</v>
       </c>
@@ -5262,7 +5262,7 @@
       </c>
     </row>
     <row r="159" spans="1:21">
-      <c r="A159" s="20"/>
+      <c r="A159" s="26"/>
       <c r="B159" s="2">
         <v>9116</v>
       </c>
@@ -5290,7 +5290,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A160" s="21"/>
+      <c r="A160" s="27"/>
       <c r="B160" s="6">
         <v>9925</v>
       </c>
@@ -5318,7 +5318,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" ht="15.75">
-      <c r="A161" s="19" t="s">
+      <c r="A161" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B161" s="13">
@@ -5348,7 +5348,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" ht="15.75">
-      <c r="A162" s="20"/>
+      <c r="A162" s="26"/>
       <c r="B162" s="12">
         <v>9931</v>
       </c>
@@ -5376,7 +5376,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" ht="15.75">
-      <c r="A163" s="20"/>
+      <c r="A163" s="26"/>
       <c r="B163" s="12">
         <v>9696</v>
       </c>
@@ -5404,7 +5404,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" ht="15.75">
-      <c r="A164" s="20"/>
+      <c r="A164" s="26"/>
       <c r="B164" s="12">
         <v>1947</v>
       </c>
@@ -5432,7 +5432,7 @@
       </c>
     </row>
     <row r="165" spans="1:21">
-      <c r="A165" s="20"/>
+      <c r="A165" s="26"/>
       <c r="B165" s="2">
         <v>4425</v>
       </c>
@@ -5460,7 +5460,7 @@
       </c>
     </row>
     <row r="166" spans="1:21">
-      <c r="A166" s="20"/>
+      <c r="A166" s="26"/>
       <c r="B166" s="2">
         <v>5683</v>
       </c>
@@ -5488,7 +5488,7 @@
       </c>
     </row>
     <row r="167" spans="1:21">
-      <c r="A167" s="20"/>
+      <c r="A167" s="26"/>
       <c r="B167" s="2">
         <v>1223</v>
       </c>
@@ -5516,7 +5516,7 @@
       </c>
     </row>
     <row r="168" spans="1:21">
-      <c r="A168" s="20"/>
+      <c r="A168" s="26"/>
       <c r="B168" s="2">
         <v>3946</v>
       </c>
@@ -5544,7 +5544,7 @@
       </c>
     </row>
     <row r="169" spans="1:21">
-      <c r="A169" s="20"/>
+      <c r="A169" s="26"/>
       <c r="B169" s="2">
         <v>3940</v>
       </c>
@@ -5572,7 +5572,7 @@
       </c>
     </row>
     <row r="170" spans="1:21">
-      <c r="A170" s="20"/>
+      <c r="A170" s="26"/>
       <c r="B170" s="2">
         <v>8311</v>
       </c>
@@ -5600,7 +5600,7 @@
       </c>
     </row>
     <row r="171" spans="1:21">
-      <c r="A171" s="20"/>
+      <c r="A171" s="26"/>
       <c r="B171" s="2">
         <v>3134</v>
       </c>
@@ -5628,7 +5628,7 @@
       </c>
     </row>
     <row r="172" spans="1:21">
-      <c r="A172" s="20"/>
+      <c r="A172" s="26"/>
       <c r="B172" s="2">
         <v>9774</v>
       </c>
@@ -5656,7 +5656,7 @@
       </c>
     </row>
     <row r="173" spans="1:21">
-      <c r="A173" s="20"/>
+      <c r="A173" s="26"/>
       <c r="B173" s="2">
         <v>9711</v>
       </c>
@@ -5684,7 +5684,7 @@
       </c>
     </row>
     <row r="174" spans="1:21">
-      <c r="A174" s="20"/>
+      <c r="A174" s="26"/>
       <c r="B174" s="2">
         <v>3333</v>
       </c>
@@ -5712,7 +5712,7 @@
       </c>
     </row>
     <row r="175" spans="1:21">
-      <c r="A175" s="20"/>
+      <c r="A175" s="26"/>
       <c r="B175" s="2">
         <v>8820</v>
       </c>
@@ -5740,7 +5740,7 @@
       </c>
     </row>
     <row r="176" spans="1:21">
-      <c r="A176" s="20"/>
+      <c r="A176" s="26"/>
       <c r="B176" s="2">
         <v>7290</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
     </row>
     <row r="177" spans="1:21">
-      <c r="A177" s="20"/>
+      <c r="A177" s="26"/>
       <c r="B177" s="2">
         <v>5694</v>
       </c>
@@ -5796,7 +5796,7 @@
       </c>
     </row>
     <row r="178" spans="1:21">
-      <c r="A178" s="20"/>
+      <c r="A178" s="26"/>
       <c r="B178" s="2">
         <v>6806</v>
       </c>
@@ -5824,7 +5824,7 @@
       </c>
     </row>
     <row r="179" spans="1:21">
-      <c r="A179" s="20"/>
+      <c r="A179" s="26"/>
       <c r="B179" s="2">
         <v>7369</v>
       </c>
@@ -5852,7 +5852,7 @@
       </c>
     </row>
     <row r="180" spans="1:21">
-      <c r="A180" s="20"/>
+      <c r="A180" s="26"/>
       <c r="B180" s="2">
         <v>5894</v>
       </c>
@@ -5880,7 +5880,7 @@
       </c>
     </row>
     <row r="181" spans="1:21">
-      <c r="A181" s="20"/>
+      <c r="A181" s="26"/>
       <c r="B181" s="2">
         <v>4515</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
     </row>
     <row r="182" spans="1:21">
-      <c r="A182" s="20"/>
+      <c r="A182" s="26"/>
       <c r="B182" s="2">
         <v>7035</v>
       </c>
@@ -5936,7 +5936,7 @@
       </c>
     </row>
     <row r="183" spans="1:21">
-      <c r="A183" s="20"/>
+      <c r="A183" s="26"/>
       <c r="B183" s="2">
         <v>9271</v>
       </c>
@@ -5964,7 +5964,7 @@
       </c>
     </row>
     <row r="184" spans="1:21">
-      <c r="A184" s="20"/>
+      <c r="A184" s="26"/>
       <c r="B184" s="2">
         <v>8769</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="185" spans="1:21">
-      <c r="A185" s="20"/>
+      <c r="A185" s="26"/>
       <c r="B185" s="2">
         <v>4497</v>
       </c>
@@ -6020,7 +6020,7 @@
       </c>
     </row>
     <row r="186" spans="1:21">
-      <c r="A186" s="20"/>
+      <c r="A186" s="26"/>
       <c r="B186" s="2">
         <v>3218</v>
       </c>
@@ -6048,7 +6048,7 @@
       </c>
     </row>
     <row r="187" spans="1:21">
-      <c r="A187" s="20"/>
+      <c r="A187" s="26"/>
       <c r="B187" s="2">
         <v>4283</v>
       </c>
@@ -6076,7 +6076,7 @@
       </c>
     </row>
     <row r="188" spans="1:21">
-      <c r="A188" s="20"/>
+      <c r="A188" s="26"/>
       <c r="B188" s="2">
         <v>7703</v>
       </c>
@@ -6104,7 +6104,7 @@
       </c>
     </row>
     <row r="189" spans="1:21">
-      <c r="A189" s="20"/>
+      <c r="A189" s="26"/>
       <c r="B189" s="2">
         <v>5541</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A190" s="21"/>
+      <c r="A190" s="27"/>
       <c r="B190" s="6">
         <v>9182</v>
       </c>
@@ -6160,7 +6160,7 @@
       </c>
     </row>
     <row r="191" spans="1:21">
-      <c r="A191" s="19" t="s">
+      <c r="A191" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B191" s="8">
@@ -6190,7 +6190,7 @@
       </c>
     </row>
     <row r="192" spans="1:21">
-      <c r="A192" s="20"/>
+      <c r="A192" s="26"/>
       <c r="B192" s="2">
         <v>4642</v>
       </c>
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="193" spans="1:21">
-      <c r="A193" s="20"/>
+      <c r="A193" s="26"/>
       <c r="B193" s="2">
         <v>4488</v>
       </c>
@@ -6246,7 +6246,7 @@
       </c>
     </row>
     <row r="194" spans="1:21">
-      <c r="A194" s="20"/>
+      <c r="A194" s="26"/>
       <c r="B194" s="2">
         <v>9765</v>
       </c>
@@ -6274,7 +6274,7 @@
       </c>
     </row>
     <row r="195" spans="1:21">
-      <c r="A195" s="20"/>
+      <c r="A195" s="26"/>
       <c r="B195" s="2">
         <v>4954</v>
       </c>
@@ -6302,7 +6302,7 @@
       </c>
     </row>
     <row r="196" spans="1:21">
-      <c r="A196" s="20"/>
+      <c r="A196" s="26"/>
       <c r="B196" s="2">
         <v>5537</v>
       </c>
@@ -6330,7 +6330,7 @@
       </c>
     </row>
     <row r="197" spans="1:21">
-      <c r="A197" s="20"/>
+      <c r="A197" s="26"/>
       <c r="B197" s="2">
         <v>6431</v>
       </c>
@@ -6358,7 +6358,7 @@
       </c>
     </row>
     <row r="198" spans="1:21">
-      <c r="A198" s="20"/>
+      <c r="A198" s="26"/>
       <c r="B198" s="2">
         <v>7193</v>
       </c>
@@ -6386,7 +6386,7 @@
       </c>
     </row>
     <row r="199" spans="1:21">
-      <c r="A199" s="20"/>
+      <c r="A199" s="26"/>
       <c r="B199" s="2">
         <v>5621</v>
       </c>
@@ -6414,7 +6414,7 @@
       </c>
     </row>
     <row r="200" spans="1:21">
-      <c r="A200" s="20"/>
+      <c r="A200" s="26"/>
       <c r="B200" s="2">
         <v>5847</v>
       </c>
@@ -6442,7 +6442,7 @@
       </c>
     </row>
     <row r="201" spans="1:21">
-      <c r="A201" s="20"/>
+      <c r="A201" s="26"/>
       <c r="B201" s="2">
         <v>4769</v>
       </c>
@@ -6470,7 +6470,7 @@
       </c>
     </row>
     <row r="202" spans="1:21">
-      <c r="A202" s="20"/>
+      <c r="A202" s="26"/>
       <c r="B202" s="2">
         <v>9930</v>
       </c>
@@ -6498,7 +6498,7 @@
       </c>
     </row>
     <row r="203" spans="1:21">
-      <c r="A203" s="20"/>
+      <c r="A203" s="26"/>
       <c r="B203" s="2">
         <v>3226</v>
       </c>
@@ -6526,7 +6526,7 @@
       </c>
     </row>
     <row r="204" spans="1:21">
-      <c r="A204" s="20"/>
+      <c r="A204" s="26"/>
       <c r="B204" s="2">
         <v>6861</v>
       </c>
@@ -6554,7 +6554,7 @@
       </c>
     </row>
     <row r="205" spans="1:21">
-      <c r="A205" s="20"/>
+      <c r="A205" s="26"/>
       <c r="B205" s="2">
         <v>5032</v>
       </c>
@@ -6582,7 +6582,7 @@
       </c>
     </row>
     <row r="206" spans="1:21">
-      <c r="A206" s="20"/>
+      <c r="A206" s="26"/>
       <c r="B206" s="2">
         <v>2033</v>
       </c>
@@ -6610,7 +6610,7 @@
       </c>
     </row>
     <row r="207" spans="1:21">
-      <c r="A207" s="20"/>
+      <c r="A207" s="26"/>
       <c r="B207" s="2">
         <v>5108</v>
       </c>
@@ -6638,7 +6638,7 @@
       </c>
     </row>
     <row r="208" spans="1:21">
-      <c r="A208" s="20"/>
+      <c r="A208" s="26"/>
       <c r="B208" s="2">
         <v>3567</v>
       </c>
@@ -6666,7 +6666,7 @@
       </c>
     </row>
     <row r="209" spans="1:21">
-      <c r="A209" s="20"/>
+      <c r="A209" s="26"/>
       <c r="B209" s="2">
         <v>2205</v>
       </c>
@@ -6694,7 +6694,7 @@
       </c>
     </row>
     <row r="210" spans="1:21">
-      <c r="A210" s="20"/>
+      <c r="A210" s="26"/>
       <c r="B210" s="2">
         <v>4372</v>
       </c>
@@ -6722,7 +6722,7 @@
       </c>
     </row>
     <row r="211" spans="1:21">
-      <c r="A211" s="20"/>
+      <c r="A211" s="26"/>
       <c r="B211" s="2">
         <v>4463</v>
       </c>
@@ -6750,7 +6750,7 @@
       </c>
     </row>
     <row r="212" spans="1:21">
-      <c r="A212" s="20"/>
+      <c r="A212" s="26"/>
       <c r="B212" s="2">
         <v>1668</v>
       </c>
@@ -6778,7 +6778,7 @@
       </c>
     </row>
     <row r="213" spans="1:21">
-      <c r="A213" s="24"/>
+      <c r="A213" s="28"/>
       <c r="B213" s="9">
         <v>2137</v>
       </c>
@@ -6806,7 +6806,7 @@
       </c>
     </row>
     <row r="214" spans="1:21">
-      <c r="A214" s="24"/>
+      <c r="A214" s="28"/>
       <c r="B214" s="9">
         <v>9417</v>
       </c>
@@ -6834,7 +6834,7 @@
       </c>
     </row>
     <row r="215" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A215" s="21"/>
+      <c r="A215" s="27"/>
       <c r="B215" s="6">
         <v>3148</v>
       </c>
@@ -6862,7 +6862,7 @@
       </c>
     </row>
     <row r="216" spans="1:21">
-      <c r="A216" s="19" t="s">
+      <c r="A216" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B216" s="8">
@@ -6892,7 +6892,7 @@
       </c>
     </row>
     <row r="217" spans="1:21">
-      <c r="A217" s="20"/>
+      <c r="A217" s="26"/>
       <c r="B217" s="2">
         <v>3951</v>
       </c>
@@ -6920,7 +6920,7 @@
       </c>
     </row>
     <row r="218" spans="1:21">
-      <c r="A218" s="20"/>
+      <c r="A218" s="26"/>
       <c r="B218" s="2">
         <v>6409</v>
       </c>
@@ -6948,7 +6948,7 @@
       </c>
     </row>
     <row r="219" spans="1:21">
-      <c r="A219" s="20"/>
+      <c r="A219" s="26"/>
       <c r="B219" s="2">
         <v>3290</v>
       </c>
@@ -6976,7 +6976,7 @@
       </c>
     </row>
     <row r="220" spans="1:21">
-      <c r="A220" s="20"/>
+      <c r="A220" s="26"/>
       <c r="B220" s="2">
         <v>4342</v>
       </c>
@@ -7004,7 +7004,7 @@
       </c>
     </row>
     <row r="221" spans="1:21">
-      <c r="A221" s="20"/>
+      <c r="A221" s="26"/>
       <c r="B221" s="2">
         <v>2386</v>
       </c>
@@ -7032,7 +7032,7 @@
       </c>
     </row>
     <row r="222" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A222" s="20"/>
+      <c r="A222" s="26"/>
       <c r="B222" s="6">
         <v>9159</v>
       </c>
@@ -7056,7 +7056,7 @@
       <c r="T222" s="5"/>
     </row>
     <row r="223" spans="1:21">
-      <c r="A223" s="20"/>
+      <c r="A223" s="26"/>
       <c r="B223" s="2">
         <v>5309</v>
       </c>
@@ -7084,7 +7084,7 @@
       </c>
     </row>
     <row r="224" spans="1:21">
-      <c r="A224" s="20"/>
+      <c r="A224" s="26"/>
       <c r="B224" s="2">
         <v>5345</v>
       </c>
@@ -7112,7 +7112,7 @@
       </c>
     </row>
     <row r="225" spans="1:21">
-      <c r="A225" s="20"/>
+      <c r="A225" s="26"/>
       <c r="B225" s="2">
         <v>6812</v>
       </c>
@@ -7140,7 +7140,7 @@
       </c>
     </row>
     <row r="226" spans="1:21">
-      <c r="A226" s="20"/>
+      <c r="A226" s="26"/>
       <c r="B226" s="2">
         <v>7343</v>
       </c>
@@ -7168,7 +7168,7 @@
       </c>
     </row>
     <row r="227" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A227" s="21"/>
+      <c r="A227" s="27"/>
       <c r="B227" s="6">
         <v>7060</v>
       </c>
@@ -7196,7 +7196,7 @@
       </c>
     </row>
     <row r="228" spans="1:21" ht="15.75">
-      <c r="A228" s="19" t="s">
+      <c r="A228" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B228" s="13">
@@ -7226,7 +7226,7 @@
       </c>
     </row>
     <row r="229" spans="1:21" ht="15.75">
-      <c r="A229" s="20"/>
+      <c r="A229" s="26"/>
       <c r="B229" s="12">
         <v>1516</v>
       </c>
@@ -7254,7 +7254,7 @@
       </c>
     </row>
     <row r="230" spans="1:21" ht="15.75">
-      <c r="A230" s="20"/>
+      <c r="A230" s="26"/>
       <c r="B230" s="12">
         <v>9062</v>
       </c>
@@ -7282,7 +7282,7 @@
       </c>
     </row>
     <row r="231" spans="1:21">
-      <c r="A231" s="20"/>
+      <c r="A231" s="26"/>
       <c r="B231" s="2">
         <v>8861</v>
       </c>
@@ -7310,7 +7310,7 @@
       </c>
     </row>
     <row r="232" spans="1:21">
-      <c r="A232" s="20"/>
+      <c r="A232" s="26"/>
       <c r="B232" s="2">
         <v>5164</v>
       </c>
@@ -7338,7 +7338,7 @@
       </c>
     </row>
     <row r="233" spans="1:21">
-      <c r="A233" s="20"/>
+      <c r="A233" s="26"/>
       <c r="B233" s="2">
         <v>2030</v>
       </c>
@@ -7366,7 +7366,7 @@
       </c>
     </row>
     <row r="234" spans="1:21">
-      <c r="A234" s="20"/>
+      <c r="A234" s="26"/>
       <c r="B234" s="2">
         <v>7649</v>
       </c>
@@ -7394,7 +7394,7 @@
       </c>
     </row>
     <row r="235" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A235" s="21"/>
+      <c r="A235" s="27"/>
       <c r="B235" s="6">
         <v>2354</v>
       </c>
@@ -7422,7 +7422,7 @@
       </c>
     </row>
     <row r="236" spans="1:21">
-      <c r="A236" s="19" t="s">
+      <c r="A236" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B236" s="8">
@@ -7452,7 +7452,7 @@
       </c>
     </row>
     <row r="237" spans="1:21">
-      <c r="A237" s="20"/>
+      <c r="A237" s="26"/>
       <c r="B237" s="2">
         <v>1212</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
     </row>
     <row r="238" spans="1:21">
-      <c r="A238" s="20"/>
+      <c r="A238" s="26"/>
       <c r="B238" s="2">
         <v>9472</v>
       </c>
@@ -7508,7 +7508,7 @@
       </c>
     </row>
     <row r="239" spans="1:21">
-      <c r="A239" s="20"/>
+      <c r="A239" s="26"/>
       <c r="B239" s="2">
         <v>5081</v>
       </c>
@@ -7536,7 +7536,7 @@
       </c>
     </row>
     <row r="240" spans="1:21">
-      <c r="A240" s="20"/>
+      <c r="A240" s="26"/>
       <c r="B240" s="2">
         <v>6454</v>
       </c>
@@ -7564,7 +7564,7 @@
       </c>
     </row>
     <row r="241" spans="1:21">
-      <c r="A241" s="20"/>
+      <c r="A241" s="26"/>
       <c r="B241" s="2">
         <v>6882</v>
       </c>
@@ -7592,7 +7592,7 @@
       </c>
     </row>
     <row r="242" spans="1:21">
-      <c r="A242" s="20"/>
+      <c r="A242" s="26"/>
       <c r="B242" s="2">
         <v>3784</v>
       </c>
@@ -7620,7 +7620,7 @@
       </c>
     </row>
     <row r="243" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A243" s="21"/>
+      <c r="A243" s="27"/>
       <c r="B243" s="6">
         <v>6732</v>
       </c>
@@ -7648,7 +7648,7 @@
       </c>
     </row>
     <row r="244" spans="1:21" ht="15.75">
-      <c r="A244" s="19" t="s">
+      <c r="A244" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B244" s="13">
@@ -7678,7 +7678,7 @@
       </c>
     </row>
     <row r="245" spans="1:21">
-      <c r="A245" s="20"/>
+      <c r="A245" s="26"/>
       <c r="B245" s="2">
         <v>3185</v>
       </c>
@@ -7706,7 +7706,7 @@
       </c>
     </row>
     <row r="246" spans="1:21">
-      <c r="A246" s="20"/>
+      <c r="A246" s="26"/>
       <c r="B246" s="2">
         <v>9914</v>
       </c>
@@ -7734,7 +7734,7 @@
       </c>
     </row>
     <row r="247" spans="1:21">
-      <c r="A247" s="20"/>
+      <c r="A247" s="26"/>
       <c r="B247" s="2">
         <v>6011</v>
       </c>
@@ -7762,7 +7762,7 @@
       </c>
     </row>
     <row r="248" spans="1:21">
-      <c r="A248" s="20"/>
+      <c r="A248" s="26"/>
       <c r="B248" s="2">
         <v>6037</v>
       </c>
@@ -7790,7 +7790,7 @@
       </c>
     </row>
     <row r="249" spans="1:21">
-      <c r="A249" s="20"/>
+      <c r="A249" s="26"/>
       <c r="B249" s="2">
         <v>2809</v>
       </c>
@@ -7818,7 +7818,7 @@
       </c>
     </row>
     <row r="250" spans="1:21">
-      <c r="A250" s="20"/>
+      <c r="A250" s="26"/>
       <c r="B250" s="2">
         <v>7297</v>
       </c>
@@ -7846,7 +7846,7 @@
       </c>
     </row>
     <row r="251" spans="1:21">
-      <c r="A251" s="20"/>
+      <c r="A251" s="26"/>
       <c r="B251" s="2">
         <v>5242</v>
       </c>
@@ -7874,7 +7874,7 @@
       </c>
     </row>
     <row r="252" spans="1:21">
-      <c r="A252" s="20"/>
+      <c r="A252" s="26"/>
       <c r="B252" s="2">
         <v>1379</v>
       </c>
@@ -7902,7 +7902,7 @@
       </c>
     </row>
     <row r="253" spans="1:21">
-      <c r="A253" s="20"/>
+      <c r="A253" s="26"/>
       <c r="B253" s="2">
         <v>2401</v>
       </c>
@@ -7930,7 +7930,7 @@
       </c>
     </row>
     <row r="254" spans="1:21">
-      <c r="A254" s="20"/>
+      <c r="A254" s="26"/>
       <c r="B254" s="2">
         <v>5421</v>
       </c>
@@ -7958,7 +7958,7 @@
       </c>
     </row>
     <row r="255" spans="1:21">
-      <c r="A255" s="20"/>
+      <c r="A255" s="26"/>
       <c r="B255" s="2">
         <v>9713</v>
       </c>
@@ -7986,7 +7986,7 @@
       </c>
     </row>
     <row r="256" spans="1:21">
-      <c r="A256" s="20"/>
+      <c r="A256" s="26"/>
       <c r="B256" s="2">
         <v>7301</v>
       </c>
@@ -8014,7 +8014,7 @@
       </c>
     </row>
     <row r="257" spans="1:21">
-      <c r="A257" s="20"/>
+      <c r="A257" s="26"/>
       <c r="B257" s="2">
         <v>6981</v>
       </c>
@@ -8042,7 +8042,7 @@
       </c>
     </row>
     <row r="258" spans="1:21">
-      <c r="A258" s="20"/>
+      <c r="A258" s="26"/>
       <c r="B258" s="2">
         <v>2000</v>
       </c>
@@ -8070,7 +8070,7 @@
       </c>
     </row>
     <row r="259" spans="1:21">
-      <c r="A259" s="20"/>
+      <c r="A259" s="26"/>
       <c r="B259" s="2">
         <v>5449</v>
       </c>
@@ -8098,7 +8098,7 @@
       </c>
     </row>
     <row r="260" spans="1:21">
-      <c r="A260" s="20"/>
+      <c r="A260" s="26"/>
       <c r="B260" s="2">
         <v>2662</v>
       </c>
@@ -8126,7 +8126,7 @@
       </c>
     </row>
     <row r="261" spans="1:21">
-      <c r="A261" s="20"/>
+      <c r="A261" s="26"/>
       <c r="B261" s="2">
         <v>4147</v>
       </c>
@@ -8154,7 +8154,7 @@
       </c>
     </row>
     <row r="262" spans="1:21">
-      <c r="A262" s="20"/>
+      <c r="A262" s="26"/>
       <c r="B262" s="2">
         <v>1953</v>
       </c>
@@ -8182,7 +8182,7 @@
       </c>
     </row>
     <row r="263" spans="1:21">
-      <c r="A263" s="20"/>
+      <c r="A263" s="26"/>
       <c r="B263" s="2">
         <v>3956</v>
       </c>
@@ -8210,7 +8210,7 @@
       </c>
     </row>
     <row r="264" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A264" s="21"/>
+      <c r="A264" s="27"/>
       <c r="B264" s="6">
         <v>8403</v>
       </c>
@@ -8238,7 +8238,7 @@
       </c>
     </row>
     <row r="265" spans="1:21">
-      <c r="A265" s="19" t="s">
+      <c r="A265" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B265" s="8">
@@ -8268,7 +8268,7 @@
       </c>
     </row>
     <row r="266" spans="1:21">
-      <c r="A266" s="20"/>
+      <c r="A266" s="26"/>
       <c r="B266" s="2">
         <v>5087</v>
       </c>
@@ -8296,7 +8296,7 @@
       </c>
     </row>
     <row r="267" spans="1:21">
-      <c r="A267" s="20"/>
+      <c r="A267" s="26"/>
       <c r="B267" s="2">
         <v>9990</v>
       </c>
@@ -8324,7 +8324,7 @@
       </c>
     </row>
     <row r="268" spans="1:21">
-      <c r="A268" s="20"/>
+      <c r="A268" s="26"/>
       <c r="B268" s="2">
         <v>7738</v>
       </c>
@@ -8352,7 +8352,7 @@
       </c>
     </row>
     <row r="269" spans="1:21">
-      <c r="A269" s="20"/>
+      <c r="A269" s="26"/>
       <c r="B269" s="2">
         <v>9924</v>
       </c>
@@ -8380,7 +8380,7 @@
       </c>
     </row>
     <row r="270" spans="1:21">
-      <c r="A270" s="24"/>
+      <c r="A270" s="28"/>
       <c r="B270" s="9">
         <v>7657</v>
       </c>
@@ -8408,7 +8408,7 @@
       </c>
     </row>
     <row r="271" spans="1:21">
-      <c r="A271" s="24"/>
+      <c r="A271" s="28"/>
       <c r="B271" s="9">
         <v>8258</v>
       </c>
@@ -8436,7 +8436,7 @@
       </c>
     </row>
     <row r="272" spans="1:21">
-      <c r="A272" s="24"/>
+      <c r="A272" s="28"/>
       <c r="B272" s="9">
         <v>7186</v>
       </c>
@@ -8464,7 +8464,7 @@
       </c>
     </row>
     <row r="273" spans="1:21">
-      <c r="A273" s="24"/>
+      <c r="A273" s="28"/>
       <c r="B273" s="9">
         <v>1457</v>
       </c>
@@ -8492,7 +8492,7 @@
       </c>
     </row>
     <row r="274" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A274" s="21"/>
+      <c r="A274" s="27"/>
       <c r="B274" s="6">
         <v>6876</v>
       </c>
@@ -8520,7 +8520,7 @@
       </c>
     </row>
     <row r="275" spans="1:21">
-      <c r="A275" s="19" t="s">
+      <c r="A275" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B275" s="8">
@@ -8550,7 +8550,7 @@
       </c>
     </row>
     <row r="276" spans="1:21">
-      <c r="A276" s="20"/>
+      <c r="A276" s="26"/>
       <c r="B276" s="2">
         <v>2070</v>
       </c>
@@ -8578,7 +8578,7 @@
       </c>
     </row>
     <row r="277" spans="1:21">
-      <c r="A277" s="20"/>
+      <c r="A277" s="26"/>
       <c r="B277" s="2">
         <v>7693</v>
       </c>
@@ -8606,7 +8606,7 @@
       </c>
     </row>
     <row r="278" spans="1:21">
-      <c r="A278" s="20"/>
+      <c r="A278" s="26"/>
       <c r="B278" s="2">
         <v>8718</v>
       </c>
@@ -8634,7 +8634,7 @@
       </c>
     </row>
     <row r="279" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A279" s="21"/>
+      <c r="A279" s="27"/>
       <c r="B279" s="6">
         <v>7248</v>
       </c>
@@ -8662,7 +8662,7 @@
       </c>
     </row>
     <row r="280" spans="1:21" ht="15.75">
-      <c r="A280" s="19" t="s">
+      <c r="A280" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B280" s="13">
@@ -8692,7 +8692,7 @@
       </c>
     </row>
     <row r="281" spans="1:21" ht="15.75">
-      <c r="A281" s="20"/>
+      <c r="A281" s="26"/>
       <c r="B281" s="12">
         <v>3083</v>
       </c>
@@ -8720,7 +8720,7 @@
       </c>
     </row>
     <row r="282" spans="1:21" ht="15.75">
-      <c r="A282" s="20"/>
+      <c r="A282" s="26"/>
       <c r="B282" s="12">
         <v>7546</v>
       </c>
@@ -8748,7 +8748,7 @@
       </c>
     </row>
     <row r="283" spans="1:21">
-      <c r="A283" s="20"/>
+      <c r="A283" s="26"/>
       <c r="B283" s="2">
         <v>7170</v>
       </c>
@@ -8776,7 +8776,7 @@
       </c>
     </row>
     <row r="284" spans="1:21">
-      <c r="A284" s="20"/>
+      <c r="A284" s="26"/>
       <c r="B284" s="2">
         <v>2709</v>
       </c>
@@ -8804,7 +8804,7 @@
       </c>
     </row>
     <row r="285" spans="1:21">
-      <c r="A285" s="20"/>
+      <c r="A285" s="26"/>
       <c r="B285" s="2">
         <v>3402</v>
       </c>
@@ -8832,7 +8832,7 @@
       </c>
     </row>
     <row r="286" spans="1:21">
-      <c r="A286" s="20"/>
+      <c r="A286" s="26"/>
       <c r="B286" s="2">
         <v>8781</v>
       </c>
@@ -8860,7 +8860,7 @@
       </c>
     </row>
     <row r="287" spans="1:21">
-      <c r="A287" s="20"/>
+      <c r="A287" s="26"/>
       <c r="B287" s="2">
         <v>8771</v>
       </c>
@@ -8888,7 +8888,7 @@
       </c>
     </row>
     <row r="288" spans="1:21">
-      <c r="A288" s="20"/>
+      <c r="A288" s="26"/>
       <c r="B288" s="2">
         <v>3091</v>
       </c>
@@ -8916,7 +8916,7 @@
       </c>
     </row>
     <row r="289" spans="1:21">
-      <c r="A289" s="20"/>
+      <c r="A289" s="26"/>
       <c r="B289" s="2">
         <v>2195</v>
       </c>
@@ -8944,7 +8944,7 @@
       </c>
     </row>
     <row r="290" spans="1:21">
-      <c r="A290" s="20"/>
+      <c r="A290" s="26"/>
       <c r="B290" s="2">
         <v>1184</v>
       </c>
@@ -8972,7 +8972,7 @@
       </c>
     </row>
     <row r="291" spans="1:21">
-      <c r="A291" s="20"/>
+      <c r="A291" s="26"/>
       <c r="B291" s="2">
         <v>2667</v>
       </c>
@@ -9000,7 +9000,7 @@
       </c>
     </row>
     <row r="292" spans="1:21">
-      <c r="A292" s="20"/>
+      <c r="A292" s="26"/>
       <c r="B292" s="2">
         <v>5917</v>
       </c>
@@ -9028,7 +9028,7 @@
       </c>
     </row>
     <row r="293" spans="1:21">
-      <c r="A293" s="20"/>
+      <c r="A293" s="26"/>
       <c r="B293" s="2">
         <v>8545</v>
       </c>
@@ -9056,7 +9056,7 @@
       </c>
     </row>
     <row r="294" spans="1:21">
-      <c r="A294" s="20"/>
+      <c r="A294" s="26"/>
       <c r="B294" s="2">
         <v>1288</v>
       </c>
@@ -9084,7 +9084,7 @@
       </c>
     </row>
     <row r="295" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A295" s="21"/>
+      <c r="A295" s="27"/>
       <c r="B295" s="6">
         <v>2614</v>
       </c>
@@ -9112,7 +9112,7 @@
       </c>
     </row>
     <row r="296" spans="1:21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B296" s="8">
@@ -9142,7 +9142,7 @@
       </c>
     </row>
     <row r="297" spans="1:21">
-      <c r="A297" s="20"/>
+      <c r="A297" s="26"/>
       <c r="B297" s="2">
         <v>6598</v>
       </c>
@@ -9170,7 +9170,7 @@
       </c>
     </row>
     <row r="298" spans="1:21">
-      <c r="A298" s="20"/>
+      <c r="A298" s="26"/>
       <c r="B298" s="2">
         <v>3093</v>
       </c>
@@ -9198,7 +9198,7 @@
       </c>
     </row>
     <row r="299" spans="1:21">
-      <c r="A299" s="20"/>
+      <c r="A299" s="26"/>
       <c r="B299" s="2">
         <v>8805</v>
       </c>
@@ -9226,7 +9226,7 @@
       </c>
     </row>
     <row r="300" spans="1:21">
-      <c r="A300" s="20"/>
+      <c r="A300" s="26"/>
       <c r="B300" s="2">
         <v>8158</v>
       </c>
@@ -9254,7 +9254,7 @@
       </c>
     </row>
     <row r="301" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A301" s="21"/>
+      <c r="A301" s="27"/>
       <c r="B301" s="6">
         <v>6499</v>
       </c>
@@ -9282,7 +9282,7 @@
       </c>
     </row>
     <row r="302" spans="1:21">
-      <c r="A302" s="19" t="s">
+      <c r="A302" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B302" s="8">
@@ -9312,7 +9312,7 @@
       </c>
     </row>
     <row r="303" spans="1:21">
-      <c r="A303" s="20"/>
+      <c r="A303" s="26"/>
       <c r="B303" s="2">
         <v>7560</v>
       </c>
@@ -9340,7 +9340,7 @@
       </c>
     </row>
     <row r="304" spans="1:21">
-      <c r="A304" s="20"/>
+      <c r="A304" s="26"/>
       <c r="B304" s="2">
         <v>9002</v>
       </c>
@@ -9368,7 +9368,7 @@
       </c>
     </row>
     <row r="305" spans="1:21">
-      <c r="A305" s="20"/>
+      <c r="A305" s="26"/>
       <c r="B305" s="2">
         <v>7432</v>
       </c>
@@ -9396,7 +9396,7 @@
       </c>
     </row>
     <row r="306" spans="1:21">
-      <c r="A306" s="20"/>
+      <c r="A306" s="26"/>
       <c r="B306" s="2">
         <v>1954</v>
       </c>
@@ -9424,7 +9424,7 @@
       </c>
     </row>
     <row r="307" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A307" s="21"/>
+      <c r="A307" s="27"/>
       <c r="B307" s="6">
         <v>2048</v>
       </c>
@@ -13077,6 +13077,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A228:A235"/>
+    <mergeCell ref="A236:A243"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
     <mergeCell ref="A275:A279"/>
@@ -13093,8 +13095,6 @@
     <mergeCell ref="A144:A160"/>
     <mergeCell ref="A101:A143"/>
     <mergeCell ref="A20:A60"/>
-    <mergeCell ref="A228:A235"/>
-    <mergeCell ref="A236:A243"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task 2092 to reduce difference from example
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$283</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$284</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -524,6 +524,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,24 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,11 +861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W915"/>
+  <dimension ref="A1:W916"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,56 +882,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>2732</v>
+        <v>5404</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="26"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="32"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -961,7 +961,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -991,7 +991,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1019,7 +1019,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1299,7 +1299,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="27" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1581,7 +1581,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1889,7 +1889,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2113,7 +2113,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2281,7 +2281,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2337,7 +2337,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="34"/>
+      <c r="A54" s="28"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="34"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="34"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2477,7 +2477,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="34"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2533,7 +2533,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2561,7 +2561,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="35"/>
+      <c r="A63" s="29"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -6293,7 +6293,7 @@
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="30"/>
+      <c r="A195" s="26"/>
       <c r="B195" s="9">
         <v>1618</v>
       </c>
@@ -6349,7 +6349,7 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="33" t="s">
+      <c r="A197" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B197" s="8">
@@ -6379,7 +6379,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="34"/>
+      <c r="A198" s="28"/>
       <c r="B198" s="2">
         <v>4488</v>
       </c>
@@ -6407,7 +6407,7 @@
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="34"/>
+      <c r="A199" s="28"/>
       <c r="B199" s="2">
         <v>4954</v>
       </c>
@@ -6435,7 +6435,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="34"/>
+      <c r="A200" s="28"/>
       <c r="B200" s="2">
         <v>4642</v>
       </c>
@@ -6463,7 +6463,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="34"/>
+      <c r="A201" s="28"/>
       <c r="B201" s="2">
         <v>5537</v>
       </c>
@@ -6491,7 +6491,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="34"/>
+      <c r="A202" s="28"/>
       <c r="B202" s="2">
         <v>5847</v>
       </c>
@@ -6519,7 +6519,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="34"/>
+      <c r="A203" s="28"/>
       <c r="B203" s="2">
         <v>4769</v>
       </c>
@@ -6547,7 +6547,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="34"/>
+      <c r="A204" s="28"/>
       <c r="B204" s="2">
         <v>9930</v>
       </c>
@@ -6570,12 +6570,12 @@
       <c r="S204" s="2"/>
       <c r="T204" s="5"/>
       <c r="U204">
-        <f t="shared" ref="U204:U277" ca="1" si="6">IF(B204=$W$1,1,0)</f>
+        <f t="shared" ref="U204:U278" ca="1" si="6">IF(B204=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="34"/>
+      <c r="A205" s="28"/>
       <c r="B205" s="2">
         <v>6861</v>
       </c>
@@ -6603,7 +6603,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="34"/>
+      <c r="A206" s="28"/>
       <c r="B206" s="2">
         <v>3226</v>
       </c>
@@ -6631,7 +6631,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="34"/>
+      <c r="A207" s="28"/>
       <c r="B207" s="2">
         <v>4372</v>
       </c>
@@ -6659,7 +6659,7 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="34"/>
+      <c r="A208" s="28"/>
       <c r="B208" s="2">
         <v>4463</v>
       </c>
@@ -6687,7 +6687,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="34"/>
+      <c r="A209" s="28"/>
       <c r="B209" s="2">
         <v>1668</v>
       </c>
@@ -6715,7 +6715,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="34"/>
+      <c r="A210" s="28"/>
       <c r="B210" s="2">
         <v>9417</v>
       </c>
@@ -6743,7 +6743,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="34"/>
+      <c r="A211" s="28"/>
       <c r="B211" s="2">
         <v>3148</v>
       </c>
@@ -6771,7 +6771,7 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="34"/>
+      <c r="A212" s="28"/>
       <c r="B212" s="2">
         <v>2137</v>
       </c>
@@ -6799,7 +6799,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="35"/>
+      <c r="A213" s="29"/>
       <c r="B213" s="6">
         <v>5621</v>
       </c>
@@ -7701,7 +7701,7 @@
     <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245" s="22"/>
       <c r="B245" s="2">
-        <v>9914</v>
+        <v>2092</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7729,7 +7729,7 @@
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246" s="22"/>
       <c r="B246" s="2">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7757,7 +7757,7 @@
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247" s="22"/>
       <c r="B247" s="2">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7785,7 +7785,7 @@
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="22"/>
       <c r="B248" s="2">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7813,7 +7813,7 @@
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" s="22"/>
       <c r="B249" s="2">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -7841,7 +7841,7 @@
     <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" s="22"/>
       <c r="B250" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -7869,7 +7869,7 @@
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" s="22"/>
       <c r="B251" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7897,7 +7897,7 @@
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" s="22"/>
       <c r="B252" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7925,7 +7925,7 @@
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="22"/>
       <c r="B253" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7953,7 +7953,7 @@
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="22"/>
       <c r="B254" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7981,7 +7981,7 @@
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="22"/>
       <c r="B255" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8009,7 +8009,7 @@
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="22"/>
       <c r="B256" s="2">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8037,7 +8037,7 @@
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="22"/>
       <c r="B257" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8065,7 +8065,7 @@
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="22"/>
       <c r="B258" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8093,7 +8093,7 @@
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="22"/>
       <c r="B259" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8121,7 +8121,7 @@
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" s="22"/>
       <c r="B260" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8149,7 +8149,7 @@
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="22"/>
       <c r="B261" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8177,7 +8177,7 @@
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="22"/>
       <c r="B262" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8205,7 +8205,7 @@
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="22"/>
       <c r="B263" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8233,7 +8233,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="22"/>
       <c r="B264" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8261,7 +8261,7 @@
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="22"/>
       <c r="B265" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8289,7 +8289,7 @@
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="22"/>
       <c r="B266" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8314,87 +8314,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="23"/>
-      <c r="B267" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C267" s="6"/>
-      <c r="D267" s="6"/>
-      <c r="E267" s="6"/>
-      <c r="F267" s="6"/>
-      <c r="G267" s="6"/>
-      <c r="H267" s="6"/>
-      <c r="I267" s="6"/>
-      <c r="J267" s="6"/>
-      <c r="K267" s="6"/>
-      <c r="L267" s="6"/>
-      <c r="M267" s="6"/>
-      <c r="N267" s="6"/>
-      <c r="O267" s="6"/>
-      <c r="P267" s="6"/>
-      <c r="Q267" s="6"/>
-      <c r="R267" s="6"/>
-      <c r="S267" s="6"/>
-      <c r="T267" s="7"/>
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A267" s="22"/>
+      <c r="B267" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C267" s="2"/>
+      <c r="D267" s="2"/>
+      <c r="E267" s="2"/>
+      <c r="F267" s="2"/>
+      <c r="G267" s="2"/>
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+      <c r="J267" s="2"/>
+      <c r="K267" s="2"/>
+      <c r="L267" s="2"/>
+      <c r="M267" s="2"/>
+      <c r="N267" s="2"/>
+      <c r="O267" s="2"/>
+      <c r="P267" s="2"/>
+      <c r="Q267" s="2"/>
+      <c r="R267" s="2"/>
+      <c r="S267" s="2"/>
+      <c r="T267" s="5"/>
       <c r="U267">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B268" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C268" s="8"/>
-      <c r="D268" s="8"/>
-      <c r="E268" s="8"/>
-      <c r="F268" s="8"/>
-      <c r="G268" s="8"/>
-      <c r="H268" s="8"/>
-      <c r="I268" s="8"/>
-      <c r="J268" s="8"/>
-      <c r="K268" s="8"/>
-      <c r="L268" s="8"/>
-      <c r="M268" s="8"/>
-      <c r="N268" s="8"/>
-      <c r="O268" s="8"/>
-      <c r="P268" s="8"/>
-      <c r="Q268" s="8"/>
-      <c r="R268" s="8"/>
-      <c r="S268" s="8"/>
-      <c r="T268" s="14"/>
+    <row r="268" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="23"/>
+      <c r="B268" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C268" s="6"/>
+      <c r="D268" s="6"/>
+      <c r="E268" s="6"/>
+      <c r="F268" s="6"/>
+      <c r="G268" s="6"/>
+      <c r="H268" s="6"/>
+      <c r="I268" s="6"/>
+      <c r="J268" s="6"/>
+      <c r="K268" s="6"/>
+      <c r="L268" s="6"/>
+      <c r="M268" s="6"/>
+      <c r="N268" s="6"/>
+      <c r="O268" s="6"/>
+      <c r="P268" s="6"/>
+      <c r="Q268" s="6"/>
+      <c r="R268" s="6"/>
+      <c r="S268" s="6"/>
+      <c r="T268" s="7"/>
       <c r="U268">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="22"/>
-      <c r="B269" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="E269" s="2"/>
-      <c r="F269" s="2"/>
-      <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
-      <c r="I269" s="2"/>
-      <c r="J269" s="2"/>
-      <c r="K269" s="2"/>
-      <c r="L269" s="2"/>
-      <c r="M269" s="2"/>
-      <c r="N269" s="2"/>
-      <c r="O269" s="2"/>
-      <c r="P269" s="2"/>
-      <c r="Q269" s="2"/>
-      <c r="R269" s="2"/>
-      <c r="S269" s="2"/>
-      <c r="T269" s="5"/>
+      <c r="A269" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B269" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C269" s="8"/>
+      <c r="D269" s="8"/>
+      <c r="E269" s="8"/>
+      <c r="F269" s="8"/>
+      <c r="G269" s="8"/>
+      <c r="H269" s="8"/>
+      <c r="I269" s="8"/>
+      <c r="J269" s="8"/>
+      <c r="K269" s="8"/>
+      <c r="L269" s="8"/>
+      <c r="M269" s="8"/>
+      <c r="N269" s="8"/>
+      <c r="O269" s="8"/>
+      <c r="P269" s="8"/>
+      <c r="Q269" s="8"/>
+      <c r="R269" s="8"/>
+      <c r="S269" s="8"/>
+      <c r="T269" s="14"/>
       <c r="U269">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8403,7 +8403,7 @@
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="22"/>
       <c r="B270" s="2">
-        <v>9990</v>
+        <v>5087</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8431,7 +8431,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="22"/>
       <c r="B271" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8459,7 +8459,7 @@
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="22"/>
       <c r="B272" s="2">
-        <v>9924</v>
+        <v>7738</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8485,37 +8485,37 @@
       </c>
     </row>
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="30"/>
-      <c r="B273" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C273" s="9"/>
-      <c r="D273" s="9"/>
-      <c r="E273" s="9"/>
-      <c r="F273" s="9"/>
-      <c r="G273" s="9"/>
-      <c r="H273" s="9"/>
-      <c r="I273" s="9"/>
-      <c r="J273" s="9"/>
-      <c r="K273" s="9"/>
-      <c r="L273" s="9"/>
-      <c r="M273" s="9"/>
-      <c r="N273" s="9"/>
-      <c r="O273" s="9"/>
-      <c r="P273" s="9"/>
-      <c r="Q273" s="9"/>
-      <c r="R273" s="9"/>
-      <c r="S273" s="9"/>
-      <c r="T273" s="15"/>
+      <c r="A273" s="22"/>
+      <c r="B273" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C273" s="2"/>
+      <c r="D273" s="2"/>
+      <c r="E273" s="2"/>
+      <c r="F273" s="2"/>
+      <c r="G273" s="2"/>
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+      <c r="J273" s="2"/>
+      <c r="K273" s="2"/>
+      <c r="L273" s="2"/>
+      <c r="M273" s="2"/>
+      <c r="N273" s="2"/>
+      <c r="O273" s="2"/>
+      <c r="P273" s="2"/>
+      <c r="Q273" s="2"/>
+      <c r="R273" s="2"/>
+      <c r="S273" s="2"/>
+      <c r="T273" s="5"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="30"/>
+      <c r="A274" s="26"/>
       <c r="B274" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C274" s="9"/>
       <c r="D274" s="9"/>
@@ -8541,9 +8541,9 @@
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="30"/>
+      <c r="A275" s="26"/>
       <c r="B275" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C275" s="9"/>
       <c r="D275" s="9"/>
@@ -8569,9 +8569,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="30"/>
+      <c r="A276" s="26"/>
       <c r="B276" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C276" s="9"/>
       <c r="D276" s="9"/>
@@ -8597,9 +8597,9 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="30"/>
+      <c r="A277" s="26"/>
       <c r="B277" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C277" s="9"/>
       <c r="D277" s="9"/>
@@ -8624,87 +8624,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="23"/>
-      <c r="B278" s="6">
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A278" s="26"/>
+      <c r="B278" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C278" s="9"/>
+      <c r="D278" s="9"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
+      <c r="G278" s="9"/>
+      <c r="H278" s="9"/>
+      <c r="I278" s="9"/>
+      <c r="J278" s="9"/>
+      <c r="K278" s="9"/>
+      <c r="L278" s="9"/>
+      <c r="M278" s="9"/>
+      <c r="N278" s="9"/>
+      <c r="O278" s="9"/>
+      <c r="P278" s="9"/>
+      <c r="Q278" s="9"/>
+      <c r="R278" s="9"/>
+      <c r="S278" s="9"/>
+      <c r="T278" s="15"/>
+      <c r="U278">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A279" s="23"/>
+      <c r="B279" s="6">
         <v>6876</v>
       </c>
-      <c r="C278" s="6"/>
-      <c r="D278" s="6"/>
-      <c r="E278" s="6"/>
-      <c r="F278" s="6"/>
-      <c r="G278" s="6"/>
-      <c r="H278" s="6"/>
-      <c r="I278" s="6"/>
-      <c r="J278" s="6"/>
-      <c r="K278" s="6"/>
-      <c r="L278" s="6"/>
-      <c r="M278" s="6"/>
-      <c r="N278" s="6"/>
-      <c r="O278" s="6"/>
-      <c r="P278" s="6"/>
-      <c r="Q278" s="6"/>
-      <c r="R278" s="6"/>
-      <c r="S278" s="6"/>
-      <c r="T278" s="7"/>
-      <c r="U278">
-        <f t="shared" ref="U278:U341" ca="1" si="7">IF(B278=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="21" t="s">
+      <c r="C279" s="6"/>
+      <c r="D279" s="6"/>
+      <c r="E279" s="6"/>
+      <c r="F279" s="6"/>
+      <c r="G279" s="6"/>
+      <c r="H279" s="6"/>
+      <c r="I279" s="6"/>
+      <c r="J279" s="6"/>
+      <c r="K279" s="6"/>
+      <c r="L279" s="6"/>
+      <c r="M279" s="6"/>
+      <c r="N279" s="6"/>
+      <c r="O279" s="6"/>
+      <c r="P279" s="6"/>
+      <c r="Q279" s="6"/>
+      <c r="R279" s="6"/>
+      <c r="S279" s="6"/>
+      <c r="T279" s="7"/>
+      <c r="U279">
+        <f t="shared" ref="U279:U342" ca="1" si="7">IF(B279=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A280" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B279" s="8">
+      <c r="B280" s="8">
         <v>4304</v>
       </c>
-      <c r="C279" s="8"/>
-      <c r="D279" s="8"/>
-      <c r="E279" s="8"/>
-      <c r="F279" s="8"/>
-      <c r="G279" s="8"/>
-      <c r="H279" s="8"/>
-      <c r="I279" s="8"/>
-      <c r="J279" s="8"/>
-      <c r="K279" s="8"/>
-      <c r="L279" s="8"/>
-      <c r="M279" s="8"/>
-      <c r="N279" s="8"/>
-      <c r="O279" s="8"/>
-      <c r="P279" s="8"/>
-      <c r="Q279" s="8"/>
-      <c r="R279" s="8"/>
-      <c r="S279" s="8"/>
-      <c r="T279" s="14"/>
-      <c r="U279">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="22"/>
-      <c r="B280" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="E280" s="2"/>
-      <c r="F280" s="2"/>
-      <c r="G280" s="2"/>
-      <c r="H280" s="2"/>
-      <c r="I280" s="2"/>
-      <c r="J280" s="2"/>
-      <c r="K280" s="2"/>
-      <c r="L280" s="2"/>
-      <c r="M280" s="2"/>
-      <c r="N280" s="2"/>
-      <c r="O280" s="2"/>
-      <c r="P280" s="2"/>
-      <c r="Q280" s="2"/>
-      <c r="R280" s="2"/>
-      <c r="S280" s="2"/>
-      <c r="T280" s="5"/>
+      <c r="C280" s="8"/>
+      <c r="D280" s="8"/>
+      <c r="E280" s="8"/>
+      <c r="F280" s="8"/>
+      <c r="G280" s="8"/>
+      <c r="H280" s="8"/>
+      <c r="I280" s="8"/>
+      <c r="J280" s="8"/>
+      <c r="K280" s="8"/>
+      <c r="L280" s="8"/>
+      <c r="M280" s="8"/>
+      <c r="N280" s="8"/>
+      <c r="O280" s="8"/>
+      <c r="P280" s="8"/>
+      <c r="Q280" s="8"/>
+      <c r="R280" s="8"/>
+      <c r="S280" s="8"/>
+      <c r="T280" s="14"/>
       <c r="U280">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8713,7 +8713,7 @@
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="22"/>
       <c r="B281" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8741,7 +8741,7 @@
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="22"/>
       <c r="B282" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8766,87 +8766,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="23"/>
-      <c r="B283" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C283" s="6"/>
-      <c r="D283" s="6"/>
-      <c r="E283" s="6"/>
-      <c r="F283" s="6"/>
-      <c r="G283" s="6"/>
-      <c r="H283" s="6"/>
-      <c r="I283" s="6"/>
-      <c r="J283" s="6"/>
-      <c r="K283" s="6"/>
-      <c r="L283" s="6"/>
-      <c r="M283" s="6"/>
-      <c r="N283" s="6"/>
-      <c r="O283" s="6"/>
-      <c r="P283" s="6"/>
-      <c r="Q283" s="6"/>
-      <c r="R283" s="6"/>
-      <c r="S283" s="6"/>
-      <c r="T283" s="7"/>
+    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A283" s="22"/>
+      <c r="B283" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C283" s="2"/>
+      <c r="D283" s="2"/>
+      <c r="E283" s="2"/>
+      <c r="F283" s="2"/>
+      <c r="G283" s="2"/>
+      <c r="H283" s="2"/>
+      <c r="I283" s="2"/>
+      <c r="J283" s="2"/>
+      <c r="K283" s="2"/>
+      <c r="L283" s="2"/>
+      <c r="M283" s="2"/>
+      <c r="N283" s="2"/>
+      <c r="O283" s="2"/>
+      <c r="P283" s="2"/>
+      <c r="Q283" s="2"/>
+      <c r="R283" s="2"/>
+      <c r="S283" s="2"/>
+      <c r="T283" s="5"/>
       <c r="U283">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A284" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B284" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C284" s="8"/>
-      <c r="D284" s="8"/>
-      <c r="E284" s="8"/>
-      <c r="F284" s="8"/>
-      <c r="G284" s="8"/>
-      <c r="H284" s="8"/>
-      <c r="I284" s="8"/>
-      <c r="J284" s="8"/>
-      <c r="K284" s="8"/>
-      <c r="L284" s="8"/>
-      <c r="M284" s="8"/>
-      <c r="N284" s="8"/>
-      <c r="O284" s="8"/>
-      <c r="P284" s="8"/>
-      <c r="Q284" s="8"/>
-      <c r="R284" s="8"/>
-      <c r="S284" s="8"/>
-      <c r="T284" s="14"/>
+    <row r="284" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A284" s="23"/>
+      <c r="B284" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C284" s="6"/>
+      <c r="D284" s="6"/>
+      <c r="E284" s="6"/>
+      <c r="F284" s="6"/>
+      <c r="G284" s="6"/>
+      <c r="H284" s="6"/>
+      <c r="I284" s="6"/>
+      <c r="J284" s="6"/>
+      <c r="K284" s="6"/>
+      <c r="L284" s="6"/>
+      <c r="M284" s="6"/>
+      <c r="N284" s="6"/>
+      <c r="O284" s="6"/>
+      <c r="P284" s="6"/>
+      <c r="Q284" s="6"/>
+      <c r="R284" s="6"/>
+      <c r="S284" s="6"/>
+      <c r="T284" s="7"/>
       <c r="U284">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A285" s="22"/>
-      <c r="B285" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2"/>
-      <c r="E285" s="2"/>
-      <c r="F285" s="2"/>
-      <c r="G285" s="2"/>
-      <c r="H285" s="2"/>
-      <c r="I285" s="2"/>
-      <c r="J285" s="2"/>
-      <c r="K285" s="2"/>
-      <c r="L285" s="2"/>
-      <c r="M285" s="2"/>
-      <c r="N285" s="2"/>
-      <c r="O285" s="2"/>
-      <c r="P285" s="2"/>
-      <c r="Q285" s="2"/>
-      <c r="R285" s="2"/>
-      <c r="S285" s="2"/>
-      <c r="T285" s="5"/>
+      <c r="A285" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B285" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C285" s="8"/>
+      <c r="D285" s="8"/>
+      <c r="E285" s="8"/>
+      <c r="F285" s="8"/>
+      <c r="G285" s="8"/>
+      <c r="H285" s="8"/>
+      <c r="I285" s="8"/>
+      <c r="J285" s="8"/>
+      <c r="K285" s="8"/>
+      <c r="L285" s="8"/>
+      <c r="M285" s="8"/>
+      <c r="N285" s="8"/>
+      <c r="O285" s="8"/>
+      <c r="P285" s="8"/>
+      <c r="Q285" s="8"/>
+      <c r="R285" s="8"/>
+      <c r="S285" s="8"/>
+      <c r="T285" s="14"/>
       <c r="U285">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8855,7 +8855,7 @@
     <row r="286" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A286" s="22"/>
       <c r="B286" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8880,10 +8880,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="22"/>
-      <c r="B287" s="2">
-        <v>7170</v>
+      <c r="B287" s="12">
+        <v>7546</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8911,7 +8911,7 @@
     <row r="288" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A288" s="22"/>
       <c r="B288" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -8939,7 +8939,7 @@
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" s="22"/>
       <c r="B289" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -8967,7 +8967,7 @@
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="22"/>
       <c r="B290" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8995,7 +8995,7 @@
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="22"/>
       <c r="B291" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9023,7 +9023,7 @@
     <row r="292" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A292" s="22"/>
       <c r="B292" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9051,7 +9051,7 @@
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293" s="22"/>
       <c r="B293" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9079,7 +9079,7 @@
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A294" s="22"/>
       <c r="B294" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9107,7 +9107,7 @@
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" s="22"/>
       <c r="B295" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9135,7 +9135,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="22"/>
       <c r="B296" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9163,7 +9163,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="22"/>
       <c r="B297" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9191,7 +9191,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="22"/>
       <c r="B298" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9216,87 +9216,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="23"/>
-      <c r="B299" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C299" s="6"/>
-      <c r="D299" s="6"/>
-      <c r="E299" s="6"/>
-      <c r="F299" s="6"/>
-      <c r="G299" s="6"/>
-      <c r="H299" s="6"/>
-      <c r="I299" s="6"/>
-      <c r="J299" s="6"/>
-      <c r="K299" s="6"/>
-      <c r="L299" s="6"/>
-      <c r="M299" s="6"/>
-      <c r="N299" s="6"/>
-      <c r="O299" s="6"/>
-      <c r="P299" s="6"/>
-      <c r="Q299" s="6"/>
-      <c r="R299" s="6"/>
-      <c r="S299" s="6"/>
-      <c r="T299" s="7"/>
+    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A299" s="22"/>
+      <c r="B299" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C299" s="2"/>
+      <c r="D299" s="2"/>
+      <c r="E299" s="2"/>
+      <c r="F299" s="2"/>
+      <c r="G299" s="2"/>
+      <c r="H299" s="2"/>
+      <c r="I299" s="2"/>
+      <c r="J299" s="2"/>
+      <c r="K299" s="2"/>
+      <c r="L299" s="2"/>
+      <c r="M299" s="2"/>
+      <c r="N299" s="2"/>
+      <c r="O299" s="2"/>
+      <c r="P299" s="2"/>
+      <c r="Q299" s="2"/>
+      <c r="R299" s="2"/>
+      <c r="S299" s="2"/>
+      <c r="T299" s="5"/>
       <c r="U299">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A300" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B300" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C300" s="8"/>
-      <c r="D300" s="8"/>
-      <c r="E300" s="8"/>
-      <c r="F300" s="8"/>
-      <c r="G300" s="8"/>
-      <c r="H300" s="8"/>
-      <c r="I300" s="8"/>
-      <c r="J300" s="8"/>
-      <c r="K300" s="8"/>
-      <c r="L300" s="8"/>
-      <c r="M300" s="8"/>
-      <c r="N300" s="8"/>
-      <c r="O300" s="8"/>
-      <c r="P300" s="8"/>
-      <c r="Q300" s="8"/>
-      <c r="R300" s="8"/>
-      <c r="S300" s="8"/>
-      <c r="T300" s="14"/>
+    <row r="300" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="23"/>
+      <c r="B300" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C300" s="6"/>
+      <c r="D300" s="6"/>
+      <c r="E300" s="6"/>
+      <c r="F300" s="6"/>
+      <c r="G300" s="6"/>
+      <c r="H300" s="6"/>
+      <c r="I300" s="6"/>
+      <c r="J300" s="6"/>
+      <c r="K300" s="6"/>
+      <c r="L300" s="6"/>
+      <c r="M300" s="6"/>
+      <c r="N300" s="6"/>
+      <c r="O300" s="6"/>
+      <c r="P300" s="6"/>
+      <c r="Q300" s="6"/>
+      <c r="R300" s="6"/>
+      <c r="S300" s="6"/>
+      <c r="T300" s="7"/>
       <c r="U300">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="22"/>
-      <c r="B301" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C301" s="2"/>
-      <c r="D301" s="2"/>
-      <c r="E301" s="2"/>
-      <c r="F301" s="2"/>
-      <c r="G301" s="2"/>
-      <c r="H301" s="2"/>
-      <c r="I301" s="2"/>
-      <c r="J301" s="2"/>
-      <c r="K301" s="2"/>
-      <c r="L301" s="2"/>
-      <c r="M301" s="2"/>
-      <c r="N301" s="2"/>
-      <c r="O301" s="2"/>
-      <c r="P301" s="2"/>
-      <c r="Q301" s="2"/>
-      <c r="R301" s="2"/>
-      <c r="S301" s="2"/>
-      <c r="T301" s="5"/>
+      <c r="A301" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B301" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C301" s="8"/>
+      <c r="D301" s="8"/>
+      <c r="E301" s="8"/>
+      <c r="F301" s="8"/>
+      <c r="G301" s="8"/>
+      <c r="H301" s="8"/>
+      <c r="I301" s="8"/>
+      <c r="J301" s="8"/>
+      <c r="K301" s="8"/>
+      <c r="L301" s="8"/>
+      <c r="M301" s="8"/>
+      <c r="N301" s="8"/>
+      <c r="O301" s="8"/>
+      <c r="P301" s="8"/>
+      <c r="Q301" s="8"/>
+      <c r="R301" s="8"/>
+      <c r="S301" s="8"/>
+      <c r="T301" s="14"/>
       <c r="U301">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9305,7 +9305,7 @@
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="22"/>
       <c r="B302" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9333,7 +9333,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="22"/>
       <c r="B303" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9361,7 +9361,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="22"/>
       <c r="B304" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9386,87 +9386,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="23"/>
-      <c r="B305" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C305" s="6"/>
-      <c r="D305" s="6"/>
-      <c r="E305" s="6"/>
-      <c r="F305" s="6"/>
-      <c r="G305" s="6"/>
-      <c r="H305" s="6"/>
-      <c r="I305" s="6"/>
-      <c r="J305" s="6"/>
-      <c r="K305" s="6"/>
-      <c r="L305" s="6"/>
-      <c r="M305" s="6"/>
-      <c r="N305" s="6"/>
-      <c r="O305" s="6"/>
-      <c r="P305" s="6"/>
-      <c r="Q305" s="6"/>
-      <c r="R305" s="6"/>
-      <c r="S305" s="6"/>
-      <c r="T305" s="7"/>
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A305" s="22"/>
+      <c r="B305" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C305" s="2"/>
+      <c r="D305" s="2"/>
+      <c r="E305" s="2"/>
+      <c r="F305" s="2"/>
+      <c r="G305" s="2"/>
+      <c r="H305" s="2"/>
+      <c r="I305" s="2"/>
+      <c r="J305" s="2"/>
+      <c r="K305" s="2"/>
+      <c r="L305" s="2"/>
+      <c r="M305" s="2"/>
+      <c r="N305" s="2"/>
+      <c r="O305" s="2"/>
+      <c r="P305" s="2"/>
+      <c r="Q305" s="2"/>
+      <c r="R305" s="2"/>
+      <c r="S305" s="2"/>
+      <c r="T305" s="5"/>
       <c r="U305">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A306" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B306" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C306" s="8"/>
-      <c r="D306" s="8"/>
-      <c r="E306" s="8"/>
-      <c r="F306" s="8"/>
-      <c r="G306" s="8"/>
-      <c r="H306" s="8"/>
-      <c r="I306" s="8"/>
-      <c r="J306" s="8"/>
-      <c r="K306" s="8"/>
-      <c r="L306" s="8"/>
-      <c r="M306" s="8"/>
-      <c r="N306" s="8"/>
-      <c r="O306" s="8"/>
-      <c r="P306" s="8"/>
-      <c r="Q306" s="8"/>
-      <c r="R306" s="8"/>
-      <c r="S306" s="8"/>
-      <c r="T306" s="14"/>
+    <row r="306" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="23"/>
+      <c r="B306" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C306" s="6"/>
+      <c r="D306" s="6"/>
+      <c r="E306" s="6"/>
+      <c r="F306" s="6"/>
+      <c r="G306" s="6"/>
+      <c r="H306" s="6"/>
+      <c r="I306" s="6"/>
+      <c r="J306" s="6"/>
+      <c r="K306" s="6"/>
+      <c r="L306" s="6"/>
+      <c r="M306" s="6"/>
+      <c r="N306" s="6"/>
+      <c r="O306" s="6"/>
+      <c r="P306" s="6"/>
+      <c r="Q306" s="6"/>
+      <c r="R306" s="6"/>
+      <c r="S306" s="6"/>
+      <c r="T306" s="7"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A307" s="22"/>
-      <c r="B307" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2"/>
-      <c r="E307" s="2"/>
-      <c r="F307" s="2"/>
-      <c r="G307" s="2"/>
-      <c r="H307" s="2"/>
-      <c r="I307" s="2"/>
-      <c r="J307" s="2"/>
-      <c r="K307" s="2"/>
-      <c r="L307" s="2"/>
-      <c r="M307" s="2"/>
-      <c r="N307" s="2"/>
-      <c r="O307" s="2"/>
-      <c r="P307" s="2"/>
-      <c r="Q307" s="2"/>
-      <c r="R307" s="2"/>
-      <c r="S307" s="2"/>
-      <c r="T307" s="5"/>
+      <c r="A307" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B307" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C307" s="8"/>
+      <c r="D307" s="8"/>
+      <c r="E307" s="8"/>
+      <c r="F307" s="8"/>
+      <c r="G307" s="8"/>
+      <c r="H307" s="8"/>
+      <c r="I307" s="8"/>
+      <c r="J307" s="8"/>
+      <c r="K307" s="8"/>
+      <c r="L307" s="8"/>
+      <c r="M307" s="8"/>
+      <c r="N307" s="8"/>
+      <c r="O307" s="8"/>
+      <c r="P307" s="8"/>
+      <c r="Q307" s="8"/>
+      <c r="R307" s="8"/>
+      <c r="S307" s="8"/>
+      <c r="T307" s="14"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9475,7 +9475,7 @@
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A308" s="22"/>
       <c r="B308" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -9503,7 +9503,7 @@
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="22"/>
       <c r="B309" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9531,7 +9531,7 @@
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="22"/>
       <c r="B310" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9556,35 +9556,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="23"/>
-      <c r="B311" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C311" s="6"/>
-      <c r="D311" s="6"/>
-      <c r="E311" s="6"/>
-      <c r="F311" s="6"/>
-      <c r="G311" s="6"/>
-      <c r="H311" s="6"/>
-      <c r="I311" s="6"/>
-      <c r="J311" s="6"/>
-      <c r="K311" s="6"/>
-      <c r="L311" s="6"/>
-      <c r="M311" s="6"/>
-      <c r="N311" s="6"/>
-      <c r="O311" s="6"/>
-      <c r="P311" s="6"/>
-      <c r="Q311" s="6"/>
-      <c r="R311" s="6"/>
-      <c r="S311" s="6"/>
-      <c r="T311" s="7"/>
+    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A311" s="22"/>
+      <c r="B311" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C311" s="2"/>
+      <c r="D311" s="2"/>
+      <c r="E311" s="2"/>
+      <c r="F311" s="2"/>
+      <c r="G311" s="2"/>
+      <c r="H311" s="2"/>
+      <c r="I311" s="2"/>
+      <c r="J311" s="2"/>
+      <c r="K311" s="2"/>
+      <c r="L311" s="2"/>
+      <c r="M311" s="2"/>
+      <c r="N311" s="2"/>
+      <c r="O311" s="2"/>
+      <c r="P311" s="2"/>
+      <c r="Q311" s="2"/>
+      <c r="R311" s="2"/>
+      <c r="S311" s="2"/>
+      <c r="T311" s="5"/>
       <c r="U311">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A312" s="23"/>
+      <c r="B312" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C312" s="6"/>
+      <c r="D312" s="6"/>
+      <c r="E312" s="6"/>
+      <c r="F312" s="6"/>
+      <c r="G312" s="6"/>
+      <c r="H312" s="6"/>
+      <c r="I312" s="6"/>
+      <c r="J312" s="6"/>
+      <c r="K312" s="6"/>
+      <c r="L312" s="6"/>
+      <c r="M312" s="6"/>
+      <c r="N312" s="6"/>
+      <c r="O312" s="6"/>
+      <c r="P312" s="6"/>
+      <c r="Q312" s="6"/>
+      <c r="R312" s="6"/>
+      <c r="S312" s="6"/>
+      <c r="T312" s="7"/>
       <c r="U312">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9766,13 +9788,13 @@
     </row>
     <row r="342" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U342">
-        <f t="shared" ref="U342:U405" ca="1" si="8">IF(B342=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="343" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U343">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U343:U406" ca="1" si="8">IF(B343=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10150,13 +10172,13 @@
     </row>
     <row r="406" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U406">
-        <f t="shared" ref="U406:U469" ca="1" si="9">IF(B406=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="407" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U407">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U407:U470" ca="1" si="9">IF(B407=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10534,13 +10556,13 @@
     </row>
     <row r="470" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U470">
-        <f t="shared" ref="U470:U533" ca="1" si="10">IF(B470=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="471" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U471">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U471:U534" ca="1" si="10">IF(B471=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10918,13 +10940,13 @@
     </row>
     <row r="534" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U534">
-        <f t="shared" ref="U534:U597" ca="1" si="11">IF(B534=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="535" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U535">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U535:U598" ca="1" si="11">IF(B535=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11302,13 +11324,13 @@
     </row>
     <row r="598" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U598">
-        <f t="shared" ref="U598:U661" ca="1" si="12">IF(B598=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="599" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U599">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U599:U662" ca="1" si="12">IF(B599=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11686,13 +11708,13 @@
     </row>
     <row r="662" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U662">
-        <f t="shared" ref="U662:U725" ca="1" si="13">IF(B662=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="663" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U663">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U663:U726" ca="1" si="13">IF(B663=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12070,13 +12092,13 @@
     </row>
     <row r="726" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U726">
-        <f t="shared" ref="U726:U789" ca="1" si="14">IF(B726=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="727" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U727">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U727:U790" ca="1" si="14">IF(B727=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12454,13 +12476,13 @@
     </row>
     <row r="790" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U790">
-        <f t="shared" ref="U790:U853" ca="1" si="15">IF(B790=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="791" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U791">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U791:U854" ca="1" si="15">IF(B791=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12838,13 +12860,13 @@
     </row>
     <row r="854" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U854">
-        <f t="shared" ref="U854:U915" ca="1" si="16">IF(B854=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="855" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U855">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U855:U916" ca="1" si="16">IF(B855=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13208,13 +13230,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="916" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U916">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A306:A311"/>
-    <mergeCell ref="A242:A267"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A280:A284"/>
+    <mergeCell ref="A269:A279"/>
+    <mergeCell ref="A307:A312"/>
+    <mergeCell ref="A242:A268"/>
     <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A284:A299"/>
-    <mergeCell ref="A300:A305"/>
+    <mergeCell ref="A285:A300"/>
+    <mergeCell ref="A301:A306"/>
     <mergeCell ref="A64:A102"/>
     <mergeCell ref="A214:A225"/>
     <mergeCell ref="A147:A178"/>
@@ -13224,10 +13256,6 @@
     <mergeCell ref="A197:A213"/>
     <mergeCell ref="A226:A233"/>
     <mergeCell ref="A234:A241"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A279:A283"/>
-    <mergeCell ref="A268:A278"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task 1292 to conditions and arrays
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$284</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$285</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -524,24 +524,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,6 +541,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,11 +861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W916"/>
+  <dimension ref="A1:W917"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,60 +878,60 @@
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V1">
         <f ca="1">SUM(U:U)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>5404</v>
+        <v>9300</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="35"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="32"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -961,7 +961,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -991,7 +991,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1019,7 +1019,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1299,7 +1299,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1581,7 +1581,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1889,7 +1889,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2057,7 +2057,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2113,7 +2113,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+      <c r="A47" s="34"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
+      <c r="A51" s="34"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2281,7 +2281,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+      <c r="A52" s="34"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="34"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2337,7 +2337,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
+      <c r="A54" s="34"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
+      <c r="A56" s="34"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="34"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
+      <c r="A58" s="34"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2477,7 +2477,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
+      <c r="A59" s="34"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
+      <c r="A60" s="34"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2533,7 +2533,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
+      <c r="A61" s="34"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2561,7 +2561,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="34"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="29"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -2838,7 +2838,7 @@
       <c r="S71" s="2"/>
       <c r="T71" s="5"/>
       <c r="U71">
-        <f t="shared" ref="U71:U136" ca="1" si="3">IF(B71=$W$1,1,0)</f>
+        <f t="shared" ref="U71:U137" ca="1" si="3">IF(B71=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="22"/>
       <c r="B95" s="2">
-        <v>4527</v>
+        <v>1292</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -3517,7 +3517,7 @@
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="22"/>
       <c r="B96" s="2">
-        <v>6556</v>
+        <v>4527</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -3545,7 +3545,7 @@
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
       <c r="B97" s="2">
-        <v>5635</v>
+        <v>6556</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -3573,7 +3573,7 @@
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="22"/>
       <c r="B98" s="2">
-        <v>3878</v>
+        <v>5635</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -3601,7 +3601,7 @@
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="22"/>
       <c r="B99" s="2">
-        <v>1217</v>
+        <v>3878</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3629,7 +3629,7 @@
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="22"/>
       <c r="B100" s="2">
-        <v>1438</v>
+        <v>1217</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3657,7 +3657,7 @@
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="22"/>
       <c r="B101" s="2">
-        <v>2153</v>
+        <v>1438</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -3682,96 +3682,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="23"/>
-      <c r="B102" s="6">
-        <v>7937</v>
-      </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
-      <c r="S102" s="6"/>
-      <c r="T102" s="7"/>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A102" s="22"/>
+      <c r="B102" s="2">
+        <v>2153</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+      <c r="S102" s="2"/>
+      <c r="T102" s="5"/>
       <c r="U102">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="13">
-        <v>7779</v>
-      </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="8"/>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8"/>
-      <c r="L103" s="8"/>
-      <c r="M103" s="8"/>
-      <c r="N103" s="8"/>
-      <c r="O103" s="8"/>
-      <c r="P103" s="8"/>
-      <c r="Q103" s="8"/>
-      <c r="R103" s="8"/>
-      <c r="S103" s="8"/>
-      <c r="T103" s="14"/>
+    <row r="103" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="23"/>
+      <c r="B103" s="6">
+        <v>7937</v>
+      </c>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
+      <c r="P103" s="6"/>
+      <c r="Q103" s="6"/>
+      <c r="R103" s="6"/>
+      <c r="S103" s="6"/>
+      <c r="T103" s="7"/>
       <c r="U103">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="22"/>
-      <c r="B104" s="12">
-        <v>1881</v>
-      </c>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
-      <c r="N104" s="2"/>
-      <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
-      <c r="Q104" s="2"/>
-      <c r="R104" s="2"/>
-      <c r="S104" s="2"/>
-      <c r="T104" s="5"/>
+      <c r="A104" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="13">
+        <v>7779</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="8"/>
+      <c r="N104" s="8"/>
+      <c r="O104" s="8"/>
+      <c r="P104" s="8"/>
+      <c r="Q104" s="8"/>
+      <c r="R104" s="8"/>
+      <c r="S104" s="8"/>
+      <c r="T104" s="14"/>
       <c r="U104">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="22"/>
-      <c r="B105" s="2">
-        <v>8495</v>
+      <c r="B105" s="12">
+        <v>1881</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -3799,7 +3799,7 @@
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="22"/>
       <c r="B106" s="2">
-        <v>1315</v>
+        <v>8495</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -3827,7 +3827,7 @@
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="22"/>
       <c r="B107" s="2">
-        <v>6066</v>
+        <v>1315</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -3855,7 +3855,7 @@
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="22"/>
       <c r="B108" s="2">
-        <v>2565</v>
+        <v>6066</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -3883,7 +3883,7 @@
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
       <c r="B109" s="2">
-        <v>2594</v>
+        <v>2565</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -3911,7 +3911,7 @@
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="22"/>
       <c r="B110" s="2">
-        <v>2321</v>
+        <v>2594</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -3939,7 +3939,7 @@
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="22"/>
       <c r="B111" s="2">
-        <v>5053</v>
+        <v>2321</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -3967,7 +3967,7 @@
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="22"/>
       <c r="B112" s="2">
-        <v>3762</v>
+        <v>5053</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -3995,7 +3995,7 @@
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="22"/>
       <c r="B113" s="2">
-        <v>3550</v>
+        <v>3762</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -4023,7 +4023,7 @@
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="22"/>
       <c r="B114" s="2">
-        <v>4264</v>
+        <v>3550</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -4051,7 +4051,7 @@
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="22"/>
       <c r="B115" s="2">
-        <v>2475</v>
+        <v>4264</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -4079,7 +4079,7 @@
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="22"/>
       <c r="B116" s="2">
-        <v>9180</v>
+        <v>2475</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -4107,7 +4107,7 @@
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
       <c r="B117" s="2">
-        <v>1544</v>
+        <v>9180</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -4135,7 +4135,7 @@
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="22"/>
       <c r="B118" s="2">
-        <v>9562</v>
+        <v>1544</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -4163,7 +4163,7 @@
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="22"/>
       <c r="B119" s="2">
-        <v>3669</v>
+        <v>9562</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -4191,7 +4191,7 @@
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="22"/>
       <c r="B120" s="2">
-        <v>5951</v>
+        <v>3669</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -4219,7 +4219,7 @@
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="22"/>
       <c r="B121" s="2">
-        <v>2802</v>
+        <v>5951</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -4247,7 +4247,7 @@
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="22"/>
       <c r="B122" s="2">
-        <v>2324</v>
+        <v>2802</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -4275,7 +4275,7 @@
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="22"/>
       <c r="B123" s="2">
-        <v>8731</v>
+        <v>2324</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -4303,7 +4303,7 @@
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="22"/>
       <c r="B124" s="2">
-        <v>4082</v>
+        <v>8731</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -4331,7 +4331,7 @@
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="22"/>
       <c r="B125" s="2">
-        <v>6280</v>
+        <v>4082</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -4359,7 +4359,7 @@
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="22"/>
       <c r="B126" s="2">
-        <v>7585</v>
+        <v>6280</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -4387,7 +4387,7 @@
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" s="22"/>
       <c r="B127" s="2">
-        <v>1483</v>
+        <v>7585</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -4415,7 +4415,7 @@
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" s="22"/>
       <c r="B128" s="2">
-        <v>3983</v>
+        <v>1483</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -4443,7 +4443,7 @@
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="22"/>
       <c r="B129" s="2">
-        <v>8770</v>
+        <v>3983</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -4471,7 +4471,7 @@
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130" s="22"/>
       <c r="B130" s="2">
-        <v>4236</v>
+        <v>8770</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -4499,7 +4499,7 @@
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131" s="22"/>
       <c r="B131" s="2">
-        <v>8696</v>
+        <v>4236</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -4527,7 +4527,7 @@
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132" s="22"/>
       <c r="B132" s="2">
-        <v>5969</v>
+        <v>8696</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -4555,7 +4555,7 @@
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" s="22"/>
       <c r="B133" s="2">
-        <v>8418</v>
+        <v>5969</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -4583,7 +4583,7 @@
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" s="22"/>
       <c r="B134" s="2">
-        <v>5170</v>
+        <v>8418</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -4611,7 +4611,7 @@
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135" s="22"/>
       <c r="B135" s="2">
-        <v>8395</v>
+        <v>5170</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
@@ -4639,7 +4639,7 @@
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" s="22"/>
       <c r="B136" s="2">
-        <v>5568</v>
+        <v>8395</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -4667,7 +4667,7 @@
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" s="22"/>
       <c r="B137" s="2">
-        <v>2592</v>
+        <v>5568</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -4688,14 +4688,14 @@
       <c r="S137" s="2"/>
       <c r="T137" s="5"/>
       <c r="U137">
-        <f t="shared" ref="U137:U203" ca="1" si="4">IF(B137=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="22"/>
       <c r="B138" s="2">
-        <v>4075</v>
+        <v>2592</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -4716,14 +4716,14 @@
       <c r="S138" s="2"/>
       <c r="T138" s="5"/>
       <c r="U138">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="U138:U204" ca="1" si="4">IF(B138=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" s="22"/>
       <c r="B139" s="2">
-        <v>7517</v>
+        <v>4075</v>
       </c>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -4751,7 +4751,7 @@
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140" s="22"/>
       <c r="B140" s="2">
-        <v>5448</v>
+        <v>7517</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -4779,7 +4779,7 @@
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141" s="22"/>
       <c r="B141" s="2">
-        <v>6582</v>
+        <v>5448</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -4807,7 +4807,7 @@
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142" s="22"/>
       <c r="B142" s="2">
-        <v>5238</v>
+        <v>6582</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -4835,7 +4835,7 @@
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143" s="22"/>
       <c r="B143" s="2">
-        <v>2084</v>
+        <v>5238</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -4863,7 +4863,7 @@
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" s="22"/>
       <c r="B144" s="2">
-        <v>5411</v>
+        <v>2084</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -4891,7 +4891,7 @@
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="22"/>
       <c r="B145" s="2">
-        <v>5171</v>
+        <v>5411</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -4916,87 +4916,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="23"/>
-      <c r="B146" s="6">
-        <v>1862</v>
-      </c>
-      <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="6"/>
-      <c r="F146" s="6"/>
-      <c r="G146" s="6"/>
-      <c r="H146" s="6"/>
-      <c r="I146" s="6"/>
-      <c r="J146" s="6"/>
-      <c r="K146" s="6"/>
-      <c r="L146" s="6"/>
-      <c r="M146" s="6"/>
-      <c r="N146" s="6"/>
-      <c r="O146" s="6"/>
-      <c r="P146" s="6"/>
-      <c r="Q146" s="6"/>
-      <c r="R146" s="6"/>
-      <c r="S146" s="6"/>
-      <c r="T146" s="7"/>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A146" s="22"/>
+      <c r="B146" s="2">
+        <v>5171</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
+      <c r="R146" s="2"/>
+      <c r="S146" s="2"/>
+      <c r="T146" s="5"/>
       <c r="U146">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B147" s="13">
-        <v>2885</v>
-      </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8"/>
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
-      <c r="I147" s="8"/>
-      <c r="J147" s="8"/>
-      <c r="K147" s="8"/>
-      <c r="L147" s="8"/>
-      <c r="M147" s="8"/>
-      <c r="N147" s="8"/>
-      <c r="O147" s="8"/>
-      <c r="P147" s="8"/>
-      <c r="Q147" s="8"/>
-      <c r="R147" s="8"/>
-      <c r="S147" s="8"/>
-      <c r="T147" s="14"/>
+    <row r="147" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="23"/>
+      <c r="B147" s="6">
+        <v>1862</v>
+      </c>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="6"/>
+      <c r="M147" s="6"/>
+      <c r="N147" s="6"/>
+      <c r="O147" s="6"/>
+      <c r="P147" s="6"/>
+      <c r="Q147" s="6"/>
+      <c r="R147" s="6"/>
+      <c r="S147" s="6"/>
+      <c r="T147" s="7"/>
       <c r="U147">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="22"/>
-      <c r="B148" s="12">
-        <v>9931</v>
-      </c>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
-      <c r="O148" s="2"/>
-      <c r="P148" s="2"/>
-      <c r="Q148" s="2"/>
-      <c r="R148" s="2"/>
-      <c r="S148" s="2"/>
-      <c r="T148" s="5"/>
+      <c r="A148" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" s="13">
+        <v>2885</v>
+      </c>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="8"/>
+      <c r="J148" s="8"/>
+      <c r="K148" s="8"/>
+      <c r="L148" s="8"/>
+      <c r="M148" s="8"/>
+      <c r="N148" s="8"/>
+      <c r="O148" s="8"/>
+      <c r="P148" s="8"/>
+      <c r="Q148" s="8"/>
+      <c r="R148" s="8"/>
+      <c r="S148" s="8"/>
+      <c r="T148" s="14"/>
       <c r="U148">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -5005,7 +5005,7 @@
     <row r="149" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="22"/>
       <c r="B149" s="12">
-        <v>9696</v>
+        <v>9931</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
@@ -5033,7 +5033,7 @@
     <row r="150" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="22"/>
       <c r="B150" s="12">
-        <v>1947</v>
+        <v>9696</v>
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
@@ -5058,10 +5058,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="22"/>
-      <c r="B151" s="2">
-        <v>4425</v>
+      <c r="B151" s="12">
+        <v>1947</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
@@ -5089,7 +5089,7 @@
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="22"/>
       <c r="B152" s="2">
-        <v>5683</v>
+        <v>4425</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -5117,7 +5117,7 @@
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" s="22"/>
       <c r="B153" s="2">
-        <v>1223</v>
+        <v>5683</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -5145,7 +5145,7 @@
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="22"/>
       <c r="B154" s="2">
-        <v>8311</v>
+        <v>1223</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
@@ -5173,7 +5173,7 @@
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="22"/>
       <c r="B155" s="2">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -5201,7 +5201,7 @@
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="22"/>
       <c r="B156" s="2">
-        <v>9711</v>
+        <v>3134</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -5229,7 +5229,7 @@
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="22"/>
       <c r="B157" s="2">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -5257,7 +5257,7 @@
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="22"/>
       <c r="B158" s="2">
-        <v>8820</v>
+        <v>3333</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -5285,7 +5285,7 @@
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="22"/>
       <c r="B159" s="2">
-        <v>5694</v>
+        <v>8820</v>
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -5313,7 +5313,7 @@
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="22"/>
       <c r="B160" s="2">
-        <v>6806</v>
+        <v>5694</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
@@ -5341,7 +5341,7 @@
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="22"/>
       <c r="B161" s="2">
-        <v>7369</v>
+        <v>6806</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
@@ -5369,7 +5369,7 @@
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="22"/>
       <c r="B162" s="2">
-        <v>5894</v>
+        <v>7369</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -5397,7 +5397,7 @@
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="22"/>
       <c r="B163" s="2">
-        <v>4515</v>
+        <v>5894</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -5425,7 +5425,7 @@
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" s="22"/>
       <c r="B164" s="2">
-        <v>9774</v>
+        <v>4515</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -5453,7 +5453,7 @@
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="22"/>
       <c r="B165" s="2">
-        <v>3946</v>
+        <v>9774</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -5481,7 +5481,7 @@
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="22"/>
       <c r="B166" s="2">
-        <v>6497</v>
+        <v>3946</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -5509,7 +5509,7 @@
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="22"/>
       <c r="B167" s="2">
-        <v>5648</v>
+        <v>6497</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
@@ -5537,7 +5537,7 @@
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="22"/>
       <c r="B168" s="2">
-        <v>3940</v>
+        <v>5648</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -5565,7 +5565,7 @@
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="22"/>
       <c r="B169" s="2">
-        <v>7290</v>
+        <v>3940</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -5593,7 +5593,7 @@
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="22"/>
       <c r="B170" s="2">
-        <v>7035</v>
+        <v>7290</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -5621,7 +5621,7 @@
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="22"/>
       <c r="B171" s="2">
-        <v>9271</v>
+        <v>7035</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -5649,7 +5649,7 @@
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="22"/>
       <c r="B172" s="2">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -5677,7 +5677,7 @@
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="22"/>
       <c r="B173" s="2">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -5705,7 +5705,7 @@
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="22"/>
       <c r="B174" s="2">
-        <v>3218</v>
+        <v>4497</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -5733,7 +5733,7 @@
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="22"/>
       <c r="B175" s="2">
-        <v>4293</v>
+        <v>3218</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -5761,7 +5761,7 @@
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="22"/>
       <c r="B176" s="2">
-        <v>7703</v>
+        <v>4293</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -5789,7 +5789,7 @@
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="22"/>
       <c r="B177" s="2">
-        <v>5541</v>
+        <v>7703</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
@@ -5814,96 +5814,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="23"/>
-      <c r="B178" s="6">
-        <v>9182</v>
-      </c>
-      <c r="C178" s="6"/>
-      <c r="D178" s="6"/>
-      <c r="E178" s="6"/>
-      <c r="F178" s="6"/>
-      <c r="G178" s="6"/>
-      <c r="H178" s="6"/>
-      <c r="I178" s="6"/>
-      <c r="J178" s="6"/>
-      <c r="K178" s="6"/>
-      <c r="L178" s="6"/>
-      <c r="M178" s="6"/>
-      <c r="N178" s="6"/>
-      <c r="O178" s="6"/>
-      <c r="P178" s="6"/>
-      <c r="Q178" s="6"/>
-      <c r="R178" s="6"/>
-      <c r="S178" s="6"/>
-      <c r="T178" s="7"/>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A178" s="22"/>
+      <c r="B178" s="2">
+        <v>5541</v>
+      </c>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+      <c r="J178" s="2"/>
+      <c r="K178" s="2"/>
+      <c r="L178" s="2"/>
+      <c r="M178" s="2"/>
+      <c r="N178" s="2"/>
+      <c r="O178" s="2"/>
+      <c r="P178" s="2"/>
+      <c r="Q178" s="2"/>
+      <c r="R178" s="2"/>
+      <c r="S178" s="2"/>
+      <c r="T178" s="5"/>
       <c r="U178">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" s="21" t="s">
+    <row r="179" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="23"/>
+      <c r="B179" s="6">
+        <v>9182</v>
+      </c>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+      <c r="J179" s="6"/>
+      <c r="K179" s="6"/>
+      <c r="L179" s="6"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="6"/>
+      <c r="S179" s="6"/>
+      <c r="T179" s="7"/>
+      <c r="U179">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A180" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B179" s="13">
+      <c r="B180" s="13">
         <v>8165</v>
       </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
-      <c r="E179" s="8"/>
-      <c r="F179" s="8"/>
-      <c r="G179" s="8"/>
-      <c r="H179" s="8"/>
-      <c r="I179" s="8"/>
-      <c r="J179" s="8"/>
-      <c r="K179" s="8"/>
-      <c r="L179" s="8"/>
-      <c r="M179" s="8"/>
-      <c r="N179" s="8"/>
-      <c r="O179" s="8"/>
-      <c r="P179" s="8"/>
-      <c r="Q179" s="8"/>
-      <c r="R179" s="8"/>
-      <c r="S179" s="8"/>
-      <c r="T179" s="14"/>
-      <c r="U179">
-        <f t="shared" ref="U179:U196" ca="1" si="5">IF(B179=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="22"/>
-      <c r="B180" s="12">
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+      <c r="E180" s="8"/>
+      <c r="F180" s="8"/>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
+      <c r="I180" s="8"/>
+      <c r="J180" s="8"/>
+      <c r="K180" s="8"/>
+      <c r="L180" s="8"/>
+      <c r="M180" s="8"/>
+      <c r="N180" s="8"/>
+      <c r="O180" s="8"/>
+      <c r="P180" s="8"/>
+      <c r="Q180" s="8"/>
+      <c r="R180" s="8"/>
+      <c r="S180" s="8"/>
+      <c r="T180" s="14"/>
+      <c r="U180">
+        <f t="shared" ref="U180:U197" ca="1" si="5">IF(B180=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="22"/>
+      <c r="B181" s="12">
         <v>9001</v>
-      </c>
-      <c r="C180" s="2"/>
-      <c r="D180" s="2"/>
-      <c r="E180" s="2"/>
-      <c r="F180" s="2"/>
-      <c r="G180" s="2"/>
-      <c r="H180" s="2"/>
-      <c r="I180" s="2"/>
-      <c r="J180" s="2"/>
-      <c r="K180" s="2"/>
-      <c r="L180" s="2"/>
-      <c r="M180" s="2"/>
-      <c r="N180" s="2"/>
-      <c r="O180" s="2"/>
-      <c r="P180" s="2"/>
-      <c r="Q180" s="2"/>
-      <c r="R180" s="2"/>
-      <c r="S180" s="2"/>
-      <c r="T180" s="5"/>
-      <c r="U180">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A181" s="22"/>
-      <c r="B181" s="2">
-        <v>7491</v>
       </c>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
@@ -5931,7 +5931,7 @@
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="22"/>
       <c r="B182" s="2">
-        <v>9531</v>
+        <v>7491</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
@@ -5959,7 +5959,7 @@
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="22"/>
       <c r="B183" s="2">
-        <v>9812</v>
+        <v>9531</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
@@ -5987,7 +5987,7 @@
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="22"/>
       <c r="B184" s="2">
-        <v>9279</v>
+        <v>9812</v>
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
@@ -6015,7 +6015,7 @@
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="22"/>
       <c r="B185" s="2">
-        <v>4845</v>
+        <v>9279</v>
       </c>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
@@ -6043,7 +6043,7 @@
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" s="22"/>
       <c r="B186" s="2">
-        <v>5728</v>
+        <v>4845</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
@@ -6071,7 +6071,7 @@
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="22"/>
       <c r="B187" s="2">
-        <v>7222</v>
+        <v>5728</v>
       </c>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
@@ -6099,7 +6099,7 @@
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" s="22"/>
       <c r="B188" s="2">
-        <v>5923</v>
+        <v>7222</v>
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -6127,7 +6127,7 @@
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="22"/>
       <c r="B189" s="2">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
@@ -6155,7 +6155,7 @@
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="22"/>
       <c r="B190" s="2">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
@@ -6183,7 +6183,7 @@
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="22"/>
       <c r="B191" s="2">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
@@ -6211,7 +6211,7 @@
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="22"/>
       <c r="B192" s="2">
-        <v>9925</v>
+        <v>9116</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -6239,7 +6239,7 @@
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="22"/>
       <c r="B193" s="2">
-        <v>3657</v>
+        <v>9925</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -6267,7 +6267,7 @@
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
       <c r="B194" s="2">
-        <v>6599</v>
+        <v>3657</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
@@ -6293,123 +6293,123 @@
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="26"/>
-      <c r="B195" s="9">
-        <v>1618</v>
-      </c>
-      <c r="C195" s="9"/>
-      <c r="D195" s="9"/>
-      <c r="E195" s="9"/>
-      <c r="F195" s="9"/>
-      <c r="G195" s="9"/>
-      <c r="H195" s="9"/>
-      <c r="I195" s="9"/>
-      <c r="J195" s="9"/>
-      <c r="K195" s="9"/>
-      <c r="L195" s="9"/>
-      <c r="M195" s="9"/>
-      <c r="N195" s="9"/>
-      <c r="O195" s="9"/>
-      <c r="P195" s="9"/>
-      <c r="Q195" s="9"/>
-      <c r="R195" s="9"/>
-      <c r="S195" s="9"/>
-      <c r="T195" s="15"/>
+      <c r="A195" s="22"/>
+      <c r="B195" s="2">
+        <v>6599</v>
+      </c>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+      <c r="E195" s="2"/>
+      <c r="F195" s="2"/>
+      <c r="G195" s="2"/>
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+      <c r="J195" s="2"/>
+      <c r="K195" s="2"/>
+      <c r="L195" s="2"/>
+      <c r="M195" s="2"/>
+      <c r="N195" s="2"/>
+      <c r="O195" s="2"/>
+      <c r="P195" s="2"/>
+      <c r="Q195" s="2"/>
+      <c r="R195" s="2"/>
+      <c r="S195" s="2"/>
+      <c r="T195" s="5"/>
       <c r="U195">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="23"/>
-      <c r="B196" s="6">
-        <v>1703</v>
-      </c>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
-      <c r="G196" s="6"/>
-      <c r="H196" s="6"/>
-      <c r="I196" s="6"/>
-      <c r="J196" s="6"/>
-      <c r="K196" s="6"/>
-      <c r="L196" s="6"/>
-      <c r="M196" s="6"/>
-      <c r="N196" s="6"/>
-      <c r="O196" s="6"/>
-      <c r="P196" s="6"/>
-      <c r="Q196" s="6"/>
-      <c r="R196" s="6"/>
-      <c r="S196" s="6"/>
-      <c r="T196" s="7"/>
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A196" s="30"/>
+      <c r="B196" s="9">
+        <v>1618</v>
+      </c>
+      <c r="C196" s="9"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="9"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="9"/>
+      <c r="K196" s="9"/>
+      <c r="L196" s="9"/>
+      <c r="M196" s="9"/>
+      <c r="N196" s="9"/>
+      <c r="O196" s="9"/>
+      <c r="P196" s="9"/>
+      <c r="Q196" s="9"/>
+      <c r="R196" s="9"/>
+      <c r="S196" s="9"/>
+      <c r="T196" s="15"/>
       <c r="U196">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="27" t="s">
+    <row r="197" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="23"/>
+      <c r="B197" s="6">
+        <v>1703</v>
+      </c>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="6"/>
+      <c r="I197" s="6"/>
+      <c r="J197" s="6"/>
+      <c r="K197" s="6"/>
+      <c r="L197" s="6"/>
+      <c r="M197" s="6"/>
+      <c r="N197" s="6"/>
+      <c r="O197" s="6"/>
+      <c r="P197" s="6"/>
+      <c r="Q197" s="6"/>
+      <c r="R197" s="6"/>
+      <c r="S197" s="6"/>
+      <c r="T197" s="7"/>
+      <c r="U197">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A198" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B197" s="8">
+      <c r="B198" s="8">
         <v>6175</v>
       </c>
-      <c r="C197" s="8"/>
-      <c r="D197" s="8"/>
-      <c r="E197" s="8"/>
-      <c r="F197" s="8"/>
-      <c r="G197" s="8"/>
-      <c r="H197" s="8"/>
-      <c r="I197" s="8"/>
-      <c r="J197" s="8"/>
-      <c r="K197" s="8"/>
-      <c r="L197" s="8"/>
-      <c r="M197" s="8"/>
-      <c r="N197" s="8"/>
-      <c r="O197" s="8"/>
-      <c r="P197" s="8"/>
-      <c r="Q197" s="8"/>
-      <c r="R197" s="8"/>
-      <c r="S197" s="8"/>
-      <c r="T197" s="14"/>
-      <c r="U197">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="28"/>
-      <c r="B198" s="2">
-        <v>4488</v>
-      </c>
-      <c r="C198" s="2"/>
-      <c r="D198" s="2"/>
-      <c r="E198" s="2"/>
-      <c r="F198" s="2"/>
-      <c r="G198" s="2"/>
-      <c r="H198" s="2"/>
-      <c r="I198" s="2"/>
-      <c r="J198" s="2"/>
-      <c r="K198" s="2"/>
-      <c r="L198" s="2"/>
-      <c r="M198" s="2"/>
-      <c r="N198" s="2"/>
-      <c r="O198" s="2"/>
-      <c r="P198" s="2"/>
-      <c r="Q198" s="2"/>
-      <c r="R198" s="2"/>
-      <c r="S198" s="2"/>
-      <c r="T198" s="5"/>
+      <c r="C198" s="8"/>
+      <c r="D198" s="8"/>
+      <c r="E198" s="8"/>
+      <c r="F198" s="8"/>
+      <c r="G198" s="8"/>
+      <c r="H198" s="8"/>
+      <c r="I198" s="8"/>
+      <c r="J198" s="8"/>
+      <c r="K198" s="8"/>
+      <c r="L198" s="8"/>
+      <c r="M198" s="8"/>
+      <c r="N198" s="8"/>
+      <c r="O198" s="8"/>
+      <c r="P198" s="8"/>
+      <c r="Q198" s="8"/>
+      <c r="R198" s="8"/>
+      <c r="S198" s="8"/>
+      <c r="T198" s="14"/>
       <c r="U198">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="28"/>
+      <c r="A199" s="34"/>
       <c r="B199" s="2">
-        <v>4954</v>
+        <v>4488</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
@@ -6435,9 +6435,9 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="28"/>
+      <c r="A200" s="34"/>
       <c r="B200" s="2">
-        <v>4642</v>
+        <v>4954</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
@@ -6463,9 +6463,9 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="28"/>
+      <c r="A201" s="34"/>
       <c r="B201" s="2">
-        <v>5537</v>
+        <v>4642</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
@@ -6491,9 +6491,9 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="28"/>
+      <c r="A202" s="34"/>
       <c r="B202" s="2">
-        <v>5847</v>
+        <v>5537</v>
       </c>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
@@ -6519,9 +6519,9 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="28"/>
+      <c r="A203" s="34"/>
       <c r="B203" s="2">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
@@ -6547,9 +6547,9 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="28"/>
+      <c r="A204" s="34"/>
       <c r="B204" s="2">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
@@ -6570,14 +6570,14 @@
       <c r="S204" s="2"/>
       <c r="T204" s="5"/>
       <c r="U204">
-        <f t="shared" ref="U204:U278" ca="1" si="6">IF(B204=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="28"/>
+      <c r="A205" s="34"/>
       <c r="B205" s="2">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
@@ -6598,14 +6598,14 @@
       <c r="S205" s="2"/>
       <c r="T205" s="5"/>
       <c r="U205">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="U205:U279" ca="1" si="6">IF(B205=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="28"/>
+      <c r="A206" s="34"/>
       <c r="B206" s="2">
-        <v>3226</v>
+        <v>6861</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -6631,9 +6631,9 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="28"/>
+      <c r="A207" s="34"/>
       <c r="B207" s="2">
-        <v>4372</v>
+        <v>3226</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6659,9 +6659,9 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="28"/>
+      <c r="A208" s="34"/>
       <c r="B208" s="2">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6687,9 +6687,9 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="28"/>
+      <c r="A209" s="34"/>
       <c r="B209" s="2">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6715,9 +6715,9 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="28"/>
+      <c r="A210" s="34"/>
       <c r="B210" s="2">
-        <v>9417</v>
+        <v>1668</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -6743,9 +6743,9 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="28"/>
+      <c r="A211" s="34"/>
       <c r="B211" s="2">
-        <v>3148</v>
+        <v>9417</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -6771,9 +6771,9 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="28"/>
+      <c r="A212" s="34"/>
       <c r="B212" s="2">
-        <v>2137</v>
+        <v>3148</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -6798,96 +6798,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="29"/>
-      <c r="B213" s="6">
-        <v>5621</v>
-      </c>
-      <c r="C213" s="6"/>
-      <c r="D213" s="6"/>
-      <c r="E213" s="6"/>
-      <c r="F213" s="6"/>
-      <c r="G213" s="6"/>
-      <c r="H213" s="6"/>
-      <c r="I213" s="6"/>
-      <c r="J213" s="6"/>
-      <c r="K213" s="6"/>
-      <c r="L213" s="6"/>
-      <c r="M213" s="6"/>
-      <c r="N213" s="6"/>
-      <c r="O213" s="6"/>
-      <c r="P213" s="6"/>
-      <c r="Q213" s="6"/>
-      <c r="R213" s="6"/>
-      <c r="S213" s="6"/>
-      <c r="T213" s="7"/>
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A213" s="34"/>
+      <c r="B213" s="2">
+        <v>2137</v>
+      </c>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+      <c r="J213" s="2"/>
+      <c r="K213" s="2"/>
+      <c r="L213" s="2"/>
+      <c r="M213" s="2"/>
+      <c r="N213" s="2"/>
+      <c r="O213" s="2"/>
+      <c r="P213" s="2"/>
+      <c r="Q213" s="2"/>
+      <c r="R213" s="2"/>
+      <c r="S213" s="2"/>
+      <c r="T213" s="5"/>
       <c r="U213">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B214" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C214" s="8"/>
-      <c r="D214" s="8"/>
-      <c r="E214" s="8"/>
-      <c r="F214" s="8"/>
-      <c r="G214" s="8"/>
-      <c r="H214" s="8"/>
-      <c r="I214" s="8"/>
-      <c r="J214" s="8"/>
-      <c r="K214" s="8"/>
-      <c r="L214" s="8"/>
-      <c r="M214" s="8"/>
-      <c r="N214" s="8"/>
-      <c r="O214" s="8"/>
-      <c r="P214" s="8"/>
-      <c r="Q214" s="8"/>
-      <c r="R214" s="8"/>
-      <c r="S214" s="8"/>
-      <c r="T214" s="14"/>
+    <row r="214" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="35"/>
+      <c r="B214" s="6">
+        <v>5621</v>
+      </c>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6"/>
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
+      <c r="I214" s="6"/>
+      <c r="J214" s="6"/>
+      <c r="K214" s="6"/>
+      <c r="L214" s="6"/>
+      <c r="M214" s="6"/>
+      <c r="N214" s="6"/>
+      <c r="O214" s="6"/>
+      <c r="P214" s="6"/>
+      <c r="Q214" s="6"/>
+      <c r="R214" s="6"/>
+      <c r="S214" s="6"/>
+      <c r="T214" s="7"/>
       <c r="U214">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="22"/>
-      <c r="B215" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="2"/>
-      <c r="J215" s="2"/>
-      <c r="K215" s="2"/>
-      <c r="L215" s="2"/>
-      <c r="M215" s="2"/>
-      <c r="N215" s="2"/>
-      <c r="O215" s="2"/>
-      <c r="P215" s="2"/>
-      <c r="Q215" s="2"/>
-      <c r="R215" s="2"/>
-      <c r="S215" s="2"/>
-      <c r="T215" s="5"/>
+      <c r="A215" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B215" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C215" s="8"/>
+      <c r="D215" s="8"/>
+      <c r="E215" s="8"/>
+      <c r="F215" s="8"/>
+      <c r="G215" s="8"/>
+      <c r="H215" s="8"/>
+      <c r="I215" s="8"/>
+      <c r="J215" s="8"/>
+      <c r="K215" s="8"/>
+      <c r="L215" s="8"/>
+      <c r="M215" s="8"/>
+      <c r="N215" s="8"/>
+      <c r="O215" s="8"/>
+      <c r="P215" s="8"/>
+      <c r="Q215" s="8"/>
+      <c r="R215" s="8"/>
+      <c r="S215" s="8"/>
+      <c r="T215" s="14"/>
       <c r="U215">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="22"/>
       <c r="B216" s="2">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -6915,7 +6915,7 @@
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="22"/>
       <c r="B217" s="2">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6943,7 +6943,7 @@
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="22"/>
       <c r="B218" s="2">
-        <v>6409</v>
+        <v>7060</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6971,7 +6971,7 @@
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="22"/>
       <c r="B219" s="2">
-        <v>2386</v>
+        <v>6409</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -6996,10 +6996,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="22"/>
-      <c r="B220" s="6">
-        <v>7372</v>
+      <c r="B220" s="2">
+        <v>2386</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -7019,11 +7019,15 @@
       <c r="R220" s="2"/>
       <c r="S220" s="2"/>
       <c r="T220" s="5"/>
-    </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U220">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="22"/>
-      <c r="B221" s="2">
-        <v>9159</v>
+      <c r="B221" s="6">
+        <v>7372</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
@@ -7043,15 +7047,11 @@
       <c r="R221" s="2"/>
       <c r="S221" s="2"/>
       <c r="T221" s="5"/>
-      <c r="U221">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="22"/>
       <c r="B222" s="2">
-        <v>5309</v>
+        <v>9159</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -7079,7 +7079,7 @@
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="22"/>
       <c r="B223" s="2">
-        <v>3290</v>
+        <v>5309</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
@@ -7107,7 +7107,7 @@
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="22"/>
       <c r="B224" s="2">
-        <v>5345</v>
+        <v>3290</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7132,87 +7132,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="23"/>
-      <c r="B225" s="6">
-        <v>6812</v>
-      </c>
-      <c r="C225" s="6"/>
-      <c r="D225" s="6"/>
-      <c r="E225" s="6"/>
-      <c r="F225" s="6"/>
-      <c r="G225" s="6"/>
-      <c r="H225" s="6"/>
-      <c r="I225" s="6"/>
-      <c r="J225" s="6"/>
-      <c r="K225" s="6"/>
-      <c r="L225" s="6"/>
-      <c r="M225" s="6"/>
-      <c r="N225" s="6"/>
-      <c r="O225" s="6"/>
-      <c r="P225" s="6"/>
-      <c r="Q225" s="6"/>
-      <c r="R225" s="6"/>
-      <c r="S225" s="6"/>
-      <c r="T225" s="7"/>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A225" s="22"/>
+      <c r="B225" s="2">
+        <v>5345</v>
+      </c>
+      <c r="C225" s="2"/>
+      <c r="D225" s="2"/>
+      <c r="E225" s="2"/>
+      <c r="F225" s="2"/>
+      <c r="G225" s="2"/>
+      <c r="H225" s="2"/>
+      <c r="I225" s="2"/>
+      <c r="J225" s="2"/>
+      <c r="K225" s="2"/>
+      <c r="L225" s="2"/>
+      <c r="M225" s="2"/>
+      <c r="N225" s="2"/>
+      <c r="O225" s="2"/>
+      <c r="P225" s="2"/>
+      <c r="Q225" s="2"/>
+      <c r="R225" s="2"/>
+      <c r="S225" s="2"/>
+      <c r="T225" s="5"/>
       <c r="U225">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B226" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C226" s="8"/>
-      <c r="D226" s="8"/>
-      <c r="E226" s="8"/>
-      <c r="F226" s="8"/>
-      <c r="G226" s="8"/>
-      <c r="H226" s="8"/>
-      <c r="I226" s="8"/>
-      <c r="J226" s="8"/>
-      <c r="K226" s="8"/>
-      <c r="L226" s="8"/>
-      <c r="M226" s="8"/>
-      <c r="N226" s="8"/>
-      <c r="O226" s="8"/>
-      <c r="P226" s="8"/>
-      <c r="Q226" s="8"/>
-      <c r="R226" s="8"/>
-      <c r="S226" s="8"/>
-      <c r="T226" s="14"/>
+    <row r="226" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="23"/>
+      <c r="B226" s="6">
+        <v>6812</v>
+      </c>
+      <c r="C226" s="6"/>
+      <c r="D226" s="6"/>
+      <c r="E226" s="6"/>
+      <c r="F226" s="6"/>
+      <c r="G226" s="6"/>
+      <c r="H226" s="6"/>
+      <c r="I226" s="6"/>
+      <c r="J226" s="6"/>
+      <c r="K226" s="6"/>
+      <c r="L226" s="6"/>
+      <c r="M226" s="6"/>
+      <c r="N226" s="6"/>
+      <c r="O226" s="6"/>
+      <c r="P226" s="6"/>
+      <c r="Q226" s="6"/>
+      <c r="R226" s="6"/>
+      <c r="S226" s="6"/>
+      <c r="T226" s="7"/>
       <c r="U226">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="22"/>
-      <c r="B227" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="2"/>
-      <c r="F227" s="2"/>
-      <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
-      <c r="I227" s="2"/>
-      <c r="J227" s="2"/>
-      <c r="K227" s="2"/>
-      <c r="L227" s="2"/>
-      <c r="M227" s="2"/>
-      <c r="N227" s="2"/>
-      <c r="O227" s="2"/>
-      <c r="P227" s="2"/>
-      <c r="Q227" s="2"/>
-      <c r="R227" s="2"/>
-      <c r="S227" s="2"/>
-      <c r="T227" s="5"/>
+      <c r="A227" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B227" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C227" s="8"/>
+      <c r="D227" s="8"/>
+      <c r="E227" s="8"/>
+      <c r="F227" s="8"/>
+      <c r="G227" s="8"/>
+      <c r="H227" s="8"/>
+      <c r="I227" s="8"/>
+      <c r="J227" s="8"/>
+      <c r="K227" s="8"/>
+      <c r="L227" s="8"/>
+      <c r="M227" s="8"/>
+      <c r="N227" s="8"/>
+      <c r="O227" s="8"/>
+      <c r="P227" s="8"/>
+      <c r="Q227" s="8"/>
+      <c r="R227" s="8"/>
+      <c r="S227" s="8"/>
+      <c r="T227" s="14"/>
       <c r="U227">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7221,7 +7221,7 @@
     <row r="228" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="22"/>
       <c r="B228" s="12">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -7246,10 +7246,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="22"/>
-      <c r="B229" s="19">
-        <v>8861</v>
+      <c r="B229" s="12">
+        <v>9062</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -7276,8 +7276,8 @@
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="22"/>
-      <c r="B230" s="2">
-        <v>5164</v>
+      <c r="B230" s="19">
+        <v>8861</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
@@ -7305,7 +7305,7 @@
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="22"/>
       <c r="B231" s="2">
-        <v>2354</v>
+        <v>5164</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
@@ -7333,7 +7333,7 @@
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="22"/>
       <c r="B232" s="2">
-        <v>2030</v>
+        <v>2354</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -7358,87 +7358,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="23"/>
-      <c r="B233" s="6">
-        <v>7649</v>
-      </c>
-      <c r="C233" s="6"/>
-      <c r="D233" s="6"/>
-      <c r="E233" s="6"/>
-      <c r="F233" s="6"/>
-      <c r="G233" s="6"/>
-      <c r="H233" s="6"/>
-      <c r="I233" s="6"/>
-      <c r="J233" s="6"/>
-      <c r="K233" s="6"/>
-      <c r="L233" s="6"/>
-      <c r="M233" s="6"/>
-      <c r="N233" s="6"/>
-      <c r="O233" s="6"/>
-      <c r="P233" s="6"/>
-      <c r="Q233" s="6"/>
-      <c r="R233" s="6"/>
-      <c r="S233" s="6"/>
-      <c r="T233" s="7"/>
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A233" s="22"/>
+      <c r="B233" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+      <c r="L233" s="2"/>
+      <c r="M233" s="2"/>
+      <c r="N233" s="2"/>
+      <c r="O233" s="2"/>
+      <c r="P233" s="2"/>
+      <c r="Q233" s="2"/>
+      <c r="R233" s="2"/>
+      <c r="S233" s="2"/>
+      <c r="T233" s="5"/>
       <c r="U233">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A234" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C234" s="8"/>
-      <c r="D234" s="8"/>
-      <c r="E234" s="8"/>
-      <c r="F234" s="8"/>
-      <c r="G234" s="8"/>
-      <c r="H234" s="8"/>
-      <c r="I234" s="8"/>
-      <c r="J234" s="8"/>
-      <c r="K234" s="8"/>
-      <c r="L234" s="8"/>
-      <c r="M234" s="8"/>
-      <c r="N234" s="8"/>
-      <c r="O234" s="8"/>
-      <c r="P234" s="8"/>
-      <c r="Q234" s="8"/>
-      <c r="R234" s="8"/>
-      <c r="S234" s="8"/>
-      <c r="T234" s="14"/>
+    <row r="234" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="23"/>
+      <c r="B234" s="6">
+        <v>7649</v>
+      </c>
+      <c r="C234" s="6"/>
+      <c r="D234" s="6"/>
+      <c r="E234" s="6"/>
+      <c r="F234" s="6"/>
+      <c r="G234" s="6"/>
+      <c r="H234" s="6"/>
+      <c r="I234" s="6"/>
+      <c r="J234" s="6"/>
+      <c r="K234" s="6"/>
+      <c r="L234" s="6"/>
+      <c r="M234" s="6"/>
+      <c r="N234" s="6"/>
+      <c r="O234" s="6"/>
+      <c r="P234" s="6"/>
+      <c r="Q234" s="6"/>
+      <c r="R234" s="6"/>
+      <c r="S234" s="6"/>
+      <c r="T234" s="7"/>
       <c r="U234">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A235" s="22"/>
-      <c r="B235" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C235" s="2"/>
-      <c r="D235" s="2"/>
-      <c r="E235" s="2"/>
-      <c r="F235" s="2"/>
-      <c r="G235" s="2"/>
-      <c r="H235" s="2"/>
-      <c r="I235" s="2"/>
-      <c r="J235" s="2"/>
-      <c r="K235" s="2"/>
-      <c r="L235" s="2"/>
-      <c r="M235" s="2"/>
-      <c r="N235" s="2"/>
-      <c r="O235" s="2"/>
-      <c r="P235" s="2"/>
-      <c r="Q235" s="2"/>
-      <c r="R235" s="2"/>
-      <c r="S235" s="2"/>
-      <c r="T235" s="5"/>
+      <c r="A235" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B235" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C235" s="8"/>
+      <c r="D235" s="8"/>
+      <c r="E235" s="8"/>
+      <c r="F235" s="8"/>
+      <c r="G235" s="8"/>
+      <c r="H235" s="8"/>
+      <c r="I235" s="8"/>
+      <c r="J235" s="8"/>
+      <c r="K235" s="8"/>
+      <c r="L235" s="8"/>
+      <c r="M235" s="8"/>
+      <c r="N235" s="8"/>
+      <c r="O235" s="8"/>
+      <c r="P235" s="8"/>
+      <c r="Q235" s="8"/>
+      <c r="R235" s="8"/>
+      <c r="S235" s="8"/>
+      <c r="T235" s="14"/>
       <c r="U235">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7447,7 +7447,7 @@
     <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236" s="22"/>
       <c r="B236" s="2">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
@@ -7475,7 +7475,7 @@
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" s="22"/>
       <c r="B237" s="2">
-        <v>6882</v>
+        <v>6732</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
@@ -7503,7 +7503,7 @@
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="22"/>
       <c r="B238" s="2">
-        <v>1212</v>
+        <v>6882</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -7531,7 +7531,7 @@
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239" s="22"/>
       <c r="B239" s="2">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -7559,7 +7559,7 @@
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="22"/>
       <c r="B240" s="2">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
@@ -7584,87 +7584,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="23"/>
-      <c r="B241" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="6"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="6"/>
-      <c r="J241" s="6"/>
-      <c r="K241" s="6"/>
-      <c r="L241" s="6"/>
-      <c r="M241" s="6"/>
-      <c r="N241" s="6"/>
-      <c r="O241" s="6"/>
-      <c r="P241" s="6"/>
-      <c r="Q241" s="6"/>
-      <c r="R241" s="6"/>
-      <c r="S241" s="6"/>
-      <c r="T241" s="7"/>
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A241" s="22"/>
+      <c r="B241" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="2"/>
+      <c r="N241" s="2"/>
+      <c r="O241" s="2"/>
+      <c r="P241" s="2"/>
+      <c r="Q241" s="2"/>
+      <c r="R241" s="2"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="5"/>
       <c r="U241">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B242" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8"/>
-      <c r="H242" s="8"/>
-      <c r="I242" s="8"/>
-      <c r="J242" s="8"/>
-      <c r="K242" s="8"/>
-      <c r="L242" s="8"/>
-      <c r="M242" s="8"/>
-      <c r="N242" s="8"/>
-      <c r="O242" s="8"/>
-      <c r="P242" s="8"/>
-      <c r="Q242" s="8"/>
-      <c r="R242" s="8"/>
-      <c r="S242" s="8"/>
-      <c r="T242" s="14"/>
+    <row r="242" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="23"/>
+      <c r="B242" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C242" s="6"/>
+      <c r="D242" s="6"/>
+      <c r="E242" s="6"/>
+      <c r="F242" s="6"/>
+      <c r="G242" s="6"/>
+      <c r="H242" s="6"/>
+      <c r="I242" s="6"/>
+      <c r="J242" s="6"/>
+      <c r="K242" s="6"/>
+      <c r="L242" s="6"/>
+      <c r="M242" s="6"/>
+      <c r="N242" s="6"/>
+      <c r="O242" s="6"/>
+      <c r="P242" s="6"/>
+      <c r="Q242" s="6"/>
+      <c r="R242" s="6"/>
+      <c r="S242" s="6"/>
+      <c r="T242" s="7"/>
       <c r="U242">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="22"/>
-      <c r="B243" s="2">
-        <v>8403</v>
-      </c>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
-      <c r="G243" s="2"/>
-      <c r="H243" s="2"/>
-      <c r="I243" s="2"/>
-      <c r="J243" s="2"/>
-      <c r="K243" s="2"/>
-      <c r="L243" s="2"/>
-      <c r="M243" s="2"/>
-      <c r="N243" s="2"/>
-      <c r="O243" s="2"/>
-      <c r="P243" s="2"/>
-      <c r="Q243" s="2"/>
-      <c r="R243" s="2"/>
-      <c r="S243" s="2"/>
-      <c r="T243" s="5"/>
+    <row r="243" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A243" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B243" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C243" s="8"/>
+      <c r="D243" s="8"/>
+      <c r="E243" s="8"/>
+      <c r="F243" s="8"/>
+      <c r="G243" s="8"/>
+      <c r="H243" s="8"/>
+      <c r="I243" s="8"/>
+      <c r="J243" s="8"/>
+      <c r="K243" s="8"/>
+      <c r="L243" s="8"/>
+      <c r="M243" s="8"/>
+      <c r="N243" s="8"/>
+      <c r="O243" s="8"/>
+      <c r="P243" s="8"/>
+      <c r="Q243" s="8"/>
+      <c r="R243" s="8"/>
+      <c r="S243" s="8"/>
+      <c r="T243" s="14"/>
       <c r="U243">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7673,7 +7673,7 @@
     <row r="244" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A244" s="22"/>
       <c r="B244" s="2">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
@@ -7701,7 +7701,7 @@
     <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245" s="22"/>
       <c r="B245" s="2">
-        <v>2092</v>
+        <v>3185</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7729,7 +7729,7 @@
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246" s="22"/>
       <c r="B246" s="2">
-        <v>9914</v>
+        <v>2092</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7757,7 +7757,7 @@
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247" s="22"/>
       <c r="B247" s="2">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7785,7 +7785,7 @@
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="22"/>
       <c r="B248" s="2">
-        <v>6037</v>
+        <v>6011</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7813,7 +7813,7 @@
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" s="22"/>
       <c r="B249" s="2">
-        <v>2809</v>
+        <v>6037</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -7841,7 +7841,7 @@
     <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" s="22"/>
       <c r="B250" s="2">
-        <v>7297</v>
+        <v>2809</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -7869,7 +7869,7 @@
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" s="22"/>
       <c r="B251" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7897,7 +7897,7 @@
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" s="22"/>
       <c r="B252" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7925,7 +7925,7 @@
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="22"/>
       <c r="B253" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7953,7 +7953,7 @@
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="22"/>
       <c r="B254" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7981,7 +7981,7 @@
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="22"/>
       <c r="B255" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8009,7 +8009,7 @@
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="22"/>
       <c r="B256" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8037,7 +8037,7 @@
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="22"/>
       <c r="B257" s="2">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8065,7 +8065,7 @@
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="22"/>
       <c r="B258" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8093,7 +8093,7 @@
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="22"/>
       <c r="B259" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8121,7 +8121,7 @@
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" s="22"/>
       <c r="B260" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8149,7 +8149,7 @@
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="22"/>
       <c r="B261" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8177,7 +8177,7 @@
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="22"/>
       <c r="B262" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8205,7 +8205,7 @@
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="22"/>
       <c r="B263" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8233,7 +8233,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="22"/>
       <c r="B264" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8261,7 +8261,7 @@
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="22"/>
       <c r="B265" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8289,7 +8289,7 @@
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="22"/>
       <c r="B266" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8317,7 +8317,7 @@
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="22"/>
       <c r="B267" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8342,87 +8342,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="23"/>
-      <c r="B268" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C268" s="6"/>
-      <c r="D268" s="6"/>
-      <c r="E268" s="6"/>
-      <c r="F268" s="6"/>
-      <c r="G268" s="6"/>
-      <c r="H268" s="6"/>
-      <c r="I268" s="6"/>
-      <c r="J268" s="6"/>
-      <c r="K268" s="6"/>
-      <c r="L268" s="6"/>
-      <c r="M268" s="6"/>
-      <c r="N268" s="6"/>
-      <c r="O268" s="6"/>
-      <c r="P268" s="6"/>
-      <c r="Q268" s="6"/>
-      <c r="R268" s="6"/>
-      <c r="S268" s="6"/>
-      <c r="T268" s="7"/>
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A268" s="22"/>
+      <c r="B268" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C268" s="2"/>
+      <c r="D268" s="2"/>
+      <c r="E268" s="2"/>
+      <c r="F268" s="2"/>
+      <c r="G268" s="2"/>
+      <c r="H268" s="2"/>
+      <c r="I268" s="2"/>
+      <c r="J268" s="2"/>
+      <c r="K268" s="2"/>
+      <c r="L268" s="2"/>
+      <c r="M268" s="2"/>
+      <c r="N268" s="2"/>
+      <c r="O268" s="2"/>
+      <c r="P268" s="2"/>
+      <c r="Q268" s="2"/>
+      <c r="R268" s="2"/>
+      <c r="S268" s="2"/>
+      <c r="T268" s="5"/>
       <c r="U268">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B269" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C269" s="8"/>
-      <c r="D269" s="8"/>
-      <c r="E269" s="8"/>
-      <c r="F269" s="8"/>
-      <c r="G269" s="8"/>
-      <c r="H269" s="8"/>
-      <c r="I269" s="8"/>
-      <c r="J269" s="8"/>
-      <c r="K269" s="8"/>
-      <c r="L269" s="8"/>
-      <c r="M269" s="8"/>
-      <c r="N269" s="8"/>
-      <c r="O269" s="8"/>
-      <c r="P269" s="8"/>
-      <c r="Q269" s="8"/>
-      <c r="R269" s="8"/>
-      <c r="S269" s="8"/>
-      <c r="T269" s="14"/>
+    <row r="269" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="23"/>
+      <c r="B269" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C269" s="6"/>
+      <c r="D269" s="6"/>
+      <c r="E269" s="6"/>
+      <c r="F269" s="6"/>
+      <c r="G269" s="6"/>
+      <c r="H269" s="6"/>
+      <c r="I269" s="6"/>
+      <c r="J269" s="6"/>
+      <c r="K269" s="6"/>
+      <c r="L269" s="6"/>
+      <c r="M269" s="6"/>
+      <c r="N269" s="6"/>
+      <c r="O269" s="6"/>
+      <c r="P269" s="6"/>
+      <c r="Q269" s="6"/>
+      <c r="R269" s="6"/>
+      <c r="S269" s="6"/>
+      <c r="T269" s="7"/>
       <c r="U269">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="22"/>
-      <c r="B270" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C270" s="2"/>
-      <c r="D270" s="2"/>
-      <c r="E270" s="2"/>
-      <c r="F270" s="2"/>
-      <c r="G270" s="2"/>
-      <c r="H270" s="2"/>
-      <c r="I270" s="2"/>
-      <c r="J270" s="2"/>
-      <c r="K270" s="2"/>
-      <c r="L270" s="2"/>
-      <c r="M270" s="2"/>
-      <c r="N270" s="2"/>
-      <c r="O270" s="2"/>
-      <c r="P270" s="2"/>
-      <c r="Q270" s="2"/>
-      <c r="R270" s="2"/>
-      <c r="S270" s="2"/>
-      <c r="T270" s="5"/>
+      <c r="A270" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B270" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C270" s="8"/>
+      <c r="D270" s="8"/>
+      <c r="E270" s="8"/>
+      <c r="F270" s="8"/>
+      <c r="G270" s="8"/>
+      <c r="H270" s="8"/>
+      <c r="I270" s="8"/>
+      <c r="J270" s="8"/>
+      <c r="K270" s="8"/>
+      <c r="L270" s="8"/>
+      <c r="M270" s="8"/>
+      <c r="N270" s="8"/>
+      <c r="O270" s="8"/>
+      <c r="P270" s="8"/>
+      <c r="Q270" s="8"/>
+      <c r="R270" s="8"/>
+      <c r="S270" s="8"/>
+      <c r="T270" s="14"/>
       <c r="U270">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8431,7 +8431,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="22"/>
       <c r="B271" s="2">
-        <v>9990</v>
+        <v>5087</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8459,7 +8459,7 @@
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="22"/>
       <c r="B272" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8487,7 +8487,7 @@
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" s="22"/>
       <c r="B273" s="2">
-        <v>9924</v>
+        <v>7738</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8513,37 +8513,37 @@
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="26"/>
-      <c r="B274" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C274" s="9"/>
-      <c r="D274" s="9"/>
-      <c r="E274" s="9"/>
-      <c r="F274" s="9"/>
-      <c r="G274" s="9"/>
-      <c r="H274" s="9"/>
-      <c r="I274" s="9"/>
-      <c r="J274" s="9"/>
-      <c r="K274" s="9"/>
-      <c r="L274" s="9"/>
-      <c r="M274" s="9"/>
-      <c r="N274" s="9"/>
-      <c r="O274" s="9"/>
-      <c r="P274" s="9"/>
-      <c r="Q274" s="9"/>
-      <c r="R274" s="9"/>
-      <c r="S274" s="9"/>
-      <c r="T274" s="15"/>
+      <c r="A274" s="22"/>
+      <c r="B274" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C274" s="2"/>
+      <c r="D274" s="2"/>
+      <c r="E274" s="2"/>
+      <c r="F274" s="2"/>
+      <c r="G274" s="2"/>
+      <c r="H274" s="2"/>
+      <c r="I274" s="2"/>
+      <c r="J274" s="2"/>
+      <c r="K274" s="2"/>
+      <c r="L274" s="2"/>
+      <c r="M274" s="2"/>
+      <c r="N274" s="2"/>
+      <c r="O274" s="2"/>
+      <c r="P274" s="2"/>
+      <c r="Q274" s="2"/>
+      <c r="R274" s="2"/>
+      <c r="S274" s="2"/>
+      <c r="T274" s="5"/>
       <c r="U274">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="26"/>
+      <c r="A275" s="30"/>
       <c r="B275" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C275" s="9"/>
       <c r="D275" s="9"/>
@@ -8569,9 +8569,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="26"/>
+      <c r="A276" s="30"/>
       <c r="B276" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C276" s="9"/>
       <c r="D276" s="9"/>
@@ -8597,9 +8597,9 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="26"/>
+      <c r="A277" s="30"/>
       <c r="B277" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C277" s="9"/>
       <c r="D277" s="9"/>
@@ -8625,9 +8625,9 @@
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A278" s="26"/>
+      <c r="A278" s="30"/>
       <c r="B278" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C278" s="9"/>
       <c r="D278" s="9"/>
@@ -8652,87 +8652,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="23"/>
-      <c r="B279" s="6">
+    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A279" s="30"/>
+      <c r="B279" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C279" s="9"/>
+      <c r="D279" s="9"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
+      <c r="G279" s="9"/>
+      <c r="H279" s="9"/>
+      <c r="I279" s="9"/>
+      <c r="J279" s="9"/>
+      <c r="K279" s="9"/>
+      <c r="L279" s="9"/>
+      <c r="M279" s="9"/>
+      <c r="N279" s="9"/>
+      <c r="O279" s="9"/>
+      <c r="P279" s="9"/>
+      <c r="Q279" s="9"/>
+      <c r="R279" s="9"/>
+      <c r="S279" s="9"/>
+      <c r="T279" s="15"/>
+      <c r="U279">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A280" s="23"/>
+      <c r="B280" s="6">
         <v>6876</v>
       </c>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-      <c r="E279" s="6"/>
-      <c r="F279" s="6"/>
-      <c r="G279" s="6"/>
-      <c r="H279" s="6"/>
-      <c r="I279" s="6"/>
-      <c r="J279" s="6"/>
-      <c r="K279" s="6"/>
-      <c r="L279" s="6"/>
-      <c r="M279" s="6"/>
-      <c r="N279" s="6"/>
-      <c r="O279" s="6"/>
-      <c r="P279" s="6"/>
-      <c r="Q279" s="6"/>
-      <c r="R279" s="6"/>
-      <c r="S279" s="6"/>
-      <c r="T279" s="7"/>
-      <c r="U279">
-        <f t="shared" ref="U279:U342" ca="1" si="7">IF(B279=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="21" t="s">
+      <c r="C280" s="6"/>
+      <c r="D280" s="6"/>
+      <c r="E280" s="6"/>
+      <c r="F280" s="6"/>
+      <c r="G280" s="6"/>
+      <c r="H280" s="6"/>
+      <c r="I280" s="6"/>
+      <c r="J280" s="6"/>
+      <c r="K280" s="6"/>
+      <c r="L280" s="6"/>
+      <c r="M280" s="6"/>
+      <c r="N280" s="6"/>
+      <c r="O280" s="6"/>
+      <c r="P280" s="6"/>
+      <c r="Q280" s="6"/>
+      <c r="R280" s="6"/>
+      <c r="S280" s="6"/>
+      <c r="T280" s="7"/>
+      <c r="U280">
+        <f t="shared" ref="U280:U343" ca="1" si="7">IF(B280=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A281" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B280" s="8">
+      <c r="B281" s="8">
         <v>4304</v>
       </c>
-      <c r="C280" s="8"/>
-      <c r="D280" s="8"/>
-      <c r="E280" s="8"/>
-      <c r="F280" s="8"/>
-      <c r="G280" s="8"/>
-      <c r="H280" s="8"/>
-      <c r="I280" s="8"/>
-      <c r="J280" s="8"/>
-      <c r="K280" s="8"/>
-      <c r="L280" s="8"/>
-      <c r="M280" s="8"/>
-      <c r="N280" s="8"/>
-      <c r="O280" s="8"/>
-      <c r="P280" s="8"/>
-      <c r="Q280" s="8"/>
-      <c r="R280" s="8"/>
-      <c r="S280" s="8"/>
-      <c r="T280" s="14"/>
-      <c r="U280">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="22"/>
-      <c r="B281" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="E281" s="2"/>
-      <c r="F281" s="2"/>
-      <c r="G281" s="2"/>
-      <c r="H281" s="2"/>
-      <c r="I281" s="2"/>
-      <c r="J281" s="2"/>
-      <c r="K281" s="2"/>
-      <c r="L281" s="2"/>
-      <c r="M281" s="2"/>
-      <c r="N281" s="2"/>
-      <c r="O281" s="2"/>
-      <c r="P281" s="2"/>
-      <c r="Q281" s="2"/>
-      <c r="R281" s="2"/>
-      <c r="S281" s="2"/>
-      <c r="T281" s="5"/>
+      <c r="C281" s="8"/>
+      <c r="D281" s="8"/>
+      <c r="E281" s="8"/>
+      <c r="F281" s="8"/>
+      <c r="G281" s="8"/>
+      <c r="H281" s="8"/>
+      <c r="I281" s="8"/>
+      <c r="J281" s="8"/>
+      <c r="K281" s="8"/>
+      <c r="L281" s="8"/>
+      <c r="M281" s="8"/>
+      <c r="N281" s="8"/>
+      <c r="O281" s="8"/>
+      <c r="P281" s="8"/>
+      <c r="Q281" s="8"/>
+      <c r="R281" s="8"/>
+      <c r="S281" s="8"/>
+      <c r="T281" s="14"/>
       <c r="U281">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8741,7 +8741,7 @@
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="22"/>
       <c r="B282" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8769,7 +8769,7 @@
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" s="22"/>
       <c r="B283" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8794,87 +8794,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="23"/>
-      <c r="B284" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C284" s="6"/>
-      <c r="D284" s="6"/>
-      <c r="E284" s="6"/>
-      <c r="F284" s="6"/>
-      <c r="G284" s="6"/>
-      <c r="H284" s="6"/>
-      <c r="I284" s="6"/>
-      <c r="J284" s="6"/>
-      <c r="K284" s="6"/>
-      <c r="L284" s="6"/>
-      <c r="M284" s="6"/>
-      <c r="N284" s="6"/>
-      <c r="O284" s="6"/>
-      <c r="P284" s="6"/>
-      <c r="Q284" s="6"/>
-      <c r="R284" s="6"/>
-      <c r="S284" s="6"/>
-      <c r="T284" s="7"/>
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A284" s="22"/>
+      <c r="B284" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C284" s="2"/>
+      <c r="D284" s="2"/>
+      <c r="E284" s="2"/>
+      <c r="F284" s="2"/>
+      <c r="G284" s="2"/>
+      <c r="H284" s="2"/>
+      <c r="I284" s="2"/>
+      <c r="J284" s="2"/>
+      <c r="K284" s="2"/>
+      <c r="L284" s="2"/>
+      <c r="M284" s="2"/>
+      <c r="N284" s="2"/>
+      <c r="O284" s="2"/>
+      <c r="P284" s="2"/>
+      <c r="Q284" s="2"/>
+      <c r="R284" s="2"/>
+      <c r="S284" s="2"/>
+      <c r="T284" s="5"/>
       <c r="U284">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A285" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B285" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C285" s="8"/>
-      <c r="D285" s="8"/>
-      <c r="E285" s="8"/>
-      <c r="F285" s="8"/>
-      <c r="G285" s="8"/>
-      <c r="H285" s="8"/>
-      <c r="I285" s="8"/>
-      <c r="J285" s="8"/>
-      <c r="K285" s="8"/>
-      <c r="L285" s="8"/>
-      <c r="M285" s="8"/>
-      <c r="N285" s="8"/>
-      <c r="O285" s="8"/>
-      <c r="P285" s="8"/>
-      <c r="Q285" s="8"/>
-      <c r="R285" s="8"/>
-      <c r="S285" s="8"/>
-      <c r="T285" s="14"/>
+    <row r="285" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="23"/>
+      <c r="B285" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C285" s="6"/>
+      <c r="D285" s="6"/>
+      <c r="E285" s="6"/>
+      <c r="F285" s="6"/>
+      <c r="G285" s="6"/>
+      <c r="H285" s="6"/>
+      <c r="I285" s="6"/>
+      <c r="J285" s="6"/>
+      <c r="K285" s="6"/>
+      <c r="L285" s="6"/>
+      <c r="M285" s="6"/>
+      <c r="N285" s="6"/>
+      <c r="O285" s="6"/>
+      <c r="P285" s="6"/>
+      <c r="Q285" s="6"/>
+      <c r="R285" s="6"/>
+      <c r="S285" s="6"/>
+      <c r="T285" s="7"/>
       <c r="U285">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A286" s="22"/>
-      <c r="B286" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2"/>
-      <c r="E286" s="2"/>
-      <c r="F286" s="2"/>
-      <c r="G286" s="2"/>
-      <c r="H286" s="2"/>
-      <c r="I286" s="2"/>
-      <c r="J286" s="2"/>
-      <c r="K286" s="2"/>
-      <c r="L286" s="2"/>
-      <c r="M286" s="2"/>
-      <c r="N286" s="2"/>
-      <c r="O286" s="2"/>
-      <c r="P286" s="2"/>
-      <c r="Q286" s="2"/>
-      <c r="R286" s="2"/>
-      <c r="S286" s="2"/>
-      <c r="T286" s="5"/>
+      <c r="A286" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B286" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C286" s="8"/>
+      <c r="D286" s="8"/>
+      <c r="E286" s="8"/>
+      <c r="F286" s="8"/>
+      <c r="G286" s="8"/>
+      <c r="H286" s="8"/>
+      <c r="I286" s="8"/>
+      <c r="J286" s="8"/>
+      <c r="K286" s="8"/>
+      <c r="L286" s="8"/>
+      <c r="M286" s="8"/>
+      <c r="N286" s="8"/>
+      <c r="O286" s="8"/>
+      <c r="P286" s="8"/>
+      <c r="Q286" s="8"/>
+      <c r="R286" s="8"/>
+      <c r="S286" s="8"/>
+      <c r="T286" s="14"/>
       <c r="U286">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8883,7 +8883,7 @@
     <row r="287" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="22"/>
       <c r="B287" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8908,10 +8908,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A288" s="22"/>
-      <c r="B288" s="2">
-        <v>7170</v>
+      <c r="B288" s="12">
+        <v>7546</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -8939,7 +8939,7 @@
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" s="22"/>
       <c r="B289" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -8967,7 +8967,7 @@
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="22"/>
       <c r="B290" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8995,7 +8995,7 @@
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="22"/>
       <c r="B291" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9023,7 +9023,7 @@
     <row r="292" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A292" s="22"/>
       <c r="B292" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9051,7 +9051,7 @@
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293" s="22"/>
       <c r="B293" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9079,7 +9079,7 @@
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A294" s="22"/>
       <c r="B294" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9107,7 +9107,7 @@
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" s="22"/>
       <c r="B295" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9135,7 +9135,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="22"/>
       <c r="B296" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9163,7 +9163,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="22"/>
       <c r="B297" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9191,7 +9191,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="22"/>
       <c r="B298" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9219,7 +9219,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="22"/>
       <c r="B299" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9244,87 +9244,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="23"/>
-      <c r="B300" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-      <c r="E300" s="6"/>
-      <c r="F300" s="6"/>
-      <c r="G300" s="6"/>
-      <c r="H300" s="6"/>
-      <c r="I300" s="6"/>
-      <c r="J300" s="6"/>
-      <c r="K300" s="6"/>
-      <c r="L300" s="6"/>
-      <c r="M300" s="6"/>
-      <c r="N300" s="6"/>
-      <c r="O300" s="6"/>
-      <c r="P300" s="6"/>
-      <c r="Q300" s="6"/>
-      <c r="R300" s="6"/>
-      <c r="S300" s="6"/>
-      <c r="T300" s="7"/>
+    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A300" s="22"/>
+      <c r="B300" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C300" s="2"/>
+      <c r="D300" s="2"/>
+      <c r="E300" s="2"/>
+      <c r="F300" s="2"/>
+      <c r="G300" s="2"/>
+      <c r="H300" s="2"/>
+      <c r="I300" s="2"/>
+      <c r="J300" s="2"/>
+      <c r="K300" s="2"/>
+      <c r="L300" s="2"/>
+      <c r="M300" s="2"/>
+      <c r="N300" s="2"/>
+      <c r="O300" s="2"/>
+      <c r="P300" s="2"/>
+      <c r="Q300" s="2"/>
+      <c r="R300" s="2"/>
+      <c r="S300" s="2"/>
+      <c r="T300" s="5"/>
       <c r="U300">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B301" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
-      <c r="F301" s="8"/>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-      <c r="K301" s="8"/>
-      <c r="L301" s="8"/>
-      <c r="M301" s="8"/>
-      <c r="N301" s="8"/>
-      <c r="O301" s="8"/>
-      <c r="P301" s="8"/>
-      <c r="Q301" s="8"/>
-      <c r="R301" s="8"/>
-      <c r="S301" s="8"/>
-      <c r="T301" s="14"/>
+    <row r="301" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="23"/>
+      <c r="B301" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
+      <c r="H301" s="6"/>
+      <c r="I301" s="6"/>
+      <c r="J301" s="6"/>
+      <c r="K301" s="6"/>
+      <c r="L301" s="6"/>
+      <c r="M301" s="6"/>
+      <c r="N301" s="6"/>
+      <c r="O301" s="6"/>
+      <c r="P301" s="6"/>
+      <c r="Q301" s="6"/>
+      <c r="R301" s="6"/>
+      <c r="S301" s="6"/>
+      <c r="T301" s="7"/>
       <c r="U301">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A302" s="22"/>
-      <c r="B302" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2"/>
-      <c r="E302" s="2"/>
-      <c r="F302" s="2"/>
-      <c r="G302" s="2"/>
-      <c r="H302" s="2"/>
-      <c r="I302" s="2"/>
-      <c r="J302" s="2"/>
-      <c r="K302" s="2"/>
-      <c r="L302" s="2"/>
-      <c r="M302" s="2"/>
-      <c r="N302" s="2"/>
-      <c r="O302" s="2"/>
-      <c r="P302" s="2"/>
-      <c r="Q302" s="2"/>
-      <c r="R302" s="2"/>
-      <c r="S302" s="2"/>
-      <c r="T302" s="5"/>
+      <c r="A302" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B302" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C302" s="8"/>
+      <c r="D302" s="8"/>
+      <c r="E302" s="8"/>
+      <c r="F302" s="8"/>
+      <c r="G302" s="8"/>
+      <c r="H302" s="8"/>
+      <c r="I302" s="8"/>
+      <c r="J302" s="8"/>
+      <c r="K302" s="8"/>
+      <c r="L302" s="8"/>
+      <c r="M302" s="8"/>
+      <c r="N302" s="8"/>
+      <c r="O302" s="8"/>
+      <c r="P302" s="8"/>
+      <c r="Q302" s="8"/>
+      <c r="R302" s="8"/>
+      <c r="S302" s="8"/>
+      <c r="T302" s="14"/>
       <c r="U302">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9333,7 +9333,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="22"/>
       <c r="B303" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9361,7 +9361,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="22"/>
       <c r="B304" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9389,7 +9389,7 @@
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="22"/>
       <c r="B305" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9414,87 +9414,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A306" s="23"/>
-      <c r="B306" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C306" s="6"/>
-      <c r="D306" s="6"/>
-      <c r="E306" s="6"/>
-      <c r="F306" s="6"/>
-      <c r="G306" s="6"/>
-      <c r="H306" s="6"/>
-      <c r="I306" s="6"/>
-      <c r="J306" s="6"/>
-      <c r="K306" s="6"/>
-      <c r="L306" s="6"/>
-      <c r="M306" s="6"/>
-      <c r="N306" s="6"/>
-      <c r="O306" s="6"/>
-      <c r="P306" s="6"/>
-      <c r="Q306" s="6"/>
-      <c r="R306" s="6"/>
-      <c r="S306" s="6"/>
-      <c r="T306" s="7"/>
+    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A306" s="22"/>
+      <c r="B306" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C306" s="2"/>
+      <c r="D306" s="2"/>
+      <c r="E306" s="2"/>
+      <c r="F306" s="2"/>
+      <c r="G306" s="2"/>
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+      <c r="J306" s="2"/>
+      <c r="K306" s="2"/>
+      <c r="L306" s="2"/>
+      <c r="M306" s="2"/>
+      <c r="N306" s="2"/>
+      <c r="O306" s="2"/>
+      <c r="P306" s="2"/>
+      <c r="Q306" s="2"/>
+      <c r="R306" s="2"/>
+      <c r="S306" s="2"/>
+      <c r="T306" s="5"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A307" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B307" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C307" s="8"/>
-      <c r="D307" s="8"/>
-      <c r="E307" s="8"/>
-      <c r="F307" s="8"/>
-      <c r="G307" s="8"/>
-      <c r="H307" s="8"/>
-      <c r="I307" s="8"/>
-      <c r="J307" s="8"/>
-      <c r="K307" s="8"/>
-      <c r="L307" s="8"/>
-      <c r="M307" s="8"/>
-      <c r="N307" s="8"/>
-      <c r="O307" s="8"/>
-      <c r="P307" s="8"/>
-      <c r="Q307" s="8"/>
-      <c r="R307" s="8"/>
-      <c r="S307" s="8"/>
-      <c r="T307" s="14"/>
+    <row r="307" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="23"/>
+      <c r="B307" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C307" s="6"/>
+      <c r="D307" s="6"/>
+      <c r="E307" s="6"/>
+      <c r="F307" s="6"/>
+      <c r="G307" s="6"/>
+      <c r="H307" s="6"/>
+      <c r="I307" s="6"/>
+      <c r="J307" s="6"/>
+      <c r="K307" s="6"/>
+      <c r="L307" s="6"/>
+      <c r="M307" s="6"/>
+      <c r="N307" s="6"/>
+      <c r="O307" s="6"/>
+      <c r="P307" s="6"/>
+      <c r="Q307" s="6"/>
+      <c r="R307" s="6"/>
+      <c r="S307" s="6"/>
+      <c r="T307" s="7"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A308" s="22"/>
-      <c r="B308" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
-      <c r="E308" s="2"/>
-      <c r="F308" s="2"/>
-      <c r="G308" s="2"/>
-      <c r="H308" s="2"/>
-      <c r="I308" s="2"/>
-      <c r="J308" s="2"/>
-      <c r="K308" s="2"/>
-      <c r="L308" s="2"/>
-      <c r="M308" s="2"/>
-      <c r="N308" s="2"/>
-      <c r="O308" s="2"/>
-      <c r="P308" s="2"/>
-      <c r="Q308" s="2"/>
-      <c r="R308" s="2"/>
-      <c r="S308" s="2"/>
-      <c r="T308" s="5"/>
+      <c r="A308" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B308" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C308" s="8"/>
+      <c r="D308" s="8"/>
+      <c r="E308" s="8"/>
+      <c r="F308" s="8"/>
+      <c r="G308" s="8"/>
+      <c r="H308" s="8"/>
+      <c r="I308" s="8"/>
+      <c r="J308" s="8"/>
+      <c r="K308" s="8"/>
+      <c r="L308" s="8"/>
+      <c r="M308" s="8"/>
+      <c r="N308" s="8"/>
+      <c r="O308" s="8"/>
+      <c r="P308" s="8"/>
+      <c r="Q308" s="8"/>
+      <c r="R308" s="8"/>
+      <c r="S308" s="8"/>
+      <c r="T308" s="14"/>
       <c r="U308">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9503,7 +9503,7 @@
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="22"/>
       <c r="B309" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9531,7 +9531,7 @@
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="22"/>
       <c r="B310" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9559,7 +9559,7 @@
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A311" s="22"/>
       <c r="B311" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9584,35 +9584,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="23"/>
-      <c r="B312" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C312" s="6"/>
-      <c r="D312" s="6"/>
-      <c r="E312" s="6"/>
-      <c r="F312" s="6"/>
-      <c r="G312" s="6"/>
-      <c r="H312" s="6"/>
-      <c r="I312" s="6"/>
-      <c r="J312" s="6"/>
-      <c r="K312" s="6"/>
-      <c r="L312" s="6"/>
-      <c r="M312" s="6"/>
-      <c r="N312" s="6"/>
-      <c r="O312" s="6"/>
-      <c r="P312" s="6"/>
-      <c r="Q312" s="6"/>
-      <c r="R312" s="6"/>
-      <c r="S312" s="6"/>
-      <c r="T312" s="7"/>
+    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A312" s="22"/>
+      <c r="B312" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C312" s="2"/>
+      <c r="D312" s="2"/>
+      <c r="E312" s="2"/>
+      <c r="F312" s="2"/>
+      <c r="G312" s="2"/>
+      <c r="H312" s="2"/>
+      <c r="I312" s="2"/>
+      <c r="J312" s="2"/>
+      <c r="K312" s="2"/>
+      <c r="L312" s="2"/>
+      <c r="M312" s="2"/>
+      <c r="N312" s="2"/>
+      <c r="O312" s="2"/>
+      <c r="P312" s="2"/>
+      <c r="Q312" s="2"/>
+      <c r="R312" s="2"/>
+      <c r="S312" s="2"/>
+      <c r="T312" s="5"/>
       <c r="U312">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="23"/>
+      <c r="B313" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C313" s="6"/>
+      <c r="D313" s="6"/>
+      <c r="E313" s="6"/>
+      <c r="F313" s="6"/>
+      <c r="G313" s="6"/>
+      <c r="H313" s="6"/>
+      <c r="I313" s="6"/>
+      <c r="J313" s="6"/>
+      <c r="K313" s="6"/>
+      <c r="L313" s="6"/>
+      <c r="M313" s="6"/>
+      <c r="N313" s="6"/>
+      <c r="O313" s="6"/>
+      <c r="P313" s="6"/>
+      <c r="Q313" s="6"/>
+      <c r="R313" s="6"/>
+      <c r="S313" s="6"/>
+      <c r="T313" s="7"/>
       <c r="U313">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9794,13 +9816,13 @@
     </row>
     <row r="343" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U343">
-        <f t="shared" ref="U343:U406" ca="1" si="8">IF(B343=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="344" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U344">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U344:U407" ca="1" si="8">IF(B344=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10178,13 +10200,13 @@
     </row>
     <row r="407" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U407">
-        <f t="shared" ref="U407:U470" ca="1" si="9">IF(B407=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="408" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U408">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U408:U471" ca="1" si="9">IF(B408=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10562,13 +10584,13 @@
     </row>
     <row r="471" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U471">
-        <f t="shared" ref="U471:U534" ca="1" si="10">IF(B471=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="472" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U472">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U472:U535" ca="1" si="10">IF(B472=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10946,13 +10968,13 @@
     </row>
     <row r="535" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U535">
-        <f t="shared" ref="U535:U598" ca="1" si="11">IF(B535=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="536" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U536">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U536:U599" ca="1" si="11">IF(B536=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11330,13 +11352,13 @@
     </row>
     <row r="599" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U599">
-        <f t="shared" ref="U599:U662" ca="1" si="12">IF(B599=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="600" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U600">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U600:U663" ca="1" si="12">IF(B600=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11714,13 +11736,13 @@
     </row>
     <row r="663" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U663">
-        <f t="shared" ref="U663:U726" ca="1" si="13">IF(B663=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="664" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U664">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U664:U727" ca="1" si="13">IF(B664=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12098,13 +12120,13 @@
     </row>
     <row r="727" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U727">
-        <f t="shared" ref="U727:U790" ca="1" si="14">IF(B727=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="728" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U728">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U728:U791" ca="1" si="14">IF(B728=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12482,13 +12504,13 @@
     </row>
     <row r="791" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U791">
-        <f t="shared" ref="U791:U854" ca="1" si="15">IF(B791=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="792" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U792">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U792:U855" ca="1" si="15">IF(B792=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12866,13 +12888,13 @@
     </row>
     <row r="855" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U855">
-        <f t="shared" ref="U855:U916" ca="1" si="16">IF(B855=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="856" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U856">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U856:U917" ca="1" si="16">IF(B856=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13236,26 +13258,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="917" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U917">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A308:A313"/>
+    <mergeCell ref="A243:A269"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A286:A301"/>
+    <mergeCell ref="A302:A307"/>
+    <mergeCell ref="A64:A103"/>
+    <mergeCell ref="A215:A226"/>
+    <mergeCell ref="A148:A179"/>
+    <mergeCell ref="A180:A197"/>
+    <mergeCell ref="A104:A147"/>
+    <mergeCell ref="A19:A63"/>
+    <mergeCell ref="A198:A214"/>
+    <mergeCell ref="A227:A234"/>
+    <mergeCell ref="A235:A242"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A280:A284"/>
-    <mergeCell ref="A269:A279"/>
-    <mergeCell ref="A307:A312"/>
-    <mergeCell ref="A242:A268"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A285:A300"/>
-    <mergeCell ref="A301:A306"/>
-    <mergeCell ref="A64:A102"/>
-    <mergeCell ref="A214:A225"/>
-    <mergeCell ref="A147:A178"/>
-    <mergeCell ref="A179:A196"/>
-    <mergeCell ref="A103:A146"/>
-    <mergeCell ref="A19:A63"/>
-    <mergeCell ref="A197:A213"/>
-    <mergeCell ref="A226:A233"/>
-    <mergeCell ref="A234:A241"/>
+    <mergeCell ref="A281:A285"/>
+    <mergeCell ref="A270:A280"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task for implementation of Point.equals
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$287</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$289</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -483,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -515,6 +515,34 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,33 +560,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,11 +862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W919"/>
+  <dimension ref="A1:W921"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,56 +883,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>5326</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="26"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="23"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="33"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -961,7 +962,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -991,7 +992,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1019,7 +1020,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1047,7 +1048,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3">
         <v>1662</v>
       </c>
@@ -1075,7 +1076,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2">
         <v>1860</v>
       </c>
@@ -1103,7 +1104,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2">
         <v>4764</v>
       </c>
@@ -1131,7 +1132,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2">
         <v>2429</v>
       </c>
@@ -1159,7 +1160,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2">
         <v>7472</v>
       </c>
@@ -1187,7 +1188,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2">
         <v>4140</v>
       </c>
@@ -1215,7 +1216,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2">
         <v>2959</v>
       </c>
@@ -1243,7 +1244,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2">
         <v>7271</v>
       </c>
@@ -1271,7 +1272,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2">
         <v>2632</v>
       </c>
@@ -1299,7 +1300,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1327,7 +1328,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1355,7 +1356,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1385,7 +1386,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1413,7 +1414,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1441,7 +1442,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1469,7 +1470,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1497,7 +1498,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1525,7 +1526,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1553,7 +1554,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1581,7 +1582,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1609,7 +1610,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1637,7 +1638,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1665,7 +1666,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1693,7 +1694,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1721,7 +1722,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1749,7 +1750,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1777,7 +1778,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1805,7 +1806,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1833,7 +1834,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1861,7 +1862,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1889,7 +1890,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1917,7 +1918,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1945,7 +1946,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1973,7 +1974,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2001,7 +2002,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2029,7 +2030,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2057,7 +2058,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2085,7 +2086,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2113,7 +2114,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2141,7 +2142,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2169,7 +2170,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2197,7 +2198,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2225,7 +2226,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2253,7 +2254,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2281,7 +2282,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2309,7 +2310,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2337,7 +2338,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="34"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2365,7 +2366,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="34"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2393,7 +2394,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2421,7 +2422,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="34"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2449,7 +2450,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2477,7 +2478,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2505,7 +2506,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="34"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2533,7 +2534,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2561,7 +2562,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2589,7 +2590,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="35"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -2617,7 +2618,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="13">
@@ -2647,7 +2648,7 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="28"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="12">
         <v>2217</v>
       </c>
@@ -2675,7 +2676,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="28"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="12">
         <v>1824</v>
       </c>
@@ -2703,7 +2704,7 @@
       </c>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="28"/>
+      <c r="A67" s="23"/>
       <c r="B67" s="12">
         <v>2564</v>
       </c>
@@ -2731,7 +2732,7 @@
       </c>
     </row>
     <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="28"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="12">
         <v>8487</v>
       </c>
@@ -2759,7 +2760,7 @@
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="28"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="2">
         <v>8878</v>
       </c>
@@ -2787,7 +2788,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="28"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="2">
         <v>3072</v>
       </c>
@@ -2815,7 +2816,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="28"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="2">
         <v>5980</v>
       </c>
@@ -2843,7 +2844,7 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="2">
         <v>8174</v>
       </c>
@@ -2871,7 +2872,7 @@
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="28"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="2">
         <v>4257</v>
       </c>
@@ -2899,7 +2900,7 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="2">
         <v>2291</v>
       </c>
@@ -2927,7 +2928,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="28"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="2">
         <v>1763</v>
       </c>
@@ -2955,7 +2956,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="2">
         <v>5662</v>
       </c>
@@ -2983,7 +2984,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="28"/>
+      <c r="A77" s="23"/>
       <c r="B77" s="2">
         <v>1945</v>
       </c>
@@ -3011,7 +3012,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
+      <c r="A78" s="23"/>
       <c r="B78" s="2">
         <v>1186</v>
       </c>
@@ -3039,7 +3040,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="28"/>
+      <c r="A79" s="23"/>
       <c r="B79" s="2">
         <v>8715</v>
       </c>
@@ -3067,7 +3068,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
+      <c r="A80" s="23"/>
       <c r="B80" s="2">
         <v>8518</v>
       </c>
@@ -3095,7 +3096,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
+      <c r="A81" s="23"/>
       <c r="B81" s="2">
         <v>4847</v>
       </c>
@@ -3123,7 +3124,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="28"/>
+      <c r="A82" s="23"/>
       <c r="B82" s="2">
         <v>6589</v>
       </c>
@@ -3151,7 +3152,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="28"/>
+      <c r="A83" s="23"/>
       <c r="B83" s="2">
         <v>7991</v>
       </c>
@@ -3179,7 +3180,7 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="28"/>
+      <c r="A84" s="23"/>
       <c r="B84" s="2">
         <v>6291</v>
       </c>
@@ -3207,7 +3208,7 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
+      <c r="A85" s="23"/>
       <c r="B85" s="2">
         <v>3770</v>
       </c>
@@ -3235,7 +3236,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="28"/>
+      <c r="A86" s="23"/>
       <c r="B86" s="2">
         <v>7178</v>
       </c>
@@ -3263,7 +3264,7 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
+      <c r="A87" s="23"/>
       <c r="B87" s="2">
         <v>3883</v>
       </c>
@@ -3291,7 +3292,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="2">
         <v>1999</v>
       </c>
@@ -3319,7 +3320,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
+      <c r="A89" s="23"/>
       <c r="B89" s="2">
         <v>4042</v>
       </c>
@@ -3347,7 +3348,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
+      <c r="A90" s="23"/>
       <c r="B90" s="2">
         <v>6351</v>
       </c>
@@ -3375,7 +3376,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="28"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="2">
         <v>5382</v>
       </c>
@@ -3403,7 +3404,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="28"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="2">
         <v>7088</v>
       </c>
@@ -3431,7 +3432,7 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="2">
         <v>7250</v>
       </c>
@@ -3459,7 +3460,7 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="2">
         <v>6740</v>
       </c>
@@ -3487,7 +3488,7 @@
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="2">
         <v>9038</v>
       </c>
@@ -3515,7 +3516,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="28"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="2">
         <v>1292</v>
       </c>
@@ -3543,7 +3544,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="28"/>
+      <c r="A97" s="23"/>
       <c r="B97" s="2">
         <v>4527</v>
       </c>
@@ -3571,7 +3572,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="28"/>
+      <c r="A98" s="23"/>
       <c r="B98" s="2">
         <v>6556</v>
       </c>
@@ -3599,7 +3600,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="28"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="2">
         <v>5635</v>
       </c>
@@ -3627,7 +3628,7 @@
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
+      <c r="A100" s="23"/>
       <c r="B100" s="2">
         <v>3878</v>
       </c>
@@ -3655,7 +3656,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A101" s="28"/>
+      <c r="A101" s="23"/>
       <c r="B101" s="2">
         <v>1217</v>
       </c>
@@ -3683,7 +3684,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A102" s="28"/>
+      <c r="A102" s="23"/>
       <c r="B102" s="2">
         <v>1438</v>
       </c>
@@ -3711,7 +3712,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
+      <c r="A103" s="23"/>
       <c r="B103" s="2">
         <v>2153</v>
       </c>
@@ -3739,7 +3740,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="29"/>
+      <c r="A104" s="24"/>
       <c r="B104" s="6">
         <v>7937</v>
       </c>
@@ -3767,7 +3768,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="27" t="s">
+      <c r="A105" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B105" s="13">
@@ -3797,7 +3798,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="12">
         <v>1881</v>
       </c>
@@ -3825,7 +3826,7 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" s="28"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="2">
         <v>8495</v>
       </c>
@@ -3853,7 +3854,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" s="28"/>
+      <c r="A108" s="23"/>
       <c r="B108" s="2">
         <v>1315</v>
       </c>
@@ -3881,7 +3882,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A109" s="28"/>
+      <c r="A109" s="23"/>
       <c r="B109" s="2">
         <v>6066</v>
       </c>
@@ -3909,7 +3910,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A110" s="28"/>
+      <c r="A110" s="23"/>
       <c r="B110" s="2">
         <v>2565</v>
       </c>
@@ -3937,7 +3938,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A111" s="28"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="2">
         <v>2594</v>
       </c>
@@ -3965,7 +3966,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="28"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="2">
         <v>2321</v>
       </c>
@@ -3993,7 +3994,7 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" s="28"/>
+      <c r="A113" s="23"/>
       <c r="B113" s="2">
         <v>5053</v>
       </c>
@@ -4021,7 +4022,7 @@
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114" s="28"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="2">
         <v>4338</v>
       </c>
@@ -4049,7 +4050,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="2">
         <v>3762</v>
       </c>
@@ -4077,7 +4078,7 @@
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" s="28"/>
+      <c r="A116" s="23"/>
       <c r="B116" s="2">
         <v>3550</v>
       </c>
@@ -4105,7 +4106,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
+      <c r="A117" s="23"/>
       <c r="B117" s="2">
         <v>4264</v>
       </c>
@@ -4133,7 +4134,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="28"/>
+      <c r="A118" s="23"/>
       <c r="B118" s="2">
         <v>2475</v>
       </c>
@@ -4161,7 +4162,7 @@
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
+      <c r="A119" s="23"/>
       <c r="B119" s="2">
         <v>9180</v>
       </c>
@@ -4189,7 +4190,7 @@
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" s="28"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="2">
         <v>1544</v>
       </c>
@@ -4217,7 +4218,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="28"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="2">
         <v>9562</v>
       </c>
@@ -4245,7 +4246,7 @@
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122" s="28"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="2">
         <v>3669</v>
       </c>
@@ -4273,7 +4274,7 @@
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="28"/>
+      <c r="A123" s="23"/>
       <c r="B123" s="2">
         <v>5951</v>
       </c>
@@ -4301,7 +4302,7 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="28"/>
+      <c r="A124" s="23"/>
       <c r="B124" s="2">
         <v>2802</v>
       </c>
@@ -4329,7 +4330,7 @@
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="28"/>
+      <c r="A125" s="23"/>
       <c r="B125" s="2">
         <v>2324</v>
       </c>
@@ -4357,7 +4358,7 @@
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126" s="28"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="2">
         <v>8731</v>
       </c>
@@ -4385,7 +4386,7 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127" s="28"/>
+      <c r="A127" s="23"/>
       <c r="B127" s="2">
         <v>4082</v>
       </c>
@@ -4413,7 +4414,7 @@
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128" s="28"/>
+      <c r="A128" s="23"/>
       <c r="B128" s="2">
         <v>6280</v>
       </c>
@@ -4441,7 +4442,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A129" s="28"/>
+      <c r="A129" s="23"/>
       <c r="B129" s="2">
         <v>7585</v>
       </c>
@@ -4469,7 +4470,7 @@
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A130" s="28"/>
+      <c r="A130" s="23"/>
       <c r="B130" s="2">
         <v>1483</v>
       </c>
@@ -4497,7 +4498,7 @@
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
+      <c r="A131" s="23"/>
       <c r="B131" s="2">
         <v>3983</v>
       </c>
@@ -4525,7 +4526,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="28"/>
+      <c r="A132" s="23"/>
       <c r="B132" s="2">
         <v>8770</v>
       </c>
@@ -4553,7 +4554,7 @@
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A133" s="28"/>
+      <c r="A133" s="23"/>
       <c r="B133" s="2">
         <v>4236</v>
       </c>
@@ -4580,8 +4581,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A134" s="28"/>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A134" s="23"/>
       <c r="B134" s="2">
         <v>8696</v>
       </c>
@@ -4609,7 +4610,7 @@
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A135" s="28"/>
+      <c r="A135" s="23"/>
       <c r="B135" s="2">
         <v>5969</v>
       </c>
@@ -4637,7 +4638,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A136" s="28"/>
+      <c r="A136" s="23"/>
       <c r="B136" s="2">
         <v>8418</v>
       </c>
@@ -4665,7 +4666,7 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
+      <c r="A137" s="23"/>
       <c r="B137" s="2">
         <v>5170</v>
       </c>
@@ -4693,7 +4694,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A138" s="28"/>
+      <c r="A138" s="23"/>
       <c r="B138" s="2">
         <v>8395</v>
       </c>
@@ -4721,7 +4722,7 @@
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A139" s="28"/>
+      <c r="A139" s="23"/>
       <c r="B139" s="2">
         <v>5568</v>
       </c>
@@ -4749,7 +4750,7 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="28"/>
+      <c r="A140" s="23"/>
       <c r="B140" s="2">
         <v>2592</v>
       </c>
@@ -4777,7 +4778,7 @@
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A141" s="28"/>
+      <c r="A141" s="23"/>
       <c r="B141" s="2">
         <v>4075</v>
       </c>
@@ -4805,7 +4806,7 @@
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A142" s="28"/>
+      <c r="A142" s="23"/>
       <c r="B142" s="2">
         <v>7517</v>
       </c>
@@ -4833,7 +4834,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A143" s="28"/>
+      <c r="A143" s="23"/>
       <c r="B143" s="2">
         <v>5448</v>
       </c>
@@ -4861,7 +4862,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A144" s="28"/>
+      <c r="A144" s="23"/>
       <c r="B144" s="2">
         <v>6582</v>
       </c>
@@ -4889,7 +4890,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A145" s="28"/>
+      <c r="A145" s="23"/>
       <c r="B145" s="2">
         <v>5238</v>
       </c>
@@ -4917,7 +4918,7 @@
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A146" s="28"/>
+      <c r="A146" s="23"/>
       <c r="B146" s="2">
         <v>2084</v>
       </c>
@@ -4945,7 +4946,7 @@
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A147" s="28"/>
+      <c r="A147" s="23"/>
       <c r="B147" s="2">
         <v>5411</v>
       </c>
@@ -4973,7 +4974,7 @@
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A148" s="28"/>
+      <c r="A148" s="23"/>
       <c r="B148" s="2">
         <v>5171</v>
       </c>
@@ -5001,7 +5002,7 @@
       </c>
     </row>
     <row r="149" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="29"/>
+      <c r="A149" s="24"/>
       <c r="B149" s="6">
         <v>1862</v>
       </c>
@@ -5029,7 +5030,7 @@
       </c>
     </row>
     <row r="150" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="27" t="s">
+      <c r="A150" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B150" s="13">
@@ -5059,7 +5060,7 @@
       </c>
     </row>
     <row r="151" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="28"/>
+      <c r="A151" s="23"/>
       <c r="B151" s="12">
         <v>9931</v>
       </c>
@@ -5087,7 +5088,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="28"/>
+      <c r="A152" s="23"/>
       <c r="B152" s="12">
         <v>9696</v>
       </c>
@@ -5115,7 +5116,7 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="28"/>
+      <c r="A153" s="23"/>
       <c r="B153" s="12">
         <v>1947</v>
       </c>
@@ -5143,7 +5144,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A154" s="28"/>
+      <c r="A154" s="23"/>
       <c r="B154" s="2">
         <v>4425</v>
       </c>
@@ -5171,7 +5172,7 @@
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A155" s="28"/>
+      <c r="A155" s="23"/>
       <c r="B155" s="2">
         <v>5683</v>
       </c>
@@ -5199,7 +5200,7 @@
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A156" s="28"/>
+      <c r="A156" s="23"/>
       <c r="B156" s="2">
         <v>1223</v>
       </c>
@@ -5227,7 +5228,7 @@
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A157" s="28"/>
+      <c r="A157" s="23"/>
       <c r="B157" s="2">
         <v>8311</v>
       </c>
@@ -5255,7 +5256,7 @@
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A158" s="28"/>
+      <c r="A158" s="23"/>
       <c r="B158" s="2">
         <v>3134</v>
       </c>
@@ -5283,7 +5284,7 @@
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="28"/>
+      <c r="A159" s="23"/>
       <c r="B159" s="2">
         <v>9711</v>
       </c>
@@ -5311,7 +5312,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A160" s="28"/>
+      <c r="A160" s="23"/>
       <c r="B160" s="2">
         <v>3333</v>
       </c>
@@ -5339,7 +5340,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A161" s="28"/>
+      <c r="A161" s="23"/>
       <c r="B161" s="2">
         <v>8820</v>
       </c>
@@ -5367,7 +5368,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A162" s="28"/>
+      <c r="A162" s="23"/>
       <c r="B162" s="2">
         <v>5694</v>
       </c>
@@ -5395,7 +5396,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A163" s="28"/>
+      <c r="A163" s="23"/>
       <c r="B163" s="2">
         <v>6806</v>
       </c>
@@ -5423,7 +5424,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A164" s="28"/>
+      <c r="A164" s="23"/>
       <c r="B164" s="2">
         <v>7369</v>
       </c>
@@ -5451,7 +5452,7 @@
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A165" s="28"/>
+      <c r="A165" s="23"/>
       <c r="B165" s="2">
         <v>5894</v>
       </c>
@@ -5479,7 +5480,7 @@
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A166" s="28"/>
+      <c r="A166" s="23"/>
       <c r="B166" s="2">
         <v>4515</v>
       </c>
@@ -5507,7 +5508,7 @@
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A167" s="28"/>
+      <c r="A167" s="23"/>
       <c r="B167" s="2">
         <v>9774</v>
       </c>
@@ -5535,7 +5536,7 @@
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168" s="28"/>
+      <c r="A168" s="23"/>
       <c r="B168" s="2">
         <v>3946</v>
       </c>
@@ -5563,7 +5564,7 @@
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A169" s="28"/>
+      <c r="A169" s="23"/>
       <c r="B169" s="2">
         <v>6497</v>
       </c>
@@ -5591,7 +5592,7 @@
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A170" s="28"/>
+      <c r="A170" s="23"/>
       <c r="B170" s="2">
         <v>5648</v>
       </c>
@@ -5619,7 +5620,7 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A171" s="28"/>
+      <c r="A171" s="23"/>
       <c r="B171" s="2">
         <v>3940</v>
       </c>
@@ -5647,7 +5648,7 @@
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A172" s="28"/>
+      <c r="A172" s="23"/>
       <c r="B172" s="2">
         <v>7290</v>
       </c>
@@ -5675,7 +5676,7 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173" s="28"/>
+      <c r="A173" s="23"/>
       <c r="B173" s="2">
         <v>7035</v>
       </c>
@@ -5703,7 +5704,7 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="28"/>
+      <c r="A174" s="23"/>
       <c r="B174" s="2">
         <v>9271</v>
       </c>
@@ -5731,7 +5732,7 @@
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A175" s="28"/>
+      <c r="A175" s="23"/>
       <c r="B175" s="2">
         <v>8769</v>
       </c>
@@ -5759,7 +5760,7 @@
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" s="28"/>
+      <c r="A176" s="23"/>
       <c r="B176" s="2">
         <v>4497</v>
       </c>
@@ -5787,7 +5788,7 @@
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A177" s="28"/>
+      <c r="A177" s="23"/>
       <c r="B177" s="2">
         <v>3218</v>
       </c>
@@ -5815,7 +5816,7 @@
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A178" s="28"/>
+      <c r="A178" s="23"/>
       <c r="B178" s="2">
         <v>4293</v>
       </c>
@@ -5843,7 +5844,7 @@
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A179" s="28"/>
+      <c r="A179" s="23"/>
       <c r="B179" s="2">
         <v>7703</v>
       </c>
@@ -5871,7 +5872,7 @@
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A180" s="28"/>
+      <c r="A180" s="23"/>
       <c r="B180" s="2">
         <v>5541</v>
       </c>
@@ -5899,7 +5900,7 @@
       </c>
     </row>
     <row r="181" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="29"/>
+      <c r="A181" s="24"/>
       <c r="B181" s="6">
         <v>9182</v>
       </c>
@@ -5927,7 +5928,7 @@
       </c>
     </row>
     <row r="182" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="27" t="s">
+      <c r="A182" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B182" s="13">
@@ -5957,7 +5958,7 @@
       </c>
     </row>
     <row r="183" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="28"/>
+      <c r="A183" s="23"/>
       <c r="B183" s="12">
         <v>9001</v>
       </c>
@@ -5985,7 +5986,7 @@
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="28"/>
+      <c r="A184" s="23"/>
       <c r="B184" s="2">
         <v>7491</v>
       </c>
@@ -6013,7 +6014,7 @@
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A185" s="28"/>
+      <c r="A185" s="23"/>
       <c r="B185" s="2">
         <v>9531</v>
       </c>
@@ -6041,7 +6042,7 @@
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A186" s="28"/>
+      <c r="A186" s="23"/>
       <c r="B186" s="2">
         <v>9812</v>
       </c>
@@ -6069,7 +6070,7 @@
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A187" s="28"/>
+      <c r="A187" s="23"/>
       <c r="B187" s="2">
         <v>9279</v>
       </c>
@@ -6097,7 +6098,7 @@
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="28"/>
+      <c r="A188" s="23"/>
       <c r="B188" s="2">
         <v>4845</v>
       </c>
@@ -6125,7 +6126,7 @@
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A189" s="28"/>
+      <c r="A189" s="23"/>
       <c r="B189" s="2">
         <v>5728</v>
       </c>
@@ -6153,7 +6154,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A190" s="28"/>
+      <c r="A190" s="23"/>
       <c r="B190" s="2">
         <v>7222</v>
       </c>
@@ -6181,7 +6182,7 @@
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A191" s="28"/>
+      <c r="A191" s="23"/>
       <c r="B191" s="2">
         <v>5923</v>
       </c>
@@ -6209,7 +6210,7 @@
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A192" s="28"/>
+      <c r="A192" s="23"/>
       <c r="B192" s="2">
         <v>4265</v>
       </c>
@@ -6237,7 +6238,7 @@
       </c>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A193" s="28"/>
+      <c r="A193" s="23"/>
       <c r="B193" s="2">
         <v>2166</v>
       </c>
@@ -6265,7 +6266,7 @@
       </c>
     </row>
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A194" s="28"/>
+      <c r="A194" s="23"/>
       <c r="B194" s="2">
         <v>9116</v>
       </c>
@@ -6293,7 +6294,7 @@
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="28"/>
+      <c r="A195" s="23"/>
       <c r="B195" s="2">
         <v>9925</v>
       </c>
@@ -6321,7 +6322,7 @@
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A196" s="28"/>
+      <c r="A196" s="23"/>
       <c r="B196" s="2">
         <v>3657</v>
       </c>
@@ -6349,7 +6350,7 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="28"/>
+      <c r="A197" s="23"/>
       <c r="B197" s="2">
         <v>6599</v>
       </c>
@@ -6377,7 +6378,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="30"/>
+      <c r="A198" s="27"/>
       <c r="B198" s="9">
         <v>1618</v>
       </c>
@@ -6405,7 +6406,7 @@
       </c>
     </row>
     <row r="199" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="29"/>
+      <c r="A199" s="24"/>
       <c r="B199" s="6">
         <v>1703</v>
       </c>
@@ -6433,7 +6434,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="33" t="s">
+      <c r="A200" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B200" s="8">
@@ -6463,7 +6464,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="34"/>
+      <c r="A201" s="29"/>
       <c r="B201" s="2">
         <v>4488</v>
       </c>
@@ -6491,7 +6492,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="34"/>
+      <c r="A202" s="29"/>
       <c r="B202" s="2">
         <v>4954</v>
       </c>
@@ -6519,7 +6520,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="34"/>
+      <c r="A203" s="29"/>
       <c r="B203" s="2">
         <v>4642</v>
       </c>
@@ -6547,7 +6548,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="34"/>
+      <c r="A204" s="29"/>
       <c r="B204" s="2">
         <v>5537</v>
       </c>
@@ -6575,7 +6576,7 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="34"/>
+      <c r="A205" s="29"/>
       <c r="B205" s="2">
         <v>5847</v>
       </c>
@@ -6603,7 +6604,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="34"/>
+      <c r="A206" s="29"/>
       <c r="B206" s="2">
         <v>4769</v>
       </c>
@@ -6631,7 +6632,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="34"/>
+      <c r="A207" s="29"/>
       <c r="B207" s="2">
         <v>9930</v>
       </c>
@@ -6654,12 +6655,12 @@
       <c r="S207" s="2"/>
       <c r="T207" s="5"/>
       <c r="U207">
-        <f t="shared" ref="U207:U281" ca="1" si="6">IF(B207=$W$1,1,0)</f>
+        <f t="shared" ref="U207:U283" ca="1" si="6">IF(B207=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="34"/>
+      <c r="A208" s="29"/>
       <c r="B208" s="2">
         <v>6861</v>
       </c>
@@ -6687,7 +6688,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="34"/>
+      <c r="A209" s="29"/>
       <c r="B209" s="2">
         <v>3226</v>
       </c>
@@ -6715,7 +6716,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="34"/>
+      <c r="A210" s="29"/>
       <c r="B210" s="2">
         <v>4372</v>
       </c>
@@ -6743,7 +6744,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="34"/>
+      <c r="A211" s="29"/>
       <c r="B211" s="2">
         <v>4463</v>
       </c>
@@ -6771,7 +6772,7 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="34"/>
+      <c r="A212" s="29"/>
       <c r="B212" s="2">
         <v>1668</v>
       </c>
@@ -6799,7 +6800,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="34"/>
+      <c r="A213" s="29"/>
       <c r="B213" s="2">
         <v>9417</v>
       </c>
@@ -6827,7 +6828,7 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="34"/>
+      <c r="A214" s="29"/>
       <c r="B214" s="2">
         <v>3148</v>
       </c>
@@ -6855,7 +6856,7 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="34"/>
+      <c r="A215" s="29"/>
       <c r="B215" s="2">
         <v>2137</v>
       </c>
@@ -6883,7 +6884,7 @@
       </c>
     </row>
     <row r="216" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="35"/>
+      <c r="A216" s="30"/>
       <c r="B216" s="6">
         <v>5621</v>
       </c>
@@ -6911,7 +6912,7 @@
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A217" s="27" t="s">
+      <c r="A217" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B217" s="8">
@@ -6941,7 +6942,7 @@
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A218" s="28"/>
+      <c r="A218" s="23"/>
       <c r="B218" s="2">
         <v>3951</v>
       </c>
@@ -6969,7 +6970,7 @@
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A219" s="28"/>
+      <c r="A219" s="23"/>
       <c r="B219" s="2">
         <v>7343</v>
       </c>
@@ -6997,7 +6998,7 @@
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A220" s="28"/>
+      <c r="A220" s="23"/>
       <c r="B220" s="2">
         <v>7060</v>
       </c>
@@ -7025,7 +7026,7 @@
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A221" s="28"/>
+      <c r="A221" s="23"/>
       <c r="B221" s="2">
         <v>6409</v>
       </c>
@@ -7053,7 +7054,7 @@
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A222" s="28"/>
+      <c r="A222" s="23"/>
       <c r="B222" s="2">
         <v>2386</v>
       </c>
@@ -7081,7 +7082,7 @@
       </c>
     </row>
     <row r="223" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="28"/>
+      <c r="A223" s="23"/>
       <c r="B223" s="6">
         <v>7372</v>
       </c>
@@ -7105,7 +7106,7 @@
       <c r="T223" s="5"/>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A224" s="28"/>
+      <c r="A224" s="23"/>
       <c r="B224" s="2">
         <v>9159</v>
       </c>
@@ -7133,7 +7134,7 @@
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A225" s="28"/>
+      <c r="A225" s="23"/>
       <c r="B225" s="2">
         <v>5309</v>
       </c>
@@ -7161,7 +7162,7 @@
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A226" s="28"/>
+      <c r="A226" s="23"/>
       <c r="B226" s="2">
         <v>3290</v>
       </c>
@@ -7189,7 +7190,7 @@
       </c>
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A227" s="28"/>
+      <c r="A227" s="23"/>
       <c r="B227" s="2">
         <v>5345</v>
       </c>
@@ -7217,7 +7218,7 @@
       </c>
     </row>
     <row r="228" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="29"/>
+      <c r="A228" s="24"/>
       <c r="B228" s="6">
         <v>6812</v>
       </c>
@@ -7245,7 +7246,7 @@
       </c>
     </row>
     <row r="229" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="27" t="s">
+      <c r="A229" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B229" s="13">
@@ -7275,7 +7276,7 @@
       </c>
     </row>
     <row r="230" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A230" s="28"/>
+      <c r="A230" s="23"/>
       <c r="B230" s="12">
         <v>1516</v>
       </c>
@@ -7303,7 +7304,7 @@
       </c>
     </row>
     <row r="231" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A231" s="28"/>
+      <c r="A231" s="23"/>
       <c r="B231" s="12">
         <v>9062</v>
       </c>
@@ -7331,7 +7332,7 @@
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A232" s="28"/>
+      <c r="A232" s="23"/>
       <c r="B232" s="19">
         <v>8861</v>
       </c>
@@ -7359,7 +7360,7 @@
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A233" s="28"/>
+      <c r="A233" s="23"/>
       <c r="B233" s="2">
         <v>5164</v>
       </c>
@@ -7387,7 +7388,7 @@
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A234" s="28"/>
+      <c r="A234" s="23"/>
       <c r="B234" s="2">
         <v>2354</v>
       </c>
@@ -7415,7 +7416,7 @@
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A235" s="28"/>
+      <c r="A235" s="23"/>
       <c r="B235" s="2">
         <v>2030</v>
       </c>
@@ -7443,7 +7444,7 @@
       </c>
     </row>
     <row r="236" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="29"/>
+      <c r="A236" s="24"/>
       <c r="B236" s="6">
         <v>7649</v>
       </c>
@@ -7471,7 +7472,7 @@
       </c>
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A237" s="27" t="s">
+      <c r="A237" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B237" s="8">
@@ -7501,7 +7502,7 @@
       </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="28"/>
+      <c r="A238" s="23"/>
       <c r="B238" s="2">
         <v>3784</v>
       </c>
@@ -7529,7 +7530,7 @@
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="28"/>
+      <c r="A239" s="23"/>
       <c r="B239" s="2">
         <v>6732</v>
       </c>
@@ -7557,7 +7558,7 @@
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A240" s="28"/>
+      <c r="A240" s="23"/>
       <c r="B240" s="2">
         <v>6882</v>
       </c>
@@ -7585,7 +7586,7 @@
       </c>
     </row>
     <row r="241" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A241" s="28"/>
+      <c r="A241" s="23"/>
       <c r="B241" s="2">
         <v>1212</v>
       </c>
@@ -7613,7 +7614,7 @@
       </c>
     </row>
     <row r="242" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A242" s="28"/>
+      <c r="A242" s="23"/>
       <c r="B242" s="2">
         <v>9472</v>
       </c>
@@ -7641,7 +7642,7 @@
       </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="28"/>
+      <c r="A243" s="23"/>
       <c r="B243" s="2">
         <v>5081</v>
       </c>
@@ -7669,7 +7670,7 @@
       </c>
     </row>
     <row r="244" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="29"/>
+      <c r="A244" s="24"/>
       <c r="B244" s="6">
         <v>6454</v>
       </c>
@@ -7697,7 +7698,7 @@
       </c>
     </row>
     <row r="245" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="27" t="s">
+      <c r="A245" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B245" s="13">
@@ -7727,9 +7728,9 @@
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="28"/>
+      <c r="A246" s="23"/>
       <c r="B246" s="2">
-        <v>8403</v>
+        <v>6011</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7755,9 +7756,9 @@
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="28"/>
+      <c r="A247" s="23"/>
       <c r="B247" s="2">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7783,9 +7784,9 @@
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A248" s="28"/>
+      <c r="A248" s="23"/>
       <c r="B248" s="2">
-        <v>2092</v>
+        <v>3185</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7811,9 +7812,9 @@
       </c>
     </row>
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A249" s="28"/>
-      <c r="B249" s="2">
-        <v>9914</v>
+      <c r="A249" s="23"/>
+      <c r="B249" s="21">
+        <v>6037</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -7839,9 +7840,9 @@
       </c>
     </row>
     <row r="250" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A250" s="28"/>
+      <c r="A250" s="23"/>
       <c r="B250" s="2">
-        <v>6011</v>
+        <v>9914</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -7867,9 +7868,9 @@
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="28"/>
+      <c r="A251" s="23"/>
       <c r="B251" s="2">
-        <v>6037</v>
+        <v>4916</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7895,7 +7896,7 @@
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A252" s="28"/>
+      <c r="A252" s="23"/>
       <c r="B252" s="2">
         <v>2809</v>
       </c>
@@ -7923,9 +7924,9 @@
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A253" s="28"/>
+      <c r="A253" s="23"/>
       <c r="B253" s="2">
-        <v>7297</v>
+        <v>8265</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7951,9 +7952,9 @@
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" s="28"/>
+      <c r="A254" s="23"/>
       <c r="B254" s="2">
-        <v>5242</v>
+        <v>2092</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7979,9 +7980,9 @@
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A255" s="28"/>
+      <c r="A255" s="23"/>
       <c r="B255" s="2">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8007,9 +8008,9 @@
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="28"/>
+      <c r="A256" s="23"/>
       <c r="B256" s="2">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8035,9 +8036,9 @@
       </c>
     </row>
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A257" s="28"/>
+      <c r="A257" s="23"/>
       <c r="B257" s="2">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8063,9 +8064,9 @@
       </c>
     </row>
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A258" s="28"/>
+      <c r="A258" s="23"/>
       <c r="B258" s="2">
-        <v>9713</v>
+        <v>2401</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8091,9 +8092,9 @@
       </c>
     </row>
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A259" s="28"/>
+      <c r="A259" s="23"/>
       <c r="B259" s="2">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8119,9 +8120,9 @@
       </c>
     </row>
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="28"/>
+      <c r="A260" s="23"/>
       <c r="B260" s="2">
-        <v>2000</v>
+        <v>9713</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8147,9 +8148,9 @@
       </c>
     </row>
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A261" s="28"/>
+      <c r="A261" s="23"/>
       <c r="B261" s="2">
-        <v>5449</v>
+        <v>7301</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8175,9 +8176,9 @@
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="28"/>
+      <c r="A262" s="23"/>
       <c r="B262" s="2">
-        <v>2662</v>
+        <v>2000</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8203,9 +8204,9 @@
       </c>
     </row>
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A263" s="28"/>
+      <c r="A263" s="23"/>
       <c r="B263" s="2">
-        <v>4147</v>
+        <v>5449</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8231,9 +8232,9 @@
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A264" s="28"/>
+      <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>1953</v>
+        <v>2662</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8259,9 +8260,9 @@
       </c>
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A265" s="28"/>
+      <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8287,9 +8288,9 @@
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="28"/>
+      <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>5032</v>
+        <v>1953</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8315,9 +8316,9 @@
       </c>
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="28"/>
+      <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>3567</v>
+        <v>3956</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8343,9 +8344,9 @@
       </c>
     </row>
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="28"/>
+      <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>5108</v>
+        <v>5032</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8371,9 +8372,9 @@
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="28"/>
+      <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>2033</v>
+        <v>3567</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8399,9 +8400,9 @@
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="28"/>
+      <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>6981</v>
+        <v>5108</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8426,124 +8427,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="29"/>
-      <c r="B271" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C271" s="6"/>
-      <c r="D271" s="6"/>
-      <c r="E271" s="6"/>
-      <c r="F271" s="6"/>
-      <c r="G271" s="6"/>
-      <c r="H271" s="6"/>
-      <c r="I271" s="6"/>
-      <c r="J271" s="6"/>
-      <c r="K271" s="6"/>
-      <c r="L271" s="6"/>
-      <c r="M271" s="6"/>
-      <c r="N271" s="6"/>
-      <c r="O271" s="6"/>
-      <c r="P271" s="6"/>
-      <c r="Q271" s="6"/>
-      <c r="R271" s="6"/>
-      <c r="S271" s="6"/>
-      <c r="T271" s="7"/>
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A271" s="23"/>
+      <c r="B271" s="2">
+        <v>2033</v>
+      </c>
+      <c r="C271" s="2"/>
+      <c r="D271" s="2"/>
+      <c r="E271" s="2"/>
+      <c r="F271" s="2"/>
+      <c r="G271" s="2"/>
+      <c r="H271" s="2"/>
+      <c r="I271" s="2"/>
+      <c r="J271" s="2"/>
+      <c r="K271" s="2"/>
+      <c r="L271" s="2"/>
+      <c r="M271" s="2"/>
+      <c r="N271" s="2"/>
+      <c r="O271" s="2"/>
+      <c r="P271" s="2"/>
+      <c r="Q271" s="2"/>
+      <c r="R271" s="2"/>
+      <c r="S271" s="2"/>
+      <c r="T271" s="5"/>
       <c r="U271">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B272" s="8">
-        <v>8787</v>
-      </c>
-      <c r="C272" s="8"/>
-      <c r="D272" s="8"/>
-      <c r="E272" s="8"/>
-      <c r="F272" s="8"/>
-      <c r="G272" s="8"/>
-      <c r="H272" s="8"/>
-      <c r="I272" s="8"/>
-      <c r="J272" s="8"/>
-      <c r="K272" s="8"/>
-      <c r="L272" s="8"/>
-      <c r="M272" s="8"/>
-      <c r="N272" s="8"/>
-      <c r="O272" s="8"/>
-      <c r="P272" s="8"/>
-      <c r="Q272" s="8"/>
-      <c r="R272" s="8"/>
-      <c r="S272" s="8"/>
-      <c r="T272" s="14"/>
+      <c r="A272" s="23"/>
+      <c r="B272" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C272" s="2"/>
+      <c r="D272" s="2"/>
+      <c r="E272" s="2"/>
+      <c r="F272" s="2"/>
+      <c r="G272" s="2"/>
+      <c r="H272" s="2"/>
+      <c r="I272" s="2"/>
+      <c r="J272" s="2"/>
+      <c r="K272" s="2"/>
+      <c r="L272" s="2"/>
+      <c r="M272" s="2"/>
+      <c r="N272" s="2"/>
+      <c r="O272" s="2"/>
+      <c r="P272" s="2"/>
+      <c r="Q272" s="2"/>
+      <c r="R272" s="2"/>
+      <c r="S272" s="2"/>
+      <c r="T272" s="5"/>
       <c r="U272">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="28"/>
-      <c r="B273" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="E273" s="2"/>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="2"/>
-      <c r="J273" s="2"/>
-      <c r="K273" s="2"/>
-      <c r="L273" s="2"/>
-      <c r="M273" s="2"/>
-      <c r="N273" s="2"/>
-      <c r="O273" s="2"/>
-      <c r="P273" s="2"/>
-      <c r="Q273" s="2"/>
-      <c r="R273" s="2"/>
-      <c r="S273" s="2"/>
-      <c r="T273" s="5"/>
+    <row r="273" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A273" s="24"/>
+      <c r="B273" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C273" s="6"/>
+      <c r="D273" s="6"/>
+      <c r="E273" s="6"/>
+      <c r="F273" s="6"/>
+      <c r="G273" s="6"/>
+      <c r="H273" s="6"/>
+      <c r="I273" s="6"/>
+      <c r="J273" s="6"/>
+      <c r="K273" s="6"/>
+      <c r="L273" s="6"/>
+      <c r="M273" s="6"/>
+      <c r="N273" s="6"/>
+      <c r="O273" s="6"/>
+      <c r="P273" s="6"/>
+      <c r="Q273" s="6"/>
+      <c r="R273" s="6"/>
+      <c r="S273" s="6"/>
+      <c r="T273" s="7"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="28"/>
-      <c r="B274" s="2">
-        <v>9990</v>
-      </c>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2"/>
-      <c r="E274" s="2"/>
-      <c r="F274" s="2"/>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="2"/>
-      <c r="J274" s="2"/>
-      <c r="K274" s="2"/>
-      <c r="L274" s="2"/>
-      <c r="M274" s="2"/>
-      <c r="N274" s="2"/>
-      <c r="O274" s="2"/>
-      <c r="P274" s="2"/>
-      <c r="Q274" s="2"/>
-      <c r="R274" s="2"/>
-      <c r="S274" s="2"/>
-      <c r="T274" s="5"/>
+      <c r="A274" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B274" s="8">
+        <v>8787</v>
+      </c>
+      <c r="C274" s="8"/>
+      <c r="D274" s="8"/>
+      <c r="E274" s="8"/>
+      <c r="F274" s="8"/>
+      <c r="G274" s="8"/>
+      <c r="H274" s="8"/>
+      <c r="I274" s="8"/>
+      <c r="J274" s="8"/>
+      <c r="K274" s="8"/>
+      <c r="L274" s="8"/>
+      <c r="M274" s="8"/>
+      <c r="N274" s="8"/>
+      <c r="O274" s="8"/>
+      <c r="P274" s="8"/>
+      <c r="Q274" s="8"/>
+      <c r="R274" s="8"/>
+      <c r="S274" s="8"/>
+      <c r="T274" s="14"/>
       <c r="U274">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="28"/>
+      <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>7738</v>
+        <v>5087</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8569,9 +8570,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="28"/>
+      <c r="A276" s="23"/>
       <c r="B276" s="2">
-        <v>9924</v>
+        <v>9990</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8597,65 +8598,65 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="30"/>
-      <c r="B277" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C277" s="9"/>
-      <c r="D277" s="9"/>
-      <c r="E277" s="9"/>
-      <c r="F277" s="9"/>
-      <c r="G277" s="9"/>
-      <c r="H277" s="9"/>
-      <c r="I277" s="9"/>
-      <c r="J277" s="9"/>
-      <c r="K277" s="9"/>
-      <c r="L277" s="9"/>
-      <c r="M277" s="9"/>
-      <c r="N277" s="9"/>
-      <c r="O277" s="9"/>
-      <c r="P277" s="9"/>
-      <c r="Q277" s="9"/>
-      <c r="R277" s="9"/>
-      <c r="S277" s="9"/>
-      <c r="T277" s="15"/>
+      <c r="A277" s="23"/>
+      <c r="B277" s="2">
+        <v>7738</v>
+      </c>
+      <c r="C277" s="2"/>
+      <c r="D277" s="2"/>
+      <c r="E277" s="2"/>
+      <c r="F277" s="2"/>
+      <c r="G277" s="2"/>
+      <c r="H277" s="2"/>
+      <c r="I277" s="2"/>
+      <c r="J277" s="2"/>
+      <c r="K277" s="2"/>
+      <c r="L277" s="2"/>
+      <c r="M277" s="2"/>
+      <c r="N277" s="2"/>
+      <c r="O277" s="2"/>
+      <c r="P277" s="2"/>
+      <c r="Q277" s="2"/>
+      <c r="R277" s="2"/>
+      <c r="S277" s="2"/>
+      <c r="T277" s="5"/>
       <c r="U277">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A278" s="30"/>
-      <c r="B278" s="9">
-        <v>2973</v>
-      </c>
-      <c r="C278" s="9"/>
-      <c r="D278" s="9"/>
-      <c r="E278" s="9"/>
-      <c r="F278" s="9"/>
-      <c r="G278" s="9"/>
-      <c r="H278" s="9"/>
-      <c r="I278" s="9"/>
-      <c r="J278" s="9"/>
-      <c r="K278" s="9"/>
-      <c r="L278" s="9"/>
-      <c r="M278" s="9"/>
-      <c r="N278" s="9"/>
-      <c r="O278" s="9"/>
-      <c r="P278" s="9"/>
-      <c r="Q278" s="9"/>
-      <c r="R278" s="9"/>
-      <c r="S278" s="9"/>
-      <c r="T278" s="15"/>
+      <c r="A278" s="23"/>
+      <c r="B278" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C278" s="2"/>
+      <c r="D278" s="2"/>
+      <c r="E278" s="2"/>
+      <c r="F278" s="2"/>
+      <c r="G278" s="2"/>
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+      <c r="L278" s="2"/>
+      <c r="M278" s="2"/>
+      <c r="N278" s="2"/>
+      <c r="O278" s="2"/>
+      <c r="P278" s="2"/>
+      <c r="Q278" s="2"/>
+      <c r="R278" s="2"/>
+      <c r="S278" s="2"/>
+      <c r="T278" s="5"/>
       <c r="U278">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="30"/>
+      <c r="A279" s="27"/>
       <c r="B279" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C279" s="9"/>
       <c r="D279" s="9"/>
@@ -8681,9 +8682,9 @@
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="30"/>
+      <c r="A280" s="27"/>
       <c r="B280" s="9">
-        <v>7186</v>
+        <v>2973</v>
       </c>
       <c r="C280" s="9"/>
       <c r="D280" s="9"/>
@@ -8709,9 +8710,9 @@
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="30"/>
+      <c r="A281" s="27"/>
       <c r="B281" s="9">
-        <v>1457</v>
+        <v>8258</v>
       </c>
       <c r="C281" s="9"/>
       <c r="D281" s="9"/>
@@ -8736,124 +8737,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="29"/>
-      <c r="B282" s="6">
+    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A282" s="27"/>
+      <c r="B282" s="9">
+        <v>7186</v>
+      </c>
+      <c r="C282" s="9"/>
+      <c r="D282" s="9"/>
+      <c r="E282" s="9"/>
+      <c r="F282" s="9"/>
+      <c r="G282" s="9"/>
+      <c r="H282" s="9"/>
+      <c r="I282" s="9"/>
+      <c r="J282" s="9"/>
+      <c r="K282" s="9"/>
+      <c r="L282" s="9"/>
+      <c r="M282" s="9"/>
+      <c r="N282" s="9"/>
+      <c r="O282" s="9"/>
+      <c r="P282" s="9"/>
+      <c r="Q282" s="9"/>
+      <c r="R282" s="9"/>
+      <c r="S282" s="9"/>
+      <c r="T282" s="15"/>
+      <c r="U282">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A283" s="27"/>
+      <c r="B283" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C283" s="9"/>
+      <c r="D283" s="9"/>
+      <c r="E283" s="9"/>
+      <c r="F283" s="9"/>
+      <c r="G283" s="9"/>
+      <c r="H283" s="9"/>
+      <c r="I283" s="9"/>
+      <c r="J283" s="9"/>
+      <c r="K283" s="9"/>
+      <c r="L283" s="9"/>
+      <c r="M283" s="9"/>
+      <c r="N283" s="9"/>
+      <c r="O283" s="9"/>
+      <c r="P283" s="9"/>
+      <c r="Q283" s="9"/>
+      <c r="R283" s="9"/>
+      <c r="S283" s="9"/>
+      <c r="T283" s="15"/>
+      <c r="U283">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A284" s="24"/>
+      <c r="B284" s="6">
         <v>6876</v>
       </c>
-      <c r="C282" s="6"/>
-      <c r="D282" s="6"/>
-      <c r="E282" s="6"/>
-      <c r="F282" s="6"/>
-      <c r="G282" s="6"/>
-      <c r="H282" s="6"/>
-      <c r="I282" s="6"/>
-      <c r="J282" s="6"/>
-      <c r="K282" s="6"/>
-      <c r="L282" s="6"/>
-      <c r="M282" s="6"/>
-      <c r="N282" s="6"/>
-      <c r="O282" s="6"/>
-      <c r="P282" s="6"/>
-      <c r="Q282" s="6"/>
-      <c r="R282" s="6"/>
-      <c r="S282" s="6"/>
-      <c r="T282" s="7"/>
-      <c r="U282">
-        <f t="shared" ref="U282:U345" ca="1" si="7">IF(B282=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="27" t="s">
+      <c r="C284" s="6"/>
+      <c r="D284" s="6"/>
+      <c r="E284" s="6"/>
+      <c r="F284" s="6"/>
+      <c r="G284" s="6"/>
+      <c r="H284" s="6"/>
+      <c r="I284" s="6"/>
+      <c r="J284" s="6"/>
+      <c r="K284" s="6"/>
+      <c r="L284" s="6"/>
+      <c r="M284" s="6"/>
+      <c r="N284" s="6"/>
+      <c r="O284" s="6"/>
+      <c r="P284" s="6"/>
+      <c r="Q284" s="6"/>
+      <c r="R284" s="6"/>
+      <c r="S284" s="6"/>
+      <c r="T284" s="7"/>
+      <c r="U284">
+        <f t="shared" ref="U284:U347" ca="1" si="7">IF(B284=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A285" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B283" s="8">
+      <c r="B285" s="8">
         <v>4304</v>
       </c>
-      <c r="C283" s="8"/>
-      <c r="D283" s="8"/>
-      <c r="E283" s="8"/>
-      <c r="F283" s="8"/>
-      <c r="G283" s="8"/>
-      <c r="H283" s="8"/>
-      <c r="I283" s="8"/>
-      <c r="J283" s="8"/>
-      <c r="K283" s="8"/>
-      <c r="L283" s="8"/>
-      <c r="M283" s="8"/>
-      <c r="N283" s="8"/>
-      <c r="O283" s="8"/>
-      <c r="P283" s="8"/>
-      <c r="Q283" s="8"/>
-      <c r="R283" s="8"/>
-      <c r="S283" s="8"/>
-      <c r="T283" s="14"/>
-      <c r="U283">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="28"/>
-      <c r="B284" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C284" s="2"/>
-      <c r="D284" s="2"/>
-      <c r="E284" s="2"/>
-      <c r="F284" s="2"/>
-      <c r="G284" s="2"/>
-      <c r="H284" s="2"/>
-      <c r="I284" s="2"/>
-      <c r="J284" s="2"/>
-      <c r="K284" s="2"/>
-      <c r="L284" s="2"/>
-      <c r="M284" s="2"/>
-      <c r="N284" s="2"/>
-      <c r="O284" s="2"/>
-      <c r="P284" s="2"/>
-      <c r="Q284" s="2"/>
-      <c r="R284" s="2"/>
-      <c r="S284" s="2"/>
-      <c r="T284" s="5"/>
-      <c r="U284">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="28"/>
-      <c r="B285" s="2">
-        <v>7693</v>
-      </c>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2"/>
-      <c r="E285" s="2"/>
-      <c r="F285" s="2"/>
-      <c r="G285" s="2"/>
-      <c r="H285" s="2"/>
-      <c r="I285" s="2"/>
-      <c r="J285" s="2"/>
-      <c r="K285" s="2"/>
-      <c r="L285" s="2"/>
-      <c r="M285" s="2"/>
-      <c r="N285" s="2"/>
-      <c r="O285" s="2"/>
-      <c r="P285" s="2"/>
-      <c r="Q285" s="2"/>
-      <c r="R285" s="2"/>
-      <c r="S285" s="2"/>
-      <c r="T285" s="5"/>
+      <c r="C285" s="8"/>
+      <c r="D285" s="8"/>
+      <c r="E285" s="8"/>
+      <c r="F285" s="8"/>
+      <c r="G285" s="8"/>
+      <c r="H285" s="8"/>
+      <c r="I285" s="8"/>
+      <c r="J285" s="8"/>
+      <c r="K285" s="8"/>
+      <c r="L285" s="8"/>
+      <c r="M285" s="8"/>
+      <c r="N285" s="8"/>
+      <c r="O285" s="8"/>
+      <c r="P285" s="8"/>
+      <c r="Q285" s="8"/>
+      <c r="R285" s="8"/>
+      <c r="S285" s="8"/>
+      <c r="T285" s="14"/>
       <c r="U285">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="28"/>
+      <c r="A286" s="23"/>
       <c r="B286" s="2">
-        <v>8718</v>
+        <v>2070</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8878,124 +8879,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="29"/>
-      <c r="B287" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C287" s="6"/>
-      <c r="D287" s="6"/>
-      <c r="E287" s="6"/>
-      <c r="F287" s="6"/>
-      <c r="G287" s="6"/>
-      <c r="H287" s="6"/>
-      <c r="I287" s="6"/>
-      <c r="J287" s="6"/>
-      <c r="K287" s="6"/>
-      <c r="L287" s="6"/>
-      <c r="M287" s="6"/>
-      <c r="N287" s="6"/>
-      <c r="O287" s="6"/>
-      <c r="P287" s="6"/>
-      <c r="Q287" s="6"/>
-      <c r="R287" s="6"/>
-      <c r="S287" s="6"/>
-      <c r="T287" s="7"/>
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A287" s="23"/>
+      <c r="B287" s="2">
+        <v>7693</v>
+      </c>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
+      <c r="E287" s="2"/>
+      <c r="F287" s="2"/>
+      <c r="G287" s="2"/>
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+      <c r="J287" s="2"/>
+      <c r="K287" s="2"/>
+      <c r="L287" s="2"/>
+      <c r="M287" s="2"/>
+      <c r="N287" s="2"/>
+      <c r="O287" s="2"/>
+      <c r="P287" s="2"/>
+      <c r="Q287" s="2"/>
+      <c r="R287" s="2"/>
+      <c r="S287" s="2"/>
+      <c r="T287" s="5"/>
       <c r="U287">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A288" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B288" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C288" s="8"/>
-      <c r="D288" s="8"/>
-      <c r="E288" s="8"/>
-      <c r="F288" s="8"/>
-      <c r="G288" s="8"/>
-      <c r="H288" s="8"/>
-      <c r="I288" s="8"/>
-      <c r="J288" s="8"/>
-      <c r="K288" s="8"/>
-      <c r="L288" s="8"/>
-      <c r="M288" s="8"/>
-      <c r="N288" s="8"/>
-      <c r="O288" s="8"/>
-      <c r="P288" s="8"/>
-      <c r="Q288" s="8"/>
-      <c r="R288" s="8"/>
-      <c r="S288" s="8"/>
-      <c r="T288" s="14"/>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A288" s="23"/>
+      <c r="B288" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C288" s="2"/>
+      <c r="D288" s="2"/>
+      <c r="E288" s="2"/>
+      <c r="F288" s="2"/>
+      <c r="G288" s="2"/>
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+      <c r="J288" s="2"/>
+      <c r="K288" s="2"/>
+      <c r="L288" s="2"/>
+      <c r="M288" s="2"/>
+      <c r="N288" s="2"/>
+      <c r="O288" s="2"/>
+      <c r="P288" s="2"/>
+      <c r="Q288" s="2"/>
+      <c r="R288" s="2"/>
+      <c r="S288" s="2"/>
+      <c r="T288" s="5"/>
       <c r="U288">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A289" s="28"/>
-      <c r="B289" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="E289" s="2"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
-      <c r="I289" s="2"/>
-      <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-      <c r="N289" s="2"/>
-      <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-      <c r="Q289" s="2"/>
-      <c r="R289" s="2"/>
-      <c r="S289" s="2"/>
-      <c r="T289" s="5"/>
+    <row r="289" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="24"/>
+      <c r="B289" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
+      <c r="E289" s="6"/>
+      <c r="F289" s="6"/>
+      <c r="G289" s="6"/>
+      <c r="H289" s="6"/>
+      <c r="I289" s="6"/>
+      <c r="J289" s="6"/>
+      <c r="K289" s="6"/>
+      <c r="L289" s="6"/>
+      <c r="M289" s="6"/>
+      <c r="N289" s="6"/>
+      <c r="O289" s="6"/>
+      <c r="P289" s="6"/>
+      <c r="Q289" s="6"/>
+      <c r="R289" s="6"/>
+      <c r="S289" s="6"/>
+      <c r="T289" s="7"/>
       <c r="U289">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A290" s="28"/>
-      <c r="B290" s="12">
-        <v>7546</v>
-      </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="E290" s="2"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
-      <c r="I290" s="2"/>
-      <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-      <c r="N290" s="2"/>
-      <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-      <c r="Q290" s="2"/>
-      <c r="R290" s="2"/>
-      <c r="S290" s="2"/>
-      <c r="T290" s="5"/>
+      <c r="A290" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B290" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C290" s="8"/>
+      <c r="D290" s="8"/>
+      <c r="E290" s="8"/>
+      <c r="F290" s="8"/>
+      <c r="G290" s="8"/>
+      <c r="H290" s="8"/>
+      <c r="I290" s="8"/>
+      <c r="J290" s="8"/>
+      <c r="K290" s="8"/>
+      <c r="L290" s="8"/>
+      <c r="M290" s="8"/>
+      <c r="N290" s="8"/>
+      <c r="O290" s="8"/>
+      <c r="P290" s="8"/>
+      <c r="Q290" s="8"/>
+      <c r="R290" s="8"/>
+      <c r="S290" s="8"/>
+      <c r="T290" s="14"/>
       <c r="U290">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A291" s="28"/>
-      <c r="B291" s="2">
-        <v>7170</v>
+    <row r="291" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A291" s="23"/>
+      <c r="B291" s="12">
+        <v>3083</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9020,10 +9021,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A292" s="28"/>
-      <c r="B292" s="2">
-        <v>2709</v>
+    <row r="292" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A292" s="23"/>
+      <c r="B292" s="12">
+        <v>7546</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9049,9 +9050,9 @@
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="28"/>
+      <c r="A293" s="23"/>
       <c r="B293" s="2">
-        <v>3402</v>
+        <v>7170</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9077,9 +9078,9 @@
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="28"/>
+      <c r="A294" s="23"/>
       <c r="B294" s="2">
-        <v>8781</v>
+        <v>2709</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9105,9 +9106,9 @@
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="28"/>
+      <c r="A295" s="23"/>
       <c r="B295" s="2">
-        <v>8771</v>
+        <v>3402</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9133,9 +9134,9 @@
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A296" s="28"/>
+      <c r="A296" s="23"/>
       <c r="B296" s="2">
-        <v>3091</v>
+        <v>8781</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9161,9 +9162,9 @@
       </c>
     </row>
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A297" s="28"/>
+      <c r="A297" s="23"/>
       <c r="B297" s="2">
-        <v>2195</v>
+        <v>8771</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9189,9 +9190,9 @@
       </c>
     </row>
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A298" s="28"/>
+      <c r="A298" s="23"/>
       <c r="B298" s="2">
-        <v>1184</v>
+        <v>3091</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9217,9 +9218,9 @@
       </c>
     </row>
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A299" s="28"/>
+      <c r="A299" s="23"/>
       <c r="B299" s="2">
-        <v>2667</v>
+        <v>2195</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9245,9 +9246,9 @@
       </c>
     </row>
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A300" s="28"/>
+      <c r="A300" s="23"/>
       <c r="B300" s="2">
-        <v>5917</v>
+        <v>1184</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9273,9 +9274,9 @@
       </c>
     </row>
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="28"/>
+      <c r="A301" s="23"/>
       <c r="B301" s="2">
-        <v>8545</v>
+        <v>2667</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9301,9 +9302,9 @@
       </c>
     </row>
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A302" s="28"/>
+      <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>1288</v>
+        <v>5917</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9328,124 +9329,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A303" s="29"/>
-      <c r="B303" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C303" s="6"/>
-      <c r="D303" s="6"/>
-      <c r="E303" s="6"/>
-      <c r="F303" s="6"/>
-      <c r="G303" s="6"/>
-      <c r="H303" s="6"/>
-      <c r="I303" s="6"/>
-      <c r="J303" s="6"/>
-      <c r="K303" s="6"/>
-      <c r="L303" s="6"/>
-      <c r="M303" s="6"/>
-      <c r="N303" s="6"/>
-      <c r="O303" s="6"/>
-      <c r="P303" s="6"/>
-      <c r="Q303" s="6"/>
-      <c r="R303" s="6"/>
-      <c r="S303" s="6"/>
-      <c r="T303" s="7"/>
+    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A303" s="23"/>
+      <c r="B303" s="2">
+        <v>8545</v>
+      </c>
+      <c r="C303" s="2"/>
+      <c r="D303" s="2"/>
+      <c r="E303" s="2"/>
+      <c r="F303" s="2"/>
+      <c r="G303" s="2"/>
+      <c r="H303" s="2"/>
+      <c r="I303" s="2"/>
+      <c r="J303" s="2"/>
+      <c r="K303" s="2"/>
+      <c r="L303" s="2"/>
+      <c r="M303" s="2"/>
+      <c r="N303" s="2"/>
+      <c r="O303" s="2"/>
+      <c r="P303" s="2"/>
+      <c r="Q303" s="2"/>
+      <c r="R303" s="2"/>
+      <c r="S303" s="2"/>
+      <c r="T303" s="5"/>
       <c r="U303">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A304" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B304" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C304" s="8"/>
-      <c r="D304" s="8"/>
-      <c r="E304" s="8"/>
-      <c r="F304" s="8"/>
-      <c r="G304" s="8"/>
-      <c r="H304" s="8"/>
-      <c r="I304" s="8"/>
-      <c r="J304" s="8"/>
-      <c r="K304" s="8"/>
-      <c r="L304" s="8"/>
-      <c r="M304" s="8"/>
-      <c r="N304" s="8"/>
-      <c r="O304" s="8"/>
-      <c r="P304" s="8"/>
-      <c r="Q304" s="8"/>
-      <c r="R304" s="8"/>
-      <c r="S304" s="8"/>
-      <c r="T304" s="14"/>
+      <c r="A304" s="23"/>
+      <c r="B304" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C304" s="2"/>
+      <c r="D304" s="2"/>
+      <c r="E304" s="2"/>
+      <c r="F304" s="2"/>
+      <c r="G304" s="2"/>
+      <c r="H304" s="2"/>
+      <c r="I304" s="2"/>
+      <c r="J304" s="2"/>
+      <c r="K304" s="2"/>
+      <c r="L304" s="2"/>
+      <c r="M304" s="2"/>
+      <c r="N304" s="2"/>
+      <c r="O304" s="2"/>
+      <c r="P304" s="2"/>
+      <c r="Q304" s="2"/>
+      <c r="R304" s="2"/>
+      <c r="S304" s="2"/>
+      <c r="T304" s="5"/>
       <c r="U304">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A305" s="28"/>
-      <c r="B305" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C305" s="2"/>
-      <c r="D305" s="2"/>
-      <c r="E305" s="2"/>
-      <c r="F305" s="2"/>
-      <c r="G305" s="2"/>
-      <c r="H305" s="2"/>
-      <c r="I305" s="2"/>
-      <c r="J305" s="2"/>
-      <c r="K305" s="2"/>
-      <c r="L305" s="2"/>
-      <c r="M305" s="2"/>
-      <c r="N305" s="2"/>
-      <c r="O305" s="2"/>
-      <c r="P305" s="2"/>
-      <c r="Q305" s="2"/>
-      <c r="R305" s="2"/>
-      <c r="S305" s="2"/>
-      <c r="T305" s="5"/>
+    <row r="305" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="24"/>
+      <c r="B305" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C305" s="6"/>
+      <c r="D305" s="6"/>
+      <c r="E305" s="6"/>
+      <c r="F305" s="6"/>
+      <c r="G305" s="6"/>
+      <c r="H305" s="6"/>
+      <c r="I305" s="6"/>
+      <c r="J305" s="6"/>
+      <c r="K305" s="6"/>
+      <c r="L305" s="6"/>
+      <c r="M305" s="6"/>
+      <c r="N305" s="6"/>
+      <c r="O305" s="6"/>
+      <c r="P305" s="6"/>
+      <c r="Q305" s="6"/>
+      <c r="R305" s="6"/>
+      <c r="S305" s="6"/>
+      <c r="T305" s="7"/>
       <c r="U305">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A306" s="28"/>
-      <c r="B306" s="2">
-        <v>3093</v>
-      </c>
-      <c r="C306" s="2"/>
-      <c r="D306" s="2"/>
-      <c r="E306" s="2"/>
-      <c r="F306" s="2"/>
-      <c r="G306" s="2"/>
-      <c r="H306" s="2"/>
-      <c r="I306" s="2"/>
-      <c r="J306" s="2"/>
-      <c r="K306" s="2"/>
-      <c r="L306" s="2"/>
-      <c r="M306" s="2"/>
-      <c r="N306" s="2"/>
-      <c r="O306" s="2"/>
-      <c r="P306" s="2"/>
-      <c r="Q306" s="2"/>
-      <c r="R306" s="2"/>
-      <c r="S306" s="2"/>
-      <c r="T306" s="5"/>
+      <c r="A306" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B306" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C306" s="8"/>
+      <c r="D306" s="8"/>
+      <c r="E306" s="8"/>
+      <c r="F306" s="8"/>
+      <c r="G306" s="8"/>
+      <c r="H306" s="8"/>
+      <c r="I306" s="8"/>
+      <c r="J306" s="8"/>
+      <c r="K306" s="8"/>
+      <c r="L306" s="8"/>
+      <c r="M306" s="8"/>
+      <c r="N306" s="8"/>
+      <c r="O306" s="8"/>
+      <c r="P306" s="8"/>
+      <c r="Q306" s="8"/>
+      <c r="R306" s="8"/>
+      <c r="S306" s="8"/>
+      <c r="T306" s="14"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A307" s="28"/>
+      <c r="A307" s="23"/>
       <c r="B307" s="2">
-        <v>8805</v>
+        <v>6598</v>
       </c>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
@@ -9471,9 +9472,9 @@
       </c>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A308" s="28"/>
+      <c r="A308" s="23"/>
       <c r="B308" s="2">
-        <v>8158</v>
+        <v>3093</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -9498,124 +9499,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="29"/>
-      <c r="B309" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C309" s="6"/>
-      <c r="D309" s="6"/>
-      <c r="E309" s="6"/>
-      <c r="F309" s="6"/>
-      <c r="G309" s="6"/>
-      <c r="H309" s="6"/>
-      <c r="I309" s="6"/>
-      <c r="J309" s="6"/>
-      <c r="K309" s="6"/>
-      <c r="L309" s="6"/>
-      <c r="M309" s="6"/>
-      <c r="N309" s="6"/>
-      <c r="O309" s="6"/>
-      <c r="P309" s="6"/>
-      <c r="Q309" s="6"/>
-      <c r="R309" s="6"/>
-      <c r="S309" s="6"/>
-      <c r="T309" s="7"/>
+    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A309" s="23"/>
+      <c r="B309" s="2">
+        <v>8805</v>
+      </c>
+      <c r="C309" s="2"/>
+      <c r="D309" s="2"/>
+      <c r="E309" s="2"/>
+      <c r="F309" s="2"/>
+      <c r="G309" s="2"/>
+      <c r="H309" s="2"/>
+      <c r="I309" s="2"/>
+      <c r="J309" s="2"/>
+      <c r="K309" s="2"/>
+      <c r="L309" s="2"/>
+      <c r="M309" s="2"/>
+      <c r="N309" s="2"/>
+      <c r="O309" s="2"/>
+      <c r="P309" s="2"/>
+      <c r="Q309" s="2"/>
+      <c r="R309" s="2"/>
+      <c r="S309" s="2"/>
+      <c r="T309" s="5"/>
       <c r="U309">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A310" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B310" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C310" s="8"/>
-      <c r="D310" s="8"/>
-      <c r="E310" s="8"/>
-      <c r="F310" s="8"/>
-      <c r="G310" s="8"/>
-      <c r="H310" s="8"/>
-      <c r="I310" s="8"/>
-      <c r="J310" s="8"/>
-      <c r="K310" s="8"/>
-      <c r="L310" s="8"/>
-      <c r="M310" s="8"/>
-      <c r="N310" s="8"/>
-      <c r="O310" s="8"/>
-      <c r="P310" s="8"/>
-      <c r="Q310" s="8"/>
-      <c r="R310" s="8"/>
-      <c r="S310" s="8"/>
-      <c r="T310" s="14"/>
+      <c r="A310" s="23"/>
+      <c r="B310" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C310" s="2"/>
+      <c r="D310" s="2"/>
+      <c r="E310" s="2"/>
+      <c r="F310" s="2"/>
+      <c r="G310" s="2"/>
+      <c r="H310" s="2"/>
+      <c r="I310" s="2"/>
+      <c r="J310" s="2"/>
+      <c r="K310" s="2"/>
+      <c r="L310" s="2"/>
+      <c r="M310" s="2"/>
+      <c r="N310" s="2"/>
+      <c r="O310" s="2"/>
+      <c r="P310" s="2"/>
+      <c r="Q310" s="2"/>
+      <c r="R310" s="2"/>
+      <c r="S310" s="2"/>
+      <c r="T310" s="5"/>
       <c r="U310">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A311" s="28"/>
-      <c r="B311" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C311" s="2"/>
-      <c r="D311" s="2"/>
-      <c r="E311" s="2"/>
-      <c r="F311" s="2"/>
-      <c r="G311" s="2"/>
-      <c r="H311" s="2"/>
-      <c r="I311" s="2"/>
-      <c r="J311" s="2"/>
-      <c r="K311" s="2"/>
-      <c r="L311" s="2"/>
-      <c r="M311" s="2"/>
-      <c r="N311" s="2"/>
-      <c r="O311" s="2"/>
-      <c r="P311" s="2"/>
-      <c r="Q311" s="2"/>
-      <c r="R311" s="2"/>
-      <c r="S311" s="2"/>
-      <c r="T311" s="5"/>
+    <row r="311" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="24"/>
+      <c r="B311" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C311" s="6"/>
+      <c r="D311" s="6"/>
+      <c r="E311" s="6"/>
+      <c r="F311" s="6"/>
+      <c r="G311" s="6"/>
+      <c r="H311" s="6"/>
+      <c r="I311" s="6"/>
+      <c r="J311" s="6"/>
+      <c r="K311" s="6"/>
+      <c r="L311" s="6"/>
+      <c r="M311" s="6"/>
+      <c r="N311" s="6"/>
+      <c r="O311" s="6"/>
+      <c r="P311" s="6"/>
+      <c r="Q311" s="6"/>
+      <c r="R311" s="6"/>
+      <c r="S311" s="6"/>
+      <c r="T311" s="7"/>
       <c r="U311">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A312" s="28"/>
-      <c r="B312" s="2">
-        <v>9002</v>
-      </c>
-      <c r="C312" s="2"/>
-      <c r="D312" s="2"/>
-      <c r="E312" s="2"/>
-      <c r="F312" s="2"/>
-      <c r="G312" s="2"/>
-      <c r="H312" s="2"/>
-      <c r="I312" s="2"/>
-      <c r="J312" s="2"/>
-      <c r="K312" s="2"/>
-      <c r="L312" s="2"/>
-      <c r="M312" s="2"/>
-      <c r="N312" s="2"/>
-      <c r="O312" s="2"/>
-      <c r="P312" s="2"/>
-      <c r="Q312" s="2"/>
-      <c r="R312" s="2"/>
-      <c r="S312" s="2"/>
-      <c r="T312" s="5"/>
+      <c r="A312" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B312" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C312" s="8"/>
+      <c r="D312" s="8"/>
+      <c r="E312" s="8"/>
+      <c r="F312" s="8"/>
+      <c r="G312" s="8"/>
+      <c r="H312" s="8"/>
+      <c r="I312" s="8"/>
+      <c r="J312" s="8"/>
+      <c r="K312" s="8"/>
+      <c r="L312" s="8"/>
+      <c r="M312" s="8"/>
+      <c r="N312" s="8"/>
+      <c r="O312" s="8"/>
+      <c r="P312" s="8"/>
+      <c r="Q312" s="8"/>
+      <c r="R312" s="8"/>
+      <c r="S312" s="8"/>
+      <c r="T312" s="14"/>
       <c r="U312">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A313" s="28"/>
+      <c r="A313" s="23"/>
       <c r="B313" s="2">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
@@ -9641,9 +9642,9 @@
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="28"/>
+      <c r="A314" s="23"/>
       <c r="B314" s="2">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -9668,41 +9669,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A315" s="29"/>
-      <c r="B315" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C315" s="6"/>
-      <c r="D315" s="6"/>
-      <c r="E315" s="6"/>
-      <c r="F315" s="6"/>
-      <c r="G315" s="6"/>
-      <c r="H315" s="6"/>
-      <c r="I315" s="6"/>
-      <c r="J315" s="6"/>
-      <c r="K315" s="6"/>
-      <c r="L315" s="6"/>
-      <c r="M315" s="6"/>
-      <c r="N315" s="6"/>
-      <c r="O315" s="6"/>
-      <c r="P315" s="6"/>
-      <c r="Q315" s="6"/>
-      <c r="R315" s="6"/>
-      <c r="S315" s="6"/>
-      <c r="T315" s="7"/>
+    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A315" s="23"/>
+      <c r="B315" s="2">
+        <v>7432</v>
+      </c>
+      <c r="C315" s="2"/>
+      <c r="D315" s="2"/>
+      <c r="E315" s="2"/>
+      <c r="F315" s="2"/>
+      <c r="G315" s="2"/>
+      <c r="H315" s="2"/>
+      <c r="I315" s="2"/>
+      <c r="J315" s="2"/>
+      <c r="K315" s="2"/>
+      <c r="L315" s="2"/>
+      <c r="M315" s="2"/>
+      <c r="N315" s="2"/>
+      <c r="O315" s="2"/>
+      <c r="P315" s="2"/>
+      <c r="Q315" s="2"/>
+      <c r="R315" s="2"/>
+      <c r="S315" s="2"/>
+      <c r="T315" s="5"/>
       <c r="U315">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A316" s="23"/>
+      <c r="B316" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C316" s="2"/>
+      <c r="D316" s="2"/>
+      <c r="E316" s="2"/>
+      <c r="F316" s="2"/>
+      <c r="G316" s="2"/>
+      <c r="H316" s="2"/>
+      <c r="I316" s="2"/>
+      <c r="J316" s="2"/>
+      <c r="K316" s="2"/>
+      <c r="L316" s="2"/>
+      <c r="M316" s="2"/>
+      <c r="N316" s="2"/>
+      <c r="O316" s="2"/>
+      <c r="P316" s="2"/>
+      <c r="Q316" s="2"/>
+      <c r="R316" s="2"/>
+      <c r="S316" s="2"/>
+      <c r="T316" s="5"/>
       <c r="U316">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="24"/>
+      <c r="B317" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C317" s="6"/>
+      <c r="D317" s="6"/>
+      <c r="E317" s="6"/>
+      <c r="F317" s="6"/>
+      <c r="G317" s="6"/>
+      <c r="H317" s="6"/>
+      <c r="I317" s="6"/>
+      <c r="J317" s="6"/>
+      <c r="K317" s="6"/>
+      <c r="L317" s="6"/>
+      <c r="M317" s="6"/>
+      <c r="N317" s="6"/>
+      <c r="O317" s="6"/>
+      <c r="P317" s="6"/>
+      <c r="Q317" s="6"/>
+      <c r="R317" s="6"/>
+      <c r="S317" s="6"/>
+      <c r="T317" s="7"/>
       <c r="U317">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9878,19 +9923,19 @@
     </row>
     <row r="346" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U346">
-        <f t="shared" ref="U346:U409" ca="1" si="8">IF(B346=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="347" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U347">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="348" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U348">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U348:U411" ca="1" si="8">IF(B348=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10262,19 +10307,19 @@
     </row>
     <row r="410" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U410">
-        <f t="shared" ref="U410:U473" ca="1" si="9">IF(B410=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="411" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U411">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="412" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U412">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U412:U475" ca="1" si="9">IF(B412=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10646,19 +10691,19 @@
     </row>
     <row r="474" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U474">
-        <f t="shared" ref="U474:U537" ca="1" si="10">IF(B474=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="475" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U475">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="476" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U476">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U476:U539" ca="1" si="10">IF(B476=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11030,19 +11075,19 @@
     </row>
     <row r="538" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U538">
-        <f t="shared" ref="U538:U601" ca="1" si="11">IF(B538=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="539" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U539">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="540" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U540">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U540:U603" ca="1" si="11">IF(B540=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11414,19 +11459,19 @@
     </row>
     <row r="602" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U602">
-        <f t="shared" ref="U602:U665" ca="1" si="12">IF(B602=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="603" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U603">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="604" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U604">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U604:U667" ca="1" si="12">IF(B604=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11798,19 +11843,19 @@
     </row>
     <row r="666" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U666">
-        <f t="shared" ref="U666:U729" ca="1" si="13">IF(B666=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="667" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U667">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="668" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U668">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U668:U731" ca="1" si="13">IF(B668=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12182,19 +12227,19 @@
     </row>
     <row r="730" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U730">
-        <f t="shared" ref="U730:U793" ca="1" si="14">IF(B730=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="731" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U731">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="732" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U732">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U732:U795" ca="1" si="14">IF(B732=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12566,19 +12611,19 @@
     </row>
     <row r="794" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U794">
-        <f t="shared" ref="U794:U857" ca="1" si="15">IF(B794=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="795" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U795">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="796" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U796">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U796:U859" ca="1" si="15">IF(B796=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12950,19 +12995,19 @@
     </row>
     <row r="858" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U858">
-        <f t="shared" ref="U858:U919" ca="1" si="16">IF(B858=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="859" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U859">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="860" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U860">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U860:U921" ca="1" si="16">IF(B860=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13320,19 +13365,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="920" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U920">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="921" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U921">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A229:A236"/>
-    <mergeCell ref="A237:A244"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A283:A287"/>
-    <mergeCell ref="A272:A282"/>
-    <mergeCell ref="A310:A315"/>
-    <mergeCell ref="A245:A271"/>
+    <mergeCell ref="A285:A289"/>
+    <mergeCell ref="A274:A284"/>
+    <mergeCell ref="A312:A317"/>
+    <mergeCell ref="A245:A273"/>
     <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A288:A303"/>
-    <mergeCell ref="A304:A309"/>
+    <mergeCell ref="A290:A305"/>
+    <mergeCell ref="A306:A311"/>
     <mergeCell ref="A64:A104"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A150:A181"/>
@@ -13340,6 +13395,8 @@
     <mergeCell ref="A105:A149"/>
     <mergeCell ref="A19:A63"/>
     <mergeCell ref="A200:A216"/>
+    <mergeCell ref="A229:A236"/>
+    <mergeCell ref="A237:A244"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rewrite initial tasks for java collections
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$289</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$291</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -525,24 +525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,6 +542,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,11 +862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W921"/>
+  <dimension ref="A1:W923"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B254" sqref="B254"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J279" sqref="J279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,56 +883,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>1046</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="33"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -962,7 +962,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -992,7 +992,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1300,7 +1300,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1414,7 +1414,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1722,7 +1722,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1750,7 +1750,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1946,7 +1946,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2030,7 +2030,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2086,7 +2086,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2170,7 +2170,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2226,7 +2226,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2310,7 +2310,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2338,7 +2338,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2394,7 +2394,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2422,7 +2422,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="35"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
+      <c r="A58" s="35"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2478,7 +2478,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="35"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2534,7 +2534,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2590,7 +2590,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="30"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -6378,7 +6378,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="27"/>
+      <c r="A198" s="31"/>
       <c r="B198" s="9">
         <v>1618</v>
       </c>
@@ -6434,7 +6434,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="28" t="s">
+      <c r="A200" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B200" s="8">
@@ -6464,7 +6464,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
+      <c r="A201" s="35"/>
       <c r="B201" s="2">
         <v>4488</v>
       </c>
@@ -6492,7 +6492,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="29"/>
+      <c r="A202" s="35"/>
       <c r="B202" s="2">
         <v>4954</v>
       </c>
@@ -6520,7 +6520,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="29"/>
+      <c r="A203" s="35"/>
       <c r="B203" s="2">
         <v>4642</v>
       </c>
@@ -6548,7 +6548,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
+      <c r="A204" s="35"/>
       <c r="B204" s="2">
         <v>5537</v>
       </c>
@@ -6576,7 +6576,7 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="29"/>
+      <c r="A205" s="35"/>
       <c r="B205" s="2">
         <v>5847</v>
       </c>
@@ -6604,7 +6604,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="29"/>
+      <c r="A206" s="35"/>
       <c r="B206" s="2">
         <v>4769</v>
       </c>
@@ -6632,7 +6632,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="29"/>
+      <c r="A207" s="35"/>
       <c r="B207" s="2">
         <v>9930</v>
       </c>
@@ -6655,12 +6655,12 @@
       <c r="S207" s="2"/>
       <c r="T207" s="5"/>
       <c r="U207">
-        <f t="shared" ref="U207:U283" ca="1" si="6">IF(B207=$W$1,1,0)</f>
+        <f t="shared" ref="U207:U285" ca="1" si="6">IF(B207=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="29"/>
+      <c r="A208" s="35"/>
       <c r="B208" s="2">
         <v>6861</v>
       </c>
@@ -6688,7 +6688,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="29"/>
+      <c r="A209" s="35"/>
       <c r="B209" s="2">
         <v>3226</v>
       </c>
@@ -6716,7 +6716,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="29"/>
+      <c r="A210" s="35"/>
       <c r="B210" s="2">
         <v>4372</v>
       </c>
@@ -6744,7 +6744,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="29"/>
+      <c r="A211" s="35"/>
       <c r="B211" s="2">
         <v>4463</v>
       </c>
@@ -6772,7 +6772,7 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="29"/>
+      <c r="A212" s="35"/>
       <c r="B212" s="2">
         <v>1668</v>
       </c>
@@ -6800,7 +6800,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="29"/>
+      <c r="A213" s="35"/>
       <c r="B213" s="2">
         <v>9417</v>
       </c>
@@ -6828,7 +6828,7 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="29"/>
+      <c r="A214" s="35"/>
       <c r="B214" s="2">
         <v>3148</v>
       </c>
@@ -6856,7 +6856,7 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="29"/>
+      <c r="A215" s="35"/>
       <c r="B215" s="2">
         <v>2137</v>
       </c>
@@ -6884,7 +6884,7 @@
       </c>
     </row>
     <row r="216" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="30"/>
+      <c r="A216" s="36"/>
       <c r="B216" s="6">
         <v>5621</v>
       </c>
@@ -8515,8 +8515,8 @@
       <c r="A274" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B274" s="8">
-        <v>8787</v>
+      <c r="B274" s="2">
+        <v>5087</v>
       </c>
       <c r="C274" s="8"/>
       <c r="D274" s="8"/>
@@ -8544,7 +8544,7 @@
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>5087</v>
+        <v>1056</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8628,7 +8628,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="23"/>
       <c r="B278" s="2">
-        <v>9924</v>
+        <v>8418</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8654,65 +8654,65 @@
       </c>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="27"/>
-      <c r="B279" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C279" s="9"/>
-      <c r="D279" s="9"/>
-      <c r="E279" s="9"/>
-      <c r="F279" s="9"/>
-      <c r="G279" s="9"/>
-      <c r="H279" s="9"/>
-      <c r="I279" s="9"/>
-      <c r="J279" s="9"/>
-      <c r="K279" s="9"/>
-      <c r="L279" s="9"/>
-      <c r="M279" s="9"/>
-      <c r="N279" s="9"/>
-      <c r="O279" s="9"/>
-      <c r="P279" s="9"/>
-      <c r="Q279" s="9"/>
-      <c r="R279" s="9"/>
-      <c r="S279" s="9"/>
-      <c r="T279" s="15"/>
+      <c r="A279" s="23"/>
+      <c r="B279" s="2">
+        <v>9512</v>
+      </c>
+      <c r="C279" s="2"/>
+      <c r="D279" s="2"/>
+      <c r="E279" s="2"/>
+      <c r="F279" s="2"/>
+      <c r="G279" s="2"/>
+      <c r="H279" s="2"/>
+      <c r="I279" s="2"/>
+      <c r="J279" s="2"/>
+      <c r="K279" s="2"/>
+      <c r="L279" s="2"/>
+      <c r="M279" s="2"/>
+      <c r="N279" s="2"/>
+      <c r="O279" s="2"/>
+      <c r="P279" s="2"/>
+      <c r="Q279" s="2"/>
+      <c r="R279" s="2"/>
+      <c r="S279" s="2"/>
+      <c r="T279" s="5"/>
       <c r="U279">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="27"/>
-      <c r="B280" s="9">
-        <v>2973</v>
-      </c>
-      <c r="C280" s="9"/>
-      <c r="D280" s="9"/>
-      <c r="E280" s="9"/>
-      <c r="F280" s="9"/>
-      <c r="G280" s="9"/>
-      <c r="H280" s="9"/>
-      <c r="I280" s="9"/>
-      <c r="J280" s="9"/>
-      <c r="K280" s="9"/>
-      <c r="L280" s="9"/>
-      <c r="M280" s="9"/>
-      <c r="N280" s="9"/>
-      <c r="O280" s="9"/>
-      <c r="P280" s="9"/>
-      <c r="Q280" s="9"/>
-      <c r="R280" s="9"/>
-      <c r="S280" s="9"/>
-      <c r="T280" s="15"/>
+      <c r="A280" s="23"/>
+      <c r="B280" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C280" s="2"/>
+      <c r="D280" s="2"/>
+      <c r="E280" s="2"/>
+      <c r="F280" s="2"/>
+      <c r="G280" s="2"/>
+      <c r="H280" s="2"/>
+      <c r="I280" s="2"/>
+      <c r="J280" s="2"/>
+      <c r="K280" s="2"/>
+      <c r="L280" s="2"/>
+      <c r="M280" s="2"/>
+      <c r="N280" s="2"/>
+      <c r="O280" s="2"/>
+      <c r="P280" s="2"/>
+      <c r="Q280" s="2"/>
+      <c r="R280" s="2"/>
+      <c r="S280" s="2"/>
+      <c r="T280" s="5"/>
       <c r="U280">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="27"/>
+      <c r="A281" s="31"/>
       <c r="B281" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C281" s="9"/>
       <c r="D281" s="9"/>
@@ -8738,9 +8738,9 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="27"/>
+      <c r="A282" s="31"/>
       <c r="B282" s="9">
-        <v>7186</v>
+        <v>2973</v>
       </c>
       <c r="C282" s="9"/>
       <c r="D282" s="9"/>
@@ -8766,9 +8766,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="27"/>
+      <c r="A283" s="31"/>
       <c r="B283" s="9">
-        <v>1457</v>
+        <v>8258</v>
       </c>
       <c r="C283" s="9"/>
       <c r="D283" s="9"/>
@@ -8793,115 +8793,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="24"/>
-      <c r="B284" s="6">
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A284" s="31"/>
+      <c r="B284" s="9">
+        <v>7186</v>
+      </c>
+      <c r="C284" s="9"/>
+      <c r="D284" s="9"/>
+      <c r="E284" s="9"/>
+      <c r="F284" s="9"/>
+      <c r="G284" s="9"/>
+      <c r="H284" s="9"/>
+      <c r="I284" s="9"/>
+      <c r="J284" s="9"/>
+      <c r="K284" s="9"/>
+      <c r="L284" s="9"/>
+      <c r="M284" s="9"/>
+      <c r="N284" s="9"/>
+      <c r="O284" s="9"/>
+      <c r="P284" s="9"/>
+      <c r="Q284" s="9"/>
+      <c r="R284" s="9"/>
+      <c r="S284" s="9"/>
+      <c r="T284" s="15"/>
+      <c r="U284">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A285" s="31"/>
+      <c r="B285" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C285" s="9"/>
+      <c r="D285" s="9"/>
+      <c r="E285" s="9"/>
+      <c r="F285" s="9"/>
+      <c r="G285" s="9"/>
+      <c r="H285" s="9"/>
+      <c r="I285" s="9"/>
+      <c r="J285" s="9"/>
+      <c r="K285" s="9"/>
+      <c r="L285" s="9"/>
+      <c r="M285" s="9"/>
+      <c r="N285" s="9"/>
+      <c r="O285" s="9"/>
+      <c r="P285" s="9"/>
+      <c r="Q285" s="9"/>
+      <c r="R285" s="9"/>
+      <c r="S285" s="9"/>
+      <c r="T285" s="15"/>
+      <c r="U285">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="24"/>
+      <c r="B286" s="6">
         <v>6876</v>
       </c>
-      <c r="C284" s="6"/>
-      <c r="D284" s="6"/>
-      <c r="E284" s="6"/>
-      <c r="F284" s="6"/>
-      <c r="G284" s="6"/>
-      <c r="H284" s="6"/>
-      <c r="I284" s="6"/>
-      <c r="J284" s="6"/>
-      <c r="K284" s="6"/>
-      <c r="L284" s="6"/>
-      <c r="M284" s="6"/>
-      <c r="N284" s="6"/>
-      <c r="O284" s="6"/>
-      <c r="P284" s="6"/>
-      <c r="Q284" s="6"/>
-      <c r="R284" s="6"/>
-      <c r="S284" s="6"/>
-      <c r="T284" s="7"/>
-      <c r="U284">
-        <f t="shared" ref="U284:U347" ca="1" si="7">IF(B284=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="22" t="s">
+      <c r="C286" s="6"/>
+      <c r="D286" s="6"/>
+      <c r="E286" s="6"/>
+      <c r="F286" s="6"/>
+      <c r="G286" s="6"/>
+      <c r="H286" s="6"/>
+      <c r="I286" s="6"/>
+      <c r="J286" s="6"/>
+      <c r="K286" s="6"/>
+      <c r="L286" s="6"/>
+      <c r="M286" s="6"/>
+      <c r="N286" s="6"/>
+      <c r="O286" s="6"/>
+      <c r="P286" s="6"/>
+      <c r="Q286" s="6"/>
+      <c r="R286" s="6"/>
+      <c r="S286" s="6"/>
+      <c r="T286" s="7"/>
+      <c r="U286">
+        <f t="shared" ref="U286:U349" ca="1" si="7">IF(B286=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A287" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B285" s="8">
+      <c r="B287" s="8">
         <v>4304</v>
       </c>
-      <c r="C285" s="8"/>
-      <c r="D285" s="8"/>
-      <c r="E285" s="8"/>
-      <c r="F285" s="8"/>
-      <c r="G285" s="8"/>
-      <c r="H285" s="8"/>
-      <c r="I285" s="8"/>
-      <c r="J285" s="8"/>
-      <c r="K285" s="8"/>
-      <c r="L285" s="8"/>
-      <c r="M285" s="8"/>
-      <c r="N285" s="8"/>
-      <c r="O285" s="8"/>
-      <c r="P285" s="8"/>
-      <c r="Q285" s="8"/>
-      <c r="R285" s="8"/>
-      <c r="S285" s="8"/>
-      <c r="T285" s="14"/>
-      <c r="U285">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="23"/>
-      <c r="B286" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2"/>
-      <c r="E286" s="2"/>
-      <c r="F286" s="2"/>
-      <c r="G286" s="2"/>
-      <c r="H286" s="2"/>
-      <c r="I286" s="2"/>
-      <c r="J286" s="2"/>
-      <c r="K286" s="2"/>
-      <c r="L286" s="2"/>
-      <c r="M286" s="2"/>
-      <c r="N286" s="2"/>
-      <c r="O286" s="2"/>
-      <c r="P286" s="2"/>
-      <c r="Q286" s="2"/>
-      <c r="R286" s="2"/>
-      <c r="S286" s="2"/>
-      <c r="T286" s="5"/>
-      <c r="U286">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="23"/>
-      <c r="B287" s="2">
-        <v>7693</v>
-      </c>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="E287" s="2"/>
-      <c r="F287" s="2"/>
-      <c r="G287" s="2"/>
-      <c r="H287" s="2"/>
-      <c r="I287" s="2"/>
-      <c r="J287" s="2"/>
-      <c r="K287" s="2"/>
-      <c r="L287" s="2"/>
-      <c r="M287" s="2"/>
-      <c r="N287" s="2"/>
-      <c r="O287" s="2"/>
-      <c r="P287" s="2"/>
-      <c r="Q287" s="2"/>
-      <c r="R287" s="2"/>
-      <c r="S287" s="2"/>
-      <c r="T287" s="5"/>
+      <c r="C287" s="8"/>
+      <c r="D287" s="8"/>
+      <c r="E287" s="8"/>
+      <c r="F287" s="8"/>
+      <c r="G287" s="8"/>
+      <c r="H287" s="8"/>
+      <c r="I287" s="8"/>
+      <c r="J287" s="8"/>
+      <c r="K287" s="8"/>
+      <c r="L287" s="8"/>
+      <c r="M287" s="8"/>
+      <c r="N287" s="8"/>
+      <c r="O287" s="8"/>
+      <c r="P287" s="8"/>
+      <c r="Q287" s="8"/>
+      <c r="R287" s="8"/>
+      <c r="S287" s="8"/>
+      <c r="T287" s="14"/>
       <c r="U287">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8910,7 +8910,7 @@
     <row r="288" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A288" s="23"/>
       <c r="B288" s="2">
-        <v>8718</v>
+        <v>2070</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -8935,124 +8935,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A289" s="24"/>
-      <c r="B289" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C289" s="6"/>
-      <c r="D289" s="6"/>
-      <c r="E289" s="6"/>
-      <c r="F289" s="6"/>
-      <c r="G289" s="6"/>
-      <c r="H289" s="6"/>
-      <c r="I289" s="6"/>
-      <c r="J289" s="6"/>
-      <c r="K289" s="6"/>
-      <c r="L289" s="6"/>
-      <c r="M289" s="6"/>
-      <c r="N289" s="6"/>
-      <c r="O289" s="6"/>
-      <c r="P289" s="6"/>
-      <c r="Q289" s="6"/>
-      <c r="R289" s="6"/>
-      <c r="S289" s="6"/>
-      <c r="T289" s="7"/>
+    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A289" s="23"/>
+      <c r="B289" s="2">
+        <v>7693</v>
+      </c>
+      <c r="C289" s="2"/>
+      <c r="D289" s="2"/>
+      <c r="E289" s="2"/>
+      <c r="F289" s="2"/>
+      <c r="G289" s="2"/>
+      <c r="H289" s="2"/>
+      <c r="I289" s="2"/>
+      <c r="J289" s="2"/>
+      <c r="K289" s="2"/>
+      <c r="L289" s="2"/>
+      <c r="M289" s="2"/>
+      <c r="N289" s="2"/>
+      <c r="O289" s="2"/>
+      <c r="P289" s="2"/>
+      <c r="Q289" s="2"/>
+      <c r="R289" s="2"/>
+      <c r="S289" s="2"/>
+      <c r="T289" s="5"/>
       <c r="U289">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A290" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B290" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C290" s="8"/>
-      <c r="D290" s="8"/>
-      <c r="E290" s="8"/>
-      <c r="F290" s="8"/>
-      <c r="G290" s="8"/>
-      <c r="H290" s="8"/>
-      <c r="I290" s="8"/>
-      <c r="J290" s="8"/>
-      <c r="K290" s="8"/>
-      <c r="L290" s="8"/>
-      <c r="M290" s="8"/>
-      <c r="N290" s="8"/>
-      <c r="O290" s="8"/>
-      <c r="P290" s="8"/>
-      <c r="Q290" s="8"/>
-      <c r="R290" s="8"/>
-      <c r="S290" s="8"/>
-      <c r="T290" s="14"/>
+    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A290" s="23"/>
+      <c r="B290" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C290" s="2"/>
+      <c r="D290" s="2"/>
+      <c r="E290" s="2"/>
+      <c r="F290" s="2"/>
+      <c r="G290" s="2"/>
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
+      <c r="J290" s="2"/>
+      <c r="K290" s="2"/>
+      <c r="L290" s="2"/>
+      <c r="M290" s="2"/>
+      <c r="N290" s="2"/>
+      <c r="O290" s="2"/>
+      <c r="P290" s="2"/>
+      <c r="Q290" s="2"/>
+      <c r="R290" s="2"/>
+      <c r="S290" s="2"/>
+      <c r="T290" s="5"/>
       <c r="U290">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A291" s="23"/>
-      <c r="B291" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2"/>
-      <c r="E291" s="2"/>
-      <c r="F291" s="2"/>
-      <c r="G291" s="2"/>
-      <c r="H291" s="2"/>
-      <c r="I291" s="2"/>
-      <c r="J291" s="2"/>
-      <c r="K291" s="2"/>
-      <c r="L291" s="2"/>
-      <c r="M291" s="2"/>
-      <c r="N291" s="2"/>
-      <c r="O291" s="2"/>
-      <c r="P291" s="2"/>
-      <c r="Q291" s="2"/>
-      <c r="R291" s="2"/>
-      <c r="S291" s="2"/>
-      <c r="T291" s="5"/>
+    <row r="291" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="24"/>
+      <c r="B291" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C291" s="6"/>
+      <c r="D291" s="6"/>
+      <c r="E291" s="6"/>
+      <c r="F291" s="6"/>
+      <c r="G291" s="6"/>
+      <c r="H291" s="6"/>
+      <c r="I291" s="6"/>
+      <c r="J291" s="6"/>
+      <c r="K291" s="6"/>
+      <c r="L291" s="6"/>
+      <c r="M291" s="6"/>
+      <c r="N291" s="6"/>
+      <c r="O291" s="6"/>
+      <c r="P291" s="6"/>
+      <c r="Q291" s="6"/>
+      <c r="R291" s="6"/>
+      <c r="S291" s="6"/>
+      <c r="T291" s="7"/>
       <c r="U291">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A292" s="23"/>
-      <c r="B292" s="12">
-        <v>7546</v>
-      </c>
-      <c r="C292" s="2"/>
-      <c r="D292" s="2"/>
-      <c r="E292" s="2"/>
-      <c r="F292" s="2"/>
-      <c r="G292" s="2"/>
-      <c r="H292" s="2"/>
-      <c r="I292" s="2"/>
-      <c r="J292" s="2"/>
-      <c r="K292" s="2"/>
-      <c r="L292" s="2"/>
-      <c r="M292" s="2"/>
-      <c r="N292" s="2"/>
-      <c r="O292" s="2"/>
-      <c r="P292" s="2"/>
-      <c r="Q292" s="2"/>
-      <c r="R292" s="2"/>
-      <c r="S292" s="2"/>
-      <c r="T292" s="5"/>
+      <c r="A292" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B292" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C292" s="8"/>
+      <c r="D292" s="8"/>
+      <c r="E292" s="8"/>
+      <c r="F292" s="8"/>
+      <c r="G292" s="8"/>
+      <c r="H292" s="8"/>
+      <c r="I292" s="8"/>
+      <c r="J292" s="8"/>
+      <c r="K292" s="8"/>
+      <c r="L292" s="8"/>
+      <c r="M292" s="8"/>
+      <c r="N292" s="8"/>
+      <c r="O292" s="8"/>
+      <c r="P292" s="8"/>
+      <c r="Q292" s="8"/>
+      <c r="R292" s="8"/>
+      <c r="S292" s="8"/>
+      <c r="T292" s="14"/>
       <c r="U292">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A293" s="23"/>
-      <c r="B293" s="2">
-        <v>7170</v>
+      <c r="B293" s="12">
+        <v>3083</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9077,10 +9077,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A294" s="23"/>
-      <c r="B294" s="2">
-        <v>2709</v>
+      <c r="B294" s="12">
+        <v>7546</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9108,7 +9108,7 @@
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" s="23"/>
       <c r="B295" s="2">
-        <v>3402</v>
+        <v>7170</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9136,7 +9136,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="23"/>
       <c r="B296" s="2">
-        <v>8781</v>
+        <v>2709</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9164,7 +9164,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="23"/>
       <c r="B297" s="2">
-        <v>8771</v>
+        <v>3402</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9192,7 +9192,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="23"/>
       <c r="B298" s="2">
-        <v>3091</v>
+        <v>8781</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9220,7 +9220,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="23"/>
       <c r="B299" s="2">
-        <v>2195</v>
+        <v>8771</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9248,7 +9248,7 @@
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" s="23"/>
       <c r="B300" s="2">
-        <v>1184</v>
+        <v>3091</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9276,7 +9276,7 @@
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A301" s="23"/>
       <c r="B301" s="2">
-        <v>2667</v>
+        <v>2195</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9304,7 +9304,7 @@
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>5917</v>
+        <v>1184</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9332,7 +9332,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>8545</v>
+        <v>2667</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9360,7 +9360,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>1288</v>
+        <v>5917</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9385,115 +9385,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="24"/>
-      <c r="B305" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C305" s="6"/>
-      <c r="D305" s="6"/>
-      <c r="E305" s="6"/>
-      <c r="F305" s="6"/>
-      <c r="G305" s="6"/>
-      <c r="H305" s="6"/>
-      <c r="I305" s="6"/>
-      <c r="J305" s="6"/>
-      <c r="K305" s="6"/>
-      <c r="L305" s="6"/>
-      <c r="M305" s="6"/>
-      <c r="N305" s="6"/>
-      <c r="O305" s="6"/>
-      <c r="P305" s="6"/>
-      <c r="Q305" s="6"/>
-      <c r="R305" s="6"/>
-      <c r="S305" s="6"/>
-      <c r="T305" s="7"/>
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A305" s="23"/>
+      <c r="B305" s="2">
+        <v>8545</v>
+      </c>
+      <c r="C305" s="2"/>
+      <c r="D305" s="2"/>
+      <c r="E305" s="2"/>
+      <c r="F305" s="2"/>
+      <c r="G305" s="2"/>
+      <c r="H305" s="2"/>
+      <c r="I305" s="2"/>
+      <c r="J305" s="2"/>
+      <c r="K305" s="2"/>
+      <c r="L305" s="2"/>
+      <c r="M305" s="2"/>
+      <c r="N305" s="2"/>
+      <c r="O305" s="2"/>
+      <c r="P305" s="2"/>
+      <c r="Q305" s="2"/>
+      <c r="R305" s="2"/>
+      <c r="S305" s="2"/>
+      <c r="T305" s="5"/>
       <c r="U305">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A306" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B306" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C306" s="8"/>
-      <c r="D306" s="8"/>
-      <c r="E306" s="8"/>
-      <c r="F306" s="8"/>
-      <c r="G306" s="8"/>
-      <c r="H306" s="8"/>
-      <c r="I306" s="8"/>
-      <c r="J306" s="8"/>
-      <c r="K306" s="8"/>
-      <c r="L306" s="8"/>
-      <c r="M306" s="8"/>
-      <c r="N306" s="8"/>
-      <c r="O306" s="8"/>
-      <c r="P306" s="8"/>
-      <c r="Q306" s="8"/>
-      <c r="R306" s="8"/>
-      <c r="S306" s="8"/>
-      <c r="T306" s="14"/>
+      <c r="A306" s="23"/>
+      <c r="B306" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C306" s="2"/>
+      <c r="D306" s="2"/>
+      <c r="E306" s="2"/>
+      <c r="F306" s="2"/>
+      <c r="G306" s="2"/>
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+      <c r="J306" s="2"/>
+      <c r="K306" s="2"/>
+      <c r="L306" s="2"/>
+      <c r="M306" s="2"/>
+      <c r="N306" s="2"/>
+      <c r="O306" s="2"/>
+      <c r="P306" s="2"/>
+      <c r="Q306" s="2"/>
+      <c r="R306" s="2"/>
+      <c r="S306" s="2"/>
+      <c r="T306" s="5"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A307" s="23"/>
-      <c r="B307" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2"/>
-      <c r="E307" s="2"/>
-      <c r="F307" s="2"/>
-      <c r="G307" s="2"/>
-      <c r="H307" s="2"/>
-      <c r="I307" s="2"/>
-      <c r="J307" s="2"/>
-      <c r="K307" s="2"/>
-      <c r="L307" s="2"/>
-      <c r="M307" s="2"/>
-      <c r="N307" s="2"/>
-      <c r="O307" s="2"/>
-      <c r="P307" s="2"/>
-      <c r="Q307" s="2"/>
-      <c r="R307" s="2"/>
-      <c r="S307" s="2"/>
-      <c r="T307" s="5"/>
+    <row r="307" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="24"/>
+      <c r="B307" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C307" s="6"/>
+      <c r="D307" s="6"/>
+      <c r="E307" s="6"/>
+      <c r="F307" s="6"/>
+      <c r="G307" s="6"/>
+      <c r="H307" s="6"/>
+      <c r="I307" s="6"/>
+      <c r="J307" s="6"/>
+      <c r="K307" s="6"/>
+      <c r="L307" s="6"/>
+      <c r="M307" s="6"/>
+      <c r="N307" s="6"/>
+      <c r="O307" s="6"/>
+      <c r="P307" s="6"/>
+      <c r="Q307" s="6"/>
+      <c r="R307" s="6"/>
+      <c r="S307" s="6"/>
+      <c r="T307" s="7"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A308" s="23"/>
-      <c r="B308" s="2">
-        <v>3093</v>
-      </c>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
-      <c r="E308" s="2"/>
-      <c r="F308" s="2"/>
-      <c r="G308" s="2"/>
-      <c r="H308" s="2"/>
-      <c r="I308" s="2"/>
-      <c r="J308" s="2"/>
-      <c r="K308" s="2"/>
-      <c r="L308" s="2"/>
-      <c r="M308" s="2"/>
-      <c r="N308" s="2"/>
-      <c r="O308" s="2"/>
-      <c r="P308" s="2"/>
-      <c r="Q308" s="2"/>
-      <c r="R308" s="2"/>
-      <c r="S308" s="2"/>
-      <c r="T308" s="5"/>
+      <c r="A308" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B308" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C308" s="8"/>
+      <c r="D308" s="8"/>
+      <c r="E308" s="8"/>
+      <c r="F308" s="8"/>
+      <c r="G308" s="8"/>
+      <c r="H308" s="8"/>
+      <c r="I308" s="8"/>
+      <c r="J308" s="8"/>
+      <c r="K308" s="8"/>
+      <c r="L308" s="8"/>
+      <c r="M308" s="8"/>
+      <c r="N308" s="8"/>
+      <c r="O308" s="8"/>
+      <c r="P308" s="8"/>
+      <c r="Q308" s="8"/>
+      <c r="R308" s="8"/>
+      <c r="S308" s="8"/>
+      <c r="T308" s="14"/>
       <c r="U308">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9502,7 +9502,7 @@
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="23"/>
       <c r="B309" s="2">
-        <v>8805</v>
+        <v>6598</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9530,7 +9530,7 @@
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="23"/>
       <c r="B310" s="2">
-        <v>8158</v>
+        <v>3093</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9555,115 +9555,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="24"/>
-      <c r="B311" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C311" s="6"/>
-      <c r="D311" s="6"/>
-      <c r="E311" s="6"/>
-      <c r="F311" s="6"/>
-      <c r="G311" s="6"/>
-      <c r="H311" s="6"/>
-      <c r="I311" s="6"/>
-      <c r="J311" s="6"/>
-      <c r="K311" s="6"/>
-      <c r="L311" s="6"/>
-      <c r="M311" s="6"/>
-      <c r="N311" s="6"/>
-      <c r="O311" s="6"/>
-      <c r="P311" s="6"/>
-      <c r="Q311" s="6"/>
-      <c r="R311" s="6"/>
-      <c r="S311" s="6"/>
-      <c r="T311" s="7"/>
+    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A311" s="23"/>
+      <c r="B311" s="2">
+        <v>8805</v>
+      </c>
+      <c r="C311" s="2"/>
+      <c r="D311" s="2"/>
+      <c r="E311" s="2"/>
+      <c r="F311" s="2"/>
+      <c r="G311" s="2"/>
+      <c r="H311" s="2"/>
+      <c r="I311" s="2"/>
+      <c r="J311" s="2"/>
+      <c r="K311" s="2"/>
+      <c r="L311" s="2"/>
+      <c r="M311" s="2"/>
+      <c r="N311" s="2"/>
+      <c r="O311" s="2"/>
+      <c r="P311" s="2"/>
+      <c r="Q311" s="2"/>
+      <c r="R311" s="2"/>
+      <c r="S311" s="2"/>
+      <c r="T311" s="5"/>
       <c r="U311">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A312" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B312" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C312" s="8"/>
-      <c r="D312" s="8"/>
-      <c r="E312" s="8"/>
-      <c r="F312" s="8"/>
-      <c r="G312" s="8"/>
-      <c r="H312" s="8"/>
-      <c r="I312" s="8"/>
-      <c r="J312" s="8"/>
-      <c r="K312" s="8"/>
-      <c r="L312" s="8"/>
-      <c r="M312" s="8"/>
-      <c r="N312" s="8"/>
-      <c r="O312" s="8"/>
-      <c r="P312" s="8"/>
-      <c r="Q312" s="8"/>
-      <c r="R312" s="8"/>
-      <c r="S312" s="8"/>
-      <c r="T312" s="14"/>
+      <c r="A312" s="23"/>
+      <c r="B312" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C312" s="2"/>
+      <c r="D312" s="2"/>
+      <c r="E312" s="2"/>
+      <c r="F312" s="2"/>
+      <c r="G312" s="2"/>
+      <c r="H312" s="2"/>
+      <c r="I312" s="2"/>
+      <c r="J312" s="2"/>
+      <c r="K312" s="2"/>
+      <c r="L312" s="2"/>
+      <c r="M312" s="2"/>
+      <c r="N312" s="2"/>
+      <c r="O312" s="2"/>
+      <c r="P312" s="2"/>
+      <c r="Q312" s="2"/>
+      <c r="R312" s="2"/>
+      <c r="S312" s="2"/>
+      <c r="T312" s="5"/>
       <c r="U312">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A313" s="23"/>
-      <c r="B313" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C313" s="2"/>
-      <c r="D313" s="2"/>
-      <c r="E313" s="2"/>
-      <c r="F313" s="2"/>
-      <c r="G313" s="2"/>
-      <c r="H313" s="2"/>
-      <c r="I313" s="2"/>
-      <c r="J313" s="2"/>
-      <c r="K313" s="2"/>
-      <c r="L313" s="2"/>
-      <c r="M313" s="2"/>
-      <c r="N313" s="2"/>
-      <c r="O313" s="2"/>
-      <c r="P313" s="2"/>
-      <c r="Q313" s="2"/>
-      <c r="R313" s="2"/>
-      <c r="S313" s="2"/>
-      <c r="T313" s="5"/>
+    <row r="313" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="24"/>
+      <c r="B313" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C313" s="6"/>
+      <c r="D313" s="6"/>
+      <c r="E313" s="6"/>
+      <c r="F313" s="6"/>
+      <c r="G313" s="6"/>
+      <c r="H313" s="6"/>
+      <c r="I313" s="6"/>
+      <c r="J313" s="6"/>
+      <c r="K313" s="6"/>
+      <c r="L313" s="6"/>
+      <c r="M313" s="6"/>
+      <c r="N313" s="6"/>
+      <c r="O313" s="6"/>
+      <c r="P313" s="6"/>
+      <c r="Q313" s="6"/>
+      <c r="R313" s="6"/>
+      <c r="S313" s="6"/>
+      <c r="T313" s="7"/>
       <c r="U313">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="23"/>
-      <c r="B314" s="2">
-        <v>9002</v>
-      </c>
-      <c r="C314" s="2"/>
-      <c r="D314" s="2"/>
-      <c r="E314" s="2"/>
-      <c r="F314" s="2"/>
-      <c r="G314" s="2"/>
-      <c r="H314" s="2"/>
-      <c r="I314" s="2"/>
-      <c r="J314" s="2"/>
-      <c r="K314" s="2"/>
-      <c r="L314" s="2"/>
-      <c r="M314" s="2"/>
-      <c r="N314" s="2"/>
-      <c r="O314" s="2"/>
-      <c r="P314" s="2"/>
-      <c r="Q314" s="2"/>
-      <c r="R314" s="2"/>
-      <c r="S314" s="2"/>
-      <c r="T314" s="5"/>
+      <c r="A314" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B314" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C314" s="8"/>
+      <c r="D314" s="8"/>
+      <c r="E314" s="8"/>
+      <c r="F314" s="8"/>
+      <c r="G314" s="8"/>
+      <c r="H314" s="8"/>
+      <c r="I314" s="8"/>
+      <c r="J314" s="8"/>
+      <c r="K314" s="8"/>
+      <c r="L314" s="8"/>
+      <c r="M314" s="8"/>
+      <c r="N314" s="8"/>
+      <c r="O314" s="8"/>
+      <c r="P314" s="8"/>
+      <c r="Q314" s="8"/>
+      <c r="R314" s="8"/>
+      <c r="S314" s="8"/>
+      <c r="T314" s="14"/>
       <c r="U314">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9672,7 +9672,7 @@
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A315" s="23"/>
       <c r="B315" s="2">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -9700,7 +9700,7 @@
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A316" s="23"/>
       <c r="B316" s="2">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9725,41 +9725,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A317" s="24"/>
-      <c r="B317" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C317" s="6"/>
-      <c r="D317" s="6"/>
-      <c r="E317" s="6"/>
-      <c r="F317" s="6"/>
-      <c r="G317" s="6"/>
-      <c r="H317" s="6"/>
-      <c r="I317" s="6"/>
-      <c r="J317" s="6"/>
-      <c r="K317" s="6"/>
-      <c r="L317" s="6"/>
-      <c r="M317" s="6"/>
-      <c r="N317" s="6"/>
-      <c r="O317" s="6"/>
-      <c r="P317" s="6"/>
-      <c r="Q317" s="6"/>
-      <c r="R317" s="6"/>
-      <c r="S317" s="6"/>
-      <c r="T317" s="7"/>
+    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A317" s="23"/>
+      <c r="B317" s="2">
+        <v>7432</v>
+      </c>
+      <c r="C317" s="2"/>
+      <c r="D317" s="2"/>
+      <c r="E317" s="2"/>
+      <c r="F317" s="2"/>
+      <c r="G317" s="2"/>
+      <c r="H317" s="2"/>
+      <c r="I317" s="2"/>
+      <c r="J317" s="2"/>
+      <c r="K317" s="2"/>
+      <c r="L317" s="2"/>
+      <c r="M317" s="2"/>
+      <c r="N317" s="2"/>
+      <c r="O317" s="2"/>
+      <c r="P317" s="2"/>
+      <c r="Q317" s="2"/>
+      <c r="R317" s="2"/>
+      <c r="S317" s="2"/>
+      <c r="T317" s="5"/>
       <c r="U317">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A318" s="23"/>
+      <c r="B318" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C318" s="2"/>
+      <c r="D318" s="2"/>
+      <c r="E318" s="2"/>
+      <c r="F318" s="2"/>
+      <c r="G318" s="2"/>
+      <c r="H318" s="2"/>
+      <c r="I318" s="2"/>
+      <c r="J318" s="2"/>
+      <c r="K318" s="2"/>
+      <c r="L318" s="2"/>
+      <c r="M318" s="2"/>
+      <c r="N318" s="2"/>
+      <c r="O318" s="2"/>
+      <c r="P318" s="2"/>
+      <c r="Q318" s="2"/>
+      <c r="R318" s="2"/>
+      <c r="S318" s="2"/>
+      <c r="T318" s="5"/>
       <c r="U318">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="24"/>
+      <c r="B319" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C319" s="6"/>
+      <c r="D319" s="6"/>
+      <c r="E319" s="6"/>
+      <c r="F319" s="6"/>
+      <c r="G319" s="6"/>
+      <c r="H319" s="6"/>
+      <c r="I319" s="6"/>
+      <c r="J319" s="6"/>
+      <c r="K319" s="6"/>
+      <c r="L319" s="6"/>
+      <c r="M319" s="6"/>
+      <c r="N319" s="6"/>
+      <c r="O319" s="6"/>
+      <c r="P319" s="6"/>
+      <c r="Q319" s="6"/>
+      <c r="R319" s="6"/>
+      <c r="S319" s="6"/>
+      <c r="T319" s="7"/>
       <c r="U319">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9935,19 +9979,19 @@
     </row>
     <row r="348" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U348">
-        <f t="shared" ref="U348:U411" ca="1" si="8">IF(B348=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="349" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U349">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="350" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U350">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U350:U413" ca="1" si="8">IF(B350=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10319,19 +10363,19 @@
     </row>
     <row r="412" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U412">
-        <f t="shared" ref="U412:U475" ca="1" si="9">IF(B412=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="413" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U413">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="414" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U414">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U414:U477" ca="1" si="9">IF(B414=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10703,19 +10747,19 @@
     </row>
     <row r="476" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U476">
-        <f t="shared" ref="U476:U539" ca="1" si="10">IF(B476=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="477" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U477">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="478" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U478">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U478:U541" ca="1" si="10">IF(B478=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11087,19 +11131,19 @@
     </row>
     <row r="540" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U540">
-        <f t="shared" ref="U540:U603" ca="1" si="11">IF(B540=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="541" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U541">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="542" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U542">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U542:U605" ca="1" si="11">IF(B542=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11471,19 +11515,19 @@
     </row>
     <row r="604" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U604">
-        <f t="shared" ref="U604:U667" ca="1" si="12">IF(B604=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="605" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U605">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="606" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U606">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U606:U669" ca="1" si="12">IF(B606=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11855,19 +11899,19 @@
     </row>
     <row r="668" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U668">
-        <f t="shared" ref="U668:U731" ca="1" si="13">IF(B668=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="669" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U669">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="670" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U670">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U670:U733" ca="1" si="13">IF(B670=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12239,19 +12283,19 @@
     </row>
     <row r="732" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U732">
-        <f t="shared" ref="U732:U795" ca="1" si="14">IF(B732=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="733" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U733">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="734" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U734">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U734:U797" ca="1" si="14">IF(B734=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12623,19 +12667,19 @@
     </row>
     <row r="796" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U796">
-        <f t="shared" ref="U796:U859" ca="1" si="15">IF(B796=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="797" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U797">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="798" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U798">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U798:U861" ca="1" si="15">IF(B798=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13007,19 +13051,19 @@
     </row>
     <row r="860" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U860">
-        <f t="shared" ref="U860:U921" ca="1" si="16">IF(B860=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="861" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U861">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="862" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U862">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U862:U923" ca="1" si="16">IF(B862=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13377,17 +13421,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="922" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U922">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="923" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U923">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A285:A289"/>
-    <mergeCell ref="A274:A284"/>
-    <mergeCell ref="A312:A317"/>
+    <mergeCell ref="A314:A319"/>
     <mergeCell ref="A245:A273"/>
     <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A290:A305"/>
-    <mergeCell ref="A306:A311"/>
+    <mergeCell ref="A292:A307"/>
+    <mergeCell ref="A308:A313"/>
     <mergeCell ref="A64:A104"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A150:A181"/>
@@ -13397,6 +13449,10 @@
     <mergeCell ref="A200:A216"/>
     <mergeCell ref="A229:A236"/>
     <mergeCell ref="A237:A244"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A287:A291"/>
+    <mergeCell ref="A274:A286"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rewrite tasks in lab15 and preliminary tasks in other labs for java and csharp. replace bullets with numbers
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tfa\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="7680"/>
   </bookViews>
@@ -12,9 +17,9 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$291</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$292</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -525,6 +530,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,24 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,6 +575,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -618,7 +626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,7 +661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -862,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W923"/>
+  <dimension ref="A1:W924"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J279" sqref="J279"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U261" sqref="U261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,56 +891,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>1297</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="33"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -962,7 +970,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -992,7 +1000,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1020,7 +1028,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1300,7 +1308,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1328,7 +1336,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1356,7 +1364,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1386,7 +1394,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1414,7 +1422,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1442,7 +1450,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1470,7 +1478,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1498,7 +1506,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1526,7 +1534,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1554,7 +1562,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1582,7 +1590,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1610,7 +1618,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1638,7 +1646,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1666,7 +1674,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1694,7 +1702,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1722,7 +1730,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1750,7 +1758,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1778,7 +1786,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1806,7 +1814,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1834,7 +1842,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1862,7 +1870,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1890,7 +1898,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1918,7 +1926,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1946,7 +1954,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1974,7 +1982,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2002,7 +2010,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2030,7 +2038,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2058,7 +2066,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2086,7 +2094,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2114,7 +2122,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2142,7 +2150,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2170,7 +2178,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2198,7 +2206,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2226,7 +2234,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2254,7 +2262,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2282,7 +2290,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2310,7 +2318,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2338,7 +2346,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2366,7 +2374,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2394,7 +2402,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2422,7 +2430,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2450,7 +2458,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2478,7 +2486,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2506,7 +2514,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2534,7 +2542,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2562,7 +2570,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2590,7 +2598,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="36"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -6378,7 +6386,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="31"/>
+      <c r="A198" s="27"/>
       <c r="B198" s="9">
         <v>1618</v>
       </c>
@@ -6434,7 +6442,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="34" t="s">
+      <c r="A200" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B200" s="8">
@@ -6464,7 +6472,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="35"/>
+      <c r="A201" s="29"/>
       <c r="B201" s="2">
         <v>4488</v>
       </c>
@@ -6492,7 +6500,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="35"/>
+      <c r="A202" s="29"/>
       <c r="B202" s="2">
         <v>4954</v>
       </c>
@@ -6520,7 +6528,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="35"/>
+      <c r="A203" s="29"/>
       <c r="B203" s="2">
         <v>4642</v>
       </c>
@@ -6548,7 +6556,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="35"/>
+      <c r="A204" s="29"/>
       <c r="B204" s="2">
         <v>5537</v>
       </c>
@@ -6576,7 +6584,7 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="35"/>
+      <c r="A205" s="29"/>
       <c r="B205" s="2">
         <v>5847</v>
       </c>
@@ -6604,7 +6612,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="35"/>
+      <c r="A206" s="29"/>
       <c r="B206" s="2">
         <v>4769</v>
       </c>
@@ -6632,7 +6640,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="35"/>
+      <c r="A207" s="29"/>
       <c r="B207" s="2">
         <v>9930</v>
       </c>
@@ -6655,12 +6663,12 @@
       <c r="S207" s="2"/>
       <c r="T207" s="5"/>
       <c r="U207">
-        <f t="shared" ref="U207:U285" ca="1" si="6">IF(B207=$W$1,1,0)</f>
+        <f t="shared" ref="U207:U286" ca="1" si="6">IF(B207=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="35"/>
+      <c r="A208" s="29"/>
       <c r="B208" s="2">
         <v>6861</v>
       </c>
@@ -6688,7 +6696,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="35"/>
+      <c r="A209" s="29"/>
       <c r="B209" s="2">
         <v>3226</v>
       </c>
@@ -6716,7 +6724,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="35"/>
+      <c r="A210" s="29"/>
       <c r="B210" s="2">
         <v>4372</v>
       </c>
@@ -6744,7 +6752,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="35"/>
+      <c r="A211" s="29"/>
       <c r="B211" s="2">
         <v>4463</v>
       </c>
@@ -6772,7 +6780,7 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="35"/>
+      <c r="A212" s="29"/>
       <c r="B212" s="2">
         <v>1668</v>
       </c>
@@ -6800,7 +6808,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="35"/>
+      <c r="A213" s="29"/>
       <c r="B213" s="2">
         <v>9417</v>
       </c>
@@ -6828,7 +6836,7 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="35"/>
+      <c r="A214" s="29"/>
       <c r="B214" s="2">
         <v>3148</v>
       </c>
@@ -6856,7 +6864,7 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="35"/>
+      <c r="A215" s="29"/>
       <c r="B215" s="2">
         <v>2137</v>
       </c>
@@ -6884,7 +6892,7 @@
       </c>
     </row>
     <row r="216" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="36"/>
+      <c r="A216" s="30"/>
       <c r="B216" s="6">
         <v>5621</v>
       </c>
@@ -8234,7 +8242,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>2662</v>
+        <v>9238</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8262,7 +8270,7 @@
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8290,7 +8298,7 @@
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8318,7 +8326,7 @@
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8346,7 +8354,7 @@
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8374,7 +8382,7 @@
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8402,7 +8410,7 @@
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8430,7 +8438,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="23"/>
       <c r="B271" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8458,7 +8466,7 @@
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="23"/>
       <c r="B272" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8483,87 +8491,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="24"/>
-      <c r="B273" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C273" s="6"/>
-      <c r="D273" s="6"/>
-      <c r="E273" s="6"/>
-      <c r="F273" s="6"/>
-      <c r="G273" s="6"/>
-      <c r="H273" s="6"/>
-      <c r="I273" s="6"/>
-      <c r="J273" s="6"/>
-      <c r="K273" s="6"/>
-      <c r="L273" s="6"/>
-      <c r="M273" s="6"/>
-      <c r="N273" s="6"/>
-      <c r="O273" s="6"/>
-      <c r="P273" s="6"/>
-      <c r="Q273" s="6"/>
-      <c r="R273" s="6"/>
-      <c r="S273" s="6"/>
-      <c r="T273" s="7"/>
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A273" s="23"/>
+      <c r="B273" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C273" s="2"/>
+      <c r="D273" s="2"/>
+      <c r="E273" s="2"/>
+      <c r="F273" s="2"/>
+      <c r="G273" s="2"/>
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+      <c r="J273" s="2"/>
+      <c r="K273" s="2"/>
+      <c r="L273" s="2"/>
+      <c r="M273" s="2"/>
+      <c r="N273" s="2"/>
+      <c r="O273" s="2"/>
+      <c r="P273" s="2"/>
+      <c r="Q273" s="2"/>
+      <c r="R273" s="2"/>
+      <c r="S273" s="2"/>
+      <c r="T273" s="5"/>
       <c r="U273">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B274" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C274" s="8"/>
-      <c r="D274" s="8"/>
-      <c r="E274" s="8"/>
-      <c r="F274" s="8"/>
-      <c r="G274" s="8"/>
-      <c r="H274" s="8"/>
-      <c r="I274" s="8"/>
-      <c r="J274" s="8"/>
-      <c r="K274" s="8"/>
-      <c r="L274" s="8"/>
-      <c r="M274" s="8"/>
-      <c r="N274" s="8"/>
-      <c r="O274" s="8"/>
-      <c r="P274" s="8"/>
-      <c r="Q274" s="8"/>
-      <c r="R274" s="8"/>
-      <c r="S274" s="8"/>
-      <c r="T274" s="14"/>
+    <row r="274" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A274" s="24"/>
+      <c r="B274" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C274" s="6"/>
+      <c r="D274" s="6"/>
+      <c r="E274" s="6"/>
+      <c r="F274" s="6"/>
+      <c r="G274" s="6"/>
+      <c r="H274" s="6"/>
+      <c r="I274" s="6"/>
+      <c r="J274" s="6"/>
+      <c r="K274" s="6"/>
+      <c r="L274" s="6"/>
+      <c r="M274" s="6"/>
+      <c r="N274" s="6"/>
+      <c r="O274" s="6"/>
+      <c r="P274" s="6"/>
+      <c r="Q274" s="6"/>
+      <c r="R274" s="6"/>
+      <c r="S274" s="6"/>
+      <c r="T274" s="7"/>
       <c r="U274">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="23"/>
+      <c r="A275" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="B275" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2"/>
-      <c r="E275" s="2"/>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="2"/>
-      <c r="J275" s="2"/>
-      <c r="K275" s="2"/>
-      <c r="L275" s="2"/>
-      <c r="M275" s="2"/>
-      <c r="N275" s="2"/>
-      <c r="O275" s="2"/>
-      <c r="P275" s="2"/>
-      <c r="Q275" s="2"/>
-      <c r="R275" s="2"/>
-      <c r="S275" s="2"/>
-      <c r="T275" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C275" s="8"/>
+      <c r="D275" s="8"/>
+      <c r="E275" s="8"/>
+      <c r="F275" s="8"/>
+      <c r="G275" s="8"/>
+      <c r="H275" s="8"/>
+      <c r="I275" s="8"/>
+      <c r="J275" s="8"/>
+      <c r="K275" s="8"/>
+      <c r="L275" s="8"/>
+      <c r="M275" s="8"/>
+      <c r="N275" s="8"/>
+      <c r="O275" s="8"/>
+      <c r="P275" s="8"/>
+      <c r="Q275" s="8"/>
+      <c r="R275" s="8"/>
+      <c r="S275" s="8"/>
+      <c r="T275" s="14"/>
       <c r="U275">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8572,7 +8580,7 @@
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A276" s="23"/>
       <c r="B276" s="2">
-        <v>9990</v>
+        <v>1056</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8600,7 +8608,7 @@
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" s="23"/>
       <c r="B277" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8628,7 +8636,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="23"/>
       <c r="B278" s="2">
-        <v>8418</v>
+        <v>7738</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8656,7 +8664,7 @@
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" s="23"/>
       <c r="B279" s="2">
-        <v>9512</v>
+        <v>8418</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8684,7 +8692,7 @@
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" s="23"/>
       <c r="B280" s="2">
-        <v>9924</v>
+        <v>9512</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8710,37 +8718,37 @@
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="31"/>
-      <c r="B281" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C281" s="9"/>
-      <c r="D281" s="9"/>
-      <c r="E281" s="9"/>
-      <c r="F281" s="9"/>
-      <c r="G281" s="9"/>
-      <c r="H281" s="9"/>
-      <c r="I281" s="9"/>
-      <c r="J281" s="9"/>
-      <c r="K281" s="9"/>
-      <c r="L281" s="9"/>
-      <c r="M281" s="9"/>
-      <c r="N281" s="9"/>
-      <c r="O281" s="9"/>
-      <c r="P281" s="9"/>
-      <c r="Q281" s="9"/>
-      <c r="R281" s="9"/>
-      <c r="S281" s="9"/>
-      <c r="T281" s="15"/>
+      <c r="A281" s="23"/>
+      <c r="B281" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C281" s="2"/>
+      <c r="D281" s="2"/>
+      <c r="E281" s="2"/>
+      <c r="F281" s="2"/>
+      <c r="G281" s="2"/>
+      <c r="H281" s="2"/>
+      <c r="I281" s="2"/>
+      <c r="J281" s="2"/>
+      <c r="K281" s="2"/>
+      <c r="L281" s="2"/>
+      <c r="M281" s="2"/>
+      <c r="N281" s="2"/>
+      <c r="O281" s="2"/>
+      <c r="P281" s="2"/>
+      <c r="Q281" s="2"/>
+      <c r="R281" s="2"/>
+      <c r="S281" s="2"/>
+      <c r="T281" s="5"/>
       <c r="U281">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="31"/>
+      <c r="A282" s="27"/>
       <c r="B282" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C282" s="9"/>
       <c r="D282" s="9"/>
@@ -8766,9 +8774,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="31"/>
+      <c r="A283" s="27"/>
       <c r="B283" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C283" s="9"/>
       <c r="D283" s="9"/>
@@ -8794,9 +8802,9 @@
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="31"/>
+      <c r="A284" s="27"/>
       <c r="B284" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C284" s="9"/>
       <c r="D284" s="9"/>
@@ -8822,9 +8830,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="31"/>
+      <c r="A285" s="27"/>
       <c r="B285" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C285" s="9"/>
       <c r="D285" s="9"/>
@@ -8849,87 +8857,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="24"/>
-      <c r="B286" s="6">
+    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A286" s="27"/>
+      <c r="B286" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C286" s="9"/>
+      <c r="D286" s="9"/>
+      <c r="E286" s="9"/>
+      <c r="F286" s="9"/>
+      <c r="G286" s="9"/>
+      <c r="H286" s="9"/>
+      <c r="I286" s="9"/>
+      <c r="J286" s="9"/>
+      <c r="K286" s="9"/>
+      <c r="L286" s="9"/>
+      <c r="M286" s="9"/>
+      <c r="N286" s="9"/>
+      <c r="O286" s="9"/>
+      <c r="P286" s="9"/>
+      <c r="Q286" s="9"/>
+      <c r="R286" s="9"/>
+      <c r="S286" s="9"/>
+      <c r="T286" s="15"/>
+      <c r="U286">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="24"/>
+      <c r="B287" s="6">
         <v>6876</v>
       </c>
-      <c r="C286" s="6"/>
-      <c r="D286" s="6"/>
-      <c r="E286" s="6"/>
-      <c r="F286" s="6"/>
-      <c r="G286" s="6"/>
-      <c r="H286" s="6"/>
-      <c r="I286" s="6"/>
-      <c r="J286" s="6"/>
-      <c r="K286" s="6"/>
-      <c r="L286" s="6"/>
-      <c r="M286" s="6"/>
-      <c r="N286" s="6"/>
-      <c r="O286" s="6"/>
-      <c r="P286" s="6"/>
-      <c r="Q286" s="6"/>
-      <c r="R286" s="6"/>
-      <c r="S286" s="6"/>
-      <c r="T286" s="7"/>
-      <c r="U286">
-        <f t="shared" ref="U286:U349" ca="1" si="7">IF(B286=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="22" t="s">
+      <c r="C287" s="6"/>
+      <c r="D287" s="6"/>
+      <c r="E287" s="6"/>
+      <c r="F287" s="6"/>
+      <c r="G287" s="6"/>
+      <c r="H287" s="6"/>
+      <c r="I287" s="6"/>
+      <c r="J287" s="6"/>
+      <c r="K287" s="6"/>
+      <c r="L287" s="6"/>
+      <c r="M287" s="6"/>
+      <c r="N287" s="6"/>
+      <c r="O287" s="6"/>
+      <c r="P287" s="6"/>
+      <c r="Q287" s="6"/>
+      <c r="R287" s="6"/>
+      <c r="S287" s="6"/>
+      <c r="T287" s="7"/>
+      <c r="U287">
+        <f t="shared" ref="U287:U350" ca="1" si="7">IF(B287=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A288" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B287" s="8">
+      <c r="B288" s="8">
         <v>4304</v>
       </c>
-      <c r="C287" s="8"/>
-      <c r="D287" s="8"/>
-      <c r="E287" s="8"/>
-      <c r="F287" s="8"/>
-      <c r="G287" s="8"/>
-      <c r="H287" s="8"/>
-      <c r="I287" s="8"/>
-      <c r="J287" s="8"/>
-      <c r="K287" s="8"/>
-      <c r="L287" s="8"/>
-      <c r="M287" s="8"/>
-      <c r="N287" s="8"/>
-      <c r="O287" s="8"/>
-      <c r="P287" s="8"/>
-      <c r="Q287" s="8"/>
-      <c r="R287" s="8"/>
-      <c r="S287" s="8"/>
-      <c r="T287" s="14"/>
-      <c r="U287">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="23"/>
-      <c r="B288" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2"/>
-      <c r="E288" s="2"/>
-      <c r="F288" s="2"/>
-      <c r="G288" s="2"/>
-      <c r="H288" s="2"/>
-      <c r="I288" s="2"/>
-      <c r="J288" s="2"/>
-      <c r="K288" s="2"/>
-      <c r="L288" s="2"/>
-      <c r="M288" s="2"/>
-      <c r="N288" s="2"/>
-      <c r="O288" s="2"/>
-      <c r="P288" s="2"/>
-      <c r="Q288" s="2"/>
-      <c r="R288" s="2"/>
-      <c r="S288" s="2"/>
-      <c r="T288" s="5"/>
+      <c r="C288" s="8"/>
+      <c r="D288" s="8"/>
+      <c r="E288" s="8"/>
+      <c r="F288" s="8"/>
+      <c r="G288" s="8"/>
+      <c r="H288" s="8"/>
+      <c r="I288" s="8"/>
+      <c r="J288" s="8"/>
+      <c r="K288" s="8"/>
+      <c r="L288" s="8"/>
+      <c r="M288" s="8"/>
+      <c r="N288" s="8"/>
+      <c r="O288" s="8"/>
+      <c r="P288" s="8"/>
+      <c r="Q288" s="8"/>
+      <c r="R288" s="8"/>
+      <c r="S288" s="8"/>
+      <c r="T288" s="14"/>
       <c r="U288">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -8938,7 +8946,7 @@
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" s="23"/>
       <c r="B289" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -8966,7 +8974,7 @@
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="23"/>
       <c r="B290" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8991,87 +8999,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="24"/>
-      <c r="B291" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C291" s="6"/>
-      <c r="D291" s="6"/>
-      <c r="E291" s="6"/>
-      <c r="F291" s="6"/>
-      <c r="G291" s="6"/>
-      <c r="H291" s="6"/>
-      <c r="I291" s="6"/>
-      <c r="J291" s="6"/>
-      <c r="K291" s="6"/>
-      <c r="L291" s="6"/>
-      <c r="M291" s="6"/>
-      <c r="N291" s="6"/>
-      <c r="O291" s="6"/>
-      <c r="P291" s="6"/>
-      <c r="Q291" s="6"/>
-      <c r="R291" s="6"/>
-      <c r="S291" s="6"/>
-      <c r="T291" s="7"/>
+    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A291" s="23"/>
+      <c r="B291" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C291" s="2"/>
+      <c r="D291" s="2"/>
+      <c r="E291" s="2"/>
+      <c r="F291" s="2"/>
+      <c r="G291" s="2"/>
+      <c r="H291" s="2"/>
+      <c r="I291" s="2"/>
+      <c r="J291" s="2"/>
+      <c r="K291" s="2"/>
+      <c r="L291" s="2"/>
+      <c r="M291" s="2"/>
+      <c r="N291" s="2"/>
+      <c r="O291" s="2"/>
+      <c r="P291" s="2"/>
+      <c r="Q291" s="2"/>
+      <c r="R291" s="2"/>
+      <c r="S291" s="2"/>
+      <c r="T291" s="5"/>
       <c r="U291">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A292" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B292" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C292" s="8"/>
-      <c r="D292" s="8"/>
-      <c r="E292" s="8"/>
-      <c r="F292" s="8"/>
-      <c r="G292" s="8"/>
-      <c r="H292" s="8"/>
-      <c r="I292" s="8"/>
-      <c r="J292" s="8"/>
-      <c r="K292" s="8"/>
-      <c r="L292" s="8"/>
-      <c r="M292" s="8"/>
-      <c r="N292" s="8"/>
-      <c r="O292" s="8"/>
-      <c r="P292" s="8"/>
-      <c r="Q292" s="8"/>
-      <c r="R292" s="8"/>
-      <c r="S292" s="8"/>
-      <c r="T292" s="14"/>
+    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="24"/>
+      <c r="B292" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C292" s="6"/>
+      <c r="D292" s="6"/>
+      <c r="E292" s="6"/>
+      <c r="F292" s="6"/>
+      <c r="G292" s="6"/>
+      <c r="H292" s="6"/>
+      <c r="I292" s="6"/>
+      <c r="J292" s="6"/>
+      <c r="K292" s="6"/>
+      <c r="L292" s="6"/>
+      <c r="M292" s="6"/>
+      <c r="N292" s="6"/>
+      <c r="O292" s="6"/>
+      <c r="P292" s="6"/>
+      <c r="Q292" s="6"/>
+      <c r="R292" s="6"/>
+      <c r="S292" s="6"/>
+      <c r="T292" s="7"/>
       <c r="U292">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A293" s="23"/>
-      <c r="B293" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2"/>
-      <c r="E293" s="2"/>
-      <c r="F293" s="2"/>
-      <c r="G293" s="2"/>
-      <c r="H293" s="2"/>
-      <c r="I293" s="2"/>
-      <c r="J293" s="2"/>
-      <c r="K293" s="2"/>
-      <c r="L293" s="2"/>
-      <c r="M293" s="2"/>
-      <c r="N293" s="2"/>
-      <c r="O293" s="2"/>
-      <c r="P293" s="2"/>
-      <c r="Q293" s="2"/>
-      <c r="R293" s="2"/>
-      <c r="S293" s="2"/>
-      <c r="T293" s="5"/>
+      <c r="A293" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B293" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C293" s="8"/>
+      <c r="D293" s="8"/>
+      <c r="E293" s="8"/>
+      <c r="F293" s="8"/>
+      <c r="G293" s="8"/>
+      <c r="H293" s="8"/>
+      <c r="I293" s="8"/>
+      <c r="J293" s="8"/>
+      <c r="K293" s="8"/>
+      <c r="L293" s="8"/>
+      <c r="M293" s="8"/>
+      <c r="N293" s="8"/>
+      <c r="O293" s="8"/>
+      <c r="P293" s="8"/>
+      <c r="Q293" s="8"/>
+      <c r="R293" s="8"/>
+      <c r="S293" s="8"/>
+      <c r="T293" s="14"/>
       <c r="U293">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9080,7 +9088,7 @@
     <row r="294" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A294" s="23"/>
       <c r="B294" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9105,10 +9113,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A295" s="23"/>
-      <c r="B295" s="2">
-        <v>7170</v>
+      <c r="B295" s="12">
+        <v>7546</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9136,7 +9144,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="23"/>
       <c r="B296" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9164,7 +9172,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="23"/>
       <c r="B297" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9192,7 +9200,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="23"/>
       <c r="B298" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9220,7 +9228,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="23"/>
       <c r="B299" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9248,7 +9256,7 @@
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" s="23"/>
       <c r="B300" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9276,7 +9284,7 @@
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A301" s="23"/>
       <c r="B301" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9304,7 +9312,7 @@
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9332,7 +9340,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9360,7 +9368,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9388,7 +9396,7 @@
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="23"/>
       <c r="B305" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9416,7 +9424,7 @@
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A306" s="23"/>
       <c r="B306" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -9441,87 +9449,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A307" s="24"/>
-      <c r="B307" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C307" s="6"/>
-      <c r="D307" s="6"/>
-      <c r="E307" s="6"/>
-      <c r="F307" s="6"/>
-      <c r="G307" s="6"/>
-      <c r="H307" s="6"/>
-      <c r="I307" s="6"/>
-      <c r="J307" s="6"/>
-      <c r="K307" s="6"/>
-      <c r="L307" s="6"/>
-      <c r="M307" s="6"/>
-      <c r="N307" s="6"/>
-      <c r="O307" s="6"/>
-      <c r="P307" s="6"/>
-      <c r="Q307" s="6"/>
-      <c r="R307" s="6"/>
-      <c r="S307" s="6"/>
-      <c r="T307" s="7"/>
+    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A307" s="23"/>
+      <c r="B307" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C307" s="2"/>
+      <c r="D307" s="2"/>
+      <c r="E307" s="2"/>
+      <c r="F307" s="2"/>
+      <c r="G307" s="2"/>
+      <c r="H307" s="2"/>
+      <c r="I307" s="2"/>
+      <c r="J307" s="2"/>
+      <c r="K307" s="2"/>
+      <c r="L307" s="2"/>
+      <c r="M307" s="2"/>
+      <c r="N307" s="2"/>
+      <c r="O307" s="2"/>
+      <c r="P307" s="2"/>
+      <c r="Q307" s="2"/>
+      <c r="R307" s="2"/>
+      <c r="S307" s="2"/>
+      <c r="T307" s="5"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A308" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B308" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C308" s="8"/>
-      <c r="D308" s="8"/>
-      <c r="E308" s="8"/>
-      <c r="F308" s="8"/>
-      <c r="G308" s="8"/>
-      <c r="H308" s="8"/>
-      <c r="I308" s="8"/>
-      <c r="J308" s="8"/>
-      <c r="K308" s="8"/>
-      <c r="L308" s="8"/>
-      <c r="M308" s="8"/>
-      <c r="N308" s="8"/>
-      <c r="O308" s="8"/>
-      <c r="P308" s="8"/>
-      <c r="Q308" s="8"/>
-      <c r="R308" s="8"/>
-      <c r="S308" s="8"/>
-      <c r="T308" s="14"/>
+    <row r="308" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A308" s="24"/>
+      <c r="B308" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C308" s="6"/>
+      <c r="D308" s="6"/>
+      <c r="E308" s="6"/>
+      <c r="F308" s="6"/>
+      <c r="G308" s="6"/>
+      <c r="H308" s="6"/>
+      <c r="I308" s="6"/>
+      <c r="J308" s="6"/>
+      <c r="K308" s="6"/>
+      <c r="L308" s="6"/>
+      <c r="M308" s="6"/>
+      <c r="N308" s="6"/>
+      <c r="O308" s="6"/>
+      <c r="P308" s="6"/>
+      <c r="Q308" s="6"/>
+      <c r="R308" s="6"/>
+      <c r="S308" s="6"/>
+      <c r="T308" s="7"/>
       <c r="U308">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A309" s="23"/>
-      <c r="B309" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C309" s="2"/>
-      <c r="D309" s="2"/>
-      <c r="E309" s="2"/>
-      <c r="F309" s="2"/>
-      <c r="G309" s="2"/>
-      <c r="H309" s="2"/>
-      <c r="I309" s="2"/>
-      <c r="J309" s="2"/>
-      <c r="K309" s="2"/>
-      <c r="L309" s="2"/>
-      <c r="M309" s="2"/>
-      <c r="N309" s="2"/>
-      <c r="O309" s="2"/>
-      <c r="P309" s="2"/>
-      <c r="Q309" s="2"/>
-      <c r="R309" s="2"/>
-      <c r="S309" s="2"/>
-      <c r="T309" s="5"/>
+      <c r="A309" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B309" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C309" s="8"/>
+      <c r="D309" s="8"/>
+      <c r="E309" s="8"/>
+      <c r="F309" s="8"/>
+      <c r="G309" s="8"/>
+      <c r="H309" s="8"/>
+      <c r="I309" s="8"/>
+      <c r="J309" s="8"/>
+      <c r="K309" s="8"/>
+      <c r="L309" s="8"/>
+      <c r="M309" s="8"/>
+      <c r="N309" s="8"/>
+      <c r="O309" s="8"/>
+      <c r="P309" s="8"/>
+      <c r="Q309" s="8"/>
+      <c r="R309" s="8"/>
+      <c r="S309" s="8"/>
+      <c r="T309" s="14"/>
       <c r="U309">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9530,7 +9538,7 @@
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="23"/>
       <c r="B310" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9558,7 +9566,7 @@
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A311" s="23"/>
       <c r="B311" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9586,7 +9594,7 @@
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A312" s="23"/>
       <c r="B312" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -9611,87 +9619,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A313" s="24"/>
-      <c r="B313" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C313" s="6"/>
-      <c r="D313" s="6"/>
-      <c r="E313" s="6"/>
-      <c r="F313" s="6"/>
-      <c r="G313" s="6"/>
-      <c r="H313" s="6"/>
-      <c r="I313" s="6"/>
-      <c r="J313" s="6"/>
-      <c r="K313" s="6"/>
-      <c r="L313" s="6"/>
-      <c r="M313" s="6"/>
-      <c r="N313" s="6"/>
-      <c r="O313" s="6"/>
-      <c r="P313" s="6"/>
-      <c r="Q313" s="6"/>
-      <c r="R313" s="6"/>
-      <c r="S313" s="6"/>
-      <c r="T313" s="7"/>
+    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A313" s="23"/>
+      <c r="B313" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C313" s="2"/>
+      <c r="D313" s="2"/>
+      <c r="E313" s="2"/>
+      <c r="F313" s="2"/>
+      <c r="G313" s="2"/>
+      <c r="H313" s="2"/>
+      <c r="I313" s="2"/>
+      <c r="J313" s="2"/>
+      <c r="K313" s="2"/>
+      <c r="L313" s="2"/>
+      <c r="M313" s="2"/>
+      <c r="N313" s="2"/>
+      <c r="O313" s="2"/>
+      <c r="P313" s="2"/>
+      <c r="Q313" s="2"/>
+      <c r="R313" s="2"/>
+      <c r="S313" s="2"/>
+      <c r="T313" s="5"/>
       <c r="U313">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B314" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C314" s="8"/>
-      <c r="D314" s="8"/>
-      <c r="E314" s="8"/>
-      <c r="F314" s="8"/>
-      <c r="G314" s="8"/>
-      <c r="H314" s="8"/>
-      <c r="I314" s="8"/>
-      <c r="J314" s="8"/>
-      <c r="K314" s="8"/>
-      <c r="L314" s="8"/>
-      <c r="M314" s="8"/>
-      <c r="N314" s="8"/>
-      <c r="O314" s="8"/>
-      <c r="P314" s="8"/>
-      <c r="Q314" s="8"/>
-      <c r="R314" s="8"/>
-      <c r="S314" s="8"/>
-      <c r="T314" s="14"/>
+    <row r="314" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="24"/>
+      <c r="B314" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C314" s="6"/>
+      <c r="D314" s="6"/>
+      <c r="E314" s="6"/>
+      <c r="F314" s="6"/>
+      <c r="G314" s="6"/>
+      <c r="H314" s="6"/>
+      <c r="I314" s="6"/>
+      <c r="J314" s="6"/>
+      <c r="K314" s="6"/>
+      <c r="L314" s="6"/>
+      <c r="M314" s="6"/>
+      <c r="N314" s="6"/>
+      <c r="O314" s="6"/>
+      <c r="P314" s="6"/>
+      <c r="Q314" s="6"/>
+      <c r="R314" s="6"/>
+      <c r="S314" s="6"/>
+      <c r="T314" s="7"/>
       <c r="U314">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="23"/>
-      <c r="B315" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C315" s="2"/>
-      <c r="D315" s="2"/>
-      <c r="E315" s="2"/>
-      <c r="F315" s="2"/>
-      <c r="G315" s="2"/>
-      <c r="H315" s="2"/>
-      <c r="I315" s="2"/>
-      <c r="J315" s="2"/>
-      <c r="K315" s="2"/>
-      <c r="L315" s="2"/>
-      <c r="M315" s="2"/>
-      <c r="N315" s="2"/>
-      <c r="O315" s="2"/>
-      <c r="P315" s="2"/>
-      <c r="Q315" s="2"/>
-      <c r="R315" s="2"/>
-      <c r="S315" s="2"/>
-      <c r="T315" s="5"/>
+      <c r="A315" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B315" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C315" s="8"/>
+      <c r="D315" s="8"/>
+      <c r="E315" s="8"/>
+      <c r="F315" s="8"/>
+      <c r="G315" s="8"/>
+      <c r="H315" s="8"/>
+      <c r="I315" s="8"/>
+      <c r="J315" s="8"/>
+      <c r="K315" s="8"/>
+      <c r="L315" s="8"/>
+      <c r="M315" s="8"/>
+      <c r="N315" s="8"/>
+      <c r="O315" s="8"/>
+      <c r="P315" s="8"/>
+      <c r="Q315" s="8"/>
+      <c r="R315" s="8"/>
+      <c r="S315" s="8"/>
+      <c r="T315" s="14"/>
       <c r="U315">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9700,7 +9708,7 @@
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A316" s="23"/>
       <c r="B316" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9728,7 +9736,7 @@
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A317" s="23"/>
       <c r="B317" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -9756,7 +9764,7 @@
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A318" s="23"/>
       <c r="B318" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -9781,35 +9789,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A319" s="24"/>
-      <c r="B319" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C319" s="6"/>
-      <c r="D319" s="6"/>
-      <c r="E319" s="6"/>
-      <c r="F319" s="6"/>
-      <c r="G319" s="6"/>
-      <c r="H319" s="6"/>
-      <c r="I319" s="6"/>
-      <c r="J319" s="6"/>
-      <c r="K319" s="6"/>
-      <c r="L319" s="6"/>
-      <c r="M319" s="6"/>
-      <c r="N319" s="6"/>
-      <c r="O319" s="6"/>
-      <c r="P319" s="6"/>
-      <c r="Q319" s="6"/>
-      <c r="R319" s="6"/>
-      <c r="S319" s="6"/>
-      <c r="T319" s="7"/>
+    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A319" s="23"/>
+      <c r="B319" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C319" s="2"/>
+      <c r="D319" s="2"/>
+      <c r="E319" s="2"/>
+      <c r="F319" s="2"/>
+      <c r="G319" s="2"/>
+      <c r="H319" s="2"/>
+      <c r="I319" s="2"/>
+      <c r="J319" s="2"/>
+      <c r="K319" s="2"/>
+      <c r="L319" s="2"/>
+      <c r="M319" s="2"/>
+      <c r="N319" s="2"/>
+      <c r="O319" s="2"/>
+      <c r="P319" s="2"/>
+      <c r="Q319" s="2"/>
+      <c r="R319" s="2"/>
+      <c r="S319" s="2"/>
+      <c r="T319" s="5"/>
       <c r="U319">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="24"/>
+      <c r="B320" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C320" s="6"/>
+      <c r="D320" s="6"/>
+      <c r="E320" s="6"/>
+      <c r="F320" s="6"/>
+      <c r="G320" s="6"/>
+      <c r="H320" s="6"/>
+      <c r="I320" s="6"/>
+      <c r="J320" s="6"/>
+      <c r="K320" s="6"/>
+      <c r="L320" s="6"/>
+      <c r="M320" s="6"/>
+      <c r="N320" s="6"/>
+      <c r="O320" s="6"/>
+      <c r="P320" s="6"/>
+      <c r="Q320" s="6"/>
+      <c r="R320" s="6"/>
+      <c r="S320" s="6"/>
+      <c r="T320" s="7"/>
       <c r="U320">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9991,13 +10021,13 @@
     </row>
     <row r="350" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U350">
-        <f t="shared" ref="U350:U413" ca="1" si="8">IF(B350=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="351" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U351">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U351:U414" ca="1" si="8">IF(B351=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10375,13 +10405,13 @@
     </row>
     <row r="414" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U414">
-        <f t="shared" ref="U414:U477" ca="1" si="9">IF(B414=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="415" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U415">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U415:U478" ca="1" si="9">IF(B415=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10759,13 +10789,13 @@
     </row>
     <row r="478" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U478">
-        <f t="shared" ref="U478:U541" ca="1" si="10">IF(B478=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="479" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U479">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U479:U542" ca="1" si="10">IF(B479=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11143,13 +11173,13 @@
     </row>
     <row r="542" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U542">
-        <f t="shared" ref="U542:U605" ca="1" si="11">IF(B542=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="543" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U543">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U543:U606" ca="1" si="11">IF(B543=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11527,13 +11557,13 @@
     </row>
     <row r="606" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U606">
-        <f t="shared" ref="U606:U669" ca="1" si="12">IF(B606=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="607" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U607">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U607:U670" ca="1" si="12">IF(B607=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11911,13 +11941,13 @@
     </row>
     <row r="670" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U670">
-        <f t="shared" ref="U670:U733" ca="1" si="13">IF(B670=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="671" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U671">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U671:U734" ca="1" si="13">IF(B671=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12295,13 +12325,13 @@
     </row>
     <row r="734" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U734">
-        <f t="shared" ref="U734:U797" ca="1" si="14">IF(B734=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="735" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U735">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U735:U798" ca="1" si="14">IF(B735=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12679,13 +12709,13 @@
     </row>
     <row r="798" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U798">
-        <f t="shared" ref="U798:U861" ca="1" si="15">IF(B798=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="799" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U799">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U799:U862" ca="1" si="15">IF(B799=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13063,13 +13093,13 @@
     </row>
     <row r="862" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U862">
-        <f t="shared" ref="U862:U923" ca="1" si="16">IF(B862=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="863" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U863">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U863:U924" ca="1" si="16">IF(B863=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13433,13 +13463,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="924" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U924">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A314:A319"/>
-    <mergeCell ref="A245:A273"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A288:A292"/>
+    <mergeCell ref="A275:A287"/>
+    <mergeCell ref="A315:A320"/>
+    <mergeCell ref="A245:A274"/>
     <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A292:A307"/>
-    <mergeCell ref="A308:A313"/>
+    <mergeCell ref="A293:A308"/>
+    <mergeCell ref="A309:A314"/>
     <mergeCell ref="A64:A104"/>
     <mergeCell ref="A217:A228"/>
     <mergeCell ref="A150:A181"/>
@@ -13449,10 +13489,6 @@
     <mergeCell ref="A200:A216"/>
     <mergeCell ref="A229:A236"/>
     <mergeCell ref="A237:A244"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A287:A291"/>
-    <mergeCell ref="A274:A286"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add more tasks to lab07 for better understanding of theme
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$292</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$294</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -530,24 +530,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,6 +547,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W924"/>
+  <dimension ref="A1:W926"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U261" sqref="U261"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M162" sqref="M162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,56 +891,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>2574</v>
+        <v>9571</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="33"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -970,7 +970,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1898,7 +1898,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1926,7 +1926,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1954,7 +1954,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="35"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
+      <c r="A58" s="35"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="35"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2542,7 +2542,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2598,7 +2598,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="30"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -4781,7 +4781,7 @@
       <c r="S140" s="2"/>
       <c r="T140" s="5"/>
       <c r="U140">
-        <f t="shared" ref="U140:U206" ca="1" si="4">IF(B140=$W$1,1,0)</f>
+        <f t="shared" ref="U140:U208" ca="1" si="4">IF(B140=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5182,7 +5182,7 @@
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="23"/>
       <c r="B155" s="2">
-        <v>5683</v>
+        <v>1433</v>
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -5210,7 +5210,7 @@
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="23"/>
       <c r="B156" s="2">
-        <v>1223</v>
+        <v>5683</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -5238,7 +5238,7 @@
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="23"/>
       <c r="B157" s="2">
-        <v>8311</v>
+        <v>1223</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -5266,7 +5266,7 @@
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="23"/>
       <c r="B158" s="2">
-        <v>3134</v>
+        <v>8311</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -5294,7 +5294,7 @@
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="23"/>
       <c r="B159" s="2">
-        <v>9711</v>
+        <v>3134</v>
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -5322,7 +5322,7 @@
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="23"/>
       <c r="B160" s="2">
-        <v>3333</v>
+        <v>9711</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
@@ -5350,7 +5350,7 @@
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="23"/>
       <c r="B161" s="2">
-        <v>8820</v>
+        <v>7085</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
@@ -5378,7 +5378,7 @@
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="23"/>
       <c r="B162" s="2">
-        <v>5694</v>
+        <v>3333</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -5406,7 +5406,7 @@
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="23"/>
       <c r="B163" s="2">
-        <v>6806</v>
+        <v>8820</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -5434,7 +5434,7 @@
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" s="23"/>
       <c r="B164" s="2">
-        <v>7369</v>
+        <v>5694</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -5462,7 +5462,7 @@
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="23"/>
       <c r="B165" s="2">
-        <v>5894</v>
+        <v>6806</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -5490,7 +5490,7 @@
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="23"/>
       <c r="B166" s="2">
-        <v>4515</v>
+        <v>7369</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -5518,7 +5518,7 @@
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="23"/>
       <c r="B167" s="2">
-        <v>9774</v>
+        <v>5894</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
@@ -5546,7 +5546,7 @@
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="23"/>
       <c r="B168" s="2">
-        <v>3946</v>
+        <v>4515</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -5574,7 +5574,7 @@
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="23"/>
       <c r="B169" s="2">
-        <v>6497</v>
+        <v>9774</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -5602,7 +5602,7 @@
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="23"/>
       <c r="B170" s="2">
-        <v>5648</v>
+        <v>3946</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -5630,7 +5630,7 @@
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="23"/>
       <c r="B171" s="2">
-        <v>3940</v>
+        <v>6497</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -5658,7 +5658,7 @@
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="23"/>
       <c r="B172" s="2">
-        <v>7290</v>
+        <v>5648</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -5686,7 +5686,7 @@
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="23"/>
       <c r="B173" s="2">
-        <v>7035</v>
+        <v>3940</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -5714,7 +5714,7 @@
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="23"/>
       <c r="B174" s="2">
-        <v>9271</v>
+        <v>7290</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -5742,7 +5742,7 @@
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="23"/>
       <c r="B175" s="2">
-        <v>8769</v>
+        <v>7035</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -5770,7 +5770,7 @@
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="23"/>
       <c r="B176" s="2">
-        <v>4497</v>
+        <v>9271</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -5798,7 +5798,7 @@
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="23"/>
       <c r="B177" s="2">
-        <v>3218</v>
+        <v>8769</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
@@ -5826,7 +5826,7 @@
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="23"/>
       <c r="B178" s="2">
-        <v>4293</v>
+        <v>4497</v>
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
@@ -5854,7 +5854,7 @@
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="23"/>
       <c r="B179" s="2">
-        <v>7703</v>
+        <v>3218</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
@@ -5882,7 +5882,7 @@
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="23"/>
       <c r="B180" s="2">
-        <v>5541</v>
+        <v>4293</v>
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
@@ -5907,124 +5907,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="24"/>
-      <c r="B181" s="6">
-        <v>9182</v>
-      </c>
-      <c r="C181" s="6"/>
-      <c r="D181" s="6"/>
-      <c r="E181" s="6"/>
-      <c r="F181" s="6"/>
-      <c r="G181" s="6"/>
-      <c r="H181" s="6"/>
-      <c r="I181" s="6"/>
-      <c r="J181" s="6"/>
-      <c r="K181" s="6"/>
-      <c r="L181" s="6"/>
-      <c r="M181" s="6"/>
-      <c r="N181" s="6"/>
-      <c r="O181" s="6"/>
-      <c r="P181" s="6"/>
-      <c r="Q181" s="6"/>
-      <c r="R181" s="6"/>
-      <c r="S181" s="6"/>
-      <c r="T181" s="7"/>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A181" s="23"/>
+      <c r="B181" s="2">
+        <v>7703</v>
+      </c>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+      <c r="J181" s="2"/>
+      <c r="K181" s="2"/>
+      <c r="L181" s="2"/>
+      <c r="M181" s="2"/>
+      <c r="N181" s="2"/>
+      <c r="O181" s="2"/>
+      <c r="P181" s="2"/>
+      <c r="Q181" s="2"/>
+      <c r="R181" s="2"/>
+      <c r="S181" s="2"/>
+      <c r="T181" s="5"/>
       <c r="U181">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="22" t="s">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A182" s="23"/>
+      <c r="B182" s="2">
+        <v>5541</v>
+      </c>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+      <c r="J182" s="2"/>
+      <c r="K182" s="2"/>
+      <c r="L182" s="2"/>
+      <c r="M182" s="2"/>
+      <c r="N182" s="2"/>
+      <c r="O182" s="2"/>
+      <c r="P182" s="2"/>
+      <c r="Q182" s="2"/>
+      <c r="R182" s="2"/>
+      <c r="S182" s="2"/>
+      <c r="T182" s="5"/>
+      <c r="U182">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="24"/>
+      <c r="B183" s="6">
+        <v>9182</v>
+      </c>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
+      <c r="I183" s="6"/>
+      <c r="J183" s="6"/>
+      <c r="K183" s="6"/>
+      <c r="L183" s="6"/>
+      <c r="M183" s="6"/>
+      <c r="N183" s="6"/>
+      <c r="O183" s="6"/>
+      <c r="P183" s="6"/>
+      <c r="Q183" s="6"/>
+      <c r="R183" s="6"/>
+      <c r="S183" s="6"/>
+      <c r="T183" s="7"/>
+      <c r="U183">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A184" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B182" s="13">
+      <c r="B184" s="13">
         <v>8165</v>
       </c>
-      <c r="C182" s="8"/>
-      <c r="D182" s="8"/>
-      <c r="E182" s="8"/>
-      <c r="F182" s="8"/>
-      <c r="G182" s="8"/>
-      <c r="H182" s="8"/>
-      <c r="I182" s="8"/>
-      <c r="J182" s="8"/>
-      <c r="K182" s="8"/>
-      <c r="L182" s="8"/>
-      <c r="M182" s="8"/>
-      <c r="N182" s="8"/>
-      <c r="O182" s="8"/>
-      <c r="P182" s="8"/>
-      <c r="Q182" s="8"/>
-      <c r="R182" s="8"/>
-      <c r="S182" s="8"/>
-      <c r="T182" s="14"/>
-      <c r="U182">
-        <f t="shared" ref="U182:U199" ca="1" si="5">IF(B182=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="23"/>
-      <c r="B183" s="12">
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="8"/>
+      <c r="F184" s="8"/>
+      <c r="G184" s="8"/>
+      <c r="H184" s="8"/>
+      <c r="I184" s="8"/>
+      <c r="J184" s="8"/>
+      <c r="K184" s="8"/>
+      <c r="L184" s="8"/>
+      <c r="M184" s="8"/>
+      <c r="N184" s="8"/>
+      <c r="O184" s="8"/>
+      <c r="P184" s="8"/>
+      <c r="Q184" s="8"/>
+      <c r="R184" s="8"/>
+      <c r="S184" s="8"/>
+      <c r="T184" s="14"/>
+      <c r="U184">
+        <f t="shared" ref="U184:U201" ca="1" si="5">IF(B184=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="23"/>
+      <c r="B185" s="12">
         <v>9001</v>
-      </c>
-      <c r="C183" s="2"/>
-      <c r="D183" s="2"/>
-      <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
-      <c r="G183" s="2"/>
-      <c r="H183" s="2"/>
-      <c r="I183" s="2"/>
-      <c r="J183" s="2"/>
-      <c r="K183" s="2"/>
-      <c r="L183" s="2"/>
-      <c r="M183" s="2"/>
-      <c r="N183" s="2"/>
-      <c r="O183" s="2"/>
-      <c r="P183" s="2"/>
-      <c r="Q183" s="2"/>
-      <c r="R183" s="2"/>
-      <c r="S183" s="2"/>
-      <c r="T183" s="5"/>
-      <c r="U183">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="23"/>
-      <c r="B184" s="2">
-        <v>7491</v>
-      </c>
-      <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
-      <c r="E184" s="2"/>
-      <c r="F184" s="2"/>
-      <c r="G184" s="2"/>
-      <c r="H184" s="2"/>
-      <c r="I184" s="2"/>
-      <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
-      <c r="L184" s="2"/>
-      <c r="M184" s="2"/>
-      <c r="N184" s="2"/>
-      <c r="O184" s="2"/>
-      <c r="P184" s="2"/>
-      <c r="Q184" s="2"/>
-      <c r="R184" s="2"/>
-      <c r="S184" s="2"/>
-      <c r="T184" s="5"/>
-      <c r="U184">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A185" s="23"/>
-      <c r="B185" s="2">
-        <v>9531</v>
       </c>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
@@ -6052,7 +6052,7 @@
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" s="23"/>
       <c r="B186" s="2">
-        <v>9812</v>
+        <v>7491</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
@@ -6080,7 +6080,7 @@
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="23"/>
       <c r="B187" s="2">
-        <v>9279</v>
+        <v>9531</v>
       </c>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
@@ -6108,7 +6108,7 @@
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" s="23"/>
       <c r="B188" s="2">
-        <v>4845</v>
+        <v>9812</v>
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -6136,7 +6136,7 @@
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="23"/>
       <c r="B189" s="2">
-        <v>5728</v>
+        <v>9279</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
@@ -6164,7 +6164,7 @@
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="23"/>
       <c r="B190" s="2">
-        <v>7222</v>
+        <v>4845</v>
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
@@ -6192,7 +6192,7 @@
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="23"/>
       <c r="B191" s="2">
-        <v>5923</v>
+        <v>5728</v>
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
@@ -6220,7 +6220,7 @@
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="23"/>
       <c r="B192" s="2">
-        <v>4265</v>
+        <v>7222</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -6248,7 +6248,7 @@
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="23"/>
       <c r="B193" s="2">
-        <v>2166</v>
+        <v>5923</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -6276,7 +6276,7 @@
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="23"/>
       <c r="B194" s="2">
-        <v>9116</v>
+        <v>4265</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
@@ -6304,7 +6304,7 @@
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="23"/>
       <c r="B195" s="2">
-        <v>9925</v>
+        <v>2166</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
@@ -6332,7 +6332,7 @@
     <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196" s="23"/>
       <c r="B196" s="2">
-        <v>3657</v>
+        <v>9116</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
@@ -6360,7 +6360,7 @@
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" s="23"/>
       <c r="B197" s="2">
-        <v>6599</v>
+        <v>9925</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -6386,151 +6386,151 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="27"/>
-      <c r="B198" s="9">
-        <v>1618</v>
-      </c>
-      <c r="C198" s="9"/>
-      <c r="D198" s="9"/>
-      <c r="E198" s="9"/>
-      <c r="F198" s="9"/>
-      <c r="G198" s="9"/>
-      <c r="H198" s="9"/>
-      <c r="I198" s="9"/>
-      <c r="J198" s="9"/>
-      <c r="K198" s="9"/>
-      <c r="L198" s="9"/>
-      <c r="M198" s="9"/>
-      <c r="N198" s="9"/>
-      <c r="O198" s="9"/>
-      <c r="P198" s="9"/>
-      <c r="Q198" s="9"/>
-      <c r="R198" s="9"/>
-      <c r="S198" s="9"/>
-      <c r="T198" s="15"/>
+      <c r="A198" s="23"/>
+      <c r="B198" s="2">
+        <v>3657</v>
+      </c>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
+      <c r="E198" s="2"/>
+      <c r="F198" s="2"/>
+      <c r="G198" s="2"/>
+      <c r="H198" s="2"/>
+      <c r="I198" s="2"/>
+      <c r="J198" s="2"/>
+      <c r="K198" s="2"/>
+      <c r="L198" s="2"/>
+      <c r="M198" s="2"/>
+      <c r="N198" s="2"/>
+      <c r="O198" s="2"/>
+      <c r="P198" s="2"/>
+      <c r="Q198" s="2"/>
+      <c r="R198" s="2"/>
+      <c r="S198" s="2"/>
+      <c r="T198" s="5"/>
       <c r="U198">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="24"/>
-      <c r="B199" s="6">
-        <v>1703</v>
-      </c>
-      <c r="C199" s="6"/>
-      <c r="D199" s="6"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
-      <c r="G199" s="6"/>
-      <c r="H199" s="6"/>
-      <c r="I199" s="6"/>
-      <c r="J199" s="6"/>
-      <c r="K199" s="6"/>
-      <c r="L199" s="6"/>
-      <c r="M199" s="6"/>
-      <c r="N199" s="6"/>
-      <c r="O199" s="6"/>
-      <c r="P199" s="6"/>
-      <c r="Q199" s="6"/>
-      <c r="R199" s="6"/>
-      <c r="S199" s="6"/>
-      <c r="T199" s="7"/>
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A199" s="23"/>
+      <c r="B199" s="2">
+        <v>6599</v>
+      </c>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
+      <c r="E199" s="2"/>
+      <c r="F199" s="2"/>
+      <c r="G199" s="2"/>
+      <c r="H199" s="2"/>
+      <c r="I199" s="2"/>
+      <c r="J199" s="2"/>
+      <c r="K199" s="2"/>
+      <c r="L199" s="2"/>
+      <c r="M199" s="2"/>
+      <c r="N199" s="2"/>
+      <c r="O199" s="2"/>
+      <c r="P199" s="2"/>
+      <c r="Q199" s="2"/>
+      <c r="R199" s="2"/>
+      <c r="S199" s="2"/>
+      <c r="T199" s="5"/>
       <c r="U199">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="28" t="s">
+      <c r="A200" s="31"/>
+      <c r="B200" s="9">
+        <v>1618</v>
+      </c>
+      <c r="C200" s="9"/>
+      <c r="D200" s="9"/>
+      <c r="E200" s="9"/>
+      <c r="F200" s="9"/>
+      <c r="G200" s="9"/>
+      <c r="H200" s="9"/>
+      <c r="I200" s="9"/>
+      <c r="J200" s="9"/>
+      <c r="K200" s="9"/>
+      <c r="L200" s="9"/>
+      <c r="M200" s="9"/>
+      <c r="N200" s="9"/>
+      <c r="O200" s="9"/>
+      <c r="P200" s="9"/>
+      <c r="Q200" s="9"/>
+      <c r="R200" s="9"/>
+      <c r="S200" s="9"/>
+      <c r="T200" s="15"/>
+      <c r="U200">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="24"/>
+      <c r="B201" s="6">
+        <v>1703</v>
+      </c>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+      <c r="J201" s="6"/>
+      <c r="K201" s="6"/>
+      <c r="L201" s="6"/>
+      <c r="M201" s="6"/>
+      <c r="N201" s="6"/>
+      <c r="O201" s="6"/>
+      <c r="P201" s="6"/>
+      <c r="Q201" s="6"/>
+      <c r="R201" s="6"/>
+      <c r="S201" s="6"/>
+      <c r="T201" s="7"/>
+      <c r="U201">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A202" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B200" s="8">
+      <c r="B202" s="8">
         <v>6175</v>
       </c>
-      <c r="C200" s="8"/>
-      <c r="D200" s="8"/>
-      <c r="E200" s="8"/>
-      <c r="F200" s="8"/>
-      <c r="G200" s="8"/>
-      <c r="H200" s="8"/>
-      <c r="I200" s="8"/>
-      <c r="J200" s="8"/>
-      <c r="K200" s="8"/>
-      <c r="L200" s="8"/>
-      <c r="M200" s="8"/>
-      <c r="N200" s="8"/>
-      <c r="O200" s="8"/>
-      <c r="P200" s="8"/>
-      <c r="Q200" s="8"/>
-      <c r="R200" s="8"/>
-      <c r="S200" s="8"/>
-      <c r="T200" s="14"/>
-      <c r="U200">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
-      <c r="B201" s="2">
-        <v>4488</v>
-      </c>
-      <c r="C201" s="2"/>
-      <c r="D201" s="2"/>
-      <c r="E201" s="2"/>
-      <c r="F201" s="2"/>
-      <c r="G201" s="2"/>
-      <c r="H201" s="2"/>
-      <c r="I201" s="2"/>
-      <c r="J201" s="2"/>
-      <c r="K201" s="2"/>
-      <c r="L201" s="2"/>
-      <c r="M201" s="2"/>
-      <c r="N201" s="2"/>
-      <c r="O201" s="2"/>
-      <c r="P201" s="2"/>
-      <c r="Q201" s="2"/>
-      <c r="R201" s="2"/>
-      <c r="S201" s="2"/>
-      <c r="T201" s="5"/>
-      <c r="U201">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="29"/>
-      <c r="B202" s="2">
-        <v>4954</v>
-      </c>
-      <c r="C202" s="2"/>
-      <c r="D202" s="2"/>
-      <c r="E202" s="2"/>
-      <c r="F202" s="2"/>
-      <c r="G202" s="2"/>
-      <c r="H202" s="2"/>
-      <c r="I202" s="2"/>
-      <c r="J202" s="2"/>
-      <c r="K202" s="2"/>
-      <c r="L202" s="2"/>
-      <c r="M202" s="2"/>
-      <c r="N202" s="2"/>
-      <c r="O202" s="2"/>
-      <c r="P202" s="2"/>
-      <c r="Q202" s="2"/>
-      <c r="R202" s="2"/>
-      <c r="S202" s="2"/>
-      <c r="T202" s="5"/>
+      <c r="C202" s="8"/>
+      <c r="D202" s="8"/>
+      <c r="E202" s="8"/>
+      <c r="F202" s="8"/>
+      <c r="G202" s="8"/>
+      <c r="H202" s="8"/>
+      <c r="I202" s="8"/>
+      <c r="J202" s="8"/>
+      <c r="K202" s="8"/>
+      <c r="L202" s="8"/>
+      <c r="M202" s="8"/>
+      <c r="N202" s="8"/>
+      <c r="O202" s="8"/>
+      <c r="P202" s="8"/>
+      <c r="Q202" s="8"/>
+      <c r="R202" s="8"/>
+      <c r="S202" s="8"/>
+      <c r="T202" s="14"/>
       <c r="U202">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="29"/>
+      <c r="A203" s="35"/>
       <c r="B203" s="2">
-        <v>4642</v>
+        <v>4488</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
@@ -6556,9 +6556,9 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
+      <c r="A204" s="35"/>
       <c r="B204" s="2">
-        <v>5537</v>
+        <v>4954</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
@@ -6584,9 +6584,9 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="29"/>
+      <c r="A205" s="35"/>
       <c r="B205" s="2">
-        <v>5847</v>
+        <v>4642</v>
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
@@ -6612,9 +6612,9 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="29"/>
+      <c r="A206" s="35"/>
       <c r="B206" s="2">
-        <v>4769</v>
+        <v>5537</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -6640,9 +6640,9 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="29"/>
+      <c r="A207" s="35"/>
       <c r="B207" s="2">
-        <v>9930</v>
+        <v>5847</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6663,14 +6663,14 @@
       <c r="S207" s="2"/>
       <c r="T207" s="5"/>
       <c r="U207">
-        <f t="shared" ref="U207:U286" ca="1" si="6">IF(B207=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="29"/>
+      <c r="A208" s="35"/>
       <c r="B208" s="2">
-        <v>6861</v>
+        <v>4769</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6691,14 +6691,14 @@
       <c r="S208" s="2"/>
       <c r="T208" s="5"/>
       <c r="U208">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="29"/>
+      <c r="A209" s="35"/>
       <c r="B209" s="2">
-        <v>3226</v>
+        <v>9930</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6719,14 +6719,14 @@
       <c r="S209" s="2"/>
       <c r="T209" s="5"/>
       <c r="U209">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="U209:U288" ca="1" si="6">IF(B209=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="29"/>
+      <c r="A210" s="35"/>
       <c r="B210" s="2">
-        <v>4372</v>
+        <v>6861</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -6752,9 +6752,9 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="29"/>
+      <c r="A211" s="35"/>
       <c r="B211" s="2">
-        <v>4463</v>
+        <v>3226</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -6780,9 +6780,9 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="29"/>
+      <c r="A212" s="35"/>
       <c r="B212" s="2">
-        <v>1668</v>
+        <v>4372</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -6808,9 +6808,9 @@
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="29"/>
+      <c r="A213" s="35"/>
       <c r="B213" s="2">
-        <v>9417</v>
+        <v>4463</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -6836,9 +6836,9 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="29"/>
+      <c r="A214" s="35"/>
       <c r="B214" s="2">
-        <v>3148</v>
+        <v>1668</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -6864,9 +6864,9 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="29"/>
+      <c r="A215" s="35"/>
       <c r="B215" s="2">
-        <v>2137</v>
+        <v>9417</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -6891,115 +6891,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="30"/>
-      <c r="B216" s="6">
-        <v>5621</v>
-      </c>
-      <c r="C216" s="6"/>
-      <c r="D216" s="6"/>
-      <c r="E216" s="6"/>
-      <c r="F216" s="6"/>
-      <c r="G216" s="6"/>
-      <c r="H216" s="6"/>
-      <c r="I216" s="6"/>
-      <c r="J216" s="6"/>
-      <c r="K216" s="6"/>
-      <c r="L216" s="6"/>
-      <c r="M216" s="6"/>
-      <c r="N216" s="6"/>
-      <c r="O216" s="6"/>
-      <c r="P216" s="6"/>
-      <c r="Q216" s="6"/>
-      <c r="R216" s="6"/>
-      <c r="S216" s="6"/>
-      <c r="T216" s="7"/>
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A216" s="35"/>
+      <c r="B216" s="2">
+        <v>3148</v>
+      </c>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+      <c r="E216" s="2"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="2"/>
+      <c r="O216" s="2"/>
+      <c r="P216" s="2"/>
+      <c r="Q216" s="2"/>
+      <c r="R216" s="2"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="5"/>
       <c r="U216">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A217" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B217" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C217" s="8"/>
-      <c r="D217" s="8"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="8"/>
-      <c r="H217" s="8"/>
-      <c r="I217" s="8"/>
-      <c r="J217" s="8"/>
-      <c r="K217" s="8"/>
-      <c r="L217" s="8"/>
-      <c r="M217" s="8"/>
-      <c r="N217" s="8"/>
-      <c r="O217" s="8"/>
-      <c r="P217" s="8"/>
-      <c r="Q217" s="8"/>
-      <c r="R217" s="8"/>
-      <c r="S217" s="8"/>
-      <c r="T217" s="14"/>
+      <c r="A217" s="35"/>
+      <c r="B217" s="2">
+        <v>2137</v>
+      </c>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
+      <c r="P217" s="2"/>
+      <c r="Q217" s="2"/>
+      <c r="R217" s="2"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="5"/>
       <c r="U217">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A218" s="23"/>
-      <c r="B218" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C218" s="2"/>
-      <c r="D218" s="2"/>
-      <c r="E218" s="2"/>
-      <c r="F218" s="2"/>
-      <c r="G218" s="2"/>
-      <c r="H218" s="2"/>
-      <c r="I218" s="2"/>
-      <c r="J218" s="2"/>
-      <c r="K218" s="2"/>
-      <c r="L218" s="2"/>
-      <c r="M218" s="2"/>
-      <c r="N218" s="2"/>
-      <c r="O218" s="2"/>
-      <c r="P218" s="2"/>
-      <c r="Q218" s="2"/>
-      <c r="R218" s="2"/>
-      <c r="S218" s="2"/>
-      <c r="T218" s="5"/>
+    <row r="218" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="36"/>
+      <c r="B218" s="6">
+        <v>5621</v>
+      </c>
+      <c r="C218" s="6"/>
+      <c r="D218" s="6"/>
+      <c r="E218" s="6"/>
+      <c r="F218" s="6"/>
+      <c r="G218" s="6"/>
+      <c r="H218" s="6"/>
+      <c r="I218" s="6"/>
+      <c r="J218" s="6"/>
+      <c r="K218" s="6"/>
+      <c r="L218" s="6"/>
+      <c r="M218" s="6"/>
+      <c r="N218" s="6"/>
+      <c r="O218" s="6"/>
+      <c r="P218" s="6"/>
+      <c r="Q218" s="6"/>
+      <c r="R218" s="6"/>
+      <c r="S218" s="6"/>
+      <c r="T218" s="7"/>
       <c r="U218">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A219" s="23"/>
-      <c r="B219" s="2">
-        <v>7343</v>
-      </c>
-      <c r="C219" s="2"/>
-      <c r="D219" s="2"/>
-      <c r="E219" s="2"/>
-      <c r="F219" s="2"/>
-      <c r="G219" s="2"/>
-      <c r="H219" s="2"/>
-      <c r="I219" s="2"/>
-      <c r="J219" s="2"/>
-      <c r="K219" s="2"/>
-      <c r="L219" s="2"/>
-      <c r="M219" s="2"/>
-      <c r="N219" s="2"/>
-      <c r="O219" s="2"/>
-      <c r="P219" s="2"/>
-      <c r="Q219" s="2"/>
-      <c r="R219" s="2"/>
-      <c r="S219" s="2"/>
-      <c r="T219" s="5"/>
+      <c r="A219" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C219" s="8"/>
+      <c r="D219" s="8"/>
+      <c r="E219" s="8"/>
+      <c r="F219" s="8"/>
+      <c r="G219" s="8"/>
+      <c r="H219" s="8"/>
+      <c r="I219" s="8"/>
+      <c r="J219" s="8"/>
+      <c r="K219" s="8"/>
+      <c r="L219" s="8"/>
+      <c r="M219" s="8"/>
+      <c r="N219" s="8"/>
+      <c r="O219" s="8"/>
+      <c r="P219" s="8"/>
+      <c r="Q219" s="8"/>
+      <c r="R219" s="8"/>
+      <c r="S219" s="8"/>
+      <c r="T219" s="14"/>
       <c r="U219">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7008,7 +7008,7 @@
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="23"/>
       <c r="B220" s="2">
-        <v>7060</v>
+        <v>3951</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -7036,7 +7036,7 @@
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="23"/>
       <c r="B221" s="2">
-        <v>6409</v>
+        <v>7343</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
@@ -7064,7 +7064,7 @@
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="23"/>
       <c r="B222" s="2">
-        <v>2386</v>
+        <v>7060</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -7089,10 +7089,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="23"/>
-      <c r="B223" s="6">
-        <v>7372</v>
+      <c r="B223" s="2">
+        <v>6409</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
@@ -7112,11 +7112,15 @@
       <c r="R223" s="2"/>
       <c r="S223" s="2"/>
       <c r="T223" s="5"/>
+      <c r="U223">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="23"/>
       <c r="B224" s="2">
-        <v>9159</v>
+        <v>2386</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7141,10 +7145,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="23"/>
-      <c r="B225" s="2">
-        <v>5309</v>
+      <c r="B225" s="6">
+        <v>7372</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -7164,15 +7168,11 @@
       <c r="R225" s="2"/>
       <c r="S225" s="2"/>
       <c r="T225" s="5"/>
-      <c r="U225">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="23"/>
       <c r="B226" s="2">
-        <v>3290</v>
+        <v>9159</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
@@ -7200,7 +7200,7 @@
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="23"/>
       <c r="B227" s="2">
-        <v>5345</v>
+        <v>5309</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
@@ -7225,124 +7225,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="24"/>
-      <c r="B228" s="6">
-        <v>6812</v>
-      </c>
-      <c r="C228" s="6"/>
-      <c r="D228" s="6"/>
-      <c r="E228" s="6"/>
-      <c r="F228" s="6"/>
-      <c r="G228" s="6"/>
-      <c r="H228" s="6"/>
-      <c r="I228" s="6"/>
-      <c r="J228" s="6"/>
-      <c r="K228" s="6"/>
-      <c r="L228" s="6"/>
-      <c r="M228" s="6"/>
-      <c r="N228" s="6"/>
-      <c r="O228" s="6"/>
-      <c r="P228" s="6"/>
-      <c r="Q228" s="6"/>
-      <c r="R228" s="6"/>
-      <c r="S228" s="6"/>
-      <c r="T228" s="7"/>
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A228" s="23"/>
+      <c r="B228" s="2">
+        <v>3290</v>
+      </c>
+      <c r="C228" s="2"/>
+      <c r="D228" s="2"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="2"/>
+      <c r="H228" s="2"/>
+      <c r="I228" s="2"/>
+      <c r="J228" s="2"/>
+      <c r="K228" s="2"/>
+      <c r="L228" s="2"/>
+      <c r="M228" s="2"/>
+      <c r="N228" s="2"/>
+      <c r="O228" s="2"/>
+      <c r="P228" s="2"/>
+      <c r="Q228" s="2"/>
+      <c r="R228" s="2"/>
+      <c r="S228" s="2"/>
+      <c r="T228" s="5"/>
       <c r="U228">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B229" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C229" s="8"/>
-      <c r="D229" s="8"/>
-      <c r="E229" s="8"/>
-      <c r="F229" s="8"/>
-      <c r="G229" s="8"/>
-      <c r="H229" s="8"/>
-      <c r="I229" s="8"/>
-      <c r="J229" s="8"/>
-      <c r="K229" s="8"/>
-      <c r="L229" s="8"/>
-      <c r="M229" s="8"/>
-      <c r="N229" s="8"/>
-      <c r="O229" s="8"/>
-      <c r="P229" s="8"/>
-      <c r="Q229" s="8"/>
-      <c r="R229" s="8"/>
-      <c r="S229" s="8"/>
-      <c r="T229" s="14"/>
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A229" s="23"/>
+      <c r="B229" s="2">
+        <v>5345</v>
+      </c>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+      <c r="M229" s="2"/>
+      <c r="N229" s="2"/>
+      <c r="O229" s="2"/>
+      <c r="P229" s="2"/>
+      <c r="Q229" s="2"/>
+      <c r="R229" s="2"/>
+      <c r="S229" s="2"/>
+      <c r="T229" s="5"/>
       <c r="U229">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A230" s="23"/>
-      <c r="B230" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C230" s="2"/>
-      <c r="D230" s="2"/>
-      <c r="E230" s="2"/>
-      <c r="F230" s="2"/>
-      <c r="G230" s="2"/>
-      <c r="H230" s="2"/>
-      <c r="I230" s="2"/>
-      <c r="J230" s="2"/>
-      <c r="K230" s="2"/>
-      <c r="L230" s="2"/>
-      <c r="M230" s="2"/>
-      <c r="N230" s="2"/>
-      <c r="O230" s="2"/>
-      <c r="P230" s="2"/>
-      <c r="Q230" s="2"/>
-      <c r="R230" s="2"/>
-      <c r="S230" s="2"/>
-      <c r="T230" s="5"/>
+    <row r="230" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="24"/>
+      <c r="B230" s="6">
+        <v>6812</v>
+      </c>
+      <c r="C230" s="6"/>
+      <c r="D230" s="6"/>
+      <c r="E230" s="6"/>
+      <c r="F230" s="6"/>
+      <c r="G230" s="6"/>
+      <c r="H230" s="6"/>
+      <c r="I230" s="6"/>
+      <c r="J230" s="6"/>
+      <c r="K230" s="6"/>
+      <c r="L230" s="6"/>
+      <c r="M230" s="6"/>
+      <c r="N230" s="6"/>
+      <c r="O230" s="6"/>
+      <c r="P230" s="6"/>
+      <c r="Q230" s="6"/>
+      <c r="R230" s="6"/>
+      <c r="S230" s="6"/>
+      <c r="T230" s="7"/>
       <c r="U230">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A231" s="23"/>
-      <c r="B231" s="12">
-        <v>9062</v>
-      </c>
-      <c r="C231" s="2"/>
-      <c r="D231" s="2"/>
-      <c r="E231" s="2"/>
-      <c r="F231" s="2"/>
-      <c r="G231" s="2"/>
-      <c r="H231" s="2"/>
-      <c r="I231" s="2"/>
-      <c r="J231" s="2"/>
-      <c r="K231" s="2"/>
-      <c r="L231" s="2"/>
-      <c r="M231" s="2"/>
-      <c r="N231" s="2"/>
-      <c r="O231" s="2"/>
-      <c r="P231" s="2"/>
-      <c r="Q231" s="2"/>
-      <c r="R231" s="2"/>
-      <c r="S231" s="2"/>
-      <c r="T231" s="5"/>
+      <c r="A231" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B231" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C231" s="8"/>
+      <c r="D231" s="8"/>
+      <c r="E231" s="8"/>
+      <c r="F231" s="8"/>
+      <c r="G231" s="8"/>
+      <c r="H231" s="8"/>
+      <c r="I231" s="8"/>
+      <c r="J231" s="8"/>
+      <c r="K231" s="8"/>
+      <c r="L231" s="8"/>
+      <c r="M231" s="8"/>
+      <c r="N231" s="8"/>
+      <c r="O231" s="8"/>
+      <c r="P231" s="8"/>
+      <c r="Q231" s="8"/>
+      <c r="R231" s="8"/>
+      <c r="S231" s="8"/>
+      <c r="T231" s="14"/>
       <c r="U231">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="23"/>
-      <c r="B232" s="19">
-        <v>8861</v>
+      <c r="B232" s="12">
+        <v>1516</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -7367,10 +7367,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="23"/>
-      <c r="B233" s="2">
-        <v>5164</v>
+      <c r="B233" s="12">
+        <v>9062</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
@@ -7397,8 +7397,8 @@
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="23"/>
-      <c r="B234" s="2">
-        <v>2354</v>
+      <c r="B234" s="19">
+        <v>8861</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
@@ -7426,7 +7426,7 @@
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="23"/>
       <c r="B235" s="2">
-        <v>2030</v>
+        <v>5164</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -7451,115 +7451,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="24"/>
-      <c r="B236" s="6">
-        <v>7649</v>
-      </c>
-      <c r="C236" s="6"/>
-      <c r="D236" s="6"/>
-      <c r="E236" s="6"/>
-      <c r="F236" s="6"/>
-      <c r="G236" s="6"/>
-      <c r="H236" s="6"/>
-      <c r="I236" s="6"/>
-      <c r="J236" s="6"/>
-      <c r="K236" s="6"/>
-      <c r="L236" s="6"/>
-      <c r="M236" s="6"/>
-      <c r="N236" s="6"/>
-      <c r="O236" s="6"/>
-      <c r="P236" s="6"/>
-      <c r="Q236" s="6"/>
-      <c r="R236" s="6"/>
-      <c r="S236" s="6"/>
-      <c r="T236" s="7"/>
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A236" s="23"/>
+      <c r="B236" s="2">
+        <v>2354</v>
+      </c>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="2"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="2"/>
+      <c r="I236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="K236" s="2"/>
+      <c r="L236" s="2"/>
+      <c r="M236" s="2"/>
+      <c r="N236" s="2"/>
+      <c r="O236" s="2"/>
+      <c r="P236" s="2"/>
+      <c r="Q236" s="2"/>
+      <c r="R236" s="2"/>
+      <c r="S236" s="2"/>
+      <c r="T236" s="5"/>
       <c r="U236">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A237" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C237" s="8"/>
-      <c r="D237" s="8"/>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="8"/>
-      <c r="H237" s="8"/>
-      <c r="I237" s="8"/>
-      <c r="J237" s="8"/>
-      <c r="K237" s="8"/>
-      <c r="L237" s="8"/>
-      <c r="M237" s="8"/>
-      <c r="N237" s="8"/>
-      <c r="O237" s="8"/>
-      <c r="P237" s="8"/>
-      <c r="Q237" s="8"/>
-      <c r="R237" s="8"/>
-      <c r="S237" s="8"/>
-      <c r="T237" s="14"/>
+      <c r="A237" s="23"/>
+      <c r="B237" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+      <c r="L237" s="2"/>
+      <c r="M237" s="2"/>
+      <c r="N237" s="2"/>
+      <c r="O237" s="2"/>
+      <c r="P237" s="2"/>
+      <c r="Q237" s="2"/>
+      <c r="R237" s="2"/>
+      <c r="S237" s="2"/>
+      <c r="T237" s="5"/>
       <c r="U237">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="23"/>
-      <c r="B238" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C238" s="2"/>
-      <c r="D238" s="2"/>
-      <c r="E238" s="2"/>
-      <c r="F238" s="2"/>
-      <c r="G238" s="2"/>
-      <c r="H238" s="2"/>
-      <c r="I238" s="2"/>
-      <c r="J238" s="2"/>
-      <c r="K238" s="2"/>
-      <c r="L238" s="2"/>
-      <c r="M238" s="2"/>
-      <c r="N238" s="2"/>
-      <c r="O238" s="2"/>
-      <c r="P238" s="2"/>
-      <c r="Q238" s="2"/>
-      <c r="R238" s="2"/>
-      <c r="S238" s="2"/>
-      <c r="T238" s="5"/>
+    <row r="238" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="24"/>
+      <c r="B238" s="6">
+        <v>7649</v>
+      </c>
+      <c r="C238" s="6"/>
+      <c r="D238" s="6"/>
+      <c r="E238" s="6"/>
+      <c r="F238" s="6"/>
+      <c r="G238" s="6"/>
+      <c r="H238" s="6"/>
+      <c r="I238" s="6"/>
+      <c r="J238" s="6"/>
+      <c r="K238" s="6"/>
+      <c r="L238" s="6"/>
+      <c r="M238" s="6"/>
+      <c r="N238" s="6"/>
+      <c r="O238" s="6"/>
+      <c r="P238" s="6"/>
+      <c r="Q238" s="6"/>
+      <c r="R238" s="6"/>
+      <c r="S238" s="6"/>
+      <c r="T238" s="7"/>
       <c r="U238">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="23"/>
-      <c r="B239" s="2">
-        <v>6732</v>
-      </c>
-      <c r="C239" s="2"/>
-      <c r="D239" s="2"/>
-      <c r="E239" s="2"/>
-      <c r="F239" s="2"/>
-      <c r="G239" s="2"/>
-      <c r="H239" s="2"/>
-      <c r="I239" s="2"/>
-      <c r="J239" s="2"/>
-      <c r="K239" s="2"/>
-      <c r="L239" s="2"/>
-      <c r="M239" s="2"/>
-      <c r="N239" s="2"/>
-      <c r="O239" s="2"/>
-      <c r="P239" s="2"/>
-      <c r="Q239" s="2"/>
-      <c r="R239" s="2"/>
-      <c r="S239" s="2"/>
-      <c r="T239" s="5"/>
+      <c r="A239" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B239" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C239" s="8"/>
+      <c r="D239" s="8"/>
+      <c r="E239" s="8"/>
+      <c r="F239" s="8"/>
+      <c r="G239" s="8"/>
+      <c r="H239" s="8"/>
+      <c r="I239" s="8"/>
+      <c r="J239" s="8"/>
+      <c r="K239" s="8"/>
+      <c r="L239" s="8"/>
+      <c r="M239" s="8"/>
+      <c r="N239" s="8"/>
+      <c r="O239" s="8"/>
+      <c r="P239" s="8"/>
+      <c r="Q239" s="8"/>
+      <c r="R239" s="8"/>
+      <c r="S239" s="8"/>
+      <c r="T239" s="14"/>
       <c r="U239">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7568,7 +7568,7 @@
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="23"/>
       <c r="B240" s="2">
-        <v>6882</v>
+        <v>3784</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
@@ -7596,7 +7596,7 @@
     <row r="241" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A241" s="23"/>
       <c r="B241" s="2">
-        <v>1212</v>
+        <v>6732</v>
       </c>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
@@ -7624,7 +7624,7 @@
     <row r="242" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A242" s="23"/>
       <c r="B242" s="2">
-        <v>9472</v>
+        <v>6882</v>
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
@@ -7652,7 +7652,7 @@
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A243" s="23"/>
       <c r="B243" s="2">
-        <v>5081</v>
+        <v>1212</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
@@ -7677,115 +7677,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="24"/>
-      <c r="B244" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C244" s="6"/>
-      <c r="D244" s="6"/>
-      <c r="E244" s="6"/>
-      <c r="F244" s="6"/>
-      <c r="G244" s="6"/>
-      <c r="H244" s="6"/>
-      <c r="I244" s="6"/>
-      <c r="J244" s="6"/>
-      <c r="K244" s="6"/>
-      <c r="L244" s="6"/>
-      <c r="M244" s="6"/>
-      <c r="N244" s="6"/>
-      <c r="O244" s="6"/>
-      <c r="P244" s="6"/>
-      <c r="Q244" s="6"/>
-      <c r="R244" s="6"/>
-      <c r="S244" s="6"/>
-      <c r="T244" s="7"/>
+    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A244" s="23"/>
+      <c r="B244" s="2">
+        <v>9472</v>
+      </c>
+      <c r="C244" s="2"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="2"/>
+      <c r="F244" s="2"/>
+      <c r="G244" s="2"/>
+      <c r="H244" s="2"/>
+      <c r="I244" s="2"/>
+      <c r="J244" s="2"/>
+      <c r="K244" s="2"/>
+      <c r="L244" s="2"/>
+      <c r="M244" s="2"/>
+      <c r="N244" s="2"/>
+      <c r="O244" s="2"/>
+      <c r="P244" s="2"/>
+      <c r="Q244" s="2"/>
+      <c r="R244" s="2"/>
+      <c r="S244" s="2"/>
+      <c r="T244" s="5"/>
       <c r="U244">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B245" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C245" s="8"/>
-      <c r="D245" s="8"/>
-      <c r="E245" s="8"/>
-      <c r="F245" s="8"/>
-      <c r="G245" s="8"/>
-      <c r="H245" s="8"/>
-      <c r="I245" s="8"/>
-      <c r="J245" s="8"/>
-      <c r="K245" s="8"/>
-      <c r="L245" s="8"/>
-      <c r="M245" s="8"/>
-      <c r="N245" s="8"/>
-      <c r="O245" s="8"/>
-      <c r="P245" s="8"/>
-      <c r="Q245" s="8"/>
-      <c r="R245" s="8"/>
-      <c r="S245" s="8"/>
-      <c r="T245" s="14"/>
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A245" s="23"/>
+      <c r="B245" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C245" s="2"/>
+      <c r="D245" s="2"/>
+      <c r="E245" s="2"/>
+      <c r="F245" s="2"/>
+      <c r="G245" s="2"/>
+      <c r="H245" s="2"/>
+      <c r="I245" s="2"/>
+      <c r="J245" s="2"/>
+      <c r="K245" s="2"/>
+      <c r="L245" s="2"/>
+      <c r="M245" s="2"/>
+      <c r="N245" s="2"/>
+      <c r="O245" s="2"/>
+      <c r="P245" s="2"/>
+      <c r="Q245" s="2"/>
+      <c r="R245" s="2"/>
+      <c r="S245" s="2"/>
+      <c r="T245" s="5"/>
       <c r="U245">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="23"/>
-      <c r="B246" s="2">
-        <v>6011</v>
-      </c>
-      <c r="C246" s="2"/>
-      <c r="D246" s="2"/>
-      <c r="E246" s="2"/>
-      <c r="F246" s="2"/>
-      <c r="G246" s="2"/>
-      <c r="H246" s="2"/>
-      <c r="I246" s="2"/>
-      <c r="J246" s="2"/>
-      <c r="K246" s="2"/>
-      <c r="L246" s="2"/>
-      <c r="M246" s="2"/>
-      <c r="N246" s="2"/>
-      <c r="O246" s="2"/>
-      <c r="P246" s="2"/>
-      <c r="Q246" s="2"/>
-      <c r="R246" s="2"/>
-      <c r="S246" s="2"/>
-      <c r="T246" s="5"/>
+    <row r="246" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="24"/>
+      <c r="B246" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C246" s="6"/>
+      <c r="D246" s="6"/>
+      <c r="E246" s="6"/>
+      <c r="F246" s="6"/>
+      <c r="G246" s="6"/>
+      <c r="H246" s="6"/>
+      <c r="I246" s="6"/>
+      <c r="J246" s="6"/>
+      <c r="K246" s="6"/>
+      <c r="L246" s="6"/>
+      <c r="M246" s="6"/>
+      <c r="N246" s="6"/>
+      <c r="O246" s="6"/>
+      <c r="P246" s="6"/>
+      <c r="Q246" s="6"/>
+      <c r="R246" s="6"/>
+      <c r="S246" s="6"/>
+      <c r="T246" s="7"/>
       <c r="U246">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="23"/>
-      <c r="B247" s="2">
-        <v>8403</v>
-      </c>
-      <c r="C247" s="2"/>
-      <c r="D247" s="2"/>
-      <c r="E247" s="2"/>
-      <c r="F247" s="2"/>
-      <c r="G247" s="2"/>
-      <c r="H247" s="2"/>
-      <c r="I247" s="2"/>
-      <c r="J247" s="2"/>
-      <c r="K247" s="2"/>
-      <c r="L247" s="2"/>
-      <c r="M247" s="2"/>
-      <c r="N247" s="2"/>
-      <c r="O247" s="2"/>
-      <c r="P247" s="2"/>
-      <c r="Q247" s="2"/>
-      <c r="R247" s="2"/>
-      <c r="S247" s="2"/>
-      <c r="T247" s="5"/>
+    <row r="247" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A247" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B247" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C247" s="8"/>
+      <c r="D247" s="8"/>
+      <c r="E247" s="8"/>
+      <c r="F247" s="8"/>
+      <c r="G247" s="8"/>
+      <c r="H247" s="8"/>
+      <c r="I247" s="8"/>
+      <c r="J247" s="8"/>
+      <c r="K247" s="8"/>
+      <c r="L247" s="8"/>
+      <c r="M247" s="8"/>
+      <c r="N247" s="8"/>
+      <c r="O247" s="8"/>
+      <c r="P247" s="8"/>
+      <c r="Q247" s="8"/>
+      <c r="R247" s="8"/>
+      <c r="S247" s="8"/>
+      <c r="T247" s="14"/>
       <c r="U247">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7794,7 +7794,7 @@
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="23"/>
       <c r="B248" s="2">
-        <v>3185</v>
+        <v>6011</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7821,8 +7821,8 @@
     </row>
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" s="23"/>
-      <c r="B249" s="21">
-        <v>6037</v>
+      <c r="B249" s="2">
+        <v>8403</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -7850,7 +7850,7 @@
     <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" s="23"/>
       <c r="B250" s="2">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -7877,8 +7877,8 @@
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" s="23"/>
-      <c r="B251" s="2">
-        <v>4916</v>
+      <c r="B251" s="21">
+        <v>6037</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7906,7 +7906,7 @@
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" s="23"/>
       <c r="B252" s="2">
-        <v>2809</v>
+        <v>9914</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7934,7 +7934,7 @@
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="23"/>
       <c r="B253" s="2">
-        <v>8265</v>
+        <v>4916</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7962,7 +7962,7 @@
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="23"/>
       <c r="B254" s="2">
-        <v>2092</v>
+        <v>2809</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7990,7 +7990,7 @@
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="23"/>
       <c r="B255" s="2">
-        <v>7297</v>
+        <v>8265</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8018,7 +8018,7 @@
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="23"/>
       <c r="B256" s="2">
-        <v>5242</v>
+        <v>2092</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8046,7 +8046,7 @@
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="23"/>
       <c r="B257" s="2">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8074,7 +8074,7 @@
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="23"/>
       <c r="B258" s="2">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8102,7 +8102,7 @@
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="23"/>
       <c r="B259" s="2">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8130,7 +8130,7 @@
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" s="23"/>
       <c r="B260" s="2">
-        <v>9713</v>
+        <v>2401</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8158,7 +8158,7 @@
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="23"/>
       <c r="B261" s="2">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8186,7 +8186,7 @@
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="23"/>
       <c r="B262" s="2">
-        <v>2000</v>
+        <v>9713</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8214,7 +8214,7 @@
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="23"/>
       <c r="B263" s="2">
-        <v>5449</v>
+        <v>7301</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8242,7 +8242,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>9238</v>
+        <v>2000</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8270,7 +8270,7 @@
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8298,7 +8298,7 @@
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>4147</v>
+        <v>9238</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8326,7 +8326,7 @@
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>1953</v>
+        <v>2662</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8354,7 +8354,7 @@
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8382,7 +8382,7 @@
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>5032</v>
+        <v>1953</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8410,7 +8410,7 @@
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>3567</v>
+        <v>3956</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8438,7 +8438,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="23"/>
       <c r="B271" s="2">
-        <v>5108</v>
+        <v>5032</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8466,7 +8466,7 @@
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="23"/>
       <c r="B272" s="2">
-        <v>2033</v>
+        <v>3567</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8494,7 +8494,7 @@
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" s="23"/>
       <c r="B273" s="2">
-        <v>6981</v>
+        <v>5108</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8519,115 +8519,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="24"/>
-      <c r="B274" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C274" s="6"/>
-      <c r="D274" s="6"/>
-      <c r="E274" s="6"/>
-      <c r="F274" s="6"/>
-      <c r="G274" s="6"/>
-      <c r="H274" s="6"/>
-      <c r="I274" s="6"/>
-      <c r="J274" s="6"/>
-      <c r="K274" s="6"/>
-      <c r="L274" s="6"/>
-      <c r="M274" s="6"/>
-      <c r="N274" s="6"/>
-      <c r="O274" s="6"/>
-      <c r="P274" s="6"/>
-      <c r="Q274" s="6"/>
-      <c r="R274" s="6"/>
-      <c r="S274" s="6"/>
-      <c r="T274" s="7"/>
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A274" s="23"/>
+      <c r="B274" s="2">
+        <v>2033</v>
+      </c>
+      <c r="C274" s="2"/>
+      <c r="D274" s="2"/>
+      <c r="E274" s="2"/>
+      <c r="F274" s="2"/>
+      <c r="G274" s="2"/>
+      <c r="H274" s="2"/>
+      <c r="I274" s="2"/>
+      <c r="J274" s="2"/>
+      <c r="K274" s="2"/>
+      <c r="L274" s="2"/>
+      <c r="M274" s="2"/>
+      <c r="N274" s="2"/>
+      <c r="O274" s="2"/>
+      <c r="P274" s="2"/>
+      <c r="Q274" s="2"/>
+      <c r="R274" s="2"/>
+      <c r="S274" s="2"/>
+      <c r="T274" s="5"/>
       <c r="U274">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C275" s="8"/>
-      <c r="D275" s="8"/>
-      <c r="E275" s="8"/>
-      <c r="F275" s="8"/>
-      <c r="G275" s="8"/>
-      <c r="H275" s="8"/>
-      <c r="I275" s="8"/>
-      <c r="J275" s="8"/>
-      <c r="K275" s="8"/>
-      <c r="L275" s="8"/>
-      <c r="M275" s="8"/>
-      <c r="N275" s="8"/>
-      <c r="O275" s="8"/>
-      <c r="P275" s="8"/>
-      <c r="Q275" s="8"/>
-      <c r="R275" s="8"/>
-      <c r="S275" s="8"/>
-      <c r="T275" s="14"/>
+        <v>6981</v>
+      </c>
+      <c r="C275" s="2"/>
+      <c r="D275" s="2"/>
+      <c r="E275" s="2"/>
+      <c r="F275" s="2"/>
+      <c r="G275" s="2"/>
+      <c r="H275" s="2"/>
+      <c r="I275" s="2"/>
+      <c r="J275" s="2"/>
+      <c r="K275" s="2"/>
+      <c r="L275" s="2"/>
+      <c r="M275" s="2"/>
+      <c r="N275" s="2"/>
+      <c r="O275" s="2"/>
+      <c r="P275" s="2"/>
+      <c r="Q275" s="2"/>
+      <c r="R275" s="2"/>
+      <c r="S275" s="2"/>
+      <c r="T275" s="5"/>
       <c r="U275">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="23"/>
-      <c r="B276" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C276" s="2"/>
-      <c r="D276" s="2"/>
-      <c r="E276" s="2"/>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="2"/>
-      <c r="J276" s="2"/>
-      <c r="K276" s="2"/>
-      <c r="L276" s="2"/>
-      <c r="M276" s="2"/>
-      <c r="N276" s="2"/>
-      <c r="O276" s="2"/>
-      <c r="P276" s="2"/>
-      <c r="Q276" s="2"/>
-      <c r="R276" s="2"/>
-      <c r="S276" s="2"/>
-      <c r="T276" s="5"/>
+    <row r="276" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A276" s="24"/>
+      <c r="B276" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C276" s="6"/>
+      <c r="D276" s="6"/>
+      <c r="E276" s="6"/>
+      <c r="F276" s="6"/>
+      <c r="G276" s="6"/>
+      <c r="H276" s="6"/>
+      <c r="I276" s="6"/>
+      <c r="J276" s="6"/>
+      <c r="K276" s="6"/>
+      <c r="L276" s="6"/>
+      <c r="M276" s="6"/>
+      <c r="N276" s="6"/>
+      <c r="O276" s="6"/>
+      <c r="P276" s="6"/>
+      <c r="Q276" s="6"/>
+      <c r="R276" s="6"/>
+      <c r="S276" s="6"/>
+      <c r="T276" s="7"/>
       <c r="U276">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="23"/>
+      <c r="A277" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="B277" s="2">
-        <v>9990</v>
-      </c>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2"/>
-      <c r="E277" s="2"/>
-      <c r="F277" s="2"/>
-      <c r="G277" s="2"/>
-      <c r="H277" s="2"/>
-      <c r="I277" s="2"/>
-      <c r="J277" s="2"/>
-      <c r="K277" s="2"/>
-      <c r="L277" s="2"/>
-      <c r="M277" s="2"/>
-      <c r="N277" s="2"/>
-      <c r="O277" s="2"/>
-      <c r="P277" s="2"/>
-      <c r="Q277" s="2"/>
-      <c r="R277" s="2"/>
-      <c r="S277" s="2"/>
-      <c r="T277" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C277" s="8"/>
+      <c r="D277" s="8"/>
+      <c r="E277" s="8"/>
+      <c r="F277" s="8"/>
+      <c r="G277" s="8"/>
+      <c r="H277" s="8"/>
+      <c r="I277" s="8"/>
+      <c r="J277" s="8"/>
+      <c r="K277" s="8"/>
+      <c r="L277" s="8"/>
+      <c r="M277" s="8"/>
+      <c r="N277" s="8"/>
+      <c r="O277" s="8"/>
+      <c r="P277" s="8"/>
+      <c r="Q277" s="8"/>
+      <c r="R277" s="8"/>
+      <c r="S277" s="8"/>
+      <c r="T277" s="14"/>
       <c r="U277">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8636,7 +8636,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="23"/>
       <c r="B278" s="2">
-        <v>7738</v>
+        <v>1056</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8664,7 +8664,7 @@
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" s="23"/>
       <c r="B279" s="2">
-        <v>8418</v>
+        <v>9990</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8692,7 +8692,7 @@
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" s="23"/>
       <c r="B280" s="2">
-        <v>9512</v>
+        <v>7738</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8720,7 +8720,7 @@
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="23"/>
       <c r="B281" s="2">
-        <v>9924</v>
+        <v>8418</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8746,65 +8746,65 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="27"/>
-      <c r="B282" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C282" s="9"/>
-      <c r="D282" s="9"/>
-      <c r="E282" s="9"/>
-      <c r="F282" s="9"/>
-      <c r="G282" s="9"/>
-      <c r="H282" s="9"/>
-      <c r="I282" s="9"/>
-      <c r="J282" s="9"/>
-      <c r="K282" s="9"/>
-      <c r="L282" s="9"/>
-      <c r="M282" s="9"/>
-      <c r="N282" s="9"/>
-      <c r="O282" s="9"/>
-      <c r="P282" s="9"/>
-      <c r="Q282" s="9"/>
-      <c r="R282" s="9"/>
-      <c r="S282" s="9"/>
-      <c r="T282" s="15"/>
+      <c r="A282" s="23"/>
+      <c r="B282" s="2">
+        <v>9512</v>
+      </c>
+      <c r="C282" s="2"/>
+      <c r="D282" s="2"/>
+      <c r="E282" s="2"/>
+      <c r="F282" s="2"/>
+      <c r="G282" s="2"/>
+      <c r="H282" s="2"/>
+      <c r="I282" s="2"/>
+      <c r="J282" s="2"/>
+      <c r="K282" s="2"/>
+      <c r="L282" s="2"/>
+      <c r="M282" s="2"/>
+      <c r="N282" s="2"/>
+      <c r="O282" s="2"/>
+      <c r="P282" s="2"/>
+      <c r="Q282" s="2"/>
+      <c r="R282" s="2"/>
+      <c r="S282" s="2"/>
+      <c r="T282" s="5"/>
       <c r="U282">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="27"/>
-      <c r="B283" s="9">
-        <v>2973</v>
-      </c>
-      <c r="C283" s="9"/>
-      <c r="D283" s="9"/>
-      <c r="E283" s="9"/>
-      <c r="F283" s="9"/>
-      <c r="G283" s="9"/>
-      <c r="H283" s="9"/>
-      <c r="I283" s="9"/>
-      <c r="J283" s="9"/>
-      <c r="K283" s="9"/>
-      <c r="L283" s="9"/>
-      <c r="M283" s="9"/>
-      <c r="N283" s="9"/>
-      <c r="O283" s="9"/>
-      <c r="P283" s="9"/>
-      <c r="Q283" s="9"/>
-      <c r="R283" s="9"/>
-      <c r="S283" s="9"/>
-      <c r="T283" s="15"/>
+      <c r="A283" s="23"/>
+      <c r="B283" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C283" s="2"/>
+      <c r="D283" s="2"/>
+      <c r="E283" s="2"/>
+      <c r="F283" s="2"/>
+      <c r="G283" s="2"/>
+      <c r="H283" s="2"/>
+      <c r="I283" s="2"/>
+      <c r="J283" s="2"/>
+      <c r="K283" s="2"/>
+      <c r="L283" s="2"/>
+      <c r="M283" s="2"/>
+      <c r="N283" s="2"/>
+      <c r="O283" s="2"/>
+      <c r="P283" s="2"/>
+      <c r="Q283" s="2"/>
+      <c r="R283" s="2"/>
+      <c r="S283" s="2"/>
+      <c r="T283" s="5"/>
       <c r="U283">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="27"/>
+      <c r="A284" s="31"/>
       <c r="B284" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C284" s="9"/>
       <c r="D284" s="9"/>
@@ -8830,9 +8830,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="27"/>
+      <c r="A285" s="31"/>
       <c r="B285" s="9">
-        <v>7186</v>
+        <v>2973</v>
       </c>
       <c r="C285" s="9"/>
       <c r="D285" s="9"/>
@@ -8858,9 +8858,9 @@
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="27"/>
+      <c r="A286" s="31"/>
       <c r="B286" s="9">
-        <v>1457</v>
+        <v>8258</v>
       </c>
       <c r="C286" s="9"/>
       <c r="D286" s="9"/>
@@ -8885,115 +8885,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="24"/>
-      <c r="B287" s="6">
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A287" s="31"/>
+      <c r="B287" s="9">
+        <v>7186</v>
+      </c>
+      <c r="C287" s="9"/>
+      <c r="D287" s="9"/>
+      <c r="E287" s="9"/>
+      <c r="F287" s="9"/>
+      <c r="G287" s="9"/>
+      <c r="H287" s="9"/>
+      <c r="I287" s="9"/>
+      <c r="J287" s="9"/>
+      <c r="K287" s="9"/>
+      <c r="L287" s="9"/>
+      <c r="M287" s="9"/>
+      <c r="N287" s="9"/>
+      <c r="O287" s="9"/>
+      <c r="P287" s="9"/>
+      <c r="Q287" s="9"/>
+      <c r="R287" s="9"/>
+      <c r="S287" s="9"/>
+      <c r="T287" s="15"/>
+      <c r="U287">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A288" s="31"/>
+      <c r="B288" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C288" s="9"/>
+      <c r="D288" s="9"/>
+      <c r="E288" s="9"/>
+      <c r="F288" s="9"/>
+      <c r="G288" s="9"/>
+      <c r="H288" s="9"/>
+      <c r="I288" s="9"/>
+      <c r="J288" s="9"/>
+      <c r="K288" s="9"/>
+      <c r="L288" s="9"/>
+      <c r="M288" s="9"/>
+      <c r="N288" s="9"/>
+      <c r="O288" s="9"/>
+      <c r="P288" s="9"/>
+      <c r="Q288" s="9"/>
+      <c r="R288" s="9"/>
+      <c r="S288" s="9"/>
+      <c r="T288" s="15"/>
+      <c r="U288">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="24"/>
+      <c r="B289" s="6">
         <v>6876</v>
       </c>
-      <c r="C287" s="6"/>
-      <c r="D287" s="6"/>
-      <c r="E287" s="6"/>
-      <c r="F287" s="6"/>
-      <c r="G287" s="6"/>
-      <c r="H287" s="6"/>
-      <c r="I287" s="6"/>
-      <c r="J287" s="6"/>
-      <c r="K287" s="6"/>
-      <c r="L287" s="6"/>
-      <c r="M287" s="6"/>
-      <c r="N287" s="6"/>
-      <c r="O287" s="6"/>
-      <c r="P287" s="6"/>
-      <c r="Q287" s="6"/>
-      <c r="R287" s="6"/>
-      <c r="S287" s="6"/>
-      <c r="T287" s="7"/>
-      <c r="U287">
-        <f t="shared" ref="U287:U350" ca="1" si="7">IF(B287=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="22" t="s">
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
+      <c r="E289" s="6"/>
+      <c r="F289" s="6"/>
+      <c r="G289" s="6"/>
+      <c r="H289" s="6"/>
+      <c r="I289" s="6"/>
+      <c r="J289" s="6"/>
+      <c r="K289" s="6"/>
+      <c r="L289" s="6"/>
+      <c r="M289" s="6"/>
+      <c r="N289" s="6"/>
+      <c r="O289" s="6"/>
+      <c r="P289" s="6"/>
+      <c r="Q289" s="6"/>
+      <c r="R289" s="6"/>
+      <c r="S289" s="6"/>
+      <c r="T289" s="7"/>
+      <c r="U289">
+        <f t="shared" ref="U289:U352" ca="1" si="7">IF(B289=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A290" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B288" s="8">
+      <c r="B290" s="8">
         <v>4304</v>
       </c>
-      <c r="C288" s="8"/>
-      <c r="D288" s="8"/>
-      <c r="E288" s="8"/>
-      <c r="F288" s="8"/>
-      <c r="G288" s="8"/>
-      <c r="H288" s="8"/>
-      <c r="I288" s="8"/>
-      <c r="J288" s="8"/>
-      <c r="K288" s="8"/>
-      <c r="L288" s="8"/>
-      <c r="M288" s="8"/>
-      <c r="N288" s="8"/>
-      <c r="O288" s="8"/>
-      <c r="P288" s="8"/>
-      <c r="Q288" s="8"/>
-      <c r="R288" s="8"/>
-      <c r="S288" s="8"/>
-      <c r="T288" s="14"/>
-      <c r="U288">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="23"/>
-      <c r="B289" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="E289" s="2"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
-      <c r="I289" s="2"/>
-      <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-      <c r="N289" s="2"/>
-      <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-      <c r="Q289" s="2"/>
-      <c r="R289" s="2"/>
-      <c r="S289" s="2"/>
-      <c r="T289" s="5"/>
-      <c r="U289">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="23"/>
-      <c r="B290" s="2">
-        <v>7693</v>
-      </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="E290" s="2"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
-      <c r="I290" s="2"/>
-      <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-      <c r="N290" s="2"/>
-      <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-      <c r="Q290" s="2"/>
-      <c r="R290" s="2"/>
-      <c r="S290" s="2"/>
-      <c r="T290" s="5"/>
+      <c r="C290" s="8"/>
+      <c r="D290" s="8"/>
+      <c r="E290" s="8"/>
+      <c r="F290" s="8"/>
+      <c r="G290" s="8"/>
+      <c r="H290" s="8"/>
+      <c r="I290" s="8"/>
+      <c r="J290" s="8"/>
+      <c r="K290" s="8"/>
+      <c r="L290" s="8"/>
+      <c r="M290" s="8"/>
+      <c r="N290" s="8"/>
+      <c r="O290" s="8"/>
+      <c r="P290" s="8"/>
+      <c r="Q290" s="8"/>
+      <c r="R290" s="8"/>
+      <c r="S290" s="8"/>
+      <c r="T290" s="14"/>
       <c r="U290">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9002,7 +9002,7 @@
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="23"/>
       <c r="B291" s="2">
-        <v>8718</v>
+        <v>2070</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9027,124 +9027,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="24"/>
-      <c r="B292" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="6"/>
-      <c r="H292" s="6"/>
-      <c r="I292" s="6"/>
-      <c r="J292" s="6"/>
-      <c r="K292" s="6"/>
-      <c r="L292" s="6"/>
-      <c r="M292" s="6"/>
-      <c r="N292" s="6"/>
-      <c r="O292" s="6"/>
-      <c r="P292" s="6"/>
-      <c r="Q292" s="6"/>
-      <c r="R292" s="6"/>
-      <c r="S292" s="6"/>
-      <c r="T292" s="7"/>
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A292" s="23"/>
+      <c r="B292" s="2">
+        <v>7693</v>
+      </c>
+      <c r="C292" s="2"/>
+      <c r="D292" s="2"/>
+      <c r="E292" s="2"/>
+      <c r="F292" s="2"/>
+      <c r="G292" s="2"/>
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+      <c r="J292" s="2"/>
+      <c r="K292" s="2"/>
+      <c r="L292" s="2"/>
+      <c r="M292" s="2"/>
+      <c r="N292" s="2"/>
+      <c r="O292" s="2"/>
+      <c r="P292" s="2"/>
+      <c r="Q292" s="2"/>
+      <c r="R292" s="2"/>
+      <c r="S292" s="2"/>
+      <c r="T292" s="5"/>
       <c r="U292">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A293" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B293" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="14"/>
+    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A293" s="23"/>
+      <c r="B293" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C293" s="2"/>
+      <c r="D293" s="2"/>
+      <c r="E293" s="2"/>
+      <c r="F293" s="2"/>
+      <c r="G293" s="2"/>
+      <c r="H293" s="2"/>
+      <c r="I293" s="2"/>
+      <c r="J293" s="2"/>
+      <c r="K293" s="2"/>
+      <c r="L293" s="2"/>
+      <c r="M293" s="2"/>
+      <c r="N293" s="2"/>
+      <c r="O293" s="2"/>
+      <c r="P293" s="2"/>
+      <c r="Q293" s="2"/>
+      <c r="R293" s="2"/>
+      <c r="S293" s="2"/>
+      <c r="T293" s="5"/>
       <c r="U293">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A294" s="23"/>
-      <c r="B294" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
-      <c r="E294" s="2"/>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
-      <c r="H294" s="2"/>
-      <c r="I294" s="2"/>
-      <c r="J294" s="2"/>
-      <c r="K294" s="2"/>
-      <c r="L294" s="2"/>
-      <c r="M294" s="2"/>
-      <c r="N294" s="2"/>
-      <c r="O294" s="2"/>
-      <c r="P294" s="2"/>
-      <c r="Q294" s="2"/>
-      <c r="R294" s="2"/>
-      <c r="S294" s="2"/>
-      <c r="T294" s="5"/>
+    <row r="294" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="24"/>
+      <c r="B294" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C294" s="6"/>
+      <c r="D294" s="6"/>
+      <c r="E294" s="6"/>
+      <c r="F294" s="6"/>
+      <c r="G294" s="6"/>
+      <c r="H294" s="6"/>
+      <c r="I294" s="6"/>
+      <c r="J294" s="6"/>
+      <c r="K294" s="6"/>
+      <c r="L294" s="6"/>
+      <c r="M294" s="6"/>
+      <c r="N294" s="6"/>
+      <c r="O294" s="6"/>
+      <c r="P294" s="6"/>
+      <c r="Q294" s="6"/>
+      <c r="R294" s="6"/>
+      <c r="S294" s="6"/>
+      <c r="T294" s="7"/>
       <c r="U294">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A295" s="23"/>
-      <c r="B295" s="12">
-        <v>7546</v>
-      </c>
-      <c r="C295" s="2"/>
-      <c r="D295" s="2"/>
-      <c r="E295" s="2"/>
-      <c r="F295" s="2"/>
-      <c r="G295" s="2"/>
-      <c r="H295" s="2"/>
-      <c r="I295" s="2"/>
-      <c r="J295" s="2"/>
-      <c r="K295" s="2"/>
-      <c r="L295" s="2"/>
-      <c r="M295" s="2"/>
-      <c r="N295" s="2"/>
-      <c r="O295" s="2"/>
-      <c r="P295" s="2"/>
-      <c r="Q295" s="2"/>
-      <c r="R295" s="2"/>
-      <c r="S295" s="2"/>
-      <c r="T295" s="5"/>
+      <c r="A295" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B295" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C295" s="8"/>
+      <c r="D295" s="8"/>
+      <c r="E295" s="8"/>
+      <c r="F295" s="8"/>
+      <c r="G295" s="8"/>
+      <c r="H295" s="8"/>
+      <c r="I295" s="8"/>
+      <c r="J295" s="8"/>
+      <c r="K295" s="8"/>
+      <c r="L295" s="8"/>
+      <c r="M295" s="8"/>
+      <c r="N295" s="8"/>
+      <c r="O295" s="8"/>
+      <c r="P295" s="8"/>
+      <c r="Q295" s="8"/>
+      <c r="R295" s="8"/>
+      <c r="S295" s="8"/>
+      <c r="T295" s="14"/>
       <c r="U295">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A296" s="23"/>
-      <c r="B296" s="2">
-        <v>7170</v>
+      <c r="B296" s="12">
+        <v>3083</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9169,10 +9169,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A297" s="23"/>
-      <c r="B297" s="2">
-        <v>2709</v>
+      <c r="B297" s="12">
+        <v>7546</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -9200,7 +9200,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="23"/>
       <c r="B298" s="2">
-        <v>3402</v>
+        <v>7170</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -9228,7 +9228,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="23"/>
       <c r="B299" s="2">
-        <v>8781</v>
+        <v>2709</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9256,7 +9256,7 @@
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" s="23"/>
       <c r="B300" s="2">
-        <v>8771</v>
+        <v>3402</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9284,7 +9284,7 @@
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A301" s="23"/>
       <c r="B301" s="2">
-        <v>3091</v>
+        <v>8781</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9312,7 +9312,7 @@
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>2195</v>
+        <v>8771</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9340,7 +9340,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>1184</v>
+        <v>3091</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9368,7 +9368,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>2667</v>
+        <v>2195</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9396,7 +9396,7 @@
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="23"/>
       <c r="B305" s="2">
-        <v>5917</v>
+        <v>1184</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9424,7 +9424,7 @@
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A306" s="23"/>
       <c r="B306" s="2">
-        <v>8545</v>
+        <v>2667</v>
       </c>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -9452,7 +9452,7 @@
     <row r="307" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A307" s="23"/>
       <c r="B307" s="2">
-        <v>1288</v>
+        <v>5917</v>
       </c>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
@@ -9477,115 +9477,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A308" s="24"/>
-      <c r="B308" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C308" s="6"/>
-      <c r="D308" s="6"/>
-      <c r="E308" s="6"/>
-      <c r="F308" s="6"/>
-      <c r="G308" s="6"/>
-      <c r="H308" s="6"/>
-      <c r="I308" s="6"/>
-      <c r="J308" s="6"/>
-      <c r="K308" s="6"/>
-      <c r="L308" s="6"/>
-      <c r="M308" s="6"/>
-      <c r="N308" s="6"/>
-      <c r="O308" s="6"/>
-      <c r="P308" s="6"/>
-      <c r="Q308" s="6"/>
-      <c r="R308" s="6"/>
-      <c r="S308" s="6"/>
-      <c r="T308" s="7"/>
+    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A308" s="23"/>
+      <c r="B308" s="2">
+        <v>8545</v>
+      </c>
+      <c r="C308" s="2"/>
+      <c r="D308" s="2"/>
+      <c r="E308" s="2"/>
+      <c r="F308" s="2"/>
+      <c r="G308" s="2"/>
+      <c r="H308" s="2"/>
+      <c r="I308" s="2"/>
+      <c r="J308" s="2"/>
+      <c r="K308" s="2"/>
+      <c r="L308" s="2"/>
+      <c r="M308" s="2"/>
+      <c r="N308" s="2"/>
+      <c r="O308" s="2"/>
+      <c r="P308" s="2"/>
+      <c r="Q308" s="2"/>
+      <c r="R308" s="2"/>
+      <c r="S308" s="2"/>
+      <c r="T308" s="5"/>
       <c r="U308">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A309" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B309" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C309" s="8"/>
-      <c r="D309" s="8"/>
-      <c r="E309" s="8"/>
-      <c r="F309" s="8"/>
-      <c r="G309" s="8"/>
-      <c r="H309" s="8"/>
-      <c r="I309" s="8"/>
-      <c r="J309" s="8"/>
-      <c r="K309" s="8"/>
-      <c r="L309" s="8"/>
-      <c r="M309" s="8"/>
-      <c r="N309" s="8"/>
-      <c r="O309" s="8"/>
-      <c r="P309" s="8"/>
-      <c r="Q309" s="8"/>
-      <c r="R309" s="8"/>
-      <c r="S309" s="8"/>
-      <c r="T309" s="14"/>
+      <c r="A309" s="23"/>
+      <c r="B309" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C309" s="2"/>
+      <c r="D309" s="2"/>
+      <c r="E309" s="2"/>
+      <c r="F309" s="2"/>
+      <c r="G309" s="2"/>
+      <c r="H309" s="2"/>
+      <c r="I309" s="2"/>
+      <c r="J309" s="2"/>
+      <c r="K309" s="2"/>
+      <c r="L309" s="2"/>
+      <c r="M309" s="2"/>
+      <c r="N309" s="2"/>
+      <c r="O309" s="2"/>
+      <c r="P309" s="2"/>
+      <c r="Q309" s="2"/>
+      <c r="R309" s="2"/>
+      <c r="S309" s="2"/>
+      <c r="T309" s="5"/>
       <c r="U309">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A310" s="23"/>
-      <c r="B310" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C310" s="2"/>
-      <c r="D310" s="2"/>
-      <c r="E310" s="2"/>
-      <c r="F310" s="2"/>
-      <c r="G310" s="2"/>
-      <c r="H310" s="2"/>
-      <c r="I310" s="2"/>
-      <c r="J310" s="2"/>
-      <c r="K310" s="2"/>
-      <c r="L310" s="2"/>
-      <c r="M310" s="2"/>
-      <c r="N310" s="2"/>
-      <c r="O310" s="2"/>
-      <c r="P310" s="2"/>
-      <c r="Q310" s="2"/>
-      <c r="R310" s="2"/>
-      <c r="S310" s="2"/>
-      <c r="T310" s="5"/>
+    <row r="310" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A310" s="24"/>
+      <c r="B310" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C310" s="6"/>
+      <c r="D310" s="6"/>
+      <c r="E310" s="6"/>
+      <c r="F310" s="6"/>
+      <c r="G310" s="6"/>
+      <c r="H310" s="6"/>
+      <c r="I310" s="6"/>
+      <c r="J310" s="6"/>
+      <c r="K310" s="6"/>
+      <c r="L310" s="6"/>
+      <c r="M310" s="6"/>
+      <c r="N310" s="6"/>
+      <c r="O310" s="6"/>
+      <c r="P310" s="6"/>
+      <c r="Q310" s="6"/>
+      <c r="R310" s="6"/>
+      <c r="S310" s="6"/>
+      <c r="T310" s="7"/>
       <c r="U310">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A311" s="23"/>
-      <c r="B311" s="2">
-        <v>3093</v>
-      </c>
-      <c r="C311" s="2"/>
-      <c r="D311" s="2"/>
-      <c r="E311" s="2"/>
-      <c r="F311" s="2"/>
-      <c r="G311" s="2"/>
-      <c r="H311" s="2"/>
-      <c r="I311" s="2"/>
-      <c r="J311" s="2"/>
-      <c r="K311" s="2"/>
-      <c r="L311" s="2"/>
-      <c r="M311" s="2"/>
-      <c r="N311" s="2"/>
-      <c r="O311" s="2"/>
-      <c r="P311" s="2"/>
-      <c r="Q311" s="2"/>
-      <c r="R311" s="2"/>
-      <c r="S311" s="2"/>
-      <c r="T311" s="5"/>
+      <c r="A311" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B311" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C311" s="8"/>
+      <c r="D311" s="8"/>
+      <c r="E311" s="8"/>
+      <c r="F311" s="8"/>
+      <c r="G311" s="8"/>
+      <c r="H311" s="8"/>
+      <c r="I311" s="8"/>
+      <c r="J311" s="8"/>
+      <c r="K311" s="8"/>
+      <c r="L311" s="8"/>
+      <c r="M311" s="8"/>
+      <c r="N311" s="8"/>
+      <c r="O311" s="8"/>
+      <c r="P311" s="8"/>
+      <c r="Q311" s="8"/>
+      <c r="R311" s="8"/>
+      <c r="S311" s="8"/>
+      <c r="T311" s="14"/>
       <c r="U311">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9594,7 +9594,7 @@
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A312" s="23"/>
       <c r="B312" s="2">
-        <v>8805</v>
+        <v>6598</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -9622,7 +9622,7 @@
     <row r="313" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A313" s="23"/>
       <c r="B313" s="2">
-        <v>8158</v>
+        <v>3093</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
@@ -9647,115 +9647,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A314" s="24"/>
-      <c r="B314" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C314" s="6"/>
-      <c r="D314" s="6"/>
-      <c r="E314" s="6"/>
-      <c r="F314" s="6"/>
-      <c r="G314" s="6"/>
-      <c r="H314" s="6"/>
-      <c r="I314" s="6"/>
-      <c r="J314" s="6"/>
-      <c r="K314" s="6"/>
-      <c r="L314" s="6"/>
-      <c r="M314" s="6"/>
-      <c r="N314" s="6"/>
-      <c r="O314" s="6"/>
-      <c r="P314" s="6"/>
-      <c r="Q314" s="6"/>
-      <c r="R314" s="6"/>
-      <c r="S314" s="6"/>
-      <c r="T314" s="7"/>
+    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A314" s="23"/>
+      <c r="B314" s="2">
+        <v>8805</v>
+      </c>
+      <c r="C314" s="2"/>
+      <c r="D314" s="2"/>
+      <c r="E314" s="2"/>
+      <c r="F314" s="2"/>
+      <c r="G314" s="2"/>
+      <c r="H314" s="2"/>
+      <c r="I314" s="2"/>
+      <c r="J314" s="2"/>
+      <c r="K314" s="2"/>
+      <c r="L314" s="2"/>
+      <c r="M314" s="2"/>
+      <c r="N314" s="2"/>
+      <c r="O314" s="2"/>
+      <c r="P314" s="2"/>
+      <c r="Q314" s="2"/>
+      <c r="R314" s="2"/>
+      <c r="S314" s="2"/>
+      <c r="T314" s="5"/>
       <c r="U314">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B315" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C315" s="8"/>
-      <c r="D315" s="8"/>
-      <c r="E315" s="8"/>
-      <c r="F315" s="8"/>
-      <c r="G315" s="8"/>
-      <c r="H315" s="8"/>
-      <c r="I315" s="8"/>
-      <c r="J315" s="8"/>
-      <c r="K315" s="8"/>
-      <c r="L315" s="8"/>
-      <c r="M315" s="8"/>
-      <c r="N315" s="8"/>
-      <c r="O315" s="8"/>
-      <c r="P315" s="8"/>
-      <c r="Q315" s="8"/>
-      <c r="R315" s="8"/>
-      <c r="S315" s="8"/>
-      <c r="T315" s="14"/>
+      <c r="A315" s="23"/>
+      <c r="B315" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C315" s="2"/>
+      <c r="D315" s="2"/>
+      <c r="E315" s="2"/>
+      <c r="F315" s="2"/>
+      <c r="G315" s="2"/>
+      <c r="H315" s="2"/>
+      <c r="I315" s="2"/>
+      <c r="J315" s="2"/>
+      <c r="K315" s="2"/>
+      <c r="L315" s="2"/>
+      <c r="M315" s="2"/>
+      <c r="N315" s="2"/>
+      <c r="O315" s="2"/>
+      <c r="P315" s="2"/>
+      <c r="Q315" s="2"/>
+      <c r="R315" s="2"/>
+      <c r="S315" s="2"/>
+      <c r="T315" s="5"/>
       <c r="U315">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A316" s="23"/>
-      <c r="B316" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C316" s="2"/>
-      <c r="D316" s="2"/>
-      <c r="E316" s="2"/>
-      <c r="F316" s="2"/>
-      <c r="G316" s="2"/>
-      <c r="H316" s="2"/>
-      <c r="I316" s="2"/>
-      <c r="J316" s="2"/>
-      <c r="K316" s="2"/>
-      <c r="L316" s="2"/>
-      <c r="M316" s="2"/>
-      <c r="N316" s="2"/>
-      <c r="O316" s="2"/>
-      <c r="P316" s="2"/>
-      <c r="Q316" s="2"/>
-      <c r="R316" s="2"/>
-      <c r="S316" s="2"/>
-      <c r="T316" s="5"/>
+    <row r="316" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="24"/>
+      <c r="B316" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C316" s="6"/>
+      <c r="D316" s="6"/>
+      <c r="E316" s="6"/>
+      <c r="F316" s="6"/>
+      <c r="G316" s="6"/>
+      <c r="H316" s="6"/>
+      <c r="I316" s="6"/>
+      <c r="J316" s="6"/>
+      <c r="K316" s="6"/>
+      <c r="L316" s="6"/>
+      <c r="M316" s="6"/>
+      <c r="N316" s="6"/>
+      <c r="O316" s="6"/>
+      <c r="P316" s="6"/>
+      <c r="Q316" s="6"/>
+      <c r="R316" s="6"/>
+      <c r="S316" s="6"/>
+      <c r="T316" s="7"/>
       <c r="U316">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A317" s="23"/>
-      <c r="B317" s="2">
-        <v>9002</v>
-      </c>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2"/>
-      <c r="E317" s="2"/>
-      <c r="F317" s="2"/>
-      <c r="G317" s="2"/>
-      <c r="H317" s="2"/>
-      <c r="I317" s="2"/>
-      <c r="J317" s="2"/>
-      <c r="K317" s="2"/>
-      <c r="L317" s="2"/>
-      <c r="M317" s="2"/>
-      <c r="N317" s="2"/>
-      <c r="O317" s="2"/>
-      <c r="P317" s="2"/>
-      <c r="Q317" s="2"/>
-      <c r="R317" s="2"/>
-      <c r="S317" s="2"/>
-      <c r="T317" s="5"/>
+      <c r="A317" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B317" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C317" s="8"/>
+      <c r="D317" s="8"/>
+      <c r="E317" s="8"/>
+      <c r="F317" s="8"/>
+      <c r="G317" s="8"/>
+      <c r="H317" s="8"/>
+      <c r="I317" s="8"/>
+      <c r="J317" s="8"/>
+      <c r="K317" s="8"/>
+      <c r="L317" s="8"/>
+      <c r="M317" s="8"/>
+      <c r="N317" s="8"/>
+      <c r="O317" s="8"/>
+      <c r="P317" s="8"/>
+      <c r="Q317" s="8"/>
+      <c r="R317" s="8"/>
+      <c r="S317" s="8"/>
+      <c r="T317" s="14"/>
       <c r="U317">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9764,7 +9764,7 @@
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A318" s="23"/>
       <c r="B318" s="2">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -9792,7 +9792,7 @@
     <row r="319" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A319" s="23"/>
       <c r="B319" s="2">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
@@ -9817,125 +9817,169 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A320" s="24"/>
-      <c r="B320" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C320" s="6"/>
-      <c r="D320" s="6"/>
-      <c r="E320" s="6"/>
-      <c r="F320" s="6"/>
-      <c r="G320" s="6"/>
-      <c r="H320" s="6"/>
-      <c r="I320" s="6"/>
-      <c r="J320" s="6"/>
-      <c r="K320" s="6"/>
-      <c r="L320" s="6"/>
-      <c r="M320" s="6"/>
-      <c r="N320" s="6"/>
-      <c r="O320" s="6"/>
-      <c r="P320" s="6"/>
-      <c r="Q320" s="6"/>
-      <c r="R320" s="6"/>
-      <c r="S320" s="6"/>
-      <c r="T320" s="7"/>
+    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A320" s="23"/>
+      <c r="B320" s="2">
+        <v>7432</v>
+      </c>
+      <c r="C320" s="2"/>
+      <c r="D320" s="2"/>
+      <c r="E320" s="2"/>
+      <c r="F320" s="2"/>
+      <c r="G320" s="2"/>
+      <c r="H320" s="2"/>
+      <c r="I320" s="2"/>
+      <c r="J320" s="2"/>
+      <c r="K320" s="2"/>
+      <c r="L320" s="2"/>
+      <c r="M320" s="2"/>
+      <c r="N320" s="2"/>
+      <c r="O320" s="2"/>
+      <c r="P320" s="2"/>
+      <c r="Q320" s="2"/>
+      <c r="R320" s="2"/>
+      <c r="S320" s="2"/>
+      <c r="T320" s="5"/>
       <c r="U320">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A321" s="23"/>
+      <c r="B321" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C321" s="2"/>
+      <c r="D321" s="2"/>
+      <c r="E321" s="2"/>
+      <c r="F321" s="2"/>
+      <c r="G321" s="2"/>
+      <c r="H321" s="2"/>
+      <c r="I321" s="2"/>
+      <c r="J321" s="2"/>
+      <c r="K321" s="2"/>
+      <c r="L321" s="2"/>
+      <c r="M321" s="2"/>
+      <c r="N321" s="2"/>
+      <c r="O321" s="2"/>
+      <c r="P321" s="2"/>
+      <c r="Q321" s="2"/>
+      <c r="R321" s="2"/>
+      <c r="S321" s="2"/>
+      <c r="T321" s="5"/>
       <c r="U321">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="24"/>
+      <c r="B322" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C322" s="6"/>
+      <c r="D322" s="6"/>
+      <c r="E322" s="6"/>
+      <c r="F322" s="6"/>
+      <c r="G322" s="6"/>
+      <c r="H322" s="6"/>
+      <c r="I322" s="6"/>
+      <c r="J322" s="6"/>
+      <c r="K322" s="6"/>
+      <c r="L322" s="6"/>
+      <c r="M322" s="6"/>
+      <c r="N322" s="6"/>
+      <c r="O322" s="6"/>
+      <c r="P322" s="6"/>
+      <c r="Q322" s="6"/>
+      <c r="R322" s="6"/>
+      <c r="S322" s="6"/>
+      <c r="T322" s="7"/>
       <c r="U322">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U323">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U324">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U325">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U326">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U327">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U328">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U329">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U330">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U331">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U332">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U333">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U334">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U335">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U336">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -10027,19 +10071,19 @@
     </row>
     <row r="351" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U351">
-        <f t="shared" ref="U351:U414" ca="1" si="8">IF(B351=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="352" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U352">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="353" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U353">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U353:U416" ca="1" si="8">IF(B353=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10411,19 +10455,19 @@
     </row>
     <row r="415" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U415">
-        <f t="shared" ref="U415:U478" ca="1" si="9">IF(B415=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="416" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U416">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="417" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U417">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U417:U480" ca="1" si="9">IF(B417=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10795,19 +10839,19 @@
     </row>
     <row r="479" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U479">
-        <f t="shared" ref="U479:U542" ca="1" si="10">IF(B479=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="480" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U480">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="481" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U481">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U481:U544" ca="1" si="10">IF(B481=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11179,19 +11223,19 @@
     </row>
     <row r="543" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U543">
-        <f t="shared" ref="U543:U606" ca="1" si="11">IF(B543=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="544" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U544">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="545" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U545">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U545:U608" ca="1" si="11">IF(B545=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11563,19 +11607,19 @@
     </row>
     <row r="607" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U607">
-        <f t="shared" ref="U607:U670" ca="1" si="12">IF(B607=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="608" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U608">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="609" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U609">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U609:U672" ca="1" si="12">IF(B609=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11947,19 +11991,19 @@
     </row>
     <row r="671" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U671">
-        <f t="shared" ref="U671:U734" ca="1" si="13">IF(B671=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="672" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U672">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="673" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U673">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U673:U736" ca="1" si="13">IF(B673=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12331,19 +12375,19 @@
     </row>
     <row r="735" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U735">
-        <f t="shared" ref="U735:U798" ca="1" si="14">IF(B735=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="736" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U736">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="737" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U737">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U737:U800" ca="1" si="14">IF(B737=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12715,19 +12759,19 @@
     </row>
     <row r="799" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U799">
-        <f t="shared" ref="U799:U862" ca="1" si="15">IF(B799=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="800" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U800">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="801" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U801">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U801:U864" ca="1" si="15">IF(B801=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13099,19 +13143,19 @@
     </row>
     <row r="863" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U863">
-        <f t="shared" ref="U863:U924" ca="1" si="16">IF(B863=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="864" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U864">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="865" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U865">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U865:U926" ca="1" si="16">IF(B865=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13469,26 +13513,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="925" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U925">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="926" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U926">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A317:A322"/>
+    <mergeCell ref="A247:A276"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A295:A310"/>
+    <mergeCell ref="A311:A316"/>
+    <mergeCell ref="A64:A104"/>
+    <mergeCell ref="A219:A230"/>
+    <mergeCell ref="A150:A183"/>
+    <mergeCell ref="A184:A201"/>
+    <mergeCell ref="A105:A149"/>
+    <mergeCell ref="A19:A63"/>
+    <mergeCell ref="A202:A218"/>
+    <mergeCell ref="A231:A238"/>
+    <mergeCell ref="A239:A246"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A288:A292"/>
-    <mergeCell ref="A275:A287"/>
-    <mergeCell ref="A315:A320"/>
-    <mergeCell ref="A245:A274"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A293:A308"/>
-    <mergeCell ref="A309:A314"/>
-    <mergeCell ref="A64:A104"/>
-    <mergeCell ref="A217:A228"/>
-    <mergeCell ref="A150:A181"/>
-    <mergeCell ref="A182:A199"/>
-    <mergeCell ref="A105:A149"/>
-    <mergeCell ref="A19:A63"/>
-    <mergeCell ref="A200:A216"/>
-    <mergeCell ref="A229:A236"/>
-    <mergeCell ref="A237:A244"/>
+    <mergeCell ref="A290:A294"/>
+    <mergeCell ref="A277:A289"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
start work on task about parsing method call
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$296</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$297</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -521,6 +521,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,15 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W928"/>
+  <dimension ref="A1:W929"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H182" sqref="H182"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,56 +891,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>8099</v>
+        <v>6739</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -1056,7 +1056,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3">
         <v>1662</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2">
         <v>1860</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2">
         <v>4764</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2">
         <v>2429</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2">
         <v>7472</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2">
         <v>4140</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2">
         <v>2959</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2">
         <v>7271</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2">
         <v>2632</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="13">
@@ -2656,7 +2656,7 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="12">
         <v>2217</v>
       </c>
@@ -2684,7 +2684,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="12">
         <v>1824</v>
       </c>
@@ -2712,7 +2712,7 @@
       </c>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="29"/>
+      <c r="A67" s="23"/>
       <c r="B67" s="12">
         <v>2564</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
     </row>
     <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="12">
         <v>8487</v>
       </c>
@@ -2768,7 +2768,7 @@
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="2">
         <v>8878</v>
       </c>
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="2">
         <v>3072</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="2">
         <v>5980</v>
       </c>
@@ -2852,7 +2852,7 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="2">
         <v>8174</v>
       </c>
@@ -2880,7 +2880,7 @@
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="2">
         <v>4257</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="2">
         <v>2291</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="2">
         <v>1763</v>
       </c>
@@ -2964,7 +2964,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="2">
         <v>5662</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="23"/>
       <c r="B77" s="2">
         <v>1945</v>
       </c>
@@ -3020,7 +3020,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="29"/>
+      <c r="A78" s="23"/>
       <c r="B78" s="2">
         <v>1186</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="29"/>
+      <c r="A79" s="23"/>
       <c r="B79" s="2">
         <v>8715</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="23"/>
       <c r="B80" s="2">
         <v>8518</v>
       </c>
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
+      <c r="A81" s="23"/>
       <c r="B81" s="2">
         <v>4847</v>
       </c>
@@ -3132,7 +3132,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="A82" s="23"/>
       <c r="B82" s="2">
         <v>6589</v>
       </c>
@@ -3160,7 +3160,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
+      <c r="A83" s="23"/>
       <c r="B83" s="2">
         <v>7991</v>
       </c>
@@ -3188,7 +3188,7 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="23"/>
       <c r="B84" s="2">
         <v>6291</v>
       </c>
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="23"/>
       <c r="B85" s="2">
         <v>3770</v>
       </c>
@@ -3244,7 +3244,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
+      <c r="A86" s="23"/>
       <c r="B86" s="2">
         <v>7178</v>
       </c>
@@ -3272,7 +3272,7 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="23"/>
       <c r="B87" s="2">
         <v>3883</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="2">
         <v>1999</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="23"/>
       <c r="B89" s="2">
         <v>4042</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="23"/>
       <c r="B90" s="2">
         <v>6351</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="2">
         <v>5382</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="2">
         <v>7088</v>
       </c>
@@ -3440,7 +3440,7 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="2">
         <v>7250</v>
       </c>
@@ -3468,7 +3468,7 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="2">
         <v>6740</v>
       </c>
@@ -3496,7 +3496,7 @@
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="2">
         <v>9038</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="2">
         <v>1292</v>
       </c>
@@ -3552,7 +3552,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="23"/>
       <c r="B97" s="2">
         <v>4527</v>
       </c>
@@ -3580,7 +3580,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="23"/>
       <c r="B98" s="2">
         <v>6556</v>
       </c>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="2">
         <v>5635</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+      <c r="A100" s="23"/>
       <c r="B100" s="2">
         <v>3878</v>
       </c>
@@ -3664,7 +3664,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="23"/>
       <c r="B101" s="2">
         <v>1217</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="23"/>
       <c r="B102" s="2">
         <v>1438</v>
       </c>
@@ -3720,7 +3720,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
+      <c r="A103" s="23"/>
       <c r="B103" s="2">
         <v>2153</v>
       </c>
@@ -3748,7 +3748,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="30"/>
+      <c r="A104" s="24"/>
       <c r="B104" s="6">
         <v>7937</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="28" t="s">
+      <c r="A105" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B105" s="13">
@@ -3806,7 +3806,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="12">
         <v>1881</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" s="29"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="2">
         <v>8495</v>
       </c>
@@ -3862,7 +3862,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" s="29"/>
+      <c r="A108" s="23"/>
       <c r="B108" s="2">
         <v>1315</v>
       </c>
@@ -3890,7 +3890,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A109" s="29"/>
+      <c r="A109" s="23"/>
       <c r="B109" s="2">
         <v>6066</v>
       </c>
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A110" s="29"/>
+      <c r="A110" s="23"/>
       <c r="B110" s="2">
         <v>2565</v>
       </c>
@@ -3946,7 +3946,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A111" s="29"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="2">
         <v>2594</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="2">
         <v>2321</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" s="29"/>
+      <c r="A113" s="23"/>
       <c r="B113" s="2">
         <v>5053</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114" s="29"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="2">
         <v>4338</v>
       </c>
@@ -4058,7 +4058,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="29"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="2">
         <v>3762</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" s="29"/>
+      <c r="A116" s="23"/>
       <c r="B116" s="2">
         <v>3550</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
+      <c r="A117" s="23"/>
       <c r="B117" s="2">
         <v>4264</v>
       </c>
@@ -4142,7 +4142,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
+      <c r="A118" s="23"/>
       <c r="B118" s="2">
         <v>2475</v>
       </c>
@@ -4170,7 +4170,7 @@
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
+      <c r="A119" s="23"/>
       <c r="B119" s="2">
         <v>9180</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" s="29"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="2">
         <v>1544</v>
       </c>
@@ -4226,7 +4226,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="29"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="2">
         <v>9562</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="2">
         <v>3669</v>
       </c>
@@ -4282,7 +4282,7 @@
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
+      <c r="A123" s="23"/>
       <c r="B123" s="2">
         <v>5951</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
+      <c r="A124" s="23"/>
       <c r="B124" s="2">
         <v>2802</v>
       </c>
@@ -4338,7 +4338,7 @@
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
+      <c r="A125" s="23"/>
       <c r="B125" s="2">
         <v>2324</v>
       </c>
@@ -4366,7 +4366,7 @@
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="2">
         <v>8731</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
+      <c r="A127" s="23"/>
       <c r="B127" s="2">
         <v>4082</v>
       </c>
@@ -4422,7 +4422,7 @@
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128" s="29"/>
+      <c r="A128" s="23"/>
       <c r="B128" s="2">
         <v>6280</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
+      <c r="A129" s="23"/>
       <c r="B129" s="2">
         <v>7585</v>
       </c>
@@ -4478,7 +4478,7 @@
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="23"/>
       <c r="B130" s="2">
         <v>1483</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A131" s="29"/>
+      <c r="A131" s="23"/>
       <c r="B131" s="2">
         <v>3983</v>
       </c>
@@ -4534,7 +4534,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="29"/>
+      <c r="A132" s="23"/>
       <c r="B132" s="2">
         <v>8770</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
+      <c r="A133" s="23"/>
       <c r="B133" s="2">
         <v>4236</v>
       </c>
@@ -4590,7 +4590,7 @@
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="23"/>
       <c r="B134" s="2">
         <v>8696</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
+      <c r="A135" s="23"/>
       <c r="B135" s="2">
         <v>5969</v>
       </c>
@@ -4646,7 +4646,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A136" s="29"/>
+      <c r="A136" s="23"/>
       <c r="B136" s="2">
         <v>8418</v>
       </c>
@@ -4674,7 +4674,7 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A137" s="29"/>
+      <c r="A137" s="23"/>
       <c r="B137" s="2">
         <v>5170</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
+      <c r="A138" s="23"/>
       <c r="B138" s="2">
         <v>8395</v>
       </c>
@@ -4730,7 +4730,7 @@
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A139" s="29"/>
+      <c r="A139" s="23"/>
       <c r="B139" s="2">
         <v>5568</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
+      <c r="A140" s="23"/>
       <c r="B140" s="2">
         <v>2592</v>
       </c>
@@ -4781,12 +4781,12 @@
       <c r="S140" s="2"/>
       <c r="T140" s="5"/>
       <c r="U140">
-        <f t="shared" ref="U140:U210" ca="1" si="4">IF(B140=$W$1,1,0)</f>
+        <f t="shared" ref="U140:U211" ca="1" si="4">IF(B140=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A141" s="29"/>
+      <c r="A141" s="23"/>
       <c r="B141" s="2">
         <v>4075</v>
       </c>
@@ -4814,7 +4814,7 @@
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
+      <c r="A142" s="23"/>
       <c r="B142" s="2">
         <v>7517</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A143" s="29"/>
+      <c r="A143" s="23"/>
       <c r="B143" s="2">
         <v>5448</v>
       </c>
@@ -4870,7 +4870,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A144" s="29"/>
+      <c r="A144" s="23"/>
       <c r="B144" s="2">
         <v>6582</v>
       </c>
@@ -4898,7 +4898,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A145" s="29"/>
+      <c r="A145" s="23"/>
       <c r="B145" s="2">
         <v>5238</v>
       </c>
@@ -4926,7 +4926,7 @@
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A146" s="29"/>
+      <c r="A146" s="23"/>
       <c r="B146" s="2">
         <v>2084</v>
       </c>
@@ -4954,7 +4954,7 @@
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A147" s="29"/>
+      <c r="A147" s="23"/>
       <c r="B147" s="2">
         <v>5411</v>
       </c>
@@ -4982,7 +4982,7 @@
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A148" s="29"/>
+      <c r="A148" s="23"/>
       <c r="B148" s="2">
         <v>5171</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
     </row>
     <row r="149" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="30"/>
+      <c r="A149" s="24"/>
       <c r="B149" s="6">
         <v>1862</v>
       </c>
@@ -5038,7 +5038,7 @@
       </c>
     </row>
     <row r="150" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="28" t="s">
+      <c r="A150" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B150" s="13">
@@ -5068,7 +5068,7 @@
       </c>
     </row>
     <row r="151" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="29"/>
+      <c r="A151" s="23"/>
       <c r="B151" s="12">
         <v>9931</v>
       </c>
@@ -5096,7 +5096,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="29"/>
+      <c r="A152" s="23"/>
       <c r="B152" s="12">
         <v>9696</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="29"/>
+      <c r="A153" s="23"/>
       <c r="B153" s="12">
         <v>1947</v>
       </c>
@@ -5152,7 +5152,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A154" s="29"/>
+      <c r="A154" s="23"/>
       <c r="B154" s="2">
         <v>4425</v>
       </c>
@@ -5180,7 +5180,7 @@
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A155" s="29"/>
+      <c r="A155" s="23"/>
       <c r="B155" s="2">
         <v>1433</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A156" s="29"/>
+      <c r="A156" s="23"/>
       <c r="B156" s="2">
         <v>5683</v>
       </c>
@@ -5236,7 +5236,7 @@
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A157" s="29"/>
+      <c r="A157" s="23"/>
       <c r="B157" s="2">
         <v>1223</v>
       </c>
@@ -5264,7 +5264,7 @@
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A158" s="29"/>
+      <c r="A158" s="23"/>
       <c r="B158" s="2">
         <v>8311</v>
       </c>
@@ -5292,7 +5292,7 @@
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="29"/>
+      <c r="A159" s="23"/>
       <c r="B159" s="2">
         <v>3134</v>
       </c>
@@ -5320,7 +5320,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A160" s="29"/>
+      <c r="A160" s="23"/>
       <c r="B160" s="2">
         <v>9711</v>
       </c>
@@ -5348,7 +5348,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A161" s="29"/>
+      <c r="A161" s="23"/>
       <c r="B161" s="2">
         <v>7085</v>
       </c>
@@ -5376,7 +5376,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A162" s="29"/>
+      <c r="A162" s="23"/>
       <c r="B162" s="2">
         <v>3333</v>
       </c>
@@ -5404,7 +5404,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A163" s="29"/>
+      <c r="A163" s="23"/>
       <c r="B163" s="2">
         <v>8820</v>
       </c>
@@ -5432,7 +5432,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A164" s="29"/>
+      <c r="A164" s="23"/>
       <c r="B164" s="2">
         <v>5694</v>
       </c>
@@ -5460,7 +5460,7 @@
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A165" s="29"/>
+      <c r="A165" s="23"/>
       <c r="B165" s="2">
         <v>6806</v>
       </c>
@@ -5488,7 +5488,7 @@
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A166" s="29"/>
+      <c r="A166" s="23"/>
       <c r="B166" s="2">
         <v>7369</v>
       </c>
@@ -5516,7 +5516,7 @@
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A167" s="29"/>
+      <c r="A167" s="23"/>
       <c r="B167" s="2">
         <v>7534</v>
       </c>
@@ -5544,7 +5544,7 @@
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168" s="29"/>
+      <c r="A168" s="23"/>
       <c r="B168" s="2">
         <v>5894</v>
       </c>
@@ -5572,7 +5572,7 @@
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A169" s="29"/>
+      <c r="A169" s="23"/>
       <c r="B169" s="2">
         <v>4515</v>
       </c>
@@ -5600,7 +5600,7 @@
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A170" s="29"/>
+      <c r="A170" s="23"/>
       <c r="B170" s="2">
         <v>9774</v>
       </c>
@@ -5628,7 +5628,7 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A171" s="29"/>
+      <c r="A171" s="23"/>
       <c r="B171" s="2">
         <v>3946</v>
       </c>
@@ -5656,7 +5656,7 @@
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A172" s="29"/>
+      <c r="A172" s="23"/>
       <c r="B172" s="2">
         <v>6497</v>
       </c>
@@ -5684,7 +5684,7 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
+      <c r="A173" s="23"/>
       <c r="B173" s="2">
         <v>5648</v>
       </c>
@@ -5712,7 +5712,7 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="29"/>
+      <c r="A174" s="23"/>
       <c r="B174" s="2">
         <v>3940</v>
       </c>
@@ -5740,7 +5740,7 @@
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A175" s="29"/>
+      <c r="A175" s="23"/>
       <c r="B175" s="2">
         <v>7290</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" s="29"/>
+      <c r="A176" s="23"/>
       <c r="B176" s="2">
         <v>7035</v>
       </c>
@@ -5796,7 +5796,7 @@
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A177" s="29"/>
+      <c r="A177" s="23"/>
       <c r="B177" s="2">
         <v>9271</v>
       </c>
@@ -5824,7 +5824,7 @@
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A178" s="29"/>
+      <c r="A178" s="23"/>
       <c r="B178" s="2">
         <v>8769</v>
       </c>
@@ -5852,7 +5852,7 @@
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A179" s="29"/>
+      <c r="A179" s="23"/>
       <c r="B179" s="2">
         <v>4497</v>
       </c>
@@ -5880,7 +5880,7 @@
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A180" s="29"/>
+      <c r="A180" s="23"/>
       <c r="B180" s="2">
         <v>3218</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A181" s="29"/>
+      <c r="A181" s="23"/>
       <c r="B181" s="2">
         <v>6492</v>
       </c>
@@ -5936,7 +5936,7 @@
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A182" s="29"/>
+      <c r="A182" s="23"/>
       <c r="B182" s="2">
         <v>4293</v>
       </c>
@@ -5964,7 +5964,7 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A183" s="29"/>
+      <c r="A183" s="23"/>
       <c r="B183" s="2">
         <v>7703</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="29"/>
+      <c r="A184" s="23"/>
       <c r="B184" s="2">
         <v>5541</v>
       </c>
@@ -6020,7 +6020,7 @@
       </c>
     </row>
     <row r="185" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="30"/>
+      <c r="A185" s="24"/>
       <c r="B185" s="6">
         <v>9182</v>
       </c>
@@ -6048,7 +6048,7 @@
       </c>
     </row>
     <row r="186" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="28" t="s">
+      <c r="A186" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B186" s="13">
@@ -6073,12 +6073,12 @@
       <c r="S186" s="8"/>
       <c r="T186" s="14"/>
       <c r="U186">
-        <f t="shared" ref="U186:U203" ca="1" si="5">IF(B186=$W$1,1,0)</f>
+        <f t="shared" ref="U186:U204" ca="1" si="5">IF(B186=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="29"/>
+      <c r="A187" s="23"/>
       <c r="B187" s="12">
         <v>9001</v>
       </c>
@@ -6106,7 +6106,7 @@
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="29"/>
+      <c r="A188" s="23"/>
       <c r="B188" s="2">
         <v>7491</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A189" s="29"/>
+      <c r="A189" s="23"/>
       <c r="B189" s="2">
         <v>9531</v>
       </c>
@@ -6162,7 +6162,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A190" s="29"/>
+      <c r="A190" s="23"/>
       <c r="B190" s="2">
         <v>9812</v>
       </c>
@@ -6190,7 +6190,7 @@
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A191" s="29"/>
+      <c r="A191" s="23"/>
       <c r="B191" s="2">
         <v>9279</v>
       </c>
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A192" s="29"/>
+      <c r="A192" s="23"/>
       <c r="B192" s="2">
         <v>4845</v>
       </c>
@@ -6246,7 +6246,7 @@
       </c>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A193" s="29"/>
+      <c r="A193" s="23"/>
       <c r="B193" s="2">
         <v>5728</v>
       </c>
@@ -6274,7 +6274,7 @@
       </c>
     </row>
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A194" s="29"/>
+      <c r="A194" s="23"/>
       <c r="B194" s="2">
         <v>7222</v>
       </c>
@@ -6302,7 +6302,7 @@
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="29"/>
+      <c r="A195" s="23"/>
       <c r="B195" s="2">
         <v>5923</v>
       </c>
@@ -6330,7 +6330,7 @@
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A196" s="29"/>
+      <c r="A196" s="23"/>
       <c r="B196" s="2">
         <v>4265</v>
       </c>
@@ -6358,7 +6358,7 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="29"/>
+      <c r="A197" s="23"/>
       <c r="B197" s="2">
         <v>2166</v>
       </c>
@@ -6386,7 +6386,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="29"/>
+      <c r="A198" s="23"/>
       <c r="B198" s="2">
         <v>9116</v>
       </c>
@@ -6414,7 +6414,7 @@
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="29"/>
+      <c r="A199" s="23"/>
       <c r="B199" s="2">
         <v>9925</v>
       </c>
@@ -6442,7 +6442,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="29"/>
+      <c r="A200" s="23"/>
       <c r="B200" s="2">
         <v>3657</v>
       </c>
@@ -6470,7 +6470,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
+      <c r="A201" s="23"/>
       <c r="B201" s="2">
         <v>6599</v>
       </c>
@@ -6525,87 +6525,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="30"/>
-      <c r="B203" s="6">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A203" s="31"/>
+      <c r="B203" s="9">
         <v>1703</v>
       </c>
-      <c r="C203" s="6"/>
-      <c r="D203" s="6"/>
-      <c r="E203" s="6"/>
-      <c r="F203" s="6"/>
-      <c r="G203" s="6"/>
-      <c r="H203" s="6"/>
-      <c r="I203" s="6"/>
-      <c r="J203" s="6"/>
-      <c r="K203" s="6"/>
-      <c r="L203" s="6"/>
-      <c r="M203" s="6"/>
-      <c r="N203" s="6"/>
-      <c r="O203" s="6"/>
-      <c r="P203" s="6"/>
-      <c r="Q203" s="6"/>
-      <c r="R203" s="6"/>
-      <c r="S203" s="6"/>
-      <c r="T203" s="7"/>
+      <c r="C203" s="9"/>
+      <c r="D203" s="9"/>
+      <c r="E203" s="9"/>
+      <c r="F203" s="9"/>
+      <c r="G203" s="9"/>
+      <c r="H203" s="9"/>
+      <c r="I203" s="9"/>
+      <c r="J203" s="9"/>
+      <c r="K203" s="9"/>
+      <c r="L203" s="9"/>
+      <c r="M203" s="9"/>
+      <c r="N203" s="9"/>
+      <c r="O203" s="9"/>
+      <c r="P203" s="9"/>
+      <c r="Q203" s="9"/>
+      <c r="R203" s="9"/>
+      <c r="S203" s="9"/>
+      <c r="T203" s="15"/>
       <c r="U203">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="34" t="s">
+    <row r="204" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="24"/>
+      <c r="B204" s="6">
+        <v>8887</v>
+      </c>
+      <c r="C204" s="6"/>
+      <c r="D204" s="6"/>
+      <c r="E204" s="6"/>
+      <c r="F204" s="6"/>
+      <c r="G204" s="6"/>
+      <c r="H204" s="6"/>
+      <c r="I204" s="6"/>
+      <c r="J204" s="6"/>
+      <c r="K204" s="6"/>
+      <c r="L204" s="6"/>
+      <c r="M204" s="6"/>
+      <c r="N204" s="6"/>
+      <c r="O204" s="6"/>
+      <c r="P204" s="6"/>
+      <c r="Q204" s="6"/>
+      <c r="R204" s="6"/>
+      <c r="S204" s="6"/>
+      <c r="T204" s="7"/>
+      <c r="U204">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A205" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B204" s="8">
+      <c r="B205" s="8">
         <v>6175</v>
       </c>
-      <c r="C204" s="8"/>
-      <c r="D204" s="8"/>
-      <c r="E204" s="8"/>
-      <c r="F204" s="8"/>
-      <c r="G204" s="8"/>
-      <c r="H204" s="8"/>
-      <c r="I204" s="8"/>
-      <c r="J204" s="8"/>
-      <c r="K204" s="8"/>
-      <c r="L204" s="8"/>
-      <c r="M204" s="8"/>
-      <c r="N204" s="8"/>
-      <c r="O204" s="8"/>
-      <c r="P204" s="8"/>
-      <c r="Q204" s="8"/>
-      <c r="R204" s="8"/>
-      <c r="S204" s="8"/>
-      <c r="T204" s="14"/>
-      <c r="U204">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="35"/>
-      <c r="B205" s="2">
-        <v>4488</v>
-      </c>
-      <c r="C205" s="2"/>
-      <c r="D205" s="2"/>
-      <c r="E205" s="2"/>
-      <c r="F205" s="2"/>
-      <c r="G205" s="2"/>
-      <c r="H205" s="2"/>
-      <c r="I205" s="2"/>
-      <c r="J205" s="2"/>
-      <c r="K205" s="2"/>
-      <c r="L205" s="2"/>
-      <c r="M205" s="2"/>
-      <c r="N205" s="2"/>
-      <c r="O205" s="2"/>
-      <c r="P205" s="2"/>
-      <c r="Q205" s="2"/>
-      <c r="R205" s="2"/>
-      <c r="S205" s="2"/>
-      <c r="T205" s="5"/>
+      <c r="C205" s="8"/>
+      <c r="D205" s="8"/>
+      <c r="E205" s="8"/>
+      <c r="F205" s="8"/>
+      <c r="G205" s="8"/>
+      <c r="H205" s="8"/>
+      <c r="I205" s="8"/>
+      <c r="J205" s="8"/>
+      <c r="K205" s="8"/>
+      <c r="L205" s="8"/>
+      <c r="M205" s="8"/>
+      <c r="N205" s="8"/>
+      <c r="O205" s="8"/>
+      <c r="P205" s="8"/>
+      <c r="Q205" s="8"/>
+      <c r="R205" s="8"/>
+      <c r="S205" s="8"/>
+      <c r="T205" s="14"/>
       <c r="U205">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6614,7 +6614,7 @@
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
       <c r="B206" s="2">
-        <v>4954</v>
+        <v>4488</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -6642,7 +6642,7 @@
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
       <c r="B207" s="2">
-        <v>4642</v>
+        <v>4954</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6670,7 +6670,7 @@
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
       <c r="B208" s="2">
-        <v>5537</v>
+        <v>4642</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6698,7 +6698,7 @@
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
       <c r="B209" s="2">
-        <v>5847</v>
+        <v>5537</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6726,7 +6726,7 @@
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
       <c r="B210" s="2">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -6754,7 +6754,7 @@
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="35"/>
       <c r="B211" s="2">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -6775,14 +6775,14 @@
       <c r="S211" s="2"/>
       <c r="T211" s="5"/>
       <c r="U211">
-        <f t="shared" ref="U211:U290" ca="1" si="6">IF(B211=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="2">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -6803,14 +6803,14 @@
       <c r="S212" s="2"/>
       <c r="T212" s="5"/>
       <c r="U212">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="U212:U291" ca="1" si="6">IF(B212=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="2">
-        <v>3226</v>
+        <v>6861</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -6838,7 +6838,7 @@
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
       <c r="B214" s="2">
-        <v>4372</v>
+        <v>3226</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -6866,7 +6866,7 @@
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="2">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -6894,7 +6894,7 @@
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="2">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -6922,7 +6922,7 @@
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
       <c r="B217" s="2">
-        <v>9417</v>
+        <v>1668</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6950,7 +6950,7 @@
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
       <c r="B218" s="2">
-        <v>3148</v>
+        <v>9417</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6978,7 +6978,7 @@
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
       <c r="B219" s="2">
-        <v>2137</v>
+        <v>3148</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -7003,96 +7003,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="36"/>
-      <c r="B220" s="6">
-        <v>5621</v>
-      </c>
-      <c r="C220" s="6"/>
-      <c r="D220" s="6"/>
-      <c r="E220" s="6"/>
-      <c r="F220" s="6"/>
-      <c r="G220" s="6"/>
-      <c r="H220" s="6"/>
-      <c r="I220" s="6"/>
-      <c r="J220" s="6"/>
-      <c r="K220" s="6"/>
-      <c r="L220" s="6"/>
-      <c r="M220" s="6"/>
-      <c r="N220" s="6"/>
-      <c r="O220" s="6"/>
-      <c r="P220" s="6"/>
-      <c r="Q220" s="6"/>
-      <c r="R220" s="6"/>
-      <c r="S220" s="6"/>
-      <c r="T220" s="7"/>
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A220" s="35"/>
+      <c r="B220" s="2">
+        <v>2137</v>
+      </c>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
+      <c r="E220" s="2"/>
+      <c r="F220" s="2"/>
+      <c r="G220" s="2"/>
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+      <c r="J220" s="2"/>
+      <c r="K220" s="2"/>
+      <c r="L220" s="2"/>
+      <c r="M220" s="2"/>
+      <c r="N220" s="2"/>
+      <c r="O220" s="2"/>
+      <c r="P220" s="2"/>
+      <c r="Q220" s="2"/>
+      <c r="R220" s="2"/>
+      <c r="S220" s="2"/>
+      <c r="T220" s="5"/>
       <c r="U220">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A221" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B221" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C221" s="8"/>
-      <c r="D221" s="8"/>
-      <c r="E221" s="8"/>
-      <c r="F221" s="8"/>
-      <c r="G221" s="8"/>
-      <c r="H221" s="8"/>
-      <c r="I221" s="8"/>
-      <c r="J221" s="8"/>
-      <c r="K221" s="8"/>
-      <c r="L221" s="8"/>
-      <c r="M221" s="8"/>
-      <c r="N221" s="8"/>
-      <c r="O221" s="8"/>
-      <c r="P221" s="8"/>
-      <c r="Q221" s="8"/>
-      <c r="R221" s="8"/>
-      <c r="S221" s="8"/>
-      <c r="T221" s="14"/>
+    <row r="221" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="36"/>
+      <c r="B221" s="6">
+        <v>5621</v>
+      </c>
+      <c r="C221" s="6"/>
+      <c r="D221" s="6"/>
+      <c r="E221" s="6"/>
+      <c r="F221" s="6"/>
+      <c r="G221" s="6"/>
+      <c r="H221" s="6"/>
+      <c r="I221" s="6"/>
+      <c r="J221" s="6"/>
+      <c r="K221" s="6"/>
+      <c r="L221" s="6"/>
+      <c r="M221" s="6"/>
+      <c r="N221" s="6"/>
+      <c r="O221" s="6"/>
+      <c r="P221" s="6"/>
+      <c r="Q221" s="6"/>
+      <c r="R221" s="6"/>
+      <c r="S221" s="6"/>
+      <c r="T221" s="7"/>
       <c r="U221">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A222" s="29"/>
-      <c r="B222" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C222" s="2"/>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
-      <c r="I222" s="2"/>
-      <c r="J222" s="2"/>
-      <c r="K222" s="2"/>
-      <c r="L222" s="2"/>
-      <c r="M222" s="2"/>
-      <c r="N222" s="2"/>
-      <c r="O222" s="2"/>
-      <c r="P222" s="2"/>
-      <c r="Q222" s="2"/>
-      <c r="R222" s="2"/>
-      <c r="S222" s="2"/>
-      <c r="T222" s="5"/>
+      <c r="A222" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B222" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C222" s="8"/>
+      <c r="D222" s="8"/>
+      <c r="E222" s="8"/>
+      <c r="F222" s="8"/>
+      <c r="G222" s="8"/>
+      <c r="H222" s="8"/>
+      <c r="I222" s="8"/>
+      <c r="J222" s="8"/>
+      <c r="K222" s="8"/>
+      <c r="L222" s="8"/>
+      <c r="M222" s="8"/>
+      <c r="N222" s="8"/>
+      <c r="O222" s="8"/>
+      <c r="P222" s="8"/>
+      <c r="Q222" s="8"/>
+      <c r="R222" s="8"/>
+      <c r="S222" s="8"/>
+      <c r="T222" s="14"/>
       <c r="U222">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A223" s="29"/>
+      <c r="A223" s="23"/>
       <c r="B223" s="2">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
@@ -7118,9 +7118,9 @@
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A224" s="29"/>
+      <c r="A224" s="23"/>
       <c r="B224" s="2">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7146,9 +7146,9 @@
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A225" s="29"/>
+      <c r="A225" s="23"/>
       <c r="B225" s="2">
-        <v>6409</v>
+        <v>7060</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -7174,9 +7174,9 @@
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A226" s="29"/>
+      <c r="A226" s="23"/>
       <c r="B226" s="2">
-        <v>2386</v>
+        <v>6409</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
@@ -7201,10 +7201,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="29"/>
-      <c r="B227" s="6">
-        <v>7372</v>
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A227" s="23"/>
+      <c r="B227" s="2">
+        <v>2386</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
@@ -7224,11 +7224,15 @@
       <c r="R227" s="2"/>
       <c r="S227" s="2"/>
       <c r="T227" s="5"/>
-    </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A228" s="29"/>
-      <c r="B228" s="2">
-        <v>9159</v>
+      <c r="U227">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="23"/>
+      <c r="B228" s="6">
+        <v>7372</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -7248,15 +7252,11 @@
       <c r="R228" s="2"/>
       <c r="S228" s="2"/>
       <c r="T228" s="5"/>
-      <c r="U228">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A229" s="29"/>
+      <c r="A229" s="23"/>
       <c r="B229" s="2">
-        <v>5309</v>
+        <v>9159</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -7282,9 +7282,9 @@
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A230" s="29"/>
+      <c r="A230" s="23"/>
       <c r="B230" s="2">
-        <v>3290</v>
+        <v>5309</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
@@ -7310,9 +7310,9 @@
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A231" s="29"/>
+      <c r="A231" s="23"/>
       <c r="B231" s="2">
-        <v>5345</v>
+        <v>3290</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
@@ -7337,96 +7337,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="30"/>
-      <c r="B232" s="6">
-        <v>6812</v>
-      </c>
-      <c r="C232" s="6"/>
-      <c r="D232" s="6"/>
-      <c r="E232" s="6"/>
-      <c r="F232" s="6"/>
-      <c r="G232" s="6"/>
-      <c r="H232" s="6"/>
-      <c r="I232" s="6"/>
-      <c r="J232" s="6"/>
-      <c r="K232" s="6"/>
-      <c r="L232" s="6"/>
-      <c r="M232" s="6"/>
-      <c r="N232" s="6"/>
-      <c r="O232" s="6"/>
-      <c r="P232" s="6"/>
-      <c r="Q232" s="6"/>
-      <c r="R232" s="6"/>
-      <c r="S232" s="6"/>
-      <c r="T232" s="7"/>
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A232" s="23"/>
+      <c r="B232" s="2">
+        <v>5345</v>
+      </c>
+      <c r="C232" s="2"/>
+      <c r="D232" s="2"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="2"/>
+      <c r="H232" s="2"/>
+      <c r="I232" s="2"/>
+      <c r="J232" s="2"/>
+      <c r="K232" s="2"/>
+      <c r="L232" s="2"/>
+      <c r="M232" s="2"/>
+      <c r="N232" s="2"/>
+      <c r="O232" s="2"/>
+      <c r="P232" s="2"/>
+      <c r="Q232" s="2"/>
+      <c r="R232" s="2"/>
+      <c r="S232" s="2"/>
+      <c r="T232" s="5"/>
       <c r="U232">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A233" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B233" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C233" s="8"/>
-      <c r="D233" s="8"/>
-      <c r="E233" s="8"/>
-      <c r="F233" s="8"/>
-      <c r="G233" s="8"/>
-      <c r="H233" s="8"/>
-      <c r="I233" s="8"/>
-      <c r="J233" s="8"/>
-      <c r="K233" s="8"/>
-      <c r="L233" s="8"/>
-      <c r="M233" s="8"/>
-      <c r="N233" s="8"/>
-      <c r="O233" s="8"/>
-      <c r="P233" s="8"/>
-      <c r="Q233" s="8"/>
-      <c r="R233" s="8"/>
-      <c r="S233" s="8"/>
-      <c r="T233" s="14"/>
+    <row r="233" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="24"/>
+      <c r="B233" s="6">
+        <v>6812</v>
+      </c>
+      <c r="C233" s="6"/>
+      <c r="D233" s="6"/>
+      <c r="E233" s="6"/>
+      <c r="F233" s="6"/>
+      <c r="G233" s="6"/>
+      <c r="H233" s="6"/>
+      <c r="I233" s="6"/>
+      <c r="J233" s="6"/>
+      <c r="K233" s="6"/>
+      <c r="L233" s="6"/>
+      <c r="M233" s="6"/>
+      <c r="N233" s="6"/>
+      <c r="O233" s="6"/>
+      <c r="P233" s="6"/>
+      <c r="Q233" s="6"/>
+      <c r="R233" s="6"/>
+      <c r="S233" s="6"/>
+      <c r="T233" s="7"/>
       <c r="U233">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A234" s="29"/>
-      <c r="B234" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C234" s="2"/>
-      <c r="D234" s="2"/>
-      <c r="E234" s="2"/>
-      <c r="F234" s="2"/>
-      <c r="G234" s="2"/>
-      <c r="H234" s="2"/>
-      <c r="I234" s="2"/>
-      <c r="J234" s="2"/>
-      <c r="K234" s="2"/>
-      <c r="L234" s="2"/>
-      <c r="M234" s="2"/>
-      <c r="N234" s="2"/>
-      <c r="O234" s="2"/>
-      <c r="P234" s="2"/>
-      <c r="Q234" s="2"/>
-      <c r="R234" s="2"/>
-      <c r="S234" s="2"/>
-      <c r="T234" s="5"/>
+      <c r="A234" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B234" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C234" s="8"/>
+      <c r="D234" s="8"/>
+      <c r="E234" s="8"/>
+      <c r="F234" s="8"/>
+      <c r="G234" s="8"/>
+      <c r="H234" s="8"/>
+      <c r="I234" s="8"/>
+      <c r="J234" s="8"/>
+      <c r="K234" s="8"/>
+      <c r="L234" s="8"/>
+      <c r="M234" s="8"/>
+      <c r="N234" s="8"/>
+      <c r="O234" s="8"/>
+      <c r="P234" s="8"/>
+      <c r="Q234" s="8"/>
+      <c r="R234" s="8"/>
+      <c r="S234" s="8"/>
+      <c r="T234" s="14"/>
       <c r="U234">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="29"/>
+      <c r="A235" s="23"/>
       <c r="B235" s="12">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -7451,10 +7451,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A236" s="29"/>
-      <c r="B236" s="19">
-        <v>8861</v>
+    <row r="236" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A236" s="23"/>
+      <c r="B236" s="12">
+        <v>9062</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
@@ -7480,9 +7480,9 @@
       </c>
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A237" s="29"/>
-      <c r="B237" s="2">
-        <v>5164</v>
+      <c r="A237" s="23"/>
+      <c r="B237" s="19">
+        <v>8861</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
@@ -7508,9 +7508,9 @@
       </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="29"/>
+      <c r="A238" s="23"/>
       <c r="B238" s="2">
-        <v>2354</v>
+        <v>5164</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -7536,9 +7536,9 @@
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="29"/>
+      <c r="A239" s="23"/>
       <c r="B239" s="2">
-        <v>2030</v>
+        <v>2354</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -7563,96 +7563,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="30"/>
-      <c r="B240" s="6">
-        <v>7649</v>
-      </c>
-      <c r="C240" s="6"/>
-      <c r="D240" s="6"/>
-      <c r="E240" s="6"/>
-      <c r="F240" s="6"/>
-      <c r="G240" s="6"/>
-      <c r="H240" s="6"/>
-      <c r="I240" s="6"/>
-      <c r="J240" s="6"/>
-      <c r="K240" s="6"/>
-      <c r="L240" s="6"/>
-      <c r="M240" s="6"/>
-      <c r="N240" s="6"/>
-      <c r="O240" s="6"/>
-      <c r="P240" s="6"/>
-      <c r="Q240" s="6"/>
-      <c r="R240" s="6"/>
-      <c r="S240" s="6"/>
-      <c r="T240" s="7"/>
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A240" s="23"/>
+      <c r="B240" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="2"/>
+      <c r="G240" s="2"/>
+      <c r="H240" s="2"/>
+      <c r="I240" s="2"/>
+      <c r="J240" s="2"/>
+      <c r="K240" s="2"/>
+      <c r="L240" s="2"/>
+      <c r="M240" s="2"/>
+      <c r="N240" s="2"/>
+      <c r="O240" s="2"/>
+      <c r="P240" s="2"/>
+      <c r="Q240" s="2"/>
+      <c r="R240" s="2"/>
+      <c r="S240" s="2"/>
+      <c r="T240" s="5"/>
       <c r="U240">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A241" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="8"/>
-      <c r="H241" s="8"/>
-      <c r="I241" s="8"/>
-      <c r="J241" s="8"/>
-      <c r="K241" s="8"/>
-      <c r="L241" s="8"/>
-      <c r="M241" s="8"/>
-      <c r="N241" s="8"/>
-      <c r="O241" s="8"/>
-      <c r="P241" s="8"/>
-      <c r="Q241" s="8"/>
-      <c r="R241" s="8"/>
-      <c r="S241" s="8"/>
-      <c r="T241" s="14"/>
+    <row r="241" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="24"/>
+      <c r="B241" s="6">
+        <v>7649</v>
+      </c>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="E241" s="6"/>
+      <c r="F241" s="6"/>
+      <c r="G241" s="6"/>
+      <c r="H241" s="6"/>
+      <c r="I241" s="6"/>
+      <c r="J241" s="6"/>
+      <c r="K241" s="6"/>
+      <c r="L241" s="6"/>
+      <c r="M241" s="6"/>
+      <c r="N241" s="6"/>
+      <c r="O241" s="6"/>
+      <c r="P241" s="6"/>
+      <c r="Q241" s="6"/>
+      <c r="R241" s="6"/>
+      <c r="S241" s="6"/>
+      <c r="T241" s="7"/>
       <c r="U241">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A242" s="29"/>
-      <c r="B242" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C242" s="2"/>
-      <c r="D242" s="2"/>
-      <c r="E242" s="2"/>
-      <c r="F242" s="2"/>
-      <c r="G242" s="2"/>
-      <c r="H242" s="2"/>
-      <c r="I242" s="2"/>
-      <c r="J242" s="2"/>
-      <c r="K242" s="2"/>
-      <c r="L242" s="2"/>
-      <c r="M242" s="2"/>
-      <c r="N242" s="2"/>
-      <c r="O242" s="2"/>
-      <c r="P242" s="2"/>
-      <c r="Q242" s="2"/>
-      <c r="R242" s="2"/>
-      <c r="S242" s="2"/>
-      <c r="T242" s="5"/>
+      <c r="A242" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B242" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C242" s="8"/>
+      <c r="D242" s="8"/>
+      <c r="E242" s="8"/>
+      <c r="F242" s="8"/>
+      <c r="G242" s="8"/>
+      <c r="H242" s="8"/>
+      <c r="I242" s="8"/>
+      <c r="J242" s="8"/>
+      <c r="K242" s="8"/>
+      <c r="L242" s="8"/>
+      <c r="M242" s="8"/>
+      <c r="N242" s="8"/>
+      <c r="O242" s="8"/>
+      <c r="P242" s="8"/>
+      <c r="Q242" s="8"/>
+      <c r="R242" s="8"/>
+      <c r="S242" s="8"/>
+      <c r="T242" s="14"/>
       <c r="U242">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="29"/>
+      <c r="A243" s="23"/>
       <c r="B243" s="2">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
@@ -7678,9 +7678,9 @@
       </c>
     </row>
     <row r="244" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A244" s="29"/>
+      <c r="A244" s="23"/>
       <c r="B244" s="2">
-        <v>6882</v>
+        <v>6732</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
@@ -7706,9 +7706,9 @@
       </c>
     </row>
     <row r="245" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A245" s="29"/>
+      <c r="A245" s="23"/>
       <c r="B245" s="2">
-        <v>1212</v>
+        <v>6882</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7734,9 +7734,9 @@
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="29"/>
+      <c r="A246" s="23"/>
       <c r="B246" s="2">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7762,9 +7762,9 @@
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="29"/>
+      <c r="A247" s="23"/>
       <c r="B247" s="2">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7789,96 +7789,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="30"/>
-      <c r="B248" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C248" s="6"/>
-      <c r="D248" s="6"/>
-      <c r="E248" s="6"/>
-      <c r="F248" s="6"/>
-      <c r="G248" s="6"/>
-      <c r="H248" s="6"/>
-      <c r="I248" s="6"/>
-      <c r="J248" s="6"/>
-      <c r="K248" s="6"/>
-      <c r="L248" s="6"/>
-      <c r="M248" s="6"/>
-      <c r="N248" s="6"/>
-      <c r="O248" s="6"/>
-      <c r="P248" s="6"/>
-      <c r="Q248" s="6"/>
-      <c r="R248" s="6"/>
-      <c r="S248" s="6"/>
-      <c r="T248" s="7"/>
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A248" s="23"/>
+      <c r="B248" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C248" s="2"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="2"/>
+      <c r="F248" s="2"/>
+      <c r="G248" s="2"/>
+      <c r="H248" s="2"/>
+      <c r="I248" s="2"/>
+      <c r="J248" s="2"/>
+      <c r="K248" s="2"/>
+      <c r="L248" s="2"/>
+      <c r="M248" s="2"/>
+      <c r="N248" s="2"/>
+      <c r="O248" s="2"/>
+      <c r="P248" s="2"/>
+      <c r="Q248" s="2"/>
+      <c r="R248" s="2"/>
+      <c r="S248" s="2"/>
+      <c r="T248" s="5"/>
       <c r="U248">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B249" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C249" s="8"/>
-      <c r="D249" s="8"/>
-      <c r="E249" s="8"/>
-      <c r="F249" s="8"/>
-      <c r="G249" s="8"/>
-      <c r="H249" s="8"/>
-      <c r="I249" s="8"/>
-      <c r="J249" s="8"/>
-      <c r="K249" s="8"/>
-      <c r="L249" s="8"/>
-      <c r="M249" s="8"/>
-      <c r="N249" s="8"/>
-      <c r="O249" s="8"/>
-      <c r="P249" s="8"/>
-      <c r="Q249" s="8"/>
-      <c r="R249" s="8"/>
-      <c r="S249" s="8"/>
-      <c r="T249" s="14"/>
+    <row r="249" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="24"/>
+      <c r="B249" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C249" s="6"/>
+      <c r="D249" s="6"/>
+      <c r="E249" s="6"/>
+      <c r="F249" s="6"/>
+      <c r="G249" s="6"/>
+      <c r="H249" s="6"/>
+      <c r="I249" s="6"/>
+      <c r="J249" s="6"/>
+      <c r="K249" s="6"/>
+      <c r="L249" s="6"/>
+      <c r="M249" s="6"/>
+      <c r="N249" s="6"/>
+      <c r="O249" s="6"/>
+      <c r="P249" s="6"/>
+      <c r="Q249" s="6"/>
+      <c r="R249" s="6"/>
+      <c r="S249" s="6"/>
+      <c r="T249" s="7"/>
       <c r="U249">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A250" s="29"/>
-      <c r="B250" s="2">
-        <v>6011</v>
-      </c>
-      <c r="C250" s="2"/>
-      <c r="D250" s="2"/>
-      <c r="E250" s="2"/>
-      <c r="F250" s="2"/>
-      <c r="G250" s="2"/>
-      <c r="H250" s="2"/>
-      <c r="I250" s="2"/>
-      <c r="J250" s="2"/>
-      <c r="K250" s="2"/>
-      <c r="L250" s="2"/>
-      <c r="M250" s="2"/>
-      <c r="N250" s="2"/>
-      <c r="O250" s="2"/>
-      <c r="P250" s="2"/>
-      <c r="Q250" s="2"/>
-      <c r="R250" s="2"/>
-      <c r="S250" s="2"/>
-      <c r="T250" s="5"/>
+    <row r="250" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A250" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B250" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C250" s="8"/>
+      <c r="D250" s="8"/>
+      <c r="E250" s="8"/>
+      <c r="F250" s="8"/>
+      <c r="G250" s="8"/>
+      <c r="H250" s="8"/>
+      <c r="I250" s="8"/>
+      <c r="J250" s="8"/>
+      <c r="K250" s="8"/>
+      <c r="L250" s="8"/>
+      <c r="M250" s="8"/>
+      <c r="N250" s="8"/>
+      <c r="O250" s="8"/>
+      <c r="P250" s="8"/>
+      <c r="Q250" s="8"/>
+      <c r="R250" s="8"/>
+      <c r="S250" s="8"/>
+      <c r="T250" s="14"/>
       <c r="U250">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="29"/>
+      <c r="A251" s="23"/>
       <c r="B251" s="2">
-        <v>8403</v>
+        <v>6011</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
@@ -7904,9 +7904,9 @@
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A252" s="29"/>
+      <c r="A252" s="23"/>
       <c r="B252" s="2">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7932,9 +7932,9 @@
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A253" s="29"/>
-      <c r="B253" s="21">
-        <v>6037</v>
+      <c r="A253" s="23"/>
+      <c r="B253" s="2">
+        <v>3185</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7960,9 +7960,9 @@
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" s="29"/>
-      <c r="B254" s="2">
-        <v>9914</v>
+      <c r="A254" s="23"/>
+      <c r="B254" s="21">
+        <v>6037</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7988,9 +7988,9 @@
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A255" s="29"/>
+      <c r="A255" s="23"/>
       <c r="B255" s="2">
-        <v>4916</v>
+        <v>9914</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8016,9 +8016,9 @@
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="29"/>
+      <c r="A256" s="23"/>
       <c r="B256" s="2">
-        <v>2809</v>
+        <v>4916</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8044,9 +8044,9 @@
       </c>
     </row>
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A257" s="29"/>
+      <c r="A257" s="23"/>
       <c r="B257" s="2">
-        <v>8265</v>
+        <v>2809</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8072,9 +8072,9 @@
       </c>
     </row>
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A258" s="29"/>
+      <c r="A258" s="23"/>
       <c r="B258" s="2">
-        <v>2092</v>
+        <v>8265</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8100,9 +8100,9 @@
       </c>
     </row>
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A259" s="29"/>
+      <c r="A259" s="23"/>
       <c r="B259" s="2">
-        <v>7297</v>
+        <v>2092</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8128,9 +8128,9 @@
       </c>
     </row>
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="29"/>
+      <c r="A260" s="23"/>
       <c r="B260" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8156,9 +8156,9 @@
       </c>
     </row>
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A261" s="29"/>
+      <c r="A261" s="23"/>
       <c r="B261" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8184,9 +8184,9 @@
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="29"/>
+      <c r="A262" s="23"/>
       <c r="B262" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8212,9 +8212,9 @@
       </c>
     </row>
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A263" s="29"/>
+      <c r="A263" s="23"/>
       <c r="B263" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8240,9 +8240,9 @@
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A264" s="29"/>
+      <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8268,9 +8268,9 @@
       </c>
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A265" s="29"/>
+      <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8296,9 +8296,9 @@
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="29"/>
+      <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8324,9 +8324,9 @@
       </c>
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="29"/>
+      <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8352,9 +8352,9 @@
       </c>
     </row>
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="29"/>
+      <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>9238</v>
+        <v>5449</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8380,9 +8380,9 @@
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="29"/>
+      <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>2662</v>
+        <v>9238</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8408,9 +8408,9 @@
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="29"/>
+      <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8436,9 +8436,9 @@
       </c>
     </row>
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A271" s="29"/>
+      <c r="A271" s="23"/>
       <c r="B271" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8464,9 +8464,9 @@
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="29"/>
+      <c r="A272" s="23"/>
       <c r="B272" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8492,9 +8492,9 @@
       </c>
     </row>
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="29"/>
+      <c r="A273" s="23"/>
       <c r="B273" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8520,9 +8520,9 @@
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="29"/>
+      <c r="A274" s="23"/>
       <c r="B274" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8548,9 +8548,9 @@
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="29"/>
+      <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8576,9 +8576,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="29"/>
+      <c r="A276" s="23"/>
       <c r="B276" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8604,9 +8604,9 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="29"/>
+      <c r="A277" s="23"/>
       <c r="B277" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8631,96 +8631,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="30"/>
-      <c r="B278" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C278" s="6"/>
-      <c r="D278" s="6"/>
-      <c r="E278" s="6"/>
-      <c r="F278" s="6"/>
-      <c r="G278" s="6"/>
-      <c r="H278" s="6"/>
-      <c r="I278" s="6"/>
-      <c r="J278" s="6"/>
-      <c r="K278" s="6"/>
-      <c r="L278" s="6"/>
-      <c r="M278" s="6"/>
-      <c r="N278" s="6"/>
-      <c r="O278" s="6"/>
-      <c r="P278" s="6"/>
-      <c r="Q278" s="6"/>
-      <c r="R278" s="6"/>
-      <c r="S278" s="6"/>
-      <c r="T278" s="7"/>
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A278" s="23"/>
+      <c r="B278" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C278" s="2"/>
+      <c r="D278" s="2"/>
+      <c r="E278" s="2"/>
+      <c r="F278" s="2"/>
+      <c r="G278" s="2"/>
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+      <c r="L278" s="2"/>
+      <c r="M278" s="2"/>
+      <c r="N278" s="2"/>
+      <c r="O278" s="2"/>
+      <c r="P278" s="2"/>
+      <c r="Q278" s="2"/>
+      <c r="R278" s="2"/>
+      <c r="S278" s="2"/>
+      <c r="T278" s="5"/>
       <c r="U278">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B279" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C279" s="8"/>
-      <c r="D279" s="8"/>
-      <c r="E279" s="8"/>
-      <c r="F279" s="8"/>
-      <c r="G279" s="8"/>
-      <c r="H279" s="8"/>
-      <c r="I279" s="8"/>
-      <c r="J279" s="8"/>
-      <c r="K279" s="8"/>
-      <c r="L279" s="8"/>
-      <c r="M279" s="8"/>
-      <c r="N279" s="8"/>
-      <c r="O279" s="8"/>
-      <c r="P279" s="8"/>
-      <c r="Q279" s="8"/>
-      <c r="R279" s="8"/>
-      <c r="S279" s="8"/>
-      <c r="T279" s="14"/>
+    <row r="279" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A279" s="24"/>
+      <c r="B279" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C279" s="6"/>
+      <c r="D279" s="6"/>
+      <c r="E279" s="6"/>
+      <c r="F279" s="6"/>
+      <c r="G279" s="6"/>
+      <c r="H279" s="6"/>
+      <c r="I279" s="6"/>
+      <c r="J279" s="6"/>
+      <c r="K279" s="6"/>
+      <c r="L279" s="6"/>
+      <c r="M279" s="6"/>
+      <c r="N279" s="6"/>
+      <c r="O279" s="6"/>
+      <c r="P279" s="6"/>
+      <c r="Q279" s="6"/>
+      <c r="R279" s="6"/>
+      <c r="S279" s="6"/>
+      <c r="T279" s="7"/>
       <c r="U279">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="29"/>
+      <c r="A280" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="B280" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="E280" s="2"/>
-      <c r="F280" s="2"/>
-      <c r="G280" s="2"/>
-      <c r="H280" s="2"/>
-      <c r="I280" s="2"/>
-      <c r="J280" s="2"/>
-      <c r="K280" s="2"/>
-      <c r="L280" s="2"/>
-      <c r="M280" s="2"/>
-      <c r="N280" s="2"/>
-      <c r="O280" s="2"/>
-      <c r="P280" s="2"/>
-      <c r="Q280" s="2"/>
-      <c r="R280" s="2"/>
-      <c r="S280" s="2"/>
-      <c r="T280" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C280" s="8"/>
+      <c r="D280" s="8"/>
+      <c r="E280" s="8"/>
+      <c r="F280" s="8"/>
+      <c r="G280" s="8"/>
+      <c r="H280" s="8"/>
+      <c r="I280" s="8"/>
+      <c r="J280" s="8"/>
+      <c r="K280" s="8"/>
+      <c r="L280" s="8"/>
+      <c r="M280" s="8"/>
+      <c r="N280" s="8"/>
+      <c r="O280" s="8"/>
+      <c r="P280" s="8"/>
+      <c r="Q280" s="8"/>
+      <c r="R280" s="8"/>
+      <c r="S280" s="8"/>
+      <c r="T280" s="14"/>
       <c r="U280">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="29"/>
+      <c r="A281" s="23"/>
       <c r="B281" s="2">
-        <v>9990</v>
+        <v>1056</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8746,9 +8746,9 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="29"/>
+      <c r="A282" s="23"/>
       <c r="B282" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8774,9 +8774,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="29"/>
+      <c r="A283" s="23"/>
       <c r="B283" s="2">
-        <v>8418</v>
+        <v>7738</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8802,9 +8802,9 @@
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="29"/>
+      <c r="A284" s="23"/>
       <c r="B284" s="2">
-        <v>9512</v>
+        <v>8418</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8830,9 +8830,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="29"/>
+      <c r="A285" s="23"/>
       <c r="B285" s="2">
-        <v>9924</v>
+        <v>9512</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8858,28 +8858,28 @@
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="31"/>
-      <c r="B286" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C286" s="9"/>
-      <c r="D286" s="9"/>
-      <c r="E286" s="9"/>
-      <c r="F286" s="9"/>
-      <c r="G286" s="9"/>
-      <c r="H286" s="9"/>
-      <c r="I286" s="9"/>
-      <c r="J286" s="9"/>
-      <c r="K286" s="9"/>
-      <c r="L286" s="9"/>
-      <c r="M286" s="9"/>
-      <c r="N286" s="9"/>
-      <c r="O286" s="9"/>
-      <c r="P286" s="9"/>
-      <c r="Q286" s="9"/>
-      <c r="R286" s="9"/>
-      <c r="S286" s="9"/>
-      <c r="T286" s="15"/>
+      <c r="A286" s="23"/>
+      <c r="B286" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C286" s="2"/>
+      <c r="D286" s="2"/>
+      <c r="E286" s="2"/>
+      <c r="F286" s="2"/>
+      <c r="G286" s="2"/>
+      <c r="H286" s="2"/>
+      <c r="I286" s="2"/>
+      <c r="J286" s="2"/>
+      <c r="K286" s="2"/>
+      <c r="L286" s="2"/>
+      <c r="M286" s="2"/>
+      <c r="N286" s="2"/>
+      <c r="O286" s="2"/>
+      <c r="P286" s="2"/>
+      <c r="Q286" s="2"/>
+      <c r="R286" s="2"/>
+      <c r="S286" s="2"/>
+      <c r="T286" s="5"/>
       <c r="U286">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8888,7 +8888,7 @@
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A287" s="31"/>
       <c r="B287" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C287" s="9"/>
       <c r="D287" s="9"/>
@@ -8916,7 +8916,7 @@
     <row r="288" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A288" s="31"/>
       <c r="B288" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C288" s="9"/>
       <c r="D288" s="9"/>
@@ -8944,7 +8944,7 @@
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" s="31"/>
       <c r="B289" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C289" s="9"/>
       <c r="D289" s="9"/>
@@ -8972,7 +8972,7 @@
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="31"/>
       <c r="B290" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C290" s="9"/>
       <c r="D290" s="9"/>
@@ -8997,96 +8997,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="30"/>
-      <c r="B291" s="6">
+    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A291" s="31"/>
+      <c r="B291" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C291" s="9"/>
+      <c r="D291" s="9"/>
+      <c r="E291" s="9"/>
+      <c r="F291" s="9"/>
+      <c r="G291" s="9"/>
+      <c r="H291" s="9"/>
+      <c r="I291" s="9"/>
+      <c r="J291" s="9"/>
+      <c r="K291" s="9"/>
+      <c r="L291" s="9"/>
+      <c r="M291" s="9"/>
+      <c r="N291" s="9"/>
+      <c r="O291" s="9"/>
+      <c r="P291" s="9"/>
+      <c r="Q291" s="9"/>
+      <c r="R291" s="9"/>
+      <c r="S291" s="9"/>
+      <c r="T291" s="15"/>
+      <c r="U291">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="24"/>
+      <c r="B292" s="6">
         <v>6876</v>
       </c>
-      <c r="C291" s="6"/>
-      <c r="D291" s="6"/>
-      <c r="E291" s="6"/>
-      <c r="F291" s="6"/>
-      <c r="G291" s="6"/>
-      <c r="H291" s="6"/>
-      <c r="I291" s="6"/>
-      <c r="J291" s="6"/>
-      <c r="K291" s="6"/>
-      <c r="L291" s="6"/>
-      <c r="M291" s="6"/>
-      <c r="N291" s="6"/>
-      <c r="O291" s="6"/>
-      <c r="P291" s="6"/>
-      <c r="Q291" s="6"/>
-      <c r="R291" s="6"/>
-      <c r="S291" s="6"/>
-      <c r="T291" s="7"/>
-      <c r="U291">
-        <f t="shared" ref="U291:U354" ca="1" si="7">IF(B291=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A292" s="28" t="s">
+      <c r="C292" s="6"/>
+      <c r="D292" s="6"/>
+      <c r="E292" s="6"/>
+      <c r="F292" s="6"/>
+      <c r="G292" s="6"/>
+      <c r="H292" s="6"/>
+      <c r="I292" s="6"/>
+      <c r="J292" s="6"/>
+      <c r="K292" s="6"/>
+      <c r="L292" s="6"/>
+      <c r="M292" s="6"/>
+      <c r="N292" s="6"/>
+      <c r="O292" s="6"/>
+      <c r="P292" s="6"/>
+      <c r="Q292" s="6"/>
+      <c r="R292" s="6"/>
+      <c r="S292" s="6"/>
+      <c r="T292" s="7"/>
+      <c r="U292">
+        <f t="shared" ref="U292:U355" ca="1" si="7">IF(B292=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A293" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B292" s="8">
+      <c r="B293" s="8">
         <v>4304</v>
       </c>
-      <c r="C292" s="8"/>
-      <c r="D292" s="8"/>
-      <c r="E292" s="8"/>
-      <c r="F292" s="8"/>
-      <c r="G292" s="8"/>
-      <c r="H292" s="8"/>
-      <c r="I292" s="8"/>
-      <c r="J292" s="8"/>
-      <c r="K292" s="8"/>
-      <c r="L292" s="8"/>
-      <c r="M292" s="8"/>
-      <c r="N292" s="8"/>
-      <c r="O292" s="8"/>
-      <c r="P292" s="8"/>
-      <c r="Q292" s="8"/>
-      <c r="R292" s="8"/>
-      <c r="S292" s="8"/>
-      <c r="T292" s="14"/>
-      <c r="U292">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="29"/>
-      <c r="B293" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2"/>
-      <c r="E293" s="2"/>
-      <c r="F293" s="2"/>
-      <c r="G293" s="2"/>
-      <c r="H293" s="2"/>
-      <c r="I293" s="2"/>
-      <c r="J293" s="2"/>
-      <c r="K293" s="2"/>
-      <c r="L293" s="2"/>
-      <c r="M293" s="2"/>
-      <c r="N293" s="2"/>
-      <c r="O293" s="2"/>
-      <c r="P293" s="2"/>
-      <c r="Q293" s="2"/>
-      <c r="R293" s="2"/>
-      <c r="S293" s="2"/>
-      <c r="T293" s="5"/>
+      <c r="C293" s="8"/>
+      <c r="D293" s="8"/>
+      <c r="E293" s="8"/>
+      <c r="F293" s="8"/>
+      <c r="G293" s="8"/>
+      <c r="H293" s="8"/>
+      <c r="I293" s="8"/>
+      <c r="J293" s="8"/>
+      <c r="K293" s="8"/>
+      <c r="L293" s="8"/>
+      <c r="M293" s="8"/>
+      <c r="N293" s="8"/>
+      <c r="O293" s="8"/>
+      <c r="P293" s="8"/>
+      <c r="Q293" s="8"/>
+      <c r="R293" s="8"/>
+      <c r="S293" s="8"/>
+      <c r="T293" s="14"/>
       <c r="U293">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="29"/>
+      <c r="A294" s="23"/>
       <c r="B294" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9112,9 +9112,9 @@
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="29"/>
+      <c r="A295" s="23"/>
       <c r="B295" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9139,96 +9139,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="30"/>
-      <c r="B296" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C296" s="6"/>
-      <c r="D296" s="6"/>
-      <c r="E296" s="6"/>
-      <c r="F296" s="6"/>
-      <c r="G296" s="6"/>
-      <c r="H296" s="6"/>
-      <c r="I296" s="6"/>
-      <c r="J296" s="6"/>
-      <c r="K296" s="6"/>
-      <c r="L296" s="6"/>
-      <c r="M296" s="6"/>
-      <c r="N296" s="6"/>
-      <c r="O296" s="6"/>
-      <c r="P296" s="6"/>
-      <c r="Q296" s="6"/>
-      <c r="R296" s="6"/>
-      <c r="S296" s="6"/>
-      <c r="T296" s="7"/>
+    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A296" s="23"/>
+      <c r="B296" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C296" s="2"/>
+      <c r="D296" s="2"/>
+      <c r="E296" s="2"/>
+      <c r="F296" s="2"/>
+      <c r="G296" s="2"/>
+      <c r="H296" s="2"/>
+      <c r="I296" s="2"/>
+      <c r="J296" s="2"/>
+      <c r="K296" s="2"/>
+      <c r="L296" s="2"/>
+      <c r="M296" s="2"/>
+      <c r="N296" s="2"/>
+      <c r="O296" s="2"/>
+      <c r="P296" s="2"/>
+      <c r="Q296" s="2"/>
+      <c r="R296" s="2"/>
+      <c r="S296" s="2"/>
+      <c r="T296" s="5"/>
       <c r="U296">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A297" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B297" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C297" s="8"/>
-      <c r="D297" s="8"/>
-      <c r="E297" s="8"/>
-      <c r="F297" s="8"/>
-      <c r="G297" s="8"/>
-      <c r="H297" s="8"/>
-      <c r="I297" s="8"/>
-      <c r="J297" s="8"/>
-      <c r="K297" s="8"/>
-      <c r="L297" s="8"/>
-      <c r="M297" s="8"/>
-      <c r="N297" s="8"/>
-      <c r="O297" s="8"/>
-      <c r="P297" s="8"/>
-      <c r="Q297" s="8"/>
-      <c r="R297" s="8"/>
-      <c r="S297" s="8"/>
-      <c r="T297" s="14"/>
+    <row r="297" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="24"/>
+      <c r="B297" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C297" s="6"/>
+      <c r="D297" s="6"/>
+      <c r="E297" s="6"/>
+      <c r="F297" s="6"/>
+      <c r="G297" s="6"/>
+      <c r="H297" s="6"/>
+      <c r="I297" s="6"/>
+      <c r="J297" s="6"/>
+      <c r="K297" s="6"/>
+      <c r="L297" s="6"/>
+      <c r="M297" s="6"/>
+      <c r="N297" s="6"/>
+      <c r="O297" s="6"/>
+      <c r="P297" s="6"/>
+      <c r="Q297" s="6"/>
+      <c r="R297" s="6"/>
+      <c r="S297" s="6"/>
+      <c r="T297" s="7"/>
       <c r="U297">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A298" s="29"/>
-      <c r="B298" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C298" s="2"/>
-      <c r="D298" s="2"/>
-      <c r="E298" s="2"/>
-      <c r="F298" s="2"/>
-      <c r="G298" s="2"/>
-      <c r="H298" s="2"/>
-      <c r="I298" s="2"/>
-      <c r="J298" s="2"/>
-      <c r="K298" s="2"/>
-      <c r="L298" s="2"/>
-      <c r="M298" s="2"/>
-      <c r="N298" s="2"/>
-      <c r="O298" s="2"/>
-      <c r="P298" s="2"/>
-      <c r="Q298" s="2"/>
-      <c r="R298" s="2"/>
-      <c r="S298" s="2"/>
-      <c r="T298" s="5"/>
+      <c r="A298" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B298" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C298" s="8"/>
+      <c r="D298" s="8"/>
+      <c r="E298" s="8"/>
+      <c r="F298" s="8"/>
+      <c r="G298" s="8"/>
+      <c r="H298" s="8"/>
+      <c r="I298" s="8"/>
+      <c r="J298" s="8"/>
+      <c r="K298" s="8"/>
+      <c r="L298" s="8"/>
+      <c r="M298" s="8"/>
+      <c r="N298" s="8"/>
+      <c r="O298" s="8"/>
+      <c r="P298" s="8"/>
+      <c r="Q298" s="8"/>
+      <c r="R298" s="8"/>
+      <c r="S298" s="8"/>
+      <c r="T298" s="14"/>
       <c r="U298">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A299" s="29"/>
+      <c r="A299" s="23"/>
       <c r="B299" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -9253,10 +9253,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A300" s="29"/>
-      <c r="B300" s="2">
-        <v>7170</v>
+    <row r="300" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A300" s="23"/>
+      <c r="B300" s="12">
+        <v>7546</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9282,9 +9282,9 @@
       </c>
     </row>
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="29"/>
+      <c r="A301" s="23"/>
       <c r="B301" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9310,9 +9310,9 @@
       </c>
     </row>
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A302" s="29"/>
+      <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9338,9 +9338,9 @@
       </c>
     </row>
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A303" s="29"/>
+      <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9366,9 +9366,9 @@
       </c>
     </row>
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A304" s="29"/>
+      <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9394,9 +9394,9 @@
       </c>
     </row>
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A305" s="29"/>
+      <c r="A305" s="23"/>
       <c r="B305" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9422,9 +9422,9 @@
       </c>
     </row>
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A306" s="29"/>
+      <c r="A306" s="23"/>
       <c r="B306" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -9450,9 +9450,9 @@
       </c>
     </row>
     <row r="307" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A307" s="29"/>
+      <c r="A307" s="23"/>
       <c r="B307" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
@@ -9478,9 +9478,9 @@
       </c>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A308" s="29"/>
+      <c r="A308" s="23"/>
       <c r="B308" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -9506,9 +9506,9 @@
       </c>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A309" s="29"/>
+      <c r="A309" s="23"/>
       <c r="B309" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9534,9 +9534,9 @@
       </c>
     </row>
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A310" s="29"/>
+      <c r="A310" s="23"/>
       <c r="B310" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9562,9 +9562,9 @@
       </c>
     </row>
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A311" s="29"/>
+      <c r="A311" s="23"/>
       <c r="B311" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9589,96 +9589,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312" s="30"/>
-      <c r="B312" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C312" s="6"/>
-      <c r="D312" s="6"/>
-      <c r="E312" s="6"/>
-      <c r="F312" s="6"/>
-      <c r="G312" s="6"/>
-      <c r="H312" s="6"/>
-      <c r="I312" s="6"/>
-      <c r="J312" s="6"/>
-      <c r="K312" s="6"/>
-      <c r="L312" s="6"/>
-      <c r="M312" s="6"/>
-      <c r="N312" s="6"/>
-      <c r="O312" s="6"/>
-      <c r="P312" s="6"/>
-      <c r="Q312" s="6"/>
-      <c r="R312" s="6"/>
-      <c r="S312" s="6"/>
-      <c r="T312" s="7"/>
+    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A312" s="23"/>
+      <c r="B312" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C312" s="2"/>
+      <c r="D312" s="2"/>
+      <c r="E312" s="2"/>
+      <c r="F312" s="2"/>
+      <c r="G312" s="2"/>
+      <c r="H312" s="2"/>
+      <c r="I312" s="2"/>
+      <c r="J312" s="2"/>
+      <c r="K312" s="2"/>
+      <c r="L312" s="2"/>
+      <c r="M312" s="2"/>
+      <c r="N312" s="2"/>
+      <c r="O312" s="2"/>
+      <c r="P312" s="2"/>
+      <c r="Q312" s="2"/>
+      <c r="R312" s="2"/>
+      <c r="S312" s="2"/>
+      <c r="T312" s="5"/>
       <c r="U312">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A313" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B313" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C313" s="8"/>
-      <c r="D313" s="8"/>
-      <c r="E313" s="8"/>
-      <c r="F313" s="8"/>
-      <c r="G313" s="8"/>
-      <c r="H313" s="8"/>
-      <c r="I313" s="8"/>
-      <c r="J313" s="8"/>
-      <c r="K313" s="8"/>
-      <c r="L313" s="8"/>
-      <c r="M313" s="8"/>
-      <c r="N313" s="8"/>
-      <c r="O313" s="8"/>
-      <c r="P313" s="8"/>
-      <c r="Q313" s="8"/>
-      <c r="R313" s="8"/>
-      <c r="S313" s="8"/>
-      <c r="T313" s="14"/>
+    <row r="313" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="24"/>
+      <c r="B313" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C313" s="6"/>
+      <c r="D313" s="6"/>
+      <c r="E313" s="6"/>
+      <c r="F313" s="6"/>
+      <c r="G313" s="6"/>
+      <c r="H313" s="6"/>
+      <c r="I313" s="6"/>
+      <c r="J313" s="6"/>
+      <c r="K313" s="6"/>
+      <c r="L313" s="6"/>
+      <c r="M313" s="6"/>
+      <c r="N313" s="6"/>
+      <c r="O313" s="6"/>
+      <c r="P313" s="6"/>
+      <c r="Q313" s="6"/>
+      <c r="R313" s="6"/>
+      <c r="S313" s="6"/>
+      <c r="T313" s="7"/>
       <c r="U313">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="29"/>
-      <c r="B314" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C314" s="2"/>
-      <c r="D314" s="2"/>
-      <c r="E314" s="2"/>
-      <c r="F314" s="2"/>
-      <c r="G314" s="2"/>
-      <c r="H314" s="2"/>
-      <c r="I314" s="2"/>
-      <c r="J314" s="2"/>
-      <c r="K314" s="2"/>
-      <c r="L314" s="2"/>
-      <c r="M314" s="2"/>
-      <c r="N314" s="2"/>
-      <c r="O314" s="2"/>
-      <c r="P314" s="2"/>
-      <c r="Q314" s="2"/>
-      <c r="R314" s="2"/>
-      <c r="S314" s="2"/>
-      <c r="T314" s="5"/>
+      <c r="A314" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B314" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C314" s="8"/>
+      <c r="D314" s="8"/>
+      <c r="E314" s="8"/>
+      <c r="F314" s="8"/>
+      <c r="G314" s="8"/>
+      <c r="H314" s="8"/>
+      <c r="I314" s="8"/>
+      <c r="J314" s="8"/>
+      <c r="K314" s="8"/>
+      <c r="L314" s="8"/>
+      <c r="M314" s="8"/>
+      <c r="N314" s="8"/>
+      <c r="O314" s="8"/>
+      <c r="P314" s="8"/>
+      <c r="Q314" s="8"/>
+      <c r="R314" s="8"/>
+      <c r="S314" s="8"/>
+      <c r="T314" s="14"/>
       <c r="U314">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="29"/>
+      <c r="A315" s="23"/>
       <c r="B315" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -9704,9 +9704,9 @@
       </c>
     </row>
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A316" s="29"/>
+      <c r="A316" s="23"/>
       <c r="B316" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9732,9 +9732,9 @@
       </c>
     </row>
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A317" s="29"/>
+      <c r="A317" s="23"/>
       <c r="B317" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -9759,96 +9759,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A318" s="30"/>
-      <c r="B318" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C318" s="6"/>
-      <c r="D318" s="6"/>
-      <c r="E318" s="6"/>
-      <c r="F318" s="6"/>
-      <c r="G318" s="6"/>
-      <c r="H318" s="6"/>
-      <c r="I318" s="6"/>
-      <c r="J318" s="6"/>
-      <c r="K318" s="6"/>
-      <c r="L318" s="6"/>
-      <c r="M318" s="6"/>
-      <c r="N318" s="6"/>
-      <c r="O318" s="6"/>
-      <c r="P318" s="6"/>
-      <c r="Q318" s="6"/>
-      <c r="R318" s="6"/>
-      <c r="S318" s="6"/>
-      <c r="T318" s="7"/>
+    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A318" s="23"/>
+      <c r="B318" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C318" s="2"/>
+      <c r="D318" s="2"/>
+      <c r="E318" s="2"/>
+      <c r="F318" s="2"/>
+      <c r="G318" s="2"/>
+      <c r="H318" s="2"/>
+      <c r="I318" s="2"/>
+      <c r="J318" s="2"/>
+      <c r="K318" s="2"/>
+      <c r="L318" s="2"/>
+      <c r="M318" s="2"/>
+      <c r="N318" s="2"/>
+      <c r="O318" s="2"/>
+      <c r="P318" s="2"/>
+      <c r="Q318" s="2"/>
+      <c r="R318" s="2"/>
+      <c r="S318" s="2"/>
+      <c r="T318" s="5"/>
       <c r="U318">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A319" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B319" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C319" s="8"/>
-      <c r="D319" s="8"/>
-      <c r="E319" s="8"/>
-      <c r="F319" s="8"/>
-      <c r="G319" s="8"/>
-      <c r="H319" s="8"/>
-      <c r="I319" s="8"/>
-      <c r="J319" s="8"/>
-      <c r="K319" s="8"/>
-      <c r="L319" s="8"/>
-      <c r="M319" s="8"/>
-      <c r="N319" s="8"/>
-      <c r="O319" s="8"/>
-      <c r="P319" s="8"/>
-      <c r="Q319" s="8"/>
-      <c r="R319" s="8"/>
-      <c r="S319" s="8"/>
-      <c r="T319" s="14"/>
+    <row r="319" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="24"/>
+      <c r="B319" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C319" s="6"/>
+      <c r="D319" s="6"/>
+      <c r="E319" s="6"/>
+      <c r="F319" s="6"/>
+      <c r="G319" s="6"/>
+      <c r="H319" s="6"/>
+      <c r="I319" s="6"/>
+      <c r="J319" s="6"/>
+      <c r="K319" s="6"/>
+      <c r="L319" s="6"/>
+      <c r="M319" s="6"/>
+      <c r="N319" s="6"/>
+      <c r="O319" s="6"/>
+      <c r="P319" s="6"/>
+      <c r="Q319" s="6"/>
+      <c r="R319" s="6"/>
+      <c r="S319" s="6"/>
+      <c r="T319" s="7"/>
       <c r="U319">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A320" s="29"/>
-      <c r="B320" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C320" s="2"/>
-      <c r="D320" s="2"/>
-      <c r="E320" s="2"/>
-      <c r="F320" s="2"/>
-      <c r="G320" s="2"/>
-      <c r="H320" s="2"/>
-      <c r="I320" s="2"/>
-      <c r="J320" s="2"/>
-      <c r="K320" s="2"/>
-      <c r="L320" s="2"/>
-      <c r="M320" s="2"/>
-      <c r="N320" s="2"/>
-      <c r="O320" s="2"/>
-      <c r="P320" s="2"/>
-      <c r="Q320" s="2"/>
-      <c r="R320" s="2"/>
-      <c r="S320" s="2"/>
-      <c r="T320" s="5"/>
+      <c r="A320" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B320" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C320" s="8"/>
+      <c r="D320" s="8"/>
+      <c r="E320" s="8"/>
+      <c r="F320" s="8"/>
+      <c r="G320" s="8"/>
+      <c r="H320" s="8"/>
+      <c r="I320" s="8"/>
+      <c r="J320" s="8"/>
+      <c r="K320" s="8"/>
+      <c r="L320" s="8"/>
+      <c r="M320" s="8"/>
+      <c r="N320" s="8"/>
+      <c r="O320" s="8"/>
+      <c r="P320" s="8"/>
+      <c r="Q320" s="8"/>
+      <c r="R320" s="8"/>
+      <c r="S320" s="8"/>
+      <c r="T320" s="14"/>
       <c r="U320">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A321" s="29"/>
+      <c r="A321" s="23"/>
       <c r="B321" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
@@ -9874,9 +9874,9 @@
       </c>
     </row>
     <row r="322" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A322" s="29"/>
+      <c r="A322" s="23"/>
       <c r="B322" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
@@ -9902,9 +9902,9 @@
       </c>
     </row>
     <row r="323" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A323" s="29"/>
+      <c r="A323" s="23"/>
       <c r="B323" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
@@ -9929,35 +9929,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A324" s="30"/>
-      <c r="B324" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C324" s="6"/>
-      <c r="D324" s="6"/>
-      <c r="E324" s="6"/>
-      <c r="F324" s="6"/>
-      <c r="G324" s="6"/>
-      <c r="H324" s="6"/>
-      <c r="I324" s="6"/>
-      <c r="J324" s="6"/>
-      <c r="K324" s="6"/>
-      <c r="L324" s="6"/>
-      <c r="M324" s="6"/>
-      <c r="N324" s="6"/>
-      <c r="O324" s="6"/>
-      <c r="P324" s="6"/>
-      <c r="Q324" s="6"/>
-      <c r="R324" s="6"/>
-      <c r="S324" s="6"/>
-      <c r="T324" s="7"/>
+    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A324" s="23"/>
+      <c r="B324" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C324" s="2"/>
+      <c r="D324" s="2"/>
+      <c r="E324" s="2"/>
+      <c r="F324" s="2"/>
+      <c r="G324" s="2"/>
+      <c r="H324" s="2"/>
+      <c r="I324" s="2"/>
+      <c r="J324" s="2"/>
+      <c r="K324" s="2"/>
+      <c r="L324" s="2"/>
+      <c r="M324" s="2"/>
+      <c r="N324" s="2"/>
+      <c r="O324" s="2"/>
+      <c r="P324" s="2"/>
+      <c r="Q324" s="2"/>
+      <c r="R324" s="2"/>
+      <c r="S324" s="2"/>
+      <c r="T324" s="5"/>
       <c r="U324">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A325" s="24"/>
+      <c r="B325" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
+      <c r="E325" s="6"/>
+      <c r="F325" s="6"/>
+      <c r="G325" s="6"/>
+      <c r="H325" s="6"/>
+      <c r="I325" s="6"/>
+      <c r="J325" s="6"/>
+      <c r="K325" s="6"/>
+      <c r="L325" s="6"/>
+      <c r="M325" s="6"/>
+      <c r="N325" s="6"/>
+      <c r="O325" s="6"/>
+      <c r="P325" s="6"/>
+      <c r="Q325" s="6"/>
+      <c r="R325" s="6"/>
+      <c r="S325" s="6"/>
+      <c r="T325" s="7"/>
       <c r="U325">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -10139,13 +10161,13 @@
     </row>
     <row r="355" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U355">
-        <f t="shared" ref="U355:U418" ca="1" si="8">IF(B355=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="356" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U356">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U356:U419" ca="1" si="8">IF(B356=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10523,13 +10545,13 @@
     </row>
     <row r="419" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U419">
-        <f t="shared" ref="U419:U482" ca="1" si="9">IF(B419=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="420" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U420">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U420:U483" ca="1" si="9">IF(B420=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10907,13 +10929,13 @@
     </row>
     <row r="483" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U483">
-        <f t="shared" ref="U483:U546" ca="1" si="10">IF(B483=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="484" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U484">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U484:U547" ca="1" si="10">IF(B484=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11291,13 +11313,13 @@
     </row>
     <row r="547" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U547">
-        <f t="shared" ref="U547:U610" ca="1" si="11">IF(B547=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="548" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U548">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U548:U611" ca="1" si="11">IF(B548=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11675,13 +11697,13 @@
     </row>
     <row r="611" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U611">
-        <f t="shared" ref="U611:U674" ca="1" si="12">IF(B611=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="612" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U612">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U612:U675" ca="1" si="12">IF(B612=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12059,13 +12081,13 @@
     </row>
     <row r="675" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U675">
-        <f t="shared" ref="U675:U738" ca="1" si="13">IF(B675=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="676" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U676">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U676:U739" ca="1" si="13">IF(B676=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12443,13 +12465,13 @@
     </row>
     <row r="739" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U739">
-        <f t="shared" ref="U739:U802" ca="1" si="14">IF(B739=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="740" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U740">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U740:U803" ca="1" si="14">IF(B740=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12827,13 +12849,13 @@
     </row>
     <row r="803" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U803">
-        <f t="shared" ref="U803:U866" ca="1" si="15">IF(B803=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="804" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U804">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U804:U867" ca="1" si="15">IF(B804=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13211,13 +13233,13 @@
     </row>
     <row r="867" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U867">
-        <f t="shared" ref="U867:U928" ca="1" si="16">IF(B867=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="868" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U868">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U868:U929" ca="1" si="16">IF(B868=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13581,26 +13603,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="929" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U929">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A233:A240"/>
-    <mergeCell ref="A241:A248"/>
+    <mergeCell ref="A320:A325"/>
+    <mergeCell ref="A250:A279"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A298:A313"/>
+    <mergeCell ref="A314:A319"/>
+    <mergeCell ref="A64:A104"/>
+    <mergeCell ref="A222:A233"/>
+    <mergeCell ref="A150:A185"/>
+    <mergeCell ref="A186:A204"/>
+    <mergeCell ref="A105:A149"/>
+    <mergeCell ref="A19:A63"/>
+    <mergeCell ref="A205:A221"/>
+    <mergeCell ref="A234:A241"/>
+    <mergeCell ref="A242:A249"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A292:A296"/>
-    <mergeCell ref="A279:A291"/>
-    <mergeCell ref="A319:A324"/>
-    <mergeCell ref="A249:A278"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A297:A312"/>
-    <mergeCell ref="A313:A318"/>
-    <mergeCell ref="A64:A104"/>
-    <mergeCell ref="A221:A232"/>
-    <mergeCell ref="A150:A185"/>
-    <mergeCell ref="A186:A203"/>
-    <mergeCell ref="A105:A149"/>
-    <mergeCell ref="A19:A63"/>
-    <mergeCell ref="A204:A220"/>
+    <mergeCell ref="A293:A297"/>
+    <mergeCell ref="A280:A292"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task for arrays
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$297</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$298</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -530,6 +530,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,24 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W929"/>
+  <dimension ref="A1:W930"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,56 +891,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>6739</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="33"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -970,7 +970,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="9">
         <v>7474</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="9">
         <v>4343</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="13">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="12">
         <v>3730</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="12">
         <v>9007</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="12">
         <v>9578</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="20">
         <v>3862</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="20">
         <v>9231</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="2">
         <v>4411</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="2">
         <v>3832</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="2">
         <v>7457</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="2">
         <v>9865</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="2">
         <v>8428</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2">
         <v>7711</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="2">
         <v>1262</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="2">
         <v>9164</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="2">
         <v>3558</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2">
         <v>9298</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="2">
         <v>4312</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="2">
         <v>3354</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="2">
         <v>5201</v>
       </c>
@@ -1898,7 +1898,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="2">
         <v>2981</v>
       </c>
@@ -1926,7 +1926,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="2">
         <v>8833</v>
       </c>
@@ -1954,7 +1954,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="2">
         <v>9020</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="2">
         <v>1934</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="2">
         <v>3943</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="2">
         <v>2361</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="2">
         <v>5063</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="2">
         <v>5870</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="2">
         <v>8237</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="2">
         <v>7619</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="2">
         <v>1346</v>
       </c>
@@ -2206,7 +2206,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="2">
         <v>9622</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="2">
         <v>8873</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="2">
         <v>7799</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="2">
         <v>9354</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="2">
         <v>9130</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="2">
         <v>5895</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="2">
         <v>2461</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="2">
         <v>2790</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="2">
         <v>2624</v>
       </c>
@@ -2458,7 +2458,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="2">
         <v>5871</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="2">
         <v>3591</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="2">
         <v>4366</v>
       </c>
@@ -2542,7 +2542,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="2">
         <v>5789</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="9">
         <v>6522</v>
       </c>
@@ -2598,7 +2598,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="36"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="6">
         <v>3490</v>
       </c>
@@ -4781,7 +4781,7 @@
       <c r="S140" s="2"/>
       <c r="T140" s="5"/>
       <c r="U140">
-        <f t="shared" ref="U140:U211" ca="1" si="4">IF(B140=$W$1,1,0)</f>
+        <f t="shared" ref="U140:U212" ca="1" si="4">IF(B140=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5546,7 +5546,7 @@
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="23"/>
       <c r="B168" s="2">
-        <v>5894</v>
+        <v>2173</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -5574,7 +5574,7 @@
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="23"/>
       <c r="B169" s="2">
-        <v>4515</v>
+        <v>5894</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -5602,7 +5602,7 @@
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="23"/>
       <c r="B170" s="2">
-        <v>9774</v>
+        <v>4515</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -5630,7 +5630,7 @@
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="23"/>
       <c r="B171" s="2">
-        <v>3946</v>
+        <v>9774</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -5658,7 +5658,7 @@
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="23"/>
       <c r="B172" s="2">
-        <v>6497</v>
+        <v>3946</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -5686,7 +5686,7 @@
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="23"/>
       <c r="B173" s="2">
-        <v>5648</v>
+        <v>6497</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -5714,7 +5714,7 @@
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="23"/>
       <c r="B174" s="2">
-        <v>3940</v>
+        <v>5648</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -5742,7 +5742,7 @@
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="23"/>
       <c r="B175" s="2">
-        <v>7290</v>
+        <v>3940</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -5770,7 +5770,7 @@
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="23"/>
       <c r="B176" s="2">
-        <v>7035</v>
+        <v>7290</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
@@ -5798,7 +5798,7 @@
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="23"/>
       <c r="B177" s="2">
-        <v>9271</v>
+        <v>7035</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
@@ -5826,7 +5826,7 @@
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="23"/>
       <c r="B178" s="2">
-        <v>8769</v>
+        <v>9271</v>
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
@@ -5854,7 +5854,7 @@
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="23"/>
       <c r="B179" s="2">
-        <v>4497</v>
+        <v>8769</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
@@ -5882,7 +5882,7 @@
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="23"/>
       <c r="B180" s="2">
-        <v>3218</v>
+        <v>4497</v>
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
@@ -5910,7 +5910,7 @@
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="23"/>
       <c r="B181" s="2">
-        <v>6492</v>
+        <v>3218</v>
       </c>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
@@ -5938,7 +5938,7 @@
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="23"/>
       <c r="B182" s="2">
-        <v>4293</v>
+        <v>6492</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
@@ -5966,7 +5966,7 @@
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="23"/>
       <c r="B183" s="2">
-        <v>7703</v>
+        <v>4293</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
@@ -5994,7 +5994,7 @@
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="23"/>
       <c r="B184" s="2">
-        <v>5541</v>
+        <v>7703</v>
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
@@ -6019,96 +6019,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="24"/>
-      <c r="B185" s="6">
-        <v>9182</v>
-      </c>
-      <c r="C185" s="6"/>
-      <c r="D185" s="6"/>
-      <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
-      <c r="G185" s="6"/>
-      <c r="H185" s="6"/>
-      <c r="I185" s="6"/>
-      <c r="J185" s="6"/>
-      <c r="K185" s="6"/>
-      <c r="L185" s="6"/>
-      <c r="M185" s="6"/>
-      <c r="N185" s="6"/>
-      <c r="O185" s="6"/>
-      <c r="P185" s="6"/>
-      <c r="Q185" s="6"/>
-      <c r="R185" s="6"/>
-      <c r="S185" s="6"/>
-      <c r="T185" s="7"/>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A185" s="23"/>
+      <c r="B185" s="2">
+        <v>5541</v>
+      </c>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+      <c r="L185" s="2"/>
+      <c r="M185" s="2"/>
+      <c r="N185" s="2"/>
+      <c r="O185" s="2"/>
+      <c r="P185" s="2"/>
+      <c r="Q185" s="2"/>
+      <c r="R185" s="2"/>
+      <c r="S185" s="2"/>
+      <c r="T185" s="5"/>
       <c r="U185">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="22" t="s">
+    <row r="186" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="24"/>
+      <c r="B186" s="6">
+        <v>9182</v>
+      </c>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+      <c r="J186" s="6"/>
+      <c r="K186" s="6"/>
+      <c r="L186" s="6"/>
+      <c r="M186" s="6"/>
+      <c r="N186" s="6"/>
+      <c r="O186" s="6"/>
+      <c r="P186" s="6"/>
+      <c r="Q186" s="6"/>
+      <c r="R186" s="6"/>
+      <c r="S186" s="6"/>
+      <c r="T186" s="7"/>
+      <c r="U186">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A187" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B186" s="13">
+      <c r="B187" s="13">
         <v>8165</v>
       </c>
-      <c r="C186" s="8"/>
-      <c r="D186" s="8"/>
-      <c r="E186" s="8"/>
-      <c r="F186" s="8"/>
-      <c r="G186" s="8"/>
-      <c r="H186" s="8"/>
-      <c r="I186" s="8"/>
-      <c r="J186" s="8"/>
-      <c r="K186" s="8"/>
-      <c r="L186" s="8"/>
-      <c r="M186" s="8"/>
-      <c r="N186" s="8"/>
-      <c r="O186" s="8"/>
-      <c r="P186" s="8"/>
-      <c r="Q186" s="8"/>
-      <c r="R186" s="8"/>
-      <c r="S186" s="8"/>
-      <c r="T186" s="14"/>
-      <c r="U186">
-        <f t="shared" ref="U186:U204" ca="1" si="5">IF(B186=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="23"/>
-      <c r="B187" s="12">
+      <c r="C187" s="8"/>
+      <c r="D187" s="8"/>
+      <c r="E187" s="8"/>
+      <c r="F187" s="8"/>
+      <c r="G187" s="8"/>
+      <c r="H187" s="8"/>
+      <c r="I187" s="8"/>
+      <c r="J187" s="8"/>
+      <c r="K187" s="8"/>
+      <c r="L187" s="8"/>
+      <c r="M187" s="8"/>
+      <c r="N187" s="8"/>
+      <c r="O187" s="8"/>
+      <c r="P187" s="8"/>
+      <c r="Q187" s="8"/>
+      <c r="R187" s="8"/>
+      <c r="S187" s="8"/>
+      <c r="T187" s="14"/>
+      <c r="U187">
+        <f t="shared" ref="U187:U205" ca="1" si="5">IF(B187=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A188" s="23"/>
+      <c r="B188" s="12">
         <v>9001</v>
-      </c>
-      <c r="C187" s="2"/>
-      <c r="D187" s="2"/>
-      <c r="E187" s="2"/>
-      <c r="F187" s="2"/>
-      <c r="G187" s="2"/>
-      <c r="H187" s="2"/>
-      <c r="I187" s="2"/>
-      <c r="J187" s="2"/>
-      <c r="K187" s="2"/>
-      <c r="L187" s="2"/>
-      <c r="M187" s="2"/>
-      <c r="N187" s="2"/>
-      <c r="O187" s="2"/>
-      <c r="P187" s="2"/>
-      <c r="Q187" s="2"/>
-      <c r="R187" s="2"/>
-      <c r="S187" s="2"/>
-      <c r="T187" s="5"/>
-      <c r="U187">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="23"/>
-      <c r="B188" s="2">
-        <v>7491</v>
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -6136,7 +6136,7 @@
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="23"/>
       <c r="B189" s="2">
-        <v>9531</v>
+        <v>7491</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
@@ -6164,7 +6164,7 @@
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="23"/>
       <c r="B190" s="2">
-        <v>9812</v>
+        <v>9531</v>
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
@@ -6192,7 +6192,7 @@
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="23"/>
       <c r="B191" s="2">
-        <v>9279</v>
+        <v>9812</v>
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
@@ -6220,7 +6220,7 @@
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="23"/>
       <c r="B192" s="2">
-        <v>4845</v>
+        <v>9279</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -6248,7 +6248,7 @@
     <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="23"/>
       <c r="B193" s="2">
-        <v>5728</v>
+        <v>4845</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -6276,7 +6276,7 @@
     <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="23"/>
       <c r="B194" s="2">
-        <v>7222</v>
+        <v>5728</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
@@ -6304,7 +6304,7 @@
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="23"/>
       <c r="B195" s="2">
-        <v>5923</v>
+        <v>7222</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
@@ -6332,7 +6332,7 @@
     <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196" s="23"/>
       <c r="B196" s="2">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
@@ -6360,7 +6360,7 @@
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" s="23"/>
       <c r="B197" s="2">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -6388,7 +6388,7 @@
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" s="23"/>
       <c r="B198" s="2">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
@@ -6416,7 +6416,7 @@
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199" s="23"/>
       <c r="B199" s="2">
-        <v>9925</v>
+        <v>9116</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
@@ -6444,7 +6444,7 @@
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200" s="23"/>
       <c r="B200" s="2">
-        <v>3657</v>
+        <v>9925</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
@@ -6472,7 +6472,7 @@
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A201" s="23"/>
       <c r="B201" s="2">
-        <v>6599</v>
+        <v>3657</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
@@ -6498,37 +6498,37 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="31"/>
-      <c r="B202" s="9">
-        <v>1618</v>
-      </c>
-      <c r="C202" s="9"/>
-      <c r="D202" s="9"/>
-      <c r="E202" s="9"/>
-      <c r="F202" s="9"/>
-      <c r="G202" s="9"/>
-      <c r="H202" s="9"/>
-      <c r="I202" s="9"/>
-      <c r="J202" s="9"/>
-      <c r="K202" s="9"/>
-      <c r="L202" s="9"/>
-      <c r="M202" s="9"/>
-      <c r="N202" s="9"/>
-      <c r="O202" s="9"/>
-      <c r="P202" s="9"/>
-      <c r="Q202" s="9"/>
-      <c r="R202" s="9"/>
-      <c r="S202" s="9"/>
-      <c r="T202" s="15"/>
+      <c r="A202" s="23"/>
+      <c r="B202" s="2">
+        <v>6599</v>
+      </c>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2"/>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
+      <c r="O202" s="2"/>
+      <c r="P202" s="2"/>
+      <c r="Q202" s="2"/>
+      <c r="R202" s="2"/>
+      <c r="S202" s="2"/>
+      <c r="T202" s="5"/>
       <c r="U202">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="31"/>
+      <c r="A203" s="27"/>
       <c r="B203" s="9">
-        <v>1703</v>
+        <v>1618</v>
       </c>
       <c r="C203" s="9"/>
       <c r="D203" s="9"/>
@@ -6553,96 +6553,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="24"/>
-      <c r="B204" s="6">
-        <v>8887</v>
-      </c>
-      <c r="C204" s="6"/>
-      <c r="D204" s="6"/>
-      <c r="E204" s="6"/>
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="6"/>
-      <c r="J204" s="6"/>
-      <c r="K204" s="6"/>
-      <c r="L204" s="6"/>
-      <c r="M204" s="6"/>
-      <c r="N204" s="6"/>
-      <c r="O204" s="6"/>
-      <c r="P204" s="6"/>
-      <c r="Q204" s="6"/>
-      <c r="R204" s="6"/>
-      <c r="S204" s="6"/>
-      <c r="T204" s="7"/>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A204" s="27"/>
+      <c r="B204" s="9">
+        <v>1703</v>
+      </c>
+      <c r="C204" s="9"/>
+      <c r="D204" s="9"/>
+      <c r="E204" s="9"/>
+      <c r="F204" s="9"/>
+      <c r="G204" s="9"/>
+      <c r="H204" s="9"/>
+      <c r="I204" s="9"/>
+      <c r="J204" s="9"/>
+      <c r="K204" s="9"/>
+      <c r="L204" s="9"/>
+      <c r="M204" s="9"/>
+      <c r="N204" s="9"/>
+      <c r="O204" s="9"/>
+      <c r="P204" s="9"/>
+      <c r="Q204" s="9"/>
+      <c r="R204" s="9"/>
+      <c r="S204" s="9"/>
+      <c r="T204" s="15"/>
       <c r="U204">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="34" t="s">
+    <row r="205" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="24"/>
+      <c r="B205" s="6">
+        <v>8887</v>
+      </c>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
+      <c r="E205" s="6"/>
+      <c r="F205" s="6"/>
+      <c r="G205" s="6"/>
+      <c r="H205" s="6"/>
+      <c r="I205" s="6"/>
+      <c r="J205" s="6"/>
+      <c r="K205" s="6"/>
+      <c r="L205" s="6"/>
+      <c r="M205" s="6"/>
+      <c r="N205" s="6"/>
+      <c r="O205" s="6"/>
+      <c r="P205" s="6"/>
+      <c r="Q205" s="6"/>
+      <c r="R205" s="6"/>
+      <c r="S205" s="6"/>
+      <c r="T205" s="7"/>
+      <c r="U205">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A206" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B205" s="8">
+      <c r="B206" s="8">
         <v>6175</v>
       </c>
-      <c r="C205" s="8"/>
-      <c r="D205" s="8"/>
-      <c r="E205" s="8"/>
-      <c r="F205" s="8"/>
-      <c r="G205" s="8"/>
-      <c r="H205" s="8"/>
-      <c r="I205" s="8"/>
-      <c r="J205" s="8"/>
-      <c r="K205" s="8"/>
-      <c r="L205" s="8"/>
-      <c r="M205" s="8"/>
-      <c r="N205" s="8"/>
-      <c r="O205" s="8"/>
-      <c r="P205" s="8"/>
-      <c r="Q205" s="8"/>
-      <c r="R205" s="8"/>
-      <c r="S205" s="8"/>
-      <c r="T205" s="14"/>
-      <c r="U205">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="35"/>
-      <c r="B206" s="2">
-        <v>4488</v>
-      </c>
-      <c r="C206" s="2"/>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2"/>
-      <c r="F206" s="2"/>
-      <c r="G206" s="2"/>
-      <c r="H206" s="2"/>
-      <c r="I206" s="2"/>
-      <c r="J206" s="2"/>
-      <c r="K206" s="2"/>
-      <c r="L206" s="2"/>
-      <c r="M206" s="2"/>
-      <c r="N206" s="2"/>
-      <c r="O206" s="2"/>
-      <c r="P206" s="2"/>
-      <c r="Q206" s="2"/>
-      <c r="R206" s="2"/>
-      <c r="S206" s="2"/>
-      <c r="T206" s="5"/>
+      <c r="C206" s="8"/>
+      <c r="D206" s="8"/>
+      <c r="E206" s="8"/>
+      <c r="F206" s="8"/>
+      <c r="G206" s="8"/>
+      <c r="H206" s="8"/>
+      <c r="I206" s="8"/>
+      <c r="J206" s="8"/>
+      <c r="K206" s="8"/>
+      <c r="L206" s="8"/>
+      <c r="M206" s="8"/>
+      <c r="N206" s="8"/>
+      <c r="O206" s="8"/>
+      <c r="P206" s="8"/>
+      <c r="Q206" s="8"/>
+      <c r="R206" s="8"/>
+      <c r="S206" s="8"/>
+      <c r="T206" s="14"/>
       <c r="U206">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="35"/>
+      <c r="A207" s="29"/>
       <c r="B207" s="2">
-        <v>4954</v>
+        <v>4488</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6668,9 +6668,9 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="35"/>
+      <c r="A208" s="29"/>
       <c r="B208" s="2">
-        <v>4642</v>
+        <v>4954</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6696,9 +6696,9 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="35"/>
+      <c r="A209" s="29"/>
       <c r="B209" s="2">
-        <v>5537</v>
+        <v>4642</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6724,9 +6724,9 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="35"/>
+      <c r="A210" s="29"/>
       <c r="B210" s="2">
-        <v>5847</v>
+        <v>5537</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -6752,9 +6752,9 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A211" s="35"/>
+      <c r="A211" s="29"/>
       <c r="B211" s="2">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -6780,9 +6780,9 @@
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A212" s="35"/>
+      <c r="A212" s="29"/>
       <c r="B212" s="2">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -6803,14 +6803,14 @@
       <c r="S212" s="2"/>
       <c r="T212" s="5"/>
       <c r="U212">
-        <f t="shared" ref="U212:U291" ca="1" si="6">IF(B212=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="35"/>
+      <c r="A213" s="29"/>
       <c r="B213" s="2">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -6831,14 +6831,14 @@
       <c r="S213" s="2"/>
       <c r="T213" s="5"/>
       <c r="U213">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="U213:U292" ca="1" si="6">IF(B213=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="35"/>
+      <c r="A214" s="29"/>
       <c r="B214" s="2">
-        <v>3226</v>
+        <v>6861</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -6864,9 +6864,9 @@
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A215" s="35"/>
+      <c r="A215" s="29"/>
       <c r="B215" s="2">
-        <v>4372</v>
+        <v>3226</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -6892,9 +6892,9 @@
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A216" s="35"/>
+      <c r="A216" s="29"/>
       <c r="B216" s="2">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -6920,9 +6920,9 @@
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A217" s="35"/>
+      <c r="A217" s="29"/>
       <c r="B217" s="2">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6948,9 +6948,9 @@
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A218" s="35"/>
+      <c r="A218" s="29"/>
       <c r="B218" s="2">
-        <v>9417</v>
+        <v>1668</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6976,9 +6976,9 @@
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A219" s="35"/>
+      <c r="A219" s="29"/>
       <c r="B219" s="2">
-        <v>3148</v>
+        <v>9417</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -7004,9 +7004,9 @@
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A220" s="35"/>
+      <c r="A220" s="29"/>
       <c r="B220" s="2">
-        <v>2137</v>
+        <v>3148</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -7031,87 +7031,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="36"/>
-      <c r="B221" s="6">
-        <v>5621</v>
-      </c>
-      <c r="C221" s="6"/>
-      <c r="D221" s="6"/>
-      <c r="E221" s="6"/>
-      <c r="F221" s="6"/>
-      <c r="G221" s="6"/>
-      <c r="H221" s="6"/>
-      <c r="I221" s="6"/>
-      <c r="J221" s="6"/>
-      <c r="K221" s="6"/>
-      <c r="L221" s="6"/>
-      <c r="M221" s="6"/>
-      <c r="N221" s="6"/>
-      <c r="O221" s="6"/>
-      <c r="P221" s="6"/>
-      <c r="Q221" s="6"/>
-      <c r="R221" s="6"/>
-      <c r="S221" s="6"/>
-      <c r="T221" s="7"/>
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A221" s="29"/>
+      <c r="B221" s="2">
+        <v>2137</v>
+      </c>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
+      <c r="E221" s="2"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="2"/>
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+      <c r="J221" s="2"/>
+      <c r="K221" s="2"/>
+      <c r="L221" s="2"/>
+      <c r="M221" s="2"/>
+      <c r="N221" s="2"/>
+      <c r="O221" s="2"/>
+      <c r="P221" s="2"/>
+      <c r="Q221" s="2"/>
+      <c r="R221" s="2"/>
+      <c r="S221" s="2"/>
+      <c r="T221" s="5"/>
       <c r="U221">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A222" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B222" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C222" s="8"/>
-      <c r="D222" s="8"/>
-      <c r="E222" s="8"/>
-      <c r="F222" s="8"/>
-      <c r="G222" s="8"/>
-      <c r="H222" s="8"/>
-      <c r="I222" s="8"/>
-      <c r="J222" s="8"/>
-      <c r="K222" s="8"/>
-      <c r="L222" s="8"/>
-      <c r="M222" s="8"/>
-      <c r="N222" s="8"/>
-      <c r="O222" s="8"/>
-      <c r="P222" s="8"/>
-      <c r="Q222" s="8"/>
-      <c r="R222" s="8"/>
-      <c r="S222" s="8"/>
-      <c r="T222" s="14"/>
+    <row r="222" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="30"/>
+      <c r="B222" s="6">
+        <v>5621</v>
+      </c>
+      <c r="C222" s="6"/>
+      <c r="D222" s="6"/>
+      <c r="E222" s="6"/>
+      <c r="F222" s="6"/>
+      <c r="G222" s="6"/>
+      <c r="H222" s="6"/>
+      <c r="I222" s="6"/>
+      <c r="J222" s="6"/>
+      <c r="K222" s="6"/>
+      <c r="L222" s="6"/>
+      <c r="M222" s="6"/>
+      <c r="N222" s="6"/>
+      <c r="O222" s="6"/>
+      <c r="P222" s="6"/>
+      <c r="Q222" s="6"/>
+      <c r="R222" s="6"/>
+      <c r="S222" s="6"/>
+      <c r="T222" s="7"/>
       <c r="U222">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A223" s="23"/>
-      <c r="B223" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C223" s="2"/>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
-      <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
-      <c r="I223" s="2"/>
-      <c r="J223" s="2"/>
-      <c r="K223" s="2"/>
-      <c r="L223" s="2"/>
-      <c r="M223" s="2"/>
-      <c r="N223" s="2"/>
-      <c r="O223" s="2"/>
-      <c r="P223" s="2"/>
-      <c r="Q223" s="2"/>
-      <c r="R223" s="2"/>
-      <c r="S223" s="2"/>
-      <c r="T223" s="5"/>
+      <c r="A223" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B223" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C223" s="8"/>
+      <c r="D223" s="8"/>
+      <c r="E223" s="8"/>
+      <c r="F223" s="8"/>
+      <c r="G223" s="8"/>
+      <c r="H223" s="8"/>
+      <c r="I223" s="8"/>
+      <c r="J223" s="8"/>
+      <c r="K223" s="8"/>
+      <c r="L223" s="8"/>
+      <c r="M223" s="8"/>
+      <c r="N223" s="8"/>
+      <c r="O223" s="8"/>
+      <c r="P223" s="8"/>
+      <c r="Q223" s="8"/>
+      <c r="R223" s="8"/>
+      <c r="S223" s="8"/>
+      <c r="T223" s="14"/>
       <c r="U223">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7120,7 +7120,7 @@
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="23"/>
       <c r="B224" s="2">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7148,7 +7148,7 @@
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="23"/>
       <c r="B225" s="2">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -7176,7 +7176,7 @@
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="23"/>
       <c r="B226" s="2">
-        <v>6409</v>
+        <v>7060</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
@@ -7204,7 +7204,7 @@
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="23"/>
       <c r="B227" s="2">
-        <v>2386</v>
+        <v>6409</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
@@ -7229,10 +7229,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="23"/>
-      <c r="B228" s="6">
-        <v>7372</v>
+      <c r="B228" s="2">
+        <v>2386</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -7252,11 +7252,15 @@
       <c r="R228" s="2"/>
       <c r="S228" s="2"/>
       <c r="T228" s="5"/>
-    </row>
-    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U228">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="23"/>
-      <c r="B229" s="2">
-        <v>9159</v>
+      <c r="B229" s="6">
+        <v>7372</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -7276,15 +7280,11 @@
       <c r="R229" s="2"/>
       <c r="S229" s="2"/>
       <c r="T229" s="5"/>
-      <c r="U229">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="23"/>
       <c r="B230" s="2">
-        <v>5309</v>
+        <v>9159</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
@@ -7312,7 +7312,7 @@
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="23"/>
       <c r="B231" s="2">
-        <v>3290</v>
+        <v>5309</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
@@ -7340,7 +7340,7 @@
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="23"/>
       <c r="B232" s="2">
-        <v>5345</v>
+        <v>3290</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -7365,87 +7365,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="24"/>
-      <c r="B233" s="6">
-        <v>6812</v>
-      </c>
-      <c r="C233" s="6"/>
-      <c r="D233" s="6"/>
-      <c r="E233" s="6"/>
-      <c r="F233" s="6"/>
-      <c r="G233" s="6"/>
-      <c r="H233" s="6"/>
-      <c r="I233" s="6"/>
-      <c r="J233" s="6"/>
-      <c r="K233" s="6"/>
-      <c r="L233" s="6"/>
-      <c r="M233" s="6"/>
-      <c r="N233" s="6"/>
-      <c r="O233" s="6"/>
-      <c r="P233" s="6"/>
-      <c r="Q233" s="6"/>
-      <c r="R233" s="6"/>
-      <c r="S233" s="6"/>
-      <c r="T233" s="7"/>
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A233" s="23"/>
+      <c r="B233" s="2">
+        <v>5345</v>
+      </c>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+      <c r="L233" s="2"/>
+      <c r="M233" s="2"/>
+      <c r="N233" s="2"/>
+      <c r="O233" s="2"/>
+      <c r="P233" s="2"/>
+      <c r="Q233" s="2"/>
+      <c r="R233" s="2"/>
+      <c r="S233" s="2"/>
+      <c r="T233" s="5"/>
       <c r="U233">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A234" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B234" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C234" s="8"/>
-      <c r="D234" s="8"/>
-      <c r="E234" s="8"/>
-      <c r="F234" s="8"/>
-      <c r="G234" s="8"/>
-      <c r="H234" s="8"/>
-      <c r="I234" s="8"/>
-      <c r="J234" s="8"/>
-      <c r="K234" s="8"/>
-      <c r="L234" s="8"/>
-      <c r="M234" s="8"/>
-      <c r="N234" s="8"/>
-      <c r="O234" s="8"/>
-      <c r="P234" s="8"/>
-      <c r="Q234" s="8"/>
-      <c r="R234" s="8"/>
-      <c r="S234" s="8"/>
-      <c r="T234" s="14"/>
+    <row r="234" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="24"/>
+      <c r="B234" s="6">
+        <v>6812</v>
+      </c>
+      <c r="C234" s="6"/>
+      <c r="D234" s="6"/>
+      <c r="E234" s="6"/>
+      <c r="F234" s="6"/>
+      <c r="G234" s="6"/>
+      <c r="H234" s="6"/>
+      <c r="I234" s="6"/>
+      <c r="J234" s="6"/>
+      <c r="K234" s="6"/>
+      <c r="L234" s="6"/>
+      <c r="M234" s="6"/>
+      <c r="N234" s="6"/>
+      <c r="O234" s="6"/>
+      <c r="P234" s="6"/>
+      <c r="Q234" s="6"/>
+      <c r="R234" s="6"/>
+      <c r="S234" s="6"/>
+      <c r="T234" s="7"/>
       <c r="U234">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="23"/>
-      <c r="B235" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C235" s="2"/>
-      <c r="D235" s="2"/>
-      <c r="E235" s="2"/>
-      <c r="F235" s="2"/>
-      <c r="G235" s="2"/>
-      <c r="H235" s="2"/>
-      <c r="I235" s="2"/>
-      <c r="J235" s="2"/>
-      <c r="K235" s="2"/>
-      <c r="L235" s="2"/>
-      <c r="M235" s="2"/>
-      <c r="N235" s="2"/>
-      <c r="O235" s="2"/>
-      <c r="P235" s="2"/>
-      <c r="Q235" s="2"/>
-      <c r="R235" s="2"/>
-      <c r="S235" s="2"/>
-      <c r="T235" s="5"/>
+      <c r="A235" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B235" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C235" s="8"/>
+      <c r="D235" s="8"/>
+      <c r="E235" s="8"/>
+      <c r="F235" s="8"/>
+      <c r="G235" s="8"/>
+      <c r="H235" s="8"/>
+      <c r="I235" s="8"/>
+      <c r="J235" s="8"/>
+      <c r="K235" s="8"/>
+      <c r="L235" s="8"/>
+      <c r="M235" s="8"/>
+      <c r="N235" s="8"/>
+      <c r="O235" s="8"/>
+      <c r="P235" s="8"/>
+      <c r="Q235" s="8"/>
+      <c r="R235" s="8"/>
+      <c r="S235" s="8"/>
+      <c r="T235" s="14"/>
       <c r="U235">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7454,7 +7454,7 @@
     <row r="236" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="23"/>
       <c r="B236" s="12">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
@@ -7479,10 +7479,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="23"/>
-      <c r="B237" s="19">
-        <v>8861</v>
+      <c r="B237" s="12">
+        <v>9062</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
@@ -7509,8 +7509,8 @@
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="23"/>
-      <c r="B238" s="2">
-        <v>5164</v>
+      <c r="B238" s="19">
+        <v>8861</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -7538,7 +7538,7 @@
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239" s="23"/>
       <c r="B239" s="2">
-        <v>2354</v>
+        <v>5164</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -7566,7 +7566,7 @@
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="23"/>
       <c r="B240" s="2">
-        <v>2030</v>
+        <v>2354</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
@@ -7591,87 +7591,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="24"/>
-      <c r="B241" s="6">
-        <v>7649</v>
-      </c>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="6"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="6"/>
-      <c r="J241" s="6"/>
-      <c r="K241" s="6"/>
-      <c r="L241" s="6"/>
-      <c r="M241" s="6"/>
-      <c r="N241" s="6"/>
-      <c r="O241" s="6"/>
-      <c r="P241" s="6"/>
-      <c r="Q241" s="6"/>
-      <c r="R241" s="6"/>
-      <c r="S241" s="6"/>
-      <c r="T241" s="7"/>
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A241" s="23"/>
+      <c r="B241" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="2"/>
+      <c r="N241" s="2"/>
+      <c r="O241" s="2"/>
+      <c r="P241" s="2"/>
+      <c r="Q241" s="2"/>
+      <c r="R241" s="2"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="5"/>
       <c r="U241">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A242" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8"/>
-      <c r="H242" s="8"/>
-      <c r="I242" s="8"/>
-      <c r="J242" s="8"/>
-      <c r="K242" s="8"/>
-      <c r="L242" s="8"/>
-      <c r="M242" s="8"/>
-      <c r="N242" s="8"/>
-      <c r="O242" s="8"/>
-      <c r="P242" s="8"/>
-      <c r="Q242" s="8"/>
-      <c r="R242" s="8"/>
-      <c r="S242" s="8"/>
-      <c r="T242" s="14"/>
+    <row r="242" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="24"/>
+      <c r="B242" s="6">
+        <v>7649</v>
+      </c>
+      <c r="C242" s="6"/>
+      <c r="D242" s="6"/>
+      <c r="E242" s="6"/>
+      <c r="F242" s="6"/>
+      <c r="G242" s="6"/>
+      <c r="H242" s="6"/>
+      <c r="I242" s="6"/>
+      <c r="J242" s="6"/>
+      <c r="K242" s="6"/>
+      <c r="L242" s="6"/>
+      <c r="M242" s="6"/>
+      <c r="N242" s="6"/>
+      <c r="O242" s="6"/>
+      <c r="P242" s="6"/>
+      <c r="Q242" s="6"/>
+      <c r="R242" s="6"/>
+      <c r="S242" s="6"/>
+      <c r="T242" s="7"/>
       <c r="U242">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A243" s="23"/>
-      <c r="B243" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
-      <c r="G243" s="2"/>
-      <c r="H243" s="2"/>
-      <c r="I243" s="2"/>
-      <c r="J243" s="2"/>
-      <c r="K243" s="2"/>
-      <c r="L243" s="2"/>
-      <c r="M243" s="2"/>
-      <c r="N243" s="2"/>
-      <c r="O243" s="2"/>
-      <c r="P243" s="2"/>
-      <c r="Q243" s="2"/>
-      <c r="R243" s="2"/>
-      <c r="S243" s="2"/>
-      <c r="T243" s="5"/>
+      <c r="A243" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B243" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C243" s="8"/>
+      <c r="D243" s="8"/>
+      <c r="E243" s="8"/>
+      <c r="F243" s="8"/>
+      <c r="G243" s="8"/>
+      <c r="H243" s="8"/>
+      <c r="I243" s="8"/>
+      <c r="J243" s="8"/>
+      <c r="K243" s="8"/>
+      <c r="L243" s="8"/>
+      <c r="M243" s="8"/>
+      <c r="N243" s="8"/>
+      <c r="O243" s="8"/>
+      <c r="P243" s="8"/>
+      <c r="Q243" s="8"/>
+      <c r="R243" s="8"/>
+      <c r="S243" s="8"/>
+      <c r="T243" s="14"/>
       <c r="U243">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7680,7 +7680,7 @@
     <row r="244" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A244" s="23"/>
       <c r="B244" s="2">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
@@ -7708,7 +7708,7 @@
     <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245" s="23"/>
       <c r="B245" s="2">
-        <v>6882</v>
+        <v>6732</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7736,7 +7736,7 @@
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246" s="23"/>
       <c r="B246" s="2">
-        <v>1212</v>
+        <v>6882</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7764,7 +7764,7 @@
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247" s="23"/>
       <c r="B247" s="2">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7792,7 +7792,7 @@
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="23"/>
       <c r="B248" s="2">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7817,87 +7817,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="24"/>
-      <c r="B249" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C249" s="6"/>
-      <c r="D249" s="6"/>
-      <c r="E249" s="6"/>
-      <c r="F249" s="6"/>
-      <c r="G249" s="6"/>
-      <c r="H249" s="6"/>
-      <c r="I249" s="6"/>
-      <c r="J249" s="6"/>
-      <c r="K249" s="6"/>
-      <c r="L249" s="6"/>
-      <c r="M249" s="6"/>
-      <c r="N249" s="6"/>
-      <c r="O249" s="6"/>
-      <c r="P249" s="6"/>
-      <c r="Q249" s="6"/>
-      <c r="R249" s="6"/>
-      <c r="S249" s="6"/>
-      <c r="T249" s="7"/>
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A249" s="23"/>
+      <c r="B249" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C249" s="2"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+      <c r="G249" s="2"/>
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+      <c r="L249" s="2"/>
+      <c r="M249" s="2"/>
+      <c r="N249" s="2"/>
+      <c r="O249" s="2"/>
+      <c r="P249" s="2"/>
+      <c r="Q249" s="2"/>
+      <c r="R249" s="2"/>
+      <c r="S249" s="2"/>
+      <c r="T249" s="5"/>
       <c r="U249">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A250" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B250" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C250" s="8"/>
-      <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
-      <c r="F250" s="8"/>
-      <c r="G250" s="8"/>
-      <c r="H250" s="8"/>
-      <c r="I250" s="8"/>
-      <c r="J250" s="8"/>
-      <c r="K250" s="8"/>
-      <c r="L250" s="8"/>
-      <c r="M250" s="8"/>
-      <c r="N250" s="8"/>
-      <c r="O250" s="8"/>
-      <c r="P250" s="8"/>
-      <c r="Q250" s="8"/>
-      <c r="R250" s="8"/>
-      <c r="S250" s="8"/>
-      <c r="T250" s="14"/>
+    <row r="250" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="24"/>
+      <c r="B250" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C250" s="6"/>
+      <c r="D250" s="6"/>
+      <c r="E250" s="6"/>
+      <c r="F250" s="6"/>
+      <c r="G250" s="6"/>
+      <c r="H250" s="6"/>
+      <c r="I250" s="6"/>
+      <c r="J250" s="6"/>
+      <c r="K250" s="6"/>
+      <c r="L250" s="6"/>
+      <c r="M250" s="6"/>
+      <c r="N250" s="6"/>
+      <c r="O250" s="6"/>
+      <c r="P250" s="6"/>
+      <c r="Q250" s="6"/>
+      <c r="R250" s="6"/>
+      <c r="S250" s="6"/>
+      <c r="T250" s="7"/>
       <c r="U250">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="23"/>
-      <c r="B251" s="2">
-        <v>6011</v>
-      </c>
-      <c r="C251" s="2"/>
-      <c r="D251" s="2"/>
-      <c r="E251" s="2"/>
-      <c r="F251" s="2"/>
-      <c r="G251" s="2"/>
-      <c r="H251" s="2"/>
-      <c r="I251" s="2"/>
-      <c r="J251" s="2"/>
-      <c r="K251" s="2"/>
-      <c r="L251" s="2"/>
-      <c r="M251" s="2"/>
-      <c r="N251" s="2"/>
-      <c r="O251" s="2"/>
-      <c r="P251" s="2"/>
-      <c r="Q251" s="2"/>
-      <c r="R251" s="2"/>
-      <c r="S251" s="2"/>
-      <c r="T251" s="5"/>
+    <row r="251" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A251" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B251" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C251" s="8"/>
+      <c r="D251" s="8"/>
+      <c r="E251" s="8"/>
+      <c r="F251" s="8"/>
+      <c r="G251" s="8"/>
+      <c r="H251" s="8"/>
+      <c r="I251" s="8"/>
+      <c r="J251" s="8"/>
+      <c r="K251" s="8"/>
+      <c r="L251" s="8"/>
+      <c r="M251" s="8"/>
+      <c r="N251" s="8"/>
+      <c r="O251" s="8"/>
+      <c r="P251" s="8"/>
+      <c r="Q251" s="8"/>
+      <c r="R251" s="8"/>
+      <c r="S251" s="8"/>
+      <c r="T251" s="14"/>
       <c r="U251">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -7906,7 +7906,7 @@
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" s="23"/>
       <c r="B252" s="2">
-        <v>8403</v>
+        <v>6011</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7934,7 +7934,7 @@
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="23"/>
       <c r="B253" s="2">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7961,8 +7961,8 @@
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="23"/>
-      <c r="B254" s="21">
-        <v>6037</v>
+      <c r="B254" s="2">
+        <v>3185</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7989,8 +7989,8 @@
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="23"/>
-      <c r="B255" s="2">
-        <v>9914</v>
+      <c r="B255" s="21">
+        <v>6037</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8018,7 +8018,7 @@
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="23"/>
       <c r="B256" s="2">
-        <v>4916</v>
+        <v>9914</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8046,7 +8046,7 @@
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="23"/>
       <c r="B257" s="2">
-        <v>2809</v>
+        <v>4916</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8074,7 +8074,7 @@
     <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="23"/>
       <c r="B258" s="2">
-        <v>8265</v>
+        <v>2809</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
@@ -8102,7 +8102,7 @@
     <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="23"/>
       <c r="B259" s="2">
-        <v>2092</v>
+        <v>8265</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -8130,7 +8130,7 @@
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" s="23"/>
       <c r="B260" s="2">
-        <v>7297</v>
+        <v>2092</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8158,7 +8158,7 @@
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="23"/>
       <c r="B261" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8186,7 +8186,7 @@
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="23"/>
       <c r="B262" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8214,7 +8214,7 @@
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="23"/>
       <c r="B263" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8242,7 +8242,7 @@
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8270,7 +8270,7 @@
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8298,7 +8298,7 @@
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8326,7 +8326,7 @@
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8354,7 +8354,7 @@
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8382,7 +8382,7 @@
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>9238</v>
+        <v>5449</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8410,7 +8410,7 @@
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>2662</v>
+        <v>9238</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8438,7 +8438,7 @@
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="23"/>
       <c r="B271" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8466,7 +8466,7 @@
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="23"/>
       <c r="B272" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8494,7 +8494,7 @@
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" s="23"/>
       <c r="B273" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8522,7 +8522,7 @@
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A274" s="23"/>
       <c r="B274" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8550,7 +8550,7 @@
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8578,7 +8578,7 @@
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A276" s="23"/>
       <c r="B276" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8606,7 +8606,7 @@
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" s="23"/>
       <c r="B277" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8634,7 +8634,7 @@
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="23"/>
       <c r="B278" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8659,87 +8659,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="24"/>
-      <c r="B279" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-      <c r="E279" s="6"/>
-      <c r="F279" s="6"/>
-      <c r="G279" s="6"/>
-      <c r="H279" s="6"/>
-      <c r="I279" s="6"/>
-      <c r="J279" s="6"/>
-      <c r="K279" s="6"/>
-      <c r="L279" s="6"/>
-      <c r="M279" s="6"/>
-      <c r="N279" s="6"/>
-      <c r="O279" s="6"/>
-      <c r="P279" s="6"/>
-      <c r="Q279" s="6"/>
-      <c r="R279" s="6"/>
-      <c r="S279" s="6"/>
-      <c r="T279" s="7"/>
+    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A279" s="23"/>
+      <c r="B279" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C279" s="2"/>
+      <c r="D279" s="2"/>
+      <c r="E279" s="2"/>
+      <c r="F279" s="2"/>
+      <c r="G279" s="2"/>
+      <c r="H279" s="2"/>
+      <c r="I279" s="2"/>
+      <c r="J279" s="2"/>
+      <c r="K279" s="2"/>
+      <c r="L279" s="2"/>
+      <c r="M279" s="2"/>
+      <c r="N279" s="2"/>
+      <c r="O279" s="2"/>
+      <c r="P279" s="2"/>
+      <c r="Q279" s="2"/>
+      <c r="R279" s="2"/>
+      <c r="S279" s="2"/>
+      <c r="T279" s="5"/>
       <c r="U279">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B280" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C280" s="8"/>
-      <c r="D280" s="8"/>
-      <c r="E280" s="8"/>
-      <c r="F280" s="8"/>
-      <c r="G280" s="8"/>
-      <c r="H280" s="8"/>
-      <c r="I280" s="8"/>
-      <c r="J280" s="8"/>
-      <c r="K280" s="8"/>
-      <c r="L280" s="8"/>
-      <c r="M280" s="8"/>
-      <c r="N280" s="8"/>
-      <c r="O280" s="8"/>
-      <c r="P280" s="8"/>
-      <c r="Q280" s="8"/>
-      <c r="R280" s="8"/>
-      <c r="S280" s="8"/>
-      <c r="T280" s="14"/>
+    <row r="280" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A280" s="24"/>
+      <c r="B280" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C280" s="6"/>
+      <c r="D280" s="6"/>
+      <c r="E280" s="6"/>
+      <c r="F280" s="6"/>
+      <c r="G280" s="6"/>
+      <c r="H280" s="6"/>
+      <c r="I280" s="6"/>
+      <c r="J280" s="6"/>
+      <c r="K280" s="6"/>
+      <c r="L280" s="6"/>
+      <c r="M280" s="6"/>
+      <c r="N280" s="6"/>
+      <c r="O280" s="6"/>
+      <c r="P280" s="6"/>
+      <c r="Q280" s="6"/>
+      <c r="R280" s="6"/>
+      <c r="S280" s="6"/>
+      <c r="T280" s="7"/>
       <c r="U280">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="23"/>
+      <c r="A281" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="B281" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="E281" s="2"/>
-      <c r="F281" s="2"/>
-      <c r="G281" s="2"/>
-      <c r="H281" s="2"/>
-      <c r="I281" s="2"/>
-      <c r="J281" s="2"/>
-      <c r="K281" s="2"/>
-      <c r="L281" s="2"/>
-      <c r="M281" s="2"/>
-      <c r="N281" s="2"/>
-      <c r="O281" s="2"/>
-      <c r="P281" s="2"/>
-      <c r="Q281" s="2"/>
-      <c r="R281" s="2"/>
-      <c r="S281" s="2"/>
-      <c r="T281" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C281" s="8"/>
+      <c r="D281" s="8"/>
+      <c r="E281" s="8"/>
+      <c r="F281" s="8"/>
+      <c r="G281" s="8"/>
+      <c r="H281" s="8"/>
+      <c r="I281" s="8"/>
+      <c r="J281" s="8"/>
+      <c r="K281" s="8"/>
+      <c r="L281" s="8"/>
+      <c r="M281" s="8"/>
+      <c r="N281" s="8"/>
+      <c r="O281" s="8"/>
+      <c r="P281" s="8"/>
+      <c r="Q281" s="8"/>
+      <c r="R281" s="8"/>
+      <c r="S281" s="8"/>
+      <c r="T281" s="14"/>
       <c r="U281">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -8748,7 +8748,7 @@
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="23"/>
       <c r="B282" s="2">
-        <v>9990</v>
+        <v>1056</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8776,7 +8776,7 @@
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" s="23"/>
       <c r="B283" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8804,7 +8804,7 @@
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" s="23"/>
       <c r="B284" s="2">
-        <v>8418</v>
+        <v>7738</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8832,7 +8832,7 @@
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A285" s="23"/>
       <c r="B285" s="2">
-        <v>9512</v>
+        <v>8418</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8860,7 +8860,7 @@
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A286" s="23"/>
       <c r="B286" s="2">
-        <v>9924</v>
+        <v>9512</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8886,37 +8886,37 @@
       </c>
     </row>
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="31"/>
-      <c r="B287" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C287" s="9"/>
-      <c r="D287" s="9"/>
-      <c r="E287" s="9"/>
-      <c r="F287" s="9"/>
-      <c r="G287" s="9"/>
-      <c r="H287" s="9"/>
-      <c r="I287" s="9"/>
-      <c r="J287" s="9"/>
-      <c r="K287" s="9"/>
-      <c r="L287" s="9"/>
-      <c r="M287" s="9"/>
-      <c r="N287" s="9"/>
-      <c r="O287" s="9"/>
-      <c r="P287" s="9"/>
-      <c r="Q287" s="9"/>
-      <c r="R287" s="9"/>
-      <c r="S287" s="9"/>
-      <c r="T287" s="15"/>
+      <c r="A287" s="23"/>
+      <c r="B287" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
+      <c r="E287" s="2"/>
+      <c r="F287" s="2"/>
+      <c r="G287" s="2"/>
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+      <c r="J287" s="2"/>
+      <c r="K287" s="2"/>
+      <c r="L287" s="2"/>
+      <c r="M287" s="2"/>
+      <c r="N287" s="2"/>
+      <c r="O287" s="2"/>
+      <c r="P287" s="2"/>
+      <c r="Q287" s="2"/>
+      <c r="R287" s="2"/>
+      <c r="S287" s="2"/>
+      <c r="T287" s="5"/>
       <c r="U287">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="31"/>
+      <c r="A288" s="27"/>
       <c r="B288" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C288" s="9"/>
       <c r="D288" s="9"/>
@@ -8942,9 +8942,9 @@
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="31"/>
+      <c r="A289" s="27"/>
       <c r="B289" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C289" s="9"/>
       <c r="D289" s="9"/>
@@ -8970,9 +8970,9 @@
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="31"/>
+      <c r="A290" s="27"/>
       <c r="B290" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C290" s="9"/>
       <c r="D290" s="9"/>
@@ -8998,9 +8998,9 @@
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A291" s="31"/>
+      <c r="A291" s="27"/>
       <c r="B291" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C291" s="9"/>
       <c r="D291" s="9"/>
@@ -9025,87 +9025,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="24"/>
-      <c r="B292" s="6">
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A292" s="27"/>
+      <c r="B292" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C292" s="9"/>
+      <c r="D292" s="9"/>
+      <c r="E292" s="9"/>
+      <c r="F292" s="9"/>
+      <c r="G292" s="9"/>
+      <c r="H292" s="9"/>
+      <c r="I292" s="9"/>
+      <c r="J292" s="9"/>
+      <c r="K292" s="9"/>
+      <c r="L292" s="9"/>
+      <c r="M292" s="9"/>
+      <c r="N292" s="9"/>
+      <c r="O292" s="9"/>
+      <c r="P292" s="9"/>
+      <c r="Q292" s="9"/>
+      <c r="R292" s="9"/>
+      <c r="S292" s="9"/>
+      <c r="T292" s="15"/>
+      <c r="U292">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="24"/>
+      <c r="B293" s="6">
         <v>6876</v>
       </c>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="6"/>
-      <c r="H292" s="6"/>
-      <c r="I292" s="6"/>
-      <c r="J292" s="6"/>
-      <c r="K292" s="6"/>
-      <c r="L292" s="6"/>
-      <c r="M292" s="6"/>
-      <c r="N292" s="6"/>
-      <c r="O292" s="6"/>
-      <c r="P292" s="6"/>
-      <c r="Q292" s="6"/>
-      <c r="R292" s="6"/>
-      <c r="S292" s="6"/>
-      <c r="T292" s="7"/>
-      <c r="U292">
-        <f t="shared" ref="U292:U355" ca="1" si="7">IF(B292=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="22" t="s">
+      <c r="C293" s="6"/>
+      <c r="D293" s="6"/>
+      <c r="E293" s="6"/>
+      <c r="F293" s="6"/>
+      <c r="G293" s="6"/>
+      <c r="H293" s="6"/>
+      <c r="I293" s="6"/>
+      <c r="J293" s="6"/>
+      <c r="K293" s="6"/>
+      <c r="L293" s="6"/>
+      <c r="M293" s="6"/>
+      <c r="N293" s="6"/>
+      <c r="O293" s="6"/>
+      <c r="P293" s="6"/>
+      <c r="Q293" s="6"/>
+      <c r="R293" s="6"/>
+      <c r="S293" s="6"/>
+      <c r="T293" s="7"/>
+      <c r="U293">
+        <f t="shared" ref="U293:U356" ca="1" si="7">IF(B293=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A294" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B293" s="8">
+      <c r="B294" s="8">
         <v>4304</v>
       </c>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="14"/>
-      <c r="U293">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="23"/>
-      <c r="B294" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
-      <c r="E294" s="2"/>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
-      <c r="H294" s="2"/>
-      <c r="I294" s="2"/>
-      <c r="J294" s="2"/>
-      <c r="K294" s="2"/>
-      <c r="L294" s="2"/>
-      <c r="M294" s="2"/>
-      <c r="N294" s="2"/>
-      <c r="O294" s="2"/>
-      <c r="P294" s="2"/>
-      <c r="Q294" s="2"/>
-      <c r="R294" s="2"/>
-      <c r="S294" s="2"/>
-      <c r="T294" s="5"/>
+      <c r="C294" s="8"/>
+      <c r="D294" s="8"/>
+      <c r="E294" s="8"/>
+      <c r="F294" s="8"/>
+      <c r="G294" s="8"/>
+      <c r="H294" s="8"/>
+      <c r="I294" s="8"/>
+      <c r="J294" s="8"/>
+      <c r="K294" s="8"/>
+      <c r="L294" s="8"/>
+      <c r="M294" s="8"/>
+      <c r="N294" s="8"/>
+      <c r="O294" s="8"/>
+      <c r="P294" s="8"/>
+      <c r="Q294" s="8"/>
+      <c r="R294" s="8"/>
+      <c r="S294" s="8"/>
+      <c r="T294" s="14"/>
       <c r="U294">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9114,7 +9114,7 @@
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" s="23"/>
       <c r="B295" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9142,7 +9142,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="23"/>
       <c r="B296" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -9167,87 +9167,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="24"/>
-      <c r="B297" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C297" s="6"/>
-      <c r="D297" s="6"/>
-      <c r="E297" s="6"/>
-      <c r="F297" s="6"/>
-      <c r="G297" s="6"/>
-      <c r="H297" s="6"/>
-      <c r="I297" s="6"/>
-      <c r="J297" s="6"/>
-      <c r="K297" s="6"/>
-      <c r="L297" s="6"/>
-      <c r="M297" s="6"/>
-      <c r="N297" s="6"/>
-      <c r="O297" s="6"/>
-      <c r="P297" s="6"/>
-      <c r="Q297" s="6"/>
-      <c r="R297" s="6"/>
-      <c r="S297" s="6"/>
-      <c r="T297" s="7"/>
+    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A297" s="23"/>
+      <c r="B297" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C297" s="2"/>
+      <c r="D297" s="2"/>
+      <c r="E297" s="2"/>
+      <c r="F297" s="2"/>
+      <c r="G297" s="2"/>
+      <c r="H297" s="2"/>
+      <c r="I297" s="2"/>
+      <c r="J297" s="2"/>
+      <c r="K297" s="2"/>
+      <c r="L297" s="2"/>
+      <c r="M297" s="2"/>
+      <c r="N297" s="2"/>
+      <c r="O297" s="2"/>
+      <c r="P297" s="2"/>
+      <c r="Q297" s="2"/>
+      <c r="R297" s="2"/>
+      <c r="S297" s="2"/>
+      <c r="T297" s="5"/>
       <c r="U297">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A298" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B298" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C298" s="8"/>
-      <c r="D298" s="8"/>
-      <c r="E298" s="8"/>
-      <c r="F298" s="8"/>
-      <c r="G298" s="8"/>
-      <c r="H298" s="8"/>
-      <c r="I298" s="8"/>
-      <c r="J298" s="8"/>
-      <c r="K298" s="8"/>
-      <c r="L298" s="8"/>
-      <c r="M298" s="8"/>
-      <c r="N298" s="8"/>
-      <c r="O298" s="8"/>
-      <c r="P298" s="8"/>
-      <c r="Q298" s="8"/>
-      <c r="R298" s="8"/>
-      <c r="S298" s="8"/>
-      <c r="T298" s="14"/>
+    <row r="298" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="24"/>
+      <c r="B298" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C298" s="6"/>
+      <c r="D298" s="6"/>
+      <c r="E298" s="6"/>
+      <c r="F298" s="6"/>
+      <c r="G298" s="6"/>
+      <c r="H298" s="6"/>
+      <c r="I298" s="6"/>
+      <c r="J298" s="6"/>
+      <c r="K298" s="6"/>
+      <c r="L298" s="6"/>
+      <c r="M298" s="6"/>
+      <c r="N298" s="6"/>
+      <c r="O298" s="6"/>
+      <c r="P298" s="6"/>
+      <c r="Q298" s="6"/>
+      <c r="R298" s="6"/>
+      <c r="S298" s="6"/>
+      <c r="T298" s="7"/>
       <c r="U298">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A299" s="23"/>
-      <c r="B299" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C299" s="2"/>
-      <c r="D299" s="2"/>
-      <c r="E299" s="2"/>
-      <c r="F299" s="2"/>
-      <c r="G299" s="2"/>
-      <c r="H299" s="2"/>
-      <c r="I299" s="2"/>
-      <c r="J299" s="2"/>
-      <c r="K299" s="2"/>
-      <c r="L299" s="2"/>
-      <c r="M299" s="2"/>
-      <c r="N299" s="2"/>
-      <c r="O299" s="2"/>
-      <c r="P299" s="2"/>
-      <c r="Q299" s="2"/>
-      <c r="R299" s="2"/>
-      <c r="S299" s="2"/>
-      <c r="T299" s="5"/>
+      <c r="A299" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B299" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C299" s="8"/>
+      <c r="D299" s="8"/>
+      <c r="E299" s="8"/>
+      <c r="F299" s="8"/>
+      <c r="G299" s="8"/>
+      <c r="H299" s="8"/>
+      <c r="I299" s="8"/>
+      <c r="J299" s="8"/>
+      <c r="K299" s="8"/>
+      <c r="L299" s="8"/>
+      <c r="M299" s="8"/>
+      <c r="N299" s="8"/>
+      <c r="O299" s="8"/>
+      <c r="P299" s="8"/>
+      <c r="Q299" s="8"/>
+      <c r="R299" s="8"/>
+      <c r="S299" s="8"/>
+      <c r="T299" s="14"/>
       <c r="U299">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9256,7 +9256,7 @@
     <row r="300" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A300" s="23"/>
       <c r="B300" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -9281,10 +9281,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A301" s="23"/>
-      <c r="B301" s="2">
-        <v>7170</v>
+      <c r="B301" s="12">
+        <v>7546</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -9312,7 +9312,7 @@
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="23"/>
       <c r="B302" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -9340,7 +9340,7 @@
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9368,7 +9368,7 @@
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9396,7 +9396,7 @@
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="23"/>
       <c r="B305" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9424,7 +9424,7 @@
     <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A306" s="23"/>
       <c r="B306" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -9452,7 +9452,7 @@
     <row r="307" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A307" s="23"/>
       <c r="B307" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
@@ -9480,7 +9480,7 @@
     <row r="308" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A308" s="23"/>
       <c r="B308" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -9508,7 +9508,7 @@
     <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="23"/>
       <c r="B309" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9536,7 +9536,7 @@
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="23"/>
       <c r="B310" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9564,7 +9564,7 @@
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A311" s="23"/>
       <c r="B311" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9592,7 +9592,7 @@
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A312" s="23"/>
       <c r="B312" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -9617,87 +9617,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A313" s="24"/>
-      <c r="B313" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C313" s="6"/>
-      <c r="D313" s="6"/>
-      <c r="E313" s="6"/>
-      <c r="F313" s="6"/>
-      <c r="G313" s="6"/>
-      <c r="H313" s="6"/>
-      <c r="I313" s="6"/>
-      <c r="J313" s="6"/>
-      <c r="K313" s="6"/>
-      <c r="L313" s="6"/>
-      <c r="M313" s="6"/>
-      <c r="N313" s="6"/>
-      <c r="O313" s="6"/>
-      <c r="P313" s="6"/>
-      <c r="Q313" s="6"/>
-      <c r="R313" s="6"/>
-      <c r="S313" s="6"/>
-      <c r="T313" s="7"/>
+    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A313" s="23"/>
+      <c r="B313" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C313" s="2"/>
+      <c r="D313" s="2"/>
+      <c r="E313" s="2"/>
+      <c r="F313" s="2"/>
+      <c r="G313" s="2"/>
+      <c r="H313" s="2"/>
+      <c r="I313" s="2"/>
+      <c r="J313" s="2"/>
+      <c r="K313" s="2"/>
+      <c r="L313" s="2"/>
+      <c r="M313" s="2"/>
+      <c r="N313" s="2"/>
+      <c r="O313" s="2"/>
+      <c r="P313" s="2"/>
+      <c r="Q313" s="2"/>
+      <c r="R313" s="2"/>
+      <c r="S313" s="2"/>
+      <c r="T313" s="5"/>
       <c r="U313">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B314" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C314" s="8"/>
-      <c r="D314" s="8"/>
-      <c r="E314" s="8"/>
-      <c r="F314" s="8"/>
-      <c r="G314" s="8"/>
-      <c r="H314" s="8"/>
-      <c r="I314" s="8"/>
-      <c r="J314" s="8"/>
-      <c r="K314" s="8"/>
-      <c r="L314" s="8"/>
-      <c r="M314" s="8"/>
-      <c r="N314" s="8"/>
-      <c r="O314" s="8"/>
-      <c r="P314" s="8"/>
-      <c r="Q314" s="8"/>
-      <c r="R314" s="8"/>
-      <c r="S314" s="8"/>
-      <c r="T314" s="14"/>
+    <row r="314" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="24"/>
+      <c r="B314" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C314" s="6"/>
+      <c r="D314" s="6"/>
+      <c r="E314" s="6"/>
+      <c r="F314" s="6"/>
+      <c r="G314" s="6"/>
+      <c r="H314" s="6"/>
+      <c r="I314" s="6"/>
+      <c r="J314" s="6"/>
+      <c r="K314" s="6"/>
+      <c r="L314" s="6"/>
+      <c r="M314" s="6"/>
+      <c r="N314" s="6"/>
+      <c r="O314" s="6"/>
+      <c r="P314" s="6"/>
+      <c r="Q314" s="6"/>
+      <c r="R314" s="6"/>
+      <c r="S314" s="6"/>
+      <c r="T314" s="7"/>
       <c r="U314">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="23"/>
-      <c r="B315" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C315" s="2"/>
-      <c r="D315" s="2"/>
-      <c r="E315" s="2"/>
-      <c r="F315" s="2"/>
-      <c r="G315" s="2"/>
-      <c r="H315" s="2"/>
-      <c r="I315" s="2"/>
-      <c r="J315" s="2"/>
-      <c r="K315" s="2"/>
-      <c r="L315" s="2"/>
-      <c r="M315" s="2"/>
-      <c r="N315" s="2"/>
-      <c r="O315" s="2"/>
-      <c r="P315" s="2"/>
-      <c r="Q315" s="2"/>
-      <c r="R315" s="2"/>
-      <c r="S315" s="2"/>
-      <c r="T315" s="5"/>
+      <c r="A315" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B315" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C315" s="8"/>
+      <c r="D315" s="8"/>
+      <c r="E315" s="8"/>
+      <c r="F315" s="8"/>
+      <c r="G315" s="8"/>
+      <c r="H315" s="8"/>
+      <c r="I315" s="8"/>
+      <c r="J315" s="8"/>
+      <c r="K315" s="8"/>
+      <c r="L315" s="8"/>
+      <c r="M315" s="8"/>
+      <c r="N315" s="8"/>
+      <c r="O315" s="8"/>
+      <c r="P315" s="8"/>
+      <c r="Q315" s="8"/>
+      <c r="R315" s="8"/>
+      <c r="S315" s="8"/>
+      <c r="T315" s="14"/>
       <c r="U315">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9706,7 +9706,7 @@
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A316" s="23"/>
       <c r="B316" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9734,7 +9734,7 @@
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A317" s="23"/>
       <c r="B317" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -9762,7 +9762,7 @@
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A318" s="23"/>
       <c r="B318" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -9787,87 +9787,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A319" s="24"/>
-      <c r="B319" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C319" s="6"/>
-      <c r="D319" s="6"/>
-      <c r="E319" s="6"/>
-      <c r="F319" s="6"/>
-      <c r="G319" s="6"/>
-      <c r="H319" s="6"/>
-      <c r="I319" s="6"/>
-      <c r="J319" s="6"/>
-      <c r="K319" s="6"/>
-      <c r="L319" s="6"/>
-      <c r="M319" s="6"/>
-      <c r="N319" s="6"/>
-      <c r="O319" s="6"/>
-      <c r="P319" s="6"/>
-      <c r="Q319" s="6"/>
-      <c r="R319" s="6"/>
-      <c r="S319" s="6"/>
-      <c r="T319" s="7"/>
+    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A319" s="23"/>
+      <c r="B319" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C319" s="2"/>
+      <c r="D319" s="2"/>
+      <c r="E319" s="2"/>
+      <c r="F319" s="2"/>
+      <c r="G319" s="2"/>
+      <c r="H319" s="2"/>
+      <c r="I319" s="2"/>
+      <c r="J319" s="2"/>
+      <c r="K319" s="2"/>
+      <c r="L319" s="2"/>
+      <c r="M319" s="2"/>
+      <c r="N319" s="2"/>
+      <c r="O319" s="2"/>
+      <c r="P319" s="2"/>
+      <c r="Q319" s="2"/>
+      <c r="R319" s="2"/>
+      <c r="S319" s="2"/>
+      <c r="T319" s="5"/>
       <c r="U319">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A320" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B320" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C320" s="8"/>
-      <c r="D320" s="8"/>
-      <c r="E320" s="8"/>
-      <c r="F320" s="8"/>
-      <c r="G320" s="8"/>
-      <c r="H320" s="8"/>
-      <c r="I320" s="8"/>
-      <c r="J320" s="8"/>
-      <c r="K320" s="8"/>
-      <c r="L320" s="8"/>
-      <c r="M320" s="8"/>
-      <c r="N320" s="8"/>
-      <c r="O320" s="8"/>
-      <c r="P320" s="8"/>
-      <c r="Q320" s="8"/>
-      <c r="R320" s="8"/>
-      <c r="S320" s="8"/>
-      <c r="T320" s="14"/>
+    <row r="320" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="24"/>
+      <c r="B320" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C320" s="6"/>
+      <c r="D320" s="6"/>
+      <c r="E320" s="6"/>
+      <c r="F320" s="6"/>
+      <c r="G320" s="6"/>
+      <c r="H320" s="6"/>
+      <c r="I320" s="6"/>
+      <c r="J320" s="6"/>
+      <c r="K320" s="6"/>
+      <c r="L320" s="6"/>
+      <c r="M320" s="6"/>
+      <c r="N320" s="6"/>
+      <c r="O320" s="6"/>
+      <c r="P320" s="6"/>
+      <c r="Q320" s="6"/>
+      <c r="R320" s="6"/>
+      <c r="S320" s="6"/>
+      <c r="T320" s="7"/>
       <c r="U320">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A321" s="23"/>
-      <c r="B321" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C321" s="2"/>
-      <c r="D321" s="2"/>
-      <c r="E321" s="2"/>
-      <c r="F321" s="2"/>
-      <c r="G321" s="2"/>
-      <c r="H321" s="2"/>
-      <c r="I321" s="2"/>
-      <c r="J321" s="2"/>
-      <c r="K321" s="2"/>
-      <c r="L321" s="2"/>
-      <c r="M321" s="2"/>
-      <c r="N321" s="2"/>
-      <c r="O321" s="2"/>
-      <c r="P321" s="2"/>
-      <c r="Q321" s="2"/>
-      <c r="R321" s="2"/>
-      <c r="S321" s="2"/>
-      <c r="T321" s="5"/>
+      <c r="A321" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B321" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C321" s="8"/>
+      <c r="D321" s="8"/>
+      <c r="E321" s="8"/>
+      <c r="F321" s="8"/>
+      <c r="G321" s="8"/>
+      <c r="H321" s="8"/>
+      <c r="I321" s="8"/>
+      <c r="J321" s="8"/>
+      <c r="K321" s="8"/>
+      <c r="L321" s="8"/>
+      <c r="M321" s="8"/>
+      <c r="N321" s="8"/>
+      <c r="O321" s="8"/>
+      <c r="P321" s="8"/>
+      <c r="Q321" s="8"/>
+      <c r="R321" s="8"/>
+      <c r="S321" s="8"/>
+      <c r="T321" s="14"/>
       <c r="U321">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -9876,7 +9876,7 @@
     <row r="322" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A322" s="23"/>
       <c r="B322" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
@@ -9904,7 +9904,7 @@
     <row r="323" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A323" s="23"/>
       <c r="B323" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
@@ -9932,7 +9932,7 @@
     <row r="324" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A324" s="23"/>
       <c r="B324" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
@@ -9957,35 +9957,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A325" s="24"/>
-      <c r="B325" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C325" s="6"/>
-      <c r="D325" s="6"/>
-      <c r="E325" s="6"/>
-      <c r="F325" s="6"/>
-      <c r="G325" s="6"/>
-      <c r="H325" s="6"/>
-      <c r="I325" s="6"/>
-      <c r="J325" s="6"/>
-      <c r="K325" s="6"/>
-      <c r="L325" s="6"/>
-      <c r="M325" s="6"/>
-      <c r="N325" s="6"/>
-      <c r="O325" s="6"/>
-      <c r="P325" s="6"/>
-      <c r="Q325" s="6"/>
-      <c r="R325" s="6"/>
-      <c r="S325" s="6"/>
-      <c r="T325" s="7"/>
+    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A325" s="23"/>
+      <c r="B325" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C325" s="2"/>
+      <c r="D325" s="2"/>
+      <c r="E325" s="2"/>
+      <c r="F325" s="2"/>
+      <c r="G325" s="2"/>
+      <c r="H325" s="2"/>
+      <c r="I325" s="2"/>
+      <c r="J325" s="2"/>
+      <c r="K325" s="2"/>
+      <c r="L325" s="2"/>
+      <c r="M325" s="2"/>
+      <c r="N325" s="2"/>
+      <c r="O325" s="2"/>
+      <c r="P325" s="2"/>
+      <c r="Q325" s="2"/>
+      <c r="R325" s="2"/>
+      <c r="S325" s="2"/>
+      <c r="T325" s="5"/>
       <c r="U325">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A326" s="24"/>
+      <c r="B326" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C326" s="6"/>
+      <c r="D326" s="6"/>
+      <c r="E326" s="6"/>
+      <c r="F326" s="6"/>
+      <c r="G326" s="6"/>
+      <c r="H326" s="6"/>
+      <c r="I326" s="6"/>
+      <c r="J326" s="6"/>
+      <c r="K326" s="6"/>
+      <c r="L326" s="6"/>
+      <c r="M326" s="6"/>
+      <c r="N326" s="6"/>
+      <c r="O326" s="6"/>
+      <c r="P326" s="6"/>
+      <c r="Q326" s="6"/>
+      <c r="R326" s="6"/>
+      <c r="S326" s="6"/>
+      <c r="T326" s="7"/>
       <c r="U326">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -10167,13 +10189,13 @@
     </row>
     <row r="356" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U356">
-        <f t="shared" ref="U356:U419" ca="1" si="8">IF(B356=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="357" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U357">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U357:U420" ca="1" si="8">IF(B357=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10551,13 +10573,13 @@
     </row>
     <row r="420" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U420">
-        <f t="shared" ref="U420:U483" ca="1" si="9">IF(B420=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="421" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U421">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U421:U484" ca="1" si="9">IF(B421=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10935,13 +10957,13 @@
     </row>
     <row r="484" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U484">
-        <f t="shared" ref="U484:U547" ca="1" si="10">IF(B484=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="485" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U485">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U485:U548" ca="1" si="10">IF(B485=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11319,13 +11341,13 @@
     </row>
     <row r="548" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U548">
-        <f t="shared" ref="U548:U611" ca="1" si="11">IF(B548=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="549" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U549">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U549:U612" ca="1" si="11">IF(B549=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11703,13 +11725,13 @@
     </row>
     <row r="612" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U612">
-        <f t="shared" ref="U612:U675" ca="1" si="12">IF(B612=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="613" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U613">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U613:U676" ca="1" si="12">IF(B613=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12087,13 +12109,13 @@
     </row>
     <row r="676" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U676">
-        <f t="shared" ref="U676:U739" ca="1" si="13">IF(B676=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="677" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U677">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U677:U740" ca="1" si="13">IF(B677=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12471,13 +12493,13 @@
     </row>
     <row r="740" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U740">
-        <f t="shared" ref="U740:U803" ca="1" si="14">IF(B740=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="741" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U741">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U741:U804" ca="1" si="14">IF(B741=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12855,13 +12877,13 @@
     </row>
     <row r="804" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U804">
-        <f t="shared" ref="U804:U867" ca="1" si="15">IF(B804=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="805" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U805">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U805:U868" ca="1" si="15">IF(B805=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13239,13 +13261,13 @@
     </row>
     <row r="868" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U868">
-        <f t="shared" ref="U868:U929" ca="1" si="16">IF(B868=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="869" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U869">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U869:U930" ca="1" si="16">IF(B869=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13609,26 +13631,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="930" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U930">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A320:A325"/>
-    <mergeCell ref="A250:A279"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A294:A298"/>
+    <mergeCell ref="A281:A293"/>
+    <mergeCell ref="A321:A326"/>
+    <mergeCell ref="A251:A280"/>
     <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A298:A313"/>
-    <mergeCell ref="A314:A319"/>
+    <mergeCell ref="A299:A314"/>
+    <mergeCell ref="A315:A320"/>
     <mergeCell ref="A64:A104"/>
-    <mergeCell ref="A222:A233"/>
-    <mergeCell ref="A150:A185"/>
-    <mergeCell ref="A186:A204"/>
+    <mergeCell ref="A223:A234"/>
+    <mergeCell ref="A150:A186"/>
+    <mergeCell ref="A187:A205"/>
     <mergeCell ref="A105:A149"/>
     <mergeCell ref="A19:A63"/>
-    <mergeCell ref="A205:A221"/>
-    <mergeCell ref="A234:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A293:A297"/>
-    <mergeCell ref="A280:A292"/>
+    <mergeCell ref="A206:A222"/>
+    <mergeCell ref="A235:A242"/>
+    <mergeCell ref="A243:A250"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add task about displaying combinations to lab 07
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$305</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$306</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -521,6 +521,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,15 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W937"/>
+  <dimension ref="A1:W938"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N174" sqref="N174"/>
+      <selection pane="bottomLeft" activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,56 +891,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>9857</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -1056,7 +1056,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3">
         <v>1662</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3">
         <v>4131</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3">
         <v>7365</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3">
         <v>1910</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3">
         <v>1640</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2">
         <v>1860</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2">
         <v>4764</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2">
         <v>2429</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2">
         <v>7472</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="2">
         <v>4140</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2">
         <v>2959</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2">
         <v>7271</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2">
         <v>2632</v>
       </c>
@@ -2766,7 +2766,7 @@
       </c>
     </row>
     <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B69" s="13">
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="12">
         <v>2217</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="12">
         <v>1824</v>
       </c>
@@ -2852,7 +2852,7 @@
       </c>
     </row>
     <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="12">
         <v>2564</v>
       </c>
@@ -2880,7 +2880,7 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="12">
         <v>8487</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="2">
         <v>8878</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="2">
         <v>3072</v>
       </c>
@@ -2964,7 +2964,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="2">
         <v>5980</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="23"/>
       <c r="B77" s="2">
         <v>8174</v>
       </c>
@@ -3020,7 +3020,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="29"/>
+      <c r="A78" s="23"/>
       <c r="B78" s="2">
         <v>4257</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="29"/>
+      <c r="A79" s="23"/>
       <c r="B79" s="2">
         <v>2291</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="23"/>
       <c r="B80" s="2">
         <v>1763</v>
       </c>
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
+      <c r="A81" s="23"/>
       <c r="B81" s="2">
         <v>5662</v>
       </c>
@@ -3132,7 +3132,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="A82" s="23"/>
       <c r="B82" s="2">
         <v>1945</v>
       </c>
@@ -3160,7 +3160,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
+      <c r="A83" s="23"/>
       <c r="B83" s="2">
         <v>1186</v>
       </c>
@@ -3188,7 +3188,7 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="23"/>
       <c r="B84" s="2">
         <v>8715</v>
       </c>
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="23"/>
       <c r="B85" s="2">
         <v>8518</v>
       </c>
@@ -3244,7 +3244,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
+      <c r="A86" s="23"/>
       <c r="B86" s="2">
         <v>4847</v>
       </c>
@@ -3272,7 +3272,7 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="23"/>
       <c r="B87" s="2">
         <v>6589</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="2">
         <v>7991</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="23"/>
       <c r="B89" s="2">
         <v>6291</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="23"/>
       <c r="B90" s="2">
         <v>3770</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="2">
         <v>7178</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="2">
         <v>3883</v>
       </c>
@@ -3440,7 +3440,7 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="2">
         <v>1999</v>
       </c>
@@ -3468,7 +3468,7 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="2">
         <v>4042</v>
       </c>
@@ -3496,7 +3496,7 @@
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="2">
         <v>6351</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="2">
         <v>5382</v>
       </c>
@@ -3552,7 +3552,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="23"/>
       <c r="B97" s="2">
         <v>7088</v>
       </c>
@@ -3580,7 +3580,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="23"/>
       <c r="B98" s="2">
         <v>7250</v>
       </c>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="2">
         <v>6740</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+      <c r="A100" s="23"/>
       <c r="B100" s="2">
         <v>9038</v>
       </c>
@@ -3664,7 +3664,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="23"/>
       <c r="B101" s="2">
         <v>1292</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="23"/>
       <c r="B102" s="2">
         <v>4527</v>
       </c>
@@ -3720,7 +3720,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
+      <c r="A103" s="23"/>
       <c r="B103" s="2">
         <v>6556</v>
       </c>
@@ -3748,7 +3748,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A104" s="29"/>
+      <c r="A104" s="23"/>
       <c r="B104" s="2">
         <v>5635</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
+      <c r="A105" s="23"/>
       <c r="B105" s="2">
         <v>3878</v>
       </c>
@@ -3804,7 +3804,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="2">
         <v>1217</v>
       </c>
@@ -3832,7 +3832,7 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" s="29"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="2">
         <v>1438</v>
       </c>
@@ -3860,7 +3860,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" s="29"/>
+      <c r="A108" s="23"/>
       <c r="B108" s="2">
         <v>2153</v>
       </c>
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="30"/>
+      <c r="A109" s="24"/>
       <c r="B109" s="6">
         <v>7937</v>
       </c>
@@ -3916,7 +3916,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B110" s="13">
@@ -3946,7 +3946,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="29"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="12">
         <v>1881</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="2">
         <v>8495</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" s="29"/>
+      <c r="A113" s="23"/>
       <c r="B113" s="2">
         <v>1315</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114" s="29"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="2">
         <v>6066</v>
       </c>
@@ -4058,7 +4058,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="29"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="2">
         <v>2565</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" s="29"/>
+      <c r="A116" s="23"/>
       <c r="B116" s="2">
         <v>2594</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
+      <c r="A117" s="23"/>
       <c r="B117" s="2">
         <v>2321</v>
       </c>
@@ -4142,7 +4142,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
+      <c r="A118" s="23"/>
       <c r="B118" s="2">
         <v>5053</v>
       </c>
@@ -4170,7 +4170,7 @@
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
+      <c r="A119" s="23"/>
       <c r="B119" s="2">
         <v>4338</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" s="29"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="2">
         <v>3762</v>
       </c>
@@ -4226,7 +4226,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="29"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="2">
         <v>3550</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="2">
         <v>4264</v>
       </c>
@@ -4282,7 +4282,7 @@
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
+      <c r="A123" s="23"/>
       <c r="B123" s="2">
         <v>2475</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
+      <c r="A124" s="23"/>
       <c r="B124" s="2">
         <v>9180</v>
       </c>
@@ -4338,7 +4338,7 @@
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
+      <c r="A125" s="23"/>
       <c r="B125" s="2">
         <v>1544</v>
       </c>
@@ -4366,7 +4366,7 @@
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="2">
         <v>9562</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
+      <c r="A127" s="23"/>
       <c r="B127" s="2">
         <v>3669</v>
       </c>
@@ -4422,7 +4422,7 @@
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128" s="29"/>
+      <c r="A128" s="23"/>
       <c r="B128" s="2">
         <v>5951</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
+      <c r="A129" s="23"/>
       <c r="B129" s="2">
         <v>2802</v>
       </c>
@@ -4478,7 +4478,7 @@
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="23"/>
       <c r="B130" s="2">
         <v>2324</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A131" s="29"/>
+      <c r="A131" s="23"/>
       <c r="B131" s="2">
         <v>8731</v>
       </c>
@@ -4534,7 +4534,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="29"/>
+      <c r="A132" s="23"/>
       <c r="B132" s="2">
         <v>4082</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
+      <c r="A133" s="23"/>
       <c r="B133" s="2">
         <v>6280</v>
       </c>
@@ -4590,7 +4590,7 @@
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="23"/>
       <c r="B134" s="2">
         <v>7585</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
+      <c r="A135" s="23"/>
       <c r="B135" s="2">
         <v>1483</v>
       </c>
@@ -4646,7 +4646,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A136" s="29"/>
+      <c r="A136" s="23"/>
       <c r="B136" s="2">
         <v>3983</v>
       </c>
@@ -4674,7 +4674,7 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A137" s="29"/>
+      <c r="A137" s="23"/>
       <c r="B137" s="2">
         <v>8770</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
+      <c r="A138" s="23"/>
       <c r="B138" s="2">
         <v>4236</v>
       </c>
@@ -4730,7 +4730,7 @@
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A139" s="29"/>
+      <c r="A139" s="23"/>
       <c r="B139" s="2">
         <v>8696</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
+      <c r="A140" s="23"/>
       <c r="B140" s="2">
         <v>5969</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A141" s="29"/>
+      <c r="A141" s="23"/>
       <c r="B141" s="2">
         <v>8418</v>
       </c>
@@ -4814,7 +4814,7 @@
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
+      <c r="A142" s="23"/>
       <c r="B142" s="2">
         <v>5170</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A143" s="29"/>
+      <c r="A143" s="23"/>
       <c r="B143" s="2">
         <v>8395</v>
       </c>
@@ -4870,7 +4870,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A144" s="29"/>
+      <c r="A144" s="23"/>
       <c r="B144" s="2">
         <v>5568</v>
       </c>
@@ -4898,7 +4898,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A145" s="29"/>
+      <c r="A145" s="23"/>
       <c r="B145" s="2">
         <v>2592</v>
       </c>
@@ -4921,12 +4921,12 @@
       <c r="S145" s="2"/>
       <c r="T145" s="5"/>
       <c r="U145">
-        <f t="shared" ref="U145:U219" ca="1" si="4">IF(B145=$W$1,1,0)</f>
+        <f t="shared" ref="U145:U220" ca="1" si="4">IF(B145=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A146" s="29"/>
+      <c r="A146" s="23"/>
       <c r="B146" s="2">
         <v>4075</v>
       </c>
@@ -4954,7 +4954,7 @@
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A147" s="29"/>
+      <c r="A147" s="23"/>
       <c r="B147" s="2">
         <v>7517</v>
       </c>
@@ -4982,7 +4982,7 @@
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A148" s="29"/>
+      <c r="A148" s="23"/>
       <c r="B148" s="2">
         <v>5448</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A149" s="29"/>
+      <c r="A149" s="23"/>
       <c r="B149" s="2">
         <v>6582</v>
       </c>
@@ -5038,7 +5038,7 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A150" s="29"/>
+      <c r="A150" s="23"/>
       <c r="B150" s="2">
         <v>5238</v>
       </c>
@@ -5066,7 +5066,7 @@
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A151" s="29"/>
+      <c r="A151" s="23"/>
       <c r="B151" s="2">
         <v>2084</v>
       </c>
@@ -5094,7 +5094,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A152" s="29"/>
+      <c r="A152" s="23"/>
       <c r="B152" s="2">
         <v>5411</v>
       </c>
@@ -5122,7 +5122,7 @@
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A153" s="29"/>
+      <c r="A153" s="23"/>
       <c r="B153" s="2">
         <v>5171</v>
       </c>
@@ -5150,7 +5150,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="30"/>
+      <c r="A154" s="24"/>
       <c r="B154" s="6">
         <v>1862</v>
       </c>
@@ -5178,7 +5178,7 @@
       </c>
     </row>
     <row r="155" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="28" t="s">
+      <c r="A155" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B155" s="13">
@@ -5208,7 +5208,7 @@
       </c>
     </row>
     <row r="156" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="29"/>
+      <c r="A156" s="23"/>
       <c r="B156" s="12">
         <v>9931</v>
       </c>
@@ -5236,7 +5236,7 @@
       </c>
     </row>
     <row r="157" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="29"/>
+      <c r="A157" s="23"/>
       <c r="B157" s="12">
         <v>9696</v>
       </c>
@@ -5264,7 +5264,7 @@
       </c>
     </row>
     <row r="158" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="29"/>
+      <c r="A158" s="23"/>
       <c r="B158" s="12">
         <v>1947</v>
       </c>
@@ -5292,7 +5292,7 @@
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="29"/>
+      <c r="A159" s="23"/>
       <c r="B159" s="2">
         <v>4425</v>
       </c>
@@ -5320,7 +5320,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A160" s="29"/>
+      <c r="A160" s="23"/>
       <c r="B160" s="2">
         <v>1433</v>
       </c>
@@ -5348,7 +5348,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A161" s="29"/>
+      <c r="A161" s="23"/>
       <c r="B161" s="2">
         <v>7834</v>
       </c>
@@ -5376,7 +5376,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A162" s="29"/>
+      <c r="A162" s="23"/>
       <c r="B162" s="2">
         <v>5683</v>
       </c>
@@ -5404,7 +5404,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A163" s="29"/>
+      <c r="A163" s="23"/>
       <c r="B163" s="2">
         <v>1223</v>
       </c>
@@ -5432,7 +5432,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A164" s="29"/>
+      <c r="A164" s="23"/>
       <c r="B164" s="2">
         <v>8311</v>
       </c>
@@ -5460,7 +5460,7 @@
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A165" s="29"/>
+      <c r="A165" s="23"/>
       <c r="B165" s="2">
         <v>3134</v>
       </c>
@@ -5488,7 +5488,7 @@
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A166" s="29"/>
+      <c r="A166" s="23"/>
       <c r="B166" s="2">
         <v>9711</v>
       </c>
@@ -5516,7 +5516,7 @@
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A167" s="29"/>
+      <c r="A167" s="23"/>
       <c r="B167" s="2">
         <v>7085</v>
       </c>
@@ -5544,7 +5544,7 @@
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168" s="29"/>
+      <c r="A168" s="23"/>
       <c r="B168" s="2">
         <v>3333</v>
       </c>
@@ -5572,7 +5572,7 @@
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A169" s="29"/>
+      <c r="A169" s="23"/>
       <c r="B169" s="2">
         <v>8820</v>
       </c>
@@ -5600,7 +5600,7 @@
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A170" s="29"/>
+      <c r="A170" s="23"/>
       <c r="B170" s="2">
         <v>5694</v>
       </c>
@@ -5628,7 +5628,7 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A171" s="29"/>
+      <c r="A171" s="23"/>
       <c r="B171" s="2">
         <v>6806</v>
       </c>
@@ -5656,7 +5656,7 @@
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A172" s="29"/>
+      <c r="A172" s="23"/>
       <c r="B172" s="2">
         <v>7369</v>
       </c>
@@ -5684,7 +5684,7 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
+      <c r="A173" s="23"/>
       <c r="B173" s="2">
         <v>8613</v>
       </c>
@@ -5712,7 +5712,7 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="29"/>
+      <c r="A174" s="23"/>
       <c r="B174" s="2">
         <v>7534</v>
       </c>
@@ -5740,7 +5740,7 @@
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A175" s="29"/>
+      <c r="A175" s="23"/>
       <c r="B175" s="2">
         <v>2173</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" s="29"/>
+      <c r="A176" s="23"/>
       <c r="B176" s="2">
         <v>5894</v>
       </c>
@@ -5796,7 +5796,7 @@
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A177" s="29"/>
+      <c r="A177" s="23"/>
       <c r="B177" s="2">
         <v>4515</v>
       </c>
@@ -5824,7 +5824,7 @@
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A178" s="29"/>
+      <c r="A178" s="23"/>
       <c r="B178" s="2">
         <v>9774</v>
       </c>
@@ -5852,7 +5852,7 @@
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A179" s="29"/>
+      <c r="A179" s="23"/>
       <c r="B179" s="2">
         <v>3946</v>
       </c>
@@ -5880,7 +5880,7 @@
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A180" s="29"/>
+      <c r="A180" s="23"/>
       <c r="B180" s="2">
         <v>6497</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A181" s="29"/>
+      <c r="A181" s="23"/>
       <c r="B181" s="2">
         <v>5648</v>
       </c>
@@ -5936,7 +5936,7 @@
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A182" s="29"/>
+      <c r="A182" s="23"/>
       <c r="B182" s="2">
         <v>3940</v>
       </c>
@@ -5964,7 +5964,7 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A183" s="29"/>
+      <c r="A183" s="23"/>
       <c r="B183" s="2">
         <v>7290</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="29"/>
+      <c r="A184" s="23"/>
       <c r="B184" s="2">
         <v>7035</v>
       </c>
@@ -6020,7 +6020,7 @@
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A185" s="29"/>
+      <c r="A185" s="23"/>
       <c r="B185" s="2">
         <v>9271</v>
       </c>
@@ -6048,7 +6048,7 @@
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A186" s="29"/>
+      <c r="A186" s="23"/>
       <c r="B186" s="2">
         <v>8769</v>
       </c>
@@ -6076,7 +6076,7 @@
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A187" s="29"/>
+      <c r="A187" s="23"/>
       <c r="B187" s="2">
         <v>4497</v>
       </c>
@@ -6104,7 +6104,7 @@
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="29"/>
+      <c r="A188" s="23"/>
       <c r="B188" s="2">
         <v>3218</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A189" s="29"/>
+      <c r="A189" s="23"/>
       <c r="B189" s="2">
         <v>6492</v>
       </c>
@@ -6160,7 +6160,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A190" s="29"/>
+      <c r="A190" s="23"/>
       <c r="B190" s="2">
         <v>4293</v>
       </c>
@@ -6188,7 +6188,7 @@
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A191" s="29"/>
+      <c r="A191" s="23"/>
       <c r="B191" s="2">
         <v>7703</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A192" s="29"/>
+      <c r="A192" s="23"/>
       <c r="B192" s="2">
         <v>5541</v>
       </c>
@@ -6243,96 +6243,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="30"/>
-      <c r="B193" s="6">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A193" s="31"/>
+      <c r="B193" s="9">
         <v>9182</v>
       </c>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
-      <c r="G193" s="6"/>
-      <c r="H193" s="6"/>
-      <c r="I193" s="6"/>
-      <c r="J193" s="6"/>
-      <c r="K193" s="6"/>
-      <c r="L193" s="6"/>
-      <c r="M193" s="6"/>
-      <c r="N193" s="6"/>
-      <c r="O193" s="6"/>
-      <c r="P193" s="6"/>
-      <c r="Q193" s="6"/>
-      <c r="R193" s="6"/>
-      <c r="S193" s="6"/>
-      <c r="T193" s="7"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9"/>
+      <c r="E193" s="9"/>
+      <c r="F193" s="9"/>
+      <c r="G193" s="9"/>
+      <c r="H193" s="9"/>
+      <c r="I193" s="9"/>
+      <c r="J193" s="9"/>
+      <c r="K193" s="9"/>
+      <c r="L193" s="9"/>
+      <c r="M193" s="9"/>
+      <c r="N193" s="9"/>
+      <c r="O193" s="9"/>
+      <c r="P193" s="9"/>
+      <c r="Q193" s="9"/>
+      <c r="R193" s="9"/>
+      <c r="S193" s="9"/>
+      <c r="T193" s="15"/>
       <c r="U193">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="28" t="s">
+    <row r="194" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="24"/>
+      <c r="B194" s="6">
+        <v>3095</v>
+      </c>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="H194" s="6"/>
+      <c r="I194" s="6"/>
+      <c r="J194" s="6"/>
+      <c r="K194" s="6"/>
+      <c r="L194" s="6"/>
+      <c r="M194" s="6"/>
+      <c r="N194" s="6"/>
+      <c r="O194" s="6"/>
+      <c r="P194" s="6"/>
+      <c r="Q194" s="6"/>
+      <c r="R194" s="6"/>
+      <c r="S194" s="6"/>
+      <c r="T194" s="7"/>
+      <c r="U194">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A195" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B194" s="13">
+      <c r="B195" s="13">
         <v>8165</v>
       </c>
-      <c r="C194" s="8"/>
-      <c r="D194" s="8"/>
-      <c r="E194" s="8"/>
-      <c r="F194" s="8"/>
-      <c r="G194" s="8"/>
-      <c r="H194" s="8"/>
-      <c r="I194" s="8"/>
-      <c r="J194" s="8"/>
-      <c r="K194" s="8"/>
-      <c r="L194" s="8"/>
-      <c r="M194" s="8"/>
-      <c r="N194" s="8"/>
-      <c r="O194" s="8"/>
-      <c r="P194" s="8"/>
-      <c r="Q194" s="8"/>
-      <c r="R194" s="8"/>
-      <c r="S194" s="8"/>
-      <c r="T194" s="14"/>
-      <c r="U194">
-        <f t="shared" ref="U194:U212" ca="1" si="5">IF(B194=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="29"/>
-      <c r="B195" s="12">
+      <c r="C195" s="8"/>
+      <c r="D195" s="8"/>
+      <c r="E195" s="8"/>
+      <c r="F195" s="8"/>
+      <c r="G195" s="8"/>
+      <c r="H195" s="8"/>
+      <c r="I195" s="8"/>
+      <c r="J195" s="8"/>
+      <c r="K195" s="8"/>
+      <c r="L195" s="8"/>
+      <c r="M195" s="8"/>
+      <c r="N195" s="8"/>
+      <c r="O195" s="8"/>
+      <c r="P195" s="8"/>
+      <c r="Q195" s="8"/>
+      <c r="R195" s="8"/>
+      <c r="S195" s="8"/>
+      <c r="T195" s="14"/>
+      <c r="U195">
+        <f t="shared" ref="U195:U213" ca="1" si="5">IF(B195=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A196" s="23"/>
+      <c r="B196" s="12">
         <v>9001</v>
-      </c>
-      <c r="C195" s="2"/>
-      <c r="D195" s="2"/>
-      <c r="E195" s="2"/>
-      <c r="F195" s="2"/>
-      <c r="G195" s="2"/>
-      <c r="H195" s="2"/>
-      <c r="I195" s="2"/>
-      <c r="J195" s="2"/>
-      <c r="K195" s="2"/>
-      <c r="L195" s="2"/>
-      <c r="M195" s="2"/>
-      <c r="N195" s="2"/>
-      <c r="O195" s="2"/>
-      <c r="P195" s="2"/>
-      <c r="Q195" s="2"/>
-      <c r="R195" s="2"/>
-      <c r="S195" s="2"/>
-      <c r="T195" s="5"/>
-      <c r="U195">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A196" s="29"/>
-      <c r="B196" s="2">
-        <v>7491</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
@@ -6358,9 +6358,9 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="29"/>
+      <c r="A197" s="23"/>
       <c r="B197" s="2">
-        <v>9531</v>
+        <v>7491</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -6386,9 +6386,9 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="29"/>
+      <c r="A198" s="23"/>
       <c r="B198" s="2">
-        <v>9812</v>
+        <v>9531</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
@@ -6414,9 +6414,9 @@
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="29"/>
+      <c r="A199" s="23"/>
       <c r="B199" s="2">
-        <v>9279</v>
+        <v>9812</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
@@ -6442,9 +6442,9 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="29"/>
+      <c r="A200" s="23"/>
       <c r="B200" s="2">
-        <v>4845</v>
+        <v>9279</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
@@ -6470,9 +6470,9 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
+      <c r="A201" s="23"/>
       <c r="B201" s="2">
-        <v>5728</v>
+        <v>4845</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
@@ -6498,9 +6498,9 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="29"/>
+      <c r="A202" s="23"/>
       <c r="B202" s="2">
-        <v>7222</v>
+        <v>5728</v>
       </c>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
@@ -6526,9 +6526,9 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="29"/>
+      <c r="A203" s="23"/>
       <c r="B203" s="2">
-        <v>5923</v>
+        <v>7222</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
@@ -6554,9 +6554,9 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
+      <c r="A204" s="23"/>
       <c r="B204" s="2">
-        <v>4265</v>
+        <v>5923</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
@@ -6582,9 +6582,9 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="29"/>
+      <c r="A205" s="23"/>
       <c r="B205" s="2">
-        <v>2166</v>
+        <v>4265</v>
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
@@ -6610,9 +6610,9 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="29"/>
+      <c r="A206" s="23"/>
       <c r="B206" s="2">
-        <v>9116</v>
+        <v>2166</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -6638,9 +6638,9 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="29"/>
+      <c r="A207" s="23"/>
       <c r="B207" s="2">
-        <v>9925</v>
+        <v>9116</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -6666,9 +6666,9 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="29"/>
+      <c r="A208" s="23"/>
       <c r="B208" s="2">
-        <v>3657</v>
+        <v>9925</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
@@ -6694,9 +6694,9 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="29"/>
+      <c r="A209" s="23"/>
       <c r="B209" s="2">
-        <v>6599</v>
+        <v>3657</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
@@ -6722,28 +6722,28 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="31"/>
-      <c r="B210" s="9">
-        <v>1618</v>
-      </c>
-      <c r="C210" s="9"/>
-      <c r="D210" s="9"/>
-      <c r="E210" s="9"/>
-      <c r="F210" s="9"/>
-      <c r="G210" s="9"/>
-      <c r="H210" s="9"/>
-      <c r="I210" s="9"/>
-      <c r="J210" s="9"/>
-      <c r="K210" s="9"/>
-      <c r="L210" s="9"/>
-      <c r="M210" s="9"/>
-      <c r="N210" s="9"/>
-      <c r="O210" s="9"/>
-      <c r="P210" s="9"/>
-      <c r="Q210" s="9"/>
-      <c r="R210" s="9"/>
-      <c r="S210" s="9"/>
-      <c r="T210" s="15"/>
+      <c r="A210" s="23"/>
+      <c r="B210" s="2">
+        <v>6599</v>
+      </c>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+      <c r="K210" s="2"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="2"/>
+      <c r="N210" s="2"/>
+      <c r="O210" s="2"/>
+      <c r="P210" s="2"/>
+      <c r="Q210" s="2"/>
+      <c r="R210" s="2"/>
+      <c r="S210" s="2"/>
+      <c r="T210" s="5"/>
       <c r="U210">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
@@ -6752,7 +6752,7 @@
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="31"/>
       <c r="B211" s="9">
-        <v>1703</v>
+        <v>1618</v>
       </c>
       <c r="C211" s="9"/>
       <c r="D211" s="9"/>
@@ -6777,87 +6777,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="30"/>
-      <c r="B212" s="6">
-        <v>8887</v>
-      </c>
-      <c r="C212" s="6"/>
-      <c r="D212" s="6"/>
-      <c r="E212" s="6"/>
-      <c r="F212" s="6"/>
-      <c r="G212" s="6"/>
-      <c r="H212" s="6"/>
-      <c r="I212" s="6"/>
-      <c r="J212" s="6"/>
-      <c r="K212" s="6"/>
-      <c r="L212" s="6"/>
-      <c r="M212" s="6"/>
-      <c r="N212" s="6"/>
-      <c r="O212" s="6"/>
-      <c r="P212" s="6"/>
-      <c r="Q212" s="6"/>
-      <c r="R212" s="6"/>
-      <c r="S212" s="6"/>
-      <c r="T212" s="7"/>
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A212" s="31"/>
+      <c r="B212" s="9">
+        <v>1703</v>
+      </c>
+      <c r="C212" s="9"/>
+      <c r="D212" s="9"/>
+      <c r="E212" s="9"/>
+      <c r="F212" s="9"/>
+      <c r="G212" s="9"/>
+      <c r="H212" s="9"/>
+      <c r="I212" s="9"/>
+      <c r="J212" s="9"/>
+      <c r="K212" s="9"/>
+      <c r="L212" s="9"/>
+      <c r="M212" s="9"/>
+      <c r="N212" s="9"/>
+      <c r="O212" s="9"/>
+      <c r="P212" s="9"/>
+      <c r="Q212" s="9"/>
+      <c r="R212" s="9"/>
+      <c r="S212" s="9"/>
+      <c r="T212" s="15"/>
       <c r="U212">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A213" s="34" t="s">
+    <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="24"/>
+      <c r="B213" s="6">
+        <v>8887</v>
+      </c>
+      <c r="C213" s="6"/>
+      <c r="D213" s="6"/>
+      <c r="E213" s="6"/>
+      <c r="F213" s="6"/>
+      <c r="G213" s="6"/>
+      <c r="H213" s="6"/>
+      <c r="I213" s="6"/>
+      <c r="J213" s="6"/>
+      <c r="K213" s="6"/>
+      <c r="L213" s="6"/>
+      <c r="M213" s="6"/>
+      <c r="N213" s="6"/>
+      <c r="O213" s="6"/>
+      <c r="P213" s="6"/>
+      <c r="Q213" s="6"/>
+      <c r="R213" s="6"/>
+      <c r="S213" s="6"/>
+      <c r="T213" s="7"/>
+      <c r="U213">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A214" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B213" s="8">
+      <c r="B214" s="8">
         <v>6175</v>
       </c>
-      <c r="C213" s="8"/>
-      <c r="D213" s="8"/>
-      <c r="E213" s="8"/>
-      <c r="F213" s="8"/>
-      <c r="G213" s="8"/>
-      <c r="H213" s="8"/>
-      <c r="I213" s="8"/>
-      <c r="J213" s="8"/>
-      <c r="K213" s="8"/>
-      <c r="L213" s="8"/>
-      <c r="M213" s="8"/>
-      <c r="N213" s="8"/>
-      <c r="O213" s="8"/>
-      <c r="P213" s="8"/>
-      <c r="Q213" s="8"/>
-      <c r="R213" s="8"/>
-      <c r="S213" s="8"/>
-      <c r="T213" s="14"/>
-      <c r="U213">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A214" s="35"/>
-      <c r="B214" s="2">
-        <v>4488</v>
-      </c>
-      <c r="C214" s="2"/>
-      <c r="D214" s="2"/>
-      <c r="E214" s="2"/>
-      <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-      <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
-      <c r="L214" s="2"/>
-      <c r="M214" s="2"/>
-      <c r="N214" s="2"/>
-      <c r="O214" s="2"/>
-      <c r="P214" s="2"/>
-      <c r="Q214" s="2"/>
-      <c r="R214" s="2"/>
-      <c r="S214" s="2"/>
-      <c r="T214" s="5"/>
+      <c r="C214" s="8"/>
+      <c r="D214" s="8"/>
+      <c r="E214" s="8"/>
+      <c r="F214" s="8"/>
+      <c r="G214" s="8"/>
+      <c r="H214" s="8"/>
+      <c r="I214" s="8"/>
+      <c r="J214" s="8"/>
+      <c r="K214" s="8"/>
+      <c r="L214" s="8"/>
+      <c r="M214" s="8"/>
+      <c r="N214" s="8"/>
+      <c r="O214" s="8"/>
+      <c r="P214" s="8"/>
+      <c r="Q214" s="8"/>
+      <c r="R214" s="8"/>
+      <c r="S214" s="8"/>
+      <c r="T214" s="14"/>
       <c r="U214">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
@@ -6866,7 +6866,7 @@
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="2">
-        <v>4954</v>
+        <v>4488</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -6894,7 +6894,7 @@
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="2">
-        <v>4642</v>
+        <v>4954</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -6922,7 +6922,7 @@
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
       <c r="B217" s="2">
-        <v>5537</v>
+        <v>4642</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -6950,7 +6950,7 @@
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
       <c r="B218" s="2">
-        <v>5847</v>
+        <v>5537</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
@@ -6978,7 +6978,7 @@
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
       <c r="B219" s="2">
-        <v>4769</v>
+        <v>5847</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -7006,7 +7006,7 @@
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="35"/>
       <c r="B220" s="2">
-        <v>9930</v>
+        <v>4769</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
@@ -7027,14 +7027,14 @@
       <c r="S220" s="2"/>
       <c r="T220" s="5"/>
       <c r="U220">
-        <f t="shared" ref="U220:U299" ca="1" si="6">IF(B220=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="35"/>
       <c r="B221" s="2">
-        <v>6861</v>
+        <v>9930</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
@@ -7055,14 +7055,14 @@
       <c r="S221" s="2"/>
       <c r="T221" s="5"/>
       <c r="U221">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="U221:U300" ca="1" si="6">IF(B221=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="35"/>
       <c r="B222" s="2">
-        <v>3226</v>
+        <v>6861</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -7090,7 +7090,7 @@
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="35"/>
       <c r="B223" s="2">
-        <v>4372</v>
+        <v>3226</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
@@ -7118,7 +7118,7 @@
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="35"/>
       <c r="B224" s="2">
-        <v>4463</v>
+        <v>4372</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
@@ -7146,7 +7146,7 @@
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="35"/>
       <c r="B225" s="2">
-        <v>1668</v>
+        <v>4463</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -7174,7 +7174,7 @@
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="35"/>
       <c r="B226" s="2">
-        <v>9417</v>
+        <v>1668</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
@@ -7202,7 +7202,7 @@
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="35"/>
       <c r="B227" s="2">
-        <v>3148</v>
+        <v>9417</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
@@ -7230,7 +7230,7 @@
     <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
       <c r="B228" s="2">
-        <v>2137</v>
+        <v>3148</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -7255,96 +7255,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="36"/>
-      <c r="B229" s="6">
-        <v>5621</v>
-      </c>
-      <c r="C229" s="6"/>
-      <c r="D229" s="6"/>
-      <c r="E229" s="6"/>
-      <c r="F229" s="6"/>
-      <c r="G229" s="6"/>
-      <c r="H229" s="6"/>
-      <c r="I229" s="6"/>
-      <c r="J229" s="6"/>
-      <c r="K229" s="6"/>
-      <c r="L229" s="6"/>
-      <c r="M229" s="6"/>
-      <c r="N229" s="6"/>
-      <c r="O229" s="6"/>
-      <c r="P229" s="6"/>
-      <c r="Q229" s="6"/>
-      <c r="R229" s="6"/>
-      <c r="S229" s="6"/>
-      <c r="T229" s="7"/>
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A229" s="35"/>
+      <c r="B229" s="2">
+        <v>2137</v>
+      </c>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+      <c r="M229" s="2"/>
+      <c r="N229" s="2"/>
+      <c r="O229" s="2"/>
+      <c r="P229" s="2"/>
+      <c r="Q229" s="2"/>
+      <c r="R229" s="2"/>
+      <c r="S229" s="2"/>
+      <c r="T229" s="5"/>
       <c r="U229">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A230" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B230" s="8">
-        <v>9300</v>
-      </c>
-      <c r="C230" s="8"/>
-      <c r="D230" s="8"/>
-      <c r="E230" s="8"/>
-      <c r="F230" s="8"/>
-      <c r="G230" s="8"/>
-      <c r="H230" s="8"/>
-      <c r="I230" s="8"/>
-      <c r="J230" s="8"/>
-      <c r="K230" s="8"/>
-      <c r="L230" s="8"/>
-      <c r="M230" s="8"/>
-      <c r="N230" s="8"/>
-      <c r="O230" s="8"/>
-      <c r="P230" s="8"/>
-      <c r="Q230" s="8"/>
-      <c r="R230" s="8"/>
-      <c r="S230" s="8"/>
-      <c r="T230" s="14"/>
+    <row r="230" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="36"/>
+      <c r="B230" s="6">
+        <v>5621</v>
+      </c>
+      <c r="C230" s="6"/>
+      <c r="D230" s="6"/>
+      <c r="E230" s="6"/>
+      <c r="F230" s="6"/>
+      <c r="G230" s="6"/>
+      <c r="H230" s="6"/>
+      <c r="I230" s="6"/>
+      <c r="J230" s="6"/>
+      <c r="K230" s="6"/>
+      <c r="L230" s="6"/>
+      <c r="M230" s="6"/>
+      <c r="N230" s="6"/>
+      <c r="O230" s="6"/>
+      <c r="P230" s="6"/>
+      <c r="Q230" s="6"/>
+      <c r="R230" s="6"/>
+      <c r="S230" s="6"/>
+      <c r="T230" s="7"/>
       <c r="U230">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A231" s="29"/>
-      <c r="B231" s="2">
-        <v>3951</v>
-      </c>
-      <c r="C231" s="2"/>
-      <c r="D231" s="2"/>
-      <c r="E231" s="2"/>
-      <c r="F231" s="2"/>
-      <c r="G231" s="2"/>
-      <c r="H231" s="2"/>
-      <c r="I231" s="2"/>
-      <c r="J231" s="2"/>
-      <c r="K231" s="2"/>
-      <c r="L231" s="2"/>
-      <c r="M231" s="2"/>
-      <c r="N231" s="2"/>
-      <c r="O231" s="2"/>
-      <c r="P231" s="2"/>
-      <c r="Q231" s="2"/>
-      <c r="R231" s="2"/>
-      <c r="S231" s="2"/>
-      <c r="T231" s="5"/>
+      <c r="A231" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B231" s="8">
+        <v>9300</v>
+      </c>
+      <c r="C231" s="8"/>
+      <c r="D231" s="8"/>
+      <c r="E231" s="8"/>
+      <c r="F231" s="8"/>
+      <c r="G231" s="8"/>
+      <c r="H231" s="8"/>
+      <c r="I231" s="8"/>
+      <c r="J231" s="8"/>
+      <c r="K231" s="8"/>
+      <c r="L231" s="8"/>
+      <c r="M231" s="8"/>
+      <c r="N231" s="8"/>
+      <c r="O231" s="8"/>
+      <c r="P231" s="8"/>
+      <c r="Q231" s="8"/>
+      <c r="R231" s="8"/>
+      <c r="S231" s="8"/>
+      <c r="T231" s="14"/>
       <c r="U231">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A232" s="29"/>
+      <c r="A232" s="23"/>
       <c r="B232" s="2">
-        <v>7343</v>
+        <v>3951</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -7370,9 +7370,9 @@
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A233" s="29"/>
+      <c r="A233" s="23"/>
       <c r="B233" s="2">
-        <v>7060</v>
+        <v>7343</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
@@ -7398,9 +7398,9 @@
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A234" s="29"/>
+      <c r="A234" s="23"/>
       <c r="B234" s="2">
-        <v>6409</v>
+        <v>7060</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
@@ -7426,9 +7426,9 @@
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A235" s="29"/>
+      <c r="A235" s="23"/>
       <c r="B235" s="2">
-        <v>2386</v>
+        <v>6409</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -7453,10 +7453,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="29"/>
-      <c r="B236" s="6">
-        <v>7372</v>
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A236" s="23"/>
+      <c r="B236" s="2">
+        <v>2386</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
@@ -7476,11 +7476,15 @@
       <c r="R236" s="2"/>
       <c r="S236" s="2"/>
       <c r="T236" s="5"/>
-    </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A237" s="29"/>
-      <c r="B237" s="2">
-        <v>9159</v>
+      <c r="U236">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="23"/>
+      <c r="B237" s="6">
+        <v>7372</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
@@ -7500,15 +7504,11 @@
       <c r="R237" s="2"/>
       <c r="S237" s="2"/>
       <c r="T237" s="5"/>
-      <c r="U237">
-        <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="29"/>
+      <c r="A238" s="23"/>
       <c r="B238" s="2">
-        <v>5309</v>
+        <v>9159</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -7534,9 +7534,9 @@
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="29"/>
+      <c r="A239" s="23"/>
       <c r="B239" s="2">
-        <v>3290</v>
+        <v>5309</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -7562,9 +7562,9 @@
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A240" s="29"/>
+      <c r="A240" s="23"/>
       <c r="B240" s="2">
-        <v>5345</v>
+        <v>3290</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
@@ -7589,96 +7589,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="30"/>
-      <c r="B241" s="6">
-        <v>6812</v>
-      </c>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="6"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="6"/>
-      <c r="J241" s="6"/>
-      <c r="K241" s="6"/>
-      <c r="L241" s="6"/>
-      <c r="M241" s="6"/>
-      <c r="N241" s="6"/>
-      <c r="O241" s="6"/>
-      <c r="P241" s="6"/>
-      <c r="Q241" s="6"/>
-      <c r="R241" s="6"/>
-      <c r="S241" s="6"/>
-      <c r="T241" s="7"/>
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A241" s="23"/>
+      <c r="B241" s="2">
+        <v>5345</v>
+      </c>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="2"/>
+      <c r="N241" s="2"/>
+      <c r="O241" s="2"/>
+      <c r="P241" s="2"/>
+      <c r="Q241" s="2"/>
+      <c r="R241" s="2"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="5"/>
       <c r="U241">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B242" s="13">
-        <v>3939</v>
-      </c>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8"/>
-      <c r="H242" s="8"/>
-      <c r="I242" s="8"/>
-      <c r="J242" s="8"/>
-      <c r="K242" s="8"/>
-      <c r="L242" s="8"/>
-      <c r="M242" s="8"/>
-      <c r="N242" s="8"/>
-      <c r="O242" s="8"/>
-      <c r="P242" s="8"/>
-      <c r="Q242" s="8"/>
-      <c r="R242" s="8"/>
-      <c r="S242" s="8"/>
-      <c r="T242" s="14"/>
+    <row r="242" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="24"/>
+      <c r="B242" s="6">
+        <v>6812</v>
+      </c>
+      <c r="C242" s="6"/>
+      <c r="D242" s="6"/>
+      <c r="E242" s="6"/>
+      <c r="F242" s="6"/>
+      <c r="G242" s="6"/>
+      <c r="H242" s="6"/>
+      <c r="I242" s="6"/>
+      <c r="J242" s="6"/>
+      <c r="K242" s="6"/>
+      <c r="L242" s="6"/>
+      <c r="M242" s="6"/>
+      <c r="N242" s="6"/>
+      <c r="O242" s="6"/>
+      <c r="P242" s="6"/>
+      <c r="Q242" s="6"/>
+      <c r="R242" s="6"/>
+      <c r="S242" s="6"/>
+      <c r="T242" s="7"/>
       <c r="U242">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A243" s="29"/>
-      <c r="B243" s="12">
-        <v>1516</v>
-      </c>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
-      <c r="G243" s="2"/>
-      <c r="H243" s="2"/>
-      <c r="I243" s="2"/>
-      <c r="J243" s="2"/>
-      <c r="K243" s="2"/>
-      <c r="L243" s="2"/>
-      <c r="M243" s="2"/>
-      <c r="N243" s="2"/>
-      <c r="O243" s="2"/>
-      <c r="P243" s="2"/>
-      <c r="Q243" s="2"/>
-      <c r="R243" s="2"/>
-      <c r="S243" s="2"/>
-      <c r="T243" s="5"/>
+      <c r="A243" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B243" s="13">
+        <v>3939</v>
+      </c>
+      <c r="C243" s="8"/>
+      <c r="D243" s="8"/>
+      <c r="E243" s="8"/>
+      <c r="F243" s="8"/>
+      <c r="G243" s="8"/>
+      <c r="H243" s="8"/>
+      <c r="I243" s="8"/>
+      <c r="J243" s="8"/>
+      <c r="K243" s="8"/>
+      <c r="L243" s="8"/>
+      <c r="M243" s="8"/>
+      <c r="N243" s="8"/>
+      <c r="O243" s="8"/>
+      <c r="P243" s="8"/>
+      <c r="Q243" s="8"/>
+      <c r="R243" s="8"/>
+      <c r="S243" s="8"/>
+      <c r="T243" s="14"/>
       <c r="U243">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A244" s="29"/>
+      <c r="A244" s="23"/>
       <c r="B244" s="12">
-        <v>9062</v>
+        <v>1516</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
@@ -7703,10 +7703,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A245" s="29"/>
-      <c r="B245" s="19">
-        <v>8861</v>
+    <row r="245" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A245" s="23"/>
+      <c r="B245" s="12">
+        <v>9062</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
@@ -7732,9 +7732,9 @@
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="29"/>
-      <c r="B246" s="2">
-        <v>5164</v>
+      <c r="A246" s="23"/>
+      <c r="B246" s="19">
+        <v>8861</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
@@ -7760,9 +7760,9 @@
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="29"/>
+      <c r="A247" s="23"/>
       <c r="B247" s="2">
-        <v>2354</v>
+        <v>5164</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
@@ -7788,9 +7788,9 @@
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A248" s="29"/>
+      <c r="A248" s="23"/>
       <c r="B248" s="2">
-        <v>2030</v>
+        <v>2354</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -7815,96 +7815,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="30"/>
-      <c r="B249" s="6">
-        <v>7649</v>
-      </c>
-      <c r="C249" s="6"/>
-      <c r="D249" s="6"/>
-      <c r="E249" s="6"/>
-      <c r="F249" s="6"/>
-      <c r="G249" s="6"/>
-      <c r="H249" s="6"/>
-      <c r="I249" s="6"/>
-      <c r="J249" s="6"/>
-      <c r="K249" s="6"/>
-      <c r="L249" s="6"/>
-      <c r="M249" s="6"/>
-      <c r="N249" s="6"/>
-      <c r="O249" s="6"/>
-      <c r="P249" s="6"/>
-      <c r="Q249" s="6"/>
-      <c r="R249" s="6"/>
-      <c r="S249" s="6"/>
-      <c r="T249" s="7"/>
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A249" s="23"/>
+      <c r="B249" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C249" s="2"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+      <c r="G249" s="2"/>
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+      <c r="L249" s="2"/>
+      <c r="M249" s="2"/>
+      <c r="N249" s="2"/>
+      <c r="O249" s="2"/>
+      <c r="P249" s="2"/>
+      <c r="Q249" s="2"/>
+      <c r="R249" s="2"/>
+      <c r="S249" s="2"/>
+      <c r="T249" s="5"/>
       <c r="U249">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A250" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B250" s="8">
-        <v>9701</v>
-      </c>
-      <c r="C250" s="8"/>
-      <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
-      <c r="F250" s="8"/>
-      <c r="G250" s="8"/>
-      <c r="H250" s="8"/>
-      <c r="I250" s="8"/>
-      <c r="J250" s="8"/>
-      <c r="K250" s="8"/>
-      <c r="L250" s="8"/>
-      <c r="M250" s="8"/>
-      <c r="N250" s="8"/>
-      <c r="O250" s="8"/>
-      <c r="P250" s="8"/>
-      <c r="Q250" s="8"/>
-      <c r="R250" s="8"/>
-      <c r="S250" s="8"/>
-      <c r="T250" s="14"/>
+    <row r="250" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="24"/>
+      <c r="B250" s="6">
+        <v>7649</v>
+      </c>
+      <c r="C250" s="6"/>
+      <c r="D250" s="6"/>
+      <c r="E250" s="6"/>
+      <c r="F250" s="6"/>
+      <c r="G250" s="6"/>
+      <c r="H250" s="6"/>
+      <c r="I250" s="6"/>
+      <c r="J250" s="6"/>
+      <c r="K250" s="6"/>
+      <c r="L250" s="6"/>
+      <c r="M250" s="6"/>
+      <c r="N250" s="6"/>
+      <c r="O250" s="6"/>
+      <c r="P250" s="6"/>
+      <c r="Q250" s="6"/>
+      <c r="R250" s="6"/>
+      <c r="S250" s="6"/>
+      <c r="T250" s="7"/>
       <c r="U250">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="29"/>
-      <c r="B251" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C251" s="2"/>
-      <c r="D251" s="2"/>
-      <c r="E251" s="2"/>
-      <c r="F251" s="2"/>
-      <c r="G251" s="2"/>
-      <c r="H251" s="2"/>
-      <c r="I251" s="2"/>
-      <c r="J251" s="2"/>
-      <c r="K251" s="2"/>
-      <c r="L251" s="2"/>
-      <c r="M251" s="2"/>
-      <c r="N251" s="2"/>
-      <c r="O251" s="2"/>
-      <c r="P251" s="2"/>
-      <c r="Q251" s="2"/>
-      <c r="R251" s="2"/>
-      <c r="S251" s="2"/>
-      <c r="T251" s="5"/>
+      <c r="A251" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B251" s="8">
+        <v>9701</v>
+      </c>
+      <c r="C251" s="8"/>
+      <c r="D251" s="8"/>
+      <c r="E251" s="8"/>
+      <c r="F251" s="8"/>
+      <c r="G251" s="8"/>
+      <c r="H251" s="8"/>
+      <c r="I251" s="8"/>
+      <c r="J251" s="8"/>
+      <c r="K251" s="8"/>
+      <c r="L251" s="8"/>
+      <c r="M251" s="8"/>
+      <c r="N251" s="8"/>
+      <c r="O251" s="8"/>
+      <c r="P251" s="8"/>
+      <c r="Q251" s="8"/>
+      <c r="R251" s="8"/>
+      <c r="S251" s="8"/>
+      <c r="T251" s="14"/>
       <c r="U251">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A252" s="29"/>
+      <c r="A252" s="23"/>
       <c r="B252" s="2">
-        <v>6732</v>
+        <v>3784</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
@@ -7930,9 +7930,9 @@
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A253" s="29"/>
+      <c r="A253" s="23"/>
       <c r="B253" s="2">
-        <v>6882</v>
+        <v>6732</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7958,9 +7958,9 @@
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" s="29"/>
+      <c r="A254" s="23"/>
       <c r="B254" s="2">
-        <v>1212</v>
+        <v>6882</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7986,9 +7986,9 @@
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A255" s="29"/>
+      <c r="A255" s="23"/>
       <c r="B255" s="2">
-        <v>9472</v>
+        <v>1212</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8014,9 +8014,9 @@
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="29"/>
+      <c r="A256" s="23"/>
       <c r="B256" s="2">
-        <v>5081</v>
+        <v>9472</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8041,96 +8041,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A257" s="30"/>
-      <c r="B257" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C257" s="6"/>
-      <c r="D257" s="6"/>
-      <c r="E257" s="6"/>
-      <c r="F257" s="6"/>
-      <c r="G257" s="6"/>
-      <c r="H257" s="6"/>
-      <c r="I257" s="6"/>
-      <c r="J257" s="6"/>
-      <c r="K257" s="6"/>
-      <c r="L257" s="6"/>
-      <c r="M257" s="6"/>
-      <c r="N257" s="6"/>
-      <c r="O257" s="6"/>
-      <c r="P257" s="6"/>
-      <c r="Q257" s="6"/>
-      <c r="R257" s="6"/>
-      <c r="S257" s="6"/>
-      <c r="T257" s="7"/>
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A257" s="23"/>
+      <c r="B257" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C257" s="2"/>
+      <c r="D257" s="2"/>
+      <c r="E257" s="2"/>
+      <c r="F257" s="2"/>
+      <c r="G257" s="2"/>
+      <c r="H257" s="2"/>
+      <c r="I257" s="2"/>
+      <c r="J257" s="2"/>
+      <c r="K257" s="2"/>
+      <c r="L257" s="2"/>
+      <c r="M257" s="2"/>
+      <c r="N257" s="2"/>
+      <c r="O257" s="2"/>
+      <c r="P257" s="2"/>
+      <c r="Q257" s="2"/>
+      <c r="R257" s="2"/>
+      <c r="S257" s="2"/>
+      <c r="T257" s="5"/>
       <c r="U257">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A258" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B258" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C258" s="8"/>
-      <c r="D258" s="8"/>
-      <c r="E258" s="8"/>
-      <c r="F258" s="8"/>
-      <c r="G258" s="8"/>
-      <c r="H258" s="8"/>
-      <c r="I258" s="8"/>
-      <c r="J258" s="8"/>
-      <c r="K258" s="8"/>
-      <c r="L258" s="8"/>
-      <c r="M258" s="8"/>
-      <c r="N258" s="8"/>
-      <c r="O258" s="8"/>
-      <c r="P258" s="8"/>
-      <c r="Q258" s="8"/>
-      <c r="R258" s="8"/>
-      <c r="S258" s="8"/>
-      <c r="T258" s="14"/>
+    <row r="258" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="24"/>
+      <c r="B258" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C258" s="6"/>
+      <c r="D258" s="6"/>
+      <c r="E258" s="6"/>
+      <c r="F258" s="6"/>
+      <c r="G258" s="6"/>
+      <c r="H258" s="6"/>
+      <c r="I258" s="6"/>
+      <c r="J258" s="6"/>
+      <c r="K258" s="6"/>
+      <c r="L258" s="6"/>
+      <c r="M258" s="6"/>
+      <c r="N258" s="6"/>
+      <c r="O258" s="6"/>
+      <c r="P258" s="6"/>
+      <c r="Q258" s="6"/>
+      <c r="R258" s="6"/>
+      <c r="S258" s="6"/>
+      <c r="T258" s="7"/>
       <c r="U258">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A259" s="29"/>
-      <c r="B259" s="2">
-        <v>6011</v>
-      </c>
-      <c r="C259" s="2"/>
-      <c r="D259" s="2"/>
-      <c r="E259" s="2"/>
-      <c r="F259" s="2"/>
-      <c r="G259" s="2"/>
-      <c r="H259" s="2"/>
-      <c r="I259" s="2"/>
-      <c r="J259" s="2"/>
-      <c r="K259" s="2"/>
-      <c r="L259" s="2"/>
-      <c r="M259" s="2"/>
-      <c r="N259" s="2"/>
-      <c r="O259" s="2"/>
-      <c r="P259" s="2"/>
-      <c r="Q259" s="2"/>
-      <c r="R259" s="2"/>
-      <c r="S259" s="2"/>
-      <c r="T259" s="5"/>
+    <row r="259" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A259" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B259" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C259" s="8"/>
+      <c r="D259" s="8"/>
+      <c r="E259" s="8"/>
+      <c r="F259" s="8"/>
+      <c r="G259" s="8"/>
+      <c r="H259" s="8"/>
+      <c r="I259" s="8"/>
+      <c r="J259" s="8"/>
+      <c r="K259" s="8"/>
+      <c r="L259" s="8"/>
+      <c r="M259" s="8"/>
+      <c r="N259" s="8"/>
+      <c r="O259" s="8"/>
+      <c r="P259" s="8"/>
+      <c r="Q259" s="8"/>
+      <c r="R259" s="8"/>
+      <c r="S259" s="8"/>
+      <c r="T259" s="14"/>
       <c r="U259">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="29"/>
+      <c r="A260" s="23"/>
       <c r="B260" s="2">
-        <v>8403</v>
+        <v>6011</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -8156,9 +8156,9 @@
       </c>
     </row>
     <row r="261" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A261" s="29"/>
+      <c r="A261" s="23"/>
       <c r="B261" s="2">
-        <v>3185</v>
+        <v>8403</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -8184,9 +8184,9 @@
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="29"/>
-      <c r="B262" s="21">
-        <v>6037</v>
+      <c r="A262" s="23"/>
+      <c r="B262" s="2">
+        <v>3185</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8212,9 +8212,9 @@
       </c>
     </row>
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A263" s="29"/>
-      <c r="B263" s="2">
-        <v>9914</v>
+      <c r="A263" s="23"/>
+      <c r="B263" s="21">
+        <v>6037</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8240,9 +8240,9 @@
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A264" s="29"/>
+      <c r="A264" s="23"/>
       <c r="B264" s="2">
-        <v>4916</v>
+        <v>9914</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8268,9 +8268,9 @@
       </c>
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A265" s="29"/>
+      <c r="A265" s="23"/>
       <c r="B265" s="2">
-        <v>2809</v>
+        <v>4916</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8296,9 +8296,9 @@
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="29"/>
+      <c r="A266" s="23"/>
       <c r="B266" s="2">
-        <v>8265</v>
+        <v>2809</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8324,9 +8324,9 @@
       </c>
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="29"/>
+      <c r="A267" s="23"/>
       <c r="B267" s="2">
-        <v>2092</v>
+        <v>8265</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8352,9 +8352,9 @@
       </c>
     </row>
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="29"/>
+      <c r="A268" s="23"/>
       <c r="B268" s="2">
-        <v>7297</v>
+        <v>2092</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8380,9 +8380,9 @@
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="29"/>
+      <c r="A269" s="23"/>
       <c r="B269" s="2">
-        <v>5242</v>
+        <v>7297</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8408,9 +8408,9 @@
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="29"/>
+      <c r="A270" s="23"/>
       <c r="B270" s="2">
-        <v>1379</v>
+        <v>5242</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8436,9 +8436,9 @@
       </c>
     </row>
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A271" s="29"/>
+      <c r="A271" s="23"/>
       <c r="B271" s="2">
-        <v>2401</v>
+        <v>1379</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8464,9 +8464,9 @@
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="29"/>
+      <c r="A272" s="23"/>
       <c r="B272" s="2">
-        <v>5421</v>
+        <v>2401</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8492,9 +8492,9 @@
       </c>
     </row>
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="29"/>
+      <c r="A273" s="23"/>
       <c r="B273" s="2">
-        <v>9713</v>
+        <v>5421</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8520,9 +8520,9 @@
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="29"/>
+      <c r="A274" s="23"/>
       <c r="B274" s="2">
-        <v>7301</v>
+        <v>9713</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8548,9 +8548,9 @@
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="29"/>
+      <c r="A275" s="23"/>
       <c r="B275" s="2">
-        <v>2000</v>
+        <v>7301</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8576,9 +8576,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="29"/>
+      <c r="A276" s="23"/>
       <c r="B276" s="2">
-        <v>5449</v>
+        <v>2000</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8604,9 +8604,9 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="29"/>
+      <c r="A277" s="23"/>
       <c r="B277" s="2">
-        <v>9238</v>
+        <v>5449</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8632,9 +8632,9 @@
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A278" s="29"/>
+      <c r="A278" s="23"/>
       <c r="B278" s="2">
-        <v>2662</v>
+        <v>9238</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8660,9 +8660,9 @@
       </c>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="29"/>
+      <c r="A279" s="23"/>
       <c r="B279" s="2">
-        <v>4147</v>
+        <v>2662</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8688,9 +8688,9 @@
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="29"/>
+      <c r="A280" s="23"/>
       <c r="B280" s="2">
-        <v>1953</v>
+        <v>4147</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8716,9 +8716,9 @@
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="29"/>
+      <c r="A281" s="23"/>
       <c r="B281" s="2">
-        <v>3956</v>
+        <v>1953</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8744,9 +8744,9 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="29"/>
+      <c r="A282" s="23"/>
       <c r="B282" s="2">
-        <v>5032</v>
+        <v>3956</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8772,9 +8772,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="29"/>
+      <c r="A283" s="23"/>
       <c r="B283" s="2">
-        <v>3567</v>
+        <v>5032</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8800,9 +8800,9 @@
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="29"/>
+      <c r="A284" s="23"/>
       <c r="B284" s="2">
-        <v>5108</v>
+        <v>3567</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8828,9 +8828,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="29"/>
+      <c r="A285" s="23"/>
       <c r="B285" s="2">
-        <v>2033</v>
+        <v>5108</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8856,9 +8856,9 @@
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="29"/>
+      <c r="A286" s="23"/>
       <c r="B286" s="2">
-        <v>6981</v>
+        <v>2033</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8883,96 +8883,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="30"/>
-      <c r="B287" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C287" s="6"/>
-      <c r="D287" s="6"/>
-      <c r="E287" s="6"/>
-      <c r="F287" s="6"/>
-      <c r="G287" s="6"/>
-      <c r="H287" s="6"/>
-      <c r="I287" s="6"/>
-      <c r="J287" s="6"/>
-      <c r="K287" s="6"/>
-      <c r="L287" s="6"/>
-      <c r="M287" s="6"/>
-      <c r="N287" s="6"/>
-      <c r="O287" s="6"/>
-      <c r="P287" s="6"/>
-      <c r="Q287" s="6"/>
-      <c r="R287" s="6"/>
-      <c r="S287" s="6"/>
-      <c r="T287" s="7"/>
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A287" s="23"/>
+      <c r="B287" s="2">
+        <v>6981</v>
+      </c>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
+      <c r="E287" s="2"/>
+      <c r="F287" s="2"/>
+      <c r="G287" s="2"/>
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+      <c r="J287" s="2"/>
+      <c r="K287" s="2"/>
+      <c r="L287" s="2"/>
+      <c r="M287" s="2"/>
+      <c r="N287" s="2"/>
+      <c r="O287" s="2"/>
+      <c r="P287" s="2"/>
+      <c r="Q287" s="2"/>
+      <c r="R287" s="2"/>
+      <c r="S287" s="2"/>
+      <c r="T287" s="5"/>
       <c r="U287">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A288" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B288" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C288" s="8"/>
-      <c r="D288" s="8"/>
-      <c r="E288" s="8"/>
-      <c r="F288" s="8"/>
-      <c r="G288" s="8"/>
-      <c r="H288" s="8"/>
-      <c r="I288" s="8"/>
-      <c r="J288" s="8"/>
-      <c r="K288" s="8"/>
-      <c r="L288" s="8"/>
-      <c r="M288" s="8"/>
-      <c r="N288" s="8"/>
-      <c r="O288" s="8"/>
-      <c r="P288" s="8"/>
-      <c r="Q288" s="8"/>
-      <c r="R288" s="8"/>
-      <c r="S288" s="8"/>
-      <c r="T288" s="14"/>
+    <row r="288" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="24"/>
+      <c r="B288" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C288" s="6"/>
+      <c r="D288" s="6"/>
+      <c r="E288" s="6"/>
+      <c r="F288" s="6"/>
+      <c r="G288" s="6"/>
+      <c r="H288" s="6"/>
+      <c r="I288" s="6"/>
+      <c r="J288" s="6"/>
+      <c r="K288" s="6"/>
+      <c r="L288" s="6"/>
+      <c r="M288" s="6"/>
+      <c r="N288" s="6"/>
+      <c r="O288" s="6"/>
+      <c r="P288" s="6"/>
+      <c r="Q288" s="6"/>
+      <c r="R288" s="6"/>
+      <c r="S288" s="6"/>
+      <c r="T288" s="7"/>
       <c r="U288">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="29"/>
+      <c r="A289" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="B289" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="E289" s="2"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
-      <c r="I289" s="2"/>
-      <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-      <c r="N289" s="2"/>
-      <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-      <c r="Q289" s="2"/>
-      <c r="R289" s="2"/>
-      <c r="S289" s="2"/>
-      <c r="T289" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C289" s="8"/>
+      <c r="D289" s="8"/>
+      <c r="E289" s="8"/>
+      <c r="F289" s="8"/>
+      <c r="G289" s="8"/>
+      <c r="H289" s="8"/>
+      <c r="I289" s="8"/>
+      <c r="J289" s="8"/>
+      <c r="K289" s="8"/>
+      <c r="L289" s="8"/>
+      <c r="M289" s="8"/>
+      <c r="N289" s="8"/>
+      <c r="O289" s="8"/>
+      <c r="P289" s="8"/>
+      <c r="Q289" s="8"/>
+      <c r="R289" s="8"/>
+      <c r="S289" s="8"/>
+      <c r="T289" s="14"/>
       <c r="U289">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="29"/>
+      <c r="A290" s="23"/>
       <c r="B290" s="2">
-        <v>9990</v>
+        <v>1056</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -8998,9 +8998,9 @@
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A291" s="29"/>
+      <c r="A291" s="23"/>
       <c r="B291" s="2">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -9026,9 +9026,9 @@
       </c>
     </row>
     <row r="292" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A292" s="29"/>
+      <c r="A292" s="23"/>
       <c r="B292" s="2">
-        <v>8418</v>
+        <v>7738</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9054,9 +9054,9 @@
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="29"/>
+      <c r="A293" s="23"/>
       <c r="B293" s="2">
-        <v>9512</v>
+        <v>8418</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9082,9 +9082,9 @@
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="29"/>
+      <c r="A294" s="23"/>
       <c r="B294" s="2">
-        <v>9924</v>
+        <v>9512</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9110,28 +9110,28 @@
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="31"/>
-      <c r="B295" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C295" s="9"/>
-      <c r="D295" s="9"/>
-      <c r="E295" s="9"/>
-      <c r="F295" s="9"/>
-      <c r="G295" s="9"/>
-      <c r="H295" s="9"/>
-      <c r="I295" s="9"/>
-      <c r="J295" s="9"/>
-      <c r="K295" s="9"/>
-      <c r="L295" s="9"/>
-      <c r="M295" s="9"/>
-      <c r="N295" s="9"/>
-      <c r="O295" s="9"/>
-      <c r="P295" s="9"/>
-      <c r="Q295" s="9"/>
-      <c r="R295" s="9"/>
-      <c r="S295" s="9"/>
-      <c r="T295" s="15"/>
+      <c r="A295" s="23"/>
+      <c r="B295" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C295" s="2"/>
+      <c r="D295" s="2"/>
+      <c r="E295" s="2"/>
+      <c r="F295" s="2"/>
+      <c r="G295" s="2"/>
+      <c r="H295" s="2"/>
+      <c r="I295" s="2"/>
+      <c r="J295" s="2"/>
+      <c r="K295" s="2"/>
+      <c r="L295" s="2"/>
+      <c r="M295" s="2"/>
+      <c r="N295" s="2"/>
+      <c r="O295" s="2"/>
+      <c r="P295" s="2"/>
+      <c r="Q295" s="2"/>
+      <c r="R295" s="2"/>
+      <c r="S295" s="2"/>
+      <c r="T295" s="5"/>
       <c r="U295">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9140,7 +9140,7 @@
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="31"/>
       <c r="B296" s="9">
-        <v>2973</v>
+        <v>7657</v>
       </c>
       <c r="C296" s="9"/>
       <c r="D296" s="9"/>
@@ -9168,7 +9168,7 @@
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="31"/>
       <c r="B297" s="9">
-        <v>8258</v>
+        <v>2973</v>
       </c>
       <c r="C297" s="9"/>
       <c r="D297" s="9"/>
@@ -9196,7 +9196,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="31"/>
       <c r="B298" s="9">
-        <v>7186</v>
+        <v>8258</v>
       </c>
       <c r="C298" s="9"/>
       <c r="D298" s="9"/>
@@ -9224,7 +9224,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="31"/>
       <c r="B299" s="9">
-        <v>1457</v>
+        <v>7186</v>
       </c>
       <c r="C299" s="9"/>
       <c r="D299" s="9"/>
@@ -9249,96 +9249,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="30"/>
-      <c r="B300" s="6">
+    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A300" s="31"/>
+      <c r="B300" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C300" s="9"/>
+      <c r="D300" s="9"/>
+      <c r="E300" s="9"/>
+      <c r="F300" s="9"/>
+      <c r="G300" s="9"/>
+      <c r="H300" s="9"/>
+      <c r="I300" s="9"/>
+      <c r="J300" s="9"/>
+      <c r="K300" s="9"/>
+      <c r="L300" s="9"/>
+      <c r="M300" s="9"/>
+      <c r="N300" s="9"/>
+      <c r="O300" s="9"/>
+      <c r="P300" s="9"/>
+      <c r="Q300" s="9"/>
+      <c r="R300" s="9"/>
+      <c r="S300" s="9"/>
+      <c r="T300" s="15"/>
+      <c r="U300">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="24"/>
+      <c r="B301" s="6">
         <v>6876</v>
       </c>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-      <c r="E300" s="6"/>
-      <c r="F300" s="6"/>
-      <c r="G300" s="6"/>
-      <c r="H300" s="6"/>
-      <c r="I300" s="6"/>
-      <c r="J300" s="6"/>
-      <c r="K300" s="6"/>
-      <c r="L300" s="6"/>
-      <c r="M300" s="6"/>
-      <c r="N300" s="6"/>
-      <c r="O300" s="6"/>
-      <c r="P300" s="6"/>
-      <c r="Q300" s="6"/>
-      <c r="R300" s="6"/>
-      <c r="S300" s="6"/>
-      <c r="T300" s="7"/>
-      <c r="U300">
-        <f t="shared" ref="U300:U363" ca="1" si="7">IF(B300=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A301" s="28" t="s">
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
+      <c r="H301" s="6"/>
+      <c r="I301" s="6"/>
+      <c r="J301" s="6"/>
+      <c r="K301" s="6"/>
+      <c r="L301" s="6"/>
+      <c r="M301" s="6"/>
+      <c r="N301" s="6"/>
+      <c r="O301" s="6"/>
+      <c r="P301" s="6"/>
+      <c r="Q301" s="6"/>
+      <c r="R301" s="6"/>
+      <c r="S301" s="6"/>
+      <c r="T301" s="7"/>
+      <c r="U301">
+        <f t="shared" ref="U301:U364" ca="1" si="7">IF(B301=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A302" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B301" s="8">
+      <c r="B302" s="8">
         <v>4304</v>
       </c>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
-      <c r="F301" s="8"/>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-      <c r="K301" s="8"/>
-      <c r="L301" s="8"/>
-      <c r="M301" s="8"/>
-      <c r="N301" s="8"/>
-      <c r="O301" s="8"/>
-      <c r="P301" s="8"/>
-      <c r="Q301" s="8"/>
-      <c r="R301" s="8"/>
-      <c r="S301" s="8"/>
-      <c r="T301" s="14"/>
-      <c r="U301">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A302" s="29"/>
-      <c r="B302" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2"/>
-      <c r="E302" s="2"/>
-      <c r="F302" s="2"/>
-      <c r="G302" s="2"/>
-      <c r="H302" s="2"/>
-      <c r="I302" s="2"/>
-      <c r="J302" s="2"/>
-      <c r="K302" s="2"/>
-      <c r="L302" s="2"/>
-      <c r="M302" s="2"/>
-      <c r="N302" s="2"/>
-      <c r="O302" s="2"/>
-      <c r="P302" s="2"/>
-      <c r="Q302" s="2"/>
-      <c r="R302" s="2"/>
-      <c r="S302" s="2"/>
-      <c r="T302" s="5"/>
+      <c r="C302" s="8"/>
+      <c r="D302" s="8"/>
+      <c r="E302" s="8"/>
+      <c r="F302" s="8"/>
+      <c r="G302" s="8"/>
+      <c r="H302" s="8"/>
+      <c r="I302" s="8"/>
+      <c r="J302" s="8"/>
+      <c r="K302" s="8"/>
+      <c r="L302" s="8"/>
+      <c r="M302" s="8"/>
+      <c r="N302" s="8"/>
+      <c r="O302" s="8"/>
+      <c r="P302" s="8"/>
+      <c r="Q302" s="8"/>
+      <c r="R302" s="8"/>
+      <c r="S302" s="8"/>
+      <c r="T302" s="14"/>
       <c r="U302">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A303" s="29"/>
+      <c r="A303" s="23"/>
       <c r="B303" s="2">
-        <v>7693</v>
+        <v>2070</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9364,9 +9364,9 @@
       </c>
     </row>
     <row r="304" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A304" s="29"/>
+      <c r="A304" s="23"/>
       <c r="B304" s="2">
-        <v>8718</v>
+        <v>7693</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9391,96 +9391,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="30"/>
-      <c r="B305" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C305" s="6"/>
-      <c r="D305" s="6"/>
-      <c r="E305" s="6"/>
-      <c r="F305" s="6"/>
-      <c r="G305" s="6"/>
-      <c r="H305" s="6"/>
-      <c r="I305" s="6"/>
-      <c r="J305" s="6"/>
-      <c r="K305" s="6"/>
-      <c r="L305" s="6"/>
-      <c r="M305" s="6"/>
-      <c r="N305" s="6"/>
-      <c r="O305" s="6"/>
-      <c r="P305" s="6"/>
-      <c r="Q305" s="6"/>
-      <c r="R305" s="6"/>
-      <c r="S305" s="6"/>
-      <c r="T305" s="7"/>
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A305" s="23"/>
+      <c r="B305" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C305" s="2"/>
+      <c r="D305" s="2"/>
+      <c r="E305" s="2"/>
+      <c r="F305" s="2"/>
+      <c r="G305" s="2"/>
+      <c r="H305" s="2"/>
+      <c r="I305" s="2"/>
+      <c r="J305" s="2"/>
+      <c r="K305" s="2"/>
+      <c r="L305" s="2"/>
+      <c r="M305" s="2"/>
+      <c r="N305" s="2"/>
+      <c r="O305" s="2"/>
+      <c r="P305" s="2"/>
+      <c r="Q305" s="2"/>
+      <c r="R305" s="2"/>
+      <c r="S305" s="2"/>
+      <c r="T305" s="5"/>
       <c r="U305">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A306" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B306" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C306" s="8"/>
-      <c r="D306" s="8"/>
-      <c r="E306" s="8"/>
-      <c r="F306" s="8"/>
-      <c r="G306" s="8"/>
-      <c r="H306" s="8"/>
-      <c r="I306" s="8"/>
-      <c r="J306" s="8"/>
-      <c r="K306" s="8"/>
-      <c r="L306" s="8"/>
-      <c r="M306" s="8"/>
-      <c r="N306" s="8"/>
-      <c r="O306" s="8"/>
-      <c r="P306" s="8"/>
-      <c r="Q306" s="8"/>
-      <c r="R306" s="8"/>
-      <c r="S306" s="8"/>
-      <c r="T306" s="14"/>
+    <row r="306" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="24"/>
+      <c r="B306" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C306" s="6"/>
+      <c r="D306" s="6"/>
+      <c r="E306" s="6"/>
+      <c r="F306" s="6"/>
+      <c r="G306" s="6"/>
+      <c r="H306" s="6"/>
+      <c r="I306" s="6"/>
+      <c r="J306" s="6"/>
+      <c r="K306" s="6"/>
+      <c r="L306" s="6"/>
+      <c r="M306" s="6"/>
+      <c r="N306" s="6"/>
+      <c r="O306" s="6"/>
+      <c r="P306" s="6"/>
+      <c r="Q306" s="6"/>
+      <c r="R306" s="6"/>
+      <c r="S306" s="6"/>
+      <c r="T306" s="7"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A307" s="29"/>
-      <c r="B307" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2"/>
-      <c r="E307" s="2"/>
-      <c r="F307" s="2"/>
-      <c r="G307" s="2"/>
-      <c r="H307" s="2"/>
-      <c r="I307" s="2"/>
-      <c r="J307" s="2"/>
-      <c r="K307" s="2"/>
-      <c r="L307" s="2"/>
-      <c r="M307" s="2"/>
-      <c r="N307" s="2"/>
-      <c r="O307" s="2"/>
-      <c r="P307" s="2"/>
-      <c r="Q307" s="2"/>
-      <c r="R307" s="2"/>
-      <c r="S307" s="2"/>
-      <c r="T307" s="5"/>
+      <c r="A307" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B307" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C307" s="8"/>
+      <c r="D307" s="8"/>
+      <c r="E307" s="8"/>
+      <c r="F307" s="8"/>
+      <c r="G307" s="8"/>
+      <c r="H307" s="8"/>
+      <c r="I307" s="8"/>
+      <c r="J307" s="8"/>
+      <c r="K307" s="8"/>
+      <c r="L307" s="8"/>
+      <c r="M307" s="8"/>
+      <c r="N307" s="8"/>
+      <c r="O307" s="8"/>
+      <c r="P307" s="8"/>
+      <c r="Q307" s="8"/>
+      <c r="R307" s="8"/>
+      <c r="S307" s="8"/>
+      <c r="T307" s="14"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A308" s="29"/>
+      <c r="A308" s="23"/>
       <c r="B308" s="12">
-        <v>7546</v>
+        <v>3083</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -9505,10 +9505,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A309" s="29"/>
-      <c r="B309" s="2">
-        <v>7170</v>
+    <row r="309" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A309" s="23"/>
+      <c r="B309" s="12">
+        <v>7546</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -9534,9 +9534,9 @@
       </c>
     </row>
     <row r="310" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A310" s="29"/>
+      <c r="A310" s="23"/>
       <c r="B310" s="2">
-        <v>2709</v>
+        <v>7170</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9562,9 +9562,9 @@
       </c>
     </row>
     <row r="311" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A311" s="29"/>
+      <c r="A311" s="23"/>
       <c r="B311" s="2">
-        <v>3402</v>
+        <v>2709</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9590,9 +9590,9 @@
       </c>
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A312" s="29"/>
+      <c r="A312" s="23"/>
       <c r="B312" s="2">
-        <v>8781</v>
+        <v>3402</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -9618,9 +9618,9 @@
       </c>
     </row>
     <row r="313" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A313" s="29"/>
+      <c r="A313" s="23"/>
       <c r="B313" s="2">
-        <v>8771</v>
+        <v>8781</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
@@ -9646,9 +9646,9 @@
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="29"/>
+      <c r="A314" s="23"/>
       <c r="B314" s="2">
-        <v>3091</v>
+        <v>8771</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -9674,9 +9674,9 @@
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="29"/>
+      <c r="A315" s="23"/>
       <c r="B315" s="2">
-        <v>2195</v>
+        <v>3091</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -9702,9 +9702,9 @@
       </c>
     </row>
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A316" s="29"/>
+      <c r="A316" s="23"/>
       <c r="B316" s="2">
-        <v>1184</v>
+        <v>2195</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9730,9 +9730,9 @@
       </c>
     </row>
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A317" s="29"/>
+      <c r="A317" s="23"/>
       <c r="B317" s="2">
-        <v>2667</v>
+        <v>1184</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -9758,9 +9758,9 @@
       </c>
     </row>
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A318" s="29"/>
+      <c r="A318" s="23"/>
       <c r="B318" s="2">
-        <v>5917</v>
+        <v>2667</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -9786,9 +9786,9 @@
       </c>
     </row>
     <row r="319" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A319" s="29"/>
+      <c r="A319" s="23"/>
       <c r="B319" s="2">
-        <v>8545</v>
+        <v>5917</v>
       </c>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
@@ -9814,9 +9814,9 @@
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A320" s="29"/>
+      <c r="A320" s="23"/>
       <c r="B320" s="2">
-        <v>1288</v>
+        <v>8545</v>
       </c>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
@@ -9841,96 +9841,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A321" s="30"/>
-      <c r="B321" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C321" s="6"/>
-      <c r="D321" s="6"/>
-      <c r="E321" s="6"/>
-      <c r="F321" s="6"/>
-      <c r="G321" s="6"/>
-      <c r="H321" s="6"/>
-      <c r="I321" s="6"/>
-      <c r="J321" s="6"/>
-      <c r="K321" s="6"/>
-      <c r="L321" s="6"/>
-      <c r="M321" s="6"/>
-      <c r="N321" s="6"/>
-      <c r="O321" s="6"/>
-      <c r="P321" s="6"/>
-      <c r="Q321" s="6"/>
-      <c r="R321" s="6"/>
-      <c r="S321" s="6"/>
-      <c r="T321" s="7"/>
+    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A321" s="23"/>
+      <c r="B321" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C321" s="2"/>
+      <c r="D321" s="2"/>
+      <c r="E321" s="2"/>
+      <c r="F321" s="2"/>
+      <c r="G321" s="2"/>
+      <c r="H321" s="2"/>
+      <c r="I321" s="2"/>
+      <c r="J321" s="2"/>
+      <c r="K321" s="2"/>
+      <c r="L321" s="2"/>
+      <c r="M321" s="2"/>
+      <c r="N321" s="2"/>
+      <c r="O321" s="2"/>
+      <c r="P321" s="2"/>
+      <c r="Q321" s="2"/>
+      <c r="R321" s="2"/>
+      <c r="S321" s="2"/>
+      <c r="T321" s="5"/>
       <c r="U321">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A322" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B322" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C322" s="8"/>
-      <c r="D322" s="8"/>
-      <c r="E322" s="8"/>
-      <c r="F322" s="8"/>
-      <c r="G322" s="8"/>
-      <c r="H322" s="8"/>
-      <c r="I322" s="8"/>
-      <c r="J322" s="8"/>
-      <c r="K322" s="8"/>
-      <c r="L322" s="8"/>
-      <c r="M322" s="8"/>
-      <c r="N322" s="8"/>
-      <c r="O322" s="8"/>
-      <c r="P322" s="8"/>
-      <c r="Q322" s="8"/>
-      <c r="R322" s="8"/>
-      <c r="S322" s="8"/>
-      <c r="T322" s="14"/>
+    <row r="322" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="24"/>
+      <c r="B322" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C322" s="6"/>
+      <c r="D322" s="6"/>
+      <c r="E322" s="6"/>
+      <c r="F322" s="6"/>
+      <c r="G322" s="6"/>
+      <c r="H322" s="6"/>
+      <c r="I322" s="6"/>
+      <c r="J322" s="6"/>
+      <c r="K322" s="6"/>
+      <c r="L322" s="6"/>
+      <c r="M322" s="6"/>
+      <c r="N322" s="6"/>
+      <c r="O322" s="6"/>
+      <c r="P322" s="6"/>
+      <c r="Q322" s="6"/>
+      <c r="R322" s="6"/>
+      <c r="S322" s="6"/>
+      <c r="T322" s="7"/>
       <c r="U322">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A323" s="29"/>
-      <c r="B323" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C323" s="2"/>
-      <c r="D323" s="2"/>
-      <c r="E323" s="2"/>
-      <c r="F323" s="2"/>
-      <c r="G323" s="2"/>
-      <c r="H323" s="2"/>
-      <c r="I323" s="2"/>
-      <c r="J323" s="2"/>
-      <c r="K323" s="2"/>
-      <c r="L323" s="2"/>
-      <c r="M323" s="2"/>
-      <c r="N323" s="2"/>
-      <c r="O323" s="2"/>
-      <c r="P323" s="2"/>
-      <c r="Q323" s="2"/>
-      <c r="R323" s="2"/>
-      <c r="S323" s="2"/>
-      <c r="T323" s="5"/>
+      <c r="A323" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B323" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C323" s="8"/>
+      <c r="D323" s="8"/>
+      <c r="E323" s="8"/>
+      <c r="F323" s="8"/>
+      <c r="G323" s="8"/>
+      <c r="H323" s="8"/>
+      <c r="I323" s="8"/>
+      <c r="J323" s="8"/>
+      <c r="K323" s="8"/>
+      <c r="L323" s="8"/>
+      <c r="M323" s="8"/>
+      <c r="N323" s="8"/>
+      <c r="O323" s="8"/>
+      <c r="P323" s="8"/>
+      <c r="Q323" s="8"/>
+      <c r="R323" s="8"/>
+      <c r="S323" s="8"/>
+      <c r="T323" s="14"/>
       <c r="U323">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A324" s="29"/>
+      <c r="A324" s="23"/>
       <c r="B324" s="2">
-        <v>3093</v>
+        <v>6598</v>
       </c>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
@@ -9956,9 +9956,9 @@
       </c>
     </row>
     <row r="325" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A325" s="29"/>
+      <c r="A325" s="23"/>
       <c r="B325" s="2">
-        <v>8805</v>
+        <v>3093</v>
       </c>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
@@ -9984,9 +9984,9 @@
       </c>
     </row>
     <row r="326" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A326" s="29"/>
+      <c r="A326" s="23"/>
       <c r="B326" s="2">
-        <v>8158</v>
+        <v>8805</v>
       </c>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
@@ -10011,96 +10011,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A327" s="30"/>
-      <c r="B327" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C327" s="6"/>
-      <c r="D327" s="6"/>
-      <c r="E327" s="6"/>
-      <c r="F327" s="6"/>
-      <c r="G327" s="6"/>
-      <c r="H327" s="6"/>
-      <c r="I327" s="6"/>
-      <c r="J327" s="6"/>
-      <c r="K327" s="6"/>
-      <c r="L327" s="6"/>
-      <c r="M327" s="6"/>
-      <c r="N327" s="6"/>
-      <c r="O327" s="6"/>
-      <c r="P327" s="6"/>
-      <c r="Q327" s="6"/>
-      <c r="R327" s="6"/>
-      <c r="S327" s="6"/>
-      <c r="T327" s="7"/>
+    <row r="327" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A327" s="23"/>
+      <c r="B327" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C327" s="2"/>
+      <c r="D327" s="2"/>
+      <c r="E327" s="2"/>
+      <c r="F327" s="2"/>
+      <c r="G327" s="2"/>
+      <c r="H327" s="2"/>
+      <c r="I327" s="2"/>
+      <c r="J327" s="2"/>
+      <c r="K327" s="2"/>
+      <c r="L327" s="2"/>
+      <c r="M327" s="2"/>
+      <c r="N327" s="2"/>
+      <c r="O327" s="2"/>
+      <c r="P327" s="2"/>
+      <c r="Q327" s="2"/>
+      <c r="R327" s="2"/>
+      <c r="S327" s="2"/>
+      <c r="T327" s="5"/>
       <c r="U327">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A328" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B328" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C328" s="8"/>
-      <c r="D328" s="8"/>
-      <c r="E328" s="8"/>
-      <c r="F328" s="8"/>
-      <c r="G328" s="8"/>
-      <c r="H328" s="8"/>
-      <c r="I328" s="8"/>
-      <c r="J328" s="8"/>
-      <c r="K328" s="8"/>
-      <c r="L328" s="8"/>
-      <c r="M328" s="8"/>
-      <c r="N328" s="8"/>
-      <c r="O328" s="8"/>
-      <c r="P328" s="8"/>
-      <c r="Q328" s="8"/>
-      <c r="R328" s="8"/>
-      <c r="S328" s="8"/>
-      <c r="T328" s="14"/>
+    <row r="328" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A328" s="24"/>
+      <c r="B328" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C328" s="6"/>
+      <c r="D328" s="6"/>
+      <c r="E328" s="6"/>
+      <c r="F328" s="6"/>
+      <c r="G328" s="6"/>
+      <c r="H328" s="6"/>
+      <c r="I328" s="6"/>
+      <c r="J328" s="6"/>
+      <c r="K328" s="6"/>
+      <c r="L328" s="6"/>
+      <c r="M328" s="6"/>
+      <c r="N328" s="6"/>
+      <c r="O328" s="6"/>
+      <c r="P328" s="6"/>
+      <c r="Q328" s="6"/>
+      <c r="R328" s="6"/>
+      <c r="S328" s="6"/>
+      <c r="T328" s="7"/>
       <c r="U328">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A329" s="29"/>
-      <c r="B329" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C329" s="2"/>
-      <c r="D329" s="2"/>
-      <c r="E329" s="2"/>
-      <c r="F329" s="2"/>
-      <c r="G329" s="2"/>
-      <c r="H329" s="2"/>
-      <c r="I329" s="2"/>
-      <c r="J329" s="2"/>
-      <c r="K329" s="2"/>
-      <c r="L329" s="2"/>
-      <c r="M329" s="2"/>
-      <c r="N329" s="2"/>
-      <c r="O329" s="2"/>
-      <c r="P329" s="2"/>
-      <c r="Q329" s="2"/>
-      <c r="R329" s="2"/>
-      <c r="S329" s="2"/>
-      <c r="T329" s="5"/>
+      <c r="A329" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B329" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C329" s="8"/>
+      <c r="D329" s="8"/>
+      <c r="E329" s="8"/>
+      <c r="F329" s="8"/>
+      <c r="G329" s="8"/>
+      <c r="H329" s="8"/>
+      <c r="I329" s="8"/>
+      <c r="J329" s="8"/>
+      <c r="K329" s="8"/>
+      <c r="L329" s="8"/>
+      <c r="M329" s="8"/>
+      <c r="N329" s="8"/>
+      <c r="O329" s="8"/>
+      <c r="P329" s="8"/>
+      <c r="Q329" s="8"/>
+      <c r="R329" s="8"/>
+      <c r="S329" s="8"/>
+      <c r="T329" s="14"/>
       <c r="U329">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A330" s="29"/>
+      <c r="A330" s="23"/>
       <c r="B330" s="2">
-        <v>9002</v>
+        <v>7560</v>
       </c>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
@@ -10126,9 +10126,9 @@
       </c>
     </row>
     <row r="331" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A331" s="29"/>
+      <c r="A331" s="23"/>
       <c r="B331" s="2">
-        <v>7432</v>
+        <v>9002</v>
       </c>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
@@ -10154,9 +10154,9 @@
       </c>
     </row>
     <row r="332" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A332" s="29"/>
+      <c r="A332" s="23"/>
       <c r="B332" s="2">
-        <v>1954</v>
+        <v>7432</v>
       </c>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
@@ -10181,35 +10181,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A333" s="30"/>
-      <c r="B333" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C333" s="6"/>
-      <c r="D333" s="6"/>
-      <c r="E333" s="6"/>
-      <c r="F333" s="6"/>
-      <c r="G333" s="6"/>
-      <c r="H333" s="6"/>
-      <c r="I333" s="6"/>
-      <c r="J333" s="6"/>
-      <c r="K333" s="6"/>
-      <c r="L333" s="6"/>
-      <c r="M333" s="6"/>
-      <c r="N333" s="6"/>
-      <c r="O333" s="6"/>
-      <c r="P333" s="6"/>
-      <c r="Q333" s="6"/>
-      <c r="R333" s="6"/>
-      <c r="S333" s="6"/>
-      <c r="T333" s="7"/>
+    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A333" s="23"/>
+      <c r="B333" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C333" s="2"/>
+      <c r="D333" s="2"/>
+      <c r="E333" s="2"/>
+      <c r="F333" s="2"/>
+      <c r="G333" s="2"/>
+      <c r="H333" s="2"/>
+      <c r="I333" s="2"/>
+      <c r="J333" s="2"/>
+      <c r="K333" s="2"/>
+      <c r="L333" s="2"/>
+      <c r="M333" s="2"/>
+      <c r="N333" s="2"/>
+      <c r="O333" s="2"/>
+      <c r="P333" s="2"/>
+      <c r="Q333" s="2"/>
+      <c r="R333" s="2"/>
+      <c r="S333" s="2"/>
+      <c r="T333" s="5"/>
       <c r="U333">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A334" s="24"/>
+      <c r="B334" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C334" s="6"/>
+      <c r="D334" s="6"/>
+      <c r="E334" s="6"/>
+      <c r="F334" s="6"/>
+      <c r="G334" s="6"/>
+      <c r="H334" s="6"/>
+      <c r="I334" s="6"/>
+      <c r="J334" s="6"/>
+      <c r="K334" s="6"/>
+      <c r="L334" s="6"/>
+      <c r="M334" s="6"/>
+      <c r="N334" s="6"/>
+      <c r="O334" s="6"/>
+      <c r="P334" s="6"/>
+      <c r="Q334" s="6"/>
+      <c r="R334" s="6"/>
+      <c r="S334" s="6"/>
+      <c r="T334" s="7"/>
       <c r="U334">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -10391,13 +10413,13 @@
     </row>
     <row r="364" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U364">
-        <f t="shared" ref="U364:U427" ca="1" si="8">IF(B364=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="365" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U365">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U365:U428" ca="1" si="8">IF(B365=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10775,13 +10797,13 @@
     </row>
     <row r="428" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U428">
-        <f t="shared" ref="U428:U491" ca="1" si="9">IF(B428=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="429" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U429">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U429:U492" ca="1" si="9">IF(B429=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11159,13 +11181,13 @@
     </row>
     <row r="492" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U492">
-        <f t="shared" ref="U492:U555" ca="1" si="10">IF(B492=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="493" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U493">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U493:U556" ca="1" si="10">IF(B493=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11543,13 +11565,13 @@
     </row>
     <row r="556" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U556">
-        <f t="shared" ref="U556:U619" ca="1" si="11">IF(B556=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="557" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U557">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U557:U620" ca="1" si="11">IF(B557=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11927,13 +11949,13 @@
     </row>
     <row r="620" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U620">
-        <f t="shared" ref="U620:U683" ca="1" si="12">IF(B620=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="621" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U621">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U621:U684" ca="1" si="12">IF(B621=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12311,13 +12333,13 @@
     </row>
     <row r="684" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U684">
-        <f t="shared" ref="U684:U747" ca="1" si="13">IF(B684=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="685" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U685">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U685:U748" ca="1" si="13">IF(B685=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12695,13 +12717,13 @@
     </row>
     <row r="748" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U748">
-        <f t="shared" ref="U748:U811" ca="1" si="14">IF(B748=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="749" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U749">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U749:U812" ca="1" si="14">IF(B749=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13079,13 +13101,13 @@
     </row>
     <row r="812" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U812">
-        <f t="shared" ref="U812:U875" ca="1" si="15">IF(B812=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="813" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U813">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U813:U876" ca="1" si="15">IF(B813=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13463,13 +13485,13 @@
     </row>
     <row r="876" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U876">
-        <f t="shared" ref="U876:U937" ca="1" si="16">IF(B876=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="877" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U877">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U877:U938" ca="1" si="16">IF(B877=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13833,26 +13855,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="938" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U938">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A257"/>
+    <mergeCell ref="A329:A334"/>
+    <mergeCell ref="A259:A288"/>
+    <mergeCell ref="A5:A23"/>
+    <mergeCell ref="A307:A322"/>
+    <mergeCell ref="A323:A328"/>
+    <mergeCell ref="A69:A109"/>
+    <mergeCell ref="A231:A242"/>
+    <mergeCell ref="A155:A194"/>
+    <mergeCell ref="A195:A213"/>
+    <mergeCell ref="A110:A154"/>
+    <mergeCell ref="A24:A68"/>
+    <mergeCell ref="A214:A230"/>
+    <mergeCell ref="A243:A250"/>
+    <mergeCell ref="A251:A258"/>
     <mergeCell ref="C3:T3"/>
     <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A301:A305"/>
-    <mergeCell ref="A288:A300"/>
-    <mergeCell ref="A328:A333"/>
-    <mergeCell ref="A258:A287"/>
-    <mergeCell ref="A5:A23"/>
-    <mergeCell ref="A306:A321"/>
-    <mergeCell ref="A322:A327"/>
-    <mergeCell ref="A69:A109"/>
-    <mergeCell ref="A230:A241"/>
-    <mergeCell ref="A155:A193"/>
-    <mergeCell ref="A194:A212"/>
-    <mergeCell ref="A110:A154"/>
-    <mergeCell ref="A24:A68"/>
-    <mergeCell ref="A213:A229"/>
+    <mergeCell ref="A302:A306"/>
+    <mergeCell ref="A289:A301"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add tasks to handle non-number inputs in number tasks
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$306</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$308</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -134,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -484,11 +484,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,15 +534,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,6 +552,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,6 +577,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -870,11 +886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W938"/>
+  <dimension ref="A1:W940"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B195" sqref="B195"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,56 +907,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>6300</v>
+        <v>5121</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="27"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="27"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -1056,7 +1072,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="3">
         <v>1662</v>
       </c>
@@ -1084,7 +1100,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="3">
         <v>4131</v>
       </c>
@@ -1112,7 +1128,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3">
         <v>7365</v>
       </c>
@@ -1140,7 +1156,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="3">
         <v>1910</v>
       </c>
@@ -1168,7 +1184,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="3">
         <v>1640</v>
       </c>
@@ -1196,7 +1212,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="2">
         <v>1860</v>
       </c>
@@ -1224,7 +1240,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2">
         <v>4764</v>
       </c>
@@ -1252,7 +1268,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2">
         <v>2429</v>
       </c>
@@ -1280,7 +1296,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2">
         <v>7472</v>
       </c>
@@ -1308,7 +1324,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2">
         <v>4140</v>
       </c>
@@ -1336,7 +1352,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="2">
         <v>2959</v>
       </c>
@@ -1364,7 +1380,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>7271</v>
       </c>
@@ -1392,7 +1408,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="2">
         <v>2632</v>
       </c>
@@ -2766,7 +2782,7 @@
       </c>
     </row>
     <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B69" s="13">
@@ -2796,7 +2812,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="12">
         <v>2217</v>
       </c>
@@ -2824,7 +2840,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="12">
         <v>1824</v>
       </c>
@@ -2852,7 +2868,7 @@
       </c>
     </row>
     <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="29"/>
       <c r="B72" s="12">
         <v>2564</v>
       </c>
@@ -2880,7 +2896,7 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="12">
         <v>8487</v>
       </c>
@@ -2908,7 +2924,7 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="2">
         <v>8878</v>
       </c>
@@ -2936,7 +2952,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
+      <c r="A75" s="29"/>
       <c r="B75" s="2">
         <v>3072</v>
       </c>
@@ -2964,7 +2980,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="29"/>
       <c r="B76" s="2">
         <v>5980</v>
       </c>
@@ -2992,7 +3008,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="2">
         <v>8174</v>
       </c>
@@ -3020,7 +3036,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="2">
         <v>4257</v>
       </c>
@@ -3048,7 +3064,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
+      <c r="A79" s="29"/>
       <c r="B79" s="2">
         <v>2291</v>
       </c>
@@ -3076,7 +3092,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="2">
         <v>1763</v>
       </c>
@@ -3104,7 +3120,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
+      <c r="A81" s="29"/>
       <c r="B81" s="2">
         <v>5662</v>
       </c>
@@ -3132,7 +3148,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
+      <c r="A82" s="29"/>
       <c r="B82" s="2">
         <v>1945</v>
       </c>
@@ -3160,7 +3176,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="23"/>
+      <c r="A83" s="29"/>
       <c r="B83" s="2">
         <v>1186</v>
       </c>
@@ -3188,7 +3204,7 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="23"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="2">
         <v>8715</v>
       </c>
@@ -3216,7 +3232,7 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="2">
         <v>8518</v>
       </c>
@@ -3244,7 +3260,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
+      <c r="A86" s="29"/>
       <c r="B86" s="2">
         <v>4847</v>
       </c>
@@ -3272,7 +3288,7 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="2">
         <v>6589</v>
       </c>
@@ -3300,7 +3316,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A88" s="23"/>
+      <c r="A88" s="29"/>
       <c r="B88" s="2">
         <v>7991</v>
       </c>
@@ -3328,7 +3344,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A89" s="23"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="2">
         <v>6291</v>
       </c>
@@ -3356,7 +3372,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="2">
         <v>3770</v>
       </c>
@@ -3384,7 +3400,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A91" s="23"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="2">
         <v>7178</v>
       </c>
@@ -3412,7 +3428,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="23"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="2">
         <v>3883</v>
       </c>
@@ -3440,7 +3456,7 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="2">
         <v>1999</v>
       </c>
@@ -3468,7 +3484,7 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="2">
         <v>4042</v>
       </c>
@@ -3496,7 +3512,7 @@
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="2">
         <v>6351</v>
       </c>
@@ -3524,7 +3540,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="2">
         <v>5382</v>
       </c>
@@ -3552,7 +3568,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="23"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="2">
         <v>7088</v>
       </c>
@@ -3580,7 +3596,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A98" s="23"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="2">
         <v>7250</v>
       </c>
@@ -3608,7 +3624,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A99" s="23"/>
+      <c r="A99" s="29"/>
       <c r="B99" s="2">
         <v>6740</v>
       </c>
@@ -3636,7 +3652,7 @@
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" s="23"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="2">
         <v>9038</v>
       </c>
@@ -3664,7 +3680,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A101" s="23"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="2">
         <v>1292</v>
       </c>
@@ -3692,7 +3708,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A102" s="23"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="2">
         <v>4527</v>
       </c>
@@ -3720,7 +3736,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="23"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="2">
         <v>6556</v>
       </c>
@@ -3748,7 +3764,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="2">
         <v>5635</v>
       </c>
@@ -3776,7 +3792,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A105" s="23"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="2">
         <v>3878</v>
       </c>
@@ -3804,7 +3820,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="2">
         <v>1217</v>
       </c>
@@ -3832,7 +3848,7 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" s="23"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="2">
         <v>1438</v>
       </c>
@@ -3860,7 +3876,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="2">
         <v>2153</v>
       </c>
@@ -3888,7 +3904,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="24"/>
+      <c r="A109" s="30"/>
       <c r="B109" s="6">
         <v>7937</v>
       </c>
@@ -3916,7 +3932,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B110" s="13">
@@ -3946,7 +3962,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="23"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="12">
         <v>1881</v>
       </c>
@@ -3974,7 +3990,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="23"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="2">
         <v>8495</v>
       </c>
@@ -4002,7 +4018,7 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" s="23"/>
+      <c r="A113" s="29"/>
       <c r="B113" s="2">
         <v>1315</v>
       </c>
@@ -4030,7 +4046,7 @@
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114" s="23"/>
+      <c r="A114" s="29"/>
       <c r="B114" s="2">
         <v>6066</v>
       </c>
@@ -4058,7 +4074,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="23"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="2">
         <v>2565</v>
       </c>
@@ -4086,7 +4102,7 @@
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" s="23"/>
+      <c r="A116" s="29"/>
       <c r="B116" s="2">
         <v>2594</v>
       </c>
@@ -4114,7 +4130,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" s="23"/>
+      <c r="A117" s="29"/>
       <c r="B117" s="2">
         <v>2321</v>
       </c>
@@ -4142,7 +4158,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="23"/>
+      <c r="A118" s="29"/>
       <c r="B118" s="2">
         <v>5053</v>
       </c>
@@ -4170,7 +4186,7 @@
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119" s="23"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="2">
         <v>4338</v>
       </c>
@@ -4198,7 +4214,7 @@
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" s="23"/>
+      <c r="A120" s="29"/>
       <c r="B120" s="2">
         <v>3762</v>
       </c>
@@ -4226,7 +4242,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="2">
         <v>3550</v>
       </c>
@@ -4254,7 +4270,7 @@
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122" s="23"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="2">
         <v>4264</v>
       </c>
@@ -4282,7 +4298,7 @@
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="23"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="2">
         <v>2475</v>
       </c>
@@ -4310,7 +4326,7 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="2">
         <v>9180</v>
       </c>
@@ -4338,7 +4354,7 @@
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="23"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="2">
         <v>1544</v>
       </c>
@@ -4366,7 +4382,7 @@
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126" s="23"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="2">
         <v>9562</v>
       </c>
@@ -4394,7 +4410,7 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127" s="23"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="2">
         <v>3669</v>
       </c>
@@ -4422,7 +4438,7 @@
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128" s="23"/>
+      <c r="A128" s="29"/>
       <c r="B128" s="2">
         <v>5951</v>
       </c>
@@ -4450,7 +4466,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A129" s="23"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="2">
         <v>2802</v>
       </c>
@@ -4478,7 +4494,7 @@
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A130" s="23"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="2">
         <v>2324</v>
       </c>
@@ -4506,7 +4522,7 @@
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A131" s="23"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="2">
         <v>8731</v>
       </c>
@@ -4534,7 +4550,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="23"/>
+      <c r="A132" s="29"/>
       <c r="B132" s="2">
         <v>4082</v>
       </c>
@@ -4562,7 +4578,7 @@
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A133" s="23"/>
+      <c r="A133" s="29"/>
       <c r="B133" s="2">
         <v>6280</v>
       </c>
@@ -4590,7 +4606,7 @@
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A134" s="23"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="2">
         <v>7585</v>
       </c>
@@ -4618,7 +4634,7 @@
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A135" s="23"/>
+      <c r="A135" s="29"/>
       <c r="B135" s="2">
         <v>1483</v>
       </c>
@@ -4646,7 +4662,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A136" s="23"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="2">
         <v>3983</v>
       </c>
@@ -4674,7 +4690,7 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A137" s="23"/>
+      <c r="A137" s="29"/>
       <c r="B137" s="2">
         <v>8770</v>
       </c>
@@ -4702,7 +4718,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A138" s="23"/>
+      <c r="A138" s="29"/>
       <c r="B138" s="2">
         <v>4236</v>
       </c>
@@ -4730,7 +4746,7 @@
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A139" s="23"/>
+      <c r="A139" s="29"/>
       <c r="B139" s="2">
         <v>8696</v>
       </c>
@@ -4758,7 +4774,7 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="23"/>
+      <c r="A140" s="29"/>
       <c r="B140" s="2">
         <v>5969</v>
       </c>
@@ -4786,7 +4802,7 @@
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A141" s="23"/>
+      <c r="A141" s="29"/>
       <c r="B141" s="2">
         <v>8418</v>
       </c>
@@ -4814,7 +4830,7 @@
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A142" s="23"/>
+      <c r="A142" s="29"/>
       <c r="B142" s="2">
         <v>5170</v>
       </c>
@@ -4842,7 +4858,7 @@
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A143" s="23"/>
+      <c r="A143" s="29"/>
       <c r="B143" s="2">
         <v>8395</v>
       </c>
@@ -4870,7 +4886,7 @@
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A144" s="23"/>
+      <c r="A144" s="29"/>
       <c r="B144" s="2">
         <v>5568</v>
       </c>
@@ -4898,7 +4914,7 @@
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A145" s="23"/>
+      <c r="A145" s="29"/>
       <c r="B145" s="2">
         <v>2592</v>
       </c>
@@ -4926,7 +4942,7 @@
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A146" s="23"/>
+      <c r="A146" s="29"/>
       <c r="B146" s="2">
         <v>4075</v>
       </c>
@@ -4954,7 +4970,7 @@
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A147" s="23"/>
+      <c r="A147" s="29"/>
       <c r="B147" s="2">
         <v>7517</v>
       </c>
@@ -4982,7 +4998,7 @@
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A148" s="23"/>
+      <c r="A148" s="29"/>
       <c r="B148" s="2">
         <v>5448</v>
       </c>
@@ -5010,7 +5026,7 @@
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A149" s="23"/>
+      <c r="A149" s="29"/>
       <c r="B149" s="2">
         <v>6582</v>
       </c>
@@ -5038,7 +5054,7 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A150" s="23"/>
+      <c r="A150" s="29"/>
       <c r="B150" s="2">
         <v>5238</v>
       </c>
@@ -5066,7 +5082,7 @@
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A151" s="23"/>
+      <c r="A151" s="29"/>
       <c r="B151" s="2">
         <v>2084</v>
       </c>
@@ -5094,7 +5110,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A152" s="23"/>
+      <c r="A152" s="29"/>
       <c r="B152" s="2">
         <v>5411</v>
       </c>
@@ -5122,7 +5138,7 @@
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A153" s="23"/>
+      <c r="A153" s="29"/>
       <c r="B153" s="2">
         <v>5171</v>
       </c>
@@ -5150,7 +5166,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="24"/>
+      <c r="A154" s="30"/>
       <c r="B154" s="6">
         <v>1862</v>
       </c>
@@ -5178,7 +5194,7 @@
       </c>
     </row>
     <row r="155" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="22" t="s">
+      <c r="A155" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B155" s="13">
@@ -5208,7 +5224,7 @@
       </c>
     </row>
     <row r="156" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="23"/>
+      <c r="A156" s="29"/>
       <c r="B156" s="12">
         <v>9931</v>
       </c>
@@ -5236,7 +5252,7 @@
       </c>
     </row>
     <row r="157" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="23"/>
+      <c r="A157" s="29"/>
       <c r="B157" s="12">
         <v>9696</v>
       </c>
@@ -5264,7 +5280,7 @@
       </c>
     </row>
     <row r="158" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="23"/>
+      <c r="A158" s="29"/>
       <c r="B158" s="12">
         <v>1947</v>
       </c>
@@ -5292,7 +5308,7 @@
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="23"/>
+      <c r="A159" s="29"/>
       <c r="B159" s="2">
         <v>4425</v>
       </c>
@@ -5320,7 +5336,7 @@
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A160" s="23"/>
+      <c r="A160" s="29"/>
       <c r="B160" s="2">
         <v>1433</v>
       </c>
@@ -5348,7 +5364,7 @@
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A161" s="23"/>
+      <c r="A161" s="29"/>
       <c r="B161" s="2">
         <v>7834</v>
       </c>
@@ -5376,7 +5392,7 @@
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A162" s="23"/>
+      <c r="A162" s="29"/>
       <c r="B162" s="2">
         <v>5683</v>
       </c>
@@ -5404,7 +5420,7 @@
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A163" s="23"/>
+      <c r="A163" s="29"/>
       <c r="B163" s="2">
         <v>1223</v>
       </c>
@@ -5432,7 +5448,7 @@
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A164" s="23"/>
+      <c r="A164" s="29"/>
       <c r="B164" s="2">
         <v>8311</v>
       </c>
@@ -5460,7 +5476,7 @@
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A165" s="23"/>
+      <c r="A165" s="29"/>
       <c r="B165" s="2">
         <v>3134</v>
       </c>
@@ -5488,7 +5504,7 @@
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A166" s="23"/>
+      <c r="A166" s="29"/>
       <c r="B166" s="2">
         <v>9711</v>
       </c>
@@ -5516,7 +5532,7 @@
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A167" s="23"/>
+      <c r="A167" s="29"/>
       <c r="B167" s="2">
         <v>7085</v>
       </c>
@@ -5544,7 +5560,7 @@
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168" s="23"/>
+      <c r="A168" s="29"/>
       <c r="B168" s="2">
         <v>3333</v>
       </c>
@@ -5572,7 +5588,7 @@
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A169" s="23"/>
+      <c r="A169" s="29"/>
       <c r="B169" s="2">
         <v>8820</v>
       </c>
@@ -5600,7 +5616,7 @@
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A170" s="23"/>
+      <c r="A170" s="29"/>
       <c r="B170" s="2">
         <v>5694</v>
       </c>
@@ -5628,7 +5644,7 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A171" s="23"/>
+      <c r="A171" s="29"/>
       <c r="B171" s="2">
         <v>6806</v>
       </c>
@@ -5656,7 +5672,7 @@
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A172" s="23"/>
+      <c r="A172" s="29"/>
       <c r="B172" s="2">
         <v>7369</v>
       </c>
@@ -5684,7 +5700,7 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173" s="23"/>
+      <c r="A173" s="29"/>
       <c r="B173" s="2">
         <v>8613</v>
       </c>
@@ -5712,7 +5728,7 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="23"/>
+      <c r="A174" s="29"/>
       <c r="B174" s="2">
         <v>7534</v>
       </c>
@@ -5740,7 +5756,7 @@
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A175" s="23"/>
+      <c r="A175" s="29"/>
       <c r="B175" s="2">
         <v>2173</v>
       </c>
@@ -5768,7 +5784,7 @@
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" s="23"/>
+      <c r="A176" s="29"/>
       <c r="B176" s="2">
         <v>5894</v>
       </c>
@@ -5796,7 +5812,7 @@
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A177" s="23"/>
+      <c r="A177" s="29"/>
       <c r="B177" s="2">
         <v>4515</v>
       </c>
@@ -5824,7 +5840,7 @@
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A178" s="23"/>
+      <c r="A178" s="29"/>
       <c r="B178" s="2">
         <v>9774</v>
       </c>
@@ -5852,7 +5868,7 @@
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A179" s="23"/>
+      <c r="A179" s="29"/>
       <c r="B179" s="2">
         <v>3946</v>
       </c>
@@ -5880,7 +5896,7 @@
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A180" s="23"/>
+      <c r="A180" s="29"/>
       <c r="B180" s="2">
         <v>6497</v>
       </c>
@@ -5908,7 +5924,7 @@
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A181" s="23"/>
+      <c r="A181" s="29"/>
       <c r="B181" s="2">
         <v>5648</v>
       </c>
@@ -5936,7 +5952,7 @@
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A182" s="23"/>
+      <c r="A182" s="29"/>
       <c r="B182" s="2">
         <v>3940</v>
       </c>
@@ -5964,7 +5980,7 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A183" s="23"/>
+      <c r="A183" s="29"/>
       <c r="B183" s="2">
         <v>7290</v>
       </c>
@@ -5992,7 +6008,7 @@
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A184" s="23"/>
+      <c r="A184" s="29"/>
       <c r="B184" s="2">
         <v>7035</v>
       </c>
@@ -6020,7 +6036,7 @@
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A185" s="23"/>
+      <c r="A185" s="29"/>
       <c r="B185" s="2">
         <v>9271</v>
       </c>
@@ -6048,7 +6064,7 @@
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A186" s="23"/>
+      <c r="A186" s="29"/>
       <c r="B186" s="2">
         <v>8769</v>
       </c>
@@ -6076,7 +6092,7 @@
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A187" s="23"/>
+      <c r="A187" s="29"/>
       <c r="B187" s="2">
         <v>4497</v>
       </c>
@@ -6104,7 +6120,7 @@
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A188" s="23"/>
+      <c r="A188" s="29"/>
       <c r="B188" s="2">
         <v>3218</v>
       </c>
@@ -6132,7 +6148,7 @@
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A189" s="23"/>
+      <c r="A189" s="29"/>
       <c r="B189" s="2">
         <v>6492</v>
       </c>
@@ -6160,7 +6176,7 @@
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A190" s="23"/>
+      <c r="A190" s="29"/>
       <c r="B190" s="2">
         <v>4293</v>
       </c>
@@ -6188,7 +6204,7 @@
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A191" s="23"/>
+      <c r="A191" s="29"/>
       <c r="B191" s="2">
         <v>7703</v>
       </c>
@@ -6216,7 +6232,7 @@
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A192" s="23"/>
+      <c r="A192" s="29"/>
       <c r="B192" s="2">
         <v>5541</v>
       </c>
@@ -6272,7 +6288,7 @@
       </c>
     </row>
     <row r="194" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="24"/>
+      <c r="A194" s="30"/>
       <c r="B194" s="6">
         <v>3095</v>
       </c>
@@ -6300,7 +6316,7 @@
       </c>
     </row>
     <row r="195" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="22" t="s">
+      <c r="A195" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B195" s="13">
@@ -6330,7 +6346,7 @@
       </c>
     </row>
     <row r="196" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="23"/>
+      <c r="A196" s="29"/>
       <c r="B196" s="12">
         <v>9001</v>
       </c>
@@ -6358,7 +6374,7 @@
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" s="23"/>
+      <c r="A197" s="29"/>
       <c r="B197" s="2">
         <v>7491</v>
       </c>
@@ -6386,7 +6402,7 @@
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" s="23"/>
+      <c r="A198" s="29"/>
       <c r="B198" s="2">
         <v>9531</v>
       </c>
@@ -6414,7 +6430,7 @@
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A199" s="23"/>
+      <c r="A199" s="29"/>
       <c r="B199" s="2">
         <v>9812</v>
       </c>
@@ -6442,7 +6458,7 @@
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A200" s="23"/>
+      <c r="A200" s="29"/>
       <c r="B200" s="2">
         <v>9279</v>
       </c>
@@ -6470,7 +6486,7 @@
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A201" s="23"/>
+      <c r="A201" s="29"/>
       <c r="B201" s="2">
         <v>4845</v>
       </c>
@@ -6498,7 +6514,7 @@
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A202" s="23"/>
+      <c r="A202" s="29"/>
       <c r="B202" s="2">
         <v>5728</v>
       </c>
@@ -6526,7 +6542,7 @@
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A203" s="23"/>
+      <c r="A203" s="29"/>
       <c r="B203" s="2">
         <v>7222</v>
       </c>
@@ -6554,7 +6570,7 @@
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A204" s="23"/>
+      <c r="A204" s="29"/>
       <c r="B204" s="2">
         <v>5923</v>
       </c>
@@ -6582,7 +6598,7 @@
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A205" s="23"/>
+      <c r="A205" s="29"/>
       <c r="B205" s="2">
         <v>4265</v>
       </c>
@@ -6610,7 +6626,7 @@
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A206" s="23"/>
+      <c r="A206" s="29"/>
       <c r="B206" s="2">
         <v>2166</v>
       </c>
@@ -6638,7 +6654,7 @@
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A207" s="23"/>
+      <c r="A207" s="29"/>
       <c r="B207" s="2">
         <v>9116</v>
       </c>
@@ -6666,7 +6682,7 @@
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A208" s="23"/>
+      <c r="A208" s="29"/>
       <c r="B208" s="2">
         <v>9925</v>
       </c>
@@ -6694,7 +6710,7 @@
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A209" s="23"/>
+      <c r="A209" s="29"/>
       <c r="B209" s="2">
         <v>3657</v>
       </c>
@@ -6722,7 +6738,7 @@
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A210" s="23"/>
+      <c r="A210" s="29"/>
       <c r="B210" s="2">
         <v>6599</v>
       </c>
@@ -6806,7 +6822,7 @@
       </c>
     </row>
     <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="24"/>
+      <c r="A213" s="30"/>
       <c r="B213" s="6">
         <v>8887</v>
       </c>
@@ -7055,7 +7071,7 @@
       <c r="S221" s="2"/>
       <c r="T221" s="5"/>
       <c r="U221">
-        <f t="shared" ref="U221:U300" ca="1" si="6">IF(B221=$W$1,1,0)</f>
+        <f t="shared" ref="U221:U302" ca="1" si="6">IF(B221=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7312,7 +7328,7 @@
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A231" s="22" t="s">
+      <c r="A231" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B231" s="8">
@@ -7342,7 +7358,7 @@
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A232" s="23"/>
+      <c r="A232" s="29"/>
       <c r="B232" s="2">
         <v>3951</v>
       </c>
@@ -7370,7 +7386,7 @@
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A233" s="23"/>
+      <c r="A233" s="29"/>
       <c r="B233" s="2">
         <v>7343</v>
       </c>
@@ -7398,7 +7414,7 @@
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A234" s="23"/>
+      <c r="A234" s="29"/>
       <c r="B234" s="2">
         <v>7060</v>
       </c>
@@ -7426,7 +7442,7 @@
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A235" s="23"/>
+      <c r="A235" s="29"/>
       <c r="B235" s="2">
         <v>6409</v>
       </c>
@@ -7454,7 +7470,7 @@
       </c>
     </row>
     <row r="236" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A236" s="23"/>
+      <c r="A236" s="29"/>
       <c r="B236" s="2">
         <v>2386</v>
       </c>
@@ -7482,7 +7498,7 @@
       </c>
     </row>
     <row r="237" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="23"/>
+      <c r="A237" s="29"/>
       <c r="B237" s="6">
         <v>7372</v>
       </c>
@@ -7506,7 +7522,7 @@
       <c r="T237" s="5"/>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A238" s="23"/>
+      <c r="A238" s="29"/>
       <c r="B238" s="2">
         <v>9159</v>
       </c>
@@ -7534,7 +7550,7 @@
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A239" s="23"/>
+      <c r="A239" s="29"/>
       <c r="B239" s="2">
         <v>5309</v>
       </c>
@@ -7562,7 +7578,7 @@
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A240" s="23"/>
+      <c r="A240" s="29"/>
       <c r="B240" s="2">
         <v>3290</v>
       </c>
@@ -7590,7 +7606,7 @@
       </c>
     </row>
     <row r="241" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A241" s="23"/>
+      <c r="A241" s="29"/>
       <c r="B241" s="2">
         <v>5345</v>
       </c>
@@ -7618,7 +7634,7 @@
       </c>
     </row>
     <row r="242" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="24"/>
+      <c r="A242" s="30"/>
       <c r="B242" s="6">
         <v>6812</v>
       </c>
@@ -7646,7 +7662,7 @@
       </c>
     </row>
     <row r="243" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A243" s="22" t="s">
+      <c r="A243" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B243" s="13">
@@ -7676,7 +7692,7 @@
       </c>
     </row>
     <row r="244" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A244" s="23"/>
+      <c r="A244" s="29"/>
       <c r="B244" s="12">
         <v>1516</v>
       </c>
@@ -7704,7 +7720,7 @@
       </c>
     </row>
     <row r="245" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="23"/>
+      <c r="A245" s="29"/>
       <c r="B245" s="12">
         <v>9062</v>
       </c>
@@ -7732,7 +7748,7 @@
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A246" s="23"/>
+      <c r="A246" s="29"/>
       <c r="B246" s="19">
         <v>8861</v>
       </c>
@@ -7760,7 +7776,7 @@
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A247" s="23"/>
+      <c r="A247" s="29"/>
       <c r="B247" s="2">
         <v>5164</v>
       </c>
@@ -7788,7 +7804,7 @@
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A248" s="23"/>
+      <c r="A248" s="29"/>
       <c r="B248" s="2">
         <v>2354</v>
       </c>
@@ -7816,7 +7832,7 @@
       </c>
     </row>
     <row r="249" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A249" s="23"/>
+      <c r="A249" s="29"/>
       <c r="B249" s="2">
         <v>2030</v>
       </c>
@@ -7844,7 +7860,7 @@
       </c>
     </row>
     <row r="250" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="24"/>
+      <c r="A250" s="30"/>
       <c r="B250" s="6">
         <v>7649</v>
       </c>
@@ -7872,11 +7888,11 @@
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A251" s="22" t="s">
+      <c r="A251" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B251" s="8">
-        <v>9701</v>
+        <v>7740</v>
       </c>
       <c r="C251" s="8"/>
       <c r="D251" s="8"/>
@@ -7902,37 +7918,37 @@
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A252" s="23"/>
-      <c r="B252" s="2">
-        <v>3784</v>
-      </c>
-      <c r="C252" s="2"/>
-      <c r="D252" s="2"/>
-      <c r="E252" s="2"/>
-      <c r="F252" s="2"/>
-      <c r="G252" s="2"/>
-      <c r="H252" s="2"/>
-      <c r="I252" s="2"/>
-      <c r="J252" s="2"/>
-      <c r="K252" s="2"/>
-      <c r="L252" s="2"/>
-      <c r="M252" s="2"/>
-      <c r="N252" s="2"/>
-      <c r="O252" s="2"/>
-      <c r="P252" s="2"/>
-      <c r="Q252" s="2"/>
-      <c r="R252" s="2"/>
-      <c r="S252" s="2"/>
-      <c r="T252" s="5"/>
+      <c r="A252" s="37"/>
+      <c r="B252" s="3">
+        <v>1439</v>
+      </c>
+      <c r="C252" s="3"/>
+      <c r="D252" s="3"/>
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
+      <c r="H252" s="3"/>
+      <c r="I252" s="3"/>
+      <c r="J252" s="3"/>
+      <c r="K252" s="3"/>
+      <c r="L252" s="3"/>
+      <c r="M252" s="3"/>
+      <c r="N252" s="3"/>
+      <c r="O252" s="3"/>
+      <c r="P252" s="3"/>
+      <c r="Q252" s="3"/>
+      <c r="R252" s="3"/>
+      <c r="S252" s="3"/>
+      <c r="T252" s="4"/>
       <c r="U252">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A253" s="23"/>
+      <c r="A253" s="29"/>
       <c r="B253" s="2">
-        <v>6732</v>
+        <v>9701</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
@@ -7958,9 +7974,9 @@
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" s="23"/>
+      <c r="A254" s="29"/>
       <c r="B254" s="2">
-        <v>6882</v>
+        <v>3784</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -7986,9 +8002,9 @@
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A255" s="23"/>
+      <c r="A255" s="29"/>
       <c r="B255" s="2">
-        <v>1212</v>
+        <v>6732</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
@@ -8014,9 +8030,9 @@
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="23"/>
+      <c r="A256" s="29"/>
       <c r="B256" s="2">
-        <v>9472</v>
+        <v>6882</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -8042,9 +8058,9 @@
       </c>
     </row>
     <row r="257" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A257" s="23"/>
+      <c r="A257" s="29"/>
       <c r="B257" s="2">
-        <v>5081</v>
+        <v>1212</v>
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
@@ -8069,124 +8085,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A258" s="24"/>
-      <c r="B258" s="6">
-        <v>6454</v>
-      </c>
-      <c r="C258" s="6"/>
-      <c r="D258" s="6"/>
-      <c r="E258" s="6"/>
-      <c r="F258" s="6"/>
-      <c r="G258" s="6"/>
-      <c r="H258" s="6"/>
-      <c r="I258" s="6"/>
-      <c r="J258" s="6"/>
-      <c r="K258" s="6"/>
-      <c r="L258" s="6"/>
-      <c r="M258" s="6"/>
-      <c r="N258" s="6"/>
-      <c r="O258" s="6"/>
-      <c r="P258" s="6"/>
-      <c r="Q258" s="6"/>
-      <c r="R258" s="6"/>
-      <c r="S258" s="6"/>
-      <c r="T258" s="7"/>
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A258" s="29"/>
+      <c r="B258" s="2">
+        <v>9472</v>
+      </c>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="E258" s="2"/>
+      <c r="F258" s="2"/>
+      <c r="G258" s="2"/>
+      <c r="H258" s="2"/>
+      <c r="I258" s="2"/>
+      <c r="J258" s="2"/>
+      <c r="K258" s="2"/>
+      <c r="L258" s="2"/>
+      <c r="M258" s="2"/>
+      <c r="N258" s="2"/>
+      <c r="O258" s="2"/>
+      <c r="P258" s="2"/>
+      <c r="Q258" s="2"/>
+      <c r="R258" s="2"/>
+      <c r="S258" s="2"/>
+      <c r="T258" s="5"/>
       <c r="U258">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A259" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B259" s="13">
-        <v>5463</v>
-      </c>
-      <c r="C259" s="8"/>
-      <c r="D259" s="8"/>
-      <c r="E259" s="8"/>
-      <c r="F259" s="8"/>
-      <c r="G259" s="8"/>
-      <c r="H259" s="8"/>
-      <c r="I259" s="8"/>
-      <c r="J259" s="8"/>
-      <c r="K259" s="8"/>
-      <c r="L259" s="8"/>
-      <c r="M259" s="8"/>
-      <c r="N259" s="8"/>
-      <c r="O259" s="8"/>
-      <c r="P259" s="8"/>
-      <c r="Q259" s="8"/>
-      <c r="R259" s="8"/>
-      <c r="S259" s="8"/>
-      <c r="T259" s="14"/>
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A259" s="29"/>
+      <c r="B259" s="2">
+        <v>5081</v>
+      </c>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="2"/>
+      <c r="F259" s="2"/>
+      <c r="G259" s="2"/>
+      <c r="H259" s="2"/>
+      <c r="I259" s="2"/>
+      <c r="J259" s="2"/>
+      <c r="K259" s="2"/>
+      <c r="L259" s="2"/>
+      <c r="M259" s="2"/>
+      <c r="N259" s="2"/>
+      <c r="O259" s="2"/>
+      <c r="P259" s="2"/>
+      <c r="Q259" s="2"/>
+      <c r="R259" s="2"/>
+      <c r="S259" s="2"/>
+      <c r="T259" s="5"/>
       <c r="U259">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A260" s="23"/>
-      <c r="B260" s="2">
-        <v>6011</v>
-      </c>
-      <c r="C260" s="2"/>
-      <c r="D260" s="2"/>
-      <c r="E260" s="2"/>
-      <c r="F260" s="2"/>
-      <c r="G260" s="2"/>
-      <c r="H260" s="2"/>
-      <c r="I260" s="2"/>
-      <c r="J260" s="2"/>
-      <c r="K260" s="2"/>
-      <c r="L260" s="2"/>
-      <c r="M260" s="2"/>
-      <c r="N260" s="2"/>
-      <c r="O260" s="2"/>
-      <c r="P260" s="2"/>
-      <c r="Q260" s="2"/>
-      <c r="R260" s="2"/>
-      <c r="S260" s="2"/>
-      <c r="T260" s="5"/>
+    <row r="260" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="30"/>
+      <c r="B260" s="6">
+        <v>6454</v>
+      </c>
+      <c r="C260" s="6"/>
+      <c r="D260" s="6"/>
+      <c r="E260" s="6"/>
+      <c r="F260" s="6"/>
+      <c r="G260" s="6"/>
+      <c r="H260" s="6"/>
+      <c r="I260" s="6"/>
+      <c r="J260" s="6"/>
+      <c r="K260" s="6"/>
+      <c r="L260" s="6"/>
+      <c r="M260" s="6"/>
+      <c r="N260" s="6"/>
+      <c r="O260" s="6"/>
+      <c r="P260" s="6"/>
+      <c r="Q260" s="6"/>
+      <c r="R260" s="6"/>
+      <c r="S260" s="6"/>
+      <c r="T260" s="7"/>
       <c r="U260">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A261" s="23"/>
-      <c r="B261" s="2">
-        <v>8403</v>
-      </c>
-      <c r="C261" s="2"/>
-      <c r="D261" s="2"/>
-      <c r="E261" s="2"/>
-      <c r="F261" s="2"/>
-      <c r="G261" s="2"/>
-      <c r="H261" s="2"/>
-      <c r="I261" s="2"/>
-      <c r="J261" s="2"/>
-      <c r="K261" s="2"/>
-      <c r="L261" s="2"/>
-      <c r="M261" s="2"/>
-      <c r="N261" s="2"/>
-      <c r="O261" s="2"/>
-      <c r="P261" s="2"/>
-      <c r="Q261" s="2"/>
-      <c r="R261" s="2"/>
-      <c r="S261" s="2"/>
-      <c r="T261" s="5"/>
+    <row r="261" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A261" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B261" s="13">
+        <v>5463</v>
+      </c>
+      <c r="C261" s="8"/>
+      <c r="D261" s="8"/>
+      <c r="E261" s="8"/>
+      <c r="F261" s="8"/>
+      <c r="G261" s="8"/>
+      <c r="H261" s="8"/>
+      <c r="I261" s="8"/>
+      <c r="J261" s="8"/>
+      <c r="K261" s="8"/>
+      <c r="L261" s="8"/>
+      <c r="M261" s="8"/>
+      <c r="N261" s="8"/>
+      <c r="O261" s="8"/>
+      <c r="P261" s="8"/>
+      <c r="Q261" s="8"/>
+      <c r="R261" s="8"/>
+      <c r="S261" s="8"/>
+      <c r="T261" s="14"/>
       <c r="U261">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A262" s="23"/>
+      <c r="A262" s="29"/>
       <c r="B262" s="2">
-        <v>3185</v>
+        <v>6011</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -8212,9 +8228,9 @@
       </c>
     </row>
     <row r="263" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A263" s="23"/>
-      <c r="B263" s="21">
-        <v>6037</v>
+      <c r="A263" s="29"/>
+      <c r="B263" s="2">
+        <v>8403</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -8240,9 +8256,9 @@
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A264" s="23"/>
+      <c r="A264" s="29"/>
       <c r="B264" s="2">
-        <v>9914</v>
+        <v>3185</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -8268,9 +8284,9 @@
       </c>
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A265" s="23"/>
-      <c r="B265" s="2">
-        <v>4916</v>
+      <c r="A265" s="29"/>
+      <c r="B265" s="21">
+        <v>6037</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -8296,9 +8312,9 @@
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A266" s="23"/>
+      <c r="A266" s="29"/>
       <c r="B266" s="2">
-        <v>2809</v>
+        <v>9914</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -8324,9 +8340,9 @@
       </c>
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A267" s="23"/>
+      <c r="A267" s="29"/>
       <c r="B267" s="2">
-        <v>8265</v>
+        <v>4916</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -8352,9 +8368,9 @@
       </c>
     </row>
     <row r="268" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A268" s="23"/>
+      <c r="A268" s="29"/>
       <c r="B268" s="2">
-        <v>2092</v>
+        <v>2809</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -8380,9 +8396,9 @@
       </c>
     </row>
     <row r="269" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A269" s="23"/>
+      <c r="A269" s="29"/>
       <c r="B269" s="2">
-        <v>7297</v>
+        <v>8265</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -8408,9 +8424,9 @@
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A270" s="23"/>
+      <c r="A270" s="29"/>
       <c r="B270" s="2">
-        <v>5242</v>
+        <v>2092</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -8436,9 +8452,9 @@
       </c>
     </row>
     <row r="271" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A271" s="23"/>
+      <c r="A271" s="29"/>
       <c r="B271" s="2">
-        <v>1379</v>
+        <v>7297</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -8464,9 +8480,9 @@
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="23"/>
+      <c r="A272" s="29"/>
       <c r="B272" s="2">
-        <v>2401</v>
+        <v>5242</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -8492,9 +8508,9 @@
       </c>
     </row>
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="23"/>
+      <c r="A273" s="29"/>
       <c r="B273" s="2">
-        <v>5421</v>
+        <v>1379</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -8520,9 +8536,9 @@
       </c>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="23"/>
+      <c r="A274" s="29"/>
       <c r="B274" s="2">
-        <v>9713</v>
+        <v>2401</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -8548,9 +8564,9 @@
       </c>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="23"/>
+      <c r="A275" s="29"/>
       <c r="B275" s="2">
-        <v>7301</v>
+        <v>5421</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -8576,9 +8592,9 @@
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="23"/>
+      <c r="A276" s="29"/>
       <c r="B276" s="2">
-        <v>2000</v>
+        <v>9713</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -8604,9 +8620,9 @@
       </c>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="23"/>
+      <c r="A277" s="29"/>
       <c r="B277" s="2">
-        <v>5449</v>
+        <v>7301</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -8632,9 +8648,9 @@
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A278" s="23"/>
+      <c r="A278" s="29"/>
       <c r="B278" s="2">
-        <v>9238</v>
+        <v>2000</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -8660,9 +8676,9 @@
       </c>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="23"/>
+      <c r="A279" s="29"/>
       <c r="B279" s="2">
-        <v>2662</v>
+        <v>5449</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -8688,9 +8704,9 @@
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A280" s="23"/>
+      <c r="A280" s="29"/>
       <c r="B280" s="2">
-        <v>4147</v>
+        <v>9238</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -8716,9 +8732,9 @@
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A281" s="23"/>
+      <c r="A281" s="29"/>
       <c r="B281" s="2">
-        <v>1953</v>
+        <v>2662</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -8744,9 +8760,9 @@
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A282" s="23"/>
+      <c r="A282" s="29"/>
       <c r="B282" s="2">
-        <v>3956</v>
+        <v>4147</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -8772,9 +8788,9 @@
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A283" s="23"/>
+      <c r="A283" s="29"/>
       <c r="B283" s="2">
-        <v>5032</v>
+        <v>1953</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -8800,9 +8816,9 @@
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A284" s="23"/>
+      <c r="A284" s="29"/>
       <c r="B284" s="2">
-        <v>3567</v>
+        <v>3956</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -8828,9 +8844,9 @@
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A285" s="23"/>
+      <c r="A285" s="29"/>
       <c r="B285" s="2">
-        <v>5108</v>
+        <v>5032</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -8856,9 +8872,9 @@
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A286" s="23"/>
+      <c r="A286" s="29"/>
       <c r="B286" s="2">
-        <v>2033</v>
+        <v>3567</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -8884,9 +8900,9 @@
       </c>
     </row>
     <row r="287" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A287" s="23"/>
+      <c r="A287" s="29"/>
       <c r="B287" s="2">
-        <v>6981</v>
+        <v>5108</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -8911,124 +8927,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="24"/>
-      <c r="B288" s="6">
-        <v>1753</v>
-      </c>
-      <c r="C288" s="6"/>
-      <c r="D288" s="6"/>
-      <c r="E288" s="6"/>
-      <c r="F288" s="6"/>
-      <c r="G288" s="6"/>
-      <c r="H288" s="6"/>
-      <c r="I288" s="6"/>
-      <c r="J288" s="6"/>
-      <c r="K288" s="6"/>
-      <c r="L288" s="6"/>
-      <c r="M288" s="6"/>
-      <c r="N288" s="6"/>
-      <c r="O288" s="6"/>
-      <c r="P288" s="6"/>
-      <c r="Q288" s="6"/>
-      <c r="R288" s="6"/>
-      <c r="S288" s="6"/>
-      <c r="T288" s="7"/>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A288" s="29"/>
+      <c r="B288" s="2">
+        <v>2033</v>
+      </c>
+      <c r="C288" s="2"/>
+      <c r="D288" s="2"/>
+      <c r="E288" s="2"/>
+      <c r="F288" s="2"/>
+      <c r="G288" s="2"/>
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+      <c r="J288" s="2"/>
+      <c r="K288" s="2"/>
+      <c r="L288" s="2"/>
+      <c r="M288" s="2"/>
+      <c r="N288" s="2"/>
+      <c r="O288" s="2"/>
+      <c r="P288" s="2"/>
+      <c r="Q288" s="2"/>
+      <c r="R288" s="2"/>
+      <c r="S288" s="2"/>
+      <c r="T288" s="5"/>
       <c r="U288">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A289" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="A289" s="29"/>
       <c r="B289" s="2">
-        <v>5087</v>
-      </c>
-      <c r="C289" s="8"/>
-      <c r="D289" s="8"/>
-      <c r="E289" s="8"/>
-      <c r="F289" s="8"/>
-      <c r="G289" s="8"/>
-      <c r="H289" s="8"/>
-      <c r="I289" s="8"/>
-      <c r="J289" s="8"/>
-      <c r="K289" s="8"/>
-      <c r="L289" s="8"/>
-      <c r="M289" s="8"/>
-      <c r="N289" s="8"/>
-      <c r="O289" s="8"/>
-      <c r="P289" s="8"/>
-      <c r="Q289" s="8"/>
-      <c r="R289" s="8"/>
-      <c r="S289" s="8"/>
-      <c r="T289" s="14"/>
+        <v>6981</v>
+      </c>
+      <c r="C289" s="2"/>
+      <c r="D289" s="2"/>
+      <c r="E289" s="2"/>
+      <c r="F289" s="2"/>
+      <c r="G289" s="2"/>
+      <c r="H289" s="2"/>
+      <c r="I289" s="2"/>
+      <c r="J289" s="2"/>
+      <c r="K289" s="2"/>
+      <c r="L289" s="2"/>
+      <c r="M289" s="2"/>
+      <c r="N289" s="2"/>
+      <c r="O289" s="2"/>
+      <c r="P289" s="2"/>
+      <c r="Q289" s="2"/>
+      <c r="R289" s="2"/>
+      <c r="S289" s="2"/>
+      <c r="T289" s="5"/>
       <c r="U289">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A290" s="23"/>
-      <c r="B290" s="2">
-        <v>1056</v>
-      </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="E290" s="2"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
-      <c r="I290" s="2"/>
-      <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-      <c r="N290" s="2"/>
-      <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-      <c r="Q290" s="2"/>
-      <c r="R290" s="2"/>
-      <c r="S290" s="2"/>
-      <c r="T290" s="5"/>
+    <row r="290" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="30"/>
+      <c r="B290" s="6">
+        <v>1753</v>
+      </c>
+      <c r="C290" s="6"/>
+      <c r="D290" s="6"/>
+      <c r="E290" s="6"/>
+      <c r="F290" s="6"/>
+      <c r="G290" s="6"/>
+      <c r="H290" s="6"/>
+      <c r="I290" s="6"/>
+      <c r="J290" s="6"/>
+      <c r="K290" s="6"/>
+      <c r="L290" s="6"/>
+      <c r="M290" s="6"/>
+      <c r="N290" s="6"/>
+      <c r="O290" s="6"/>
+      <c r="P290" s="6"/>
+      <c r="Q290" s="6"/>
+      <c r="R290" s="6"/>
+      <c r="S290" s="6"/>
+      <c r="T290" s="7"/>
       <c r="U290">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A291" s="23"/>
+      <c r="A291" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="B291" s="2">
-        <v>9990</v>
-      </c>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2"/>
-      <c r="E291" s="2"/>
-      <c r="F291" s="2"/>
-      <c r="G291" s="2"/>
-      <c r="H291" s="2"/>
-      <c r="I291" s="2"/>
-      <c r="J291" s="2"/>
-      <c r="K291" s="2"/>
-      <c r="L291" s="2"/>
-      <c r="M291" s="2"/>
-      <c r="N291" s="2"/>
-      <c r="O291" s="2"/>
-      <c r="P291" s="2"/>
-      <c r="Q291" s="2"/>
-      <c r="R291" s="2"/>
-      <c r="S291" s="2"/>
-      <c r="T291" s="5"/>
+        <v>5087</v>
+      </c>
+      <c r="C291" s="8"/>
+      <c r="D291" s="8"/>
+      <c r="E291" s="8"/>
+      <c r="F291" s="8"/>
+      <c r="G291" s="8"/>
+      <c r="H291" s="8"/>
+      <c r="I291" s="8"/>
+      <c r="J291" s="8"/>
+      <c r="K291" s="8"/>
+      <c r="L291" s="8"/>
+      <c r="M291" s="8"/>
+      <c r="N291" s="8"/>
+      <c r="O291" s="8"/>
+      <c r="P291" s="8"/>
+      <c r="Q291" s="8"/>
+      <c r="R291" s="8"/>
+      <c r="S291" s="8"/>
+      <c r="T291" s="14"/>
       <c r="U291">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A292" s="23"/>
+      <c r="A292" s="29"/>
       <c r="B292" s="2">
-        <v>7738</v>
+        <v>1056</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -9054,9 +9070,9 @@
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A293" s="23"/>
+      <c r="A293" s="29"/>
       <c r="B293" s="2">
-        <v>8418</v>
+        <v>9990</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -9082,9 +9098,9 @@
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A294" s="23"/>
+      <c r="A294" s="29"/>
       <c r="B294" s="2">
-        <v>9512</v>
+        <v>7738</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -9110,9 +9126,9 @@
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A295" s="23"/>
+      <c r="A295" s="29"/>
       <c r="B295" s="2">
-        <v>9924</v>
+        <v>8418</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -9138,56 +9154,56 @@
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A296" s="31"/>
-      <c r="B296" s="9">
-        <v>7657</v>
-      </c>
-      <c r="C296" s="9"/>
-      <c r="D296" s="9"/>
-      <c r="E296" s="9"/>
-      <c r="F296" s="9"/>
-      <c r="G296" s="9"/>
-      <c r="H296" s="9"/>
-      <c r="I296" s="9"/>
-      <c r="J296" s="9"/>
-      <c r="K296" s="9"/>
-      <c r="L296" s="9"/>
-      <c r="M296" s="9"/>
-      <c r="N296" s="9"/>
-      <c r="O296" s="9"/>
-      <c r="P296" s="9"/>
-      <c r="Q296" s="9"/>
-      <c r="R296" s="9"/>
-      <c r="S296" s="9"/>
-      <c r="T296" s="15"/>
+      <c r="A296" s="29"/>
+      <c r="B296" s="2">
+        <v>9512</v>
+      </c>
+      <c r="C296" s="2"/>
+      <c r="D296" s="2"/>
+      <c r="E296" s="2"/>
+      <c r="F296" s="2"/>
+      <c r="G296" s="2"/>
+      <c r="H296" s="2"/>
+      <c r="I296" s="2"/>
+      <c r="J296" s="2"/>
+      <c r="K296" s="2"/>
+      <c r="L296" s="2"/>
+      <c r="M296" s="2"/>
+      <c r="N296" s="2"/>
+      <c r="O296" s="2"/>
+      <c r="P296" s="2"/>
+      <c r="Q296" s="2"/>
+      <c r="R296" s="2"/>
+      <c r="S296" s="2"/>
+      <c r="T296" s="5"/>
       <c r="U296">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A297" s="31"/>
-      <c r="B297" s="9">
-        <v>2973</v>
-      </c>
-      <c r="C297" s="9"/>
-      <c r="D297" s="9"/>
-      <c r="E297" s="9"/>
-      <c r="F297" s="9"/>
-      <c r="G297" s="9"/>
-      <c r="H297" s="9"/>
-      <c r="I297" s="9"/>
-      <c r="J297" s="9"/>
-      <c r="K297" s="9"/>
-      <c r="L297" s="9"/>
-      <c r="M297" s="9"/>
-      <c r="N297" s="9"/>
-      <c r="O297" s="9"/>
-      <c r="P297" s="9"/>
-      <c r="Q297" s="9"/>
-      <c r="R297" s="9"/>
-      <c r="S297" s="9"/>
-      <c r="T297" s="15"/>
+      <c r="A297" s="29"/>
+      <c r="B297" s="2">
+        <v>9924</v>
+      </c>
+      <c r="C297" s="2"/>
+      <c r="D297" s="2"/>
+      <c r="E297" s="2"/>
+      <c r="F297" s="2"/>
+      <c r="G297" s="2"/>
+      <c r="H297" s="2"/>
+      <c r="I297" s="2"/>
+      <c r="J297" s="2"/>
+      <c r="K297" s="2"/>
+      <c r="L297" s="2"/>
+      <c r="M297" s="2"/>
+      <c r="N297" s="2"/>
+      <c r="O297" s="2"/>
+      <c r="P297" s="2"/>
+      <c r="Q297" s="2"/>
+      <c r="R297" s="2"/>
+      <c r="S297" s="2"/>
+      <c r="T297" s="5"/>
       <c r="U297">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -9196,7 +9212,7 @@
     <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="31"/>
       <c r="B298" s="9">
-        <v>8258</v>
+        <v>7657</v>
       </c>
       <c r="C298" s="9"/>
       <c r="D298" s="9"/>
@@ -9224,7 +9240,7 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="31"/>
       <c r="B299" s="9">
-        <v>7186</v>
+        <v>2973</v>
       </c>
       <c r="C299" s="9"/>
       <c r="D299" s="9"/>
@@ -9252,7 +9268,7 @@
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" s="31"/>
       <c r="B300" s="9">
-        <v>1457</v>
+        <v>8258</v>
       </c>
       <c r="C300" s="9"/>
       <c r="D300" s="9"/>
@@ -9277,124 +9293,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="24"/>
-      <c r="B301" s="6">
+    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A301" s="31"/>
+      <c r="B301" s="9">
+        <v>7186</v>
+      </c>
+      <c r="C301" s="9"/>
+      <c r="D301" s="9"/>
+      <c r="E301" s="9"/>
+      <c r="F301" s="9"/>
+      <c r="G301" s="9"/>
+      <c r="H301" s="9"/>
+      <c r="I301" s="9"/>
+      <c r="J301" s="9"/>
+      <c r="K301" s="9"/>
+      <c r="L301" s="9"/>
+      <c r="M301" s="9"/>
+      <c r="N301" s="9"/>
+      <c r="O301" s="9"/>
+      <c r="P301" s="9"/>
+      <c r="Q301" s="9"/>
+      <c r="R301" s="9"/>
+      <c r="S301" s="9"/>
+      <c r="T301" s="15"/>
+      <c r="U301">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A302" s="31"/>
+      <c r="B302" s="9">
+        <v>1457</v>
+      </c>
+      <c r="C302" s="9"/>
+      <c r="D302" s="9"/>
+      <c r="E302" s="9"/>
+      <c r="F302" s="9"/>
+      <c r="G302" s="9"/>
+      <c r="H302" s="9"/>
+      <c r="I302" s="9"/>
+      <c r="J302" s="9"/>
+      <c r="K302" s="9"/>
+      <c r="L302" s="9"/>
+      <c r="M302" s="9"/>
+      <c r="N302" s="9"/>
+      <c r="O302" s="9"/>
+      <c r="P302" s="9"/>
+      <c r="Q302" s="9"/>
+      <c r="R302" s="9"/>
+      <c r="S302" s="9"/>
+      <c r="T302" s="15"/>
+      <c r="U302">
+        <f t="shared" ca="1" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="30"/>
+      <c r="B303" s="6">
         <v>6876</v>
       </c>
-      <c r="C301" s="6"/>
-      <c r="D301" s="6"/>
-      <c r="E301" s="6"/>
-      <c r="F301" s="6"/>
-      <c r="G301" s="6"/>
-      <c r="H301" s="6"/>
-      <c r="I301" s="6"/>
-      <c r="J301" s="6"/>
-      <c r="K301" s="6"/>
-      <c r="L301" s="6"/>
-      <c r="M301" s="6"/>
-      <c r="N301" s="6"/>
-      <c r="O301" s="6"/>
-      <c r="P301" s="6"/>
-      <c r="Q301" s="6"/>
-      <c r="R301" s="6"/>
-      <c r="S301" s="6"/>
-      <c r="T301" s="7"/>
-      <c r="U301">
-        <f t="shared" ref="U301:U364" ca="1" si="7">IF(B301=$W$1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A302" s="22" t="s">
+      <c r="C303" s="6"/>
+      <c r="D303" s="6"/>
+      <c r="E303" s="6"/>
+      <c r="F303" s="6"/>
+      <c r="G303" s="6"/>
+      <c r="H303" s="6"/>
+      <c r="I303" s="6"/>
+      <c r="J303" s="6"/>
+      <c r="K303" s="6"/>
+      <c r="L303" s="6"/>
+      <c r="M303" s="6"/>
+      <c r="N303" s="6"/>
+      <c r="O303" s="6"/>
+      <c r="P303" s="6"/>
+      <c r="Q303" s="6"/>
+      <c r="R303" s="6"/>
+      <c r="S303" s="6"/>
+      <c r="T303" s="7"/>
+      <c r="U303">
+        <f t="shared" ref="U303:U366" ca="1" si="7">IF(B303=$W$1,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A304" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B302" s="8">
+      <c r="B304" s="8">
         <v>4304</v>
       </c>
-      <c r="C302" s="8"/>
-      <c r="D302" s="8"/>
-      <c r="E302" s="8"/>
-      <c r="F302" s="8"/>
-      <c r="G302" s="8"/>
-      <c r="H302" s="8"/>
-      <c r="I302" s="8"/>
-      <c r="J302" s="8"/>
-      <c r="K302" s="8"/>
-      <c r="L302" s="8"/>
-      <c r="M302" s="8"/>
-      <c r="N302" s="8"/>
-      <c r="O302" s="8"/>
-      <c r="P302" s="8"/>
-      <c r="Q302" s="8"/>
-      <c r="R302" s="8"/>
-      <c r="S302" s="8"/>
-      <c r="T302" s="14"/>
-      <c r="U302">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A303" s="23"/>
-      <c r="B303" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C303" s="2"/>
-      <c r="D303" s="2"/>
-      <c r="E303" s="2"/>
-      <c r="F303" s="2"/>
-      <c r="G303" s="2"/>
-      <c r="H303" s="2"/>
-      <c r="I303" s="2"/>
-      <c r="J303" s="2"/>
-      <c r="K303" s="2"/>
-      <c r="L303" s="2"/>
-      <c r="M303" s="2"/>
-      <c r="N303" s="2"/>
-      <c r="O303" s="2"/>
-      <c r="P303" s="2"/>
-      <c r="Q303" s="2"/>
-      <c r="R303" s="2"/>
-      <c r="S303" s="2"/>
-      <c r="T303" s="5"/>
-      <c r="U303">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A304" s="23"/>
-      <c r="B304" s="2">
-        <v>7693</v>
-      </c>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="E304" s="2"/>
-      <c r="F304" s="2"/>
-      <c r="G304" s="2"/>
-      <c r="H304" s="2"/>
-      <c r="I304" s="2"/>
-      <c r="J304" s="2"/>
-      <c r="K304" s="2"/>
-      <c r="L304" s="2"/>
-      <c r="M304" s="2"/>
-      <c r="N304" s="2"/>
-      <c r="O304" s="2"/>
-      <c r="P304" s="2"/>
-      <c r="Q304" s="2"/>
-      <c r="R304" s="2"/>
-      <c r="S304" s="2"/>
-      <c r="T304" s="5"/>
+      <c r="C304" s="8"/>
+      <c r="D304" s="8"/>
+      <c r="E304" s="8"/>
+      <c r="F304" s="8"/>
+      <c r="G304" s="8"/>
+      <c r="H304" s="8"/>
+      <c r="I304" s="8"/>
+      <c r="J304" s="8"/>
+      <c r="K304" s="8"/>
+      <c r="L304" s="8"/>
+      <c r="M304" s="8"/>
+      <c r="N304" s="8"/>
+      <c r="O304" s="8"/>
+      <c r="P304" s="8"/>
+      <c r="Q304" s="8"/>
+      <c r="R304" s="8"/>
+      <c r="S304" s="8"/>
+      <c r="T304" s="14"/>
       <c r="U304">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A305" s="23"/>
+      <c r="A305" s="29"/>
       <c r="B305" s="2">
-        <v>8718</v>
+        <v>2070</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9419,124 +9435,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A306" s="24"/>
-      <c r="B306" s="6">
-        <v>7248</v>
-      </c>
-      <c r="C306" s="6"/>
-      <c r="D306" s="6"/>
-      <c r="E306" s="6"/>
-      <c r="F306" s="6"/>
-      <c r="G306" s="6"/>
-      <c r="H306" s="6"/>
-      <c r="I306" s="6"/>
-      <c r="J306" s="6"/>
-      <c r="K306" s="6"/>
-      <c r="L306" s="6"/>
-      <c r="M306" s="6"/>
-      <c r="N306" s="6"/>
-      <c r="O306" s="6"/>
-      <c r="P306" s="6"/>
-      <c r="Q306" s="6"/>
-      <c r="R306" s="6"/>
-      <c r="S306" s="6"/>
-      <c r="T306" s="7"/>
+    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A306" s="29"/>
+      <c r="B306" s="2">
+        <v>7693</v>
+      </c>
+      <c r="C306" s="2"/>
+      <c r="D306" s="2"/>
+      <c r="E306" s="2"/>
+      <c r="F306" s="2"/>
+      <c r="G306" s="2"/>
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+      <c r="J306" s="2"/>
+      <c r="K306" s="2"/>
+      <c r="L306" s="2"/>
+      <c r="M306" s="2"/>
+      <c r="N306" s="2"/>
+      <c r="O306" s="2"/>
+      <c r="P306" s="2"/>
+      <c r="Q306" s="2"/>
+      <c r="R306" s="2"/>
+      <c r="S306" s="2"/>
+      <c r="T306" s="5"/>
       <c r="U306">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A307" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B307" s="13">
-        <v>3929</v>
-      </c>
-      <c r="C307" s="8"/>
-      <c r="D307" s="8"/>
-      <c r="E307" s="8"/>
-      <c r="F307" s="8"/>
-      <c r="G307" s="8"/>
-      <c r="H307" s="8"/>
-      <c r="I307" s="8"/>
-      <c r="J307" s="8"/>
-      <c r="K307" s="8"/>
-      <c r="L307" s="8"/>
-      <c r="M307" s="8"/>
-      <c r="N307" s="8"/>
-      <c r="O307" s="8"/>
-      <c r="P307" s="8"/>
-      <c r="Q307" s="8"/>
-      <c r="R307" s="8"/>
-      <c r="S307" s="8"/>
-      <c r="T307" s="14"/>
+    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A307" s="29"/>
+      <c r="B307" s="2">
+        <v>8718</v>
+      </c>
+      <c r="C307" s="2"/>
+      <c r="D307" s="2"/>
+      <c r="E307" s="2"/>
+      <c r="F307" s="2"/>
+      <c r="G307" s="2"/>
+      <c r="H307" s="2"/>
+      <c r="I307" s="2"/>
+      <c r="J307" s="2"/>
+      <c r="K307" s="2"/>
+      <c r="L307" s="2"/>
+      <c r="M307" s="2"/>
+      <c r="N307" s="2"/>
+      <c r="O307" s="2"/>
+      <c r="P307" s="2"/>
+      <c r="Q307" s="2"/>
+      <c r="R307" s="2"/>
+      <c r="S307" s="2"/>
+      <c r="T307" s="5"/>
       <c r="U307">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A308" s="23"/>
-      <c r="B308" s="12">
-        <v>3083</v>
-      </c>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
-      <c r="E308" s="2"/>
-      <c r="F308" s="2"/>
-      <c r="G308" s="2"/>
-      <c r="H308" s="2"/>
-      <c r="I308" s="2"/>
-      <c r="J308" s="2"/>
-      <c r="K308" s="2"/>
-      <c r="L308" s="2"/>
-      <c r="M308" s="2"/>
-      <c r="N308" s="2"/>
-      <c r="O308" s="2"/>
-      <c r="P308" s="2"/>
-      <c r="Q308" s="2"/>
-      <c r="R308" s="2"/>
-      <c r="S308" s="2"/>
-      <c r="T308" s="5"/>
+    <row r="308" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A308" s="30"/>
+      <c r="B308" s="6">
+        <v>7248</v>
+      </c>
+      <c r="C308" s="6"/>
+      <c r="D308" s="6"/>
+      <c r="E308" s="6"/>
+      <c r="F308" s="6"/>
+      <c r="G308" s="6"/>
+      <c r="H308" s="6"/>
+      <c r="I308" s="6"/>
+      <c r="J308" s="6"/>
+      <c r="K308" s="6"/>
+      <c r="L308" s="6"/>
+      <c r="M308" s="6"/>
+      <c r="N308" s="6"/>
+      <c r="O308" s="6"/>
+      <c r="P308" s="6"/>
+      <c r="Q308" s="6"/>
+      <c r="R308" s="6"/>
+      <c r="S308" s="6"/>
+      <c r="T308" s="7"/>
       <c r="U308">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A309" s="23"/>
-      <c r="B309" s="12">
-        <v>7546</v>
-      </c>
-      <c r="C309" s="2"/>
-      <c r="D309" s="2"/>
-      <c r="E309" s="2"/>
-      <c r="F309" s="2"/>
-      <c r="G309" s="2"/>
-      <c r="H309" s="2"/>
-      <c r="I309" s="2"/>
-      <c r="J309" s="2"/>
-      <c r="K309" s="2"/>
-      <c r="L309" s="2"/>
-      <c r="M309" s="2"/>
-      <c r="N309" s="2"/>
-      <c r="O309" s="2"/>
-      <c r="P309" s="2"/>
-      <c r="Q309" s="2"/>
-      <c r="R309" s="2"/>
-      <c r="S309" s="2"/>
-      <c r="T309" s="5"/>
+      <c r="A309" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B309" s="13">
+        <v>3929</v>
+      </c>
+      <c r="C309" s="8"/>
+      <c r="D309" s="8"/>
+      <c r="E309" s="8"/>
+      <c r="F309" s="8"/>
+      <c r="G309" s="8"/>
+      <c r="H309" s="8"/>
+      <c r="I309" s="8"/>
+      <c r="J309" s="8"/>
+      <c r="K309" s="8"/>
+      <c r="L309" s="8"/>
+      <c r="M309" s="8"/>
+      <c r="N309" s="8"/>
+      <c r="O309" s="8"/>
+      <c r="P309" s="8"/>
+      <c r="Q309" s="8"/>
+      <c r="R309" s="8"/>
+      <c r="S309" s="8"/>
+      <c r="T309" s="14"/>
       <c r="U309">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A310" s="23"/>
-      <c r="B310" s="2">
-        <v>7170</v>
+    <row r="310" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A310" s="29"/>
+      <c r="B310" s="12">
+        <v>3083</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -9561,10 +9577,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A311" s="23"/>
-      <c r="B311" s="2">
-        <v>2709</v>
+    <row r="311" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A311" s="29"/>
+      <c r="B311" s="12">
+        <v>7546</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -9590,9 +9606,9 @@
       </c>
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A312" s="23"/>
+      <c r="A312" s="29"/>
       <c r="B312" s="2">
-        <v>3402</v>
+        <v>7170</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -9618,9 +9634,9 @@
       </c>
     </row>
     <row r="313" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A313" s="23"/>
+      <c r="A313" s="29"/>
       <c r="B313" s="2">
-        <v>8781</v>
+        <v>2709</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
@@ -9646,9 +9662,9 @@
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A314" s="23"/>
+      <c r="A314" s="29"/>
       <c r="B314" s="2">
-        <v>8771</v>
+        <v>3402</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -9674,9 +9690,9 @@
       </c>
     </row>
     <row r="315" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A315" s="23"/>
+      <c r="A315" s="29"/>
       <c r="B315" s="2">
-        <v>3091</v>
+        <v>8781</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -9702,9 +9718,9 @@
       </c>
     </row>
     <row r="316" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A316" s="23"/>
+      <c r="A316" s="29"/>
       <c r="B316" s="2">
-        <v>2195</v>
+        <v>8771</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -9730,9 +9746,9 @@
       </c>
     </row>
     <row r="317" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A317" s="23"/>
+      <c r="A317" s="29"/>
       <c r="B317" s="2">
-        <v>1184</v>
+        <v>3091</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -9758,9 +9774,9 @@
       </c>
     </row>
     <row r="318" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A318" s="23"/>
+      <c r="A318" s="29"/>
       <c r="B318" s="2">
-        <v>2667</v>
+        <v>2195</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -9786,9 +9802,9 @@
       </c>
     </row>
     <row r="319" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A319" s="23"/>
+      <c r="A319" s="29"/>
       <c r="B319" s="2">
-        <v>5917</v>
+        <v>1184</v>
       </c>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
@@ -9814,9 +9830,9 @@
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A320" s="23"/>
+      <c r="A320" s="29"/>
       <c r="B320" s="2">
-        <v>8545</v>
+        <v>2667</v>
       </c>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
@@ -9842,9 +9858,9 @@
       </c>
     </row>
     <row r="321" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A321" s="23"/>
+      <c r="A321" s="29"/>
       <c r="B321" s="2">
-        <v>1288</v>
+        <v>5917</v>
       </c>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
@@ -9869,124 +9885,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A322" s="24"/>
-      <c r="B322" s="6">
-        <v>2614</v>
-      </c>
-      <c r="C322" s="6"/>
-      <c r="D322" s="6"/>
-      <c r="E322" s="6"/>
-      <c r="F322" s="6"/>
-      <c r="G322" s="6"/>
-      <c r="H322" s="6"/>
-      <c r="I322" s="6"/>
-      <c r="J322" s="6"/>
-      <c r="K322" s="6"/>
-      <c r="L322" s="6"/>
-      <c r="M322" s="6"/>
-      <c r="N322" s="6"/>
-      <c r="O322" s="6"/>
-      <c r="P322" s="6"/>
-      <c r="Q322" s="6"/>
-      <c r="R322" s="6"/>
-      <c r="S322" s="6"/>
-      <c r="T322" s="7"/>
+    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A322" s="29"/>
+      <c r="B322" s="2">
+        <v>8545</v>
+      </c>
+      <c r="C322" s="2"/>
+      <c r="D322" s="2"/>
+      <c r="E322" s="2"/>
+      <c r="F322" s="2"/>
+      <c r="G322" s="2"/>
+      <c r="H322" s="2"/>
+      <c r="I322" s="2"/>
+      <c r="J322" s="2"/>
+      <c r="K322" s="2"/>
+      <c r="L322" s="2"/>
+      <c r="M322" s="2"/>
+      <c r="N322" s="2"/>
+      <c r="O322" s="2"/>
+      <c r="P322" s="2"/>
+      <c r="Q322" s="2"/>
+      <c r="R322" s="2"/>
+      <c r="S322" s="2"/>
+      <c r="T322" s="5"/>
       <c r="U322">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A323" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B323" s="8">
-        <v>6912</v>
-      </c>
-      <c r="C323" s="8"/>
-      <c r="D323" s="8"/>
-      <c r="E323" s="8"/>
-      <c r="F323" s="8"/>
-      <c r="G323" s="8"/>
-      <c r="H323" s="8"/>
-      <c r="I323" s="8"/>
-      <c r="J323" s="8"/>
-      <c r="K323" s="8"/>
-      <c r="L323" s="8"/>
-      <c r="M323" s="8"/>
-      <c r="N323" s="8"/>
-      <c r="O323" s="8"/>
-      <c r="P323" s="8"/>
-      <c r="Q323" s="8"/>
-      <c r="R323" s="8"/>
-      <c r="S323" s="8"/>
-      <c r="T323" s="14"/>
+      <c r="A323" s="29"/>
+      <c r="B323" s="2">
+        <v>1288</v>
+      </c>
+      <c r="C323" s="2"/>
+      <c r="D323" s="2"/>
+      <c r="E323" s="2"/>
+      <c r="F323" s="2"/>
+      <c r="G323" s="2"/>
+      <c r="H323" s="2"/>
+      <c r="I323" s="2"/>
+      <c r="J323" s="2"/>
+      <c r="K323" s="2"/>
+      <c r="L323" s="2"/>
+      <c r="M323" s="2"/>
+      <c r="N323" s="2"/>
+      <c r="O323" s="2"/>
+      <c r="P323" s="2"/>
+      <c r="Q323" s="2"/>
+      <c r="R323" s="2"/>
+      <c r="S323" s="2"/>
+      <c r="T323" s="5"/>
       <c r="U323">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A324" s="23"/>
-      <c r="B324" s="2">
-        <v>6598</v>
-      </c>
-      <c r="C324" s="2"/>
-      <c r="D324" s="2"/>
-      <c r="E324" s="2"/>
-      <c r="F324" s="2"/>
-      <c r="G324" s="2"/>
-      <c r="H324" s="2"/>
-      <c r="I324" s="2"/>
-      <c r="J324" s="2"/>
-      <c r="K324" s="2"/>
-      <c r="L324" s="2"/>
-      <c r="M324" s="2"/>
-      <c r="N324" s="2"/>
-      <c r="O324" s="2"/>
-      <c r="P324" s="2"/>
-      <c r="Q324" s="2"/>
-      <c r="R324" s="2"/>
-      <c r="S324" s="2"/>
-      <c r="T324" s="5"/>
+    <row r="324" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="30"/>
+      <c r="B324" s="6">
+        <v>2614</v>
+      </c>
+      <c r="C324" s="6"/>
+      <c r="D324" s="6"/>
+      <c r="E324" s="6"/>
+      <c r="F324" s="6"/>
+      <c r="G324" s="6"/>
+      <c r="H324" s="6"/>
+      <c r="I324" s="6"/>
+      <c r="J324" s="6"/>
+      <c r="K324" s="6"/>
+      <c r="L324" s="6"/>
+      <c r="M324" s="6"/>
+      <c r="N324" s="6"/>
+      <c r="O324" s="6"/>
+      <c r="P324" s="6"/>
+      <c r="Q324" s="6"/>
+      <c r="R324" s="6"/>
+      <c r="S324" s="6"/>
+      <c r="T324" s="7"/>
       <c r="U324">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A325" s="23"/>
-      <c r="B325" s="2">
-        <v>3093</v>
-      </c>
-      <c r="C325" s="2"/>
-      <c r="D325" s="2"/>
-      <c r="E325" s="2"/>
-      <c r="F325" s="2"/>
-      <c r="G325" s="2"/>
-      <c r="H325" s="2"/>
-      <c r="I325" s="2"/>
-      <c r="J325" s="2"/>
-      <c r="K325" s="2"/>
-      <c r="L325" s="2"/>
-      <c r="M325" s="2"/>
-      <c r="N325" s="2"/>
-      <c r="O325" s="2"/>
-      <c r="P325" s="2"/>
-      <c r="Q325" s="2"/>
-      <c r="R325" s="2"/>
-      <c r="S325" s="2"/>
-      <c r="T325" s="5"/>
+      <c r="A325" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B325" s="8">
+        <v>6912</v>
+      </c>
+      <c r="C325" s="8"/>
+      <c r="D325" s="8"/>
+      <c r="E325" s="8"/>
+      <c r="F325" s="8"/>
+      <c r="G325" s="8"/>
+      <c r="H325" s="8"/>
+      <c r="I325" s="8"/>
+      <c r="J325" s="8"/>
+      <c r="K325" s="8"/>
+      <c r="L325" s="8"/>
+      <c r="M325" s="8"/>
+      <c r="N325" s="8"/>
+      <c r="O325" s="8"/>
+      <c r="P325" s="8"/>
+      <c r="Q325" s="8"/>
+      <c r="R325" s="8"/>
+      <c r="S325" s="8"/>
+      <c r="T325" s="14"/>
       <c r="U325">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A326" s="23"/>
+      <c r="A326" s="29"/>
       <c r="B326" s="2">
-        <v>8805</v>
+        <v>6598</v>
       </c>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
@@ -10012,9 +10028,9 @@
       </c>
     </row>
     <row r="327" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A327" s="23"/>
+      <c r="A327" s="29"/>
       <c r="B327" s="2">
-        <v>8158</v>
+        <v>3093</v>
       </c>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
@@ -10039,124 +10055,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A328" s="24"/>
-      <c r="B328" s="6">
-        <v>6499</v>
-      </c>
-      <c r="C328" s="6"/>
-      <c r="D328" s="6"/>
-      <c r="E328" s="6"/>
-      <c r="F328" s="6"/>
-      <c r="G328" s="6"/>
-      <c r="H328" s="6"/>
-      <c r="I328" s="6"/>
-      <c r="J328" s="6"/>
-      <c r="K328" s="6"/>
-      <c r="L328" s="6"/>
-      <c r="M328" s="6"/>
-      <c r="N328" s="6"/>
-      <c r="O328" s="6"/>
-      <c r="P328" s="6"/>
-      <c r="Q328" s="6"/>
-      <c r="R328" s="6"/>
-      <c r="S328" s="6"/>
-      <c r="T328" s="7"/>
+    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A328" s="29"/>
+      <c r="B328" s="2">
+        <v>8805</v>
+      </c>
+      <c r="C328" s="2"/>
+      <c r="D328" s="2"/>
+      <c r="E328" s="2"/>
+      <c r="F328" s="2"/>
+      <c r="G328" s="2"/>
+      <c r="H328" s="2"/>
+      <c r="I328" s="2"/>
+      <c r="J328" s="2"/>
+      <c r="K328" s="2"/>
+      <c r="L328" s="2"/>
+      <c r="M328" s="2"/>
+      <c r="N328" s="2"/>
+      <c r="O328" s="2"/>
+      <c r="P328" s="2"/>
+      <c r="Q328" s="2"/>
+      <c r="R328" s="2"/>
+      <c r="S328" s="2"/>
+      <c r="T328" s="5"/>
       <c r="U328">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A329" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B329" s="8">
-        <v>9299</v>
-      </c>
-      <c r="C329" s="8"/>
-      <c r="D329" s="8"/>
-      <c r="E329" s="8"/>
-      <c r="F329" s="8"/>
-      <c r="G329" s="8"/>
-      <c r="H329" s="8"/>
-      <c r="I329" s="8"/>
-      <c r="J329" s="8"/>
-      <c r="K329" s="8"/>
-      <c r="L329" s="8"/>
-      <c r="M329" s="8"/>
-      <c r="N329" s="8"/>
-      <c r="O329" s="8"/>
-      <c r="P329" s="8"/>
-      <c r="Q329" s="8"/>
-      <c r="R329" s="8"/>
-      <c r="S329" s="8"/>
-      <c r="T329" s="14"/>
+      <c r="A329" s="29"/>
+      <c r="B329" s="2">
+        <v>8158</v>
+      </c>
+      <c r="C329" s="2"/>
+      <c r="D329" s="2"/>
+      <c r="E329" s="2"/>
+      <c r="F329" s="2"/>
+      <c r="G329" s="2"/>
+      <c r="H329" s="2"/>
+      <c r="I329" s="2"/>
+      <c r="J329" s="2"/>
+      <c r="K329" s="2"/>
+      <c r="L329" s="2"/>
+      <c r="M329" s="2"/>
+      <c r="N329" s="2"/>
+      <c r="O329" s="2"/>
+      <c r="P329" s="2"/>
+      <c r="Q329" s="2"/>
+      <c r="R329" s="2"/>
+      <c r="S329" s="2"/>
+      <c r="T329" s="5"/>
       <c r="U329">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A330" s="23"/>
-      <c r="B330" s="2">
-        <v>7560</v>
-      </c>
-      <c r="C330" s="2"/>
-      <c r="D330" s="2"/>
-      <c r="E330" s="2"/>
-      <c r="F330" s="2"/>
-      <c r="G330" s="2"/>
-      <c r="H330" s="2"/>
-      <c r="I330" s="2"/>
-      <c r="J330" s="2"/>
-      <c r="K330" s="2"/>
-      <c r="L330" s="2"/>
-      <c r="M330" s="2"/>
-      <c r="N330" s="2"/>
-      <c r="O330" s="2"/>
-      <c r="P330" s="2"/>
-      <c r="Q330" s="2"/>
-      <c r="R330" s="2"/>
-      <c r="S330" s="2"/>
-      <c r="T330" s="5"/>
+    <row r="330" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="30"/>
+      <c r="B330" s="6">
+        <v>6499</v>
+      </c>
+      <c r="C330" s="6"/>
+      <c r="D330" s="6"/>
+      <c r="E330" s="6"/>
+      <c r="F330" s="6"/>
+      <c r="G330" s="6"/>
+      <c r="H330" s="6"/>
+      <c r="I330" s="6"/>
+      <c r="J330" s="6"/>
+      <c r="K330" s="6"/>
+      <c r="L330" s="6"/>
+      <c r="M330" s="6"/>
+      <c r="N330" s="6"/>
+      <c r="O330" s="6"/>
+      <c r="P330" s="6"/>
+      <c r="Q330" s="6"/>
+      <c r="R330" s="6"/>
+      <c r="S330" s="6"/>
+      <c r="T330" s="7"/>
       <c r="U330">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A331" s="23"/>
-      <c r="B331" s="2">
-        <v>9002</v>
-      </c>
-      <c r="C331" s="2"/>
-      <c r="D331" s="2"/>
-      <c r="E331" s="2"/>
-      <c r="F331" s="2"/>
-      <c r="G331" s="2"/>
-      <c r="H331" s="2"/>
-      <c r="I331" s="2"/>
-      <c r="J331" s="2"/>
-      <c r="K331" s="2"/>
-      <c r="L331" s="2"/>
-      <c r="M331" s="2"/>
-      <c r="N331" s="2"/>
-      <c r="O331" s="2"/>
-      <c r="P331" s="2"/>
-      <c r="Q331" s="2"/>
-      <c r="R331" s="2"/>
-      <c r="S331" s="2"/>
-      <c r="T331" s="5"/>
+      <c r="A331" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B331" s="8">
+        <v>9299</v>
+      </c>
+      <c r="C331" s="8"/>
+      <c r="D331" s="8"/>
+      <c r="E331" s="8"/>
+      <c r="F331" s="8"/>
+      <c r="G331" s="8"/>
+      <c r="H331" s="8"/>
+      <c r="I331" s="8"/>
+      <c r="J331" s="8"/>
+      <c r="K331" s="8"/>
+      <c r="L331" s="8"/>
+      <c r="M331" s="8"/>
+      <c r="N331" s="8"/>
+      <c r="O331" s="8"/>
+      <c r="P331" s="8"/>
+      <c r="Q331" s="8"/>
+      <c r="R331" s="8"/>
+      <c r="S331" s="8"/>
+      <c r="T331" s="14"/>
       <c r="U331">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A332" s="23"/>
+      <c r="A332" s="29"/>
       <c r="B332" s="2">
-        <v>7432</v>
+        <v>7560</v>
       </c>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
@@ -10182,9 +10198,9 @@
       </c>
     </row>
     <row r="333" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A333" s="23"/>
+      <c r="A333" s="29"/>
       <c r="B333" s="2">
-        <v>1954</v>
+        <v>9002</v>
       </c>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
@@ -10209,41 +10225,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A334" s="24"/>
-      <c r="B334" s="6">
-        <v>2048</v>
-      </c>
-      <c r="C334" s="6"/>
-      <c r="D334" s="6"/>
-      <c r="E334" s="6"/>
-      <c r="F334" s="6"/>
-      <c r="G334" s="6"/>
-      <c r="H334" s="6"/>
-      <c r="I334" s="6"/>
-      <c r="J334" s="6"/>
-      <c r="K334" s="6"/>
-      <c r="L334" s="6"/>
-      <c r="M334" s="6"/>
-      <c r="N334" s="6"/>
-      <c r="O334" s="6"/>
-      <c r="P334" s="6"/>
-      <c r="Q334" s="6"/>
-      <c r="R334" s="6"/>
-      <c r="S334" s="6"/>
-      <c r="T334" s="7"/>
+    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A334" s="29"/>
+      <c r="B334" s="2">
+        <v>7432</v>
+      </c>
+      <c r="C334" s="2"/>
+      <c r="D334" s="2"/>
+      <c r="E334" s="2"/>
+      <c r="F334" s="2"/>
+      <c r="G334" s="2"/>
+      <c r="H334" s="2"/>
+      <c r="I334" s="2"/>
+      <c r="J334" s="2"/>
+      <c r="K334" s="2"/>
+      <c r="L334" s="2"/>
+      <c r="M334" s="2"/>
+      <c r="N334" s="2"/>
+      <c r="O334" s="2"/>
+      <c r="P334" s="2"/>
+      <c r="Q334" s="2"/>
+      <c r="R334" s="2"/>
+      <c r="S334" s="2"/>
+      <c r="T334" s="5"/>
       <c r="U334">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A335" s="29"/>
+      <c r="B335" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C335" s="2"/>
+      <c r="D335" s="2"/>
+      <c r="E335" s="2"/>
+      <c r="F335" s="2"/>
+      <c r="G335" s="2"/>
+      <c r="H335" s="2"/>
+      <c r="I335" s="2"/>
+      <c r="J335" s="2"/>
+      <c r="K335" s="2"/>
+      <c r="L335" s="2"/>
+      <c r="M335" s="2"/>
+      <c r="N335" s="2"/>
+      <c r="O335" s="2"/>
+      <c r="P335" s="2"/>
+      <c r="Q335" s="2"/>
+      <c r="R335" s="2"/>
+      <c r="S335" s="2"/>
+      <c r="T335" s="5"/>
       <c r="U335">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A336" s="30"/>
+      <c r="B336" s="6">
+        <v>2048</v>
+      </c>
+      <c r="C336" s="6"/>
+      <c r="D336" s="6"/>
+      <c r="E336" s="6"/>
+      <c r="F336" s="6"/>
+      <c r="G336" s="6"/>
+      <c r="H336" s="6"/>
+      <c r="I336" s="6"/>
+      <c r="J336" s="6"/>
+      <c r="K336" s="6"/>
+      <c r="L336" s="6"/>
+      <c r="M336" s="6"/>
+      <c r="N336" s="6"/>
+      <c r="O336" s="6"/>
+      <c r="P336" s="6"/>
+      <c r="Q336" s="6"/>
+      <c r="R336" s="6"/>
+      <c r="S336" s="6"/>
+      <c r="T336" s="7"/>
       <c r="U336">
         <f t="shared" ca="1" si="7"/>
         <v>0</v>
@@ -10419,19 +10479,19 @@
     </row>
     <row r="365" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U365">
-        <f t="shared" ref="U365:U428" ca="1" si="8">IF(B365=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="366" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U366">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="367" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U367">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ref="U367:U430" ca="1" si="8">IF(B367=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -10803,19 +10863,19 @@
     </row>
     <row r="429" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U429">
-        <f t="shared" ref="U429:U492" ca="1" si="9">IF(B429=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="430" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U430">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="431" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U431">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ref="U431:U494" ca="1" si="9">IF(B431=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11187,19 +11247,19 @@
     </row>
     <row r="493" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U493">
-        <f t="shared" ref="U493:U556" ca="1" si="10">IF(B493=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="494" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U494">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="495" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U495">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="U495:U558" ca="1" si="10">IF(B495=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11571,19 +11631,19 @@
     </row>
     <row r="557" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U557">
-        <f t="shared" ref="U557:U620" ca="1" si="11">IF(B557=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="558" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U558">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="559" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U559">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="U559:U622" ca="1" si="11">IF(B559=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11955,19 +12015,19 @@
     </row>
     <row r="621" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U621">
-        <f t="shared" ref="U621:U684" ca="1" si="12">IF(B621=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="622" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U622">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="623" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U623">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="U623:U686" ca="1" si="12">IF(B623=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12339,19 +12399,19 @@
     </row>
     <row r="685" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U685">
-        <f t="shared" ref="U685:U748" ca="1" si="13">IF(B685=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="686" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U686">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="687" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U687">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="U687:U750" ca="1" si="13">IF(B687=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12723,19 +12783,19 @@
     </row>
     <row r="749" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U749">
-        <f t="shared" ref="U749:U812" ca="1" si="14">IF(B749=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="750" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U750">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="751" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U751">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="U751:U814" ca="1" si="14">IF(B751=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13107,19 +13167,19 @@
     </row>
     <row r="813" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U813">
-        <f t="shared" ref="U813:U876" ca="1" si="15">IF(B813=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="814" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U814">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="815" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U815">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ref="U815:U878" ca="1" si="15">IF(B815=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13491,19 +13551,19 @@
     </row>
     <row r="877" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U877">
-        <f t="shared" ref="U877:U938" ca="1" si="16">IF(B877=$W$1,1,0)</f>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="878" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U878">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="879" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U879">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ref="U879:U940" ca="1" si="16">IF(B879=$W$1,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13861,13 +13921,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="939" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U939">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="940" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U940">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A329:A334"/>
-    <mergeCell ref="A259:A288"/>
+    <mergeCell ref="A243:A250"/>
+    <mergeCell ref="A251:A260"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A304:A308"/>
+    <mergeCell ref="A291:A303"/>
+    <mergeCell ref="A331:A336"/>
+    <mergeCell ref="A261:A290"/>
     <mergeCell ref="A5:A23"/>
-    <mergeCell ref="A307:A322"/>
-    <mergeCell ref="A323:A328"/>
+    <mergeCell ref="A309:A324"/>
+    <mergeCell ref="A325:A330"/>
     <mergeCell ref="A69:A109"/>
     <mergeCell ref="A231:A242"/>
     <mergeCell ref="A155:A194"/>
@@ -13875,12 +13953,6 @@
     <mergeCell ref="A110:A154"/>
     <mergeCell ref="A24:A68"/>
     <mergeCell ref="A214:A230"/>
-    <mergeCell ref="A243:A250"/>
-    <mergeCell ref="A251:A258"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A302:A306"/>
-    <mergeCell ref="A289:A301"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
group tasks in lab15 by collection class rework tasks about comparators
</commit_message>
<xml_diff>
--- a/src/numbersMap.xlsx
+++ b/src/numbersMap.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$310</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$2:$T$311</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -529,6 +529,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,15 +559,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -572,9 +575,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,11 +879,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W942"/>
+  <dimension ref="A1:W943"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,56 +900,56 @@
       </c>
       <c r="W1">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3783</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
       <c r="A3" s="16"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:23" ht="89.25" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -979,7 +979,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="15.75">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13">
@@ -1009,7 +1009,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75">
-      <c r="A6" s="33"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="12">
         <v>1413</v>
       </c>
@@ -1037,7 +1037,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75">
-      <c r="A7" s="33"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="12">
         <v>9405</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3">
         <v>1662</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="29"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3">
         <v>4131</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3">
         <v>7365</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="29"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3">
         <v>1910</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="29"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3">
         <v>1640</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="29"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2">
         <v>1860</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="29"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2">
         <v>4764</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="29"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2">
         <v>2429</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="29"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2">
         <v>7472</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="29"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="2">
         <v>4140</v>
       </c>
@@ -1345,7 +1345,7 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="29"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2">
         <v>2959</v>
       </c>
@@ -1373,7 +1373,7 @@
       </c>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="29"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2">
         <v>7271</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
  